<commit_message>
Analysis of the iGEM files - 1st version
</commit_message>
<xml_diff>
--- a/Project_python/out/All/all_model.xlsx
+++ b/Project_python/out/All/all_model.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[3, 11, 14]</t>
+          <t>[11, 14]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -479,7 +479,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.327|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.138|x11: 0.202|x12: 0.091|x13: 0.088|x14: 0.066|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.136|x4: 0.141|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.066|x9: 0.186|x10: 0.000|x11: 0.246|x12: 0.159|x13: 0.097|x14: 0.603|x15: 0.000|x16: 0.186|x17: 0.000
 TOP2VEC -&gt; x1: 0.083|x2: 0.198|x3: 0.137|x4: 0.235|x5: 0.268|x6: 0.408|x7: 0.119|x8: 0.077|x9: 0.113|x10: 0.000|x11: 0.263|x12: 0.329|x13: 0.198|x14: 0.404|x15: 0.120|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.066|x3: 0.200|x4: 0.125|x5: 0.089|x6: 0.136|x7: 0.040|x8: 0.048|x9: 0.100|x10: 0.046|x11: 0.237|x12: 0.193|x13: 0.128|x14: 0.358|x15: 0.040|x16: 0.062|x17: 0.000
+MEAN -&gt; x1: 0.028|x2: 0.066|x3: 0.200|x4: 0.125|x5: 0.089|x6: 0.136|x7: 0.040|x8: 0.048|x9: 0.100|x10: 0.046|x11: 0.237|x12: 0.193|x13: 0.128|x14: 0.323|x15: 0.040|x16: 0.062|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.064|x4: 0.060|x5: 0.057|x6: 0.060|x7: 0.055|x8: 0.055|x9: 0.058|x10: 0.055|x11: 0.067|x12: 0.064|x13: 0.060|x14: 0.073|x15: 0.055|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -500,7 +501,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 4, 8, 9]</t>
+          <t>[4, 9]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -508,7 +509,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.056|x2: 0.000|x3: 0.805|x4: 0.069|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.130|x11: 0.465|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.157|x2: 0.175|x3: 0.075|x4: 0.283|x5: 0.000|x6: 0.000|x7: 0.072|x8: 0.302|x9: 0.272|x10: 0.156|x11: 0.000|x12: 0.000|x13: 0.059|x14: 0.120|x15: 0.150|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.179|x2: 0.136|x3: 0.000|x4: 0.461|x5: 0.279|x6: 0.156|x7: 0.293|x8: 0.274|x9: 0.379|x10: 0.093|x11: 0.100|x12: 0.182|x13: 0.076|x14: 0.139|x15: 0.108|x16: 0.190|x17: 0.000
-MEAN -&gt; x1: 0.131|x2: 0.104|x3: 0.293|x4: 0.271|x5: 0.093|x6: 0.052|x7: 0.122|x8: 0.192|x9: 0.217|x10: 0.126|x11: 0.188|x12: 0.061|x13: 0.045|x14: 0.086|x15: 0.086|x16: 0.063|x17: 0.000
+MEAN -&gt; x1: 0.131|x2: 0.104|x3: 0.192|x4: 0.271|x5: 0.093|x6: 0.052|x7: 0.122|x8: 0.192|x9: 0.217|x10: 0.126|x11: 0.188|x12: 0.061|x13: 0.045|x14: 0.086|x15: 0.086|x16: 0.063|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.063|x4: 0.068|x5: 0.057|x6: 0.055|x7: 0.059|x8: 0.063|x9: 0.065|x10: 0.059|x11: 0.063|x12: 0.055|x13: 0.054|x14: 0.057|x15: 0.057|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -529,15 +531,16 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[3, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.620|x4: 0.000|x5: 0.000|x6: 0.089|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.358|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.118|x2: 0.229|x3: 0.111|x4: 0.190|x5: 0.227|x6: 0.114|x7: 0.065|x8: 0.073|x9: 0.129|x10: 0.078|x11: 0.000|x12: 0.054|x13: 0.068|x14: 0.148|x15: 0.063|x16: 0.153|x17: 0.000
-TOP2VEC -&gt; x1: 0.190|x2: 0.131|x3: 0.000|x4: 0.234|x5: 0.192|x6: 0.184|x7: 0.407|x8: 0.224|x9: 0.282|x10: 0.065|x11: 0.222|x12: 0.118|x13: 0.278|x14: 0.215|x15: 0.259|x16: 0.134|x17: 0.000
-MEAN -&gt; x1: 0.103|x2: 0.120|x3: 0.244|x4: 0.141|x5: 0.140|x6: 0.129|x7: 0.158|x8: 0.099|x9: 0.137|x10: 0.048|x11: 0.194|x12: 0.057|x13: 0.115|x14: 0.121|x15: 0.107|x16: 0.096|x17: 0.000
+TOP2VEC -&gt; x1: 0.190|x2: 0.131|x3: 0.000|x4: 0.234|x5: 0.192|x6: 0.184|x7: 0.407|x8: 0.224|x9: 0.282|x10: 0.065|x11: 0.222|x12: 0.118|x13: 0.278|x14: 0.214|x15: 0.259|x16: 0.134|x17: 0.000
+MEAN -&gt; x1: 0.103|x2: 0.120|x3: 0.204|x4: 0.141|x5: 0.140|x6: 0.129|x7: 0.158|x8: 0.099|x9: 0.137|x10: 0.048|x11: 0.194|x12: 0.057|x13: 0.115|x14: 0.121|x15: 0.107|x16: 0.096|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.059|x3: 0.064|x4: 0.060|x5: 0.060|x6: 0.060|x7: 0.061|x8: 0.058|x9: 0.060|x10: 0.055|x11: 0.064|x12: 0.055|x13: 0.059|x14: 0.059|x15: 0.058|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -565,8 +568,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.211|x2: 0.000|x3: 0.113|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.169|x9: 0.000|x10: 0.941|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.247|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.143|x3: 0.203|x4: 0.195|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.374|x9: 0.080|x10: 0.475|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.247|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.169|x2: 0.107|x3: 0.000|x4: 0.468|x5: 0.297|x6: 0.161|x7: 0.443|x8: 0.209|x9: 0.209|x10: 0.060|x11: 0.000|x12: 0.132|x13: 0.183|x14: 0.124|x15: 0.000|x16: 0.124|x17: 0.000
-MEAN -&gt; x1: 0.161|x2: 0.084|x3: 0.105|x4: 0.221|x5: 0.099|x6: 0.054|x7: 0.148|x8: 0.251|x9: 0.096|x10: 0.492|x11: 0.022|x12: 0.044|x13: 0.061|x14: 0.123|x15: 0.000|x16: 0.124|x17: 0.000
+TOP2VEC -&gt; x1: 0.169|x2: 0.107|x3: 0.000|x4: 0.468|x5: 0.297|x6: 0.161|x7: 0.443|x8: 0.209|x9: 0.209|x10: 0.060|x11: 0.000|x12: 0.132|x13: 0.183|x14: 0.124|x15: 0.000|x16: 0.123|x17: 0.000
+MEAN -&gt; x1: 0.161|x2: 0.084|x3: 0.105|x4: 0.221|x5: 0.099|x6: 0.054|x7: 0.148|x8: 0.251|x9: 0.096|x10: 0.345|x11: 0.022|x12: 0.044|x13: 0.061|x14: 0.123|x15: 0.000|x16: 0.124|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.057|x3: 0.058|x4: 0.065|x5: 0.058|x6: 0.055|x7: 0.061|x8: 0.067|x9: 0.058|x10: 0.074|x11: 0.053|x12: 0.055|x13: 0.056|x14: 0.059|x15: 0.052|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -587,7 +591,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[2, 3, 9, 12]</t>
+          <t>[2, 9, 12]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -596,6 +600,7 @@
 LDA -&gt; x1: 0.000|x2: 0.390|x3: 0.102|x4: 0.138|x5: 0.000|x6: 0.190|x7: 0.155|x8: 0.000|x9: 0.433|x10: 0.000|x11: 0.000|x12: 0.068|x13: 0.111|x14: 0.059|x15: 0.068|x16: 0.105|x17: 0.000
 TOP2VEC -&gt; x1: 0.110|x2: 0.285|x3: 0.000|x4: 0.146|x5: 0.066|x6: 0.206|x7: 0.254|x8: 0.117|x9: 0.309|x10: 0.000|x11: 0.166|x12: 0.453|x13: 0.302|x14: 0.299|x15: 0.276|x16: 0.103|x17: 0.000
 MEAN -&gt; x1: 0.037|x2: 0.263|x3: 0.199|x4: 0.095|x5: 0.022|x6: 0.132|x7: 0.136|x8: 0.039|x9: 0.278|x10: 0.000|x11: 0.159|x12: 0.242|x13: 0.138|x14: 0.119|x15: 0.115|x16: 0.069|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.068|x3: 0.063|x4: 0.057|x5: 0.053|x6: 0.059|x7: 0.060|x8: 0.054|x9: 0.069|x10: 0.052|x11: 0.061|x12: 0.066|x13: 0.060|x14: 0.059|x15: 0.058|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -616,7 +621,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 13]</t>
+          <t>[3, 11]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -624,7 +629,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.549|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.318|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.128|x2: 0.156|x3: 0.253|x4: 0.183|x5: 0.077|x6: 0.000|x7: 0.070|x8: 0.128|x9: 0.108|x10: 0.000|x11: 0.196|x12: 0.000|x13: 0.268|x14: 0.067|x15: 0.082|x16: 0.103|x17: 0.000
 TOP2VEC -&gt; x1: 0.248|x2: 0.077|x3: 0.000|x4: 0.373|x5: 0.118|x6: 0.124|x7: 0.247|x8: 0.264|x9: 0.131|x10: 0.080|x11: 0.545|x12: 0.225|x13: 0.323|x14: 0.211|x15: 0.134|x16: 0.163|x17: 0.000
-MEAN -&gt; x1: 0.125|x2: 0.078|x3: 0.267|x4: 0.185|x5: 0.065|x6: 0.041|x7: 0.106|x8: 0.131|x9: 0.080|x10: 0.027|x11: 0.353|x12: 0.075|x13: 0.197|x14: 0.092|x15: 0.072|x16: 0.089|x17: 0.000
+MEAN -&gt; x1: 0.125|x2: 0.078|x3: 0.251|x4: 0.185|x5: 0.065|x6: 0.041|x7: 0.106|x8: 0.131|x9: 0.080|x10: 0.027|x11: 0.338|x12: 0.075|x13: 0.197|x14: 0.092|x15: 0.072|x16: 0.089|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.056|x3: 0.067|x4: 0.063|x5: 0.056|x6: 0.054|x7: 0.058|x8: 0.060|x9: 0.057|x10: 0.054|x11: 0.073|x12: 0.056|x13: 0.064|x14: 0.057|x15: 0.056|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -645,15 +651,16 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[2, 3, 9, 11, 13, 15]</t>
+          <t>[2, 3, 9]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.080|x3: 0.663|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.383|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.257|x3: 0.130|x4: 0.155|x5: 0.081|x6: 0.000|x7: 0.084|x8: 0.154|x9: 0.315|x10: 0.000|x11: 0.000|x12: 0.074|x13: 0.211|x14: 0.000|x15: 0.236|x16: 0.125|x17: 0.000
-TOP2VEC -&gt; x1: 0.173|x2: 0.423|x3: 0.000|x4: 0.285|x5: 0.000|x6: 0.140|x7: 0.448|x8: 0.239|x9: 0.553|x10: 0.122|x11: 0.216|x12: 0.187|x13: 0.292|x14: 0.344|x15: 0.257|x16: 0.249|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.253|x3: 0.265|x4: 0.147|x5: 0.027|x6: 0.047|x7: 0.177|x8: 0.131|x9: 0.289|x10: 0.041|x11: 0.200|x12: 0.087|x13: 0.168|x14: 0.115|x15: 0.164|x16: 0.125|x17: 0.000
+TOP2VEC -&gt; x1: 0.173|x2: 0.423|x3: 0.000|x4: 0.285|x5: 0.000|x6: 0.141|x7: 0.448|x8: 0.239|x9: 0.553|x10: 0.122|x11: 0.216|x12: 0.187|x13: 0.292|x14: 0.344|x15: 0.257|x16: 0.249|x17: 0.000
+MEAN -&gt; x1: 0.058|x2: 0.253|x3: 0.210|x4: 0.147|x5: 0.027|x6: 0.047|x7: 0.177|x8: 0.131|x9: 0.272|x10: 0.041|x11: 0.200|x12: 0.087|x13: 0.168|x14: 0.115|x15: 0.164|x16: 0.125|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.066|x3: 0.064|x4: 0.060|x5: 0.053|x6: 0.054|x7: 0.061|x8: 0.059|x9: 0.068|x10: 0.054|x11: 0.063|x12: 0.056|x13: 0.061|x14: 0.058|x15: 0.061|x16: 0.058|x17: 0.051
 </t>
         </is>
       </c>
@@ -674,7 +681,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[3, 4, 13, 14]</t>
+          <t>[3, 13]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -682,7 +689,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.095|x2: 0.000|x3: 0.543|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.314|x12: 0.000|x13: 0.542|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.174|x2: 0.311|x3: 0.182|x4: 0.225|x5: 0.112|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.127|x13: 0.116|x14: 0.217|x15: 0.130|x16: 0.224|x17: 0.000
 TOP2VEC -&gt; x1: 0.193|x2: 0.117|x3: 0.000|x4: 0.227|x5: 0.224|x6: 0.081|x7: 0.151|x8: 0.194|x9: 0.184|x10: 0.061|x11: 0.135|x12: 0.217|x13: 0.351|x14: 0.356|x15: 0.121|x16: 0.125|x17: 0.000
-MEAN -&gt; x1: 0.154|x2: 0.143|x3: 0.242|x4: 0.151|x5: 0.112|x6: 0.027|x7: 0.050|x8: 0.065|x9: 0.061|x10: 0.020|x11: 0.150|x12: 0.115|x13: 0.336|x14: 0.191|x15: 0.084|x16: 0.116|x17: 0.000
+MEAN -&gt; x1: 0.154|x2: 0.143|x3: 0.227|x4: 0.151|x5: 0.112|x6: 0.027|x7: 0.050|x8: 0.065|x9: 0.061|x10: 0.020|x11: 0.150|x12: 0.115|x13: 0.322|x14: 0.191|x15: 0.084|x16: 0.116|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.060|x3: 0.065|x4: 0.061|x5: 0.058|x6: 0.054|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.053|x11: 0.061|x12: 0.059|x13: 0.072|x14: 0.063|x15: 0.057|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -703,15 +711,16 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 9, 11, 13]</t>
+          <t>[3, 9, 11, 13]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.510|x4: 0.000|x5: 0.000|x6: 0.113|x7: 0.000|x8: 0.067|x9: 0.000|x10: 0.000|x11: 0.295|x12: 0.000|x13: 0.302|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.146|x2: 0.124|x3: 0.180|x4: 0.259|x5: 0.000|x6: 0.000|x7: 0.105|x8: 0.131|x9: 0.217|x10: 0.159|x11: 0.061|x12: 0.000|x13: 0.200|x14: 0.108|x15: 0.130|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.189|x2: 0.154|x3: 0.000|x4: 0.276|x5: 0.084|x6: 0.291|x7: 0.445|x8: 0.236|x9: 0.406|x10: 0.000|x11: 0.245|x12: 0.129|x13: 0.298|x14: 0.182|x15: 0.112|x16: 0.072|x17: 0.000
-MEAN -&gt; x1: 0.111|x2: 0.093|x3: 0.230|x4: 0.178|x5: 0.028|x6: 0.135|x7: 0.184|x8: 0.145|x9: 0.208|x10: 0.053|x11: 0.200|x12: 0.043|x13: 0.266|x14: 0.097|x15: 0.081|x16: 0.024|x17: 0.000
+TOP2VEC -&gt; x1: 0.189|x2: 0.154|x3: 0.000|x4: 0.276|x5: 0.084|x6: 0.291|x7: 0.446|x8: 0.236|x9: 0.406|x10: 0.000|x11: 0.245|x12: 0.129|x13: 0.298|x14: 0.182|x15: 0.112|x16: 0.072|x17: 0.000
+MEAN -&gt; x1: 0.111|x2: 0.093|x3: 0.227|x4: 0.178|x5: 0.028|x6: 0.135|x7: 0.184|x8: 0.145|x9: 0.208|x10: 0.053|x11: 0.200|x12: 0.043|x13: 0.266|x14: 0.097|x15: 0.081|x16: 0.024|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.057|x3: 0.065|x4: 0.062|x5: 0.053|x6: 0.059|x7: 0.062|x8: 0.060|x9: 0.064|x10: 0.055|x11: 0.063|x12: 0.054|x13: 0.068|x14: 0.057|x15: 0.056|x16: 0.053|x17: 0.052
 </t>
         </is>
       </c>
@@ -732,15 +741,16 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[2, 3, 11]</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.175|x3: 0.446|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.258|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.068|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.077|x2: 0.462|x3: 0.000|x4: 0.315|x5: 0.105|x6: 0.000|x7: 0.000|x8: 0.075|x9: 0.152|x10: 0.216|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.086|x15: 0.195|x16: 0.071|x17: 0.000
-TOP2VEC -&gt; x1: 0.254|x2: 0.239|x3: 0.137|x4: 0.151|x5: 0.225|x6: 0.000|x7: 0.371|x8: 0.294|x9: 0.131|x10: 0.100|x11: 0.270|x12: 0.245|x13: 0.236|x14: 0.189|x15: 0.207|x16: 0.205|x17: 0.000
+TOP2VEC -&gt; x1: 0.254|x2: 0.239|x3: 0.137|x4: 0.151|x5: 0.225|x6: 0.000|x7: 0.371|x8: 0.294|x9: 0.131|x10: 0.100|x11: 0.269|x12: 0.245|x13: 0.236|x14: 0.189|x15: 0.207|x16: 0.205|x17: 0.000
 MEAN -&gt; x1: 0.110|x2: 0.292|x3: 0.194|x4: 0.155|x5: 0.110|x6: 0.000|x7: 0.124|x8: 0.123|x9: 0.094|x10: 0.106|x11: 0.198|x12: 0.082|x13: 0.079|x14: 0.092|x15: 0.157|x16: 0.092|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.070|x3: 0.063|x4: 0.061|x5: 0.058|x6: 0.052|x7: 0.059|x8: 0.059|x9: 0.057|x10: 0.058|x11: 0.064|x12: 0.057|x13: 0.056|x14: 0.057|x15: 0.061|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -761,7 +771,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[2, 3, 11, 14]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -769,7 +779,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.621|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.359|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.118|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.269|x3: 0.000|x4: 0.234|x5: 0.068|x6: 0.123|x7: 0.085|x8: 0.000|x9: 0.094|x10: 0.071|x11: 0.060|x12: 0.159|x13: 0.000|x14: 0.232|x15: 0.188|x16: 0.238|x17: 0.000
 TOP2VEC -&gt; x1: 0.170|x2: 0.302|x3: 0.000|x4: 0.170|x5: 0.197|x6: 0.166|x7: 0.364|x8: 0.213|x9: 0.178|x10: 0.066|x11: 0.146|x12: 0.291|x13: 0.148|x14: 0.207|x15: 0.089|x16: 0.134|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.190|x3: 0.207|x4: 0.135|x5: 0.088|x6: 0.096|x7: 0.150|x8: 0.071|x9: 0.091|x10: 0.045|x11: 0.188|x12: 0.150|x13: 0.049|x14: 0.146|x15: 0.132|x16: 0.124|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.190|x3: 0.167|x4: 0.135|x5: 0.088|x6: 0.096|x7: 0.150|x8: 0.071|x9: 0.091|x10: 0.045|x11: 0.188|x12: 0.150|x13: 0.049|x14: 0.146|x15: 0.132|x16: 0.124|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.064|x3: 0.062|x4: 0.060|x5: 0.057|x6: 0.058|x7: 0.061|x8: 0.056|x9: 0.058|x10: 0.055|x11: 0.063|x12: 0.061|x13: 0.055|x14: 0.061|x15: 0.060|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -790,15 +801,16 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[2, 13, 14, 15]</t>
+          <t>[2, 14, 15]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.206|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.230|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.197|x3: 0.153|x4: 0.109|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.106|x13: 0.221|x14: 0.235|x15: 0.618|x16: 0.181|x17: 0.000
-TOP2VEC -&gt; x1: 0.117|x2: 0.407|x3: 0.220|x4: 0.268|x5: 0.075|x6: 0.000|x7: 0.220|x8: 0.120|x9: 0.179|x10: 0.000|x11: 0.192|x12: 0.000|x13: 0.246|x14: 0.395|x15: 0.257|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.039|x2: 0.270|x3: 0.124|x4: 0.126|x5: 0.025|x6: 0.000|x7: 0.073|x8: 0.040|x9: 0.060|x10: 0.000|x11: 0.064|x12: 0.112|x13: 0.156|x14: 0.210|x15: 0.292|x16: 0.060|x17: 0.000
+TOP2VEC -&gt; x1: 0.117|x2: 0.406|x3: 0.220|x4: 0.268|x5: 0.075|x6: 0.000|x7: 0.220|x8: 0.119|x9: 0.179|x10: 0.000|x11: 0.192|x12: 0.000|x13: 0.246|x14: 0.395|x15: 0.257|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.039|x2: 0.270|x3: 0.124|x4: 0.126|x5: 0.025|x6: 0.000|x7: 0.073|x8: 0.040|x9: 0.060|x10: 0.000|x11: 0.064|x12: 0.112|x13: 0.156|x14: 0.210|x15: 0.252|x16: 0.060|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.070|x3: 0.060|x4: 0.060|x5: 0.055|x6: 0.053|x7: 0.057|x8: 0.055|x9: 0.057|x10: 0.053|x11: 0.057|x12: 0.060|x13: 0.062|x14: 0.066|x15: 0.069|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -819,15 +831,16 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[3, 4, 9, 11, 15]</t>
+          <t>[3, 4, 11]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.768|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.156|x3: 0.229|x4: 0.418|x5: 0.053|x6: 0.000|x7: 0.000|x8: 0.173|x9: 0.114|x10: 0.000|x11: 0.138|x12: 0.000|x13: 0.000|x14: 0.259|x15: 0.279|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.195|x2: 0.075|x3: 0.258|x4: 0.505|x5: 0.185|x6: 0.413|x7: 0.568|x8: 0.282|x9: 0.440|x10: 0.088|x11: 0.482|x12: 0.000|x13: 0.171|x14: 0.189|x15: 0.249|x16: 0.181|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.077|x3: 0.418|x4: 0.308|x5: 0.079|x6: 0.138|x7: 0.189|x8: 0.152|x9: 0.185|x10: 0.029|x11: 0.311|x12: 0.000|x13: 0.057|x14: 0.149|x15: 0.176|x16: 0.060|x17: 0.000
+TOP2VEC -&gt; x1: 0.195|x2: 0.075|x3: 0.258|x4: 0.505|x5: 0.185|x6: 0.413|x7: 0.568|x8: 0.282|x9: 0.440|x10: 0.089|x11: 0.482|x12: 0.000|x13: 0.171|x14: 0.189|x15: 0.249|x16: 0.181|x17: 0.000
+MEAN -&gt; x1: 0.065|x2: 0.077|x3: 0.329|x4: 0.306|x5: 0.079|x6: 0.138|x7: 0.167|x8: 0.152|x9: 0.185|x10: 0.030|x11: 0.311|x12: 0.000|x13: 0.057|x14: 0.149|x15: 0.176|x16: 0.060|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.071|x4: 0.069|x5: 0.055|x6: 0.059|x7: 0.060|x8: 0.060|x9: 0.062|x10: 0.053|x11: 0.070|x12: 0.051|x13: 0.054|x14: 0.059|x15: 0.061|x16: 0.054|x17: 0.051
 </t>
         </is>
       </c>
@@ -856,7 +869,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.539|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.060|x2: 0.170|x3: 0.191|x4: 0.171|x5: 0.000|x6: 0.000|x7: 0.434|x8: 0.000|x9: 0.290|x10: 0.155|x11: 0.000|x12: 0.093|x13: 0.077|x14: 0.000|x15: 0.064|x16: 0.117|x17: 0.000
 TOP2VEC -&gt; x1: 0.130|x2: 0.219|x3: 0.356|x4: 0.167|x5: 0.000|x6: 0.126|x7: 0.242|x8: 0.178|x9: 0.137|x10: 0.098|x11: 0.073|x12: 0.336|x13: 0.053|x14: 0.062|x15: 0.251|x16: 0.200|x17: 0.000
-MEAN -&gt; x1: 0.063|x2: 0.130|x3: 0.362|x4: 0.113|x5: 0.000|x6: 0.042|x7: 0.225|x8: 0.059|x9: 0.142|x10: 0.084|x11: 0.124|x12: 0.143|x13: 0.043|x14: 0.021|x15: 0.105|x16: 0.106|x17: 0.000
+MEAN -&gt; x1: 0.063|x2: 0.130|x3: 0.349|x4: 0.112|x5: 0.000|x6: 0.042|x7: 0.225|x8: 0.059|x9: 0.142|x10: 0.084|x11: 0.124|x12: 0.143|x13: 0.043|x14: 0.021|x15: 0.105|x16: 0.106|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.075|x4: 0.059|x5: 0.053|x6: 0.055|x7: 0.066|x8: 0.056|x9: 0.061|x10: 0.058|x11: 0.060|x12: 0.061|x13: 0.055|x14: 0.054|x15: 0.059|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -877,7 +891,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[3, 5, 13]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -885,7 +899,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.873|x4: 0.000|x5: 0.095|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.056|x2: 0.075|x3: 0.463|x4: 0.000|x5: 0.244|x6: 0.000|x7: 0.000|x8: 0.119|x9: 0.132|x10: 0.109|x11: 0.000|x12: 0.000|x13: 0.274|x14: 0.153|x15: 0.121|x16: 0.074|x17: 0.000
 TOP2VEC -&gt; x1: 0.104|x2: 0.087|x3: 0.326|x4: 0.000|x5: 0.230|x6: 0.136|x7: 0.219|x8: 0.079|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.093|x13: 0.228|x14: 0.164|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.054|x3: 0.554|x4: 0.000|x5: 0.190|x6: 0.045|x7: 0.073|x8: 0.066|x9: 0.044|x10: 0.036|x11: 0.104|x12: 0.031|x13: 0.167|x14: 0.106|x15: 0.040|x16: 0.025|x17: 0.000
+MEAN -&gt; x1: 0.053|x2: 0.054|x3: 0.429|x4: 0.000|x5: 0.190|x6: 0.045|x7: 0.073|x8: 0.066|x9: 0.044|x10: 0.036|x11: 0.104|x12: 0.031|x13: 0.167|x14: 0.106|x15: 0.040|x16: 0.025|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.057|x3: 0.082|x4: 0.054|x5: 0.065|x6: 0.056|x7: 0.058|x8: 0.057|x9: 0.056|x10: 0.056|x11: 0.060|x12: 0.055|x13: 0.063|x14: 0.060|x15: 0.056|x16: 0.055|x17: 0.054
 </t>
         </is>
       </c>
@@ -906,15 +921,16 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 16]</t>
+          <t>[3, 4, 11]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.688|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.398|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.100|x2: 0.207|x3: 0.163|x4: 0.318|x5: 0.000|x6: 0.000|x7: 0.053|x8: 0.132|x9: 0.195|x10: 0.000|x11: 0.090|x12: 0.124|x13: 0.107|x14: 0.000|x15: 0.109|x16: 0.221|x17: 0.000
-TOP2VEC -&gt; x1: 0.214|x2: 0.000|x3: 0.262|x4: 0.515|x5: 0.485|x6: 0.321|x7: 0.500|x8: 0.321|x9: 0.348|x10: 0.170|x11: 0.178|x12: 0.179|x13: 0.054|x14: 0.356|x15: 0.183|x16: 0.348|x17: 0.000
-MEAN -&gt; x1: 0.105|x2: 0.069|x3: 0.371|x4: 0.278|x5: 0.162|x6: 0.107|x7: 0.184|x8: 0.151|x9: 0.181|x10: 0.057|x11: 0.222|x12: 0.101|x13: 0.054|x14: 0.119|x15: 0.098|x16: 0.189|x17: 0.000
+TOP2VEC -&gt; x1: 0.214|x2: 0.000|x3: 0.262|x4: 0.516|x5: 0.485|x6: 0.321|x7: 0.500|x8: 0.321|x9: 0.348|x10: 0.170|x11: 0.178|x12: 0.179|x13: 0.054|x14: 0.356|x15: 0.184|x16: 0.348|x17: 0.000
+MEAN -&gt; x1: 0.105|x2: 0.069|x3: 0.308|x4: 0.273|x5: 0.162|x6: 0.107|x7: 0.184|x8: 0.151|x9: 0.181|x10: 0.057|x11: 0.222|x12: 0.101|x13: 0.054|x14: 0.119|x15: 0.098|x16: 0.189|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.069|x4: 0.067|x5: 0.060|x6: 0.057|x7: 0.061|x8: 0.059|x9: 0.061|x10: 0.054|x11: 0.064|x12: 0.056|x13: 0.054|x14: 0.057|x15: 0.056|x16: 0.062|x17: 0.051
 </t>
         </is>
       </c>
@@ -935,7 +951,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[14, 16]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -944,6 +960,7 @@
 LDA -&gt; x1: 0.000|x2: 0.164|x3: 0.099|x4: 0.112|x5: 0.066|x6: 0.000|x7: 0.123|x8: 0.163|x9: 0.081|x10: 0.000|x11: 0.060|x12: 0.145|x13: 0.130|x14: 0.253|x15: 0.191|x16: 0.232|x17: 0.000
 TOP2VEC -&gt; x1: 0.100|x2: 0.210|x3: 0.000|x4: 0.344|x5: 0.143|x6: 0.056|x7: 0.179|x8: 0.085|x9: 0.089|x10: 0.105|x11: 0.123|x12: 0.280|x13: 0.238|x14: 0.238|x15: 0.136|x16: 0.216|x17: 0.000
 MEAN -&gt; x1: 0.033|x2: 0.125|x3: 0.137|x4: 0.152|x5: 0.070|x6: 0.019|x7: 0.153|x8: 0.109|x9: 0.057|x10: 0.035|x11: 0.121|x12: 0.142|x13: 0.151|x14: 0.164|x15: 0.109|x16: 0.149|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.061|x4: 0.062|x5: 0.057|x6: 0.054|x7: 0.062|x8: 0.059|x9: 0.056|x10: 0.055|x11: 0.060|x12: 0.061|x13: 0.062|x14: 0.063|x15: 0.059|x16: 0.062|x17: 0.053
 </t>
         </is>
       </c>
@@ -964,7 +981,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 13]</t>
+          <t>[3, 9]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -973,6 +990,7 @@
 LDA -&gt; x1: 0.000|x2: 0.067|x3: 0.231|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.226|x8: 0.082|x9: 0.346|x10: 0.111|x11: 0.000|x12: 0.082|x13: 0.214|x14: 0.076|x15: 0.245|x16: 0.140|x17: 0.000
 TOP2VEC -&gt; x1: 0.149|x2: 0.052|x3: 0.252|x4: 0.312|x5: 0.056|x6: 0.000|x7: 0.074|x8: 0.175|x9: 0.402|x10: 0.000|x11: 0.270|x12: 0.301|x13: 0.336|x14: 0.233|x15: 0.148|x16: 0.101|x17: 0.000
 MEAN -&gt; x1: 0.050|x2: 0.040|x3: 0.297|x4: 0.104|x5: 0.019|x6: 0.000|x7: 0.100|x8: 0.086|x9: 0.270|x10: 0.037|x11: 0.169|x12: 0.128|x13: 0.183|x14: 0.103|x15: 0.131|x16: 0.080|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.071|x4: 0.059|x5: 0.054|x6: 0.053|x7: 0.058|x8: 0.057|x9: 0.069|x10: 0.055|x11: 0.062|x12: 0.060|x13: 0.063|x14: 0.058|x15: 0.060|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -1000,8 +1018,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.635|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.417|x12: 0.090|x13: 0.000|x14: 0.132|x15: 0.099|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.058|x3: 0.362|x4: 0.170|x5: 0.000|x6: 0.000|x7: 0.139|x8: 0.000|x9: 0.183|x10: 0.000|x11: 0.148|x12: 0.079|x13: 0.218|x14: 0.356|x15: 0.000|x16: 0.107|x17: 0.000
-TOP2VEC -&gt; x1: 0.151|x2: 0.198|x3: 0.000|x4: 0.151|x5: 0.126|x6: 0.332|x7: 0.260|x8: 0.101|x9: 0.193|x10: 0.000|x11: 0.322|x12: 0.494|x13: 0.508|x14: 0.401|x15: 0.398|x16: 0.088|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.085|x3: 0.332|x4: 0.107|x5: 0.042|x6: 0.111|x7: 0.133|x8: 0.034|x9: 0.125|x10: 0.000|x11: 0.296|x12: 0.221|x13: 0.242|x14: 0.296|x15: 0.166|x16: 0.065|x17: 0.000
+TOP2VEC -&gt; x1: 0.151|x2: 0.197|x3: 0.000|x4: 0.151|x5: 0.126|x6: 0.332|x7: 0.260|x8: 0.101|x9: 0.193|x10: 0.000|x11: 0.322|x12: 0.494|x13: 0.508|x14: 0.401|x15: 0.398|x16: 0.088|x17: 0.000
+MEAN -&gt; x1: 0.050|x2: 0.085|x3: 0.287|x4: 0.107|x5: 0.042|x6: 0.111|x7: 0.133|x8: 0.034|x9: 0.125|x10: 0.000|x11: 0.295|x12: 0.221|x13: 0.239|x14: 0.296|x15: 0.166|x16: 0.065|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.068|x4: 0.057|x5: 0.053|x6: 0.057|x7: 0.059|x8: 0.053|x9: 0.058|x10: 0.051|x11: 0.069|x12: 0.064|x13: 0.065|x14: 0.069|x15: 0.060|x16: 0.055|x17: 0.051
 </t>
         </is>
       </c>
@@ -1022,7 +1041,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[3, 5, 11, 13]</t>
+          <t>[3, 13]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1031,6 +1050,7 @@
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.318|x4: 0.000|x5: 0.255|x6: 0.000|x7: 0.059|x8: 0.144|x9: 0.000|x10: 0.140|x11: 0.000|x12: 0.079|x13: 0.174|x14: 0.255|x15: 0.206|x16: 0.190|x17: 0.000
 TOP2VEC -&gt; x1: 0.201|x2: 0.000|x3: 0.460|x4: 0.316|x5: 0.307|x6: 0.000|x7: 0.202|x8: 0.153|x9: 0.000|x10: 0.106|x11: 0.208|x12: 0.110|x13: 0.442|x14: 0.193|x15: 0.187|x16: 0.217|x17: 0.000
 MEAN -&gt; x1: 0.067|x2: 0.000|x3: 0.418|x4: 0.105|x5: 0.187|x6: 0.000|x7: 0.087|x8: 0.099|x9: 0.000|x10: 0.082|x11: 0.161|x12: 0.063|x13: 0.205|x14: 0.149|x15: 0.131|x16: 0.136|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.052|x3: 0.080|x4: 0.058|x5: 0.063|x6: 0.052|x7: 0.057|x8: 0.058|x9: 0.052|x10: 0.057|x11: 0.062|x12: 0.056|x13: 0.064|x14: 0.061|x15: 0.060|x16: 0.060|x17: 0.052
 </t>
         </is>
       </c>
@@ -1051,7 +1071,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[3, 4, 16]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1060,6 +1080,7 @@
 LDA -&gt; x1: 0.389|x2: 0.165|x3: 0.301|x4: 0.432|x5: 0.000|x6: 0.000|x7: 0.130|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.111|x13: 0.000|x14: 0.000|x15: 0.104|x16: 0.188|x17: 0.000
 TOP2VEC -&gt; x1: 0.088|x2: 0.089|x3: 0.158|x4: 0.480|x5: 0.220|x6: 0.169|x7: 0.161|x8: 0.089|x9: 0.355|x10: 0.198|x11: 0.235|x12: 0.207|x13: 0.326|x14: 0.235|x15: 0.136|x16: 0.405|x17: 0.000
 MEAN -&gt; x1: 0.159|x2: 0.085|x3: 0.254|x4: 0.304|x5: 0.073|x6: 0.056|x7: 0.097|x8: 0.030|x9: 0.118|x10: 0.066|x11: 0.133|x12: 0.106|x13: 0.109|x14: 0.078|x15: 0.080|x16: 0.198|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.057|x3: 0.067|x4: 0.071|x5: 0.056|x6: 0.055|x7: 0.058|x8: 0.054|x9: 0.059|x10: 0.056|x11: 0.060|x12: 0.058|x13: 0.058|x14: 0.057|x15: 0.057|x16: 0.064|x17: 0.052
 </t>
         </is>
       </c>
@@ -1080,7 +1101,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[3, 4, 14]</t>
+          <t>[3, 14]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1088,7 +1109,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.274|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.083|x9: 0.000|x10: 0.000|x11: 0.144|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.108|x3: 0.248|x4: 0.218|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.072|x9: 0.080|x10: 0.140|x11: 0.000|x12: 0.000|x13: 0.070|x14: 0.543|x15: 0.000|x16: 0.091|x17: 0.000
 TOP2VEC -&gt; x1: 0.151|x2: 0.340|x3: 0.316|x4: 0.245|x5: 0.224|x6: 0.125|x7: 0.086|x8: 0.156|x9: 0.000|x10: 0.147|x11: 0.240|x12: 0.000|x13: 0.167|x14: 0.353|x15: 0.203|x16: 0.302|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.149|x3: 0.279|x4: 0.154|x5: 0.122|x6: 0.042|x7: 0.065|x8: 0.104|x9: 0.027|x10: 0.096|x11: 0.128|x12: 0.000|x13: 0.079|x14: 0.299|x15: 0.068|x16: 0.131|x17: 0.000
+MEAN -&gt; x1: 0.050|x2: 0.149|x3: 0.279|x4: 0.154|x5: 0.122|x6: 0.042|x7: 0.065|x8: 0.104|x9: 0.027|x10: 0.096|x11: 0.128|x12: 0.000|x13: 0.079|x14: 0.284|x15: 0.068|x16: 0.131|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.070|x4: 0.062|x5: 0.060|x6: 0.055|x7: 0.056|x8: 0.059|x9: 0.054|x10: 0.058|x11: 0.060|x12: 0.053|x13: 0.057|x14: 0.070|x15: 0.057|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -1117,7 +1139,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.504|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.094|x11: 0.309|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.094|x3: 0.173|x4: 0.181|x5: 0.000|x6: 0.000|x7: 0.197|x8: 0.059|x9: 0.345|x10: 0.137|x11: 0.116|x12: 0.000|x13: 0.193|x14: 0.092|x15: 0.232|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.155|x2: 0.327|x3: 0.000|x4: 0.211|x5: 0.294|x6: 0.192|x7: 0.183|x8: 0.193|x9: 0.299|x10: 0.101|x11: 0.175|x12: 0.244|x13: 0.227|x14: 0.399|x15: 0.178|x16: 0.207|x17: 0.000
-MEAN -&gt; x1: 0.052|x2: 0.141|x3: 0.226|x4: 0.131|x5: 0.098|x6: 0.064|x7: 0.127|x8: 0.084|x9: 0.215|x10: 0.111|x11: 0.200|x12: 0.081|x13: 0.140|x14: 0.164|x15: 0.137|x16: 0.069|x17: 0.000
+MEAN -&gt; x1: 0.052|x2: 0.141|x3: 0.224|x4: 0.131|x5: 0.098|x6: 0.064|x7: 0.127|x8: 0.084|x9: 0.215|x10: 0.111|x11: 0.200|x12: 0.081|x13: 0.140|x14: 0.164|x15: 0.137|x16: 0.069|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.065|x4: 0.059|x5: 0.057|x6: 0.056|x7: 0.059|x8: 0.057|x9: 0.065|x10: 0.058|x11: 0.064|x12: 0.056|x13: 0.060|x14: 0.061|x15: 0.060|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -1138,15 +1161,16 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[3, 4, 8, 9, 11, 14]</t>
+          <t>[3, 8, 14]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.381|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.063|x10: 0.000|x11: 0.227|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.078|x2: 0.062|x3: 0.157|x4: 0.161|x5: 0.075|x6: 0.000|x7: 0.140|x8: 0.392|x9: 0.241|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.418|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.175|x2: 0.351|x3: 0.492|x4: 0.370|x5: 0.202|x6: 0.383|x7: 0.164|x8: 0.261|x9: 0.208|x10: 0.076|x11: 0.243|x12: 0.000|x13: 0.000|x14: 0.188|x15: 0.000|x16: 0.156|x17: 0.000
+TOP2VEC -&gt; x1: 0.175|x2: 0.351|x3: 0.492|x4: 0.370|x5: 0.202|x6: 0.384|x7: 0.164|x8: 0.261|x9: 0.208|x10: 0.076|x11: 0.243|x12: 0.000|x13: 0.000|x14: 0.188|x15: 0.000|x16: 0.156|x17: 0.000
 MEAN -&gt; x1: 0.084|x2: 0.138|x3: 0.343|x4: 0.177|x5: 0.092|x6: 0.128|x7: 0.101|x8: 0.218|x9: 0.171|x10: 0.057|x11: 0.157|x12: 0.000|x13: 0.000|x14: 0.202|x15: 0.000|x16: 0.052|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.074|x4: 0.062|x5: 0.057|x6: 0.059|x7: 0.058|x8: 0.065|x9: 0.062|x10: 0.055|x11: 0.061|x12: 0.052|x13: 0.052|x14: 0.064|x15: 0.052|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -1167,7 +1191,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[2, 3, 6, 7, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1175,7 +1199,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.539|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.138|x9: 0.000|x10: 0.000|x11: 0.294|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.107|x2: 0.269|x3: 0.155|x4: 0.093|x5: 0.085|x6: 0.237|x7: 0.124|x8: 0.145|x9: 0.166|x10: 0.139|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.107|x15: 0.088|x16: 0.105|x17: 0.000
 TOP2VEC -&gt; x1: 0.122|x2: 0.231|x3: 0.181|x4: 0.084|x5: 0.222|x6: 0.293|x7: 0.424|x8: 0.192|x9: 0.208|x10: 0.078|x11: 0.216|x12: 0.194|x13: 0.000|x14: 0.294|x15: 0.085|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.076|x2: 0.167|x3: 0.292|x4: 0.059|x5: 0.102|x6: 0.177|x7: 0.183|x8: 0.158|x9: 0.124|x10: 0.072|x11: 0.170|x12: 0.065|x13: 0.000|x14: 0.134|x15: 0.058|x16: 0.088|x17: 0.000
+MEAN -&gt; x1: 0.076|x2: 0.167|x3: 0.279|x4: 0.059|x5: 0.102|x6: 0.177|x7: 0.183|x8: 0.158|x9: 0.124|x10: 0.072|x11: 0.170|x12: 0.065|x13: 0.000|x14: 0.134|x15: 0.058|x16: 0.088|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.062|x3: 0.069|x4: 0.056|x5: 0.058|x6: 0.063|x7: 0.063|x8: 0.061|x9: 0.059|x10: 0.056|x11: 0.062|x12: 0.056|x13: 0.052|x14: 0.060|x15: 0.056|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -1196,7 +1221,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[2, 4, 5, 7, 9, 12]</t>
+          <t>[4, 7, 9]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1204,7 +1229,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.461|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.151|x9: 0.000|x10: 0.000|x11: 0.267|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.370|x3: 0.061|x4: 0.436|x5: 0.223|x6: 0.000|x7: 0.101|x8: 0.000|x9: 0.377|x10: 0.000|x11: 0.000|x12: 0.075|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
 TOP2VEC -&gt; x1: 0.171|x2: 0.182|x3: 0.000|x4: 0.244|x5: 0.286|x6: 0.324|x7: 0.742|x8: 0.236|x9: 0.465|x10: 0.066|x11: 0.157|x12: 0.580|x13: 0.244|x14: 0.191|x15: 0.205|x16: 0.136|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.184|x3: 0.174|x4: 0.227|x5: 0.170|x6: 0.108|x7: 0.281|x8: 0.129|x9: 0.281|x10: 0.022|x11: 0.141|x12: 0.218|x13: 0.081|x14: 0.064|x15: 0.068|x16: 0.104|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.184|x3: 0.174|x4: 0.227|x5: 0.170|x6: 0.108|x7: 0.200|x8: 0.129|x9: 0.281|x10: 0.022|x11: 0.141|x12: 0.192|x13: 0.081|x14: 0.064|x15: 0.068|x16: 0.104|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.061|x4: 0.065|x5: 0.061|x6: 0.057|x7: 0.063|x8: 0.059|x9: 0.068|x10: 0.053|x11: 0.059|x12: 0.062|x13: 0.056|x14: 0.055|x15: 0.055|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -1233,7 +1259,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.714|x4: 0.000|x5: 0.138|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.419|x3: 0.258|x4: 0.000|x5: 0.156|x6: 0.000|x7: 0.071|x8: 0.204|x9: 0.265|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.193|x14: 0.147|x15: 0.106|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.120|x2: 0.327|x3: 0.000|x4: 0.236|x5: 0.083|x6: 0.083|x7: 0.230|x8: 0.121|x9: 0.070|x10: 0.000|x11: 0.127|x12: 0.260|x13: 0.189|x14: 0.000|x15: 0.000|x16: 0.089|x17: 0.000
-MEAN -&gt; x1: 0.040|x2: 0.249|x3: 0.324|x4: 0.079|x5: 0.126|x6: 0.028|x7: 0.100|x8: 0.108|x9: 0.112|x10: 0.000|x11: 0.142|x12: 0.087|x13: 0.127|x14: 0.049|x15: 0.035|x16: 0.030|x17: 0.000
+MEAN -&gt; x1: 0.040|x2: 0.249|x3: 0.253|x4: 0.079|x5: 0.126|x6: 0.028|x7: 0.100|x8: 0.108|x9: 0.112|x10: 0.000|x11: 0.142|x12: 0.087|x13: 0.127|x14: 0.049|x15: 0.035|x16: 0.030|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.069|x3: 0.069|x4: 0.058|x5: 0.061|x6: 0.055|x7: 0.059|x8: 0.060|x9: 0.060|x10: 0.054|x11: 0.062|x12: 0.058|x13: 0.061|x14: 0.056|x15: 0.055|x16: 0.055|x17: 0.054
 </t>
         </is>
       </c>
@@ -1261,8 +1288,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.992|x4: 0.000|x5: 0.154|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.200|x12: 0.000|x13: 0.060|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.103|x3: 0.813|x4: 0.120|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.062|x11: 0.000|x12: 0.000|x13: 0.330|x14: 0.000|x15: 0.112|x16: 0.115|x17: 0.000
-TOP2VEC -&gt; x1: 0.146|x2: 0.000|x3: 0.504|x4: 0.000|x5: 0.260|x6: 0.000|x7: 0.000|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.154|x13: 0.138|x14: 0.000|x15: 0.117|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.049|x2: 0.034|x3: 0.770|x4: 0.040|x5: 0.193|x6: 0.000|x7: 0.000|x8: 0.052|x9: 0.000|x10: 0.021|x11: 0.067|x12: 0.051|x13: 0.176|x14: 0.000|x15: 0.076|x16: 0.038|x17: 0.000
+TOP2VEC -&gt; x1: 0.145|x2: 0.000|x3: 0.504|x4: 0.000|x5: 0.260|x6: 0.000|x7: 0.000|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.154|x13: 0.138|x14: 0.000|x15: 0.117|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.048|x2: 0.034|x3: 0.500|x4: 0.040|x5: 0.193|x6: 0.000|x7: 0.000|x8: 0.052|x9: 0.000|x10: 0.021|x11: 0.067|x12: 0.051|x13: 0.176|x14: 0.000|x15: 0.076|x16: 0.038|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.089|x4: 0.056|x5: 0.066|x6: 0.054|x7: 0.054|x8: 0.057|x9: 0.054|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.064|x14: 0.054|x15: 0.058|x16: 0.056|x17: 0.054
 </t>
         </is>
       </c>
@@ -1290,8 +1318,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.205|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.057|x10: 0.000|x11: 0.098|x12: 0.000|x13: 0.000|x14: 0.064|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.058|x2: 0.164|x3: 0.061|x4: 0.000|x5: 0.085|x6: 0.000|x7: 0.269|x8: 0.063|x9: 0.461|x10: 0.336|x11: 0.000|x12: 0.000|x13: 0.118|x14: 0.000|x15: 0.125|x16: 0.080|x17: 0.000
-TOP2VEC -&gt; x1: 0.114|x2: 0.000|x3: 0.179|x4: 0.000|x5: 0.289|x6: 0.228|x7: 0.119|x8: 0.157|x9: 0.228|x10: 0.160|x11: 0.219|x12: 0.309|x13: 0.111|x14: 0.071|x15: 0.240|x16: 0.327|x17: 0.000
+TOP2VEC -&gt; x1: 0.114|x2: 0.000|x3: 0.179|x4: 0.000|x5: 0.289|x6: 0.229|x7: 0.119|x8: 0.157|x9: 0.228|x10: 0.160|x11: 0.219|x12: 0.309|x13: 0.111|x14: 0.071|x15: 0.241|x16: 0.327|x17: 0.000
 MEAN -&gt; x1: 0.057|x2: 0.055|x3: 0.149|x4: 0.000|x5: 0.125|x6: 0.076|x7: 0.129|x8: 0.073|x9: 0.249|x10: 0.165|x11: 0.106|x12: 0.103|x13: 0.076|x14: 0.045|x15: 0.122|x16: 0.136|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.056|x3: 0.062|x4: 0.053|x5: 0.060|x6: 0.057|x7: 0.061|x8: 0.057|x9: 0.068|x10: 0.063|x11: 0.059|x12: 0.059|x13: 0.057|x14: 0.056|x15: 0.060|x16: 0.061|x17: 0.053
 </t>
         </is>
       </c>
@@ -1312,15 +1341,16 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[2, 3, 7, 12, 13, 15]</t>
+          <t>[2, 3, 7, 15]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.531|x4: 0.084|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.321|x3: 0.140|x4: 0.174|x5: 0.086|x6: 0.120|x7: 0.149|x8: 0.000|x9: 0.055|x10: 0.150|x11: 0.000|x12: 0.070|x13: 0.198|x14: 0.000|x15: 0.257|x16: 0.101|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.292|x3: 0.000|x4: 0.125|x5: 0.165|x6: 0.266|x7: 0.496|x8: 0.121|x9: 0.203|x10: 0.056|x11: 0.087|x12: 0.681|x13: 0.379|x14: 0.384|x15: 0.507|x16: 0.114|x17: 0.000
-MEAN -&gt; x1: 0.047|x2: 0.205|x3: 0.224|x4: 0.128|x5: 0.084|x6: 0.129|x7: 0.215|x8: 0.040|x9: 0.086|x10: 0.068|x11: 0.131|x12: 0.250|x13: 0.192|x14: 0.128|x15: 0.254|x16: 0.072|x17: 0.000
+TOP2VEC -&gt; x1: 0.140|x2: 0.292|x3: 0.000|x4: 0.125|x5: 0.165|x6: 0.266|x7: 0.496|x8: 0.121|x9: 0.202|x10: 0.056|x11: 0.087|x12: 0.681|x13: 0.379|x14: 0.384|x15: 0.507|x16: 0.114|x17: 0.000
+MEAN -&gt; x1: 0.047|x2: 0.205|x3: 0.213|x4: 0.128|x5: 0.084|x6: 0.129|x7: 0.215|x8: 0.040|x9: 0.086|x10: 0.068|x11: 0.131|x12: 0.190|x13: 0.192|x14: 0.128|x15: 0.252|x16: 0.072|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.063|x3: 0.064|x4: 0.059|x5: 0.056|x6: 0.059|x7: 0.064|x8: 0.054|x9: 0.056|x10: 0.055|x11: 0.059|x12: 0.062|x13: 0.063|x14: 0.059|x15: 0.066|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -1349,7 +1379,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.579|x4: 0.051|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.334|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.188|x3: 0.302|x4: 0.559|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.000|x9: 0.119|x10: 0.000|x11: 0.000|x12: 0.066|x13: 0.091|x14: 0.130|x15: 0.000|x16: 0.113|x17: 0.000
 TOP2VEC -&gt; x1: 0.059|x2: 0.000|x3: 0.289|x4: 0.417|x5: 0.333|x6: 0.210|x7: 0.279|x8: 0.111|x9: 0.231|x10: 0.106|x11: 0.077|x12: 0.182|x13: 0.000|x14: 0.000|x15: 0.169|x16: 0.218|x17: 0.000
-MEAN -&gt; x1: 0.020|x2: 0.063|x3: 0.390|x4: 0.342|x5: 0.158|x6: 0.070|x7: 0.130|x8: 0.037|x9: 0.117|x10: 0.035|x11: 0.137|x12: 0.083|x13: 0.030|x14: 0.043|x15: 0.056|x16: 0.110|x17: 0.000
+MEAN -&gt; x1: 0.020|x2: 0.063|x3: 0.364|x4: 0.322|x5: 0.158|x6: 0.070|x7: 0.130|x8: 0.037|x9: 0.117|x10: 0.035|x11: 0.137|x12: 0.083|x13: 0.030|x14: 0.043|x15: 0.056|x16: 0.110|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.076|x4: 0.073|x5: 0.062|x6: 0.057|x7: 0.060|x8: 0.055|x9: 0.059|x10: 0.055|x11: 0.060|x12: 0.057|x13: 0.054|x14: 0.055|x15: 0.056|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -1377,8 +1408,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.415|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.199|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.153|x2: 0.139|x3: 0.318|x4: 0.448|x5: 0.255|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.132|x10: 0.000|x11: 0.000|x12: 0.094|x13: 0.110|x14: 0.000|x15: 0.000|x16: 0.171|x17: 0.000
-TOP2VEC -&gt; x1: 0.136|x2: 0.000|x3: 0.113|x4: 0.477|x5: 0.467|x6: 0.463|x7: 0.356|x8: 0.145|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.140|x14: 0.301|x15: 0.000|x16: 0.063|x17: 0.000
-MEAN -&gt; x1: 0.096|x2: 0.046|x3: 0.282|x4: 0.308|x5: 0.241|x6: 0.154|x7: 0.119|x8: 0.048|x9: 0.044|x10: 0.000|x11: 0.171|x12: 0.031|x13: 0.083|x14: 0.100|x15: 0.000|x16: 0.078|x17: 0.000
+TOP2VEC -&gt; x1: 0.136|x2: 0.000|x3: 0.113|x4: 0.477|x5: 0.467|x6: 0.463|x7: 0.356|x8: 0.145|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.141|x14: 0.301|x15: 0.000|x16: 0.063|x17: 0.000
+MEAN -&gt; x1: 0.097|x2: 0.046|x3: 0.282|x4: 0.308|x5: 0.241|x6: 0.154|x7: 0.119|x8: 0.048|x9: 0.044|x10: 0.000|x11: 0.171|x12: 0.031|x13: 0.083|x14: 0.100|x15: 0.000|x16: 0.078|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.055|x3: 0.070|x4: 0.072|x5: 0.067|x6: 0.061|x7: 0.059|x8: 0.055|x9: 0.055|x10: 0.053|x11: 0.062|x12: 0.054|x13: 0.057|x14: 0.058|x15: 0.053|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -1399,15 +1431,16 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 9]</t>
+          <t>[2, 3]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.694|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.293|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.402|x3: 0.257|x4: 0.294|x5: 0.096|x6: 0.000|x7: 0.106|x8: 0.000|x9: 0.398|x10: 0.000|x11: 0.000|x12: 0.064|x13: 0.107|x14: 0.000|x15: 0.000|x16: 0.097|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.230|x3: 0.554|x4: 0.281|x5: 0.303|x6: 0.000|x7: 0.328|x8: 0.146|x9: 0.192|x10: 0.000|x11: 0.000|x12: 0.193|x13: 0.179|x14: 0.258|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.211|x3: 0.501|x4: 0.192|x5: 0.133|x6: 0.000|x7: 0.145|x8: 0.049|x9: 0.196|x10: 0.000|x11: 0.098|x12: 0.086|x13: 0.095|x14: 0.086|x15: 0.000|x16: 0.032|x17: 0.000
+TOP2VEC -&gt; x1: 0.123|x2: 0.230|x3: 0.553|x4: 0.281|x5: 0.303|x6: 0.000|x7: 0.328|x8: 0.146|x9: 0.192|x10: 0.000|x11: 0.000|x12: 0.193|x13: 0.179|x14: 0.258|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.041|x2: 0.211|x3: 0.419|x4: 0.192|x5: 0.133|x6: 0.000|x7: 0.145|x8: 0.049|x9: 0.196|x10: 0.000|x11: 0.098|x12: 0.086|x13: 0.095|x14: 0.086|x15: 0.000|x16: 0.032|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.065|x3: 0.080|x4: 0.064|x5: 0.060|x6: 0.053|x7: 0.061|x8: 0.055|x9: 0.064|x10: 0.053|x11: 0.058|x12: 0.057|x13: 0.058|x14: 0.057|x15: 0.053|x16: 0.054|x17: 0.053
 </t>
         </is>
       </c>
@@ -1428,7 +1461,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[3, 4, 13]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1436,7 +1469,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.786|x4: 0.000|x5: 0.153|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.279|x12: 0.077|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.224|x3: 0.340|x4: 0.307|x5: 0.191|x6: 0.000|x7: 0.000|x8: 0.090|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.071|x13: 0.232|x14: 0.000|x15: 0.188|x16: 0.177|x17: 0.000
 TOP2VEC -&gt; x1: 0.144|x2: 0.000|x3: 0.260|x4: 0.236|x5: 0.194|x6: 0.186|x7: 0.422|x8: 0.122|x9: 0.000|x10: 0.000|x11: 0.134|x12: 0.246|x13: 0.269|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.075|x3: 0.462|x4: 0.181|x5: 0.180|x6: 0.062|x7: 0.141|x8: 0.071|x9: 0.000|x10: 0.000|x11: 0.138|x12: 0.131|x13: 0.167|x14: 0.000|x15: 0.063|x16: 0.059|x17: 0.000
+MEAN -&gt; x1: 0.048|x2: 0.075|x3: 0.367|x4: 0.181|x5: 0.180|x6: 0.062|x7: 0.141|x8: 0.071|x9: 0.000|x10: 0.000|x11: 0.138|x12: 0.131|x13: 0.167|x14: 0.000|x15: 0.063|x16: 0.059|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.077|x4: 0.064|x5: 0.064|x6: 0.056|x7: 0.061|x8: 0.057|x9: 0.053|x10: 0.053|x11: 0.061|x12: 0.061|x13: 0.063|x14: 0.053|x15: 0.056|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -1457,15 +1491,16 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 11]</t>
+          <t>[3, 4, 11]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.109|x2: 0.000|x3: 0.402|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.066|x11: 0.208|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.132|x2: 0.214|x3: 0.218|x4: 0.335|x5: 0.073|x6: 0.000|x7: 0.101|x8: 0.055|x9: 0.120|x10: 0.118|x11: 0.171|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.211|x16: 0.072|x17: 0.000
-TOP2VEC -&gt; x1: 0.239|x2: 0.288|x3: 0.075|x4: 0.568|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.269|x9: 0.211|x10: 0.137|x11: 0.306|x12: 0.186|x13: 0.311|x14: 0.269|x15: 0.000|x16: 0.280|x17: 0.000
-MEAN -&gt; x1: 0.160|x2: 0.167|x3: 0.232|x4: 0.301|x5: 0.082|x6: 0.000|x7: 0.034|x8: 0.108|x9: 0.110|x10: 0.107|x11: 0.228|x12: 0.062|x13: 0.104|x14: 0.090|x15: 0.070|x16: 0.118|x17: 0.000
+TOP2VEC -&gt; x1: 0.239|x2: 0.288|x3: 0.075|x4: 0.567|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.269|x9: 0.211|x10: 0.137|x11: 0.306|x12: 0.186|x13: 0.311|x14: 0.269|x15: 0.000|x16: 0.280|x17: 0.000
+MEAN -&gt; x1: 0.160|x2: 0.167|x3: 0.232|x4: 0.278|x5: 0.082|x6: 0.000|x7: 0.034|x8: 0.108|x9: 0.110|x10: 0.107|x11: 0.228|x12: 0.062|x13: 0.104|x14: 0.090|x15: 0.070|x16: 0.118|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.062|x3: 0.066|x4: 0.069|x5: 0.057|x6: 0.052|x7: 0.054|x8: 0.058|x9: 0.058|x10: 0.058|x11: 0.066|x12: 0.056|x13: 0.058|x14: 0.057|x15: 0.056|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -1486,7 +1521,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[3, 4, 8, 9]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1495,6 +1530,7 @@
 LDA -&gt; x1: 0.000|x2: 0.298|x3: 0.000|x4: 0.180|x5: 0.000|x6: 0.000|x7: 0.079|x8: 0.272|x9: 0.295|x10: 0.067|x11: 0.000|x12: 0.184|x13: 0.000|x14: 0.000|x15: 0.133|x16: 0.312|x17: 0.000
 TOP2VEC -&gt; x1: 0.196|x2: 0.000|x3: 0.138|x4: 0.406|x5: 0.349|x6: 0.222|x7: 0.387|x8: 0.297|x9: 0.359|x10: 0.088|x11: 0.180|x12: 0.191|x13: 0.063|x14: 0.125|x15: 0.064|x16: 0.179|x17: 0.000
 MEAN -&gt; x1: 0.065|x2: 0.099|x3: 0.197|x4: 0.195|x5: 0.116|x6: 0.074|x7: 0.155|x8: 0.190|x9: 0.218|x10: 0.051|x11: 0.147|x12: 0.125|x13: 0.021|x14: 0.042|x15: 0.066|x16: 0.164|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.064|x4: 0.064|x5: 0.059|x6: 0.056|x7: 0.061|x8: 0.063|x9: 0.065|x10: 0.055|x11: 0.061|x12: 0.059|x13: 0.054|x14: 0.055|x15: 0.056|x16: 0.062|x17: 0.052
 </t>
         </is>
       </c>
@@ -1523,7 +1559,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.364|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.165|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.208|x3: 0.379|x4: 0.000|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.190|x9: 0.060|x10: 0.367|x11: 0.000|x12: 0.000|x13: 0.187|x14: 0.203|x15: 0.000|x16: 0.054|x17: 0.000
 TOP2VEC -&gt; x1: 0.201|x2: 0.000|x3: 0.298|x4: 0.242|x5: 0.268|x6: 0.069|x7: 0.465|x8: 0.253|x9: 0.095|x10: 0.076|x11: 0.190|x12: 0.326|x13: 0.099|x14: 0.000|x15: 0.000|x16: 0.156|x17: 0.000
-MEAN -&gt; x1: 0.067|x2: 0.069|x3: 0.347|x4: 0.081|x5: 0.168|x6: 0.023|x7: 0.155|x8: 0.148|x9: 0.052|x10: 0.148|x11: 0.118|x12: 0.109|x13: 0.095|x14: 0.068|x15: 0.000|x16: 0.070|x17: 0.000
+MEAN -&gt; x1: 0.067|x2: 0.069|x3: 0.347|x4: 0.081|x5: 0.168|x6: 0.023|x7: 0.155|x8: 0.148|x9: 0.052|x10: 0.148|x11: 0.119|x12: 0.109|x13: 0.095|x14: 0.068|x15: 0.000|x16: 0.070|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.057|x3: 0.075|x4: 0.057|x5: 0.063|x6: 0.054|x7: 0.062|x8: 0.061|x9: 0.056|x10: 0.061|x11: 0.060|x12: 0.059|x13: 0.058|x14: 0.057|x15: 0.053|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -1544,15 +1581,16 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[3, 9, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.063|x2: 0.000|x3: 0.587|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.054|x11: 0.236|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.224|x2: 0.064|x3: 0.290|x4: 0.183|x5: 0.000|x6: 0.000|x7: 0.051|x8: 0.100|x9: 0.184|x10: 0.135|x11: 0.000|x12: 0.096|x13: 0.389|x14: 0.000|x15: 0.000|x16: 0.104|x17: 0.000
-TOP2VEC -&gt; x1: 0.115|x2: 0.165|x3: 0.210|x4: 0.000|x5: 0.189|x6: 0.059|x7: 0.000|x8: 0.213|x9: 0.400|x10: 0.059|x11: 0.282|x12: 0.247|x13: 0.000|x14: 0.360|x15: 0.243|x16: 0.121|x17: 0.000
-MEAN -&gt; x1: 0.134|x2: 0.076|x3: 0.362|x4: 0.061|x5: 0.063|x6: 0.020|x7: 0.017|x8: 0.104|x9: 0.195|x10: 0.083|x11: 0.172|x12: 0.114|x13: 0.130|x14: 0.120|x15: 0.081|x16: 0.075|x17: 0.000
+TOP2VEC -&gt; x1: 0.115|x2: 0.165|x3: 0.210|x4: 0.000|x5: 0.190|x6: 0.059|x7: 0.000|x8: 0.213|x9: 0.400|x10: 0.059|x11: 0.282|x12: 0.247|x13: 0.000|x14: 0.360|x15: 0.243|x16: 0.121|x17: 0.000
+MEAN -&gt; x1: 0.134|x2: 0.076|x3: 0.333|x4: 0.061|x5: 0.063|x6: 0.020|x7: 0.017|x8: 0.104|x9: 0.195|x10: 0.083|x11: 0.173|x12: 0.114|x13: 0.130|x14: 0.120|x15: 0.081|x16: 0.075|x17: 0.000
+SOFTMAX -&gt; x1: 0.060|x2: 0.057|x3: 0.074|x4: 0.056|x5: 0.056|x6: 0.054|x7: 0.054|x8: 0.059|x9: 0.064|x10: 0.057|x11: 0.063|x12: 0.059|x13: 0.060|x14: 0.060|x15: 0.057|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -1573,15 +1611,16 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[7, 8, 9]</t>
+          <t>[7, 9]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.300|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.173|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.068|x3: 0.000|x4: 0.197|x5: 0.054|x6: 0.000|x7: 0.226|x8: 0.254|x9: 0.308|x10: 0.063|x11: 0.122|x12: 0.079|x13: 0.000|x14: 0.000|x15: 0.313|x16: 0.136|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.262|x3: 0.000|x4: 0.301|x5: 0.443|x6: 0.407|x7: 0.602|x8: 0.309|x9: 0.369|x10: 0.152|x11: 0.094|x12: 0.306|x13: 0.151|x14: 0.171|x15: 0.158|x16: 0.311|x17: 0.000
-MEAN -&gt; x1: 0.074|x2: 0.110|x3: 0.100|x4: 0.166|x5: 0.166|x6: 0.136|x7: 0.276|x8: 0.187|x9: 0.226|x10: 0.072|x11: 0.130|x12: 0.128|x13: 0.050|x14: 0.057|x15: 0.157|x16: 0.149|x17: 0.000
+TOP2VEC -&gt; x1: 0.221|x2: 0.262|x3: 0.000|x4: 0.301|x5: 0.443|x6: 0.407|x7: 0.601|x8: 0.309|x9: 0.369|x10: 0.152|x11: 0.094|x12: 0.306|x13: 0.151|x14: 0.171|x15: 0.158|x16: 0.311|x17: 0.000
+MEAN -&gt; x1: 0.074|x2: 0.110|x3: 0.100|x4: 0.166|x5: 0.166|x6: 0.136|x7: 0.242|x8: 0.187|x9: 0.226|x10: 0.072|x11: 0.130|x12: 0.128|x13: 0.050|x14: 0.057|x15: 0.157|x16: 0.149|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.057|x4: 0.061|x5: 0.061|x6: 0.059|x7: 0.066|x8: 0.062|x9: 0.065|x10: 0.056|x11: 0.059|x12: 0.059|x13: 0.054|x14: 0.055|x15: 0.061|x16: 0.060|x17: 0.052
 </t>
         </is>
       </c>
@@ -1602,15 +1641,16 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 9]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.939|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.499|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.182|x3: 0.295|x4: 0.397|x5: 0.177|x6: 0.000|x7: 0.070|x8: 0.000|x9: 0.264|x10: 0.000|x11: 0.000|x12: 0.066|x13: 0.093|x14: 0.000|x15: 0.134|x16: 0.142|x17: 0.000
-TOP2VEC -&gt; x1: 0.240|x2: 0.315|x3: 0.343|x4: 0.232|x5: 0.397|x6: 0.142|x7: 0.376|x8: 0.319|x9: 0.201|x10: 0.097|x11: 0.087|x12: 0.133|x13: 0.105|x14: 0.284|x15: 0.183|x16: 0.198|x17: 0.000
-MEAN -&gt; x1: 0.080|x2: 0.166|x3: 0.525|x4: 0.209|x5: 0.191|x6: 0.047|x7: 0.149|x8: 0.106|x9: 0.155|x10: 0.032|x11: 0.195|x12: 0.066|x13: 0.066|x14: 0.095|x15: 0.106|x16: 0.114|x17: 0.000
+TOP2VEC -&gt; x1: 0.240|x2: 0.315|x3: 0.343|x4: 0.231|x5: 0.397|x6: 0.142|x7: 0.376|x8: 0.319|x9: 0.201|x10: 0.097|x11: 0.087|x12: 0.133|x13: 0.105|x14: 0.284|x15: 0.183|x16: 0.198|x17: 0.000
+MEAN -&gt; x1: 0.080|x2: 0.166|x3: 0.379|x4: 0.209|x5: 0.191|x6: 0.047|x7: 0.149|x8: 0.106|x9: 0.155|x10: 0.032|x11: 0.195|x12: 0.066|x13: 0.066|x14: 0.095|x15: 0.106|x16: 0.114|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.075|x4: 0.064|x5: 0.063|x6: 0.054|x7: 0.060|x8: 0.057|x9: 0.060|x10: 0.053|x11: 0.063|x12: 0.055|x13: 0.055|x14: 0.057|x15: 0.057|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -1631,15 +1671,16 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[3, 4, 5]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.531|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.113|x3: 0.229|x4: 0.204|x5: 0.250|x6: 0.068|x7: 0.055|x8: 0.124|x9: 0.000|x10: 0.082|x11: 0.078|x12: 0.082|x13: 0.000|x14: 0.139|x15: 0.205|x16: 0.191|x17: 0.000
-TOP2VEC -&gt; x1: 0.174|x2: 0.270|x3: 0.187|x4: 0.333|x5: 0.251|x6: 0.089|x7: 0.390|x8: 0.170|x9: 0.000|x10: 0.127|x11: 0.189|x12: 0.258|x13: 0.230|x14: 0.087|x15: 0.000|x16: 0.261|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.127|x3: 0.316|x4: 0.179|x5: 0.167|x6: 0.052|x7: 0.148|x8: 0.098|x9: 0.000|x10: 0.070|x11: 0.169|x12: 0.113|x13: 0.077|x14: 0.075|x15: 0.068|x16: 0.151|x17: 0.000
+TOP2VEC -&gt; x1: 0.174|x2: 0.270|x3: 0.187|x4: 0.333|x5: 0.251|x6: 0.088|x7: 0.390|x8: 0.170|x9: 0.000|x10: 0.127|x11: 0.189|x12: 0.258|x13: 0.230|x14: 0.087|x15: 0.000|x16: 0.261|x17: 0.000
+MEAN -&gt; x1: 0.058|x2: 0.127|x3: 0.305|x4: 0.179|x5: 0.167|x6: 0.052|x7: 0.148|x8: 0.098|x9: 0.000|x10: 0.070|x11: 0.169|x12: 0.113|x13: 0.077|x14: 0.075|x15: 0.068|x16: 0.151|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.071|x4: 0.063|x5: 0.062|x6: 0.055|x7: 0.061|x8: 0.058|x9: 0.053|x10: 0.056|x11: 0.062|x12: 0.059|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.061|x17: 0.053
 </t>
         </is>
       </c>
@@ -1660,15 +1701,16 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[3, 13, 14]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.779|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.304|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.411|x4: 0.070|x5: 0.168|x6: 0.087|x7: 0.056|x8: 0.000|x9: 0.000|x10: 0.087|x11: 0.000|x12: 0.078|x13: 0.308|x14: 0.146|x15: 0.274|x16: 0.134|x17: 0.000
-TOP2VEC -&gt; x1: 0.170|x2: 0.139|x3: 0.375|x4: 0.000|x5: 0.181|x6: 0.118|x7: 0.330|x8: 0.167|x9: 0.000|x10: 0.000|x11: 0.096|x12: 0.273|x13: 0.252|x14: 0.373|x15: 0.189|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.046|x3: 0.522|x4: 0.023|x5: 0.116|x6: 0.068|x7: 0.129|x8: 0.056|x9: 0.000|x10: 0.029|x11: 0.133|x12: 0.117|x13: 0.187|x14: 0.173|x15: 0.154|x16: 0.045|x17: 0.000
+TOP2VEC -&gt; x1: 0.170|x2: 0.139|x3: 0.375|x4: 0.000|x5: 0.181|x6: 0.118|x7: 0.330|x8: 0.167|x9: 0.000|x10: 0.000|x11: 0.095|x12: 0.273|x13: 0.252|x14: 0.373|x15: 0.189|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.046|x3: 0.429|x4: 0.023|x5: 0.116|x6: 0.068|x7: 0.129|x8: 0.056|x9: 0.000|x10: 0.029|x11: 0.133|x12: 0.117|x13: 0.187|x14: 0.173|x15: 0.154|x16: 0.045|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.081|x4: 0.054|x5: 0.059|x6: 0.056|x7: 0.060|x8: 0.056|x9: 0.053|x10: 0.054|x11: 0.060|x12: 0.059|x13: 0.064|x14: 0.063|x15: 0.062|x16: 0.055|x17: 0.053
 </t>
         </is>
       </c>
@@ -1696,8 +1738,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.401|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.190|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.404|x3: 0.182|x4: 0.498|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.091|x9: 0.118|x10: 0.281|x11: 0.000|x12: 0.000|x13: 0.080|x14: 0.165|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.278|x2: 0.584|x3: 0.190|x4: 0.305|x5: 0.121|x6: 0.000|x7: 0.238|x8: 0.355|x9: 0.226|x10: 0.093|x11: 0.230|x12: 0.427|x13: 0.177|x14: 0.276|x15: 0.085|x16: 0.190|x17: 0.000
-MEAN -&gt; x1: 0.093|x2: 0.329|x3: 0.258|x4: 0.268|x5: 0.040|x6: 0.000|x7: 0.079|x8: 0.149|x9: 0.115|x10: 0.125|x11: 0.140|x12: 0.142|x13: 0.086|x14: 0.147|x15: 0.028|x16: 0.063|x17: 0.000
+TOP2VEC -&gt; x1: 0.278|x2: 0.584|x3: 0.190|x4: 0.304|x5: 0.121|x6: 0.000|x7: 0.238|x8: 0.355|x9: 0.225|x10: 0.093|x11: 0.230|x12: 0.427|x13: 0.177|x14: 0.276|x15: 0.085|x16: 0.190|x17: 0.000
+MEAN -&gt; x1: 0.093|x2: 0.301|x3: 0.258|x4: 0.267|x5: 0.040|x6: 0.000|x7: 0.079|x8: 0.149|x9: 0.115|x10: 0.125|x11: 0.140|x12: 0.142|x13: 0.086|x14: 0.147|x15: 0.028|x16: 0.063|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.070|x3: 0.067|x4: 0.068|x5: 0.054|x6: 0.052|x7: 0.056|x8: 0.060|x9: 0.058|x10: 0.059|x11: 0.060|x12: 0.060|x13: 0.057|x14: 0.060|x15: 0.053|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -1718,7 +1761,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[4, 5, 7, 9, 11, 16]</t>
+          <t>[4, 5, 7, 9]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1726,7 +1769,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.444|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.257|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.074|x3: 0.079|x4: 0.219|x5: 0.195|x6: 0.000|x7: 0.144|x8: 0.000|x9: 0.246|x10: 0.000|x11: 0.071|x12: 0.145|x13: 0.090|x14: 0.214|x15: 0.056|x16: 0.286|x17: 0.000
 TOP2VEC -&gt; x1: 0.183|x2: 0.146|x3: 0.000|x4: 0.551|x5: 0.449|x6: 0.366|x7: 0.588|x8: 0.288|x9: 0.406|x10: 0.107|x11: 0.211|x12: 0.320|x13: 0.061|x14: 0.186|x15: 0.000|x16: 0.220|x17: 0.000
-MEAN -&gt; x1: 0.061|x2: 0.073|x3: 0.174|x4: 0.257|x5: 0.214|x6: 0.122|x7: 0.244|x8: 0.096|x9: 0.217|x10: 0.036|x11: 0.180|x12: 0.155|x13: 0.050|x14: 0.133|x15: 0.019|x16: 0.169|x17: 0.000
+MEAN -&gt; x1: 0.061|x2: 0.073|x3: 0.174|x4: 0.240|x5: 0.214|x6: 0.122|x7: 0.215|x8: 0.096|x9: 0.217|x10: 0.036|x11: 0.180|x12: 0.155|x13: 0.050|x14: 0.133|x15: 0.019|x16: 0.169|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.056|x3: 0.062|x4: 0.066|x5: 0.064|x6: 0.058|x7: 0.064|x8: 0.057|x9: 0.064|x10: 0.054|x11: 0.062|x12: 0.060|x13: 0.054|x14: 0.059|x15: 0.053|x16: 0.061|x17: 0.052
 </t>
         </is>
       </c>
@@ -1747,15 +1791,16 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 13, 14, 15]</t>
+          <t>[3, 9, 13, 14, 15]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.445|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.257|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.075|x3: 0.140|x4: 0.197|x5: 0.000|x6: 0.000|x7: 0.094|x8: 0.000|x9: 0.351|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.226|x14: 0.239|x15: 0.447|x16: 0.053|x17: 0.000
-TOP2VEC -&gt; x1: 0.312|x2: 0.342|x3: 0.069|x4: 0.275|x5: 0.128|x6: 0.307|x7: 0.471|x8: 0.360|x9: 0.435|x10: 0.109|x11: 0.254|x12: 0.454|x13: 0.470|x14: 0.435|x15: 0.417|x16: 0.223|x17: 0.000
+TOP2VEC -&gt; x1: 0.312|x2: 0.342|x3: 0.069|x4: 0.276|x5: 0.128|x6: 0.307|x7: 0.471|x8: 0.360|x9: 0.435|x10: 0.109|x11: 0.254|x12: 0.454|x13: 0.470|x14: 0.435|x15: 0.417|x16: 0.223|x17: 0.000
 MEAN -&gt; x1: 0.104|x2: 0.139|x3: 0.218|x4: 0.157|x5: 0.043|x6: 0.102|x7: 0.188|x8: 0.120|x9: 0.262|x10: 0.036|x11: 0.170|x12: 0.151|x13: 0.232|x14: 0.224|x15: 0.288|x16: 0.092|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.063|x4: 0.059|x5: 0.053|x6: 0.056|x7: 0.061|x8: 0.057|x9: 0.066|x10: 0.052|x11: 0.060|x12: 0.059|x13: 0.064|x14: 0.063|x15: 0.067|x16: 0.055|x17: 0.051
 </t>
         </is>
       </c>
@@ -1783,8 +1828,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.426|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.205|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.347|x3: 0.174|x4: 0.241|x5: 0.000|x6: 0.081|x7: 0.368|x8: 0.000|x9: 0.149|x10: 0.000|x11: 0.159|x12: 0.057|x13: 0.182|x14: 0.000|x15: 0.000|x16: 0.063|x17: 0.000
-TOP2VEC -&gt; x1: 0.171|x2: 0.000|x3: 0.340|x4: 0.386|x5: 0.296|x6: 0.000|x7: 0.067|x8: 0.201|x9: 0.205|x10: 0.118|x11: 0.000|x12: 0.161|x13: 0.222|x14: 0.222|x15: 0.000|x16: 0.241|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.116|x3: 0.313|x4: 0.209|x5: 0.099|x6: 0.027|x7: 0.145|x8: 0.067|x9: 0.118|x10: 0.039|x11: 0.121|x12: 0.073|x13: 0.135|x14: 0.074|x15: 0.000|x16: 0.101|x17: 0.000
+TOP2VEC -&gt; x1: 0.171|x2: 0.000|x3: 0.339|x4: 0.386|x5: 0.295|x6: 0.000|x7: 0.067|x8: 0.201|x9: 0.205|x10: 0.118|x11: 0.000|x12: 0.161|x13: 0.222|x14: 0.222|x15: 0.000|x16: 0.241|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.116|x3: 0.313|x4: 0.209|x5: 0.098|x6: 0.027|x7: 0.145|x8: 0.067|x9: 0.118|x10: 0.039|x11: 0.121|x12: 0.073|x13: 0.135|x14: 0.074|x15: 0.000|x16: 0.101|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.073|x4: 0.065|x5: 0.059|x6: 0.055|x7: 0.061|x8: 0.057|x9: 0.060|x10: 0.055|x11: 0.060|x12: 0.057|x13: 0.061|x14: 0.057|x15: 0.053|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -1812,8 +1858,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.490|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.278|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.317|x3: 0.295|x4: 0.318|x5: 0.103|x6: 0.000|x7: 0.066|x8: 0.000|x9: 0.247|x10: 0.133|x11: 0.129|x12: 0.000|x13: 0.149|x14: 0.000|x15: 0.000|x16: 0.062|x17: 0.000
-TOP2VEC -&gt; x1: 0.070|x2: 0.321|x3: 0.445|x4: 0.122|x5: 0.216|x6: 0.136|x7: 0.000|x8: 0.117|x9: 0.165|x10: 0.148|x11: 0.268|x12: 0.174|x13: 0.000|x14: 0.154|x15: 0.192|x16: 0.302|x17: 0.000
+TOP2VEC -&gt; x1: 0.070|x2: 0.321|x3: 0.445|x4: 0.122|x5: 0.217|x6: 0.136|x7: 0.000|x8: 0.117|x9: 0.165|x10: 0.148|x11: 0.268|x12: 0.174|x13: 0.000|x14: 0.154|x15: 0.192|x16: 0.302|x17: 0.000
 MEAN -&gt; x1: 0.023|x2: 0.213|x3: 0.410|x4: 0.147|x5: 0.107|x6: 0.045|x7: 0.022|x8: 0.039|x9: 0.137|x10: 0.094|x11: 0.225|x12: 0.058|x13: 0.050|x14: 0.051|x15: 0.064|x16: 0.122|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.065|x3: 0.079|x4: 0.061|x5: 0.059|x6: 0.055|x7: 0.054|x8: 0.055|x9: 0.060|x10: 0.058|x11: 0.066|x12: 0.056|x13: 0.055|x14: 0.055|x15: 0.056|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -1834,15 +1881,16 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[4, 8]</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.078|x2: 0.000|x3: 0.333|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.206|x9: 0.000|x10: 0.000|x11: 0.147|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.140|x3: 0.094|x4: 0.236|x5: 0.000|x6: 0.000|x7: 0.125|x8: 0.443|x9: 0.468|x10: 0.108|x11: 0.108|x12: 0.000|x13: 0.097|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.139|x2: 0.000|x3: 0.091|x4: 0.335|x5: 0.340|x6: 0.335|x7: 0.257|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.167|x13: 0.124|x14: 0.000|x15: 0.185|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.139|x2: 0.000|x3: 0.091|x4: 0.336|x5: 0.340|x6: 0.335|x7: 0.257|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.168|x13: 0.124|x14: 0.000|x15: 0.185|x16: 0.000|x17: 0.000
 MEAN -&gt; x1: 0.072|x2: 0.047|x3: 0.173|x4: 0.191|x5: 0.113|x6: 0.112|x7: 0.127|x8: 0.269|x9: 0.156|x10: 0.036|x11: 0.085|x12: 0.056|x13: 0.074|x14: 0.000|x15: 0.062|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.064|x4: 0.065|x5: 0.060|x6: 0.060|x7: 0.061|x8: 0.070|x9: 0.063|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.058|x14: 0.053|x15: 0.057|x16: 0.053|x17: 0.053
 </t>
         </is>
       </c>
@@ -1863,7 +1911,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 11, 13]</t>
+          <t>[4, 11]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1871,7 +1919,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.484|x4: 0.142|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.280|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.123|x3: 0.109|x4: 0.362|x5: 0.093|x6: 0.000|x7: 0.124|x8: 0.113|x9: 0.169|x10: 0.101|x11: 0.000|x12: 0.133|x13: 0.173|x14: 0.000|x15: 0.123|x16: 0.198|x17: 0.000
 TOP2VEC -&gt; x1: 0.102|x2: 0.373|x3: 0.000|x4: 0.656|x5: 0.322|x6: 0.182|x7: 0.253|x8: 0.083|x9: 0.243|x10: 0.097|x11: 0.367|x12: 0.282|x13: 0.355|x14: 0.386|x15: 0.000|x16: 0.198|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.165|x3: 0.197|x4: 0.387|x5: 0.139|x6: 0.061|x7: 0.126|x8: 0.066|x9: 0.137|x10: 0.066|x11: 0.216|x12: 0.138|x13: 0.176|x14: 0.129|x15: 0.041|x16: 0.132|x17: 0.000
+MEAN -&gt; x1: 0.034|x2: 0.165|x3: 0.197|x4: 0.334|x5: 0.139|x6: 0.061|x7: 0.126|x8: 0.066|x9: 0.137|x10: 0.066|x11: 0.216|x12: 0.138|x13: 0.176|x14: 0.129|x15: 0.041|x16: 0.132|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.061|x3: 0.063|x4: 0.072|x5: 0.059|x6: 0.055|x7: 0.059|x8: 0.055|x9: 0.059|x10: 0.055|x11: 0.064|x12: 0.059|x13: 0.062|x14: 0.059|x15: 0.054|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -1892,15 +1941,16 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>[1, 4, 5, 14]</t>
+          <t>[1, 4, 14]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.275|x2: 0.000|x3: 0.416|x4: 0.079|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.238|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.233|x2: 0.158|x3: 0.082|x4: 0.267|x5: 0.277|x6: 0.054|x7: 0.129|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.369|x15: 0.000|x16: 0.093|x17: 0.000
-TOP2VEC -&gt; x1: 0.182|x2: 0.201|x3: 0.059|x4: 0.384|x5: 0.312|x6: 0.135|x7: 0.168|x8: 0.222|x9: 0.118|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.139|x14: 0.364|x15: 0.000|x16: 0.197|x17: 0.000
+TOP2VEC -&gt; x1: 0.182|x2: 0.200|x3: 0.059|x4: 0.384|x5: 0.312|x6: 0.134|x7: 0.168|x8: 0.222|x9: 0.118|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.139|x14: 0.364|x15: 0.000|x16: 0.197|x17: 0.000
 MEAN -&gt; x1: 0.230|x2: 0.120|x3: 0.186|x4: 0.243|x5: 0.196|x6: 0.063|x7: 0.099|x8: 0.074|x9: 0.092|x10: 0.032|x11: 0.079|x12: 0.000|x13: 0.046|x14: 0.244|x15: 0.000|x16: 0.097|x17: 0.000
+SOFTMAX -&gt; x1: 0.066|x2: 0.059|x3: 0.063|x4: 0.067|x5: 0.064|x6: 0.056|x7: 0.058|x8: 0.057|x9: 0.058|x10: 0.054|x11: 0.057|x12: 0.053|x13: 0.055|x14: 0.067|x15: 0.053|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -1929,7 +1979,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.350|x4: 0.498|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.067|x11: 0.202|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.217|x3: 0.000|x4: 0.621|x5: 0.000|x6: 0.000|x7: 0.412|x8: 0.000|x9: 0.209|x10: 0.000|x11: 0.058|x12: 0.123|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.180|x17: 0.000
 TOP2VEC -&gt; x1: 0.193|x2: 0.113|x3: 0.000|x4: 0.712|x5: 0.306|x6: 0.000|x7: 0.229|x8: 0.252|x9: 0.000|x10: 0.000|x11: 0.065|x12: 0.176|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000
-MEAN -&gt; x1: 0.064|x2: 0.110|x3: 0.117|x4: 0.610|x5: 0.102|x6: 0.000|x7: 0.214|x8: 0.084|x9: 0.070|x10: 0.022|x11: 0.109|x12: 0.099|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.078|x17: 0.000
+MEAN -&gt; x1: 0.064|x2: 0.110|x3: 0.117|x4: 0.499|x5: 0.102|x6: 0.000|x7: 0.214|x8: 0.084|x9: 0.070|x10: 0.022|x11: 0.109|x12: 0.100|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.078|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.059|x3: 0.060|x4: 0.088|x5: 0.059|x6: 0.053|x7: 0.066|x8: 0.058|x9: 0.057|x10: 0.054|x11: 0.059|x12: 0.059|x13: 0.053|x14: 0.053|x15: 0.053|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -1950,7 +2001,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 7]</t>
+          <t>[3, 4, 5]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1959,6 +2010,7 @@
 LDA -&gt; x1: 0.102|x2: 0.124|x3: 0.211|x4: 0.330|x5: 0.240|x6: 0.000|x7: 0.112|x8: 0.154|x9: 0.232|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.076|x14: 0.114|x15: 0.053|x16: 0.073|x17: 0.000
 TOP2VEC -&gt; x1: 0.078|x2: 0.117|x3: 0.115|x4: 0.436|x5: 0.493|x6: 0.217|x7: 0.378|x8: 0.076|x9: 0.134|x10: 0.000|x11: 0.000|x12: 0.166|x13: 0.186|x14: 0.000|x15: 0.000|x16: 0.098|x17: 0.000
 MEAN -&gt; x1: 0.125|x2: 0.080|x3: 0.202|x4: 0.318|x5: 0.244|x6: 0.072|x7: 0.163|x8: 0.077|x9: 0.122|x10: 0.000|x11: 0.044|x12: 0.055|x13: 0.087|x14: 0.038|x15: 0.018|x16: 0.108|x17: 0.000
+SOFTMAX -&gt; x1: 0.060|x2: 0.057|x3: 0.065|x4: 0.073|x5: 0.067|x6: 0.057|x7: 0.062|x8: 0.057|x9: 0.060|x10: 0.053|x11: 0.055|x12: 0.056|x13: 0.058|x14: 0.055|x15: 0.054|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -1979,15 +2031,16 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>[3, 4, 7]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.572|x4: 0.108|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.331|x12: 0.055|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.194|x3: 0.197|x4: 0.283|x5: 0.000|x6: 0.083|x7: 0.102|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.181|x13: 0.051|x14: 0.291|x15: 0.164|x16: 0.274|x17: 0.000
-TOP2VEC -&gt; x1: 0.177|x2: 0.224|x3: 0.202|x4: 0.473|x5: 0.212|x6: 0.000|x7: 0.377|x8: 0.212|x9: 0.152|x10: 0.096|x11: 0.091|x12: 0.332|x13: 0.172|x14: 0.000|x15: 0.000|x16: 0.196|x17: 0.000
-MEAN -&gt; x1: 0.059|x2: 0.139|x3: 0.324|x4: 0.288|x5: 0.071|x6: 0.028|x7: 0.159|x8: 0.071|x9: 0.051|x10: 0.032|x11: 0.140|x12: 0.190|x13: 0.074|x14: 0.097|x15: 0.055|x16: 0.157|x17: 0.000
+TOP2VEC -&gt; x1: 0.177|x2: 0.223|x3: 0.202|x4: 0.473|x5: 0.212|x6: 0.000|x7: 0.377|x8: 0.212|x9: 0.152|x10: 0.096|x11: 0.091|x12: 0.332|x13: 0.172|x14: 0.000|x15: 0.000|x16: 0.196|x17: 0.000
+MEAN -&gt; x1: 0.059|x2: 0.139|x3: 0.300|x4: 0.288|x5: 0.071|x6: 0.028|x7: 0.159|x8: 0.071|x9: 0.051|x10: 0.032|x11: 0.140|x12: 0.190|x13: 0.074|x14: 0.097|x15: 0.055|x16: 0.157|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.071|x4: 0.070|x5: 0.056|x6: 0.054|x7: 0.061|x8: 0.056|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.063|x13: 0.056|x14: 0.058|x15: 0.055|x16: 0.061|x17: 0.052
 </t>
         </is>
       </c>
@@ -2008,15 +2061,16 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[2, 4, 5, 6]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.498|x4: 0.110|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.288|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.430|x3: 0.000|x4: 0.588|x5: 0.180|x6: 0.208|x7: 0.057|x8: 0.000|x9: 0.208|x10: 0.094|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000
-TOP2VEC -&gt; x1: 0.208|x2: 0.162|x3: 0.000|x4: 0.496|x5: 0.353|x6: 0.255|x7: 0.426|x8: 0.211|x9: 0.076|x10: 0.087|x11: 0.000|x12: 0.000|x13: 0.294|x14: 0.259|x15: 0.101|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.069|x2: 0.197|x3: 0.166|x4: 0.398|x5: 0.177|x6: 0.154|x7: 0.161|x8: 0.070|x9: 0.095|x10: 0.060|x11: 0.096|x12: 0.000|x13: 0.098|x14: 0.086|x15: 0.034|x16: 0.078|x17: 0.000
+TOP2VEC -&gt; x1: 0.208|x2: 0.162|x3: 0.000|x4: 0.496|x5: 0.353|x6: 0.255|x7: 0.426|x8: 0.211|x9: 0.076|x10: 0.087|x11: 0.000|x12: 0.000|x13: 0.294|x14: 0.259|x15: 0.100|x16: 0.179|x17: 0.000
+MEAN -&gt; x1: 0.069|x2: 0.197|x3: 0.166|x4: 0.369|x5: 0.177|x6: 0.154|x7: 0.161|x8: 0.070|x9: 0.095|x10: 0.060|x11: 0.096|x12: 0.000|x13: 0.098|x14: 0.086|x15: 0.033|x16: 0.078|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.064|x3: 0.062|x4: 0.076|x5: 0.063|x6: 0.061|x7: 0.062|x8: 0.056|x9: 0.058|x10: 0.056|x11: 0.058|x12: 0.052|x13: 0.058|x14: 0.057|x15: 0.054|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -2037,15 +2091,16 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 13]</t>
+          <t>[4, 5, 13]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.395|x4: 0.114|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.228|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.147|x4: 0.142|x5: 0.136|x6: 0.000|x7: 0.080|x8: 0.232|x9: 0.300|x10: 0.222|x11: 0.054|x12: 0.081|x13: 0.212|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.156|x2: 0.082|x3: 0.000|x4: 0.643|x5: 0.517|x6: 0.195|x7: 0.491|x8: 0.131|x9: 0.144|x10: 0.000|x11: 0.000|x12: 0.381|x13: 0.388|x14: 0.151|x15: 0.000|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.052|x2: 0.051|x3: 0.181|x4: 0.300|x5: 0.218|x6: 0.065|x7: 0.190|x8: 0.121|x9: 0.148|x10: 0.074|x11: 0.094|x12: 0.154|x13: 0.200|x14: 0.050|x15: 0.000|x16: 0.082|x17: 0.000
+TOP2VEC -&gt; x1: 0.157|x2: 0.082|x3: 0.000|x4: 0.643|x5: 0.518|x6: 0.195|x7: 0.491|x8: 0.131|x9: 0.144|x10: 0.000|x11: 0.000|x12: 0.381|x13: 0.388|x14: 0.151|x15: 0.000|x16: 0.104|x17: 0.000
+MEAN -&gt; x1: 0.052|x2: 0.051|x3: 0.181|x4: 0.252|x5: 0.212|x6: 0.065|x7: 0.190|x8: 0.121|x9: 0.148|x10: 0.074|x11: 0.094|x12: 0.154|x13: 0.200|x14: 0.050|x15: 0.000|x16: 0.082|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.063|x4: 0.067|x5: 0.065|x6: 0.056|x7: 0.063|x8: 0.059|x9: 0.061|x10: 0.056|x11: 0.058|x12: 0.061|x13: 0.064|x14: 0.055|x15: 0.052|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -2066,7 +2121,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 16]</t>
+          <t>[4, 8, 10]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2074,7 +2129,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.263|x4: 0.000|x5: 0.083|x6: 0.000|x7: 0.000|x8: 0.163|x9: 0.000|x10: 0.188|x11: 0.152|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.156|x3: 0.000|x4: 0.199|x5: 0.244|x6: 0.000|x7: 0.000|x8: 0.267|x9: 0.000|x10: 0.433|x11: 0.000|x12: 0.166|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.354|x17: 0.000
 TOP2VEC -&gt; x1: 0.243|x2: 0.214|x3: 0.000|x4: 0.556|x5: 0.181|x6: 0.000|x7: 0.000|x8: 0.240|x9: 0.000|x10: 0.080|x11: 0.184|x12: 0.264|x13: 0.315|x14: 0.084|x15: 0.000|x16: 0.163|x17: 0.000
-MEAN -&gt; x1: 0.081|x2: 0.123|x3: 0.088|x4: 0.252|x5: 0.170|x6: 0.000|x7: 0.000|x8: 0.223|x9: 0.000|x10: 0.234|x11: 0.112|x12: 0.143|x13: 0.105|x14: 0.028|x15: 0.000|x16: 0.172|x17: 0.000
+MEAN -&gt; x1: 0.081|x2: 0.123|x3: 0.088|x4: 0.233|x5: 0.170|x6: 0.000|x7: 0.000|x8: 0.223|x9: 0.000|x10: 0.234|x11: 0.112|x12: 0.143|x13: 0.105|x14: 0.028|x15: 0.000|x16: 0.172|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.058|x4: 0.067|x5: 0.063|x6: 0.053|x7: 0.053|x8: 0.066|x9: 0.053|x10: 0.067|x11: 0.059|x12: 0.061|x13: 0.059|x14: 0.055|x15: 0.053|x16: 0.063|x17: 0.053
 </t>
         </is>
       </c>
@@ -2095,15 +2151,16 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[4, 11, 14]</t>
+          <t>[4, 11]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.333|x4: 0.118|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.217|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.179|x3: 0.099|x4: 0.350|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.180|x9: 0.203|x10: 0.135|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.350|x15: 0.083|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.155|x2: 0.235|x3: 0.061|x4: 0.455|x5: 0.456|x6: 0.155|x7: 0.238|x8: 0.146|x9: 0.000|x10: 0.076|x11: 0.364|x12: 0.209|x13: 0.229|x14: 0.244|x15: 0.000|x16: 0.156|x17: 0.000
+TOP2VEC -&gt; x1: 0.155|x2: 0.235|x3: 0.061|x4: 0.456|x5: 0.456|x6: 0.155|x7: 0.238|x8: 0.146|x9: 0.000|x10: 0.076|x11: 0.364|x12: 0.209|x13: 0.229|x14: 0.244|x15: 0.000|x16: 0.156|x17: 0.000
 MEAN -&gt; x1: 0.052|x2: 0.138|x3: 0.164|x4: 0.308|x5: 0.152|x6: 0.052|x7: 0.079|x8: 0.109|x9: 0.068|x10: 0.070|x11: 0.274|x12: 0.070|x13: 0.076|x14: 0.198|x15: 0.028|x16: 0.052|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.062|x4: 0.071|x5: 0.061|x6: 0.055|x7: 0.057|x8: 0.058|x9: 0.056|x10: 0.056|x11: 0.069|x12: 0.056|x13: 0.057|x14: 0.064|x15: 0.054|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -2124,15 +2181,16 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>[3, 4, 9, 12]</t>
+          <t>[3, 4, 9]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.440|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.256|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.092|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.101|x3: 0.097|x4: 0.237|x5: 0.075|x6: 0.000|x7: 0.104|x8: 0.150|x9: 0.389|x10: 0.000|x11: 0.000|x12: 0.203|x13: 0.155|x14: 0.000|x15: 0.000|x16: 0.308|x17: 0.000
-TOP2VEC -&gt; x1: 0.101|x2: 0.254|x3: 0.133|x4: 0.409|x5: 0.294|x6: 0.169|x7: 0.234|x8: 0.128|x9: 0.331|x10: 0.079|x11: 0.193|x12: 0.364|x13: 0.227|x14: 0.172|x15: 0.115|x16: 0.161|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.118|x3: 0.224|x4: 0.215|x5: 0.123|x6: 0.056|x7: 0.113|x8: 0.093|x9: 0.240|x10: 0.026|x11: 0.149|x12: 0.189|x13: 0.127|x14: 0.057|x15: 0.038|x16: 0.187|x17: 0.000
+TOP2VEC -&gt; x1: 0.101|x2: 0.254|x3: 0.133|x4: 0.409|x5: 0.294|x6: 0.169|x7: 0.234|x8: 0.128|x9: 0.331|x10: 0.079|x11: 0.193|x12: 0.364|x13: 0.227|x14: 0.172|x15: 0.116|x16: 0.161|x17: 0.000
+MEAN -&gt; x1: 0.034|x2: 0.118|x3: 0.224|x4: 0.215|x5: 0.123|x6: 0.056|x7: 0.113|x8: 0.093|x9: 0.240|x10: 0.026|x11: 0.149|x12: 0.189|x13: 0.127|x14: 0.057|x15: 0.039|x16: 0.187|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.059|x3: 0.065|x4: 0.065|x5: 0.059|x6: 0.055|x7: 0.058|x8: 0.057|x9: 0.066|x10: 0.054|x11: 0.061|x12: 0.063|x13: 0.059|x14: 0.055|x15: 0.054|x16: 0.063|x17: 0.052
 </t>
         </is>
       </c>
@@ -2153,7 +2211,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>[3, 13, 14]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2162,6 +2220,7 @@
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.177|x4: 0.216|x5: 0.218|x6: 0.000|x7: 0.000|x8: 0.140|x9: 0.124|x10: 0.000|x11: 0.000|x12: 0.078|x13: 0.218|x14: 0.276|x15: 0.128|x16: 0.175|x17: 0.000
 TOP2VEC -&gt; x1: 0.148|x2: 0.069|x3: 0.092|x4: 0.163|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.151|x9: 0.097|x10: 0.000|x11: 0.063|x12: 0.321|x13: 0.234|x14: 0.320|x15: 0.322|x16: 0.000|x17: 0.000
 MEAN -&gt; x1: 0.049|x2: 0.046|x3: 0.251|x4: 0.126|x5: 0.130|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.074|x10: 0.000|x11: 0.116|x12: 0.133|x13: 0.151|x14: 0.198|x15: 0.150|x16: 0.058|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.056|x3: 0.069|x4: 0.061|x5: 0.061|x6: 0.053|x7: 0.053|x8: 0.059|x9: 0.058|x10: 0.053|x11: 0.060|x12: 0.061|x13: 0.062|x14: 0.065|x15: 0.062|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -2182,7 +2241,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[2, 4, 5, 6, 14, 16]</t>
+          <t>[4, 5, 14, 16]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2190,7 +2249,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.275|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.159|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.515|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.241|x3: 0.000|x4: 0.296|x5: 0.291|x6: 0.110|x7: 0.053|x8: 0.000|x9: 0.191|x10: 0.000|x11: 0.061|x12: 0.097|x13: 0.000|x14: 0.230|x15: 0.000|x16: 0.250|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.309|x3: 0.120|x4: 0.433|x5: 0.585|x6: 0.486|x7: 0.195|x8: 0.000|x9: 0.000|x10: 0.140|x11: 0.231|x12: 0.151|x13: 0.000|x14: 0.441|x15: 0.143|x16: 0.287|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.183|x3: 0.132|x4: 0.243|x5: 0.292|x6: 0.199|x7: 0.082|x8: 0.000|x9: 0.064|x10: 0.047|x11: 0.150|x12: 0.082|x13: 0.000|x14: 0.224|x15: 0.048|x16: 0.351|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.183|x3: 0.132|x4: 0.243|x5: 0.264|x6: 0.199|x7: 0.082|x8: 0.000|x9: 0.064|x10: 0.047|x11: 0.150|x12: 0.082|x13: 0.000|x14: 0.224|x15: 0.048|x16: 0.346|x17: 0.000
+SOFTMAX -&gt; x1: 0.052|x2: 0.062|x3: 0.059|x4: 0.066|x5: 0.067|x6: 0.063|x7: 0.056|x8: 0.052|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.056|x13: 0.052|x14: 0.065|x15: 0.054|x16: 0.073|x17: 0.052
 </t>
         </is>
       </c>
@@ -2218,8 +2278,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.121|x4: 0.000|x5: 0.182|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.070|x12: 0.081|x13: 0.000|x14: 0.068|x15: 0.000|x16: 0.143|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.163|x3: 0.000|x4: 0.000|x5: 0.184|x6: 0.000|x7: 0.082|x8: 0.000|x9: 0.000|x10: 0.134|x11: 0.000|x12: 0.207|x13: 0.000|x14: 0.274|x15: 0.370|x16: 0.406|x17: 0.000
-TOP2VEC -&gt; x1: 0.141|x2: 0.233|x3: 0.000|x4: 0.183|x5: 0.395|x6: 0.000|x7: 0.000|x8: 0.172|x9: 0.000|x10: 0.190|x11: 0.000|x12: 0.000|x13: 0.054|x14: 0.386|x15: 0.335|x16: 0.388|x17: 0.000
+TOP2VEC -&gt; x1: 0.141|x2: 0.233|x3: 0.000|x4: 0.183|x5: 0.395|x6: 0.000|x7: 0.000|x8: 0.171|x9: 0.000|x10: 0.190|x11: 0.000|x12: 0.000|x13: 0.054|x14: 0.386|x15: 0.335|x16: 0.388|x17: 0.000
 MEAN -&gt; x1: 0.047|x2: 0.132|x3: 0.040|x4: 0.061|x5: 0.254|x6: 0.000|x7: 0.027|x8: 0.057|x9: 0.000|x10: 0.108|x11: 0.023|x12: 0.096|x13: 0.018|x14: 0.243|x15: 0.235|x16: 0.313|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.055|x4: 0.056|x5: 0.068|x6: 0.053|x7: 0.055|x8: 0.056|x9: 0.053|x10: 0.059|x11: 0.054|x12: 0.058|x13: 0.054|x14: 0.068|x15: 0.067|x16: 0.073|x17: 0.053
 </t>
         </is>
       </c>
@@ -2240,7 +2301,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>[5, 8, 11, 14]</t>
+          <t>[5, 11]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2248,7 +2309,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.272|x4: 0.000|x5: 0.110|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.269|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.093|x3: 0.058|x4: 0.114|x5: 0.302|x6: 0.000|x7: 0.000|x8: 0.436|x9: 0.111|x10: 0.107|x11: 0.100|x12: 0.000|x13: 0.000|x14: 0.347|x15: 0.058|x16: 0.093|x17: 0.000
 TOP2VEC -&gt; x1: 0.089|x2: 0.000|x3: 0.000|x4: 0.122|x5: 0.295|x6: 0.239|x7: 0.280|x8: 0.103|x9: 0.301|x10: 0.000|x11: 0.513|x12: 0.233|x13: 0.243|x14: 0.207|x15: 0.120|x16: 0.057|x17: 0.000
-MEAN -&gt; x1: 0.030|x2: 0.031|x3: 0.110|x4: 0.079|x5: 0.236|x6: 0.080|x7: 0.093|x8: 0.180|x9: 0.137|x10: 0.036|x11: 0.294|x12: 0.078|x13: 0.081|x14: 0.185|x15: 0.059|x16: 0.050|x17: 0.000
+MEAN -&gt; x1: 0.030|x2: 0.031|x3: 0.110|x4: 0.079|x5: 0.236|x6: 0.080|x7: 0.093|x8: 0.180|x9: 0.137|x10: 0.036|x11: 0.290|x12: 0.078|x13: 0.081|x14: 0.185|x15: 0.059|x16: 0.050|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.055|x3: 0.059|x4: 0.057|x5: 0.067|x6: 0.057|x7: 0.058|x8: 0.063|x9: 0.061|x10: 0.055|x11: 0.071|x12: 0.057|x13: 0.057|x14: 0.064|x15: 0.056|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -2269,7 +2331,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[4, 5, 8, 13]</t>
+          <t>[5, 8]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2278,6 +2340,7 @@
 LDA -&gt; x1: 0.000|x2: 0.126|x3: 0.147|x4: 0.145|x5: 0.227|x6: 0.054|x7: 0.000|x8: 0.334|x9: 0.065|x10: 0.131|x11: 0.000|x12: 0.083|x13: 0.226|x14: 0.000|x15: 0.086|x16: 0.196|x17: 0.000
 TOP2VEC -&gt; x1: 0.193|x2: 0.000|x3: 0.000|x4: 0.401|x5: 0.298|x6: 0.000|x7: 0.373|x8: 0.222|x9: 0.158|x10: 0.056|x11: 0.000|x12: 0.117|x13: 0.220|x14: 0.144|x15: 0.270|x16: 0.115|x17: 0.000
 MEAN -&gt; x1: 0.064|x2: 0.042|x3: 0.132|x4: 0.182|x5: 0.250|x6: 0.018|x7: 0.124|x8: 0.205|x9: 0.075|x10: 0.062|x11: 0.048|x12: 0.067|x13: 0.149|x14: 0.048|x15: 0.119|x16: 0.104|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.061|x4: 0.064|x5: 0.068|x6: 0.054|x7: 0.060|x8: 0.065|x9: 0.057|x10: 0.057|x11: 0.056|x12: 0.057|x13: 0.062|x14: 0.056|x15: 0.060|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -2305,8 +2368,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.388|x4: 0.000|x5: 0.365|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.224|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.339|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.113|x3: 0.000|x4: 0.332|x5: 0.381|x6: 0.000|x7: 0.148|x8: 0.113|x9: 0.216|x10: 0.000|x11: 0.068|x12: 0.000|x13: 0.000|x14: 0.176|x15: 0.099|x16: 0.175|x17: 0.000
-TOP2VEC -&gt; x1: 0.101|x2: 0.000|x3: 0.078|x4: 0.167|x5: 0.517|x6: 0.236|x7: 0.000|x8: 0.124|x9: 0.000|x10: 0.088|x11: 0.132|x12: 0.178|x13: 0.055|x14: 0.233|x15: 0.000|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.038|x3: 0.155|x4: 0.166|x5: 0.421|x6: 0.079|x7: 0.049|x8: 0.079|x9: 0.072|x10: 0.029|x11: 0.141|x12: 0.059|x13: 0.018|x14: 0.136|x15: 0.033|x16: 0.231|x17: 0.000
+TOP2VEC -&gt; x1: 0.101|x2: 0.000|x3: 0.078|x4: 0.167|x5: 0.517|x6: 0.236|x7: 0.000|x8: 0.125|x9: 0.000|x10: 0.088|x11: 0.132|x12: 0.178|x13: 0.055|x14: 0.232|x15: 0.000|x16: 0.179|x17: 0.000
+MEAN -&gt; x1: 0.034|x2: 0.038|x3: 0.155|x4: 0.166|x5: 0.415|x6: 0.079|x7: 0.049|x8: 0.079|x9: 0.072|x10: 0.029|x11: 0.141|x12: 0.059|x13: 0.018|x14: 0.136|x15: 0.033|x16: 0.231|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.062|x5: 0.080|x6: 0.057|x7: 0.056|x8: 0.057|x9: 0.057|x10: 0.054|x11: 0.061|x12: 0.056|x13: 0.054|x14: 0.061|x15: 0.055|x16: 0.067|x17: 0.053
 </t>
         </is>
       </c>
@@ -2327,15 +2391,16 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>[3, 7, 9]</t>
+          <t>[3, 9]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.278|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.087|x10: 0.180|x11: 0.157|x12: 0.073|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.248|x3: 0.236|x4: 0.065|x5: 0.064|x6: 0.000|x7: 0.147|x8: 0.000|x9: 0.152|x10: 0.288|x11: 0.000|x12: 0.193|x13: 0.000|x14: 0.125|x15: 0.000|x16: 0.302|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.088|x3: 0.332|x4: 0.432|x5: 0.178|x6: 0.107|x7: 0.359|x8: 0.174|x9: 0.460|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.153|x14: 0.288|x15: 0.173|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.112|x3: 0.282|x4: 0.166|x5: 0.081|x6: 0.036|x7: 0.169|x8: 0.058|x9: 0.233|x10: 0.156|x11: 0.052|x12: 0.089|x13: 0.051|x14: 0.138|x15: 0.058|x16: 0.101|x17: 0.000
+TOP2VEC -&gt; x1: 0.107|x2: 0.088|x3: 0.332|x4: 0.432|x5: 0.177|x6: 0.107|x7: 0.359|x8: 0.174|x9: 0.460|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.153|x14: 0.288|x15: 0.173|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.112|x3: 0.282|x4: 0.166|x5: 0.081|x6: 0.036|x7: 0.168|x8: 0.058|x9: 0.233|x10: 0.156|x11: 0.052|x12: 0.089|x13: 0.051|x14: 0.138|x15: 0.058|x16: 0.101|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.070|x4: 0.062|x5: 0.057|x6: 0.055|x7: 0.062|x8: 0.056|x9: 0.067|x10: 0.062|x11: 0.056|x12: 0.058|x13: 0.055|x14: 0.061|x15: 0.056|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -2364,7 +2429,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.750|x4: 0.055|x5: 0.067|x6: 0.092|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.200|x11: 0.330|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.085|x17: 0.000
 LDA -&gt; x1: 0.164|x2: 0.199|x3: 0.113|x4: 0.355|x5: 0.145|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.074|x10: 0.000|x11: 0.144|x12: 0.165|x13: 0.000|x14: 0.153|x15: 0.000|x16: 0.308|x17: 0.000
 TOP2VEC -&gt; x1: 0.137|x2: 0.296|x3: 0.164|x4: 0.218|x5: 0.178|x6: 0.121|x7: 0.188|x8: 0.200|x9: 0.206|x10: 0.120|x11: 0.056|x12: 0.151|x13: 0.000|x14: 0.184|x15: 0.072|x16: 0.246|x17: 0.000
-MEAN -&gt; x1: 0.100|x2: 0.165|x3: 0.342|x4: 0.210|x5: 0.130|x6: 0.071|x7: 0.063|x8: 0.067|x9: 0.093|x10: 0.107|x11: 0.177|x12: 0.105|x13: 0.000|x14: 0.112|x15: 0.024|x16: 0.213|x17: 0.000
+MEAN -&gt; x1: 0.100|x2: 0.165|x3: 0.259|x4: 0.210|x5: 0.130|x6: 0.071|x7: 0.063|x8: 0.067|x9: 0.093|x10: 0.107|x11: 0.177|x12: 0.105|x13: 0.000|x14: 0.112|x15: 0.024|x16: 0.213|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.062|x3: 0.068|x4: 0.065|x5: 0.060|x6: 0.056|x7: 0.056|x8: 0.056|x9: 0.058|x10: 0.058|x11: 0.063|x12: 0.058|x13: 0.052|x14: 0.059|x15: 0.054|x16: 0.065|x17: 0.052
 </t>
         </is>
       </c>
@@ -2393,7 +2459,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.314|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.233|x12: 0.000|x13: 0.000|x14: 0.082|x15: 0.398|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.237|x3: 0.127|x4: 0.136|x5: 0.000|x6: 0.199|x7: 0.000|x8: 0.250|x9: 0.000|x10: 0.061|x11: 0.080|x12: 0.000|x13: 0.000|x14: 0.105|x15: 0.625|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.182|x3: 0.000|x4: 0.054|x5: 0.000|x6: 0.134|x7: 0.170|x8: 0.000|x9: 0.198|x10: 0.000|x11: 0.135|x12: 0.288|x13: 0.153|x14: 0.207|x15: 0.330|x16: 0.105|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.139|x3: 0.147|x4: 0.063|x5: 0.000|x6: 0.111|x7: 0.057|x8: 0.083|x9: 0.066|x10: 0.020|x11: 0.149|x12: 0.096|x13: 0.051|x14: 0.131|x15: 0.451|x16: 0.035|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.139|x3: 0.147|x4: 0.063|x5: 0.000|x6: 0.111|x7: 0.057|x8: 0.083|x9: 0.066|x10: 0.020|x11: 0.149|x12: 0.096|x13: 0.051|x14: 0.131|x15: 0.409|x16: 0.035|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.061|x3: 0.062|x4: 0.057|x5: 0.053|x6: 0.060|x7: 0.057|x8: 0.058|x9: 0.057|x10: 0.055|x11: 0.062|x12: 0.059|x13: 0.056|x14: 0.061|x15: 0.080|x16: 0.055|x17: 0.053
 </t>
         </is>
       </c>
@@ -2414,7 +2481,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>[3, 6, 11, 12, 13, 16]</t>
+          <t>[3, 6, 12, 13]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2422,7 +2489,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.080|x2: 0.000|x3: 0.510|x4: 0.000|x5: 0.000|x6: 0.224|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.057|x2: 0.061|x3: 0.144|x4: 0.104|x5: 0.117|x6: 0.149|x7: 0.134|x8: 0.000|x9: 0.121|x10: 0.000|x11: 0.075|x12: 0.144|x13: 0.152|x14: 0.200|x15: 0.119|x16: 0.242|x17: 0.000
 TOP2VEC -&gt; x1: 0.157|x2: 0.163|x3: 0.000|x4: 0.164|x5: 0.074|x6: 0.279|x7: 0.290|x8: 0.103|x9: 0.100|x10: 0.123|x11: 0.208|x12: 0.492|x13: 0.478|x14: 0.338|x15: 0.207|x16: 0.251|x17: 0.000
-MEAN -&gt; x1: 0.098|x2: 0.075|x3: 0.218|x4: 0.089|x5: 0.064|x6: 0.217|x7: 0.141|x8: 0.034|x9: 0.074|x10: 0.041|x11: 0.197|x12: 0.212|x13: 0.210|x14: 0.179|x15: 0.109|x16: 0.164|x17: 0.000
+MEAN -&gt; x1: 0.098|x2: 0.075|x3: 0.215|x4: 0.089|x5: 0.064|x6: 0.217|x7: 0.141|x8: 0.034|x9: 0.074|x10: 0.041|x11: 0.197|x12: 0.212|x13: 0.210|x14: 0.179|x15: 0.109|x16: 0.164|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.064|x4: 0.057|x5: 0.055|x6: 0.064|x7: 0.060|x8: 0.054|x9: 0.056|x10: 0.054|x11: 0.063|x12: 0.064|x13: 0.064|x14: 0.062|x15: 0.058|x16: 0.061|x17: 0.052
 </t>
         </is>
       </c>
@@ -2443,15 +2511,16 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[6, 13, 14, 15]</t>
+          <t>[6, 14, 15]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.297|x4: 0.000|x5: 0.000|x6: 0.290|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.157|x11: 0.172|x12: 0.000|x13: 0.000|x14: 0.163|x15: 0.345|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.110|x3: 0.116|x4: 0.000|x5: 0.056|x6: 0.298|x7: 0.000|x8: 0.122|x9: 0.109|x10: 0.209|x11: 0.087|x12: 0.000|x13: 0.109|x14: 0.295|x15: 0.309|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.120|x2: 0.151|x3: 0.000|x4: 0.236|x5: 0.259|x6: 0.425|x7: 0.247|x8: 0.072|x9: 0.133|x10: 0.000|x11: 0.292|x12: 0.200|x13: 0.425|x14: 0.378|x15: 0.384|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.120|x2: 0.151|x3: 0.000|x4: 0.236|x5: 0.259|x6: 0.425|x7: 0.247|x8: 0.072|x9: 0.134|x10: 0.000|x11: 0.293|x12: 0.201|x13: 0.425|x14: 0.378|x15: 0.384|x16: 0.000|x17: 0.000
 MEAN -&gt; x1: 0.040|x2: 0.087|x3: 0.138|x4: 0.079|x5: 0.105|x6: 0.338|x7: 0.082|x8: 0.065|x9: 0.081|x10: 0.122|x11: 0.184|x12: 0.067|x13: 0.178|x14: 0.279|x15: 0.346|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.059|x4: 0.056|x5: 0.057|x6: 0.072|x7: 0.056|x8: 0.055|x9: 0.056|x10: 0.058|x11: 0.062|x12: 0.055|x13: 0.061|x14: 0.068|x15: 0.073|x16: 0.051|x17: 0.051
 </t>
         </is>
       </c>
@@ -2481,6 +2550,7 @@
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.155|x4: 0.111|x5: 0.116|x6: 0.055|x7: 0.248|x8: 0.112|x9: 0.128|x10: 0.000|x11: 0.141|x12: 0.000|x13: 0.169|x14: 0.125|x15: 0.387|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.136|x2: 0.107|x3: 0.066|x4: 0.298|x5: 0.309|x6: 0.174|x7: 0.375|x8: 0.137|x9: 0.116|x10: 0.000|x11: 0.244|x12: 0.410|x13: 0.237|x14: 0.184|x15: 0.162|x16: 0.088|x17: 0.000
 MEAN -&gt; x1: 0.045|x2: 0.059|x3: 0.216|x4: 0.136|x5: 0.142|x6: 0.076|x7: 0.208|x8: 0.083|x9: 0.081|x10: 0.000|x11: 0.211|x12: 0.137|x13: 0.157|x14: 0.133|x15: 0.232|x16: 0.029|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.056|x3: 0.065|x4: 0.060|x5: 0.060|x6: 0.056|x7: 0.064|x8: 0.057|x9: 0.057|x10: 0.052|x11: 0.065|x12: 0.060|x13: 0.061|x14: 0.060|x15: 0.066|x16: 0.054|x17: 0.052
 </t>
         </is>
       </c>
@@ -2501,15 +2571,16 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>[3, 6, 14, 15]</t>
+          <t>[3, 6, 15]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.431|x4: 0.000|x5: 0.000|x6: 0.803|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.322|x12: 0.000|x13: 0.000|x14: 0.093|x15: 0.086|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.157|x4: 0.000|x5: 0.111|x6: 0.296|x7: 0.000|x8: 0.098|x9: 0.155|x10: 0.093|x11: 0.138|x12: 0.093|x13: 0.116|x14: 0.135|x15: 0.248|x16: 0.180|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.249|x3: 0.090|x4: 0.267|x5: 0.213|x6: 0.000|x7: 0.133|x8: 0.097|x9: 0.000|x10: 0.094|x11: 0.000|x12: 0.280|x13: 0.193|x14: 0.368|x15: 0.273|x16: 0.192|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.083|x3: 0.226|x4: 0.089|x5: 0.108|x6: 0.366|x7: 0.044|x8: 0.065|x9: 0.052|x10: 0.062|x11: 0.153|x12: 0.124|x13: 0.103|x14: 0.199|x15: 0.202|x16: 0.124|x17: 0.000
+TOP2VEC -&gt; x1: 0.107|x2: 0.248|x3: 0.090|x4: 0.267|x5: 0.213|x6: 0.000|x7: 0.133|x8: 0.097|x9: 0.000|x10: 0.094|x11: 0.000|x12: 0.280|x13: 0.193|x14: 0.368|x15: 0.273|x16: 0.192|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.083|x3: 0.226|x4: 0.089|x5: 0.108|x6: 0.265|x7: 0.044|x8: 0.065|x9: 0.052|x10: 0.062|x11: 0.153|x12: 0.124|x13: 0.103|x14: 0.199|x15: 0.202|x16: 0.124|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.066|x4: 0.057|x5: 0.058|x6: 0.068|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.056|x11: 0.061|x12: 0.059|x13: 0.058|x14: 0.064|x15: 0.064|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -2530,15 +2601,16 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 12, 16]</t>
+          <t>[4, 16]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.424|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.245|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.080|x3: 0.000|x4: 0.326|x5: 0.000|x6: 0.079|x7: 0.126|x8: 0.000|x9: 0.084|x10: 0.000|x11: 0.000|x12: 0.338|x13: 0.000|x14: 0.223|x15: 0.074|x16: 0.491|x17: 0.000
-TOP2VEC -&gt; x1: 0.170|x2: 0.155|x3: 0.109|x4: 0.321|x5: 0.372|x6: 0.216|x7: 0.369|x8: 0.192|x9: 0.161|x10: 0.099|x11: 0.000|x12: 0.231|x13: 0.224|x14: 0.000|x15: 0.122|x16: 0.202|x17: 0.000
+TOP2VEC -&gt; x1: 0.170|x2: 0.155|x3: 0.109|x4: 0.321|x5: 0.372|x6: 0.215|x7: 0.369|x8: 0.192|x9: 0.161|x10: 0.099|x11: 0.000|x12: 0.231|x13: 0.224|x14: 0.000|x15: 0.122|x16: 0.202|x17: 0.000
 MEAN -&gt; x1: 0.057|x2: 0.078|x3: 0.177|x4: 0.216|x5: 0.124|x6: 0.098|x7: 0.165|x8: 0.064|x9: 0.082|x10: 0.033|x11: 0.082|x12: 0.190|x13: 0.075|x14: 0.074|x15: 0.065|x16: 0.231|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.063|x4: 0.065|x5: 0.060|x6: 0.058|x7: 0.062|x8: 0.056|x9: 0.057|x10: 0.055|x11: 0.057|x12: 0.064|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.066|x17: 0.053
 </t>
         </is>
       </c>
@@ -2559,7 +2631,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>[4, 9, 16]</t>
+          <t>[4, 9]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2567,7 +2639,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.367|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.069|x8: 0.121|x9: 0.163|x10: 0.101|x11: 0.212|x12: 0.000|x13: 0.070|x14: 0.069|x15: 0.000|x16: 0.056|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.179|x3: 0.051|x4: 0.218|x5: 0.000|x6: 0.000|x7: 0.073|x8: 0.195|x9: 0.272|x10: 0.238|x11: 0.000|x12: 0.130|x13: 0.079|x14: 0.163|x15: 0.000|x16: 0.222|x17: 0.000
 TOP2VEC -&gt; x1: 0.159|x2: 0.227|x3: 0.000|x4: 0.406|x5: 0.236|x6: 0.000|x7: 0.080|x8: 0.212|x9: 0.262|x10: 0.102|x11: 0.000|x12: 0.185|x13: 0.146|x14: 0.118|x15: 0.000|x16: 0.208|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.135|x3: 0.139|x4: 0.208|x5: 0.079|x6: 0.000|x7: 0.074|x8: 0.176|x9: 0.232|x10: 0.147|x11: 0.071|x12: 0.105|x13: 0.099|x14: 0.117|x15: 0.000|x16: 0.162|x17: 0.000
+MEAN -&gt; x1: 0.053|x2: 0.135|x3: 0.139|x4: 0.208|x5: 0.079|x6: 0.000|x7: 0.074|x8: 0.176|x9: 0.232|x10: 0.147|x11: 0.071|x12: 0.105|x13: 0.098|x14: 0.117|x15: 0.000|x16: 0.162|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.061|x4: 0.065|x5: 0.057|x6: 0.053|x7: 0.057|x8: 0.063|x9: 0.067|x10: 0.061|x11: 0.057|x12: 0.059|x13: 0.058|x14: 0.059|x15: 0.053|x16: 0.062|x17: 0.053
 </t>
         </is>
       </c>
@@ -2588,15 +2661,16 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>[3, 8]</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.209|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.448|x9: 0.000|x10: 0.000|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.201|x4: 0.117|x5: 0.000|x6: 0.000|x7: 0.129|x8: 0.245|x9: 0.167|x10: 0.216|x11: 0.000|x12: 0.146|x13: 0.000|x14: 0.262|x15: 0.153|x16: 0.183|x17: 0.000
-TOP2VEC -&gt; x1: 0.124|x2: 0.373|x3: 0.000|x4: 0.200|x5: 0.353|x6: 0.116|x7: 0.110|x8: 0.199|x9: 0.241|x10: 0.081|x11: 0.000|x12: 0.194|x13: 0.000|x14: 0.175|x15: 0.000|x16: 0.165|x17: 0.000
+TOP2VEC -&gt; x1: 0.124|x2: 0.373|x3: 0.000|x4: 0.199|x5: 0.353|x6: 0.116|x7: 0.110|x8: 0.199|x9: 0.241|x10: 0.081|x11: 0.000|x12: 0.194|x13: 0.000|x14: 0.175|x15: 0.000|x16: 0.165|x17: 0.000
 MEAN -&gt; x1: 0.041|x2: 0.124|x3: 0.137|x4: 0.105|x5: 0.118|x6: 0.039|x7: 0.080|x8: 0.297|x9: 0.136|x10: 0.099|x11: 0.040|x12: 0.113|x13: 0.000|x14: 0.146|x15: 0.051|x16: 0.116|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.061|x4: 0.059|x5: 0.060|x6: 0.055|x7: 0.058|x8: 0.072|x9: 0.061|x10: 0.059|x11: 0.055|x12: 0.060|x13: 0.053|x14: 0.062|x15: 0.056|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -2617,15 +2691,16 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[7, 12, 13, 14, 16]</t>
+          <t>[12, 16]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.466|x4: 0.000|x5: 0.054|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.054|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.098|x3: 0.084|x4: 0.240|x5: 0.170|x6: 0.000|x7: 0.134|x8: 0.114|x9: 0.067|x10: 0.000|x11: 0.000|x12: 0.220|x13: 0.133|x14: 0.236|x15: 0.000|x16: 0.323|x17: 0.000
-TOP2VEC -&gt; x1: 0.128|x2: 0.261|x3: 0.000|x4: 0.079|x5: 0.268|x6: 0.200|x7: 0.356|x8: 0.104|x9: 0.164|x10: 0.111|x11: 0.132|x12: 0.497|x13: 0.360|x14: 0.213|x15: 0.000|x16: 0.226|x17: 0.000
+TOP2VEC -&gt; x1: 0.128|x2: 0.261|x3: 0.000|x4: 0.079|x5: 0.268|x6: 0.200|x7: 0.356|x8: 0.104|x9: 0.164|x10: 0.110|x11: 0.132|x12: 0.497|x13: 0.360|x14: 0.212|x15: 0.000|x16: 0.226|x17: 0.000
 MEAN -&gt; x1: 0.043|x2: 0.120|x3: 0.183|x4: 0.106|x5: 0.164|x6: 0.067|x7: 0.163|x8: 0.073|x9: 0.077|x10: 0.037|x11: 0.134|x12: 0.239|x13: 0.164|x14: 0.150|x15: 0.000|x16: 0.201|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.063|x4: 0.058|x5: 0.062|x6: 0.056|x7: 0.062|x8: 0.056|x9: 0.057|x10: 0.054|x11: 0.060|x12: 0.067|x13: 0.062|x14: 0.061|x15: 0.052|x16: 0.064|x17: 0.052
 </t>
         </is>
       </c>
@@ -2646,7 +2721,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>[3, 4, 8]</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2655,6 +2730,7 @@
 LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.327|x4: 0.237|x5: 0.000|x6: 0.000|x7: 0.182|x8: 0.491|x9: 0.000|x10: 0.268|x11: 0.000|x12: 0.000|x13: 0.119|x14: 0.000|x15: 0.000|x16: 0.075|x17: 0.000
 TOP2VEC -&gt; x1: 0.197|x2: 0.000|x3: 0.227|x4: 0.211|x5: 0.421|x6: 0.000|x7: 0.000|x8: 0.245|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.193|x13: 0.000|x14: 0.000|x15: 0.063|x16: 0.078|x17: 0.000
 MEAN -&gt; x1: 0.066|x2: 0.041|x3: 0.245|x4: 0.181|x5: 0.140|x6: 0.000|x7: 0.061|x8: 0.337|x9: 0.000|x10: 0.089|x11: 0.032|x12: 0.064|x13: 0.040|x14: 0.000|x15: 0.021|x16: 0.051|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.069|x4: 0.065|x5: 0.062|x6: 0.054|x7: 0.057|x8: 0.076|x9: 0.054|x10: 0.059|x11: 0.056|x12: 0.058|x13: 0.056|x14: 0.054|x15: 0.055|x16: 0.057|x17: 0.054
 </t>
         </is>
       </c>
@@ -2675,15 +2751,16 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>[3, 5, 9, 13, 14]</t>
+          <t>[3, 13, 14]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.678|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.392|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.058|x3: 0.215|x4: 0.000|x5: 0.190|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.111|x10: 0.248|x11: 0.000|x12: 0.068|x13: 0.345|x14: 0.413|x15: 0.000|x16: 0.172|x17: 0.000
-TOP2VEC -&gt; x1: 0.166|x2: 0.079|x3: 0.101|x4: 0.292|x5: 0.398|x6: 0.207|x7: 0.302|x8: 0.196|x9: 0.367|x10: 0.104|x11: 0.078|x12: 0.385|x13: 0.313|x14: 0.399|x15: 0.381|x16: 0.213|x17: 0.000
-MEAN -&gt; x1: 0.055|x2: 0.046|x3: 0.332|x4: 0.097|x5: 0.196|x6: 0.069|x7: 0.101|x8: 0.065|x9: 0.159|x10: 0.117|x11: 0.157|x12: 0.151|x13: 0.219|x14: 0.271|x15: 0.127|x16: 0.128|x17: 0.000
+TOP2VEC -&gt; x1: 0.166|x2: 0.080|x3: 0.101|x4: 0.292|x5: 0.398|x6: 0.207|x7: 0.302|x8: 0.196|x9: 0.367|x10: 0.104|x11: 0.078|x12: 0.386|x13: 0.313|x14: 0.399|x15: 0.381|x16: 0.213|x17: 0.000
+MEAN -&gt; x1: 0.055|x2: 0.046|x3: 0.272|x4: 0.097|x5: 0.196|x6: 0.069|x7: 0.101|x8: 0.065|x9: 0.159|x10: 0.117|x11: 0.157|x12: 0.151|x13: 0.219|x14: 0.271|x15: 0.127|x16: 0.128|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.054|x3: 0.068|x4: 0.057|x5: 0.063|x6: 0.055|x7: 0.057|x8: 0.055|x9: 0.060|x10: 0.058|x11: 0.060|x12: 0.060|x13: 0.064|x14: 0.067|x15: 0.058|x16: 0.058|x17: 0.051
 </t>
         </is>
       </c>
@@ -2704,7 +2781,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[3, 6, 9]</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2712,7 +2789,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.543|x4: 0.000|x5: 0.000|x6: 0.154|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.314|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.061|x3: 0.089|x4: 0.092|x5: 0.000|x6: 0.317|x7: 0.079|x8: 0.086|x9: 0.295|x10: 0.140|x11: 0.000|x12: 0.075|x13: 0.000|x14: 0.346|x15: 0.000|x16: 0.139|x17: 0.000
 TOP2VEC -&gt; x1: 0.174|x2: 0.265|x3: 0.000|x4: 0.126|x5: 0.077|x6: 0.247|x7: 0.419|x8: 0.194|x9: 0.215|x10: 0.000|x11: 0.197|x12: 0.386|x13: 0.269|x14: 0.138|x15: 0.066|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.092|x2: 0.109|x3: 0.211|x4: 0.072|x5: 0.026|x6: 0.239|x7: 0.166|x8: 0.093|x9: 0.170|x10: 0.047|x11: 0.170|x12: 0.154|x13: 0.090|x14: 0.161|x15: 0.022|x16: 0.081|x17: 0.000
+MEAN -&gt; x1: 0.092|x2: 0.109|x3: 0.196|x4: 0.073|x5: 0.026|x6: 0.239|x7: 0.166|x8: 0.093|x9: 0.170|x10: 0.047|x11: 0.170|x12: 0.154|x13: 0.090|x14: 0.161|x15: 0.022|x16: 0.081|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.059|x3: 0.064|x4: 0.056|x5: 0.054|x6: 0.067|x7: 0.062|x8: 0.058|x9: 0.062|x10: 0.055|x11: 0.062|x12: 0.061|x13: 0.057|x14: 0.062|x15: 0.054|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -2733,15 +2811,16 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>[3, 6, 7, 9, 11]</t>
+          <t>[7, 9, 11]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.361|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.205|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.214|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.223|x3: 0.136|x4: 0.099|x5: 0.000|x6: 0.126|x7: 0.437|x8: 0.000|x9: 0.354|x10: 0.000|x11: 0.141|x12: 0.056|x13: 0.083|x14: 0.000|x15: 0.000|x16: 0.061|x17: 0.000
-TOP2VEC -&gt; x1: 0.146|x2: 0.184|x3: 0.000|x4: 0.066|x5: 0.000|x6: 0.407|x7: 0.548|x8: 0.146|x9: 0.425|x10: 0.000|x11: 0.350|x12: 0.107|x13: 0.449|x14: 0.000|x15: 0.191|x16: 0.056|x17: 0.000
-MEAN -&gt; x1: 0.083|x2: 0.136|x3: 0.166|x4: 0.055|x5: 0.000|x6: 0.178|x7: 0.397|x8: 0.101|x9: 0.260|x10: 0.000|x11: 0.235|x12: 0.054|x13: 0.177|x14: 0.000|x15: 0.064|x16: 0.039|x17: 0.000
+TOP2VEC -&gt; x1: 0.147|x2: 0.184|x3: 0.000|x4: 0.066|x5: 0.000|x6: 0.407|x7: 0.548|x8: 0.146|x9: 0.425|x10: 0.000|x11: 0.350|x12: 0.107|x13: 0.449|x14: 0.000|x15: 0.191|x16: 0.056|x17: 0.000
+MEAN -&gt; x1: 0.083|x2: 0.136|x3: 0.166|x4: 0.055|x5: 0.000|x6: 0.178|x7: 0.381|x8: 0.101|x9: 0.260|x10: 0.000|x11: 0.235|x12: 0.054|x13: 0.177|x14: 0.000|x15: 0.064|x16: 0.039|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.062|x4: 0.055|x5: 0.052|x6: 0.062|x7: 0.076|x8: 0.058|x9: 0.068|x10: 0.052|x11: 0.066|x12: 0.055|x13: 0.062|x14: 0.052|x15: 0.056|x16: 0.054|x17: 0.052
 </t>
         </is>
       </c>
@@ -2770,7 +2849,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.302|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.084|x10: 0.000|x11: 1.006|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.127|x4: 0.082|x5: 0.000|x6: 0.000|x7: 0.121|x8: 0.193|x9: 0.457|x10: 0.103|x11: 0.272|x12: 0.125|x13: 0.070|x14: 0.091|x15: 0.000|x16: 0.178|x17: 0.000
 TOP2VEC -&gt; x1: 0.065|x2: 0.189|x3: 0.000|x4: 0.229|x5: 0.113|x6: 0.182|x7: 0.294|x8: 0.064|x9: 0.417|x10: 0.051|x11: 0.288|x12: 0.592|x13: 0.345|x14: 0.288|x15: 0.235|x16: 0.105|x17: 0.000
-MEAN -&gt; x1: 0.022|x2: 0.063|x3: 0.143|x4: 0.104|x5: 0.038|x6: 0.061|x7: 0.139|x8: 0.086|x9: 0.319|x10: 0.052|x11: 0.522|x12: 0.239|x13: 0.138|x14: 0.126|x15: 0.078|x16: 0.094|x17: 0.000
+MEAN -&gt; x1: 0.022|x2: 0.063|x3: 0.143|x4: 0.104|x5: 0.038|x6: 0.061|x7: 0.139|x8: 0.086|x9: 0.319|x10: 0.052|x11: 0.353|x12: 0.208|x13: 0.138|x14: 0.126|x15: 0.078|x16: 0.094|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.055|x3: 0.060|x4: 0.058|x5: 0.054|x6: 0.055|x7: 0.060|x8: 0.057|x9: 0.072|x10: 0.055|x11: 0.074|x12: 0.064|x13: 0.060|x14: 0.059|x15: 0.056|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -2798,8 +2878,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.285|x4: 0.000|x5: 0.000|x6: 0.738|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.294|x12: 0.147|x13: 0.083|x14: 0.059|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.191|x4: 0.160|x5: 0.068|x6: 0.345|x7: 0.090|x8: 0.000|x9: 0.146|x10: 0.000|x11: 0.181|x12: 0.153|x13: 0.000|x14: 0.117|x15: 0.152|x16: 0.217|x17: 0.000
-TOP2VEC -&gt; x1: 0.085|x2: 0.000|x3: 0.169|x4: 0.337|x5: 0.166|x6: 0.314|x7: 0.407|x8: 0.105|x9: 0.227|x10: 0.078|x11: 0.476|x12: 0.365|x13: 0.166|x14: 0.217|x15: 0.274|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.000|x3: 0.215|x4: 0.166|x5: 0.078|x6: 0.465|x7: 0.166|x8: 0.035|x9: 0.124|x10: 0.026|x11: 0.317|x12: 0.221|x13: 0.083|x14: 0.131|x15: 0.142|x16: 0.126|x17: 0.000
+TOP2VEC -&gt; x1: 0.085|x2: 0.000|x3: 0.168|x4: 0.337|x5: 0.166|x6: 0.314|x7: 0.406|x8: 0.105|x9: 0.227|x10: 0.078|x11: 0.476|x12: 0.365|x13: 0.166|x14: 0.217|x15: 0.274|x16: 0.160|x17: 0.000
+MEAN -&gt; x1: 0.028|x2: 0.000|x3: 0.215|x4: 0.165|x5: 0.078|x6: 0.386|x7: 0.166|x8: 0.035|x9: 0.124|x10: 0.026|x11: 0.317|x12: 0.221|x13: 0.083|x14: 0.131|x15: 0.142|x16: 0.126|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.051|x3: 0.064|x4: 0.060|x5: 0.055|x6: 0.075|x7: 0.060|x8: 0.053|x9: 0.058|x10: 0.053|x11: 0.070|x12: 0.064|x13: 0.056|x14: 0.058|x15: 0.059|x16: 0.058|x17: 0.051
 </t>
         </is>
       </c>
@@ -2820,7 +2901,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>[3, 4, 14]</t>
+          <t>[3, 14]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2829,6 +2910,7 @@
 LDA -&gt; x1: 0.000|x2: 0.154|x3: 0.262|x4: 0.410|x5: 0.000|x6: 0.000|x7: 0.091|x8: 0.000|x9: 0.339|x10: 0.000|x11: 0.000|x12: 0.080|x13: 0.000|x14: 0.348|x15: 0.000|x16: 0.136|x17: 0.000
 TOP2VEC -&gt; x1: 0.160|x2: 0.288|x3: 0.336|x4: 0.105|x5: 0.222|x6: 0.271|x7: 0.272|x8: 0.182|x9: 0.191|x10: 0.101|x11: 0.238|x12: 0.312|x13: 0.227|x14: 0.410|x15: 0.161|x16: 0.206|x17: 0.000
 MEAN -&gt; x1: 0.053|x2: 0.147|x3: 0.313|x4: 0.172|x5: 0.074|x6: 0.113|x7: 0.121|x8: 0.061|x9: 0.177|x10: 0.034|x11: 0.145|x12: 0.160|x13: 0.076|x14: 0.253|x15: 0.054|x16: 0.114|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.071|x4: 0.062|x5: 0.056|x6: 0.058|x7: 0.059|x8: 0.055|x9: 0.062|x10: 0.054|x11: 0.060|x12: 0.061|x13: 0.056|x14: 0.067|x15: 0.055|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -2856,8 +2938,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.068|x2: 0.000|x3: 0.286|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.312|x9: 0.108|x10: 0.000|x11: 0.170|x12: 0.000|x13: 0.115|x14: 0.107|x15: 0.000|x16: 0.061|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.062|x4: 0.058|x5: 0.117|x6: 0.000|x7: 0.066|x8: 0.287|x9: 0.248|x10: 0.153|x11: 0.000|x12: 0.108|x13: 0.099|x14: 0.403|x15: 0.000|x16: 0.218|x17: 0.000
-TOP2VEC -&gt; x1: 0.132|x2: 0.149|x3: 0.081|x4: 0.293|x5: 0.134|x6: 0.000|x7: 0.071|x8: 0.165|x9: 0.254|x10: 0.065|x11: 0.202|x12: 0.174|x13: 0.189|x14: 0.407|x15: 0.174|x16: 0.133|x17: 0.000
-MEAN -&gt; x1: 0.067|x2: 0.050|x3: 0.143|x4: 0.117|x5: 0.084|x6: 0.000|x7: 0.046|x8: 0.255|x9: 0.203|x10: 0.073|x11: 0.124|x12: 0.094|x13: 0.134|x14: 0.306|x15: 0.058|x16: 0.137|x17: 0.000
+TOP2VEC -&gt; x1: 0.132|x2: 0.149|x3: 0.081|x4: 0.293|x5: 0.134|x6: 0.000|x7: 0.071|x8: 0.165|x9: 0.254|x10: 0.065|x11: 0.202|x12: 0.174|x13: 0.189|x14: 0.408|x15: 0.174|x16: 0.133|x17: 0.000
+MEAN -&gt; x1: 0.067|x2: 0.050|x3: 0.143|x4: 0.117|x5: 0.084|x6: 0.000|x7: 0.046|x8: 0.255|x9: 0.203|x10: 0.073|x11: 0.124|x12: 0.094|x13: 0.134|x14: 0.306|x15: 0.058|x16: 0.138|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.061|x4: 0.059|x5: 0.057|x6: 0.052|x7: 0.055|x8: 0.068|x9: 0.064|x10: 0.056|x11: 0.059|x12: 0.058|x13: 0.060|x14: 0.071|x15: 0.056|x16: 0.060|x17: 0.052
 </t>
         </is>
       </c>
@@ -2878,15 +2961,16 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>[3, 4, 8]</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.448|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.114|x9: 0.000|x10: 0.000|x11: 0.259|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.135|x2: 0.253|x3: 0.118|x4: 0.220|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.427|x9: 0.000|x10: 0.386|x11: 0.000|x12: 0.000|x13: 0.193|x14: 0.087|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.056|x2: 0.000|x3: 0.170|x4: 0.278|x5: 0.342|x6: 0.095|x7: 0.222|x8: 0.090|x9: 0.110|x10: 0.081|x11: 0.057|x12: 0.322|x13: 0.000|x14: 0.114|x15: 0.140|x16: 0.165|x17: 0.000
-MEAN -&gt; x1: 0.063|x2: 0.084|x3: 0.246|x4: 0.166|x5: 0.114|x6: 0.032|x7: 0.074|x8: 0.210|x9: 0.037|x10: 0.156|x11: 0.105|x12: 0.107|x13: 0.064|x14: 0.067|x15: 0.047|x16: 0.055|x17: 0.000
+TOP2VEC -&gt; x1: 0.056|x2: 0.000|x3: 0.170|x4: 0.278|x5: 0.342|x6: 0.095|x7: 0.222|x8: 0.090|x9: 0.110|x10: 0.081|x11: 0.057|x12: 0.323|x13: 0.000|x14: 0.114|x15: 0.140|x16: 0.165|x17: 0.000
+MEAN -&gt; x1: 0.063|x2: 0.084|x3: 0.246|x4: 0.166|x5: 0.114|x6: 0.032|x7: 0.074|x8: 0.210|x9: 0.037|x10: 0.156|x11: 0.105|x12: 0.108|x13: 0.064|x14: 0.067|x15: 0.047|x16: 0.055|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.058|x3: 0.068|x4: 0.063|x5: 0.060|x6: 0.055|x7: 0.057|x8: 0.066|x9: 0.055|x10: 0.062|x11: 0.059|x12: 0.059|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -2907,7 +2991,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2915,7 +2999,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.640|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.370|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.243|x3: 0.059|x4: 0.218|x5: 0.248|x6: 0.000|x7: 0.173|x8: 0.000|x9: 0.161|x10: 0.000|x11: 0.074|x12: 0.115|x13: 0.000|x14: 0.163|x15: 0.097|x16: 0.269|x17: 0.000
 TOP2VEC -&gt; x1: 0.143|x2: 0.103|x3: 0.103|x4: 0.310|x5: 0.265|x6: 0.000|x7: 0.296|x8: 0.155|x9: 0.138|x10: 0.096|x11: 0.132|x12: 0.080|x13: 0.216|x14: 0.114|x15: 0.000|x16: 0.197|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.115|x3: 0.268|x4: 0.176|x5: 0.171|x6: 0.000|x7: 0.156|x8: 0.052|x9: 0.100|x10: 0.032|x11: 0.192|x12: 0.065|x13: 0.072|x14: 0.092|x15: 0.032|x16: 0.156|x17: 0.000
+MEAN -&gt; x1: 0.048|x2: 0.115|x3: 0.221|x4: 0.176|x5: 0.171|x6: 0.000|x7: 0.156|x8: 0.052|x9: 0.100|x10: 0.032|x11: 0.192|x12: 0.065|x13: 0.072|x14: 0.092|x15: 0.032|x16: 0.156|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.066|x4: 0.063|x5: 0.063|x6: 0.053|x7: 0.062|x8: 0.056|x9: 0.059|x10: 0.055|x11: 0.064|x12: 0.057|x13: 0.057|x14: 0.058|x15: 0.055|x16: 0.062|x17: 0.053
 </t>
         </is>
       </c>
@@ -2936,7 +3021,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2945,6 +3030,7 @@
 LDA -&gt; x1: 0.000|x2: 0.078|x3: 0.055|x4: 0.138|x5: 0.276|x6: 0.000|x7: 0.132|x8: 0.161|x9: 0.169|x10: 0.211|x11: 0.000|x12: 0.113|x13: 0.104|x14: 0.132|x15: 0.000|x16: 0.249|x17: 0.000
 TOP2VEC -&gt; x1: 0.058|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.170|x6: 0.130|x7: 0.210|x8: 0.097|x9: 0.313|x10: 0.092|x11: 0.277|x12: 0.221|x13: 0.110|x14: 0.169|x15: 0.168|x16: 0.188|x17: 0.000
 MEAN -&gt; x1: 0.019|x2: 0.026|x3: 0.145|x4: 0.046|x5: 0.183|x6: 0.043|x7: 0.114|x8: 0.086|x9: 0.161|x10: 0.101|x11: 0.174|x12: 0.111|x13: 0.071|x14: 0.100|x15: 0.056|x16: 0.146|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.056|x5: 0.064|x6: 0.056|x7: 0.060|x8: 0.058|x9: 0.063|x10: 0.059|x11: 0.064|x12: 0.060|x13: 0.057|x14: 0.059|x15: 0.057|x16: 0.062|x17: 0.054
 </t>
         </is>
       </c>
@@ -2965,7 +3051,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>[3, 5, 11, 15]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2973,7 +3059,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.145|x2: 0.000|x3: 0.403|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.795|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.076|x2: 0.108|x3: 0.167|x4: 0.000|x5: 0.247|x6: 0.000|x7: 0.000|x8: 0.156|x9: 0.000|x10: 0.080|x11: 0.485|x12: 0.000|x13: 0.000|x14: 0.138|x15: 0.288|x16: 0.075|x17: 0.000
 TOP2VEC -&gt; x1: 0.186|x2: 0.247|x3: 0.000|x4: 0.322|x5: 0.257|x6: 0.220|x7: 0.377|x8: 0.212|x9: 0.180|x10: 0.086|x11: 0.446|x12: 0.472|x13: 0.240|x14: 0.253|x15: 0.306|x16: 0.177|x17: 0.000
-MEAN -&gt; x1: 0.136|x2: 0.118|x3: 0.190|x4: 0.107|x5: 0.168|x6: 0.073|x7: 0.126|x8: 0.123|x9: 0.060|x10: 0.055|x11: 0.575|x12: 0.157|x13: 0.080|x14: 0.130|x15: 0.198|x16: 0.084|x17: 0.000
+MEAN -&gt; x1: 0.136|x2: 0.118|x3: 0.190|x4: 0.107|x5: 0.168|x6: 0.073|x7: 0.126|x8: 0.123|x9: 0.060|x10: 0.055|x11: 0.477|x12: 0.157|x13: 0.080|x14: 0.130|x15: 0.198|x16: 0.084|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.062|x4: 0.057|x5: 0.061|x6: 0.055|x7: 0.058|x8: 0.058|x9: 0.054|x10: 0.054|x11: 0.082|x12: 0.060|x13: 0.055|x14: 0.058|x15: 0.062|x16: 0.056|x17: 0.051
 </t>
         </is>
       </c>
@@ -2994,7 +3081,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -3002,7 +3089,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.523|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.335|x12: 0.000|x13: 0.103|x14: 0.000|x15: 0.000|x16: 0.094|x17: 0.000
 LDA -&gt; x1: 0.064|x2: 0.156|x3: 0.000|x4: 0.136|x5: 0.192|x6: 0.000|x7: 0.093|x8: 0.161|x9: 0.145|x10: 0.243|x11: 0.099|x12: 0.139|x13: 0.000|x14: 0.122|x15: 0.000|x16: 0.269|x17: 0.000
 TOP2VEC -&gt; x1: 0.152|x2: 0.000|x3: 0.000|x4: 0.270|x5: 0.209|x6: 0.349|x7: 0.061|x8: 0.176|x9: 0.153|x10: 0.064|x11: 0.108|x12: 0.381|x13: 0.187|x14: 0.264|x15: 0.142|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.072|x2: 0.052|x3: 0.174|x4: 0.135|x5: 0.134|x6: 0.116|x7: 0.052|x8: 0.113|x9: 0.099|x10: 0.102|x11: 0.181|x12: 0.173|x13: 0.097|x14: 0.129|x15: 0.047|x16: 0.165|x17: 0.000
+MEAN -&gt; x1: 0.072|x2: 0.052|x3: 0.167|x4: 0.135|x5: 0.134|x6: 0.116|x7: 0.052|x8: 0.113|x9: 0.100|x10: 0.102|x11: 0.181|x12: 0.173|x13: 0.097|x14: 0.129|x15: 0.047|x16: 0.165|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.062|x4: 0.060|x5: 0.060|x6: 0.059|x7: 0.056|x8: 0.059|x9: 0.058|x10: 0.058|x11: 0.063|x12: 0.063|x13: 0.058|x14: 0.060|x15: 0.055|x16: 0.062|x17: 0.053
 </t>
         </is>
       </c>
@@ -3023,7 +3111,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>[2, 3, 7, 11, 13]</t>
+          <t>[7, 11]</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -3031,7 +3119,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.425|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.385|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.087|x2: 0.221|x3: 0.172|x4: 0.160|x5: 0.159|x6: 0.000|x7: 0.424|x8: 0.057|x9: 0.112|x10: 0.090|x11: 0.083|x12: 0.000|x13: 0.204|x14: 0.000|x15: 0.000|x16: 0.051|x17: 0.000
 TOP2VEC -&gt; x1: 0.249|x2: 0.239|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.246|x7: 0.526|x8: 0.260|x9: 0.187|x10: 0.074|x11: 0.283|x12: 0.272|x13: 0.382|x14: 0.065|x15: 0.196|x16: 0.152|x17: 0.000
-MEAN -&gt; x1: 0.112|x2: 0.153|x3: 0.199|x4: 0.053|x5: 0.053|x6: 0.082|x7: 0.317|x8: 0.106|x9: 0.100|x10: 0.055|x11: 0.250|x12: 0.091|x13: 0.195|x14: 0.022|x15: 0.065|x16: 0.068|x17: 0.000
+MEAN -&gt; x1: 0.112|x2: 0.153|x3: 0.199|x4: 0.053|x5: 0.053|x6: 0.082|x7: 0.308|x8: 0.106|x9: 0.100|x10: 0.055|x11: 0.250|x12: 0.091|x13: 0.195|x14: 0.022|x15: 0.065|x16: 0.068|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.061|x3: 0.064|x4: 0.055|x5: 0.055|x6: 0.057|x7: 0.071|x8: 0.058|x9: 0.058|x10: 0.055|x11: 0.067|x12: 0.057|x13: 0.064|x14: 0.054|x15: 0.056|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3059,8 +3148,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.299|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.080|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.099|x3: 0.324|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.109|x8: 0.065|x9: 0.198|x10: 0.136|x11: 0.649|x12: 0.057|x13: 0.087|x14: 0.000|x15: 0.000|x16: 0.096|x17: 0.000
-TOP2VEC -&gt; x1: 0.064|x2: 0.000|x3: 0.107|x4: 0.239|x5: 0.000|x6: 0.203|x7: 0.314|x8: 0.066|x9: 0.217|x10: 0.067|x11: 0.495|x12: 0.263|x13: 0.209|x14: 0.064|x15: 0.167|x16: 0.137|x17: 0.000
-MEAN -&gt; x1: 0.021|x2: 0.033|x3: 0.243|x4: 0.080|x5: 0.000|x6: 0.068|x7: 0.141|x8: 0.044|x9: 0.138|x10: 0.068|x11: 0.741|x12: 0.106|x13: 0.099|x14: 0.021|x15: 0.056|x16: 0.078|x17: 0.000
+TOP2VEC -&gt; x1: 0.064|x2: 0.000|x3: 0.107|x4: 0.239|x5: 0.000|x6: 0.203|x7: 0.314|x8: 0.066|x9: 0.217|x10: 0.067|x11: 0.495|x12: 0.263|x13: 0.210|x14: 0.064|x15: 0.167|x16: 0.137|x17: 0.000
+MEAN -&gt; x1: 0.021|x2: 0.033|x3: 0.243|x4: 0.080|x5: 0.000|x6: 0.068|x7: 0.141|x8: 0.044|x9: 0.138|x10: 0.068|x11: 0.498|x12: 0.106|x13: 0.099|x14: 0.021|x15: 0.056|x16: 0.078|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.055|x3: 0.067|x4: 0.057|x5: 0.053|x6: 0.057|x7: 0.061|x8: 0.055|x9: 0.061|x10: 0.057|x11: 0.087|x12: 0.059|x13: 0.058|x14: 0.054|x15: 0.056|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -3081,7 +3171,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3090,6 +3180,7 @@
 LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.000|x4: 0.099|x5: 0.000|x6: 0.000|x7: 0.132|x8: 0.314|x9: 0.227|x10: 0.077|x11: 0.069|x12: 0.116|x13: 0.000|x14: 0.468|x15: 0.000|x16: 0.196|x17: 0.000
 TOP2VEC -&gt; x1: 0.197|x2: 0.143|x3: 0.000|x4: 0.361|x5: 0.281|x6: 0.142|x7: 0.260|x8: 0.266|x9: 0.118|x10: 0.093|x11: 0.152|x12: 0.295|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.191|x17: 0.000
 MEAN -&gt; x1: 0.066|x2: 0.088|x3: 0.117|x4: 0.153|x5: 0.094|x6: 0.047|x7: 0.130|x8: 0.194|x9: 0.115|x10: 0.057|x11: 0.143|x12: 0.137|x13: 0.000|x14: 0.156|x15: 0.000|x16: 0.129|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.058|x3: 0.060|x4: 0.062|x5: 0.059|x6: 0.056|x7: 0.061|x8: 0.065|x9: 0.060|x10: 0.056|x11: 0.062|x12: 0.061|x13: 0.053|x14: 0.062|x15: 0.053|x16: 0.061|x17: 0.053
 </t>
         </is>
       </c>
@@ -3110,15 +3201,16 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 6, 7, 9, 11]</t>
+          <t>[6, 7, 9, 11]</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.706|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.408|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.135|x3: 0.063|x4: 0.311|x5: 0.093|x6: 0.403|x7: 0.106|x8: 0.000|x9: 0.395|x10: 0.126|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.128|x16: 0.062|x17: 0.000
-TOP2VEC -&gt; x1: 0.161|x2: 0.432|x3: 0.000|x4: 0.272|x5: 0.145|x6: 0.341|x7: 0.622|x8: 0.183|x9: 0.410|x10: 0.066|x11: 0.360|x12: 0.210|x13: 0.367|x14: 0.000|x15: 0.126|x16: 0.135|x17: 0.000
-MEAN -&gt; x1: 0.054|x2: 0.189|x3: 0.256|x4: 0.194|x5: 0.079|x6: 0.248|x7: 0.243|x8: 0.061|x9: 0.268|x10: 0.064|x11: 0.256|x12: 0.070|x13: 0.122|x14: 0.000|x15: 0.085|x16: 0.066|x17: 0.000
+TOP2VEC -&gt; x1: 0.161|x2: 0.432|x3: 0.000|x4: 0.272|x5: 0.145|x6: 0.342|x7: 0.622|x8: 0.183|x9: 0.410|x10: 0.066|x11: 0.360|x12: 0.210|x13: 0.367|x14: 0.000|x15: 0.126|x16: 0.135|x17: 0.000
+MEAN -&gt; x1: 0.054|x2: 0.189|x3: 0.188|x4: 0.194|x5: 0.079|x6: 0.248|x7: 0.202|x8: 0.061|x9: 0.268|x10: 0.064|x11: 0.256|x12: 0.070|x13: 0.122|x14: 0.000|x15: 0.085|x16: 0.066|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.062|x4: 0.063|x5: 0.056|x6: 0.066|x7: 0.063|x8: 0.055|x9: 0.068|x10: 0.055|x11: 0.067|x12: 0.055|x13: 0.058|x14: 0.052|x15: 0.056|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -3139,7 +3231,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>[3, 11, 13]</t>
+          <t>[3, 11]</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3147,7 +3239,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.614|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.529|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.063|x3: 0.280|x4: 0.163|x5: 0.181|x6: 0.000|x7: 0.111|x8: 0.073|x9: 0.111|x10: 0.059|x11: 0.287|x12: 0.000|x13: 0.204|x14: 0.053|x15: 0.157|x16: 0.080|x17: 0.000
 TOP2VEC -&gt; x1: 0.083|x2: 0.159|x3: 0.326|x4: 0.155|x5: 0.202|x6: 0.186|x7: 0.000|x8: 0.057|x9: 0.000|x10: 0.168|x11: 0.433|x12: 0.000|x13: 0.208|x14: 0.165|x15: 0.204|x16: 0.344|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.074|x3: 0.407|x4: 0.106|x5: 0.127|x6: 0.062|x7: 0.037|x8: 0.043|x9: 0.037|x10: 0.076|x11: 0.416|x12: 0.000|x13: 0.137|x14: 0.073|x15: 0.120|x16: 0.141|x17: 0.000
+MEAN -&gt; x1: 0.028|x2: 0.074|x3: 0.369|x4: 0.106|x5: 0.127|x6: 0.062|x7: 0.037|x8: 0.043|x9: 0.037|x10: 0.076|x11: 0.406|x12: 0.000|x13: 0.137|x14: 0.073|x15: 0.120|x16: 0.141|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.076|x4: 0.058|x5: 0.060|x6: 0.056|x7: 0.054|x8: 0.055|x9: 0.054|x10: 0.057|x11: 0.079|x12: 0.052|x13: 0.060|x14: 0.056|x15: 0.059|x16: 0.060|x17: 0.052
 </t>
         </is>
       </c>
@@ -3177,6 +3270,7 @@
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.174|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.124|x8: 0.072|x9: 0.467|x10: 0.000|x11: 0.145|x12: 0.099|x13: 0.202|x14: 0.368|x15: 0.000|x16: 0.168|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.189|x4: 0.257|x5: 0.296|x6: 0.162|x7: 0.000|x8: 0.074|x9: 0.330|x10: 0.122|x11: 0.493|x12: 0.350|x13: 0.106|x14: 0.392|x15: 0.250|x16: 0.249|x17: 0.000
 MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.215|x4: 0.086|x5: 0.099|x6: 0.054|x7: 0.115|x8: 0.049|x9: 0.325|x10: 0.041|x11: 0.261|x12: 0.150|x13: 0.103|x14: 0.276|x15: 0.083|x16: 0.139|x17: 0.000
+SOFTMAX -&gt; x1: 0.052|x2: 0.052|x3: 0.065|x4: 0.057|x5: 0.057|x6: 0.055|x7: 0.058|x8: 0.055|x9: 0.072|x10: 0.054|x11: 0.068|x12: 0.060|x13: 0.058|x14: 0.069|x15: 0.057|x16: 0.060|x17: 0.052
 </t>
         </is>
       </c>
@@ -3197,15 +3291,16 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>[5, 14]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.491|x4: 0.000|x5: 0.000|x6: 0.253|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.284|x12: 0.000|x13: 0.000|x14: 0.178|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.157|x3: 0.000|x4: 0.127|x5: 0.237|x6: 0.133|x7: 0.000|x8: 0.158|x9: 0.093|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.673|x15: 0.133|x16: 0.110|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.302|x3: 0.076|x4: 0.210|x5: 0.202|x6: 0.146|x7: 0.197|x8: 0.144|x9: 0.177|x10: 0.089|x11: 0.186|x12: 0.101|x13: 0.094|x14: 0.302|x15: 0.000|x16: 0.182|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.153|x3: 0.189|x4: 0.112|x5: 0.146|x6: 0.177|x7: 0.066|x8: 0.101|x9: 0.090|x10: 0.030|x11: 0.156|x12: 0.034|x13: 0.031|x14: 0.385|x15: 0.044|x16: 0.097|x17: 0.000
+TOP2VEC -&gt; x1: 0.107|x2: 0.303|x3: 0.076|x4: 0.210|x5: 0.202|x6: 0.147|x7: 0.197|x8: 0.144|x9: 0.177|x10: 0.089|x11: 0.186|x12: 0.101|x13: 0.094|x14: 0.302|x15: 0.000|x16: 0.182|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.153|x3: 0.189|x4: 0.112|x5: 0.146|x6: 0.177|x7: 0.066|x8: 0.101|x9: 0.090|x10: 0.030|x11: 0.156|x12: 0.034|x13: 0.031|x14: 0.327|x15: 0.044|x16: 0.097|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.064|x4: 0.059|x5: 0.061|x6: 0.063|x7: 0.056|x8: 0.058|x9: 0.058|x10: 0.054|x11: 0.062|x12: 0.055|x13: 0.054|x14: 0.073|x15: 0.055|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -3233,8 +3328,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.359|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.207|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.455|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.064|x2: 0.090|x3: 0.072|x4: 0.159|x5: 0.064|x6: 0.000|x7: 0.000|x8: 0.278|x9: 0.000|x10: 0.204|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.108|x15: 0.695|x16: 0.085|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.223|x3: 0.068|x4: 0.078|x5: 0.087|x6: 0.109|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.075|x11: 0.130|x12: 0.060|x13: 0.089|x14: 0.200|x15: 0.221|x16: 0.154|x17: 0.000
-MEAN -&gt; x1: 0.021|x2: 0.104|x3: 0.166|x4: 0.079|x5: 0.050|x6: 0.036|x7: 0.000|x8: 0.093|x9: 0.000|x10: 0.093|x11: 0.112|x12: 0.020|x13: 0.030|x14: 0.103|x15: 0.457|x16: 0.079|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.223|x3: 0.068|x4: 0.078|x5: 0.087|x6: 0.109|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.075|x11: 0.130|x12: 0.059|x13: 0.089|x14: 0.200|x15: 0.221|x16: 0.154|x17: 0.000
+MEAN -&gt; x1: 0.021|x2: 0.104|x3: 0.166|x4: 0.079|x5: 0.050|x6: 0.036|x7: 0.000|x8: 0.093|x9: 0.000|x10: 0.093|x11: 0.112|x12: 0.020|x13: 0.030|x14: 0.103|x15: 0.392|x16: 0.079|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.064|x4: 0.058|x5: 0.057|x6: 0.056|x7: 0.054|x8: 0.059|x9: 0.054|x10: 0.059|x11: 0.060|x12: 0.055|x13: 0.056|x14: 0.060|x15: 0.080|x16: 0.058|x17: 0.054
 </t>
         </is>
       </c>
@@ -3255,15 +3351,16 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 9, 11]</t>
+          <t>[3, 4, 7, 11]</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.553|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.139|x3: 0.191|x4: 0.379|x5: 0.134|x6: 0.000|x7: 0.176|x8: 0.120|x9: 0.260|x10: 0.077|x11: 0.068|x12: 0.000|x13: 0.189|x14: 0.000|x15: 0.000|x16: 0.086|x17: 0.000
-TOP2VEC -&gt; x1: 0.256|x2: 0.193|x3: 0.168|x4: 0.387|x5: 0.292|x6: 0.274|x7: 0.487|x8: 0.300|x9: 0.217|x10: 0.082|x11: 0.284|x12: 0.335|x13: 0.275|x14: 0.081|x15: 0.065|x16: 0.168|x17: 0.000
-MEAN -&gt; x1: 0.085|x2: 0.111|x3: 0.304|x4: 0.255|x5: 0.142|x6: 0.091|x7: 0.221|x8: 0.140|x9: 0.159|x10: 0.053|x11: 0.217|x12: 0.112|x13: 0.155|x14: 0.027|x15: 0.022|x16: 0.085|x17: 0.000
+TOP2VEC -&gt; x1: 0.256|x2: 0.193|x3: 0.168|x4: 0.387|x5: 0.292|x6: 0.275|x7: 0.487|x8: 0.300|x9: 0.217|x10: 0.082|x11: 0.284|x12: 0.335|x13: 0.275|x14: 0.081|x15: 0.065|x16: 0.168|x17: 0.000
+MEAN -&gt; x1: 0.085|x2: 0.111|x3: 0.286|x4: 0.255|x5: 0.142|x6: 0.092|x7: 0.221|x8: 0.140|x9: 0.159|x10: 0.053|x11: 0.217|x12: 0.112|x13: 0.155|x14: 0.027|x15: 0.022|x16: 0.085|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.067|x5: 0.060|x6: 0.057|x7: 0.064|x8: 0.059|x9: 0.061|x10: 0.054|x11: 0.064|x12: 0.058|x13: 0.060|x14: 0.053|x15: 0.053|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3284,7 +3381,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>[3, 5, 11, 14]</t>
+          <t>[3, 14]</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3292,7 +3389,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.454|x4: 0.000|x5: 0.000|x6: 0.053|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.263|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.094|x4: 0.074|x5: 0.264|x6: 0.114|x7: 0.000|x8: 0.146|x9: 0.158|x10: 0.070|x11: 0.000|x12: 0.080|x13: 0.150|x14: 0.311|x15: 0.148|x16: 0.210|x17: 0.000
 TOP2VEC -&gt; x1: 0.173|x2: 0.317|x3: 0.140|x4: 0.062|x5: 0.299|x6: 0.344|x7: 0.080|x8: 0.183|x9: 0.084|x10: 0.000|x11: 0.213|x12: 0.340|x13: 0.226|x14: 0.295|x15: 0.263|x16: 0.089|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.106|x3: 0.229|x4: 0.045|x5: 0.188|x6: 0.170|x7: 0.027|x8: 0.110|x9: 0.081|x10: 0.023|x11: 0.159|x12: 0.140|x13: 0.125|x14: 0.202|x15: 0.137|x16: 0.100|x17: 0.000
+MEAN -&gt; x1: 0.058|x2: 0.106|x3: 0.229|x4: 0.045|x5: 0.188|x6: 0.170|x7: 0.027|x8: 0.110|x9: 0.081|x10: 0.023|x11: 0.158|x12: 0.140|x13: 0.125|x14: 0.202|x15: 0.137|x16: 0.100|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.066|x4: 0.055|x5: 0.063|x6: 0.062|x7: 0.054|x8: 0.059|x9: 0.057|x10: 0.054|x11: 0.062|x12: 0.060|x13: 0.059|x14: 0.064|x15: 0.060|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3313,7 +3411,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>[3, 11, 13]</t>
+          <t>[3, 11]</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3321,7 +3419,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.643|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.412|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.081|x2: 0.000|x3: 0.238|x4: 0.149|x5: 0.128|x6: 0.000|x7: 0.149|x8: 0.187|x9: 0.165|x10: 0.000|x11: 0.236|x12: 0.000|x13: 0.241|x14: 0.056|x15: 0.114|x16: 0.076|x17: 0.000
 TOP2VEC -&gt; x1: 0.165|x2: 0.085|x3: 0.236|x4: 0.160|x5: 0.305|x6: 0.131|x7: 0.128|x8: 0.163|x9: 0.127|x10: 0.000|x11: 0.163|x12: 0.142|x13: 0.294|x14: 0.440|x15: 0.227|x16: 0.085|x17: 0.000
-MEAN -&gt; x1: 0.082|x2: 0.028|x3: 0.372|x4: 0.103|x5: 0.144|x6: 0.044|x7: 0.092|x8: 0.117|x9: 0.097|x10: 0.000|x11: 0.271|x12: 0.047|x13: 0.178|x14: 0.165|x15: 0.114|x16: 0.054|x17: 0.000
+MEAN -&gt; x1: 0.082|x2: 0.028|x3: 0.325|x4: 0.103|x5: 0.144|x6: 0.044|x7: 0.092|x8: 0.117|x9: 0.097|x10: 0.000|x11: 0.271|x12: 0.047|x13: 0.178|x14: 0.165|x15: 0.114|x16: 0.054|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.054|x3: 0.073|x4: 0.058|x5: 0.061|x6: 0.055|x7: 0.058|x8: 0.059|x9: 0.058|x10: 0.053|x11: 0.069|x12: 0.055|x13: 0.063|x14: 0.062|x15: 0.059|x16: 0.055|x17: 0.053
 </t>
         </is>
       </c>
@@ -3350,7 +3449,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.196|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 1.062|x10: 0.000|x11: 0.143|x12: 0.195|x13: 0.000|x14: 0.069|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.077|x4: 0.000|x5: 0.089|x6: 0.000|x7: 0.154|x8: 0.137|x9: 0.584|x10: 0.155|x11: 0.088|x12: 0.068|x13: 0.079|x14: 0.000|x15: 0.125|x16: 0.142|x17: 0.000
 TOP2VEC -&gt; x1: 0.118|x2: 0.118|x3: 0.000|x4: 0.284|x5: 0.000|x6: 0.126|x7: 0.200|x8: 0.192|x9: 0.499|x10: 0.070|x11: 0.300|x12: 0.508|x13: 0.160|x14: 0.000|x15: 0.083|x16: 0.144|x17: 0.000
-MEAN -&gt; x1: 0.039|x2: 0.080|x3: 0.091|x4: 0.095|x5: 0.030|x6: 0.042|x7: 0.118|x8: 0.110|x9: 0.715|x10: 0.075|x11: 0.177|x12: 0.257|x13: 0.080|x14: 0.023|x15: 0.069|x16: 0.095|x17: 0.000
+MEAN -&gt; x1: 0.039|x2: 0.080|x3: 0.091|x4: 0.095|x5: 0.030|x6: 0.042|x7: 0.118|x8: 0.110|x9: 0.500|x10: 0.075|x11: 0.177|x12: 0.254|x13: 0.080|x14: 0.023|x15: 0.069|x16: 0.095|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.057|x4: 0.057|x5: 0.054|x6: 0.055|x7: 0.059|x8: 0.058|x9: 0.086|x10: 0.056|x11: 0.062|x12: 0.067|x13: 0.057|x14: 0.054|x15: 0.056|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3371,7 +3471,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 13, 14]</t>
+          <t>[3, 11, 13]</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3379,7 +3479,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.553|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.320|x12: 0.000|x13: 0.947|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.063|x3: 0.292|x4: 0.193|x5: 0.000|x6: 0.000|x7: 0.055|x8: 0.170|x9: 0.204|x10: 0.000|x11: 0.080|x12: 0.073|x13: 0.344|x14: 0.232|x15: 0.000|x16: 0.115|x17: 0.000
 TOP2VEC -&gt; x1: 0.209|x2: 0.245|x3: 0.201|x4: 0.148|x5: 0.131|x6: 0.110|x7: 0.437|x8: 0.264|x9: 0.364|x10: 0.067|x11: 0.338|x12: 0.326|x13: 0.268|x14: 0.336|x15: 0.194|x16: 0.136|x17: 0.000
-MEAN -&gt; x1: 0.070|x2: 0.102|x3: 0.349|x4: 0.114|x5: 0.044|x6: 0.037|x7: 0.164|x8: 0.145|x9: 0.189|x10: 0.022|x11: 0.246|x12: 0.133|x13: 0.520|x14: 0.189|x15: 0.065|x16: 0.084|x17: 0.000
+MEAN -&gt; x1: 0.070|x2: 0.102|x3: 0.331|x4: 0.114|x5: 0.044|x6: 0.037|x7: 0.164|x8: 0.145|x9: 0.189|x10: 0.022|x11: 0.246|x12: 0.133|x13: 0.371|x14: 0.189|x15: 0.065|x16: 0.084|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.071|x4: 0.057|x5: 0.053|x6: 0.053|x7: 0.060|x8: 0.059|x9: 0.062|x10: 0.052|x11: 0.065|x12: 0.058|x13: 0.074|x14: 0.062|x15: 0.055|x16: 0.056|x17: 0.051
 </t>
         </is>
       </c>
@@ -3400,15 +3501,16 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>[4, 11, 12, 13, 14]</t>
+          <t>[4, 11, 12, 14]</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.452|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.261|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.099|x4: 0.194|x5: 0.000|x6: 0.000|x7: 0.093|x8: 0.156|x9: 0.345|x10: 0.000|x11: 0.000|x12: 0.165|x13: 0.156|x14: 0.391|x15: 0.000|x16: 0.222|x17: 0.000
-TOP2VEC -&gt; x1: 0.171|x2: 0.193|x3: 0.000|x4: 0.412|x5: 0.235|x6: 0.544|x7: 0.358|x8: 0.160|x9: 0.169|x10: 0.064|x11: 0.399|x12: 0.478|x13: 0.363|x14: 0.338|x15: 0.075|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.064|x3: 0.184|x4: 0.202|x5: 0.078|x6: 0.181|x7: 0.150|x8: 0.105|x9: 0.171|x10: 0.021|x11: 0.220|x12: 0.214|x13: 0.173|x14: 0.243|x15: 0.025|x16: 0.118|x17: 0.000
+TOP2VEC -&gt; x1: 0.171|x2: 0.194|x3: 0.000|x4: 0.412|x5: 0.235|x6: 0.544|x7: 0.358|x8: 0.160|x9: 0.169|x10: 0.064|x11: 0.399|x12: 0.478|x13: 0.363|x14: 0.338|x15: 0.075|x16: 0.131|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.065|x3: 0.184|x4: 0.202|x5: 0.078|x6: 0.167|x7: 0.151|x8: 0.105|x9: 0.171|x10: 0.021|x11: 0.220|x12: 0.214|x13: 0.173|x14: 0.243|x15: 0.025|x16: 0.118|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.063|x5: 0.056|x6: 0.061|x7: 0.060|x8: 0.057|x9: 0.061|x10: 0.053|x11: 0.064|x12: 0.064|x13: 0.061|x14: 0.066|x15: 0.053|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3429,15 +3531,16 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>[3, 6, 11, 14]</t>
+          <t>[11, 14]</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.121|x2: 0.000|x3: 0.359|x4: 0.000|x5: 0.000|x6: 0.217|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.208|x12: 0.000|x13: 0.000|x14: 0.541|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.158|x2: 0.184|x3: 0.101|x4: 0.081|x5: 0.125|x6: 0.172|x7: 0.077|x8: 0.000|x9: 0.289|x10: 0.000|x11: 0.104|x12: 0.000|x13: 0.119|x14: 0.344|x15: 0.000|x16: 0.065|x17: 0.000
-TOP2VEC -&gt; x1: 0.124|x2: 0.187|x3: 0.000|x4: 0.226|x5: 0.226|x6: 0.210|x7: 0.328|x8: 0.123|x9: 0.181|x10: 0.064|x11: 0.298|x12: 0.259|x13: 0.269|x14: 0.449|x15: 0.093|x16: 0.130|x17: 0.000
-MEAN -&gt; x1: 0.134|x2: 0.124|x3: 0.154|x4: 0.103|x5: 0.117|x6: 0.200|x7: 0.135|x8: 0.041|x9: 0.157|x10: 0.021|x11: 0.203|x12: 0.086|x13: 0.129|x14: 0.445|x15: 0.031|x16: 0.065|x17: 0.000
+TOP2VEC -&gt; x1: 0.123|x2: 0.186|x3: 0.000|x4: 0.226|x5: 0.226|x6: 0.210|x7: 0.328|x8: 0.123|x9: 0.181|x10: 0.064|x11: 0.298|x12: 0.259|x13: 0.269|x14: 0.449|x15: 0.093|x16: 0.130|x17: 0.000
+MEAN -&gt; x1: 0.134|x2: 0.124|x3: 0.154|x4: 0.103|x5: 0.117|x6: 0.200|x7: 0.135|x8: 0.041|x9: 0.157|x10: 0.021|x11: 0.203|x12: 0.086|x13: 0.129|x14: 0.431|x15: 0.031|x16: 0.065|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.060|x4: 0.057|x5: 0.058|x6: 0.063|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.053|x11: 0.063|x12: 0.056|x13: 0.059|x14: 0.079|x15: 0.053|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -3458,7 +3561,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>[13, 14, 15]</t>
+          <t>[14, 15]</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3466,7 +3569,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.182|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.152|x11: 0.105|x12: 0.000|x13: 0.057|x14: 0.549|x15: 0.168|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.150|x4: 0.070|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.158|x9: 0.000|x10: 0.000|x11: 0.064|x12: 0.077|x13: 0.204|x14: 0.443|x15: 0.523|x16: 0.132|x17: 0.000
 TOP2VEC -&gt; x1: 0.109|x2: 0.119|x3: 0.000|x4: 0.000|x5: 0.133|x6: 0.000|x7: 0.000|x8: 0.065|x9: 0.000|x10: 0.086|x11: 0.269|x12: 0.365|x13: 0.314|x14: 0.669|x15: 0.573|x16: 0.176|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.040|x3: 0.111|x4: 0.023|x5: 0.044|x6: 0.000|x7: 0.000|x8: 0.074|x9: 0.000|x10: 0.079|x11: 0.146|x12: 0.147|x13: 0.192|x14: 0.554|x15: 0.421|x16: 0.103|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.040|x3: 0.111|x4: 0.023|x5: 0.044|x6: 0.000|x7: 0.000|x8: 0.074|x9: 0.000|x10: 0.079|x11: 0.146|x12: 0.147|x13: 0.192|x14: 0.481|x15: 0.389|x16: 0.103|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.054|x3: 0.058|x4: 0.053|x5: 0.055|x6: 0.052|x7: 0.052|x8: 0.056|x9: 0.052|x10: 0.057|x11: 0.060|x12: 0.061|x13: 0.063|x14: 0.084|x15: 0.077|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3487,15 +3591,16 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>[3, 14]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.356|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.246|x12: 0.000|x13: 0.000|x14: 0.574|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.053|x2: 0.000|x3: 0.144|x4: 0.125|x5: 0.080|x6: 0.000|x7: 0.088|x8: 0.000|x9: 0.161|x10: 0.000|x11: 0.097|x12: 0.070|x13: 0.167|x14: 0.646|x15: 0.067|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.062|x2: 0.056|x3: 0.054|x4: 0.201|x5: 0.292|x6: 0.143|x7: 0.281|x8: 0.000|x9: 0.165|x10: 0.096|x11: 0.178|x12: 0.115|x13: 0.270|x14: 0.467|x15: 0.302|x16: 0.196|x17: 0.000
-MEAN -&gt; x1: 0.038|x2: 0.019|x3: 0.185|x4: 0.109|x5: 0.124|x6: 0.048|x7: 0.123|x8: 0.000|x9: 0.109|x10: 0.032|x11: 0.174|x12: 0.061|x13: 0.146|x14: 0.562|x15: 0.123|x16: 0.106|x17: 0.000
+TOP2VEC -&gt; x1: 0.062|x2: 0.056|x3: 0.054|x4: 0.201|x5: 0.292|x6: 0.143|x7: 0.281|x8: 0.000|x9: 0.166|x10: 0.096|x11: 0.178|x12: 0.115|x13: 0.270|x14: 0.467|x15: 0.302|x16: 0.196|x17: 0.000
+MEAN -&gt; x1: 0.038|x2: 0.019|x3: 0.185|x4: 0.109|x5: 0.124|x6: 0.048|x7: 0.123|x8: 0.000|x9: 0.109|x10: 0.032|x11: 0.174|x12: 0.061|x13: 0.146|x14: 0.489|x15: 0.123|x16: 0.106|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.053|x3: 0.063|x4: 0.058|x5: 0.059|x6: 0.055|x7: 0.059|x8: 0.052|x9: 0.058|x10: 0.054|x11: 0.062|x12: 0.056|x13: 0.061|x14: 0.085|x15: 0.059|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3516,15 +3621,16 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 14]</t>
+          <t>[3, 9, 14]</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.653|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.374|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.084|x3: 0.149|x4: 0.222|x5: 0.163|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.489|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.454|x15: 0.088|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.148|x2: 0.214|x3: 0.243|x4: 0.055|x5: 0.296|x6: 0.000|x7: 0.112|x8: 0.186|x9: 0.189|x10: 0.088|x11: 0.131|x12: 0.323|x13: 0.147|x14: 0.402|x15: 0.256|x16: 0.180|x17: 0.000
-MEAN -&gt; x1: 0.049|x2: 0.099|x3: 0.348|x4: 0.092|x5: 0.153|x6: 0.000|x7: 0.094|x8: 0.062|x9: 0.226|x10: 0.029|x11: 0.168|x12: 0.108|x13: 0.049|x14: 0.286|x15: 0.115|x16: 0.060|x17: 0.000
+TOP2VEC -&gt; x1: 0.148|x2: 0.214|x3: 0.243|x4: 0.055|x5: 0.296|x6: 0.000|x7: 0.112|x8: 0.186|x9: 0.189|x10: 0.088|x11: 0.131|x12: 0.323|x13: 0.147|x14: 0.403|x15: 0.256|x16: 0.180|x17: 0.000
+MEAN -&gt; x1: 0.049|x2: 0.099|x3: 0.297|x4: 0.092|x5: 0.153|x6: 0.000|x7: 0.094|x8: 0.062|x9: 0.226|x10: 0.029|x11: 0.168|x12: 0.108|x13: 0.049|x14: 0.286|x15: 0.115|x16: 0.060|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.058|x3: 0.071|x4: 0.058|x5: 0.061|x6: 0.052|x7: 0.058|x8: 0.056|x9: 0.066|x10: 0.054|x11: 0.062|x12: 0.058|x13: 0.055|x14: 0.070|x15: 0.059|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3545,7 +3651,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>[3, 6, 7, 9, 11, 14]</t>
+          <t>[6, 9, 11, 14]</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3554,6 +3660,7 @@
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.103|x4: 0.081|x5: 0.059|x6: 0.112|x7: 0.129|x8: 0.083|x9: 0.266|x10: 0.112|x11: 0.000|x12: 0.061|x13: 0.122|x14: 0.375|x15: 0.196|x16: 0.120|x17: 0.000
 TOP2VEC -&gt; x1: 0.183|x2: 0.120|x3: 0.078|x4: 0.087|x5: 0.000|x6: 0.264|x7: 0.396|x8: 0.242|x9: 0.485|x10: 0.064|x11: 0.359|x12: 0.186|x13: 0.289|x14: 0.145|x15: 0.282|x16: 0.131|x17: 0.000
 MEAN -&gt; x1: 0.061|x2: 0.040|x3: 0.195|x4: 0.056|x5: 0.020|x6: 0.274|x7: 0.175|x8: 0.108|x9: 0.250|x10: 0.059|x11: 0.208|x12: 0.082|x13: 0.137|x14: 0.267|x15: 0.159|x16: 0.084|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.054|x3: 0.063|x4: 0.055|x5: 0.053|x6: 0.068|x7: 0.061|x8: 0.057|x9: 0.066|x10: 0.055|x11: 0.064|x12: 0.056|x13: 0.059|x14: 0.067|x15: 0.060|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3574,7 +3681,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>[3, 11, 13, 14]</t>
+          <t>[11, 14]</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3582,7 +3689,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.399|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.114|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.597|x15: 0.091|x16: 0.121|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.147|x4: 0.110|x5: 0.131|x6: 0.073|x7: 0.000|x8: 0.000|x9: 0.168|x10: 0.000|x11: 0.167|x12: 0.153|x13: 0.169|x14: 0.354|x15: 0.084|x16: 0.264|x17: 0.000
 TOP2VEC -&gt; x1: 0.159|x2: 0.301|x3: 0.000|x4: 0.212|x5: 0.171|x6: 0.000|x7: 0.212|x8: 0.140|x9: 0.195|x10: 0.065|x11: 0.173|x12: 0.319|x13: 0.398|x14: 0.461|x15: 0.420|x16: 0.132|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.100|x3: 0.182|x4: 0.107|x5: 0.100|x6: 0.024|x7: 0.071|x8: 0.047|x9: 0.159|x10: 0.022|x11: 0.203|x12: 0.157|x13: 0.189|x14: 0.470|x15: 0.199|x16: 0.172|x17: 0.000
+MEAN -&gt; x1: 0.053|x2: 0.100|x3: 0.182|x4: 0.107|x5: 0.101|x6: 0.024|x7: 0.071|x8: 0.047|x9: 0.159|x10: 0.022|x11: 0.203|x12: 0.157|x13: 0.189|x14: 0.438|x15: 0.198|x16: 0.172|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.062|x4: 0.057|x5: 0.057|x6: 0.053|x7: 0.055|x8: 0.054|x9: 0.060|x10: 0.052|x11: 0.063|x12: 0.060|x13: 0.062|x14: 0.080|x15: 0.063|x16: 0.061|x17: 0.051
 </t>
         </is>
       </c>
@@ -3611,7 +3719,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.470|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.273|x12: 0.000|x13: 0.000|x14: 0.559|x15: 0.257|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.070|x3: 0.088|x4: 0.188|x5: 0.093|x6: 0.061|x7: 0.000|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.159|x12: 0.099|x13: 0.085|x14: 0.367|x15: 0.324|x16: 0.127|x17: 0.000
 TOP2VEC -&gt; x1: 0.154|x2: 0.250|x3: 0.000|x4: 0.182|x5: 0.155|x6: 0.229|x7: 0.000|x8: 0.132|x9: 0.127|x10: 0.000|x11: 0.137|x12: 0.337|x13: 0.360|x14: 0.432|x15: 0.224|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.051|x2: 0.107|x3: 0.186|x4: 0.123|x5: 0.083|x6: 0.097|x7: 0.000|x8: 0.044|x9: 0.095|x10: 0.000|x11: 0.190|x12: 0.145|x13: 0.148|x14: 0.453|x15: 0.268|x16: 0.077|x17: 0.000
+MEAN -&gt; x1: 0.051|x2: 0.107|x3: 0.186|x4: 0.123|x5: 0.083|x6: 0.097|x7: 0.000|x8: 0.044|x9: 0.095|x10: 0.000|x11: 0.190|x12: 0.145|x13: 0.148|x14: 0.433|x15: 0.268|x16: 0.077|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.058|x3: 0.062|x4: 0.059|x5: 0.056|x6: 0.057|x7: 0.052|x8: 0.054|x9: 0.057|x10: 0.052|x11: 0.063|x12: 0.060|x13: 0.060|x14: 0.080|x15: 0.068|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3632,15 +3741,16 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 15]</t>
+          <t>[3, 15]</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.561|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.181|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.164|x3: 0.172|x4: 0.218|x5: 0.095|x6: 0.000|x7: 0.000|x8: 0.200|x9: 0.070|x10: 0.098|x11: 0.060|x12: 0.063|x13: 0.056|x14: 0.198|x15: 0.302|x16: 0.123|x17: 0.000
-TOP2VEC -&gt; x1: 0.172|x2: 0.126|x3: 0.128|x4: 0.227|x5: 0.211|x6: 0.093|x7: 0.103|x8: 0.197|x9: 0.152|x10: 0.000|x11: 0.207|x12: 0.269|x13: 0.206|x14: 0.175|x15: 0.164|x16: 0.084|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.096|x3: 0.287|x4: 0.149|x5: 0.102|x6: 0.031|x7: 0.034|x8: 0.132|x9: 0.074|x10: 0.033|x11: 0.191|x12: 0.111|x13: 0.087|x14: 0.124|x15: 0.216|x16: 0.069|x17: 0.000
+TOP2VEC -&gt; x1: 0.172|x2: 0.126|x3: 0.128|x4: 0.227|x5: 0.211|x6: 0.093|x7: 0.103|x8: 0.197|x9: 0.152|x10: 0.000|x11: 0.207|x12: 0.269|x13: 0.206|x14: 0.175|x15: 0.163|x16: 0.084|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.097|x3: 0.267|x4: 0.149|x5: 0.102|x6: 0.031|x7: 0.034|x8: 0.132|x9: 0.074|x10: 0.033|x11: 0.191|x12: 0.111|x13: 0.087|x14: 0.124|x15: 0.216|x16: 0.069|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.061|x5: 0.059|x6: 0.055|x7: 0.055|x8: 0.060|x9: 0.057|x10: 0.055|x11: 0.064|x12: 0.059|x13: 0.058|x14: 0.060|x15: 0.066|x16: 0.057|x17: 0.053
 </t>
         </is>
       </c>
@@ -3661,15 +3771,16 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>[3, 11, 12, 13, 14, 15]</t>
+          <t>[3, 11, 15]</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.119|x2: 0.000|x3: 0.459|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.293|x12: 0.000|x13: 0.000|x14: 0.165|x15: 0.189|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.093|x2: 0.000|x3: 0.160|x4: 0.162|x5: 0.102|x6: 0.000|x7: 0.000|x8: 0.092|x9: 0.000|x10: 0.079|x11: 0.160|x12: 0.107|x13: 0.148|x14: 0.000|x15: 0.552|x16: 0.165|x17: 0.000
-TOP2VEC -&gt; x1: 0.131|x2: 0.280|x3: 0.000|x4: 0.148|x5: 0.111|x6: 0.000|x7: 0.000|x8: 0.080|x9: 0.130|x10: 0.085|x11: 0.186|x12: 0.409|x13: 0.451|x14: 0.389|x15: 0.435|x16: 0.175|x17: 0.000
-MEAN -&gt; x1: 0.114|x2: 0.093|x3: 0.207|x4: 0.103|x5: 0.071|x6: 0.000|x7: 0.000|x8: 0.058|x9: 0.043|x10: 0.055|x11: 0.213|x12: 0.172|x13: 0.200|x14: 0.185|x15: 0.392|x16: 0.113|x17: 0.000
+TOP2VEC -&gt; x1: 0.131|x2: 0.280|x3: 0.000|x4: 0.148|x5: 0.111|x6: 0.000|x7: 0.000|x8: 0.080|x9: 0.129|x10: 0.085|x11: 0.186|x12: 0.409|x13: 0.451|x14: 0.389|x15: 0.435|x16: 0.175|x17: 0.000
+MEAN -&gt; x1: 0.114|x2: 0.093|x3: 0.207|x4: 0.103|x5: 0.071|x6: 0.000|x7: 0.000|x8: 0.057|x9: 0.043|x10: 0.055|x11: 0.213|x12: 0.172|x13: 0.200|x14: 0.185|x15: 0.375|x16: 0.113|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.057|x3: 0.064|x4: 0.058|x5: 0.056|x6: 0.052|x7: 0.052|x8: 0.055|x9: 0.054|x10: 0.055|x11: 0.064|x12: 0.062|x13: 0.064|x14: 0.063|x15: 0.076|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -3690,15 +3801,16 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 14, 15]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.616|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.051|x9: 0.000|x10: 0.000|x11: 0.355|x12: 0.000|x13: 0.000|x14: 0.055|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.133|x3: 0.087|x4: 0.208|x5: 0.088|x6: 0.000|x7: 0.133|x8: 0.070|x9: 0.192|x10: 0.071|x11: 0.000|x12: 0.072|x13: 0.000|x14: 0.295|x15: 0.344|x16: 0.128|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.137|x3: 0.000|x4: 0.331|x5: 0.136|x6: 0.338|x7: 0.305|x8: 0.162|x9: 0.242|x10: 0.000|x11: 0.177|x12: 0.179|x13: 0.237|x14: 0.293|x15: 0.209|x16: 0.086|x17: 0.000
-MEAN -&gt; x1: 0.047|x2: 0.090|x3: 0.234|x4: 0.180|x5: 0.075|x6: 0.113|x7: 0.146|x8: 0.094|x9: 0.145|x10: 0.024|x11: 0.177|x12: 0.084|x13: 0.079|x14: 0.214|x15: 0.184|x16: 0.071|x17: 0.000
+TOP2VEC -&gt; x1: 0.140|x2: 0.137|x3: 0.000|x4: 0.331|x5: 0.136|x6: 0.339|x7: 0.305|x8: 0.162|x9: 0.242|x10: 0.000|x11: 0.177|x12: 0.179|x13: 0.237|x14: 0.293|x15: 0.209|x16: 0.086|x17: 0.000
+MEAN -&gt; x1: 0.047|x2: 0.090|x3: 0.196|x4: 0.180|x5: 0.075|x6: 0.113|x7: 0.146|x8: 0.094|x9: 0.145|x10: 0.024|x11: 0.177|x12: 0.084|x13: 0.079|x14: 0.214|x15: 0.184|x16: 0.071|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.064|x4: 0.063|x5: 0.057|x6: 0.059|x7: 0.061|x8: 0.058|x9: 0.061|x10: 0.054|x11: 0.063|x12: 0.057|x13: 0.057|x14: 0.065|x15: 0.063|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3728,6 +3840,7 @@
 LDA -&gt; x1: 0.080|x2: 0.079|x3: 0.117|x4: 0.166|x5: 0.111|x6: 0.235|x7: 0.000|x8: 0.000|x9: 0.155|x10: 0.000|x11: 0.187|x12: 0.000|x13: 0.000|x14: 0.299|x15: 0.301|x16: 0.090|x17: 0.000
 TOP2VEC -&gt; x1: 0.069|x2: 0.102|x3: 0.000|x4: 0.214|x5: 0.130|x6: 0.281|x7: 0.244|x8: 0.095|x9: 0.175|x10: 0.000|x11: 0.238|x12: 0.139|x13: 0.089|x14: 0.110|x15: 0.061|x16: 0.070|x17: 0.000
 MEAN -&gt; x1: 0.073|x2: 0.061|x3: 0.126|x4: 0.127|x5: 0.080|x6: 0.235|x7: 0.081|x8: 0.032|x9: 0.174|x10: 0.000|x11: 0.206|x12: 0.046|x13: 0.030|x14: 0.167|x15: 0.232|x16: 0.053|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.060|x4: 0.060|x5: 0.057|x6: 0.067|x7: 0.057|x8: 0.055|x9: 0.063|x10: 0.053|x11: 0.065|x12: 0.056|x13: 0.055|x14: 0.063|x15: 0.067|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -3755,8 +3868,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.405|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.234|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.469|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.092|x2: 0.132|x3: 0.152|x4: 0.276|x5: 0.000|x6: 0.000|x7: 0.074|x8: 0.068|x9: 0.278|x10: 0.082|x11: 0.159|x12: 0.000|x13: 0.067|x14: 0.000|x15: 0.440|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.163|x2: 0.055|x3: 0.136|x4: 0.111|x5: 0.198|x6: 0.164|x7: 0.300|x8: 0.230|x9: 0.197|x10: 0.000|x11: 0.106|x12: 0.098|x13: 0.057|x14: 0.212|x15: 0.237|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.163|x2: 0.055|x3: 0.136|x4: 0.111|x5: 0.198|x6: 0.164|x7: 0.300|x8: 0.230|x9: 0.197|x10: 0.000|x11: 0.106|x12: 0.099|x13: 0.057|x14: 0.212|x15: 0.237|x16: 0.000|x17: 0.000
 MEAN -&gt; x1: 0.085|x2: 0.062|x3: 0.231|x4: 0.129|x5: 0.066|x6: 0.055|x7: 0.124|x8: 0.099|x9: 0.158|x10: 0.027|x11: 0.166|x12: 0.033|x13: 0.042|x14: 0.071|x15: 0.382|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.067|x4: 0.060|x5: 0.057|x6: 0.056|x7: 0.060|x8: 0.058|x9: 0.062|x10: 0.054|x11: 0.062|x12: 0.055|x13: 0.055|x14: 0.057|x15: 0.077|x16: 0.053|x17: 0.053
 </t>
         </is>
       </c>
@@ -3785,7 +3899,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.337|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.195|x12: 0.000|x13: 0.081|x14: 0.000|x15: 0.738|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.085|x3: 0.138|x4: 0.122|x5: 0.000|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.176|x10: 0.000|x11: 0.000|x12: 0.055|x13: 0.125|x14: 0.116|x15: 0.728|x16: 0.106|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.175|x5: 0.222|x6: 0.139|x7: 0.141|x8: 0.063|x9: 0.214|x10: 0.119|x11: 0.182|x12: 0.201|x13: 0.113|x14: 0.258|x15: 0.317|x16: 0.243|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.028|x3: 0.158|x4: 0.099|x5: 0.074|x6: 0.046|x7: 0.104|x8: 0.021|x9: 0.130|x10: 0.040|x11: 0.126|x12: 0.085|x13: 0.106|x14: 0.124|x15: 0.594|x16: 0.116|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.028|x3: 0.158|x4: 0.099|x5: 0.074|x6: 0.046|x7: 0.104|x8: 0.021|x9: 0.130|x10: 0.040|x11: 0.126|x12: 0.085|x13: 0.106|x14: 0.124|x15: 0.439|x16: 0.116|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.054|x3: 0.062|x4: 0.058|x5: 0.057|x6: 0.055|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.055|x11: 0.060|x12: 0.058|x13: 0.059|x14: 0.060|x15: 0.082|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -3813,8 +3928,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.391|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.233|x12: 0.000|x13: 0.000|x14: 0.174|x15: 0.262|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.053|x3: 0.062|x4: 0.105|x5: 0.068|x6: 0.000|x7: 0.000|x8: 0.115|x9: 0.095|x10: 0.201|x11: 0.199|x12: 0.098|x13: 0.000|x14: 0.205|x15: 0.477|x16: 0.141|x17: 0.000
-TOP2VEC -&gt; x1: 0.149|x2: 0.183|x3: 0.000|x4: 0.070|x5: 0.000|x6: 0.249|x7: 0.168|x8: 0.133|x9: 0.214|x10: 0.054|x11: 0.346|x12: 0.449|x13: 0.384|x14: 0.464|x15: 0.353|x16: 0.111|x17: 0.000
+TOP2VEC -&gt; x1: 0.149|x2: 0.183|x3: 0.000|x4: 0.070|x5: 0.000|x6: 0.249|x7: 0.168|x8: 0.133|x9: 0.214|x10: 0.054|x11: 0.346|x12: 0.450|x13: 0.384|x14: 0.464|x15: 0.353|x16: 0.111|x17: 0.000
 MEAN -&gt; x1: 0.050|x2: 0.079|x3: 0.151|x4: 0.059|x5: 0.023|x6: 0.083|x7: 0.056|x8: 0.083|x9: 0.103|x10: 0.085|x11: 0.259|x12: 0.183|x13: 0.128|x14: 0.281|x15: 0.364|x16: 0.084|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.060|x4: 0.055|x5: 0.053|x6: 0.056|x7: 0.055|x8: 0.056|x9: 0.057|x10: 0.056|x11: 0.067|x12: 0.062|x13: 0.059|x14: 0.069|x15: 0.075|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -3835,15 +3951,16 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>[3, 11, 14, 15]</t>
+          <t>[3, 11, 14]</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.420|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.079|x11: 0.243|x12: 0.000|x13: 0.000|x14: 0.165|x15: 0.096|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.114|x3: 0.116|x4: 0.075|x5: 0.089|x6: 0.000|x7: 0.000|x8: 0.182|x9: 0.000|x10: 0.196|x11: 0.237|x12: 0.069|x13: 0.070|x14: 0.347|x15: 0.213|x16: 0.111|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.108|x3: 0.126|x4: 0.000|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.110|x9: 0.088|x10: 0.090|x11: 0.258|x12: 0.000|x13: 0.262|x14: 0.566|x15: 0.238|x16: 0.184|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.074|x3: 0.221|x4: 0.025|x5: 0.084|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.029|x10: 0.122|x11: 0.246|x12: 0.023|x13: 0.111|x14: 0.360|x15: 0.182|x16: 0.098|x17: 0.000
+TOP2VEC -&gt; x1: 0.123|x2: 0.108|x3: 0.126|x4: 0.000|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.110|x9: 0.088|x10: 0.090|x11: 0.258|x12: 0.000|x13: 0.262|x14: 0.566|x15: 0.238|x16: 0.183|x17: 0.000
+MEAN -&gt; x1: 0.041|x2: 0.074|x3: 0.221|x4: 0.025|x5: 0.084|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.029|x10: 0.122|x11: 0.246|x12: 0.023|x13: 0.111|x14: 0.338|x15: 0.182|x16: 0.098|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.054|x5: 0.058|x6: 0.053|x7: 0.053|x8: 0.058|x9: 0.055|x10: 0.060|x11: 0.068|x12: 0.054|x13: 0.059|x14: 0.074|x15: 0.064|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -3864,15 +3981,16 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 14, 15]</t>
+          <t>[5, 11, 15]</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.454|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.264|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.061|x3: 0.000|x4: 0.094|x5: 0.125|x6: 0.000|x7: 0.113|x8: 0.150|x9: 0.251|x10: 0.151|x11: 0.097|x12: 0.000|x13: 0.000|x14: 0.241|x15: 0.437|x16: 0.100|x17: 0.000
-TOP2VEC -&gt; x1: 0.143|x2: 0.192|x3: 0.081|x4: 0.274|x5: 0.479|x6: 0.407|x7: 0.252|x8: 0.183|x9: 0.223|x10: 0.147|x11: 0.277|x12: 0.418|x13: 0.158|x14: 0.249|x15: 0.457|x16: 0.300|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.084|x3: 0.178|x4: 0.123|x5: 0.201|x6: 0.136|x7: 0.122|x8: 0.111|x9: 0.158|x10: 0.099|x11: 0.215|x12: 0.139|x13: 0.053|x14: 0.163|x15: 0.386|x16: 0.133|x17: 0.000
+TOP2VEC -&gt; x1: 0.143|x2: 0.192|x3: 0.080|x4: 0.274|x5: 0.478|x6: 0.406|x7: 0.252|x8: 0.183|x9: 0.223|x10: 0.147|x11: 0.277|x12: 0.417|x13: 0.158|x14: 0.249|x15: 0.457|x16: 0.300|x17: 0.000
+MEAN -&gt; x1: 0.048|x2: 0.084|x3: 0.178|x4: 0.123|x5: 0.201|x6: 0.135|x7: 0.122|x8: 0.111|x9: 0.158|x10: 0.099|x11: 0.215|x12: 0.139|x13: 0.053|x14: 0.163|x15: 0.386|x16: 0.133|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.061|x4: 0.058|x5: 0.062|x6: 0.058|x7: 0.058|x8: 0.057|x9: 0.060|x10: 0.056|x11: 0.063|x12: 0.059|x13: 0.054|x14: 0.060|x15: 0.075|x16: 0.058|x17: 0.051
 </t>
         </is>
       </c>
@@ -3901,7 +4019,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.525|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.291|x12: 0.225|x13: 0.000|x14: 0.000|x15: 0.062|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.135|x2: 0.063|x3: 0.114|x4: 0.169|x5: 0.195|x6: 0.000|x7: 0.000|x8: 0.116|x9: 0.065|x10: 0.061|x11: 0.236|x12: 0.095|x13: 0.000|x14: 0.000|x15: 0.367|x16: 0.203|x17: 0.000
 TOP2VEC -&gt; x1: 0.107|x2: 0.082|x3: 0.170|x4: 0.106|x5: 0.212|x6: 0.261|x7: 0.386|x8: 0.162|x9: 0.224|x10: 0.055|x11: 0.114|x12: 0.184|x13: 0.000|x14: 0.249|x15: 0.311|x16: 0.113|x17: 0.000
-MEAN -&gt; x1: 0.080|x2: 0.048|x3: 0.270|x4: 0.092|x5: 0.136|x6: 0.087|x7: 0.129|x8: 0.093|x9: 0.097|x10: 0.039|x11: 0.214|x12: 0.168|x13: 0.000|x14: 0.083|x15: 0.247|x16: 0.105|x17: 0.000
+MEAN -&gt; x1: 0.080|x2: 0.048|x3: 0.261|x4: 0.092|x5: 0.136|x6: 0.087|x7: 0.129|x8: 0.093|x9: 0.097|x10: 0.039|x11: 0.214|x12: 0.168|x13: 0.000|x14: 0.083|x15: 0.247|x16: 0.105|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.068|x4: 0.058|x5: 0.060|x6: 0.057|x7: 0.060|x8: 0.058|x9: 0.058|x10: 0.055|x11: 0.065|x12: 0.062|x13: 0.053|x14: 0.057|x15: 0.067|x16: 0.058|x17: 0.053
 </t>
         </is>
       </c>
@@ -3922,7 +4041,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 14, 16]</t>
+          <t>[3, 11, 16]</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3930,7 +4049,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.538|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.322|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.067|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.062|x3: 0.171|x4: 0.233|x5: 0.139|x6: 0.000|x7: 0.060|x8: 0.078|x9: 0.223|x10: 0.063|x11: 0.075|x12: 0.201|x13: 0.000|x14: 0.205|x15: 0.000|x16: 0.309|x17: 0.000
 TOP2VEC -&gt; x1: 0.194|x2: 0.000|x3: 0.417|x4: 0.222|x5: 0.347|x6: 0.415|x7: 0.054|x8: 0.219|x9: 0.000|x10: 0.136|x11: 0.359|x12: 0.000|x13: 0.139|x14: 0.261|x15: 0.196|x16: 0.278|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.021|x3: 0.376|x4: 0.152|x5: 0.162|x6: 0.138|x7: 0.038|x8: 0.099|x9: 0.074|x10: 0.066|x11: 0.252|x12: 0.067|x13: 0.046|x14: 0.155|x15: 0.065|x16: 0.218|x17: 0.000
+MEAN -&gt; x1: 0.065|x2: 0.021|x3: 0.363|x4: 0.152|x5: 0.162|x6: 0.138|x7: 0.038|x8: 0.099|x9: 0.074|x10: 0.066|x11: 0.252|x12: 0.067|x13: 0.046|x14: 0.155|x15: 0.065|x16: 0.218|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.053|x3: 0.075|x4: 0.061|x5: 0.061|x6: 0.060|x7: 0.054|x8: 0.058|x9: 0.056|x10: 0.056|x11: 0.067|x12: 0.056|x13: 0.055|x14: 0.061|x15: 0.056|x16: 0.065|x17: 0.052
 </t>
         </is>
       </c>
@@ -3951,7 +4071,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 15]</t>
+          <t>[3, 4, 11]</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3959,7 +4079,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.528|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.305|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.142|x3: 0.101|x4: 0.406|x5: 0.052|x6: 0.000|x7: 0.000|x8: 0.199|x9: 0.099|x10: 0.096|x11: 0.184|x12: 0.061|x13: 0.071|x14: 0.086|x15: 0.241|x16: 0.081|x17: 0.000
 TOP2VEC -&gt; x1: 0.267|x2: 0.276|x3: 0.246|x4: 0.228|x5: 0.164|x6: 0.376|x7: 0.290|x8: 0.326|x9: 0.172|x10: 0.113|x11: 0.318|x12: 0.372|x13: 0.203|x14: 0.357|x15: 0.332|x16: 0.232|x17: 0.000
-MEAN -&gt; x1: 0.089|x2: 0.139|x3: 0.292|x4: 0.211|x5: 0.072|x6: 0.125|x7: 0.097|x8: 0.175|x9: 0.090|x10: 0.070|x11: 0.269|x12: 0.144|x13: 0.091|x14: 0.148|x15: 0.191|x16: 0.104|x17: 0.000
+MEAN -&gt; x1: 0.089|x2: 0.139|x3: 0.282|x4: 0.211|x5: 0.072|x6: 0.125|x7: 0.097|x8: 0.175|x9: 0.090|x10: 0.070|x11: 0.269|x12: 0.144|x13: 0.091|x14: 0.148|x15: 0.191|x16: 0.104|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.059|x3: 0.068|x4: 0.063|x5: 0.055|x6: 0.058|x7: 0.056|x8: 0.061|x9: 0.056|x10: 0.055|x11: 0.067|x12: 0.059|x13: 0.056|x14: 0.059|x15: 0.062|x16: 0.057|x17: 0.051
 </t>
         </is>
       </c>
@@ -3980,15 +4101,16 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 8, 13]</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.176|x2: 0.000|x3: 0.366|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.212|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.062|x2: 0.168|x3: 0.118|x4: 0.176|x5: 0.133|x6: 0.000|x7: 0.116|x8: 0.376|x9: 0.106|x10: 0.092|x11: 0.100|x12: 0.080|x13: 0.118|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
-TOP2VEC -&gt; x1: 0.258|x2: 0.274|x3: 0.070|x4: 0.362|x5: 0.426|x6: 0.000|x7: 0.143|x8: 0.234|x9: 0.075|x10: 0.000|x11: 0.079|x12: 0.376|x13: 0.464|x14: 0.211|x15: 0.184|x16: 0.073|x17: 0.000
+TOP2VEC -&gt; x1: 0.258|x2: 0.274|x3: 0.070|x4: 0.362|x5: 0.426|x6: 0.000|x7: 0.144|x8: 0.234|x9: 0.075|x10: 0.000|x11: 0.080|x12: 0.376|x13: 0.464|x14: 0.211|x15: 0.184|x16: 0.073|x17: 0.000
 MEAN -&gt; x1: 0.165|x2: 0.147|x3: 0.185|x4: 0.179|x5: 0.186|x6: 0.000|x7: 0.086|x8: 0.203|x9: 0.060|x10: 0.031|x11: 0.130|x12: 0.152|x13: 0.194|x14: 0.070|x15: 0.061|x16: 0.083|x17: 0.000
+SOFTMAX -&gt; x1: 0.062|x2: 0.061|x3: 0.063|x4: 0.063|x5: 0.063|x6: 0.052|x7: 0.057|x8: 0.064|x9: 0.056|x10: 0.054|x11: 0.060|x12: 0.061|x13: 0.064|x14: 0.056|x15: 0.056|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -4009,7 +4131,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>[1, 3, 5, 13, 14, 16]</t>
+          <t>[1, 3, 5, 14, 16]</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -4017,7 +4139,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.198|x2: 0.000|x3: 0.449|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.260|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.182|x17: 0.000
 LDA -&gt; x1: 0.161|x2: 0.099|x3: 0.122|x4: 0.072|x5: 0.269|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.156|x10: 0.000|x11: 0.000|x12: 0.211|x13: 0.151|x14: 0.190|x15: 0.000|x16: 0.387|x17: 0.000
 TOP2VEC -&gt; x1: 0.250|x2: 0.234|x3: 0.236|x4: 0.191|x5: 0.512|x6: 0.139|x7: 0.207|x8: 0.228|x9: 0.000|x10: 0.000|x11: 0.102|x12: 0.085|x13: 0.409|x14: 0.623|x15: 0.271|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.203|x2: 0.111|x3: 0.269|x4: 0.088|x5: 0.260|x6: 0.046|x7: 0.069|x8: 0.076|x9: 0.052|x10: 0.000|x11: 0.120|x12: 0.099|x13: 0.187|x14: 0.271|x15: 0.090|x16: 0.224|x17: 0.000
+MEAN -&gt; x1: 0.203|x2: 0.111|x3: 0.269|x4: 0.088|x5: 0.256|x6: 0.046|x7: 0.069|x8: 0.076|x9: 0.052|x10: 0.000|x11: 0.120|x12: 0.099|x13: 0.187|x14: 0.230|x15: 0.090|x16: 0.224|x17: 0.000
+SOFTMAX -&gt; x1: 0.063|x2: 0.058|x3: 0.068|x4: 0.056|x5: 0.067|x6: 0.054|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.052|x11: 0.058|x12: 0.057|x13: 0.062|x14: 0.065|x15: 0.057|x16: 0.065|x17: 0.052
 </t>
         </is>
       </c>
@@ -4038,7 +4161,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>[3, 5, 11, 13]</t>
+          <t>[3, 5, 11]</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -4046,7 +4169,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.501|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.304|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.146|x3: 0.392|x4: 0.000|x5: 0.112|x6: 0.000|x7: 0.000|x8: 0.105|x9: 0.179|x10: 0.000|x11: 0.180|x12: 0.080|x13: 0.239|x14: 0.138|x15: 0.108|x16: 0.142|x17: 0.000
 TOP2VEC -&gt; x1: 0.165|x2: 0.000|x3: 0.216|x4: 0.373|x5: 0.538|x6: 0.086|x7: 0.283|x8: 0.179|x9: 0.118|x10: 0.076|x11: 0.251|x12: 0.294|x13: 0.220|x14: 0.287|x15: 0.170|x16: 0.155|x17: 0.000
-MEAN -&gt; x1: 0.055|x2: 0.049|x3: 0.370|x4: 0.124|x5: 0.217|x6: 0.029|x7: 0.094|x8: 0.095|x9: 0.099|x10: 0.025|x11: 0.245|x12: 0.125|x13: 0.153|x14: 0.141|x15: 0.093|x16: 0.099|x17: 0.000
+MEAN -&gt; x1: 0.055|x2: 0.049|x3: 0.369|x4: 0.124|x5: 0.204|x6: 0.029|x7: 0.094|x8: 0.095|x9: 0.099|x10: 0.025|x11: 0.245|x12: 0.125|x13: 0.153|x14: 0.141|x15: 0.093|x16: 0.099|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.075|x4: 0.059|x5: 0.064|x6: 0.054|x7: 0.057|x8: 0.057|x9: 0.057|x10: 0.053|x11: 0.067|x12: 0.059|x13: 0.061|x14: 0.060|x15: 0.057|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -4067,15 +4191,16 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>[2, 4, 11, 12, 14]</t>
+          <t>[2, 11]</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.337|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.266|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.303|x3: 0.126|x4: 0.228|x5: 0.000|x6: 0.000|x7: 0.090|x8: 0.000|x9: 0.118|x10: 0.000|x11: 0.285|x12: 0.161|x13: 0.061|x14: 0.194|x15: 0.000|x16: 0.253|x17: 0.000
-TOP2VEC -&gt; x1: 0.178|x2: 0.383|x3: 0.000|x4: 0.226|x5: 0.000|x6: 0.075|x7: 0.230|x8: 0.185|x9: 0.223|x10: 0.064|x11: 0.447|x12: 0.371|x13: 0.333|x14: 0.365|x15: 0.249|x16: 0.131|x17: 0.000
+TOP2VEC -&gt; x1: 0.178|x2: 0.383|x3: 0.000|x4: 0.226|x5: 0.000|x6: 0.074|x7: 0.230|x8: 0.185|x9: 0.223|x10: 0.064|x11: 0.447|x12: 0.371|x13: 0.333|x14: 0.364|x15: 0.249|x16: 0.131|x17: 0.000
 MEAN -&gt; x1: 0.059|x2: 0.229|x3: 0.155|x4: 0.151|x5: 0.000|x6: 0.025|x7: 0.107|x8: 0.062|x9: 0.114|x10: 0.021|x11: 0.333|x12: 0.177|x13: 0.131|x14: 0.186|x15: 0.083|x16: 0.128|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.066|x3: 0.061|x4: 0.061|x5: 0.052|x6: 0.054|x7: 0.058|x8: 0.056|x9: 0.059|x10: 0.053|x11: 0.073|x12: 0.062|x13: 0.060|x14: 0.063|x15: 0.057|x16: 0.059|x17: 0.052
 </t>
         </is>
       </c>
@@ -4096,7 +4221,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 11]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -4105,6 +4230,7 @@
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.106|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.229|x8: 0.148|x9: 0.448|x10: 0.000|x11: 0.000|x12: 0.183|x13: 0.131|x14: 0.286|x15: 0.000|x16: 0.291|x17: 0.000
 TOP2VEC -&gt; x1: 0.102|x2: 0.000|x3: 0.000|x4: 0.159|x5: 0.135|x6: 0.218|x7: 0.246|x8: 0.109|x9: 0.241|x10: 0.060|x11: 0.263|x12: 0.328|x13: 0.246|x14: 0.188|x15: 0.255|x16: 0.122|x17: 0.000
 MEAN -&gt; x1: 0.034|x2: 0.000|x3: 0.162|x4: 0.053|x5: 0.045|x6: 0.073|x7: 0.158|x8: 0.086|x9: 0.257|x10: 0.020|x11: 0.182|x12: 0.189|x13: 0.154|x14: 0.158|x15: 0.085|x16: 0.189|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.053|x3: 0.062|x4: 0.055|x5: 0.055|x6: 0.057|x7: 0.062|x8: 0.057|x9: 0.068|x10: 0.054|x11: 0.063|x12: 0.064|x13: 0.061|x14: 0.062|x15: 0.057|x16: 0.064|x17: 0.053
 </t>
         </is>
       </c>
@@ -4125,7 +4251,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>[2, 3, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -4133,7 +4259,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.733|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.295|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.249|x3: 0.253|x4: 0.308|x5: 0.063|x6: 0.000|x7: 0.128|x8: 0.301|x9: 0.094|x10: 0.099|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.110|x15: 0.119|x16: 0.094|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.246|x3: 0.301|x4: 0.179|x5: 0.260|x6: 0.056|x7: 0.000|x8: 0.067|x9: 0.000|x10: 0.000|x11: 0.237|x12: 0.000|x13: 0.000|x14: 0.277|x15: 0.000|x16: 0.108|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.165|x3: 0.429|x4: 0.162|x5: 0.108|x6: 0.019|x7: 0.043|x8: 0.123|x9: 0.031|x10: 0.033|x11: 0.177|x12: 0.000|x13: 0.000|x14: 0.129|x15: 0.040|x16: 0.067|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.165|x3: 0.351|x4: 0.162|x5: 0.108|x6: 0.019|x7: 0.043|x8: 0.123|x9: 0.031|x10: 0.033|x11: 0.177|x12: 0.000|x13: 0.000|x14: 0.129|x15: 0.040|x16: 0.067|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.063|x3: 0.076|x4: 0.063|x5: 0.060|x6: 0.055|x7: 0.056|x8: 0.061|x9: 0.055|x10: 0.056|x11: 0.064|x12: 0.054|x13: 0.054|x14: 0.061|x15: 0.056|x16: 0.058|x17: 0.054
 </t>
         </is>
       </c>
@@ -4154,7 +4281,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>[3, 11, 13, 15, 16]</t>
+          <t>[3, 11, 13]</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -4162,7 +4289,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.761|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.440|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.056|x3: 0.169|x4: 0.119|x5: 0.321|x6: 0.000|x7: 0.000|x8: 0.131|x9: 0.149|x10: 0.098|x11: 0.136|x12: 0.057|x13: 0.206|x14: 0.000|x15: 0.194|x16: 0.184|x17: 0.000
 TOP2VEC -&gt; x1: 0.220|x2: 0.303|x3: 0.171|x4: 0.224|x5: 0.102|x6: 0.000|x7: 0.234|x8: 0.198|x9: 0.099|x10: 0.174|x11: 0.160|x12: 0.291|x13: 0.424|x14: 0.251|x15: 0.394|x16: 0.356|x17: 0.000
-MEAN -&gt; x1: 0.073|x2: 0.120|x3: 0.367|x4: 0.114|x5: 0.141|x6: 0.000|x7: 0.078|x8: 0.110|x9: 0.083|x10: 0.091|x11: 0.245|x12: 0.116|x13: 0.210|x14: 0.084|x15: 0.196|x16: 0.180|x17: 0.000
+MEAN -&gt; x1: 0.073|x2: 0.120|x3: 0.280|x4: 0.114|x5: 0.141|x6: 0.000|x7: 0.078|x8: 0.110|x9: 0.083|x10: 0.091|x11: 0.245|x12: 0.116|x13: 0.210|x14: 0.084|x15: 0.196|x16: 0.180|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.058|x5: 0.060|x6: 0.052|x7: 0.056|x8: 0.058|x9: 0.056|x10: 0.057|x11: 0.066|x12: 0.058|x13: 0.064|x14: 0.056|x15: 0.063|x16: 0.062|x17: 0.052
 </t>
         </is>
       </c>
@@ -4183,15 +4311,16 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>[3, 11, 14]</t>
+          <t>[3, 11]</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.821|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.437|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.080|x2: 0.059|x3: 0.271|x4: 0.077|x5: 0.000|x6: 0.000|x7: 0.169|x8: 0.197|x9: 0.062|x10: 0.185|x11: 0.278|x12: 0.061|x13: 0.000|x14: 0.225|x15: 0.052|x16: 0.104|x17: 0.000
-TOP2VEC -&gt; x1: 0.094|x2: 0.153|x3: 0.149|x4: 0.118|x5: 0.058|x6: 0.000|x7: 0.000|x8: 0.059|x9: 0.000|x10: 0.094|x11: 0.311|x12: 0.151|x13: 0.283|x14: 0.266|x15: 0.251|x16: 0.192|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.071|x3: 0.414|x4: 0.065|x5: 0.019|x6: 0.000|x7: 0.056|x8: 0.086|x9: 0.021|x10: 0.093|x11: 0.342|x12: 0.071|x13: 0.094|x14: 0.164|x15: 0.101|x16: 0.099|x17: 0.000
+TOP2VEC -&gt; x1: 0.094|x2: 0.153|x3: 0.149|x4: 0.118|x5: 0.058|x6: 0.000|x7: 0.000|x8: 0.059|x9: 0.000|x10: 0.094|x11: 0.311|x12: 0.151|x13: 0.283|x14: 0.266|x15: 0.250|x16: 0.192|x17: 0.000
+MEAN -&gt; x1: 0.058|x2: 0.071|x3: 0.307|x4: 0.065|x5: 0.019|x6: 0.000|x7: 0.056|x8: 0.086|x9: 0.021|x10: 0.093|x11: 0.342|x12: 0.071|x13: 0.094|x14: 0.164|x15: 0.101|x16: 0.099|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.072|x4: 0.057|x5: 0.054|x6: 0.053|x7: 0.056|x8: 0.058|x9: 0.054|x10: 0.058|x11: 0.075|x12: 0.057|x13: 0.058|x14: 0.063|x15: 0.059|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -4220,7 +4349,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.665|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.089|x11: 0.205|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.109|x2: 0.071|x3: 0.441|x4: 0.114|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.196|x9: 0.000|x10: 0.173|x11: 0.055|x12: 0.000|x13: 0.135|x14: 0.000|x15: 0.455|x16: 0.070|x17: 0.000
 TOP2VEC -&gt; x1: 0.094|x2: 0.181|x3: 0.149|x4: 0.257|x5: 0.061|x6: 0.428|x7: 0.410|x8: 0.136|x9: 0.360|x10: 0.092|x11: 0.135|x12: 0.311|x13: 0.175|x14: 0.000|x15: 0.151|x16: 0.188|x17: 0.000
-MEAN -&gt; x1: 0.068|x2: 0.084|x3: 0.418|x4: 0.124|x5: 0.020|x6: 0.143|x7: 0.137|x8: 0.111|x9: 0.120|x10: 0.118|x11: 0.132|x12: 0.104|x13: 0.103|x14: 0.000|x15: 0.202|x16: 0.086|x17: 0.000
+MEAN -&gt; x1: 0.068|x2: 0.084|x3: 0.363|x4: 0.124|x5: 0.020|x6: 0.143|x7: 0.137|x8: 0.111|x9: 0.120|x10: 0.118|x11: 0.132|x12: 0.104|x13: 0.103|x14: 0.000|x15: 0.202|x16: 0.086|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.075|x4: 0.059|x5: 0.053|x6: 0.060|x7: 0.060|x8: 0.059|x9: 0.059|x10: 0.059|x11: 0.060|x12: 0.058|x13: 0.058|x14: 0.052|x15: 0.064|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -4250,6 +4380,7 @@
 LDA -&gt; x1: 0.082|x2: 0.072|x3: 0.215|x4: 0.192|x5: 0.360|x6: 0.086|x7: 0.064|x8: 0.111|x9: 0.111|x10: 0.000|x11: 0.085|x12: 0.000|x13: 0.238|x14: 0.105|x15: 0.000|x16: 0.098|x17: 0.000
 TOP2VEC -&gt; x1: 0.205|x2: 0.131|x3: 0.201|x4: 0.198|x5: 0.276|x6: 0.148|x7: 0.453|x8: 0.173|x9: 0.000|x10: 0.000|x11: 0.131|x12: 0.217|x13: 0.382|x14: 0.171|x15: 0.176|x16: 0.100|x17: 0.000
 MEAN -&gt; x1: 0.096|x2: 0.068|x3: 0.285|x4: 0.130|x5: 0.300|x6: 0.078|x7: 0.172|x8: 0.095|x9: 0.037|x10: 0.000|x11: 0.123|x12: 0.072|x13: 0.206|x14: 0.092|x15: 0.059|x16: 0.066|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.070|x4: 0.060|x5: 0.071|x6: 0.057|x7: 0.062|x8: 0.058|x9: 0.054|x10: 0.052|x11: 0.059|x12: 0.056|x13: 0.065|x14: 0.058|x15: 0.056|x16: 0.056|x17: 0.052
 </t>
         </is>
       </c>
@@ -4270,15 +4401,16 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 11, 15]</t>
+          <t>[3, 4, 11, 15]</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.469|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.271|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.193|x3: 0.126|x4: 0.516|x5: 0.080|x6: 0.074|x7: 0.000|x8: 0.000|x9: 0.079|x10: 0.000|x11: 0.101|x12: 0.000|x13: 0.071|x14: 0.119|x15: 0.460|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.178|x2: 0.080|x3: 0.109|x4: 0.346|x5: 0.267|x6: 0.426|x7: 0.622|x8: 0.219|x9: 0.310|x10: 0.064|x11: 0.229|x12: 0.140|x13: 0.250|x14: 0.318|x15: 0.154|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.059|x2: 0.091|x3: 0.235|x4: 0.288|x5: 0.116|x6: 0.167|x7: 0.207|x8: 0.073|x9: 0.130|x10: 0.021|x11: 0.200|x12: 0.047|x13: 0.107|x14: 0.146|x15: 0.205|x16: 0.044|x17: 0.000
+TOP2VEC -&gt; x1: 0.178|x2: 0.081|x3: 0.109|x4: 0.346|x5: 0.267|x6: 0.426|x7: 0.622|x8: 0.219|x9: 0.310|x10: 0.064|x11: 0.229|x12: 0.140|x13: 0.250|x14: 0.318|x15: 0.154|x16: 0.131|x17: 0.000
+MEAN -&gt; x1: 0.059|x2: 0.091|x3: 0.235|x4: 0.282|x5: 0.116|x6: 0.167|x7: 0.167|x8: 0.073|x9: 0.130|x10: 0.021|x11: 0.200|x12: 0.047|x13: 0.107|x14: 0.146|x15: 0.205|x16: 0.044|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.069|x5: 0.058|x6: 0.061|x7: 0.061|x8: 0.056|x9: 0.059|x10: 0.053|x11: 0.063|x12: 0.054|x13: 0.058|x14: 0.060|x15: 0.064|x16: 0.054|x17: 0.052
 </t>
         </is>
       </c>
@@ -4299,15 +4431,16 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>[2, 3, 9, 14]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.473|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.197|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.318|x3: 0.133|x4: 0.297|x5: 0.170|x6: 0.000|x7: 0.140|x8: 0.000|x9: 0.282|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.102|x14: 0.204|x15: 0.000|x16: 0.078|x17: 0.000
-TOP2VEC -&gt; x1: 0.159|x2: 0.257|x3: 0.101|x4: 0.129|x5: 0.207|x6: 0.462|x7: 0.264|x8: 0.209|x9: 0.268|x10: 0.096|x11: 0.213|x12: 0.457|x13: 0.161|x14: 0.309|x15: 0.291|x16: 0.197|x17: 0.000
+TOP2VEC -&gt; x1: 0.159|x2: 0.257|x3: 0.101|x4: 0.130|x5: 0.207|x6: 0.462|x7: 0.264|x8: 0.209|x9: 0.268|x10: 0.096|x11: 0.213|x12: 0.457|x13: 0.162|x14: 0.309|x15: 0.291|x16: 0.197|x17: 0.000
 MEAN -&gt; x1: 0.053|x2: 0.192|x3: 0.236|x4: 0.142|x5: 0.126|x6: 0.154|x7: 0.135|x8: 0.070|x9: 0.183|x10: 0.064|x11: 0.137|x12: 0.152|x13: 0.088|x14: 0.171|x15: 0.097|x16: 0.092|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.063|x3: 0.066|x4: 0.060|x5: 0.059|x6: 0.061|x7: 0.059|x8: 0.056|x9: 0.062|x10: 0.055|x11: 0.060|x12: 0.060|x13: 0.057|x14: 0.062|x15: 0.057|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -4337,6 +4470,7 @@
 LDA -&gt; x1: 0.000|x2: 0.221|x3: 0.235|x4: 0.000|x5: 0.068|x6: 0.188|x7: 0.000|x8: 0.078|x9: 0.149|x10: 0.168|x11: 0.000|x12: 0.162|x13: 0.063|x14: 0.116|x15: 0.076|x16: 0.295|x17: 0.000
 TOP2VEC -&gt; x1: 0.109|x2: 0.104|x3: 0.275|x4: 0.000|x5: 0.271|x6: 0.199|x7: 0.118|x8: 0.115|x9: 0.051|x10: 0.127|x11: 0.094|x12: 0.105|x13: 0.142|x14: 0.198|x15: 0.000|x16: 0.260|x17: 0.000
 MEAN -&gt; x1: 0.036|x2: 0.108|x3: 0.272|x4: 0.000|x5: 0.113|x6: 0.156|x7: 0.039|x8: 0.064|x9: 0.067|x10: 0.098|x11: 0.072|x12: 0.089|x13: 0.068|x14: 0.105|x15: 0.025|x16: 0.252|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.070|x4: 0.053|x5: 0.060|x6: 0.063|x7: 0.056|x8: 0.057|x9: 0.057|x10: 0.059|x11: 0.057|x12: 0.058|x13: 0.057|x14: 0.059|x15: 0.055|x16: 0.069|x17: 0.053
 </t>
         </is>
       </c>
@@ -4366,6 +4500,7 @@
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.152|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.257|x8: 0.000|x9: 0.382|x10: 0.180|x11: 0.134|x12: 0.151|x13: 0.188|x14: 0.149|x15: 0.000|x16: 0.227|x17: 0.000
 TOP2VEC -&gt; x1: 0.123|x2: 0.265|x3: 0.175|x4: 0.142|x5: 0.103|x6: 0.000|x7: 0.000|x8: 0.125|x9: 0.221|x10: 0.072|x11: 0.299|x12: 0.311|x13: 0.280|x14: 0.321|x15: 0.192|x16: 0.147|x17: 0.000
 MEAN -&gt; x1: 0.041|x2: 0.088|x3: 0.266|x4: 0.047|x5: 0.034|x6: 0.000|x7: 0.086|x8: 0.042|x9: 0.201|x10: 0.128|x11: 0.266|x12: 0.154|x13: 0.156|x14: 0.157|x15: 0.064|x16: 0.125|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.069|x4: 0.055|x5: 0.054|x6: 0.053|x7: 0.057|x8: 0.055|x9: 0.064|x10: 0.060|x11: 0.069|x12: 0.061|x13: 0.061|x14: 0.061|x15: 0.056|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -4386,15 +4521,16 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>[4, 5, 9, 10]</t>
+          <t>[4, 5, 10]</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.223|x4: 0.143|x5: 0.479|x6: 0.000|x7: 0.000|x8: 0.211|x9: 0.000|x10: 0.456|x11: 0.140|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.196|x3: 0.000|x4: 0.394|x5: 0.337|x6: 0.000|x7: 0.078|x8: 0.124|x9: 0.294|x10: 0.279|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.117|x17: 0.000
-TOP2VEC -&gt; x1: 0.127|x2: 0.306|x3: 0.078|x4: 0.424|x5: 0.251|x6: 0.304|x7: 0.344|x8: 0.200|x9: 0.218|x10: 0.000|x11: 0.000|x12: 0.264|x13: 0.000|x14: 0.095|x15: 0.000|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.127|x2: 0.306|x3: 0.077|x4: 0.424|x5: 0.250|x6: 0.304|x7: 0.344|x8: 0.200|x9: 0.218|x10: 0.000|x11: 0.000|x12: 0.264|x13: 0.000|x14: 0.095|x15: 0.000|x16: 0.000|x17: 0.000
 MEAN -&gt; x1: 0.042|x2: 0.167|x3: 0.100|x4: 0.321|x5: 0.355|x6: 0.101|x7: 0.141|x8: 0.178|x9: 0.171|x10: 0.245|x11: 0.047|x12: 0.088|x13: 0.000|x14: 0.032|x15: 0.000|x16: 0.039|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.061|x3: 0.057|x4: 0.072|x5: 0.074|x6: 0.057|x7: 0.060|x8: 0.062|x9: 0.062|x10: 0.066|x11: 0.054|x12: 0.057|x13: 0.052|x14: 0.054|x15: 0.052|x16: 0.054|x17: 0.052
 </t>
         </is>
       </c>
@@ -4422,8 +4558,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.368|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.254|x3: 0.109|x4: 0.480|x5: 0.074|x6: 0.000|x7: 0.000|x8: 0.091|x9: 0.121|x10: 0.000|x11: 0.000|x12: 0.108|x13: 0.059|x14: 0.213|x15: 0.141|x16: 0.170|x17: 0.000
-TOP2VEC -&gt; x1: 0.118|x2: 0.184|x3: 0.083|x4: 0.442|x5: 0.287|x6: 0.000|x7: 0.207|x8: 0.143|x9: 0.000|x10: 0.091|x11: 0.104|x12: 0.152|x13: 0.077|x14: 0.118|x15: 0.000|x16: 0.187|x17: 0.000
+TOP2VEC -&gt; x1: 0.118|x2: 0.184|x3: 0.083|x4: 0.442|x5: 0.286|x6: 0.000|x7: 0.207|x8: 0.143|x9: 0.000|x10: 0.091|x11: 0.104|x12: 0.152|x13: 0.077|x14: 0.118|x15: 0.000|x16: 0.187|x17: 0.000
 MEAN -&gt; x1: 0.039|x2: 0.146|x3: 0.223|x4: 0.430|x5: 0.120|x6: 0.000|x7: 0.069|x8: 0.078|x9: 0.040|x10: 0.030|x11: 0.126|x12: 0.087|x13: 0.045|x14: 0.110|x15: 0.047|x16: 0.119|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.061|x3: 0.066|x4: 0.081|x5: 0.060|x6: 0.053|x7: 0.057|x8: 0.057|x9: 0.055|x10: 0.055|x11: 0.060|x12: 0.058|x13: 0.055|x14: 0.059|x15: 0.055|x16: 0.060|x17: 0.053
 </t>
         </is>
       </c>
@@ -4451,8 +4588,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.055|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.074|x10: 0.372|x11: 0.282|x12: 0.131|x13: 0.065|x14: 0.096|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.095|x3: 0.000|x4: 0.375|x5: 0.000|x6: 0.000|x7: 0.087|x8: 0.153|x9: 0.326|x10: 0.000|x11: 0.000|x12: 0.140|x13: 0.000|x14: 0.409|x15: 0.086|x16: 0.150|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.356|x3: 0.000|x4: 0.520|x5: 0.201|x6: 0.000|x7: 0.182|x8: 0.271|x9: 0.350|x10: 0.099|x11: 0.000|x12: 0.178|x13: 0.289|x14: 0.379|x15: 0.228|x16: 0.203|x17: 0.000
-MEAN -&gt; x1: 0.074|x2: 0.150|x3: 0.159|x4: 0.316|x5: 0.067|x6: 0.000|x7: 0.090|x8: 0.142|x9: 0.250|x10: 0.157|x11: 0.094|x12: 0.149|x13: 0.118|x14: 0.295|x15: 0.105|x16: 0.118|x17: 0.000
+TOP2VEC -&gt; x1: 0.221|x2: 0.356|x3: 0.000|x4: 0.519|x5: 0.201|x6: 0.000|x7: 0.182|x8: 0.271|x9: 0.350|x10: 0.099|x11: 0.000|x12: 0.178|x13: 0.289|x14: 0.379|x15: 0.228|x16: 0.203|x17: 0.000
+MEAN -&gt; x1: 0.074|x2: 0.150|x3: 0.159|x4: 0.310|x5: 0.067|x6: 0.000|x7: 0.090|x8: 0.141|x9: 0.250|x10: 0.157|x11: 0.094|x12: 0.149|x13: 0.118|x14: 0.295|x15: 0.105|x16: 0.118|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.060|x4: 0.070|x5: 0.055|x6: 0.051|x7: 0.056|x8: 0.059|x9: 0.066|x10: 0.060|x11: 0.056|x12: 0.060|x13: 0.058|x14: 0.069|x15: 0.057|x16: 0.058|x17: 0.051
 </t>
         </is>
       </c>
@@ -4481,7 +4619,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.132|x4: 0.000|x5: 0.000|x6: 0.741|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.076|x12: 0.000|x13: 0.125|x14: 0.148|x15: 0.278|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.188|x4: 0.135|x5: 0.000|x6: 0.192|x7: 0.083|x8: 0.109|x9: 0.000|x10: 0.000|x11: 0.114|x12: 0.000|x13: 0.203|x14: 0.438|x15: 0.358|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.163|x2: 0.361|x3: 0.000|x4: 0.088|x5: 0.064|x6: 0.208|x7: 0.224|x8: 0.151|x9: 0.114|x10: 0.000|x11: 0.128|x12: 0.208|x13: 0.324|x14: 0.260|x15: 0.369|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.054|x2: 0.120|x3: 0.107|x4: 0.074|x5: 0.021|x6: 0.380|x7: 0.102|x8: 0.087|x9: 0.038|x10: 0.000|x11: 0.106|x12: 0.069|x13: 0.217|x14: 0.282|x15: 0.335|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.054|x2: 0.120|x3: 0.107|x4: 0.074|x5: 0.021|x6: 0.300|x7: 0.102|x8: 0.087|x9: 0.038|x10: 0.000|x11: 0.106|x12: 0.069|x13: 0.217|x14: 0.282|x15: 0.335|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.058|x4: 0.056|x5: 0.053|x6: 0.071|x7: 0.058|x8: 0.057|x9: 0.054|x10: 0.052|x11: 0.058|x12: 0.056|x13: 0.065|x14: 0.069|x15: 0.073|x16: 0.052|x17: 0.052
 </t>
         </is>
       </c>
@@ -4502,7 +4641,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>[3, 8, 9, 14]</t>
+          <t>[9, 14]</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -4510,7 +4649,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.158|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.091|x12: 0.000|x13: 0.000|x14: 0.097|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.212|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.162|x8: 0.206|x9: 0.602|x10: 0.053|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.414|x15: 0.101|x16: 0.069|x17: 0.000
 TOP2VEC -&gt; x1: 0.242|x2: 0.327|x3: 0.225|x4: 0.000|x5: 0.346|x6: 0.000|x7: 0.221|x8: 0.256|x9: 0.344|x10: 0.108|x11: 0.269|x12: 0.166|x13: 0.457|x14: 0.531|x15: 0.332|x16: 0.222|x17: 0.000
-MEAN -&gt; x1: 0.081|x2: 0.109|x3: 0.198|x4: 0.000|x5: 0.115|x6: 0.000|x7: 0.128|x8: 0.154|x9: 0.315|x10: 0.054|x11: 0.120|x12: 0.055|x13: 0.152|x14: 0.347|x15: 0.145|x16: 0.097|x17: 0.000
+MEAN -&gt; x1: 0.081|x2: 0.109|x3: 0.198|x4: 0.000|x5: 0.115|x6: 0.000|x7: 0.128|x8: 0.154|x9: 0.281|x10: 0.054|x11: 0.120|x12: 0.055|x13: 0.152|x14: 0.337|x15: 0.145|x16: 0.097|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.063|x4: 0.052|x5: 0.058|x6: 0.052|x7: 0.059|x8: 0.061|x9: 0.069|x10: 0.055|x11: 0.059|x12: 0.055|x13: 0.061|x14: 0.073|x15: 0.060|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -4531,7 +4671,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 9, 10]</t>
+          <t>[4, 9]</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -4539,7 +4679,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.114|x2: 0.000|x3: 0.543|x4: 0.066|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.262|x11: 0.314|x12: 0.096|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.067|x2: 0.221|x3: 0.063|x4: 0.338|x5: 0.054|x6: 0.000|x7: 0.100|x8: 0.130|x9: 0.375|x10: 0.216|x11: 0.000|x12: 0.000|x13: 0.054|x14: 0.000|x15: 0.132|x16: 0.071|x17: 0.000
 TOP2VEC -&gt; x1: 0.163|x2: 0.000|x3: 0.000|x4: 0.689|x5: 0.312|x6: 0.000|x7: 0.389|x8: 0.212|x9: 0.422|x10: 0.085|x11: 0.000|x12: 0.000|x13: 0.267|x14: 0.229|x15: 0.079|x16: 0.174|x17: 0.000
-MEAN -&gt; x1: 0.115|x2: 0.074|x3: 0.202|x4: 0.364|x5: 0.122|x6: 0.000|x7: 0.163|x8: 0.114|x9: 0.266|x10: 0.187|x11: 0.105|x12: 0.032|x13: 0.107|x14: 0.076|x15: 0.070|x16: 0.082|x17: 0.000
+MEAN -&gt; x1: 0.115|x2: 0.074|x3: 0.188|x4: 0.301|x5: 0.122|x6: 0.000|x7: 0.163|x8: 0.114|x9: 0.266|x10: 0.187|x11: 0.105|x12: 0.032|x13: 0.107|x14: 0.076|x15: 0.070|x16: 0.082|x17: 0.000
+SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.063|x4: 0.070|x5: 0.059|x6: 0.052|x7: 0.061|x8: 0.058|x9: 0.068|x10: 0.063|x11: 0.058|x12: 0.054|x13: 0.058|x14: 0.056|x15: 0.056|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -4567,8 +4708,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.062|x2: 0.000|x3: 0.329|x4: 0.000|x5: 0.000|x6: 0.061|x7: 0.141|x8: 0.065|x9: 0.134|x10: 0.147|x11: 0.292|x12: 0.197|x13: 0.089|x14: 0.217|x15: 0.000|x16: 0.100|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.079|x4: 0.112|x5: 0.000|x6: 0.000|x7: 0.165|x8: 0.072|x9: 0.372|x10: 0.076|x11: 0.136|x12: 0.148|x13: 0.062|x14: 0.302|x15: 0.087|x16: 0.210|x17: 0.000
-TOP2VEC -&gt; x1: 0.106|x2: 0.111|x3: 0.000|x4: 0.239|x5: 0.110|x6: 0.000|x7: 0.209|x8: 0.114|x9: 0.225|x10: 0.071|x11: 0.200|x12: 0.068|x13: 0.241|x14: 0.381|x15: 0.207|x16: 0.145|x17: 0.000
+TOP2VEC -&gt; x1: 0.106|x2: 0.111|x3: 0.000|x4: 0.239|x5: 0.110|x6: 0.000|x7: 0.209|x8: 0.114|x9: 0.225|x10: 0.071|x11: 0.199|x12: 0.068|x13: 0.241|x14: 0.381|x15: 0.207|x16: 0.145|x17: 0.000
 MEAN -&gt; x1: 0.056|x2: 0.037|x3: 0.136|x4: 0.117|x5: 0.037|x6: 0.020|x7: 0.171|x8: 0.084|x9: 0.244|x10: 0.098|x11: 0.209|x12: 0.137|x13: 0.131|x14: 0.300|x15: 0.098|x16: 0.151|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.054|x3: 0.060|x4: 0.059|x5: 0.054|x6: 0.053|x7: 0.062|x8: 0.057|x9: 0.066|x10: 0.057|x11: 0.064|x12: 0.060|x13: 0.059|x14: 0.070|x15: 0.057|x16: 0.061|x17: 0.052
 </t>
         </is>
       </c>
@@ -4589,7 +4731,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>[4, 8, 9, 14]</t>
+          <t>[8, 9, 14]</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -4597,7 +4739,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.203|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.389|x9: 0.099|x10: 0.000|x11: 0.117|x12: 0.000|x13: 0.000|x14: 0.087|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.271|x3: 0.000|x4: 0.217|x5: 0.000|x6: 0.000|x7: 0.077|x8: 0.096|x9: 0.291|x10: 0.263|x11: 0.000|x12: 0.085|x13: 0.000|x14: 0.350|x15: 0.080|x16: 0.091|x17: 0.000
 TOP2VEC -&gt; x1: 0.087|x2: 0.143|x3: 0.000|x4: 0.217|x5: 0.250|x6: 0.000|x7: 0.103|x8: 0.118|x9: 0.215|x10: 0.100|x11: 0.142|x12: 0.000|x13: 0.116|x14: 0.385|x15: 0.103|x16: 0.206|x17: 0.000
-MEAN -&gt; x1: 0.029|x2: 0.138|x3: 0.068|x4: 0.144|x5: 0.083|x6: 0.000|x7: 0.060|x8: 0.201|x9: 0.202|x10: 0.121|x11: 0.086|x12: 0.028|x13: 0.039|x14: 0.274|x15: 0.061|x16: 0.099|x17: 0.000
+MEAN -&gt; x1: 0.029|x2: 0.138|x3: 0.068|x4: 0.144|x5: 0.083|x6: 0.000|x7: 0.060|x8: 0.201|x9: 0.202|x10: 0.121|x11: 0.087|x12: 0.028|x13: 0.039|x14: 0.274|x15: 0.061|x16: 0.099|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.061|x3: 0.057|x4: 0.062|x5: 0.058|x6: 0.053|x7: 0.057|x8: 0.065|x9: 0.065|x10: 0.060|x11: 0.058|x12: 0.055|x13: 0.055|x14: 0.070|x15: 0.057|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -4625,8 +4768,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.076|x2: 0.000|x3: 0.361|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.077|x8: 0.203|x9: 0.081|x10: 0.000|x11: 0.232|x12: 0.127|x13: 0.369|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.174|x4: 0.063|x5: 0.000|x6: 0.000|x7: 0.081|x8: 0.347|x9: 0.308|x10: 0.084|x11: 0.098|x12: 0.072|x13: 0.212|x14: 0.058|x15: 0.201|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.172|x3: 0.098|x4: 0.261|x5: 0.304|x6: 0.000|x7: 0.347|x8: 0.252|x9: 0.259|x10: 0.092|x11: 0.000|x12: 0.328|x13: 0.316|x14: 0.293|x15: 0.158|x16: 0.189|x17: 0.000
+TOP2VEC -&gt; x1: 0.221|x2: 0.172|x3: 0.097|x4: 0.261|x5: 0.304|x6: 0.000|x7: 0.347|x8: 0.252|x9: 0.259|x10: 0.092|x11: 0.000|x12: 0.328|x13: 0.316|x14: 0.293|x15: 0.158|x16: 0.189|x17: 0.000
 MEAN -&gt; x1: 0.099|x2: 0.057|x3: 0.211|x4: 0.108|x5: 0.101|x6: 0.000|x7: 0.169|x8: 0.267|x9: 0.216|x10: 0.059|x11: 0.110|x12: 0.176|x13: 0.299|x14: 0.117|x15: 0.120|x16: 0.103|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.064|x4: 0.057|x5: 0.057|x6: 0.051|x7: 0.061|x8: 0.067|x9: 0.064|x10: 0.055|x11: 0.057|x12: 0.061|x13: 0.069|x14: 0.058|x15: 0.058|x16: 0.057|x17: 0.051
 </t>
         </is>
       </c>
@@ -4647,7 +4791,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>[3, 4, 8, 10]</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -4656,6 +4800,7 @@
 LDA -&gt; x1: 0.000|x2: 0.110|x3: 0.207|x4: 0.169|x5: 0.000|x6: 0.000|x7: 0.146|x8: 0.397|x9: 0.275|x10: 0.206|x11: 0.000|x12: 0.070|x13: 0.052|x14: 0.068|x15: 0.000|x16: 0.119|x17: 0.000
 TOP2VEC -&gt; x1: 0.212|x2: 0.129|x3: 0.124|x4: 0.370|x5: 0.166|x6: 0.000|x7: 0.193|x8: 0.275|x9: 0.182|x10: 0.000|x11: 0.097|x12: 0.099|x13: 0.125|x14: 0.071|x15: 0.000|x16: 0.079|x17: 0.000
 MEAN -&gt; x1: 0.110|x2: 0.080|x3: 0.230|x4: 0.180|x5: 0.055|x6: 0.000|x7: 0.113|x8: 0.369|x9: 0.152|x10: 0.144|x11: 0.102|x12: 0.056|x13: 0.079|x14: 0.046|x15: 0.000|x16: 0.066|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.057|x3: 0.066|x4: 0.063|x5: 0.056|x6: 0.053|x7: 0.059|x8: 0.076|x9: 0.061|x10: 0.061|x11: 0.058|x12: 0.056|x13: 0.057|x14: 0.055|x15: 0.053|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -4676,15 +4821,16 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>[9, 15]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.330|x4: 0.000|x5: 0.000|x6: 0.088|x7: 0.000|x8: 0.000|x9: 0.201|x10: 0.000|x11: 0.191|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.054|x4: 0.087|x5: 0.165|x6: 0.111|x7: 0.191|x8: 0.062|x9: 0.552|x10: 0.118|x11: 0.064|x12: 0.064|x13: 0.000|x14: 0.000|x15: 0.209|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.235|x3: 0.000|x4: 0.287|x5: 0.101|x6: 0.097|x7: 0.090|x8: 0.066|x9: 0.426|x10: 0.084|x11: 0.000|x12: 0.188|x13: 0.246|x14: 0.092|x15: 0.275|x16: 0.172|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.078|x3: 0.128|x4: 0.125|x5: 0.089|x6: 0.099|x7: 0.094|x8: 0.043|x9: 0.393|x10: 0.067|x11: 0.085|x12: 0.084|x13: 0.082|x14: 0.031|x15: 0.162|x16: 0.105|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.235|x3: 0.000|x4: 0.287|x5: 0.101|x6: 0.097|x7: 0.090|x8: 0.066|x9: 0.426|x10: 0.084|x11: 0.000|x12: 0.188|x13: 0.246|x14: 0.092|x15: 0.276|x16: 0.172|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.078|x3: 0.128|x4: 0.125|x5: 0.089|x6: 0.099|x7: 0.094|x8: 0.043|x9: 0.376|x10: 0.067|x11: 0.085|x12: 0.084|x13: 0.082|x14: 0.031|x15: 0.162|x16: 0.105|x17: 0.000
+SOFTMAX -&gt; x1: 0.053|x2: 0.058|x3: 0.060|x4: 0.060|x5: 0.058|x6: 0.059|x7: 0.058|x8: 0.056|x9: 0.077|x10: 0.057|x11: 0.058|x12: 0.058|x13: 0.058|x14: 0.055|x15: 0.063|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>
@@ -4705,15 +4851,16 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 11, 13]</t>
+          <t>[7, 9, 13]</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.061|x2: 0.000|x3: 0.308|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.115|x8: 0.148|x9: 0.131|x10: 0.065|x11: 0.220|x12: 0.000|x13: 0.543|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.217|x2: 0.000|x3: 0.201|x4: 0.000|x5: 0.000|x6: 0.103|x7: 0.169|x8: 0.000|x9: 0.638|x10: 0.000|x11: 0.000|x12: 0.097|x13: 0.252|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.000|x3: 0.000|x4: 0.154|x5: 0.000|x6: 0.218|x7: 0.617|x8: 0.139|x9: 0.629|x10: 0.000|x11: 0.374|x12: 0.265|x13: 0.572|x14: 0.230|x15: 0.277|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.139|x2: 0.000|x3: 0.169|x4: 0.051|x5: 0.000|x6: 0.107|x7: 0.300|x8: 0.096|x9: 0.466|x10: 0.022|x11: 0.198|x12: 0.121|x13: 0.456|x14: 0.077|x15: 0.092|x16: 0.048|x17: 0.000
+TOP2VEC -&gt; x1: 0.140|x2: 0.000|x3: 0.000|x4: 0.154|x5: 0.000|x6: 0.218|x7: 0.616|x8: 0.139|x9: 0.629|x10: 0.000|x11: 0.373|x12: 0.265|x13: 0.572|x14: 0.230|x15: 0.277|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.139|x2: 0.000|x3: 0.169|x4: 0.051|x5: 0.000|x6: 0.107|x7: 0.261|x8: 0.096|x9: 0.377|x10: 0.022|x11: 0.198|x12: 0.121|x13: 0.417|x14: 0.077|x15: 0.092|x16: 0.048|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.051|x3: 0.061|x4: 0.054|x5: 0.051|x6: 0.057|x7: 0.067|x8: 0.057|x9: 0.075|x10: 0.052|x11: 0.063|x12: 0.058|x13: 0.078|x14: 0.055|x15: 0.056|x16: 0.054|x17: 0.051
 </t>
         </is>
       </c>
@@ -4734,15 +4881,16 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>[3, 4, 5, 11, 13, 16]</t>
+          <t>[3, 4, 5]</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.434|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.251|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.218|x3: 0.166|x4: 0.245|x5: 0.357|x6: 0.132|x7: 0.000|x8: 0.137|x9: 0.000|x10: 0.130|x11: 0.000|x12: 0.000|x13: 0.236|x14: 0.059|x15: 0.000|x16: 0.141|x17: 0.000
-TOP2VEC -&gt; x1: 0.078|x2: 0.182|x3: 0.313|x4: 0.483|x5: 0.528|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.205|x11: 0.237|x12: 0.205|x13: 0.284|x14: 0.251|x15: 0.088|x16: 0.419|x17: 0.000
-MEAN -&gt; x1: 0.026|x2: 0.133|x3: 0.304|x4: 0.242|x5: 0.315|x6: 0.044|x7: 0.000|x8: 0.046|x9: 0.000|x10: 0.112|x11: 0.163|x12: 0.068|x13: 0.173|x14: 0.103|x15: 0.029|x16: 0.187|x17: 0.000
+TOP2VEC -&gt; x1: 0.078|x2: 0.182|x3: 0.313|x4: 0.483|x5: 0.527|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.204|x11: 0.237|x12: 0.205|x13: 0.284|x14: 0.251|x15: 0.088|x16: 0.419|x17: 0.000
+MEAN -&gt; x1: 0.026|x2: 0.133|x3: 0.304|x4: 0.242|x5: 0.306|x6: 0.044|x7: 0.000|x8: 0.046|x9: 0.000|x10: 0.112|x11: 0.163|x12: 0.068|x13: 0.173|x14: 0.103|x15: 0.029|x16: 0.187|x17: 0.000
+SOFTMAX -&gt; x1: 0.054|x2: 0.060|x3: 0.071|x4: 0.067|x5: 0.071|x6: 0.055|x7: 0.052|x8: 0.055|x9: 0.052|x10: 0.058|x11: 0.061|x12: 0.056|x13: 0.062|x14: 0.058|x15: 0.054|x16: 0.063|x17: 0.052
 </t>
         </is>
       </c>
@@ -4770,8 +4918,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.103|x2: 0.000|x3: 0.287|x4: 0.000|x5: 0.082|x6: 0.000|x7: 0.000|x8: 0.119|x9: 0.000|x10: 0.000|x11: 0.177|x12: 0.000|x13: 0.431|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.061|x2: 0.000|x3: 0.173|x4: 0.000|x5: 0.251|x6: 0.000|x7: 0.074|x8: 0.331|x9: 0.273|x10: 0.081|x11: 0.112|x12: 0.000|x13: 0.202|x14: 0.063|x15: 0.078|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.166|x2: 0.327|x3: 0.196|x4: 0.348|x5: 0.160|x6: 0.000|x7: 0.000|x8: 0.159|x9: 0.080|x10: 0.098|x11: 0.120|x12: 0.187|x13: 0.286|x14: 0.258|x15: 0.081|x16: 0.201|x17: 0.000
+TOP2VEC -&gt; x1: 0.166|x2: 0.327|x3: 0.196|x4: 0.347|x5: 0.160|x6: 0.000|x7: 0.000|x8: 0.159|x9: 0.080|x10: 0.098|x11: 0.120|x12: 0.187|x13: 0.286|x14: 0.258|x15: 0.081|x16: 0.201|x17: 0.000
 MEAN -&gt; x1: 0.110|x2: 0.109|x3: 0.218|x4: 0.116|x5: 0.165|x6: 0.000|x7: 0.025|x8: 0.203|x9: 0.118|x10: 0.060|x11: 0.137|x12: 0.062|x13: 0.306|x14: 0.107|x15: 0.053|x16: 0.108|x17: 0.000
+SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.065|x4: 0.059|x5: 0.062|x6: 0.052|x7: 0.054|x8: 0.064|x9: 0.059|x10: 0.056|x11: 0.060|x12: 0.056|x13: 0.071|x14: 0.058|x15: 0.055|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -4792,15 +4941,16 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>[3, 7, 8, 9]</t>
+          <t>[3, 7, 9]</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.432|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.205|x9: 0.000|x10: 0.000|x11: 0.249|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.134|x3: 0.158|x4: 0.276|x5: 0.161|x6: 0.000|x7: 0.201|x8: 0.000|x9: 0.415|x10: 0.198|x11: 0.000|x12: 0.000|x13: 0.065|x14: 0.119|x15: 0.000|x16: 0.093|x17: 0.000
-TOP2VEC -&gt; x1: 0.167|x2: 0.285|x3: 0.172|x4: 0.151|x5: 0.197|x6: 0.090|x7: 0.401|x8: 0.208|x9: 0.245|x10: 0.113|x11: 0.148|x12: 0.222|x13: 0.197|x14: 0.204|x15: 0.084|x16: 0.231|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.140|x3: 0.254|x4: 0.142|x5: 0.120|x6: 0.030|x7: 0.201|x8: 0.138|x9: 0.220|x10: 0.104|x11: 0.132|x12: 0.074|x13: 0.087|x14: 0.108|x15: 0.028|x16: 0.108|x17: 0.000
+TOP2VEC -&gt; x1: 0.167|x2: 0.285|x3: 0.172|x4: 0.151|x5: 0.197|x6: 0.090|x7: 0.400|x8: 0.208|x9: 0.245|x10: 0.113|x11: 0.147|x12: 0.222|x13: 0.197|x14: 0.204|x15: 0.084|x16: 0.231|x17: 0.000
+MEAN -&gt; x1: 0.056|x2: 0.139|x3: 0.254|x4: 0.142|x5: 0.120|x6: 0.030|x7: 0.200|x8: 0.138|x9: 0.220|x10: 0.104|x11: 0.132|x12: 0.074|x13: 0.087|x14: 0.108|x15: 0.028|x16: 0.108|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.067|x4: 0.060|x5: 0.059|x6: 0.054|x7: 0.064|x8: 0.060|x9: 0.065|x10: 0.058|x11: 0.060|x12: 0.056|x13: 0.057|x14: 0.058|x15: 0.054|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -4821,7 +4971,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>[11, 13]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -4829,7 +4979,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.197|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.154|x12: 0.053|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.280|x4: 0.064|x5: 0.000|x6: 0.000|x7: 0.059|x8: 0.070|x9: 0.222|x10: 0.000|x11: 0.749|x12: 0.072|x13: 0.083|x14: 0.071|x15: 0.071|x16: 0.078|x17: 0.000
 TOP2VEC -&gt; x1: 0.109|x2: 0.000|x3: 0.000|x4: 0.204|x5: 0.000|x6: 0.254|x7: 0.278|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.734|x12: 0.380|x13: 0.538|x14: 0.258|x15: 0.195|x16: 0.078|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.000|x3: 0.159|x4: 0.089|x5: 0.000|x6: 0.085|x7: 0.112|x8: 0.023|x9: 0.127|x10: 0.000|x11: 0.879|x12: 0.168|x13: 0.207|x14: 0.110|x15: 0.089|x16: 0.052|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.000|x3: 0.159|x4: 0.089|x5: 0.000|x6: 0.085|x7: 0.112|x8: 0.023|x9: 0.127|x10: 0.000|x11: 0.500|x12: 0.168|x13: 0.194|x14: 0.110|x15: 0.089|x16: 0.052|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.053|x3: 0.062|x4: 0.058|x5: 0.053|x6: 0.057|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.053|x11: 0.087|x12: 0.062|x13: 0.064|x14: 0.059|x15: 0.058|x16: 0.056|x17: 0.053
 </t>
         </is>
       </c>
@@ -4850,7 +5001,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>[6, 7, 9, 14]</t>
+          <t>[6, 9, 14]</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -4858,7 +5009,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.417|x4: 0.000|x5: 0.000|x6: 0.081|x7: 0.000|x8: 0.000|x9: 0.154|x10: 0.071|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.069|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.090|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.252|x7: 0.137|x8: 0.088|x9: 0.511|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.058|x14: 0.285|x15: 0.400|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.094|x2: 0.408|x3: 0.000|x4: 0.389|x5: 0.286|x6: 0.278|x7: 0.407|x8: 0.129|x9: 0.347|x10: 0.000|x11: 0.000|x12: 0.100|x13: 0.191|x14: 0.540|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.061|x2: 0.136|x3: 0.139|x4: 0.130|x5: 0.095|x6: 0.204|x7: 0.181|x8: 0.072|x9: 0.337|x10: 0.024|x11: 0.080|x12: 0.033|x13: 0.083|x14: 0.275|x15: 0.156|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.061|x2: 0.136|x3: 0.139|x4: 0.130|x5: 0.095|x6: 0.204|x7: 0.181|x8: 0.072|x9: 0.334|x10: 0.024|x11: 0.080|x12: 0.033|x13: 0.083|x14: 0.262|x15: 0.156|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.060|x4: 0.059|x5: 0.057|x6: 0.064|x7: 0.062|x8: 0.056|x9: 0.073|x10: 0.053|x11: 0.056|x12: 0.054|x13: 0.057|x14: 0.068|x15: 0.061|x16: 0.052|x17: 0.052
 </t>
         </is>
       </c>
@@ -4879,7 +5031,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 13, 15]</t>
+          <t>[3, 4, 11, 15]</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4887,7 +5039,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.723|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.418|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.150|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.185|x3: 0.157|x4: 0.381|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.186|x9: 0.075|x10: 0.000|x11: 0.186|x12: 0.000|x13: 0.148|x14: 0.000|x15: 0.502|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.261|x2: 0.000|x3: 0.000|x4: 0.303|x5: 0.164|x6: 0.144|x7: 0.379|x8: 0.290|x9: 0.317|x10: 0.000|x11: 0.206|x12: 0.334|x13: 0.405|x14: 0.247|x15: 0.327|x16: 0.087|x17: 0.000
-MEAN -&gt; x1: 0.087|x2: 0.062|x3: 0.294|x4: 0.228|x5: 0.055|x6: 0.048|x7: 0.126|x8: 0.159|x9: 0.131|x10: 0.000|x11: 0.270|x12: 0.111|x13: 0.184|x14: 0.082|x15: 0.326|x16: 0.029|x17: 0.000
+MEAN -&gt; x1: 0.087|x2: 0.062|x3: 0.219|x4: 0.228|x5: 0.055|x6: 0.048|x7: 0.126|x8: 0.159|x9: 0.131|x10: 0.000|x11: 0.270|x12: 0.111|x13: 0.184|x14: 0.082|x15: 0.326|x16: 0.029|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.064|x4: 0.065|x5: 0.055|x6: 0.054|x7: 0.059|x8: 0.061|x9: 0.059|x10: 0.052|x11: 0.068|x12: 0.058|x13: 0.062|x14: 0.056|x15: 0.072|x16: 0.053|x17: 0.052
 </t>
         </is>
       </c>
@@ -4908,7 +5061,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>[9, 12, 14]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4916,7 +5069,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.112|x2: 0.000|x3: 0.308|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.076|x8: 0.000|x9: 0.102|x10: 0.000|x11: 0.178|x12: 0.080|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
 LDA -&gt; x1: 0.079|x2: 0.064|x3: 0.076|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.161|x8: 0.166|x9: 0.606|x10: 0.000|x11: 0.000|x12: 0.101|x13: 0.092|x14: 0.250|x15: 0.067|x16: 0.159|x17: 0.000
 TOP2VEC -&gt; x1: 0.265|x2: 0.252|x3: 0.000|x4: 0.143|x5: 0.219|x6: 0.000|x7: 0.346|x8: 0.269|x9: 0.097|x10: 0.093|x11: 0.000|x12: 0.367|x13: 0.376|x14: 0.282|x15: 0.229|x16: 0.191|x17: 0.000
-MEAN -&gt; x1: 0.152|x2: 0.105|x3: 0.128|x4: 0.048|x5: 0.073|x6: 0.000|x7: 0.194|x8: 0.145|x9: 0.268|x10: 0.031|x11: 0.059|x12: 0.182|x13: 0.156|x14: 0.177|x15: 0.098|x16: 0.175|x17: 0.000
+MEAN -&gt; x1: 0.152|x2: 0.105|x3: 0.128|x4: 0.048|x5: 0.073|x6: 0.000|x7: 0.194|x8: 0.145|x9: 0.233|x10: 0.031|x11: 0.059|x12: 0.182|x13: 0.156|x14: 0.177|x15: 0.098|x16: 0.175|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.058|x3: 0.059|x4: 0.055|x5: 0.056|x6: 0.052|x7: 0.064|x8: 0.060|x9: 0.066|x10: 0.054|x11: 0.055|x12: 0.063|x13: 0.061|x14: 0.062|x15: 0.058|x16: 0.062|x17: 0.052
 </t>
         </is>
       </c>
@@ -4944,8 +5098,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.103|x2: 0.000|x3: 0.470|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.070|x9: 0.000|x10: 0.000|x11: 0.308|x12: 0.062|x13: 0.080|x14: 0.061|x15: 0.000|x16: 0.145|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.080|x3: 0.154|x4: 0.063|x5: 0.129|x6: 0.000|x7: 0.130|x8: 0.148|x9: 0.153|x10: 0.124|x11: 0.000|x12: 0.140|x13: 0.172|x14: 0.273|x15: 0.000|x16: 0.253|x17: 0.000
-TOP2VEC -&gt; x1: 0.144|x2: 0.158|x3: 0.138|x4: 0.197|x5: 0.259|x6: 0.250|x7: 0.101|x8: 0.157|x9: 0.251|x10: 0.074|x11: 0.123|x12: 0.146|x13: 0.286|x14: 0.322|x15: 0.147|x16: 0.151|x17: 0.000
+TOP2VEC -&gt; x1: 0.144|x2: 0.158|x3: 0.138|x4: 0.197|x5: 0.259|x6: 0.250|x7: 0.101|x8: 0.157|x9: 0.251|x10: 0.074|x11: 0.123|x12: 0.146|x13: 0.285|x14: 0.322|x15: 0.147|x16: 0.151|x17: 0.000
 MEAN -&gt; x1: 0.082|x2: 0.079|x3: 0.254|x4: 0.087|x5: 0.129|x6: 0.083|x7: 0.077|x8: 0.125|x9: 0.135|x10: 0.066|x11: 0.144|x12: 0.116|x13: 0.179|x14: 0.219|x15: 0.049|x16: 0.183|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.067|x4: 0.057|x5: 0.059|x6: 0.057|x7: 0.056|x8: 0.059|x9: 0.060|x10: 0.056|x11: 0.060|x12: 0.059|x13: 0.062|x14: 0.065|x15: 0.055|x16: 0.063|x17: 0.052
 </t>
         </is>
       </c>
@@ -4974,7 +5129,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.328|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.190|x12: 0.000|x13: 0.000|x14: 0.747|x15: 0.579|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.081|x3: 0.074|x4: 0.085|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.130|x9: 0.163|x10: 0.000|x11: 0.119|x12: 0.000|x13: 0.059|x14: 0.430|x15: 0.679|x16: 0.000|x17: 0.000
 TOP2VEC -&gt; x1: 0.172|x2: 0.205|x3: 0.000|x4: 0.000|x5: 0.073|x6: 0.000|x7: 0.239|x8: 0.204|x9: 0.223|x10: 0.000|x11: 0.198|x12: 0.213|x13: 0.224|x14: 0.507|x15: 0.338|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.095|x3: 0.134|x4: 0.028|x5: 0.024|x6: 0.000|x7: 0.080|x8: 0.111|x9: 0.129|x10: 0.000|x11: 0.169|x12: 0.071|x13: 0.095|x14: 0.562|x15: 0.532|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.095|x3: 0.134|x4: 0.028|x5: 0.024|x6: 0.000|x7: 0.080|x8: 0.111|x9: 0.129|x10: 0.000|x11: 0.169|x12: 0.071|x13: 0.095|x14: 0.477|x15: 0.446|x16: 0.000|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.059|x4: 0.054|x5: 0.053|x6: 0.052|x7: 0.056|x8: 0.058|x9: 0.059|x10: 0.052|x11: 0.062|x12: 0.056|x13: 0.057|x14: 0.084|x15: 0.081|x16: 0.052|x17: 0.052
 </t>
         </is>
       </c>
@@ -4995,7 +5151,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 14]</t>
+          <t>[5, 14]</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -5003,7 +5159,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.433|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.250|x12: 0.000|x13: 0.000|x14: 0.274|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.099|x2: 0.000|x3: 0.000|x4: 0.138|x5: 0.416|x6: 0.138|x7: 0.108|x8: 0.000|x9: 0.286|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.064|x14: 0.411|x15: 0.000|x16: 0.160|x17: 0.000
 TOP2VEC -&gt; x1: 0.095|x2: 0.143|x3: 0.000|x4: 0.000|x5: 0.225|x6: 0.283|x7: 0.329|x8: 0.110|x9: 0.279|x10: 0.078|x11: 0.230|x12: 0.161|x13: 0.233|x14: 0.513|x15: 0.147|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.048|x3: 0.144|x4: 0.046|x5: 0.213|x6: 0.140|x7: 0.146|x8: 0.037|x9: 0.188|x10: 0.026|x11: 0.160|x12: 0.054|x13: 0.099|x14: 0.399|x15: 0.049|x16: 0.107|x17: 0.000
+MEAN -&gt; x1: 0.065|x2: 0.048|x3: 0.144|x4: 0.046|x5: 0.213|x6: 0.140|x7: 0.146|x8: 0.037|x9: 0.188|x10: 0.026|x11: 0.160|x12: 0.054|x13: 0.099|x14: 0.395|x15: 0.049|x16: 0.107|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.060|x4: 0.055|x5: 0.065|x6: 0.060|x7: 0.061|x8: 0.054|x9: 0.063|x10: 0.054|x11: 0.061|x12: 0.055|x13: 0.058|x14: 0.078|x15: 0.055|x16: 0.058|x17: 0.052
 </t>
         </is>
       </c>
@@ -5024,15 +5181,16 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 14]</t>
+          <t>[3, 11, 14]</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.460|x4: 0.000|x5: 0.000|x6: 0.099|x7: 0.000|x8: 0.056|x9: 0.000|x10: 0.000|x11: 0.266|x12: 0.000|x13: 0.000|x14: 0.216|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.085|x2: 0.098|x3: 0.149|x4: 0.118|x5: 0.000|x6: 0.059|x7: 0.072|x8: 0.162|x9: 0.270|x10: 0.000|x11: 0.145|x12: 0.000|x13: 0.000|x14: 0.423|x15: 0.151|x16: 0.088|x17: 0.000
-TOP2VEC -&gt; x1: 0.187|x2: 0.000|x3: 0.138|x4: 0.356|x5: 0.138|x6: 0.246|x7: 0.408|x8: 0.214|x9: 0.170|x10: 0.087|x11: 0.399|x12: 0.196|x13: 0.227|x14: 0.293|x15: 0.123|x16: 0.179|x17: 0.000
+TOP2VEC -&gt; x1: 0.187|x2: 0.000|x3: 0.138|x4: 0.356|x5: 0.138|x6: 0.246|x7: 0.408|x8: 0.214|x9: 0.170|x10: 0.087|x11: 0.399|x12: 0.195|x13: 0.227|x14: 0.293|x15: 0.122|x16: 0.179|x17: 0.000
 MEAN -&gt; x1: 0.091|x2: 0.033|x3: 0.249|x4: 0.158|x5: 0.046|x6: 0.135|x7: 0.160|x8: 0.144|x9: 0.146|x10: 0.029|x11: 0.270|x12: 0.065|x13: 0.076|x14: 0.310|x15: 0.091|x16: 0.089|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.054|x3: 0.066|x4: 0.061|x5: 0.054|x6: 0.059|x7: 0.061|x8: 0.060|x9: 0.060|x10: 0.053|x11: 0.068|x12: 0.055|x13: 0.056|x14: 0.071|x15: 0.057|x16: 0.057|x17: 0.052
 </t>
         </is>
       </c>
@@ -5053,15 +5211,16 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 9, 11, 12, 14, 15, 16]</t>
+          <t>[4, 11, 15]</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.679|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.392|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.096|x2: 0.117|x3: 0.000|x4: 0.382|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.108|x9: 0.170|x10: 0.000|x11: 0.000|x12: 0.158|x13: 0.000|x14: 0.183|x15: 0.386|x16: 0.220|x17: 0.000
-TOP2VEC -&gt; x1: 0.236|x2: 0.428|x3: 0.000|x4: 0.316|x5: 0.218|x6: 0.279|x7: 0.348|x8: 0.318|x9: 0.371|x10: 0.118|x11: 0.252|x12: 0.425|x13: 0.195|x14: 0.369|x15: 0.255|x16: 0.242|x17: 0.000
-MEAN -&gt; x1: 0.111|x2: 0.182|x3: 0.226|x4: 0.233|x5: 0.073|x6: 0.093|x7: 0.116|x8: 0.142|x9: 0.180|x10: 0.039|x11: 0.215|x12: 0.194|x13: 0.065|x14: 0.184|x15: 0.214|x16: 0.154|x17: 0.000
+TOP2VEC -&gt; x1: 0.236|x2: 0.428|x3: 0.000|x4: 0.316|x5: 0.218|x6: 0.279|x7: 0.348|x8: 0.318|x9: 0.371|x10: 0.118|x11: 0.252|x12: 0.425|x13: 0.195|x14: 0.369|x15: 0.255|x16: 0.243|x17: 0.000
+MEAN -&gt; x1: 0.111|x2: 0.182|x3: 0.167|x4: 0.233|x5: 0.073|x6: 0.093|x7: 0.116|x8: 0.142|x9: 0.180|x10: 0.039|x11: 0.215|x12: 0.194|x13: 0.065|x14: 0.184|x15: 0.214|x16: 0.154|x17: 0.000
+SOFTMAX -&gt; x1: 0.057|x2: 0.061|x3: 0.060|x4: 0.064|x5: 0.055|x6: 0.056|x7: 0.057|x8: 0.059|x9: 0.061|x10: 0.053|x11: 0.063|x12: 0.062|x13: 0.055|x14: 0.061|x15: 0.063|x16: 0.060|x17: 0.051
 </t>
         </is>
       </c>
@@ -5082,7 +5241,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>[2, 13, 14, 15]</t>
+          <t>[13, 14, 15]</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -5090,7 +5249,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.109|x2: 0.000|x3: 0.331|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.191|x12: 0.000|x13: 0.122|x14: 0.169|x15: 0.426|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.151|x2: 0.107|x3: 0.196|x4: 0.124|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.101|x11: 0.000|x12: 0.000|x13: 0.264|x14: 0.143|x15: 0.676|x16: 0.057|x17: 0.000
 TOP2VEC -&gt; x1: 0.150|x2: 0.393|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.106|x9: 0.157|x10: 0.000|x11: 0.230|x12: 0.311|x13: 0.463|x14: 0.393|x15: 0.472|x16: 0.085|x17: 0.000
-MEAN -&gt; x1: 0.137|x2: 0.167|x3: 0.176|x4: 0.041|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.035|x9: 0.052|x10: 0.034|x11: 0.141|x12: 0.104|x13: 0.283|x14: 0.235|x15: 0.525|x16: 0.047|x17: 0.000
+MEAN -&gt; x1: 0.137|x2: 0.167|x3: 0.176|x4: 0.041|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.035|x9: 0.052|x10: 0.034|x11: 0.141|x12: 0.104|x13: 0.283|x14: 0.235|x15: 0.466|x16: 0.047|x17: 0.000
+SOFTMAX -&gt; x1: 0.060|x2: 0.062|x3: 0.062|x4: 0.054|x5: 0.052|x6: 0.052|x7: 0.052|x8: 0.054|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.058|x13: 0.069|x14: 0.066|x15: 0.083|x16: 0.055|x17: 0.052
 </t>
         </is>
       </c>
@@ -5119,7 +5279,8 @@
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.688|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.398|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.054|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.121|x3: 0.116|x4: 0.305|x5: 0.131|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.101|x11: 0.183|x12: 0.059|x13: 0.115|x14: 0.083|x15: 0.396|x16: 0.108|x17: 0.000
 TOP2VEC -&gt; x1: 0.000|x2: 0.084|x3: 0.000|x4: 0.000|x5: 0.195|x6: 0.158|x7: 0.253|x8: 0.000|x9: 0.000|x10: 0.095|x11: 0.239|x12: 0.075|x13: 0.111|x14: 0.247|x15: 0.213|x16: 0.195|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.068|x3: 0.268|x4: 0.102|x5: 0.109|x6: 0.053|x7: 0.084|x8: 0.000|x9: 0.000|x10: 0.065|x11: 0.273|x12: 0.045|x13: 0.075|x14: 0.110|x15: 0.221|x16: 0.101|x17: 0.000
+MEAN -&gt; x1: 0.034|x2: 0.068|x3: 0.205|x4: 0.102|x5: 0.109|x6: 0.053|x7: 0.084|x8: 0.000|x9: 0.000|x10: 0.065|x11: 0.273|x12: 0.045|x13: 0.075|x14: 0.110|x15: 0.221|x16: 0.101|x17: 0.000
+SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.059|x5: 0.060|x6: 0.056|x7: 0.058|x8: 0.054|x9: 0.054|x10: 0.057|x11: 0.070|x12: 0.056|x13: 0.058|x14: 0.060|x15: 0.067|x16: 0.059|x17: 0.054
 </t>
         </is>
       </c>
@@ -5140,7 +5301,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>[3, 11, 12, 16]</t>
+          <t>[3, 11, 16]</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -5149,6 +5310,7 @@
 LDA -&gt; x1: 0.092|x2: 0.146|x3: 0.216|x4: 0.064|x5: 0.096|x6: 0.000|x7: 0.000|x8: 0.167|x9: 0.100|x10: 0.000|x11: 0.207|x12: 0.254|x13: 0.000|x14: 0.064|x15: 0.000|x16: 0.415|x17: 0.000
 TOP2VEC -&gt; x1: 0.078|x2: 0.101|x3: 0.137|x4: 0.168|x5: 0.268|x6: 0.129|x7: 0.000|x8: 0.088|x9: 0.070|x10: 0.143|x11: 0.370|x12: 0.257|x13: 0.098|x14: 0.310|x15: 0.240|x16: 0.293|x17: 0.000
 MEAN -&gt; x1: 0.056|x2: 0.082|x3: 0.227|x4: 0.077|x5: 0.121|x6: 0.043|x7: 0.000|x8: 0.085|x9: 0.057|x10: 0.048|x11: 0.257|x12: 0.170|x13: 0.033|x14: 0.125|x15: 0.080|x16: 0.294|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.066|x4: 0.057|x5: 0.060|x6: 0.055|x7: 0.053|x8: 0.058|x9: 0.056|x10: 0.055|x11: 0.068|x12: 0.063|x13: 0.055|x14: 0.060|x15: 0.057|x16: 0.071|x17: 0.053
 </t>
         </is>
       </c>
@@ -5176,8 +5338,9 @@
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.328|x4: 0.194|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.168|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.365|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.304|x3: 0.115|x4: 0.501|x5: 0.061|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.226|x13: 0.109|x14: 0.000|x15: 0.119|x16: 0.385|x17: 0.000
-TOP2VEC -&gt; x1: 0.169|x2: 0.391|x3: 0.201|x4: 0.430|x5: 0.145|x6: 0.000|x7: 0.062|x8: 0.220|x9: 0.182|x10: 0.139|x11: 0.106|x12: 0.000|x13: 0.122|x14: 0.136|x15: 0.000|x16: 0.284|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.232|x3: 0.214|x4: 0.375|x5: 0.069|x6: 0.000|x7: 0.021|x8: 0.073|x9: 0.061|x10: 0.046|x11: 0.091|x12: 0.075|x13: 0.077|x14: 0.045|x15: 0.040|x16: 0.345|x17: 0.000
+TOP2VEC -&gt; x1: 0.169|x2: 0.391|x3: 0.201|x4: 0.430|x5: 0.145|x6: 0.000|x7: 0.062|x8: 0.220|x9: 0.182|x10: 0.139|x11: 0.106|x12: 0.000|x13: 0.122|x14: 0.137|x15: 0.000|x16: 0.284|x17: 0.000
+MEAN -&gt; x1: 0.056|x2: 0.232|x3: 0.214|x4: 0.375|x5: 0.069|x6: 0.000|x7: 0.021|x8: 0.073|x9: 0.061|x10: 0.046|x11: 0.091|x12: 0.075|x13: 0.077|x14: 0.046|x15: 0.040|x16: 0.345|x17: 0.000
+SOFTMAX -&gt; x1: 0.056|x2: 0.066|x3: 0.065|x4: 0.076|x5: 0.056|x6: 0.053|x7: 0.054|x8: 0.056|x9: 0.056|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.057|x14: 0.055|x15: 0.055|x16: 0.074|x17: 0.053
 </t>
         </is>
       </c>
@@ -5198,15 +5361,16 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>[3, 5, 11]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
           <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.306|x2: 0.097|x3: 0.171|x4: 0.089|x5: 0.206|x6: 0.072|x7: 0.126|x8: 0.074|x9: 0.223|x10: 0.061|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.073|x15: 0.210|x16: 0.113|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.118|x3: 0.319|x4: 0.307|x5: 0.236|x6: 0.072|x7: 0.205|x8: 0.143|x9: 0.183|x10: 0.112|x11: 0.228|x12: 0.301|x13: 0.185|x14: 0.170|x15: 0.130|x16: 0.230|x17: 0.000
+TOP2VEC -&gt; x1: 0.123|x2: 0.118|x3: 0.319|x4: 0.307|x5: 0.236|x6: 0.072|x7: 0.205|x8: 0.143|x9: 0.183|x10: 0.112|x11: 0.228|x12: 0.301|x13: 0.185|x14: 0.171|x15: 0.130|x16: 0.230|x17: 0.000
 MEAN -&gt; x1: 0.143|x2: 0.072|x3: 0.322|x4: 0.132|x5: 0.147|x6: 0.048|x7: 0.110|x8: 0.072|x9: 0.135|x10: 0.058|x11: 0.168|x12: 0.100|x13: 0.062|x14: 0.081|x15: 0.114|x16: 0.114|x17: 0.000
+SOFTMAX -&gt; x1: 0.061|x2: 0.056|x3: 0.073|x4: 0.060|x5: 0.061|x6: 0.055|x7: 0.059|x8: 0.056|x9: 0.060|x10: 0.056|x11: 0.062|x12: 0.058|x13: 0.056|x14: 0.057|x15: 0.059|x16: 0.059|x17: 0.053
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
Votation model revised and models factor adjusted
</commit_message>
<xml_diff>
--- a/Project_python/out/All/all_model.xlsx
+++ b/Project_python/out/All/all_model.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Artificial Intelligence (AI) is displacing jobs and creating an upheaval in the world. It will change the way we work and the way we live. What should be the AI governance, policies, and regulations? How can AI governance, policies, and regulations mitigate and alleviate the negative aspects of AI advancement? How will AI governance, policies, and regulations impact the future of work and the future of humanity? This longitudinal multiple case studies research will study the evolution and revolution of AI governance, policies, and regulations, and how governance, policies and regulations impact AI advancement and are impacted by AI advancement. The research plans to study the top five leading countries in AI research -China, US,</t>
+          <t xml:space="preserve"> artificial intelligence (ai) is displacing jobs and creating an upheaval in the world. it will change the way we work and the way we live. what should be the ai governance, policies, and regulations? how can ai governance, policies, and regulations mitigate and alleviate the negative aspects of ai advancement? how will ai governance, policies, and regulations impact the future of work and the future of humanity? this longitudinal multiple case studies research will study the evolution and revolution of ai governance, policies, and regulations, and how governance, policies and regulations impact ai advancement and are impacted by ai advancement. the research plans to study the top five leading countries in ai research china, us,</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,11 +476,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.327|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.138|x11: 0.202|x12: 0.091|x13: 0.088|x14: 0.066|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.136|x4: 0.141|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.066|x9: 0.186|x10: 0.000|x11: 0.246|x12: 0.159|x13: 0.097|x14: 0.603|x15: 0.000|x16: 0.186|x17: 0.000
-TOP2VEC -&gt; x1: 0.083|x2: 0.198|x3: 0.137|x4: 0.235|x5: 0.268|x6: 0.408|x7: 0.119|x8: 0.077|x9: 0.113|x10: 0.000|x11: 0.263|x12: 0.329|x13: 0.198|x14: 0.404|x15: 0.120|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.066|x3: 0.200|x4: 0.125|x5: 0.089|x6: 0.136|x7: 0.040|x8: 0.048|x9: 0.100|x10: 0.046|x11: 0.237|x12: 0.193|x13: 0.128|x14: 0.323|x15: 0.040|x16: 0.062|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.064|x4: 0.060|x5: 0.057|x6: 0.060|x7: 0.055|x8: 0.055|x9: 0.058|x10: 0.055|x11: 0.067|x12: 0.064|x13: 0.060|x14: 0.073|x15: 0.055|x16: 0.056|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.197|x10: 0.000|x11: 0.173|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.136|x4: 0.141|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.066|x9: 0.186|x10: 0.000|x11: 0.246|x12: 0.159|x13: 0.097|x14: 0.500|x15: 0.000|x16: 0.186|x17: 0.000
+TOP2VEC -&gt; x1: 0.159|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.160|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.133|x12: 0.100|x13: 0.071|x14: 0.240|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.040|x2: 0.000|x3: 0.034|x4: 0.035|x5: 0.000|x6: 0.000|x7: 0.040|x8: 0.017|x9: 0.096|x10: 0.000|x11: 0.138|x12: 0.065|x13: 0.042|x14: 0.185|x15: 0.000|x16: 0.046|x17: 0.000
 </t>
         </is>
       </c>
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Deep learning has in recent years brought breakthroughs in several domains, most notably voice and image recognition. In this work we extend deep learning into a new application domain -namely classification on mobile phone datasets. Classic machine learning methods have produced good results in telecom prediction tasks, but are underutilized due to resource-intensive and domain-specific feature engineering. Moreover, traditional machine learning algorithms require separate feature engineering in different countries. In this work, we show how socio-economic status in large de-identified mobile phone datasets can be accurately classified using deep learning, thus avoiding the cumbersome and manual feature engineering process. We implement a simple deep learning architecture and compare it with traditional data mining models as our benchmarks. On average our model achieves 77% AUC on test data using location traces as the sole input. In contrast, the benchmarked state-of-the-art data mining models include various feature categories such as basic phone usage, top-up pattern, handset type, social network structure and individual mobility. The traditional machine learning models achieve 72% AUC in the best-case scenario. We believe these results are encouraging since average regional household income is an important input to a wide range of economic policies. In underdeveloped countries reliable statistics of income is often lacking, not frequently updated, and is rarely fine-grained to sub-regions of the country. Making income prediction simpler and more efficient can be of great help to policy makers and charity organizations -which will ultimately benefit the poor.</t>
+          <t xml:space="preserve"> deep learning has in recent years brought breakthroughs in several domains, most notably voice and image recognition. in this work we extend deep learning into a new application domain namely classification on mobile phone datasets. classic machine learning methods have produced good results in telecom prediction tasks, but are underutilized due to resource intensive and domain specific feature engineering. moreover, traditional machine learning algorithms require separate feature engineering in different countries. in this work, we show how socio economic status in large de identified mobile phone datasets can be accurately classified using deep learning, thus avoiding the cumbersome and manual feature engineering process. we implement a simple deep learning architecture and compare it with traditional data mining models as our benchmarks. on average our model achieves 77% auc on test data using location traces as the sole input. in contrast, the benchmarked state of the art data mining models include various feature categories such as basic phone usage, top up pattern, handset type, social network structure and individual mobility. the traditional machine learning models achieve 72% auc in the best case scenario. we believe these results are encouraging since average regional household income is an important input to a wide range of economic policies. in underdeveloped countries reliable statistics of income is often lacking, not frequently updated, and is rarely fine grained to sub regions of the country. making income prediction simpler and more efficient can be of great help to policy makers and charity organizations which will ultimately benefit the poor.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,16 +501,16 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[4, 9]</t>
+          <t>[4, 9, 10]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.056|x2: 0.000|x3: 0.805|x4: 0.069|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.130|x11: 0.465|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.140|x2: 0.000|x3: 0.000|x4: 0.260|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.070|x9: 0.116|x10: 0.144|x11: 0.066|x12: 0.062|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.157|x2: 0.175|x3: 0.075|x4: 0.283|x5: 0.000|x6: 0.000|x7: 0.072|x8: 0.302|x9: 0.272|x10: 0.156|x11: 0.000|x12: 0.000|x13: 0.059|x14: 0.120|x15: 0.150|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.179|x2: 0.136|x3: 0.000|x4: 0.461|x5: 0.279|x6: 0.156|x7: 0.293|x8: 0.274|x9: 0.379|x10: 0.093|x11: 0.100|x12: 0.182|x13: 0.076|x14: 0.139|x15: 0.108|x16: 0.190|x17: 0.000
-MEAN -&gt; x1: 0.131|x2: 0.104|x3: 0.192|x4: 0.271|x5: 0.093|x6: 0.052|x7: 0.122|x8: 0.192|x9: 0.217|x10: 0.126|x11: 0.188|x12: 0.061|x13: 0.045|x14: 0.086|x15: 0.086|x16: 0.063|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.063|x4: 0.068|x5: 0.057|x6: 0.055|x7: 0.059|x8: 0.063|x9: 0.065|x10: 0.059|x11: 0.063|x12: 0.055|x13: 0.054|x14: 0.057|x15: 0.057|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.129|x2: 0.096|x3: 0.000|x4: 0.161|x5: 0.000|x6: 0.000|x7: 0.148|x8: 0.054|x9: 0.212|x10: 0.116|x11: 0.157|x12: 0.229|x13: 0.123|x14: 0.216|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.385|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.106|x2: 0.068|x3: 0.019|x4: 0.176|x5: 0.000|x6: 0.000|x7: 0.055|x8: 0.106|x9: 0.150|x10: 0.200|x11: 0.056|x12: 0.073|x13: 0.045|x14: 0.084|x15: 0.037|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Drought over a period threatens the water resources, agriculture, and socioeconomic activities. Therefore, it is crucial for decision makers to have a realistic anticipation of drought events to mitigate its impacts. Hence, this research aims at using the standardized precipitation index (SPI) to predict drought through time series analysis techniques. These adopted techniques are autoregressive integrating moving average (ARIMA) and feed-forward backpropagation neural network (FBNN) with different activation functions (sigmoid, bipolar sigmoid, and hyperbolic tangent). After that, the adequacy of these two techniques in predicting the drought conditions has been examined under arid ecosystems. The monthly precipitation data used in calculating the SPI time series (SPI 3, 6, 12, and 24 timescales) have been obtained from the tropical rainfall measuring mission (TRMM). The prediction of SPI was carried out and compared over six lead times from 1 to 6 using the model performance statistics (coefficient of correlation (R), mean absolute error (MAE), and root mean square error (RMSE)). The overall results prove an excellent performance of both predicting models for anticipating the drought conditions concerning model accuracy measures. Despite this, the FBNN models remain somewhat better than ARIMA models with R ≥ 0.7865, MAE ≤ 1.0637, and RMSE ≤ 1.2466. Additionally, the FBNN based on hyperbolic tangent activation function demonstrated the best similarity between actual and predicted for SPI 24 by 98.44%. Eventually, all the activation function of FBNN models has good results respecting the SPI prediction with a small degree of variation among timescales. Therefore, any of these activation functions can be used equally even if the sigmoid and bipolar sigmoid functions are manifesting less adjusted R 2 and higher errors (MAE and RMSE). In conclusion, the FBNN can be considered a promising technique for predicting the SPI as a drought monitoring index under arid ecosystems.</t>
+          <t xml:space="preserve"> drought over a period threatens the water resources, agriculture, and socioeconomic activities. therefore, it is crucial for decision makers to have a realistic anticipation of drought events to mitigate its impacts. hence, this research aims at using the standardized precipitation index (spi) to predict drought through time series analysis techniques. these adopted techniques are autoregressive integrating moving average (arima) and feed forward backpropagation neural network (fbnn) with different activation functions (sigmoid, bipolar sigmoid, and hyperbolic tangent). after that, the adequacy of these two techniques in predicting the drought conditions has been examined under arid ecosystems. the monthly precipitation data used in calculating the spi time series (spi 3, 6, 12, and 24 timescales) have been obtained from the tropical rainfall measuring mission (trmm). the prediction of spi was carried out and compared over six lead times from 1 to 6 using the model performance statistics (coefficient of correlation (r), mean absolute error (mae), and root mean square error (rmse)). the overall results prove an excellent performance of both predicting models for anticipating the drought conditions concerning model accuracy measures. despite this, the fbnn models remain somewhat better than arima models with r ≥ 0.7865, mae ≤ 1.0637, and rmse ≤ 1.2466. additionally, the fbnn based on hyperbolic tangent activation function demonstrated the best similarity between actual and predicted for spi 24 by 98.44%. eventually, all the activation function of fbnn models has good results respecting the spi prediction with a small degree of variation among timescales. therefore, any of these activation functions can be used equally even if the sigmoid and bipolar sigmoid functions are manifesting less adjusted r 2 and higher errors (mae and rmse). in conclusion, the fbnn can be considered a promising technique for predicting the spi as a drought monitoring index under arid ecosystems.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -531,16 +531,16 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.620|x4: 0.000|x5: 0.000|x6: 0.089|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.358|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.139|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.290|x7: 0.000|x8: 0.000|x9: 0.074|x10: 0.000|x11: 0.000|x12: 0.080|x13: 0.000|x14: 0.078|x15: 0.138|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.118|x2: 0.229|x3: 0.111|x4: 0.190|x5: 0.227|x6: 0.114|x7: 0.065|x8: 0.073|x9: 0.129|x10: 0.078|x11: 0.000|x12: 0.054|x13: 0.068|x14: 0.148|x15: 0.063|x16: 0.153|x17: 0.000
-TOP2VEC -&gt; x1: 0.190|x2: 0.131|x3: 0.000|x4: 0.234|x5: 0.192|x6: 0.184|x7: 0.407|x8: 0.224|x9: 0.282|x10: 0.065|x11: 0.222|x12: 0.118|x13: 0.278|x14: 0.214|x15: 0.259|x16: 0.134|x17: 0.000
-MEAN -&gt; x1: 0.103|x2: 0.120|x3: 0.204|x4: 0.141|x5: 0.140|x6: 0.129|x7: 0.158|x8: 0.099|x9: 0.137|x10: 0.048|x11: 0.194|x12: 0.057|x13: 0.115|x14: 0.121|x15: 0.107|x16: 0.096|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.059|x3: 0.064|x4: 0.060|x5: 0.060|x6: 0.060|x7: 0.061|x8: 0.058|x9: 0.060|x10: 0.055|x11: 0.064|x12: 0.055|x13: 0.059|x14: 0.059|x15: 0.058|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.126|x3: 0.000|x4: 0.000|x5: 0.064|x6: 0.057|x7: 0.133|x8: 0.099|x9: 0.057|x10: 0.200|x11: 0.217|x12: 0.151|x13: 0.065|x14: 0.163|x15: 0.182|x16: 0.069|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.500|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.029|x2: 0.124|x3: 0.028|x4: 0.047|x5: 0.073|x6: 0.115|x7: 0.050|x8: 0.043|x9: 0.065|x10: 0.069|x11: 0.054|x12: 0.071|x13: 0.158|x14: 0.098|x15: 0.096|x16: 0.055|x17: 0.000
 </t>
         </is>
       </c>
@@ -551,7 +551,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper is aimed at making recommendations to establish a stewardship to embody the responsibilities and morality that will prevent the automation risks faced by Least Development Countries (LDCs) due to transition toward digital modernity. Recent studies reveal that law qualified individuals in developed countries will face the risks of jobs that are highly subject to automation. This indicates that corresponding risks will be seen in LDCs. The rise of digitalization may override developing country's opportunities to elevate itself from a low-income country to a middle or high-income country. In the aftermath of World War Ⅱ, western society tried to support LDCs in maintain the principles of a free world system and contribute to reducing poverty through market oriented development. Since the end of Cold War, defense of the free world has lost its significance but economy is getting more important political instrument. Advancement of automation technologies might aggravate opportunities for developing country's economic growth and international society needs the alternative principles.</t>
+          <t xml:space="preserve"> this paper is aimed at making recommendations to establish a stewardship to embody the responsibilities and morality that will prevent the automation risks faced by least development countries (ldcs) due to transition toward digital modernity. recent studies reveal that law qualified individuals in developed countries will face the risks of jobs that are highly subject to automation. this indicates that corresponding risks will be seen in ldcs. the rise of digitalization may override developing countrys opportunities to elevate itself from a low income country to a middle or high income country. in the aftermath of world war ⅱ, western society tried to support ldcs in maintain the principles of a free world system and contribute to reducing poverty through market oriented development. since the end of cold war, defense of the free world has lost its significance but economy is getting more important political instrument. advancement of automation technologies might aggravate opportunities for developing countrys economic growth and international society needs the alternative principles.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -561,16 +561,16 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[4, 8, 10]</t>
+          <t>[1, 8, 9, 10, 16]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.211|x2: 0.000|x3: 0.113|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.169|x9: 0.000|x10: 0.941|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.247|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.260|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.198|x9: 0.110|x10: 0.500|x11: 0.069|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.267|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.143|x3: 0.203|x4: 0.195|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.374|x9: 0.080|x10: 0.475|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.247|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.169|x2: 0.107|x3: 0.000|x4: 0.468|x5: 0.297|x6: 0.161|x7: 0.443|x8: 0.209|x9: 0.209|x10: 0.060|x11: 0.000|x12: 0.132|x13: 0.183|x14: 0.124|x15: 0.000|x16: 0.123|x17: 0.000
-MEAN -&gt; x1: 0.161|x2: 0.084|x3: 0.105|x4: 0.221|x5: 0.099|x6: 0.054|x7: 0.148|x8: 0.251|x9: 0.096|x10: 0.345|x11: 0.022|x12: 0.044|x13: 0.061|x14: 0.123|x15: 0.000|x16: 0.124|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.057|x3: 0.058|x4: 0.065|x5: 0.058|x6: 0.055|x7: 0.061|x8: 0.067|x9: 0.058|x10: 0.074|x11: 0.053|x12: 0.055|x13: 0.056|x14: 0.059|x15: 0.052|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.265|x2: 0.000|x3: 0.066|x4: 0.093|x5: 0.000|x6: 0.000|x7: 0.129|x8: 0.304|x9: 0.302|x10: 0.197|x11: 0.182|x12: 0.000|x13: 0.128|x14: 0.000|x15: 0.000|x16: 0.240|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.157|x2: 0.036|x3: 0.067|x4: 0.072|x5: 0.000|x6: 0.000|x7: 0.032|x8: 0.219|x9: 0.123|x10: 0.293|x11: 0.063|x12: 0.000|x13: 0.032|x14: 0.062|x15: 0.000|x16: 0.127|x17: 0.000
 </t>
         </is>
       </c>
@@ -581,7 +581,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Smart Farming is a development that emphasizes the use of information and communication technology in the cyber-physical farm management cycle. New technologies such as the Internet of Things and Cloud Computing are expected to leverage this development and introduce more robots and artificial intelligence in farming. This is encompassed by the phenomenon of Big Data, massive volumes of data with a wide variety that can be captured, analysed and used for decision-making. This review aims to gain insight into the state-of-the-art of Big Data applications in Smart Farming and identify the related socio-economic challenges to be addressed. Following a structured approach, a conceptual framework for analysis was developed that can also be used for future studies on this topic. The review shows that the scope of Big Data applications in Smart Farming goes beyond primary production; it is influencing the entire food supply chain. Big data are being used to provide predictive insights in farming operations, drive real-time operational decisions, and redesign business processes for game-changing business models. Several authors therefore suggest that Big Data will cause major shifts in roles and power relations among different players in current food supply chain networks. The landscape of stakeholders exhibits an interesting game between powerful tech companies, venture capitalists and often small startups and new entrants. At the same time there are several public institutions that publish open data, under the condition that the privacy of persons must be guaranteed. The future of Smart Farming may unravel in a continuum of two extreme scenarios: 1) closed, proprietary systems in which the farmer is part of a highly integrated food supply chain or 2) open, collaborative systems in which the farmer and every other stakeholder in the chain network is flexible in choosing business partners as well for the technology as for the food production side. The further development of data and application infrastructures (platforms and standards) and their institutional embedment will play a crucial role in the battle between these scenarios. From a socio-economic perspective, the authors propose to give research priority to organizational issues concerning governance issues and suitable business models for data sharing in different supply chain scenarios.</t>
+          <t xml:space="preserve"> smart farming is a development that emphasizes the use of information and communication technology in the cyber physical farm management cycle. new technologies such as the internet of things and cloud computing are expected to leverage this development and introduce more robots and artificial intelligence in farming. this is encompassed by the phenomenon of big data, massive volumes of data with a wide variety that can be captured, analysed and used for decision making. this review aims to gain insight into the state of the art of big data applications in smart farming and identify the related socio economic challenges to be addressed. following a structured approach, a conceptual framework for analysis was developed that can also be used for future studies on this topic. the review shows that the scope of big data applications in smart farming goes beyond primary production; it is influencing the entire food supply chain. big data are being used to provide predictive insights in farming operations, drive real time operational decisions, and redesign business processes for game changing business models. several authors therefore suggest that big data will cause major shifts in roles and power relations among different players in current food supply chain networks. the landscape of stakeholders exhibits an interesting game between powerful tech companies, venture capitalists and often small startups and new entrants. at the same time there are several public institutions that publish open data, under the condition that the privacy of persons must be guaranteed. the future of smart farming may unravel in a continuum of two extreme scenarios: 1) closed, proprietary systems in which the farmer is part of a highly integrated food supply chain or 2) open, collaborative systems in which the farmer and every other stakeholder in the chain network is flexible in choosing business partners as well for the technology as for the food production side. the further development of data and application infrastructures (platforms and standards) and their institutional embedment will play a crucial role in the battle between these scenarios. from a socio economic perspective, the authors propose to give research priority to organizational issues concerning governance issues and suitable business models for data sharing in different supply chain scenarios.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -591,16 +591,16 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[2, 9, 12]</t>
+          <t>[2, 9]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.116|x3: 0.495|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.091|x10: 0.000|x11: 0.311|x12: 0.204|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.189|x10: 0.000|x11: 0.108|x12: 0.123|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.390|x3: 0.102|x4: 0.138|x5: 0.000|x6: 0.190|x7: 0.155|x8: 0.000|x9: 0.433|x10: 0.000|x11: 0.000|x12: 0.068|x13: 0.111|x14: 0.059|x15: 0.068|x16: 0.105|x17: 0.000
-TOP2VEC -&gt; x1: 0.110|x2: 0.285|x3: 0.000|x4: 0.146|x5: 0.066|x6: 0.206|x7: 0.254|x8: 0.117|x9: 0.309|x10: 0.000|x11: 0.166|x12: 0.453|x13: 0.302|x14: 0.299|x15: 0.276|x16: 0.103|x17: 0.000
-MEAN -&gt; x1: 0.037|x2: 0.263|x3: 0.199|x4: 0.095|x5: 0.022|x6: 0.132|x7: 0.136|x8: 0.039|x9: 0.278|x10: 0.000|x11: 0.159|x12: 0.242|x13: 0.138|x14: 0.119|x15: 0.115|x16: 0.069|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.068|x3: 0.063|x4: 0.057|x5: 0.053|x6: 0.059|x7: 0.060|x8: 0.054|x9: 0.069|x10: 0.052|x11: 0.061|x12: 0.066|x13: 0.060|x14: 0.059|x15: 0.058|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.065|x7: 0.285|x8: 0.000|x9: 0.106|x10: 0.000|x11: 0.220|x12: 0.231|x13: 0.000|x14: 0.150|x15: 0.062|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.347|x3: 0.026|x4: 0.034|x5: 0.000|x6: 0.064|x7: 0.110|x8: 0.000|x9: 0.182|x10: 0.000|x11: 0.082|x12: 0.106|x13: 0.028|x14: 0.052|x15: 0.032|x16: 0.026|x17: 0.000
 </t>
         </is>
       </c>
@@ -611,7 +611,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper describes a fruit counting pipeline based on deep learning that accurately counts fruit in unstructured environments. Obtaining reliable fruit counts is challenging because of variations in appearance due to illumination changes and occlusions from foliage and neighboring fruits. We propose a novel approach that uses deep learning to map from input images to total fruit counts. The pipeline utilizes a custom crowd-sourcing platform to quickly label large data sets. A blob detector based on a fully convolutional network extracts candidate regions in the images. A counting algorithm based on a second convolutional network then estimates the number of fruit in each region. Finally, a linear regression model maps that fruit count estimate to a final fruit count. We analyze the performance of the pipeline on two distinct data sets of oranges in daylight, and green apples at night, utilizing human generated labels as ground truth. We also show that the pipeline has a short training time and performs well with a limited data set size. Our method generalizes across both data sets and is able to perform well even on highly occluded fruits that are challenging for human labelers to annotate.</t>
+          <t xml:space="preserve"> this paper describes a fruit counting pipeline based on deep learning that accurately counts fruit in unstructured environments. obtaining reliable fruit counts is challenging because of variations in appearance due to illumination changes and occlusions from foliage and neighboring fruits. we propose a novel approach that uses deep learning to map from input images to total fruit counts. the pipeline utilizes a custom crowd sourcing platform to quickly label large data sets. a blob detector based on a fully convolutional network extracts candidate regions in the images. a counting algorithm based on a second convolutional network then estimates the number of fruit in each region. finally, a linear regression model maps that fruit count estimate to a final fruit count. we analyze the performance of the pipeline on two distinct data sets of oranges in daylight, and green apples at night, utilizing human generated labels as ground truth. we also show that the pipeline has a short training time and performs well with a limited data set size. our method generalizes across both data sets and is able to perform well even on highly occluded fruits that are challenging for human labelers to annotate.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -621,16 +621,16 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[3, 11]</t>
+          <t>[4, 9, 11, 15]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.549|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.318|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.201|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.132|x10: 0.000|x11: 0.148|x12: 0.000|x13: 0.000|x14: 0.085|x15: 0.000|x16: 0.107|x17: 0.000
 LDA -&gt; x1: 0.128|x2: 0.156|x3: 0.253|x4: 0.183|x5: 0.077|x6: 0.000|x7: 0.070|x8: 0.128|x9: 0.108|x10: 0.000|x11: 0.196|x12: 0.000|x13: 0.268|x14: 0.067|x15: 0.082|x16: 0.103|x17: 0.000
-TOP2VEC -&gt; x1: 0.248|x2: 0.077|x3: 0.000|x4: 0.373|x5: 0.118|x6: 0.124|x7: 0.247|x8: 0.264|x9: 0.131|x10: 0.080|x11: 0.545|x12: 0.225|x13: 0.323|x14: 0.211|x15: 0.134|x16: 0.163|x17: 0.000
-MEAN -&gt; x1: 0.125|x2: 0.078|x3: 0.251|x4: 0.185|x5: 0.065|x6: 0.041|x7: 0.106|x8: 0.131|x9: 0.080|x10: 0.027|x11: 0.338|x12: 0.075|x13: 0.197|x14: 0.092|x15: 0.072|x16: 0.089|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.056|x3: 0.067|x4: 0.063|x5: 0.056|x6: 0.054|x7: 0.058|x8: 0.060|x9: 0.057|x10: 0.054|x11: 0.073|x12: 0.056|x13: 0.064|x14: 0.057|x15: 0.056|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.216|x5: 0.229|x6: 0.358|x7: 0.435|x8: 0.000|x9: 0.245|x10: 0.000|x11: 0.500|x12: 0.303|x13: 0.000|x14: 0.000|x15: 0.135|x16: 0.095|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.375|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.032|x2: 0.039|x3: 0.063|x4: 0.150|x5: 0.076|x6: 0.089|x7: 0.126|x8: 0.032|x9: 0.121|x10: 0.000|x11: 0.211|x12: 0.076|x13: 0.067|x14: 0.038|x15: 0.148|x16: 0.077|x17: 0.000
 </t>
         </is>
       </c>
@@ -641,7 +641,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In recent years, Deep Learning (DL), such as the algorithms of Convolutional Neural Networks (CNN), Recurrent Neural Networks (RNN) and Generative Adversarial Networks (GAN), has been widely studied and applied in various fields including agriculture. Researchers in the fields of agriculture often use software frameworks without sufficiently examining the ideas and mechanisms of a technique. This article provides a concise summary of major DL algorithms, including concepts, limitations, implementation, training processes, and example codes, to help researchers in agriculture to gain a holistic picture of major DL techniques quickly. Research on DL applications in agriculture is summarized and analyzed, and future opportunities are discussed in this paper, which is expected to help researchers in agriculture to better understand DL algorithms and learn major DL techniques quickly, and further to facilitate data analysis, enhance related research in agriculture, and thus promote DL applications effectively.</t>
+          <t xml:space="preserve"> in recent years, deep learning (dl), such as the algorithms of convolutional neural networks (cnn), recurrent neural networks (rnn) and generative adversarial networks (gan), has been widely studied and applied in various fields including agriculture. researchers in the fields of agriculture often use software frameworks without sufficiently examining the ideas and mechanisms of a technique. this article provides a concise summary of major dl algorithms, including concepts, limitations, implementation, training processes, and example codes, to help researchers in agriculture to gain a holistic picture of major dl techniques quickly. research on dl applications in agriculture is summarized and analyzed, and future opportunities are discussed in this paper, which is expected to help researchers in agriculture to better understand dl algorithms and learn major dl techniques quickly, and further to facilitate data analysis, enhance related research in agriculture, and thus promote dl applications effectively.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -651,16 +651,16 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[2, 3, 9]</t>
+          <t>[2, 9]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.080|x3: 0.663|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.383|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.332|x3: 0.000|x4: 0.081|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.229|x10: 0.000|x11: 0.069|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.257|x3: 0.130|x4: 0.155|x5: 0.081|x6: 0.000|x7: 0.084|x8: 0.154|x9: 0.315|x10: 0.000|x11: 0.000|x12: 0.074|x13: 0.211|x14: 0.000|x15: 0.236|x16: 0.125|x17: 0.000
-TOP2VEC -&gt; x1: 0.173|x2: 0.423|x3: 0.000|x4: 0.285|x5: 0.000|x6: 0.141|x7: 0.448|x8: 0.239|x9: 0.553|x10: 0.122|x11: 0.216|x12: 0.187|x13: 0.292|x14: 0.344|x15: 0.257|x16: 0.249|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.253|x3: 0.210|x4: 0.147|x5: 0.027|x6: 0.047|x7: 0.177|x8: 0.131|x9: 0.272|x10: 0.041|x11: 0.200|x12: 0.087|x13: 0.168|x14: 0.115|x15: 0.164|x16: 0.125|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.066|x3: 0.064|x4: 0.060|x5: 0.053|x6: 0.054|x7: 0.061|x8: 0.059|x9: 0.068|x10: 0.054|x11: 0.063|x12: 0.056|x13: 0.061|x14: 0.058|x15: 0.061|x16: 0.058|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.099|x5: 0.000|x6: 0.000|x7: 0.220|x8: 0.114|x9: 0.304|x10: 0.101|x11: 0.226|x12: 0.216|x13: 0.257|x14: 0.000|x15: 0.234|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.432|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.255|x3: 0.033|x4: 0.084|x5: 0.020|x6: 0.000|x7: 0.076|x8: 0.067|x9: 0.212|x10: 0.025|x11: 0.074|x12: 0.072|x13: 0.117|x14: 0.000|x15: 0.117|x16: 0.031|x17: 0.000
 </t>
         </is>
       </c>
@@ -671,7 +671,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Then detection and identification of extreme weather events in large-scale climate simulations is an important problem for risk management, informing governmental policy decisions and advancing our basic understanding of the climate system. Recent work has shown that fully supervised convolutional neural networks (CNNs) can yield acceptable accuracy for classifying well-known types of extreme weather events when large amounts of labeled data are available. However, many different types of spatially localized climate patterns are of interest including hurricanes, extra-tropical cyclones, weather fronts, and blocking events among others. Existing labeled data for these patterns can be incomplete in various ways, such as covering only certain years or geographic areas and having false negatives. This type of climate data therefore poses a number of interesting machine learning challenges. We present a multichannel spatiotemporal CNN architecture for semi-supervised bounding box prediction and exploratory data analysis. We demonstrate that our approach is able to leverage temporal information and unlabeled data to improve the localization of extreme weather events. Further, we explore the representations learned by our model in order to better understand this important data. We present a dataset, ExtremeWeather, to encourage machine learning research in this area and to help facilitate further work in understanding and mitigating the effects of climate change. The dataset is available at extremeweatherdataset.github.io and the code is available at https://github.com/eracah/hur-detect.</t>
+          <t xml:space="preserve"> then detection and identification of extreme weather events in large scale climate simulations is an important problem for risk management, informing governmental policy decisions and advancing our basic understanding of the climate system. recent work has shown that fully supervised convolutional neural networks (cnns) can yield acceptable accuracy for classifying well known types of extreme weather events when large amounts of labeled data are available. however, many different types of spatially localized climate patterns are of interest including hurricanes, extra tropical cyclones, weather fronts, and blocking events among others. existing labeled data for these patterns can be incomplete in various ways, such as covering only certain years or geographic areas and having false negatives. this type of climate data therefore poses a number of interesting machine learning challenges. we present a multichannel spatiotemporal cnn architecture for semi supervised bounding box prediction and exploratory data analysis. we demonstrate that our approach is able to leverage temporal information and unlabeled data to improve the localization of extreme weather events. further, we explore the representations learned by our model in order to better understand this important data. we present a dataset, extremeweather, to encourage machine learning research in this area and to help facilitate further work in understanding and mitigating the effects of climate change. the dataset is available at extremeweatherdataset.github.io and the code is available at https://github.com/eracah/hur detect.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -681,16 +681,16 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[3, 13]</t>
+          <t>[1, 2, 13]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.095|x2: 0.000|x3: 0.543|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.314|x12: 0.000|x13: 0.542|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.204|x2: 0.000|x3: 0.000|x4: 0.088|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.500|x14: 0.000|x15: 0.117|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.174|x2: 0.311|x3: 0.182|x4: 0.225|x5: 0.112|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.127|x13: 0.116|x14: 0.217|x15: 0.130|x16: 0.224|x17: 0.000
-TOP2VEC -&gt; x1: 0.193|x2: 0.117|x3: 0.000|x4: 0.227|x5: 0.224|x6: 0.081|x7: 0.151|x8: 0.194|x9: 0.184|x10: 0.061|x11: 0.135|x12: 0.217|x13: 0.351|x14: 0.356|x15: 0.121|x16: 0.125|x17: 0.000
-MEAN -&gt; x1: 0.154|x2: 0.143|x3: 0.227|x4: 0.151|x5: 0.112|x6: 0.027|x7: 0.050|x8: 0.065|x9: 0.061|x10: 0.020|x11: 0.150|x12: 0.115|x13: 0.322|x14: 0.191|x15: 0.084|x16: 0.116|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.060|x3: 0.065|x4: 0.061|x5: 0.058|x6: 0.054|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.053|x11: 0.061|x12: 0.059|x13: 0.072|x14: 0.063|x15: 0.057|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.120|x2: 0.218|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.116|x8: 0.000|x9: 0.000|x10: 0.192|x11: 0.085|x12: 0.083|x13: 0.193|x14: 0.176|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.067|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.500|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.141|x2: 0.132|x3: 0.046|x4: 0.078|x5: 0.028|x6: 0.000|x7: 0.029|x8: 0.000|x9: 0.000|x10: 0.048|x11: 0.021|x12: 0.053|x13: 0.327|x14: 0.098|x15: 0.062|x16: 0.056|x17: 0.000
 </t>
         </is>
       </c>
@@ -701,7 +701,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This study aims to project future variability of reference evapotranspiration (ET 0 ) using artificial intelligence methods, constructed with an extreme-learning machine (ELM) and support vector regression (SVR) in a mountainous inland watershed in north-west China. Eight global climate model (GCM) outputs retrieved from the Coupled Model Inter-comparison Project Phase 5 (CMIP5) were employed to downscale monthly ET 0 for the historical period 1960-2005 as a validation approach and for the future period 2010-2099 as a projection of ET 0 under the Representative Concentration Pathway (RCP) 4.5 and 8.5 scenarios. The following conclusions can be drawn: the ELM and SVR methods demonstrate a very good performance in estimating Food and Agriculture Organization (FAO)-56 Penman-Monteith ET 0 . Variation in future ET 0 mainly occurs in the spring and autumn seasons, while the summer and winter ET 0 changes are moderately small. Annually, the ET 0 values were shown to increase at a rate of approximately 7.5 mm, 7.5 mm, 0.0 mm (8.2 mm, 15.0 mm, 15.0 mm) decade −1 , respectively, for the near-term projection (2010-2039), mid-term projection (2040-2069), and long-term projection (2070-2099) under the RCP4.5 (RCP8.5) scenario. Compared to the historical period, the relative changes in ET 0 were found to be approximately 2%, 5% and 6% (2%, 7% and 13%), during the near, mid-and long-term periods, respectively, under the RCP4.5 (RCP8.5) warming scenarios. In accordance with the analyses, we aver that the opportunity to downscale monthly ET 0 with artificial intelligence is useful in practice for water-management policies.</t>
+          <t xml:space="preserve"> this study aims to project future variability of reference evapotranspiration (et 0 ) using artificial intelligence methods, constructed with an extreme learning machine (elm) and support vector regression (svr) in a mountainous inland watershed in north west china. eight global climate model (gcm) outputs retrieved from the coupled model inter comparison project phase 5 (cmip5) were employed to downscale monthly et 0 for the historical period 1960 2005 as a validation approach and for the future period 2010 2099 as a projection of et 0 under the representative concentration pathway (rcp) 4.5 and 8.5 scenarios. the following conclusions can be drawn: the elm and svr methods demonstrate a very good performance in estimating food and agriculture organization (fao) 56 penman monteith et 0 . variation in future et 0 mainly occurs in the spring and autumn seasons, while the summer and winter et 0 changes are moderately small. annually, the et 0 values were shown to increase at a rate of approximately 7.5 mm, 7.5 mm, 0.0 mm (8.2 mm, 15.0 mm, 15.0 mm) decade −1 , respectively, for the near term projection (2010 2039), mid term projection (2040 2069), and long term projection (2070 2099) under the rcp4.5 (rcp8.5) scenario. compared to the historical period, the relative changes in et 0 were found to be approximately 2%, 5% and 6% (2%, 7% and 13%), during the near, mid and long term periods, respectively, under the rcp4.5 (rcp8.5) warming scenarios. in accordance with the analyses, we aver that the opportunity to downscale monthly et 0 with artificial intelligence is useful in practice for water management policies.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -711,16 +711,16 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 13]</t>
+          <t>[2, 9, 13]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.510|x4: 0.000|x5: 0.000|x6: 0.113|x7: 0.000|x8: 0.067|x9: 0.000|x10: 0.000|x11: 0.295|x12: 0.000|x13: 0.302|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.075|x2: 0.236|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.182|x7: 0.000|x8: 0.000|x9: 0.139|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.220|x14: 0.000|x15: 0.079|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.146|x2: 0.124|x3: 0.180|x4: 0.259|x5: 0.000|x6: 0.000|x7: 0.105|x8: 0.131|x9: 0.217|x10: 0.159|x11: 0.061|x12: 0.000|x13: 0.200|x14: 0.108|x15: 0.130|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.189|x2: 0.154|x3: 0.000|x4: 0.276|x5: 0.084|x6: 0.291|x7: 0.446|x8: 0.236|x9: 0.406|x10: 0.000|x11: 0.245|x12: 0.129|x13: 0.298|x14: 0.182|x15: 0.112|x16: 0.072|x17: 0.000
-MEAN -&gt; x1: 0.111|x2: 0.093|x3: 0.227|x4: 0.178|x5: 0.028|x6: 0.135|x7: 0.184|x8: 0.145|x9: 0.208|x10: 0.053|x11: 0.200|x12: 0.043|x13: 0.266|x14: 0.097|x15: 0.081|x16: 0.024|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.057|x3: 0.065|x4: 0.062|x5: 0.053|x6: 0.059|x7: 0.062|x8: 0.060|x9: 0.064|x10: 0.055|x11: 0.063|x12: 0.054|x13: 0.068|x14: 0.057|x15: 0.056|x16: 0.053|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.171|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.130|x7: 0.105|x8: 0.086|x9: 0.161|x10: 0.151|x11: 0.208|x12: 0.218|x13: 0.181|x14: 0.060|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.244|x2: 0.176|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.125|x12: 0.074|x13: 0.366|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.116|x2: 0.177|x3: 0.045|x4: 0.065|x5: 0.000|x6: 0.078|x7: 0.052|x8: 0.054|x9: 0.129|x10: 0.077|x11: 0.099|x12: 0.073|x13: 0.242|x14: 0.042|x15: 0.052|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -731,7 +731,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper examines the use of remote sensing satellite data to predict food shortages among different categories of households in famine-prone areas. Normalized Difference Vegetation Index (NDVI) and rainfall estimate data, which can be derived from multi-spectral satellite radiometer images, has long been used to predict crop yields and hence famine. This gives an overall prediction of food insecurity in an area, though in a heterogeneous population it does not directly predict which sectors of society or households are most at risk. In this work we use information on 3094 households across Uganda collected between 2004-2005. We describe a method for clustering households in such a way that the cluster decision boundaries are both relevant for improved-specificity famine prediction and are easily communicated. We then give classification results for predicting food security status at a household level given different combinations of satellite data, demographic data, and household category indices found by our clustering method. The food security classification performance of this model demonstrates the potential of this approach for making predictions of famine for specific areas and demographic groups.</t>
+          <t xml:space="preserve"> this paper examines the use of remote sensing satellite data to predict food shortages among different categories of households in famine prone areas. normalized difference vegetation index (ndvi) and rainfall estimate data, which can be derived from multi spectral satellite radiometer images, has long been used to predict crop yields and hence famine. this gives an overall prediction of food insecurity in an area, though in a heterogeneous population it does not directly predict which sectors of society or households are most at risk. in this work we use information on 3094 households across uganda collected between 2004 2005. we describe a method for clustering households in such a way that the cluster decision boundaries are both relevant for improved specificity famine prediction and are easily communicated. we then give classification results for predicting food security status at a household level given different combinations of satellite data, demographic data, and household category indices found by our clustering method. the food security classification performance of this model demonstrates the potential of this approach for making predictions of famine for specific areas and demographic groups.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -741,16 +741,16 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[2]</t>
+          <t>[2, 15]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.175|x3: 0.446|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.258|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.068|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.063|x12: 0.066|x13: 0.000|x14: 0.000|x15: 0.189|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.077|x2: 0.462|x3: 0.000|x4: 0.315|x5: 0.105|x6: 0.000|x7: 0.000|x8: 0.075|x9: 0.152|x10: 0.216|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.086|x15: 0.195|x16: 0.071|x17: 0.000
-TOP2VEC -&gt; x1: 0.254|x2: 0.239|x3: 0.137|x4: 0.151|x5: 0.225|x6: 0.000|x7: 0.371|x8: 0.294|x9: 0.131|x10: 0.100|x11: 0.269|x12: 0.245|x13: 0.236|x14: 0.189|x15: 0.207|x16: 0.205|x17: 0.000
-MEAN -&gt; x1: 0.110|x2: 0.292|x3: 0.194|x4: 0.155|x5: 0.110|x6: 0.000|x7: 0.124|x8: 0.123|x9: 0.094|x10: 0.106|x11: 0.198|x12: 0.082|x13: 0.079|x14: 0.092|x15: 0.157|x16: 0.092|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.070|x3: 0.063|x4: 0.061|x5: 0.058|x6: 0.052|x7: 0.059|x8: 0.059|x9: 0.057|x10: 0.058|x11: 0.064|x12: 0.057|x13: 0.056|x14: 0.057|x15: 0.061|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.141|x2: 0.071|x3: 0.000|x4: 0.077|x5: 0.153|x6: 0.000|x7: 0.134|x8: 0.054|x9: 0.000|x10: 0.139|x11: 0.143|x12: 0.067|x13: 0.000|x14: 0.119|x15: 0.109|x16: 0.066|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.055|x2: 0.383|x3: 0.000|x4: 0.098|x5: 0.065|x6: 0.000|x7: 0.034|x8: 0.032|x9: 0.038|x10: 0.089|x11: 0.068|x12: 0.033|x13: 0.000|x14: 0.051|x15: 0.123|x16: 0.034|x17: 0.000
 </t>
         </is>
       </c>
@@ -761,7 +761,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Inadequacy of spatial soil information is one of the limiting factors to making evidence-based decisions to improve food security and land management in the developing countries. Various digital soil mapping (DSM) techniques have been applied in many parts of the world to improve availability and usability of soil data, but less has been done in Africa, particularly in Tanzania and at the scale necessary to make farm management decisions. The Kilombero Valley has been identified for intensified rice production. However the valley lacks detailed and up-todate soil information for decision-making. The overall objective of this study was to develop a predictive soil map of a portion of Kilombero Valley using DSM techniques. Two widely used decision tree algorithms and three sources of Digital Elevation Models (DEMs) were evaluated for their predictive ability. Firstly, a numerical classification was performed on the collected soil profile data to arrive at soil taxa. Secondly, the derived taxa were spatially predicted and mapped following SCORPAN framework using Random Forest (RF) and J48 machine learning algorithms. Datasets to train the model were derived from legacy soil map, RapidEye satellite image and three DEMs: 1 arc SRTM, 30 m ASTER, and 12 m WorldDEM. Separate predictive models were built using each DEM source. Mapping showed that RF was less sensitive to the training set sampling intensity. Results also showed that predictions of soil taxa using 1 arc SRTM and 12 m WordDEM were identical. We suggest the use of RF algorithm and the freely available SRTM DEM combination for mapping the soils for the whole Kilombero Valley. This combination can be tested and applied in other areas which have relatively flat terrain like the Kilombero Valley.</t>
+          <t xml:space="preserve"> inadequacy of spatial soil information is one of the limiting factors to making evidence based decisions to improve food security and land management in the developing countries. various digital soil mapping (dsm) techniques have been applied in many parts of the world to improve availability and usability of soil data, but less has been done in africa, particularly in tanzania and at the scale necessary to make farm management decisions. the kilombero valley has been identified for intensified rice production. however the valley lacks detailed and up todate soil information for decision making. the overall objective of this study was to develop a predictive soil map of a portion of kilombero valley using dsm techniques. two widely used decision tree algorithms and three sources of digital elevation models (dems) were evaluated for their predictive ability. firstly, a numerical classification was performed on the collected soil profile data to arrive at soil taxa. secondly, the derived taxa were spatially predicted and mapped following scorpan framework using random forest (rf) and j48 machine learning algorithms. datasets to train the model were derived from legacy soil map, rapideye satellite image and three dems: 1 arc srtm, 30 m aster, and 12 m worlddem. separate predictive models were built using each dem source. mapping showed that rf was less sensitive to the training set sampling intensity. results also showed that predictions of soil taxa using 1 arc srtm and 12 m worddem were identical. we suggest the use of rf algorithm and the freely available srtm dem combination for mapping the soils for the whole kilombero valley. this combination can be tested and applied in other areas which have relatively flat terrain like the kilombero valley.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -771,16 +771,16 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[2, 15]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.621|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.359|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.118|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.269|x3: 0.000|x4: 0.066|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.068|x10: 0.090|x11: 0.070|x12: 0.116|x13: 0.000|x14: 0.000|x15: 0.337|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.269|x3: 0.000|x4: 0.234|x5: 0.068|x6: 0.123|x7: 0.085|x8: 0.000|x9: 0.094|x10: 0.071|x11: 0.060|x12: 0.159|x13: 0.000|x14: 0.232|x15: 0.188|x16: 0.238|x17: 0.000
-TOP2VEC -&gt; x1: 0.170|x2: 0.302|x3: 0.000|x4: 0.170|x5: 0.197|x6: 0.166|x7: 0.364|x8: 0.213|x9: 0.178|x10: 0.066|x11: 0.146|x12: 0.291|x13: 0.148|x14: 0.207|x15: 0.089|x16: 0.134|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.190|x3: 0.167|x4: 0.135|x5: 0.088|x6: 0.096|x7: 0.150|x8: 0.071|x9: 0.091|x10: 0.045|x11: 0.188|x12: 0.150|x13: 0.049|x14: 0.146|x15: 0.132|x16: 0.124|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.064|x3: 0.062|x4: 0.060|x5: 0.057|x6: 0.058|x7: 0.061|x8: 0.056|x9: 0.058|x10: 0.055|x11: 0.063|x12: 0.061|x13: 0.055|x14: 0.061|x15: 0.060|x16: 0.060|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.076|x3: 0.055|x4: 0.123|x5: 0.088|x6: 0.078|x7: 0.242|x8: 0.130|x9: 0.140|x10: 0.167|x11: 0.195|x12: 0.064|x13: 0.075|x14: 0.105|x15: 0.076|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.153|x3: 0.014|x4: 0.106|x5: 0.039|x6: 0.050|x7: 0.082|x8: 0.032|x9: 0.076|x10: 0.082|x11: 0.081|x12: 0.085|x13: 0.019|x14: 0.084|x15: 0.275|x16: 0.059|x17: 0.000
 </t>
         </is>
       </c>
@@ -791,7 +791,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Smallholder production in Russia has been in decline for more than a decade. The likelihood is for continued marginalization. Smallholders confront four obstacles. First, path dependencies, which includes the fact that smallholders' production remains traditional and subsistence oriented. Second, institutions in the form of state policy restrict land and animals. Third, Russia's role in the third food regime means that smallholders are unable to help Russia's emergence as a global food superpower. Fourth, smallholders are being left behind in the ongoing technological revolution led by agroholdings. As technological advancement expands in scope, the gap between large farms and smallholders will widen.</t>
+          <t xml:space="preserve"> smallholder production in russia has been in decline for more than a decade. the likelihood is for continued marginalization. smallholders confront four obstacles. first, path dependencies, which includes the fact that smallholders production remains traditional and subsistence oriented. second, institutions in the form of state policy restrict land and animals. third, russias role in the third food regime means that smallholders are unable to help russias emergence as a global food superpower. fourth, smallholders are being left behind in the ongoing technological revolution led by agroholdings. as technological advancement expands in scope, the gap between large farms and smallholders will widen.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -801,16 +801,16 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[2, 14, 15]</t>
+          <t>[2, 14]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.206|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.230|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.197|x3: 0.153|x4: 0.109|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.106|x13: 0.221|x14: 0.235|x15: 0.618|x16: 0.181|x17: 0.000
-TOP2VEC -&gt; x1: 0.117|x2: 0.406|x3: 0.220|x4: 0.268|x5: 0.075|x6: 0.000|x7: 0.220|x8: 0.119|x9: 0.179|x10: 0.000|x11: 0.192|x12: 0.000|x13: 0.246|x14: 0.395|x15: 0.257|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.039|x2: 0.270|x3: 0.124|x4: 0.126|x5: 0.025|x6: 0.000|x7: 0.073|x8: 0.040|x9: 0.060|x10: 0.000|x11: 0.064|x12: 0.112|x13: 0.156|x14: 0.210|x15: 0.252|x16: 0.060|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.070|x3: 0.060|x4: 0.060|x5: 0.055|x6: 0.053|x7: 0.057|x8: 0.055|x9: 0.057|x10: 0.053|x11: 0.057|x12: 0.060|x13: 0.062|x14: 0.066|x15: 0.069|x16: 0.057|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.065|x10: 0.000|x11: 0.000|x12: 0.153|x13: 0.000|x14: 0.000|x15: 0.093|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.197|x3: 0.153|x4: 0.109|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.106|x13: 0.221|x14: 0.235|x15: 0.500|x16: 0.181|x17: 0.000
+TOP2VEC -&gt; x1: 0.362|x2: 0.172|x3: 0.000|x4: 0.296|x5: 0.069|x6: 0.000|x7: 0.126|x8: 0.071|x9: 0.000|x10: 0.000|x11: 0.077|x12: 0.075|x13: 0.227|x14: 0.259|x15: 0.075|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.090|x2: 0.342|x3: 0.038|x4: 0.101|x5: 0.017|x6: 0.000|x7: 0.031|x8: 0.018|x9: 0.016|x10: 0.000|x11: 0.019|x12: 0.083|x13: 0.112|x14: 0.124|x15: 0.167|x16: 0.045|x17: 0.000
 </t>
         </is>
       </c>
@@ -821,7 +821,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Crop diseases are a major threat to food security, but their rapid identification remains difficult in many parts of the world due to the lack of the necessary infrastructure. The combination of increasing global smartphone penetration and recent advances in computer vision made possible by deep learning has paved the way for smartphone-assisted disease diagnosis. Using a public dataset of 54,306 images of diseased and healthy plant leaves collected under controlled conditions, we train a deep convolutional neural network to identify 14 crop species and 26 diseases (or absence thereof). The trained model achieves an accuracy of 99.35% on a held-out test set, demonstrating the feasibility of this approach. Overall, the approach of training deep learning models on increasingly large and publicly available image datasets presents a clear path toward smartphone-assisted crop disease diagnosis on a massive global scale.</t>
+          <t xml:space="preserve"> crop diseases are a major threat to food security, but their rapid identification remains difficult in many parts of the world due to the lack of the necessary infrastructure. the combination of increasing global smartphone penetration and recent advances in computer vision made possible by deep learning has paved the way for smartphone assisted disease diagnosis. using a public dataset of 54,306 images of diseased and healthy plant leaves collected under controlled conditions, we train a deep convolutional neural network to identify 14 crop species and 26 diseases (or absence thereof). the trained model achieves an accuracy of 99.35% on a held out test set, demonstrating the feasibility of this approach. overall, the approach of training deep learning models on increasingly large and publicly available image datasets presents a clear path toward smartphone assisted crop disease diagnosis on a massive global scale.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -831,16 +831,16 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[3, 4, 11]</t>
+          <t>[2, 3, 4]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.768|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.263|x3: 0.321|x4: 0.164|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.104|x10: 0.000|x11: 0.070|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.117|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.156|x3: 0.229|x4: 0.418|x5: 0.053|x6: 0.000|x7: 0.000|x8: 0.173|x9: 0.114|x10: 0.000|x11: 0.138|x12: 0.000|x13: 0.000|x14: 0.259|x15: 0.279|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.195|x2: 0.075|x3: 0.258|x4: 0.505|x5: 0.185|x6: 0.413|x7: 0.568|x8: 0.282|x9: 0.440|x10: 0.089|x11: 0.482|x12: 0.000|x13: 0.171|x14: 0.189|x15: 0.249|x16: 0.181|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.077|x3: 0.329|x4: 0.306|x5: 0.079|x6: 0.138|x7: 0.167|x8: 0.152|x9: 0.185|x10: 0.030|x11: 0.311|x12: 0.000|x13: 0.057|x14: 0.149|x15: 0.176|x16: 0.060|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.071|x4: 0.069|x5: 0.055|x6: 0.059|x7: 0.060|x8: 0.060|x9: 0.062|x10: 0.053|x11: 0.070|x12: 0.051|x13: 0.054|x14: 0.059|x15: 0.061|x16: 0.054|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.100|x4: 0.104|x5: 0.097|x6: 0.252|x7: 0.209|x8: 0.000|x9: 0.083|x10: 0.000|x11: 0.246|x12: 0.055|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.500|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.230|x3: 0.162|x4: 0.171|x5: 0.037|x6: 0.063|x7: 0.052|x8: 0.043|x9: 0.075|x10: 0.000|x11: 0.114|x12: 0.014|x13: 0.000|x14: 0.065|x15: 0.099|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -851,7 +851,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper presents an automatic traffic surveillance system to estimate important traffic parameters from video sequences using only one camera. Different from traditional methods which classify vehicles into only cars and non-cars, the proposed method has a good capability to categorize cars into more specific classes with a new "linearity" feature. In addition, in order to reduce occlusions of vehicles, an automatic scheme of detecting lane dividing lines is proposed. With the found lane dividing lines, not only occlusions of vehicles can be reduced but also a normalization scheme can be developed for tackling the problems of feature size variations. Once all vehicle features are extracted, an optimal classifier is then designed to robustly categorize vehicles into different classes even though shadows, occlusions, and other noise exist. The designed classifier can collect different evidences from the database and the verified vehicle itself to make better decisions and thus much enhance the robustness and accuracy of classification. Experimental results show that the proposed method is much robust and powerful than other traditional methods.</t>
+          <t xml:space="preserve"> this paper presents an automatic traffic surveillance system to estimate important traffic parameters from video sequences using only one camera. different from traditional methods which classify vehicles into only cars and non cars, the proposed method has a good capability to categorize cars into more specific classes with a new "linearity" feature. in addition, in order to reduce occlusions of vehicles, an automatic scheme of detecting lane dividing lines is proposed. with the found lane dividing lines, not only occlusions of vehicles can be reduced but also a normalization scheme can be developed for tackling the problems of feature size variations. once all vehicle features are extracted, an optimal classifier is then designed to robustly categorize vehicles into different classes even though shadows, occlusions, and other noise exist. the designed classifier can collect different evidences from the database and the verified vehicle itself to make better decisions and thus much enhance the robustness and accuracy of classification. experimental results show that the proposed method is much robust and powerful than other traditional methods.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -861,16 +861,16 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[3, 7]</t>
+          <t>[3, 7, 13]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.539|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.200|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.099|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.060|x2: 0.170|x3: 0.191|x4: 0.171|x5: 0.000|x6: 0.000|x7: 0.434|x8: 0.000|x9: 0.290|x10: 0.155|x11: 0.000|x12: 0.093|x13: 0.077|x14: 0.000|x15: 0.064|x16: 0.117|x17: 0.000
-TOP2VEC -&gt; x1: 0.130|x2: 0.219|x3: 0.356|x4: 0.167|x5: 0.000|x6: 0.126|x7: 0.242|x8: 0.178|x9: 0.137|x10: 0.098|x11: 0.073|x12: 0.336|x13: 0.053|x14: 0.062|x15: 0.251|x16: 0.200|x17: 0.000
-MEAN -&gt; x1: 0.063|x2: 0.130|x3: 0.349|x4: 0.112|x5: 0.000|x6: 0.042|x7: 0.225|x8: 0.059|x9: 0.142|x10: 0.084|x11: 0.124|x12: 0.143|x13: 0.043|x14: 0.021|x15: 0.105|x16: 0.106|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.075|x4: 0.059|x5: 0.053|x6: 0.055|x7: 0.066|x8: 0.056|x9: 0.061|x10: 0.058|x11: 0.060|x12: 0.061|x13: 0.055|x14: 0.054|x15: 0.059|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.158|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.447|x8: 0.109|x9: 0.000|x10: 0.152|x11: 0.088|x12: 0.309|x13: 0.263|x14: 0.000|x15: 0.000|x16: 0.281|x17: 0.000
+BERTOPIC -&gt; x1: 0.165|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.230|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.056|x2: 0.042|x3: 0.137|x4: 0.043|x5: 0.000|x6: 0.000|x7: 0.220|x8: 0.027|x9: 0.097|x10: 0.077|x11: 0.022|x12: 0.101|x13: 0.142|x14: 0.000|x15: 0.016|x16: 0.100|x17: 0.000
 </t>
         </is>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Significant advances on smart decision support systems (DSSs) development have influenced important results on pregnancy care. Nevertheless, even considering the efforts to reduce the number of women deaths due to problems related to pregnancy, this decrease presented less impact than other areas of human development. Hypertensive disorders in pregnancy, particularly pre-eclampsia and eclampsia, account for significant proportion of perinatal morbidity and maternal mortality. In this context, this paper proposes an inference model that uses data mining (DM) techniques capable for operating in a data set to extract patterns and assist in knowledge discovery. Identifying hypertensive crises that complicate pregnancy, it can impact in a meaningful reduction the incidence of sequelae and death of pregnant women. Comparison between two Bayesian classifiers is performed in this work to better classify the hypertensive disorders severity. Results showed that Naïve Bayes classifier had an excellent performance, presenting better precision and F-measure, compared to the other experimented classifiers. Even finding a good performance to predict hypertensive disorders, other Bayesian methods need to be evaluated, as well as other DM techniques such as those based on artificial intelligence (AI) and tree-based methods.</t>
+          <t xml:space="preserve"> significant advances on smart decision support systems (dsss) development have influenced important results on pregnancy care. nevertheless, even considering the efforts to reduce the number of women deaths due to problems related to pregnancy, this decrease presented less impact than other areas of human development. hypertensive disorders in pregnancy, particularly pre eclampsia and eclampsia, account for significant proportion of perinatal morbidity and maternal mortality. in this context, this paper proposes an inference model that uses data mining (dm) techniques capable for operating in a data set to extract patterns and assist in knowledge discovery. identifying hypertensive crises that complicate pregnancy, it can impact in a meaningful reduction the incidence of sequelae and death of pregnant women. comparison between two bayesian classifiers is performed in this work to better classify the hypertensive disorders severity. results showed that naïve bayes classifier had an excellent performance, presenting better precision and f measure, compared to the other experimented classifiers. even finding a good performance to predict hypertensive disorders, other bayesian methods need to be evaluated, as well as other dm techniques such as those based on artificial intelligence (ai) and tree based methods.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -896,11 +896,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.873|x4: 0.000|x5: 0.095|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.221|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.076|x10: 0.000|x11: 0.097|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.069|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.056|x2: 0.075|x3: 0.463|x4: 0.000|x5: 0.244|x6: 0.000|x7: 0.000|x8: 0.119|x9: 0.132|x10: 0.109|x11: 0.000|x12: 0.000|x13: 0.274|x14: 0.153|x15: 0.121|x16: 0.074|x17: 0.000
-TOP2VEC -&gt; x1: 0.104|x2: 0.087|x3: 0.326|x4: 0.000|x5: 0.230|x6: 0.136|x7: 0.219|x8: 0.079|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.093|x13: 0.228|x14: 0.164|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.054|x3: 0.429|x4: 0.000|x5: 0.190|x6: 0.045|x7: 0.073|x8: 0.066|x9: 0.044|x10: 0.036|x11: 0.104|x12: 0.031|x13: 0.167|x14: 0.106|x15: 0.040|x16: 0.025|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.057|x3: 0.082|x4: 0.054|x5: 0.065|x6: 0.056|x7: 0.058|x8: 0.057|x9: 0.056|x10: 0.056|x11: 0.060|x12: 0.055|x13: 0.063|x14: 0.060|x15: 0.056|x16: 0.055|x17: 0.054
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.230|x4: 0.000|x5: 0.000|x6: 0.096|x7: 0.187|x8: 0.000|x9: 0.123|x10: 0.000|x11: 0.116|x12: 0.242|x13: 0.191|x14: 0.085|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.014|x2: 0.019|x3: 0.423|x4: 0.000|x5: 0.116|x6: 0.024|x7: 0.047|x8: 0.030|x9: 0.083|x10: 0.027|x11: 0.053|x12: 0.061|x13: 0.116|x14: 0.059|x15: 0.047|x16: 0.019|x17: 0.000
 </t>
         </is>
       </c>
@@ -911,7 +911,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Increases in throughput and installed base of biomedical research equipment led to a massive accumulation of -omics data known to be highly variable, high-dimensional, and sourced from multiple often incompatible data platforms. While this data may be useful for biomarker identification and drug discovery, the bulk of it remains underutilized. Deep neural networks (DNNs) are efficient algorithms based on the use of compositional layers of neurons, with advantages well matched to the challenges -omics data presents. While achieving state-of-the-art results and even surpassing human accuracy in many challenging tasks, the adoption of deep learning in biomedicine has been comparatively slow. Here, we discuss key features of deep learning that may give this approach an edge over other machine learning methods. We then consider limitations and review a number of applications of deep learning in biomedical studies demonstrating proof of concept and practical utility.</t>
+          <t xml:space="preserve"> increases in throughput and installed base of biomedical research equipment led to a massive accumulation of omics data known to be highly variable, high dimensional, and sourced from multiple often incompatible data platforms. while this data may be useful for biomarker identification and drug discovery, the bulk of it remains underutilized. deep neural networks (dnns) are efficient algorithms based on the use of compositional layers of neurons, with advantages well matched to the challenges omics data presents. while achieving state of the art results and even surpassing human accuracy in many challenging tasks, the adoption of deep learning in biomedicine has been comparatively slow. here, we discuss key features of deep learning that may give this approach an edge over other machine learning methods. we then consider limitations and review a number of applications of deep learning in biomedical studies demonstrating proof of concept and practical utility.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -921,16 +921,16 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[3, 4, 11]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.688|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.398|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.385|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.152|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.100|x2: 0.207|x3: 0.163|x4: 0.318|x5: 0.000|x6: 0.000|x7: 0.053|x8: 0.132|x9: 0.195|x10: 0.000|x11: 0.090|x12: 0.124|x13: 0.107|x14: 0.000|x15: 0.109|x16: 0.221|x17: 0.000
-TOP2VEC -&gt; x1: 0.214|x2: 0.000|x3: 0.262|x4: 0.516|x5: 0.485|x6: 0.321|x7: 0.500|x8: 0.321|x9: 0.348|x10: 0.170|x11: 0.178|x12: 0.179|x13: 0.054|x14: 0.356|x15: 0.184|x16: 0.348|x17: 0.000
-MEAN -&gt; x1: 0.105|x2: 0.069|x3: 0.308|x4: 0.273|x5: 0.162|x6: 0.107|x7: 0.184|x8: 0.151|x9: 0.181|x10: 0.057|x11: 0.222|x12: 0.101|x13: 0.054|x14: 0.119|x15: 0.098|x16: 0.189|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.069|x4: 0.067|x5: 0.060|x6: 0.057|x7: 0.061|x8: 0.059|x9: 0.061|x10: 0.054|x11: 0.064|x12: 0.056|x13: 0.054|x14: 0.057|x15: 0.056|x16: 0.062|x17: 0.051
+TOP2VEC -&gt; x1: 0.147|x2: 0.000|x3: 0.148|x4: 0.253|x5: 0.097|x6: 0.068|x7: 0.297|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.093|x12: 0.231|x13: 0.110|x14: 0.000|x15: 0.073|x16: 0.070|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.062|x2: 0.052|x3: 0.203|x4: 0.239|x5: 0.024|x6: 0.017|x7: 0.088|x8: 0.033|x9: 0.087|x10: 0.000|x11: 0.046|x12: 0.089|x13: 0.054|x14: 0.000|x15: 0.045|x16: 0.073|x17: 0.000
 </t>
         </is>
       </c>
@@ -941,7 +941,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A fuzzy logic control (FLC) system was developed at the Hamburg University of Applied Sciences (HAW Hamburg) for operation of biogas reactors running on energy crops. Three commercially available measuring parameters, namely pH, the methane (CH 4 ) content, and the specific gas production rate (spec. GPR ¼ m 3 /kg VS/day) were included. The objective was to avoid stabilization of pH with use of buffering supplements, like lime or manure. The developed FLC system can cover most of all applications, such as a careful start-up process and a gentle recovery strategy after a severe reactor failure, also enabling a process with a high organic loading rate (OLR) and a low hydraulic retention time (HRT), that is, a high throughput anaerobic digestion process with a stable pH and CH 4 content. A precondition for a high load process was the concept of interval feeding, for example, with 8 h of interval. The FLC system was proved to be reliable during the long term fermentation studies over 3 years in one-stage, completely stirred tank reactors (CSTR) with acidic beet silage as mono-input (pH 3.3-3.4). During fermentation of the fodder beet silage (FBS), a stable HRT of 6.0 days with an OLR of up to 15 kg VS/m 3 /day and a volumetric GPR of 9 m 3 /m 3 /day could be reached. The FLC enabled an automatic recovery of the digester after two induced severe reactor failures. In another attempt to prove the feasibility of the FLC, substrate FBS was changed to sugar beet silage (SBS), which had a substantially lower buffering capacity than that of the FBS. With SBS, the FLC accomplished a stable fermentation at a pH level between 6.5 and 6.6, and a volatile fatty acid level (VFA) below 500 mg/L, but the FLC had to interact and to change the substrate dosage permanently. In a further experiment, the reactor temperature was increased from 41 to 508C. Concomitantly, the specific GPR, pH and CH 4 dropped down. Finally, the FLC automatically enabled a complete recovery in 16 days.</t>
+          <t xml:space="preserve"> a fuzzy logic control (flc) system was developed at the hamburg university of applied sciences (haw hamburg) for operation of biogas reactors running on energy crops. three commercially available measuring parameters, namely ph, the methane (ch 4 ) content, and the specific gas production rate (spec. gpr ¼ m 3 /kg vs/day) were included. the objective was to avoid stabilization of ph with use of buffering supplements, like lime or manure. the developed flc system can cover most of all applications, such as a careful start up process and a gentle recovery strategy after a severe reactor failure, also enabling a process with a high organic loading rate (olr) and a low hydraulic retention time (hrt), that is, a high throughput anaerobic digestion process with a stable ph and ch 4 content. a precondition for a high load process was the concept of interval feeding, for example, with 8 h of interval. the flc system was proved to be reliable during the long term fermentation studies over 3 years in one stage, completely stirred tank reactors (cstr) with acidic beet silage as mono input (ph 3.3 3.4). during fermentation of the fodder beet silage (fbs), a stable hrt of 6.0 days with an olr of up to 15 kg vs/m 3 /day and a volumetric gpr of 9 m 3 /m 3 /day could be reached. the flc enabled an automatic recovery of the digester after two induced severe reactor failures. in another attempt to prove the feasibility of the flc, substrate fbs was changed to sugar beet silage (sbs), which had a substantially lower buffering capacity than that of the fbs. with sbs, the flc accomplished a stable fermentation at a ph level between 6.5 and 6.6, and a volatile fatty acid level (vfa) below 500 mg/l, but the flc had to interact and to change the substrate dosage permanently. in a further experiment, the reactor temperature was increased from 41 to 508c. concomitantly, the specific gpr, ph and ch 4 dropped down. finally, the flc automatically enabled a complete recovery in 16 days.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -951,16 +951,16 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[7, 12]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.311|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.158|x8: 0.080|x9: 0.000|x10: 0.000|x11: 0.178|x12: 0.000|x13: 0.086|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.195|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.217|x8: 0.115|x9: 0.101|x10: 0.075|x11: 0.000|x12: 0.000|x13: 0.131|x14: 0.000|x15: 0.102|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.164|x3: 0.099|x4: 0.112|x5: 0.066|x6: 0.000|x7: 0.123|x8: 0.163|x9: 0.081|x10: 0.000|x11: 0.060|x12: 0.145|x13: 0.130|x14: 0.253|x15: 0.191|x16: 0.232|x17: 0.000
-TOP2VEC -&gt; x1: 0.100|x2: 0.210|x3: 0.000|x4: 0.344|x5: 0.143|x6: 0.056|x7: 0.179|x8: 0.085|x9: 0.089|x10: 0.105|x11: 0.123|x12: 0.280|x13: 0.238|x14: 0.238|x15: 0.136|x16: 0.216|x17: 0.000
-MEAN -&gt; x1: 0.033|x2: 0.125|x3: 0.137|x4: 0.152|x5: 0.070|x6: 0.019|x7: 0.153|x8: 0.109|x9: 0.057|x10: 0.035|x11: 0.121|x12: 0.142|x13: 0.151|x14: 0.164|x15: 0.109|x16: 0.149|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.061|x4: 0.062|x5: 0.057|x6: 0.054|x7: 0.062|x8: 0.059|x9: 0.056|x10: 0.055|x11: 0.060|x12: 0.061|x13: 0.062|x14: 0.063|x15: 0.059|x16: 0.062|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.098|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.312|x8: 0.087|x9: 0.092|x10: 0.000|x11: 0.079|x12: 0.338|x13: 0.155|x14: 0.164|x15: 0.059|x16: 0.069|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.222|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.155|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.066|x3: 0.074|x4: 0.028|x5: 0.017|x6: 0.000|x7: 0.219|x8: 0.091|x9: 0.069|x10: 0.019|x11: 0.035|x12: 0.160|x13: 0.104|x14: 0.104|x15: 0.088|x16: 0.075|x17: 0.000
 </t>
         </is>
       </c>
@@ -971,7 +971,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Intuitionistic fuzzy sets (IFSs) are generalization of fuzzy sets by adding an additional attribute parameter called non-membership degree. In this paper, a max-min intuitionistic fuzzy Hopfield neural network (IFHNN) is proposed by combining IFSs with Hopfield neural networks. The stability of IFHNN is investigated. It is shown that for any given weight matrix and any given initial intuitionistic fuzzy pattern, the iteration process of IFHNN converges to a limit cycle. Furthermore, under suitable extra conditions, it converges to a stable point within finite iterations. Finally, a kind of Lyapunov stability of the stable points of IFHNN is proved, which means that if the initial state of the network is close enough to a stable point, then the network states will remain in a small neighborhood of the stable point. These stability results indicate the convergence of memory process of IFHNN. A numerical example is also provided to show the effectiveness of the Lyapunov stability of IFHNN</t>
+          <t xml:space="preserve"> intuitionistic fuzzy sets (ifss) are generalization of fuzzy sets by adding an additional attribute parameter called non membership degree. in this paper, a max min intuitionistic fuzzy hopfield neural network (ifhnn) is proposed by combining ifss with hopfield neural networks. the stability of ifhnn is investigated. it is shown that for any given weight matrix and any given initial intuitionistic fuzzy pattern, the iteration process of ifhnn converges to a limit cycle. furthermore, under suitable extra conditions, it converges to a stable point within finite iterations. finally, a kind of lyapunov stability of the stable points of ifhnn is proved, which means that if the initial state of the network is close enough to a stable point, then the network states will remain in a small neighborhood of the stable point. these stability results indicate the convergence of memory process of ifhnn. a numerical example is also provided to show the effectiveness of the lyapunov stability of ifhnn</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -981,16 +981,16 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[3, 9]</t>
+          <t>[7, 9, 13]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.409|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.061|x10: 0.000|x11: 0.237|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.362|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.067|x3: 0.231|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.226|x8: 0.082|x9: 0.346|x10: 0.111|x11: 0.000|x12: 0.082|x13: 0.214|x14: 0.076|x15: 0.245|x16: 0.140|x17: 0.000
-TOP2VEC -&gt; x1: 0.149|x2: 0.052|x3: 0.252|x4: 0.312|x5: 0.056|x6: 0.000|x7: 0.074|x8: 0.175|x9: 0.402|x10: 0.000|x11: 0.270|x12: 0.301|x13: 0.336|x14: 0.233|x15: 0.148|x16: 0.101|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.040|x3: 0.297|x4: 0.104|x5: 0.019|x6: 0.000|x7: 0.100|x8: 0.086|x9: 0.270|x10: 0.037|x11: 0.169|x12: 0.128|x13: 0.183|x14: 0.103|x15: 0.131|x16: 0.080|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.071|x4: 0.059|x5: 0.054|x6: 0.053|x7: 0.058|x8: 0.057|x9: 0.069|x10: 0.055|x11: 0.062|x12: 0.060|x13: 0.063|x14: 0.058|x15: 0.060|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.088|x3: 0.000|x4: 0.218|x5: 0.000|x6: 0.108|x7: 0.164|x8: 0.100|x9: 0.204|x10: 0.176|x11: 0.191|x12: 0.057|x13: 0.352|x14: 0.000|x15: 0.152|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.381|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.039|x3: 0.058|x4: 0.055|x5: 0.000|x6: 0.027|x7: 0.193|x8: 0.046|x9: 0.228|x10: 0.072|x11: 0.048|x12: 0.035|x13: 0.142|x14: 0.019|x15: 0.099|x16: 0.035|x17: 0.000
 </t>
         </is>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The reduction of environmental pollution and the conservation and recycling of natural resources are significant social and environmental concerns. As valuable means for pollution control, minimization and mitigation remain attractive approaches. However, interactive, dynamic and uncertain features are associated with these processes, resulting in difficulties in their management and control. Artificial intelligence (AI) is an effective approach for tackling these complexities. In this study, the recent advancements of AI-based technologies for management and control of pollution minimization and mitigation processes are examined. Literature relevant to the area of application of AI to control and management of pollution minimization and mitigation processes is investigated. Especially, technologies of expert systems, fuzzy logic, and neural networks, which emerge as the most frequently employed approaches for realizing process control, are highlighted. The results not only provide an overview of the updated progress in the study field but also, more importantly, reveal perspectives of research for more effective environmental process control through the AI-aided measures. Several demanding areas for enhanced research efforts are discussed, including issues of data availability and reliability, methodology validity, and system complexity.</t>
+          <t xml:space="preserve"> the reduction of environmental pollution and the conservation and recycling of natural resources are significant social and environmental concerns. as valuable means for pollution control, minimization and mitigation remain attractive approaches. however, interactive, dynamic and uncertain features are associated with these processes, resulting in difficulties in their management and control. artificial intelligence (ai) is an effective approach for tackling these complexities. in this study, the recent advancements of ai based technologies for management and control of pollution minimization and mitigation processes are examined. literature relevant to the area of application of ai to control and management of pollution minimization and mitigation processes is investigated. especially, technologies of expert systems, fuzzy logic, and neural networks, which emerge as the most frequently employed approaches for realizing process control, are highlighted. the results not only provide an overview of the updated progress in the study field but also, more importantly, reveal perspectives of research for more effective environmental process control through the ai aided measures. several demanding areas for enhanced research efforts are discussed, including issues of data availability and reliability, methodology validity, and system complexity.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1011,16 +1011,16 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[3, 11, 12, 13, 14]</t>
+          <t>[12, 13, 14]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.635|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.417|x12: 0.090|x13: 0.000|x14: 0.132|x15: 0.099|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.089|x4: 0.000|x5: 0.000|x6: 0.101|x7: 0.000|x8: 0.000|x9: 0.088|x10: 0.000|x11: 0.110|x12: 0.263|x13: 0.000|x14: 0.133|x15: 0.192|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.058|x3: 0.362|x4: 0.170|x5: 0.000|x6: 0.000|x7: 0.139|x8: 0.000|x9: 0.183|x10: 0.000|x11: 0.148|x12: 0.079|x13: 0.218|x14: 0.356|x15: 0.000|x16: 0.107|x17: 0.000
-TOP2VEC -&gt; x1: 0.151|x2: 0.197|x3: 0.000|x4: 0.151|x5: 0.126|x6: 0.332|x7: 0.260|x8: 0.101|x9: 0.193|x10: 0.000|x11: 0.322|x12: 0.494|x13: 0.508|x14: 0.401|x15: 0.398|x16: 0.088|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.085|x3: 0.287|x4: 0.107|x5: 0.042|x6: 0.111|x7: 0.133|x8: 0.034|x9: 0.125|x10: 0.000|x11: 0.295|x12: 0.221|x13: 0.239|x14: 0.296|x15: 0.166|x16: 0.065|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.068|x4: 0.057|x5: 0.053|x6: 0.057|x7: 0.059|x8: 0.053|x9: 0.058|x10: 0.051|x11: 0.069|x12: 0.064|x13: 0.065|x14: 0.069|x15: 0.060|x16: 0.055|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.079|x7: 0.197|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.182|x12: 0.217|x13: 0.339|x14: 0.156|x15: 0.118|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.118|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.500|x13: 0.068|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.015|x3: 0.113|x4: 0.042|x5: 0.000|x6: 0.045|x7: 0.114|x8: 0.000|x9: 0.068|x10: 0.000|x11: 0.110|x12: 0.265|x13: 0.156|x14: 0.161|x15: 0.077|x16: 0.027|x17: 0.000
 </t>
         </is>
       </c>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this work, a computer-aided tool for detection was developed to segment breast masses from clinical ultrasound (US) scans. The underlying Multi U-net algorithm is based on convolutional neural networks. Under the Mayo Clinic Institutional Review Board protocol, a prospective study of the automatic segmentation of suspicious breast masses was performed. The cohort consisted of 258 female patients who were clinically identified with suspicious breast masses and underwent clinical US scan and breast biopsy. The computer-aided detection tool effectively segmented the breast masses, achieving a mean Dice coefficient of 0.82, a true positive fraction (TPF) of 0.84, and a false positive fraction (FPF) of 0.01. By avoiding positioning of an initial seed, the algorithm is able to segment images in real time (13-55 ms per image), and can have potential clinical applications. The algorithm is at par with a conventional seeded algorithm, which had a mean Dice coefficient of 0.84 and performs significantly better (P&lt; 0.0001) than the original U-net algorithm.</t>
+          <t xml:space="preserve"> in this work, a computer aided tool for detection was developed to segment breast masses from clinical ultrasound (us) scans. the underlying multi u net algorithm is based on convolutional neural networks. under the mayo clinic institutional review board protocol, a prospective study of the automatic segmentation of suspicious breast masses was performed. the cohort consisted of 258 female patients who were clinically identified with suspicious breast masses and underwent clinical us scan and breast biopsy. the computer aided detection tool effectively segmented the breast masses, achieving a mean dice coefficient of 0.82, a true positive fraction (tpf) of 0.84, and a false positive fraction (fpf) of 0.01. by avoiding positioning of an initial seed, the algorithm is able to segment images in real time (13 55 ms per image), and can have potential clinical applications. the algorithm is at par with a conventional seeded algorithm, which had a mean dice coefficient of 0.84 and performs significantly better (p&lt; 0.0001) than the original u net algorithm.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1046,11 +1046,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.478|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.120|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.108|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.137|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.318|x4: 0.000|x5: 0.255|x6: 0.000|x7: 0.059|x8: 0.144|x9: 0.000|x10: 0.140|x11: 0.000|x12: 0.079|x13: 0.174|x14: 0.255|x15: 0.206|x16: 0.190|x17: 0.000
-TOP2VEC -&gt; x1: 0.201|x2: 0.000|x3: 0.460|x4: 0.316|x5: 0.307|x6: 0.000|x7: 0.202|x8: 0.153|x9: 0.000|x10: 0.106|x11: 0.208|x12: 0.110|x13: 0.442|x14: 0.193|x15: 0.187|x16: 0.217|x17: 0.000
-MEAN -&gt; x1: 0.067|x2: 0.000|x3: 0.418|x4: 0.105|x5: 0.187|x6: 0.000|x7: 0.087|x8: 0.099|x9: 0.000|x10: 0.082|x11: 0.161|x12: 0.063|x13: 0.205|x14: 0.149|x15: 0.131|x16: 0.136|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.052|x3: 0.080|x4: 0.058|x5: 0.063|x6: 0.052|x7: 0.057|x8: 0.058|x9: 0.052|x10: 0.057|x11: 0.062|x12: 0.056|x13: 0.064|x14: 0.061|x15: 0.060|x16: 0.060|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.215|x4: 0.000|x5: 0.092|x6: 0.079|x7: 0.129|x8: 0.000|x9: 0.088|x10: 0.136|x11: 0.127|x12: 0.000|x13: 0.383|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.288|x4: 0.000|x5: 0.087|x6: 0.020|x7: 0.047|x8: 0.036|x9: 0.049|x10: 0.069|x11: 0.032|x12: 0.020|x13: 0.139|x14: 0.064|x15: 0.086|x16: 0.048|x17: 0.000
 </t>
         </is>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The amount of coronary artery calcification (CAC) is a strong and independent predictor of cardiovascular events. CAC is clinically quantified in cardiac calcium scoring CT (CSCT), but it has been shown that cardiac CT angiography (CCTA) may also be used for this purpose. We present a method for automatic CAC quantification in CCTA. This method uses supervised learning to directly identify and quantify CAC without a need for coronary artery extraction commonly used in existing methods.</t>
+          <t xml:space="preserve"> the amount of coronary artery calcification (cac) is a strong and independent predictor of cardiovascular events. cac is clinically quantified in cardiac calcium scoring ct (csct), but it has been shown that cardiac ct angiography (ccta) may also be used for this purpose. we present a method for automatic cac quantification in ccta. this method uses supervised learning to directly identify and quantify cac without a need for coronary artery extraction commonly used in existing methods.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1071,16 +1071,16 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[3, 4]</t>
+          <t>[1, 3, 4, 12, 13]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.302|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.164|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.136|x4: 0.156|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.077|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.389|x2: 0.165|x3: 0.301|x4: 0.432|x5: 0.000|x6: 0.000|x7: 0.130|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.111|x13: 0.000|x14: 0.000|x15: 0.104|x16: 0.188|x17: 0.000
-TOP2VEC -&gt; x1: 0.088|x2: 0.089|x3: 0.158|x4: 0.480|x5: 0.220|x6: 0.169|x7: 0.161|x8: 0.089|x9: 0.355|x10: 0.198|x11: 0.235|x12: 0.207|x13: 0.326|x14: 0.235|x15: 0.136|x16: 0.405|x17: 0.000
-MEAN -&gt; x1: 0.159|x2: 0.085|x3: 0.254|x4: 0.304|x5: 0.073|x6: 0.056|x7: 0.097|x8: 0.030|x9: 0.118|x10: 0.066|x11: 0.133|x12: 0.106|x13: 0.109|x14: 0.078|x15: 0.080|x16: 0.198|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.057|x3: 0.067|x4: 0.071|x5: 0.056|x6: 0.055|x7: 0.058|x8: 0.054|x9: 0.059|x10: 0.056|x11: 0.060|x12: 0.058|x13: 0.058|x14: 0.057|x15: 0.057|x16: 0.064|x17: 0.052
+TOP2VEC -&gt; x1: 0.093|x2: 0.000|x3: 0.202|x4: 0.168|x5: 0.000|x6: 0.000|x7: 0.113|x8: 0.061|x9: 0.092|x10: 0.000|x11: 0.069|x12: 0.267|x13: 0.305|x14: 0.198|x15: 0.072|x16: 0.136|x17: 0.000
+BERTOPIC -&gt; x1: 0.236|x2: 0.177|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.089|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.122|x12: 0.091|x13: 0.271|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.179|x2: 0.086|x3: 0.160|x4: 0.189|x5: 0.000|x6: 0.000|x7: 0.083|x8: 0.015|x9: 0.023|x10: 0.000|x11: 0.048|x12: 0.136|x13: 0.144|x14: 0.050|x15: 0.044|x16: 0.081|x17: 0.000
 </t>
         </is>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Automatic license plate recognition (LPR) plays an important role in numerous applications and a number of techniques have been proposed. However, most of them worked under restricted conditions, such as fixed illumination, limited vehicle speed, designated routes, and stationary backgrounds. In this study, as few constraints as possible on the working environment are considered. The proposed LPR technique consists of two main modules: a license plate locating module and a license number identification module. The former characterized by fuzzy disciplines attempts to extract license plates from an input image, while the latter conceptualized in terms of neural subjects aims to identify the number present in a license plate. Experiments have been conducted for the respective modules. In the experiment on locating license plates, 1088 images taken from various scenes and under different conditions were employed. Of which, 23 images have been failed to locate the license plates present in the images; the license plate location rate of success is 97.9%. In the experiment on identifying license number, 1065 images, from which license plates have been successfully located, were used. Of which, 47 images have been failed to identify the numbers of the license plates located in the images; the identification rate of success is 95.6%. Combining the above two rates, the overall rate of success for our LPR algorithm is 93.7%.</t>
+          <t xml:space="preserve"> automatic license plate recognition (lpr) plays an important role in numerous applications and a number of techniques have been proposed. however, most of them worked under restricted conditions, such as fixed illumination, limited vehicle speed, designated routes, and stationary backgrounds. in this study, as few constraints as possible on the working environment are considered. the proposed lpr technique consists of two main modules: a license plate locating module and a license number identification module. the former characterized by fuzzy disciplines attempts to extract license plates from an input image, while the latter conceptualized in terms of neural subjects aims to identify the number present in a license plate. experiments have been conducted for the respective modules. in the experiment on locating license plates, 1088 images taken from various scenes and under different conditions were employed. of which, 23 images have been failed to locate the license plates present in the images; the license plate location rate of success is 97.9%. in the experiment on identifying license number, 1065 images, from which license plates have been successfully located, were used. of which, 47 images have been failed to identify the numbers of the license plates located in the images; the identification rate of success is 95.6%. combining the above two rates, the overall rate of success for our lpr algorithm is 93.7%.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1101,16 +1101,16 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[3, 14]</t>
+          <t>[3, 4, 8, 14]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.274|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.083|x9: 0.000|x10: 0.000|x11: 0.144|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.108|x3: 0.248|x4: 0.218|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.072|x9: 0.080|x10: 0.140|x11: 0.000|x12: 0.000|x13: 0.070|x14: 0.543|x15: 0.000|x16: 0.091|x17: 0.000
-TOP2VEC -&gt; x1: 0.151|x2: 0.340|x3: 0.316|x4: 0.245|x5: 0.224|x6: 0.125|x7: 0.086|x8: 0.156|x9: 0.000|x10: 0.147|x11: 0.240|x12: 0.000|x13: 0.167|x14: 0.353|x15: 0.203|x16: 0.302|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.149|x3: 0.279|x4: 0.154|x5: 0.122|x6: 0.042|x7: 0.065|x8: 0.104|x9: 0.027|x10: 0.096|x11: 0.128|x12: 0.000|x13: 0.079|x14: 0.284|x15: 0.068|x16: 0.131|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.070|x4: 0.062|x5: 0.060|x6: 0.055|x7: 0.056|x8: 0.059|x9: 0.054|x10: 0.058|x11: 0.060|x12: 0.053|x13: 0.057|x14: 0.070|x15: 0.057|x16: 0.060|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.249|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.291|x9: 0.000|x10: 0.000|x11: 0.088|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.108|x3: 0.248|x4: 0.218|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.072|x9: 0.080|x10: 0.140|x11: 0.000|x12: 0.000|x13: 0.070|x14: 0.500|x15: 0.000|x16: 0.091|x17: 0.000
+TOP2VEC -&gt; x1: 0.063|x2: 0.064|x3: 0.095|x4: 0.331|x5: 0.150|x6: 0.000|x7: 0.350|x8: 0.126|x9: 0.161|x10: 0.146|x11: 0.111|x12: 0.096|x13: 0.000|x14: 0.191|x15: 0.000|x16: 0.179|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.395|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.016|x2: 0.043|x3: 0.148|x4: 0.137|x5: 0.073|x6: 0.000|x7: 0.115|x8: 0.123|x9: 0.060|x10: 0.072|x11: 0.050|x12: 0.024|x13: 0.116|x14: 0.173|x15: 0.000|x16: 0.068|x17: 0.000
 </t>
         </is>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Perception system design is a vital step in the development of an autonomous vehicle (AV). With the vast selection of available off-the-shelf schemes and seemingly endless options of sensor systems implemented in research and commercial vehicles, it can be difficult to identify the optimal system for one's AV application. This article presents a comprehensive review of the state-of-the-art AV perception technology available today. It provides up-to-date information about the advantages, disadvantages, limits, and ideal applications of specific AV sensors; the most prevalent sensors in current research and commercial AVs; autonomous features currently on the market; and localization and mapping methods currently implemented in AV research. This information is useful for newcomers to the AV field to gain a greater understanding of the current AV solution landscape and to guide experienced researchers towards research areas requiring further development. Furthermore, this paper highlights future research areas and draws conclusions about the most effective methods for AV perception and its effect on localization and mapping. Topics discussed in the Perception and Automotive Sensors section focus on the sensors themselves, whereas topics discussed in the Localization and Mapping section focus on how the vehicle perceives where it is on the road, providing context for the use of the automotive sensors. By improving on current state-of-the-art perception systems, AVs will become more robust, reliable, safe, and accessible, ultimately providing greater efficiency, mobility, and safety benefits to the public.</t>
+          <t xml:space="preserve"> perception system design is a vital step in the development of an autonomous vehicle (av). with the vast selection of available off the shelf schemes and seemingly endless options of sensor systems implemented in research and commercial vehicles, it can be difficult to identify the optimal system for ones av application. this article presents a comprehensive review of the state of the art av perception technology available today. it provides up to date information about the advantages, disadvantages, limits, and ideal applications of specific av sensors; the most prevalent sensors in current research and commercial avs; autonomous features currently on the market; and localization and mapping methods currently implemented in av research. this information is useful for newcomers to the av field to gain a greater understanding of the current av solution landscape and to guide experienced researchers towards research areas requiring further development. furthermore, this paper highlights future research areas and draws conclusions about the most effective methods for av perception and its effect on localization and mapping. topics discussed in the perception and automotive sensors section focus on the sensors themselves, whereas topics discussed in the localization and mapping section focus on how the vehicle perceives where it is on the road, providing context for the use of the automotive sensors. by improving on current state of the art perception systems, avs will become more robust, reliable, safe, and accessible, ultimately providing greater efficiency, mobility, and safety benefits to the public.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1131,16 +1131,16 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[3, 9, 11]</t>
+          <t>[9, 11]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.504|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.094|x11: 0.309|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.069|x8: 0.000|x9: 0.144|x10: 0.089|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.103|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.094|x3: 0.173|x4: 0.181|x5: 0.000|x6: 0.000|x7: 0.197|x8: 0.059|x9: 0.345|x10: 0.137|x11: 0.116|x12: 0.000|x13: 0.193|x14: 0.092|x15: 0.232|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.155|x2: 0.327|x3: 0.000|x4: 0.211|x5: 0.294|x6: 0.192|x7: 0.183|x8: 0.193|x9: 0.299|x10: 0.101|x11: 0.175|x12: 0.244|x13: 0.227|x14: 0.399|x15: 0.178|x16: 0.207|x17: 0.000
-MEAN -&gt; x1: 0.052|x2: 0.141|x3: 0.224|x4: 0.131|x5: 0.098|x6: 0.064|x7: 0.127|x8: 0.084|x9: 0.215|x10: 0.111|x11: 0.200|x12: 0.081|x13: 0.140|x14: 0.164|x15: 0.137|x16: 0.069|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.065|x4: 0.059|x5: 0.057|x6: 0.056|x7: 0.059|x8: 0.057|x9: 0.065|x10: 0.058|x11: 0.064|x12: 0.056|x13: 0.060|x14: 0.061|x15: 0.060|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.153|x2: 0.056|x3: 0.000|x4: 0.169|x5: 0.067|x6: 0.072|x7: 0.184|x8: 0.000|x9: 0.000|x10: 0.179|x11: 0.145|x12: 0.099|x13: 0.113|x14: 0.155|x15: 0.000|x16: 0.065|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.066|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.038|x2: 0.038|x3: 0.043|x4: 0.087|x5: 0.017|x6: 0.018|x7: 0.112|x8: 0.015|x9: 0.122|x10: 0.101|x11: 0.221|x12: 0.025|x13: 0.093|x14: 0.062|x15: 0.084|x16: 0.016|x17: 0.000
 </t>
         </is>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Real-life depression, and a ect" will be the seventh competition event aimed at comparison of multimedia processing and machine learning methods for automatic audiovisual depression and emotion analysis, with all participants competing under strictly the same conditions. e goal of the Challenge is to provide a common benchmark test set for multimodal information processing and to bring together the depression and emotion recognition communities, as well as the audiovisual processing communities, to compare the relative merits of the various approaches to depression and emotion recognition from real-life data. is paper presents the novelties introduced this year, the challenge guidelines, the data used, and the performance of the baseline system on the two proposed tasks: dimensional emotion recognition (time and value-continuous), and dimensional depression estimation (value-continuous).</t>
+          <t xml:space="preserve"> real life depression, and a ect" will be the seventh competition event aimed at comparison of multimedia processing and machine learning methods for automatic audiovisual depression and emotion analysis, with all participants competing under strictly the same conditions. e goal of the challenge is to provide a common benchmark test set for multimodal information processing and to bring together the depression and emotion recognition communities, as well as the audiovisual processing communities, to compare the relative merits of the various approaches to depression and emotion recognition from real life data. is paper presents the novelties introduced this year, the challenge guidelines, the data used, and the performance of the baseline system on the two proposed tasks: dimensional emotion recognition (time and value continuous), and dimensional depression estimation (value continuous).</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1161,16 +1161,16 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[3, 8, 14]</t>
+          <t>[3, 8, 9, 14]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.381|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.063|x10: 0.000|x11: 0.227|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.241|x10: 0.000|x11: 0.112|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.078|x2: 0.062|x3: 0.157|x4: 0.161|x5: 0.075|x6: 0.000|x7: 0.140|x8: 0.392|x9: 0.241|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.418|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.175|x2: 0.351|x3: 0.492|x4: 0.370|x5: 0.202|x6: 0.384|x7: 0.164|x8: 0.261|x9: 0.208|x10: 0.076|x11: 0.243|x12: 0.000|x13: 0.000|x14: 0.188|x15: 0.000|x16: 0.156|x17: 0.000
-MEAN -&gt; x1: 0.084|x2: 0.138|x3: 0.343|x4: 0.177|x5: 0.092|x6: 0.128|x7: 0.101|x8: 0.218|x9: 0.171|x10: 0.057|x11: 0.157|x12: 0.000|x13: 0.000|x14: 0.202|x15: 0.000|x16: 0.052|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.074|x4: 0.062|x5: 0.057|x6: 0.059|x7: 0.058|x8: 0.065|x9: 0.062|x10: 0.055|x11: 0.061|x12: 0.052|x13: 0.052|x14: 0.064|x15: 0.052|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.258|x2: 0.165|x3: 0.280|x4: 0.000|x5: 0.000|x6: 0.350|x7: 0.095|x8: 0.207|x9: 0.170|x10: 0.000|x11: 0.190|x12: 0.170|x13: 0.097|x14: 0.172|x15: 0.000|x16: 0.093|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.084|x2: 0.057|x3: 0.234|x4: 0.040|x5: 0.019|x6: 0.087|x7: 0.059|x8: 0.150|x9: 0.163|x10: 0.024|x11: 0.076|x12: 0.042|x13: 0.024|x14: 0.147|x15: 0.000|x16: 0.023|x17: 0.000
 </t>
         </is>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A MIMO (multiple inputs and multiple outputs) fuzzy-logic-based model was developed to predict biogas and methane production rates in a pilot-scale 90-L mesophilic up-flow anaerobic sludge blanket (UASB) reactor treating molasses wastewater. Five input variables such as volumetric organic loading rate (OLR), volumetric total chemical oxygen demand (TCOD) removal rate (R V ), influent alkalinity, influent pH and effluent pH were fuzzified by the use of an artificial intelligence-based approach. Trapezoidal membership functions with eight levels were conducted for the fuzzy subsets, and a Mamdani-type fuzzy inference system was used to implement a total of 134 rules in the IF-THEN format. The product (prod) and the centre of gravity (COG, centroid) methods were employed as the inference operator and defuzzification methods, respectively. Fuzzy-logic predicted results were compared with the outputs of two exponential non-linear regression models derived in this study. The UASB reactor showed a remarkable performance on the treatment of molasses wastewater, with an average TCOD removal efficiency of 93 (±3)% and an average volumetric TCOD removal rate of 6.87 (±3.93) kg TCOD removed /m 3 -day, respectively. Findings of this study clearly indicated that, compared to non-linear regression models, the proposed MIMO fuzzy-logic-based model produced smaller deviations and exhibited a superior predictive performance on forecasting of both biogas and methane production rates with satisfactory determination coefficients over 0.98.</t>
+          <t xml:space="preserve"> a mimo (multiple inputs and multiple outputs) fuzzy logic based model was developed to predict biogas and methane production rates in a pilot scale 90 l mesophilic up flow anaerobic sludge blanket (uasb) reactor treating molasses wastewater. five input variables such as volumetric organic loading rate (olr), volumetric total chemical oxygen demand (tcod) removal rate (r v ), influent alkalinity, influent ph and effluent ph were fuzzified by the use of an artificial intelligence based approach. trapezoidal membership functions with eight levels were conducted for the fuzzy subsets, and a mamdani type fuzzy inference system was used to implement a total of 134 rules in the if then format. the product (prod) and the centre of gravity (cog, centroid) methods were employed as the inference operator and defuzzification methods, respectively. fuzzy logic predicted results were compared with the outputs of two exponential non linear regression models derived in this study. the uasb reactor showed a remarkable performance on the treatment of molasses wastewater, with an average tcod removal efficiency of 93 (±3)% and an average volumetric tcod removal rate of 6.87 (±3.93) kg tcod removed /m 3 day, respectively. findings of this study clearly indicated that, compared to non linear regression models, the proposed mimo fuzzy logic based model produced smaller deviations and exhibited a superior predictive performance on forecasting of both biogas and methane production rates with satisfactory determination coefficients over 0.98.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1191,16 +1191,16 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 6, 7, 9, 12]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.539|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.138|x9: 0.000|x10: 0.000|x11: 0.294|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.258|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.067|x8: 0.222|x9: 0.070|x10: 0.067|x11: 0.000|x12: 0.178|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.107|x2: 0.269|x3: 0.155|x4: 0.093|x5: 0.085|x6: 0.237|x7: 0.124|x8: 0.145|x9: 0.166|x10: 0.139|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.107|x15: 0.088|x16: 0.105|x17: 0.000
-TOP2VEC -&gt; x1: 0.122|x2: 0.231|x3: 0.181|x4: 0.084|x5: 0.222|x6: 0.293|x7: 0.424|x8: 0.192|x9: 0.208|x10: 0.078|x11: 0.216|x12: 0.194|x13: 0.000|x14: 0.294|x15: 0.085|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.076|x2: 0.167|x3: 0.279|x4: 0.059|x5: 0.102|x6: 0.177|x7: 0.183|x8: 0.158|x9: 0.124|x10: 0.072|x11: 0.170|x12: 0.065|x13: 0.000|x14: 0.134|x15: 0.058|x16: 0.088|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.062|x3: 0.069|x4: 0.056|x5: 0.058|x6: 0.063|x7: 0.063|x8: 0.061|x9: 0.059|x10: 0.056|x11: 0.062|x12: 0.056|x13: 0.052|x14: 0.060|x15: 0.056|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.092|x4: 0.109|x5: 0.000|x6: 0.088|x7: 0.419|x8: 0.058|x9: 0.368|x10: 0.132|x11: 0.000|x12: 0.319|x13: 0.172|x14: 0.151|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.027|x2: 0.067|x3: 0.126|x4: 0.050|x5: 0.021|x6: 0.206|x7: 0.153|x8: 0.106|x9: 0.151|x10: 0.084|x11: 0.000|x12: 0.124|x13: 0.043|x14: 0.065|x15: 0.022|x16: 0.026|x17: 0.000
 </t>
         </is>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A fuzzy logic model was developed to simulate the effect of leachate recirculation and sludge addition on the biogas generation in anaerobic bioreactor landfills. The model was designed using a fuzzy logic system (FLS) which incorporated 3 input variables (time, leachate recirculation, and sludge addition) and a single manipulated output (biogas generation rate). The biogas production rate was measured during the experiment and was increasing proportionally with the rate of both leachate recirculation and sludge addition. The experimental work involved the operation of six simulated laboratory-scale bioreactors for over a year under different operating schemes. The experimental results were employed in formulating the fuzzy rule base, calibrating the model, and verifying its predictions. Then, the model was validated against other measured data that was compiled from published studies. The FLS model simulations demonstrated high correlation with the experimental observations.</t>
+          <t xml:space="preserve"> a fuzzy logic model was developed to simulate the effect of leachate recirculation and sludge addition on the biogas generation in anaerobic bioreactor landfills. the model was designed using a fuzzy logic system (fls) which incorporated 3 input variables (time, leachate recirculation, and sludge addition) and a single manipulated output (biogas generation rate). the biogas production rate was measured during the experiment and was increasing proportionally with the rate of both leachate recirculation and sludge addition. the experimental work involved the operation of six simulated laboratory scale bioreactors for over a year under different operating schemes. the experimental results were employed in formulating the fuzzy rule base, calibrating the model, and verifying its predictions. then, the model was validated against other measured data that was compiled from published studies. the fls model simulations demonstrated high correlation with the experimental observations.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1221,16 +1221,16 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[4, 7, 9]</t>
+          <t>[7, 9, 12]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.461|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.151|x9: 0.000|x10: 0.000|x11: 0.267|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.238|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.287|x9: 0.082|x10: 0.000|x11: 0.000|x12: 0.209|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.370|x3: 0.061|x4: 0.436|x5: 0.223|x6: 0.000|x7: 0.101|x8: 0.000|x9: 0.377|x10: 0.000|x11: 0.000|x12: 0.075|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
-TOP2VEC -&gt; x1: 0.171|x2: 0.182|x3: 0.000|x4: 0.244|x5: 0.286|x6: 0.324|x7: 0.742|x8: 0.236|x9: 0.465|x10: 0.066|x11: 0.157|x12: 0.580|x13: 0.244|x14: 0.191|x15: 0.205|x16: 0.136|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.184|x3: 0.174|x4: 0.227|x5: 0.170|x6: 0.108|x7: 0.200|x8: 0.129|x9: 0.281|x10: 0.022|x11: 0.141|x12: 0.192|x13: 0.081|x14: 0.064|x15: 0.068|x16: 0.104|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.061|x4: 0.065|x5: 0.061|x6: 0.057|x7: 0.063|x8: 0.059|x9: 0.068|x10: 0.053|x11: 0.059|x12: 0.062|x13: 0.056|x14: 0.055|x15: 0.055|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.113|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.500|x8: 0.180|x9: 0.300|x10: 0.054|x11: 0.170|x12: 0.256|x13: 0.203|x14: 0.140|x15: 0.000|x16: 0.139|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.179|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.084|x12: 0.316|x13: 0.100|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.093|x3: 0.103|x4: 0.109|x5: 0.056|x6: 0.000|x7: 0.195|x8: 0.117|x9: 0.190|x10: 0.013|x11: 0.063|x12: 0.214|x13: 0.076|x14: 0.035|x15: 0.000|x16: 0.079|x17: 0.000
 </t>
         </is>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hypertension is the main cause of maternal death. Preeclampsia can affect pregnant women before or during pregnancy. Identification of patients with higher risk for preeclampsia allows some precautions that are taken to prevent its severe disease and subsequent complications. In medicine, there are different situations that deal with a large range of information, which needs a thorough assessment to be able to help experts in the decision-making process. Smart decision support systems allow grouping all existing information and finding pertinent information from it. Bayesian networks offer models that allow the information capture and handle situations of uncertainty. This paper proposes the construction of a system to support intelligent decision applied to the diagnosis of preeclampsia using Bayesian networks to help experts in the pregnant's care. The processes of qualitative and quantitative modeling to the construction of a network are also presented. The main contribution of this work includes the presentation of a Bayesian network built to help decision makers in moments of uncertainty in care of pregnant women.</t>
+          <t xml:space="preserve"> hypertension is the main cause of maternal death. preeclampsia can affect pregnant women before or during pregnancy. identification of patients with higher risk for preeclampsia allows some precautions that are taken to prevent its severe disease and subsequent complications. in medicine, there are different situations that deal with a large range of information, which needs a thorough assessment to be able to help experts in the decision making process. smart decision support systems allow grouping all existing information and finding pertinent information from it. bayesian networks offer models that allow the information capture and handle situations of uncertainty. this paper proposes the construction of a system to support intelligent decision applied to the diagnosis of preeclampsia using bayesian networks to help experts in the pregnants care. the processes of qualitative and quantitative modeling to the construction of a network are also presented. the main contribution of this work includes the presentation of a bayesian network built to help decision makers in moments of uncertainty in care of pregnant women.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1251,16 +1251,16 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[2, 3]</t>
+          <t>[2, 3, 9]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.714|x4: 0.000|x5: 0.138|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.419|x3: 0.258|x4: 0.000|x5: 0.156|x6: 0.000|x7: 0.071|x8: 0.204|x9: 0.265|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.193|x14: 0.147|x15: 0.106|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.120|x2: 0.327|x3: 0.000|x4: 0.236|x5: 0.083|x6: 0.083|x7: 0.230|x8: 0.121|x9: 0.070|x10: 0.000|x11: 0.127|x12: 0.260|x13: 0.189|x14: 0.000|x15: 0.000|x16: 0.089|x17: 0.000
-MEAN -&gt; x1: 0.040|x2: 0.249|x3: 0.253|x4: 0.079|x5: 0.126|x6: 0.028|x7: 0.100|x8: 0.108|x9: 0.112|x10: 0.000|x11: 0.142|x12: 0.087|x13: 0.127|x14: 0.049|x15: 0.035|x16: 0.030|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.069|x3: 0.069|x4: 0.058|x5: 0.061|x6: 0.055|x7: 0.059|x8: 0.060|x9: 0.060|x10: 0.054|x11: 0.062|x12: 0.058|x13: 0.061|x14: 0.056|x15: 0.055|x16: 0.055|x17: 0.054
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.061|x3: 0.245|x4: 0.000|x5: 0.228|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.144|x10: 0.000|x11: 0.071|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.375|x3: 0.264|x4: 0.000|x5: 0.166|x6: 0.000|x7: 0.073|x8: 0.208|x9: 0.274|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.198|x14: 0.153|x15: 0.109|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.113|x2: 0.207|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.129|x8: 0.074|x9: 0.063|x10: 0.000|x11: 0.176|x12: 0.127|x13: 0.221|x14: 0.076|x15: 0.000|x16: 0.161|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.028|x2: 0.161|x3: 0.252|x4: 0.000|x5: 0.099|x6: 0.000|x7: 0.050|x8: 0.070|x9: 0.120|x10: 0.000|x11: 0.062|x12: 0.032|x13: 0.105|x14: 0.057|x15: 0.027|x16: 0.040|x17: 0.000
 </t>
         </is>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Pregnancy is the delicate stage in every woman's life cycle. The changes in the health during this period may lead to risk in pregnancy. That is a high risk pregnancy is one that endangers the women's or baby's health or life. Hypertensive disorders are the most common cause of these pregnancy related complications. In the present era, it's a major challenge in health care because their results in increasing maternal and fetal death. There exist various techniques widely used in data mining for the early identification of health diseases. Better treatment can be provided in the early stage by the early identification of hypertensive disorders. The main intent of this paper is to pinpoint the present complications of a pregnant woman by applying a boosted random forest approach for predicting hypertensive disorders. This classification method helps to predict the risks, diagnose and thereby can decrease maternal and fetal mortality, which remains as a large problem in much of the developing nation.</t>
+          <t xml:space="preserve"> pregnancy is the delicate stage in every womans life cycle. the changes in the health during this period may lead to risk in pregnancy. that is a high risk pregnancy is one that endangers the womens or babys health or life. hypertensive disorders are the most common cause of these pregnancy related complications. in the present era, its a major challenge in health care because their results in increasing maternal and fetal death. there exist various techniques widely used in data mining for the early identification of health diseases. better treatment can be provided in the early stage by the early identification of hypertensive disorders. the main intent of this paper is to pinpoint the present complications of a pregnant woman by applying a boosted random forest approach for predicting hypertensive disorders. this classification method helps to predict the risks, diagnose and thereby can decrease maternal and fetal mortality, which remains as a large problem in much of the developing nation.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1281,16 +1281,16 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 5, 13]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.992|x4: 0.000|x5: 0.154|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.200|x12: 0.000|x13: 0.060|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.103|x3: 0.813|x4: 0.120|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.062|x11: 0.000|x12: 0.000|x13: 0.330|x14: 0.000|x15: 0.112|x16: 0.115|x17: 0.000
-TOP2VEC -&gt; x1: 0.145|x2: 0.000|x3: 0.504|x4: 0.000|x5: 0.260|x6: 0.000|x7: 0.000|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.154|x13: 0.138|x14: 0.000|x15: 0.117|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.034|x3: 0.500|x4: 0.040|x5: 0.193|x6: 0.000|x7: 0.000|x8: 0.052|x9: 0.000|x10: 0.021|x11: 0.067|x12: 0.051|x13: 0.176|x14: 0.000|x15: 0.076|x16: 0.038|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.089|x4: 0.056|x5: 0.066|x6: 0.054|x7: 0.054|x8: 0.057|x9: 0.054|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.064|x14: 0.054|x15: 0.058|x16: 0.056|x17: 0.054
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.256|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.090|x14: 0.000|x15: 0.097|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.103|x3: 0.500|x4: 0.120|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.062|x11: 0.000|x12: 0.000|x13: 0.330|x14: 0.000|x15: 0.112|x16: 0.115|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.140|x3: 0.466|x4: 0.000|x5: 0.115|x6: 0.000|x7: 0.055|x8: 0.000|x9: 0.000|x10: 0.179|x11: 0.000|x12: 0.315|x13: 0.101|x14: 0.000|x15: 0.000|x16: 0.201|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.061|x3: 0.492|x4: 0.030|x5: 0.134|x6: 0.000|x7: 0.014|x8: 0.000|x9: 0.000|x10: 0.060|x11: 0.000|x12: 0.079|x13: 0.131|x14: 0.000|x15: 0.052|x16: 0.079|x17: 0.000
 </t>
         </is>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The National Motor Vehicle Crash Causation Survey (NMVCCS), conducted from 2005 to 2007, was aimed at collecting on-scene information about the events and associated factors leading up to crashes involving light vehicles. Several facets of crash occurrence were investigated during data collection, namely the precrash movement, critical pre-crash event, critical reason, and the associated factors. A weighted sample of 5,470 crashes was investigated over a period of two and a half years, which represents an estimated 2,189,000 crashes nationwide. About 4,031,000 vehicles, 3,945,000 drivers, and 1,982,000 passengers were estimated to have been involved in these crashes. The critical reason, which is the last event in the crash causal chain, was assigned to the driver in 94 percent (±2.2%) † of the crashes. In about 2 percent (±0.7%) of the crashes, the critical reason was assigned to a vehicle component's failure or degradation, and in 2 percent (±1.3%) of crashes, it was attributed to the environment (slick roads, weather, etc.). Among an estimated 2,046,000 drivers who were assigned critical reasons, recognition errors accounted for about 41 percent (±2.1%), decision errors 33 percent (±3.7%), and performance errors 11 percent (±2.7%) of the crashes.</t>
+          <t xml:space="preserve"> the national motor vehicle crash causation survey (nmvccs), conducted from 2005 to 2007, was aimed at collecting on scene information about the events and associated factors leading up to crashes involving light vehicles. several facets of crash occurrence were investigated during data collection, namely the precrash movement, critical pre crash event, critical reason, and the associated factors. a weighted sample of 5,470 crashes was investigated over a period of two and a half years, which represents an estimated 2,189,000 crashes nationwide. about 4,031,000 vehicles, 3,945,000 drivers, and 1,982,000 passengers were estimated to have been involved in these crashes. the critical reason, which is the last event in the crash causal chain, was assigned to the driver in 94 percent (±2.2%) † of the crashes. in about 2 percent (±0.7%) of the crashes, the critical reason was assigned to a vehicle components failure or degradation, and in 2 percent (±1.3%) of crashes, it was attributed to the environment (slick roads, weather, etc.). among an estimated 2,046,000 drivers who were assigned critical reasons, recognition errors accounted for about 41 percent (±2.1%), decision errors 33 percent (±3.7%), and performance errors 11 percent (±2.7%) of the crashes.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1311,16 +1311,16 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[3, 9, 10]</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.205|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.057|x10: 0.000|x11: 0.098|x12: 0.000|x13: 0.000|x14: 0.064|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.078|x2: 0.096|x3: 0.201|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.146|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.108|x15: 0.073|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.058|x2: 0.164|x3: 0.061|x4: 0.000|x5: 0.085|x6: 0.000|x7: 0.269|x8: 0.063|x9: 0.461|x10: 0.336|x11: 0.000|x12: 0.000|x13: 0.118|x14: 0.000|x15: 0.125|x16: 0.080|x17: 0.000
-TOP2VEC -&gt; x1: 0.114|x2: 0.000|x3: 0.179|x4: 0.000|x5: 0.289|x6: 0.229|x7: 0.119|x8: 0.157|x9: 0.228|x10: 0.160|x11: 0.219|x12: 0.309|x13: 0.111|x14: 0.071|x15: 0.241|x16: 0.327|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.055|x3: 0.149|x4: 0.000|x5: 0.125|x6: 0.076|x7: 0.129|x8: 0.073|x9: 0.249|x10: 0.165|x11: 0.106|x12: 0.103|x13: 0.076|x14: 0.045|x15: 0.122|x16: 0.136|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.056|x3: 0.062|x4: 0.053|x5: 0.060|x6: 0.057|x7: 0.061|x8: 0.057|x9: 0.068|x10: 0.063|x11: 0.059|x12: 0.059|x13: 0.057|x14: 0.056|x15: 0.060|x16: 0.061|x17: 0.053
+TOP2VEC -&gt; x1: 0.204|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.091|x6: 0.062|x7: 0.125|x8: 0.165|x9: 0.210|x10: 0.170|x11: 0.171|x12: 0.055|x13: 0.000|x14: 0.000|x15: 0.097|x16: 0.160|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.085|x2: 0.065|x3: 0.190|x4: 0.000|x5: 0.044|x6: 0.016|x7: 0.099|x8: 0.057|x9: 0.204|x10: 0.126|x11: 0.043|x12: 0.014|x13: 0.029|x14: 0.027|x15: 0.074|x16: 0.060|x17: 0.000
 </t>
         </is>
       </c>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper surveys and discusses the application of data-derived soft-sensing techniques in biological wastewater treatment plants. Emphasis is given to an extensive overview of the current status and to the specific challenges and potential that allow for an effective application of these soft-sensors in full-scale scenarios. The soft-sensors presented in the case studies have been found to be effective and inexpensive technologies for extracting and modelling relevant process information directly from the process and laboratory data routinely acquired in biological wastewater treatment facilities. The extracted information is in the form of timely analysis of hard-to-measure primary process variables and process diagnostics that characterize the operation of the plants and their instrumentation. The information is invaluable for an effective utilization of advanced control and optimization strategies.</t>
+          <t xml:space="preserve"> this paper surveys and discusses the application of data derived soft sensing techniques in biological wastewater treatment plants. emphasis is given to an extensive overview of the current status and to the specific challenges and potential that allow for an effective application of these soft sensors in full scale scenarios. the soft sensors presented in the case studies have been found to be effective and inexpensive technologies for extracting and modelling relevant process information directly from the process and laboratory data routinely acquired in biological wastewater treatment facilities. the extracted information is in the form of timely analysis of hard to measure primary process variables and process diagnostics that characterize the operation of the plants and their instrumentation. the information is invaluable for an effective utilization of advanced control and optimization strategies.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1341,16 +1341,16 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[2, 3, 7, 15]</t>
+          <t>[6, 7, 15]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.531|x4: 0.084|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.158|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.130|x10: 0.000|x11: 0.124|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.115|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.321|x3: 0.140|x4: 0.174|x5: 0.086|x6: 0.120|x7: 0.149|x8: 0.000|x9: 0.055|x10: 0.150|x11: 0.000|x12: 0.070|x13: 0.198|x14: 0.000|x15: 0.257|x16: 0.101|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.292|x3: 0.000|x4: 0.125|x5: 0.165|x6: 0.266|x7: 0.496|x8: 0.121|x9: 0.202|x10: 0.056|x11: 0.087|x12: 0.681|x13: 0.379|x14: 0.384|x15: 0.507|x16: 0.114|x17: 0.000
-MEAN -&gt; x1: 0.047|x2: 0.205|x3: 0.213|x4: 0.128|x5: 0.084|x6: 0.129|x7: 0.215|x8: 0.040|x9: 0.086|x10: 0.068|x11: 0.131|x12: 0.190|x13: 0.192|x14: 0.128|x15: 0.252|x16: 0.072|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.063|x3: 0.064|x4: 0.059|x5: 0.056|x6: 0.059|x7: 0.064|x8: 0.054|x9: 0.056|x10: 0.055|x11: 0.059|x12: 0.062|x13: 0.063|x14: 0.059|x15: 0.066|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.059|x5: 0.000|x6: 0.203|x7: 0.455|x8: 0.000|x9: 0.000|x10: 0.088|x11: 0.166|x12: 0.376|x13: 0.088|x14: 0.178|x15: 0.204|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.080|x3: 0.035|x4: 0.098|x5: 0.021|x6: 0.206|x7: 0.151|x8: 0.000|x9: 0.046|x10: 0.059|x11: 0.073|x12: 0.111|x13: 0.071|x14: 0.045|x15: 0.144|x16: 0.025|x17: 0.000
 </t>
         </is>
       </c>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this paper, we aim to provide a survey on the applications of deep learning for cancer detection and diagnosis and hope to provide an overview of the progress in this field. In the survey, we firstly provide an overview on deep learning and the popular architectures used for cancer detection and diagnosis. Especially we present four popular deep learning architectures, including convolutional neural networks, fully convolutional networks, auto-encoders, and deep belief networks in the survey. Secondly, we provide a survey on the studies exploiting deep learning for cancer detection and diagnosis. The surveys in this part are organized based on the types of cancers. Thirdly, we provide a summary and comments on the recent work on the applications of deep learning to cancer detection and diagnosis and propose some future research directions.</t>
+          <t xml:space="preserve"> in this paper, we aim to provide a survey on the applications of deep learning for cancer detection and diagnosis and hope to provide an overview of the progress in this field. in the survey, we firstly provide an overview on deep learning and the popular architectures used for cancer detection and diagnosis. especially we present four popular deep learning architectures, including convolutional neural networks, fully convolutional networks, auto encoders, and deep belief networks in the survey. secondly, we provide a survey on the studies exploiting deep learning for cancer detection and diagnosis. the surveys in this part are organized based on the types of cancers. thirdly, we provide a summary and comments on the recent work on the applications of deep learning to cancer detection and diagnosis and propose some future research directions.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1376,11 +1376,11 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.579|x4: 0.051|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.334|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.188|x3: 0.302|x4: 0.559|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.000|x9: 0.119|x10: 0.000|x11: 0.000|x12: 0.066|x13: 0.091|x14: 0.130|x15: 0.000|x16: 0.113|x17: 0.000
-TOP2VEC -&gt; x1: 0.059|x2: 0.000|x3: 0.289|x4: 0.417|x5: 0.333|x6: 0.210|x7: 0.279|x8: 0.111|x9: 0.231|x10: 0.106|x11: 0.077|x12: 0.182|x13: 0.000|x14: 0.000|x15: 0.169|x16: 0.218|x17: 0.000
-MEAN -&gt; x1: 0.020|x2: 0.063|x3: 0.364|x4: 0.322|x5: 0.158|x6: 0.070|x7: 0.130|x8: 0.037|x9: 0.117|x10: 0.035|x11: 0.137|x12: 0.083|x13: 0.030|x14: 0.043|x15: 0.056|x16: 0.110|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.076|x4: 0.073|x5: 0.062|x6: 0.057|x7: 0.060|x8: 0.055|x9: 0.059|x10: 0.055|x11: 0.060|x12: 0.057|x13: 0.054|x14: 0.055|x15: 0.056|x16: 0.059|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.151|x4: 0.229|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.098|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.188|x3: 0.302|x4: 0.500|x5: 0.141|x6: 0.000|x7: 0.109|x8: 0.000|x9: 0.119|x10: 0.000|x11: 0.000|x12: 0.066|x13: 0.091|x14: 0.130|x15: 0.000|x16: 0.113|x17: 0.000
+TOP2VEC -&gt; x1: 0.172|x2: 0.000|x3: 0.188|x4: 0.353|x5: 0.152|x6: 0.000|x7: 0.135|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.111|x12: 0.080|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.076|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.043|x2: 0.047|x3: 0.286|x4: 0.271|x5: 0.073|x6: 0.000|x7: 0.061|x8: 0.000|x9: 0.054|x10: 0.000|x11: 0.028|x12: 0.037|x13: 0.023|x14: 0.033|x15: 0.000|x16: 0.047|x17: 0.000
 </t>
         </is>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Social media such as Twitter can provide urgently needed drug abuse intelligence to support the campaign of fighting against the national drug abuse crisis. We employed a targeted tweet collection approach and a two-staged annotation strategy that combines conventional annotation with crowdsourced annotation to produce annotated training dataset. In this demo, we share deep learning models trained in a boosting manner using the data from the two-staged annotation method and unlabeled data collection to detect drug abuse risk behavior in tweets.</t>
+          <t xml:space="preserve"> social media such as twitter can provide urgently needed drug abuse intelligence to support the campaign of fighting against the national drug abuse crisis. we employed a targeted tweet collection approach and a two staged annotation strategy that combines conventional annotation with crowdsourced annotation to produce annotated training dataset. in this demo, we share deep learning models trained in a boosting manner using the data from the two staged annotation method and unlabeled data collection to detect drug abuse risk behavior in tweets.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1401,16 +1401,16 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[3, 4, 5]</t>
+          <t>[3, 4, 16]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.415|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.199|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.087|x2: 0.000|x3: 0.169|x4: 0.172|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.153|x2: 0.139|x3: 0.318|x4: 0.448|x5: 0.255|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.132|x10: 0.000|x11: 0.000|x12: 0.094|x13: 0.110|x14: 0.000|x15: 0.000|x16: 0.171|x17: 0.000
-TOP2VEC -&gt; x1: 0.136|x2: 0.000|x3: 0.113|x4: 0.477|x5: 0.467|x6: 0.463|x7: 0.356|x8: 0.145|x9: 0.000|x10: 0.000|x11: 0.313|x12: 0.000|x13: 0.141|x14: 0.301|x15: 0.000|x16: 0.063|x17: 0.000
-MEAN -&gt; x1: 0.097|x2: 0.046|x3: 0.282|x4: 0.308|x5: 0.241|x6: 0.154|x7: 0.119|x8: 0.048|x9: 0.044|x10: 0.000|x11: 0.171|x12: 0.031|x13: 0.083|x14: 0.100|x15: 0.000|x16: 0.078|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.055|x3: 0.070|x4: 0.072|x5: 0.067|x6: 0.061|x7: 0.059|x8: 0.055|x9: 0.055|x10: 0.053|x11: 0.062|x12: 0.054|x13: 0.057|x14: 0.058|x15: 0.053|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.171|x3: 0.222|x4: 0.135|x5: 0.000|x6: 0.374|x7: 0.138|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.225|x12: 0.222|x13: 0.000|x14: 0.156|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.060|x2: 0.077|x3: 0.177|x4: 0.189|x5: 0.064|x6: 0.093|x7: 0.034|x8: 0.000|x9: 0.033|x10: 0.000|x11: 0.056|x12: 0.079|x13: 0.027|x14: 0.039|x15: 0.000|x16: 0.168|x17: 0.000
 </t>
         </is>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The goal of this research project is to combine our intelligent decision-aid systems with a patient decisionsupport tool to provide more information to physicians, nurses and parents when they are facing very difficult, ethical decisions regarding the care or management of neonatal intensive care (NICU) patients. Our two artificial intelligence approaches, one using case-based reasoning and the other artificial neural networks, may provide critical information such as estimates of the likelihood of survival and the use and duration of artificial ventilation. These estimates, in addition to other factors such as birth weight, gestational age and the presence of major complications, may provide eritical information to health care givers and parents to decide whether to initiate intensive care for the infant, or whether to terminate it if it has already been initiated.</t>
+          <t xml:space="preserve"> the goal of this research project is to combine our intelligent decision aid systems with a patient decisionsupport tool to provide more information to physicians, nurses and parents when they are facing very difficult, ethical decisions regarding the care or management of neonatal intensive care (nicu) patients. our two artificial intelligence approaches, one using case based reasoning and the other artificial neural networks, may provide critical information such as estimates of the likelihood of survival and the use and duration of artificial ventilation. these estimates, in addition to other factors such as birth weight, gestational age and the presence of major complications, may provide eritical information to health care givers and parents to decide whether to initiate intensive care for the infant, or whether to terminate it if it has already been initiated.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1431,16 +1431,16 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[2, 3]</t>
+          <t>[2, 3, 9]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.694|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.293|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.108|x3: 0.363|x4: 0.000|x5: 0.090|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.090|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.402|x3: 0.257|x4: 0.294|x5: 0.096|x6: 0.000|x7: 0.106|x8: 0.000|x9: 0.398|x10: 0.000|x11: 0.000|x12: 0.064|x13: 0.107|x14: 0.000|x15: 0.000|x16: 0.097|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.230|x3: 0.553|x4: 0.281|x5: 0.303|x6: 0.000|x7: 0.328|x8: 0.146|x9: 0.192|x10: 0.000|x11: 0.000|x12: 0.193|x13: 0.179|x14: 0.258|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.211|x3: 0.419|x4: 0.192|x5: 0.133|x6: 0.000|x7: 0.145|x8: 0.049|x9: 0.196|x10: 0.000|x11: 0.098|x12: 0.086|x13: 0.095|x14: 0.086|x15: 0.000|x16: 0.032|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.065|x3: 0.080|x4: 0.064|x5: 0.060|x6: 0.053|x7: 0.061|x8: 0.055|x9: 0.064|x10: 0.053|x11: 0.058|x12: 0.057|x13: 0.058|x14: 0.057|x15: 0.053|x16: 0.054|x17: 0.053
+TOP2VEC -&gt; x1: 0.075|x2: 0.146|x3: 0.171|x4: 0.123|x5: 0.099|x6: 0.155|x7: 0.000|x8: 0.000|x9: 0.159|x10: 0.130|x11: 0.057|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.019|x2: 0.164|x3: 0.323|x4: 0.104|x5: 0.071|x6: 0.039|x7: 0.027|x8: 0.000|x9: 0.162|x10: 0.033|x11: 0.014|x12: 0.016|x13: 0.027|x14: 0.000|x15: 0.000|x16: 0.024|x17: 0.000
 </t>
         </is>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Severe Maternal Morbidity is a public health issue. It may occur during pregnancy, delivery, or puerperium due to conditions (hypertensive disorders, hemorrhages, infections and others) that put in risk the women's or baby's life. These conditions are really difficult AQ1 to detect at an early stage. In response to the above, this work proposes using several machine learning techniques, which are considered most relevant in a bio-medical setting, in order to predict the risk level for Severe Maternal Morbidity in patients during pregnancy. The population studied correspond to pregnant women receiving prenatal care and final attention at E.S.E Clínica de Maternidad Rafael Calvo in Cartagena, Colombia. This paper presents the preliminary results of an ongoing project, as well as methods and materials considered for the construction of the learning models.</t>
+          <t xml:space="preserve"> severe maternal morbidity is a public health issue. it may occur during pregnancy, delivery, or puerperium due to conditions (hypertensive disorders, hemorrhages, infections and others) that put in risk the womens or babys life. these conditions are really difficult aq1 to detect at an early stage. in response to the above, this work proposes using several machine learning techniques, which are considered most relevant in a bio medical setting, in order to predict the risk level for severe maternal morbidity in patients during pregnancy. the population studied correspond to pregnant women receiving prenatal care and final attention at e.s.e clínica de maternidad rafael calvo in cartagena, colombia. this paper presents the preliminary results of an ongoing project, as well as methods and materials considered for the construction of the learning models.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1461,16 +1461,16 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.786|x4: 0.000|x5: 0.153|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.279|x12: 0.077|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.401|x4: 0.119|x5: 0.265|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.097|x12: 0.150|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.224|x3: 0.340|x4: 0.307|x5: 0.191|x6: 0.000|x7: 0.000|x8: 0.090|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.071|x13: 0.232|x14: 0.000|x15: 0.188|x16: 0.177|x17: 0.000
-TOP2VEC -&gt; x1: 0.144|x2: 0.000|x3: 0.260|x4: 0.236|x5: 0.194|x6: 0.186|x7: 0.422|x8: 0.122|x9: 0.000|x10: 0.000|x11: 0.134|x12: 0.246|x13: 0.269|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.075|x3: 0.367|x4: 0.181|x5: 0.180|x6: 0.062|x7: 0.141|x8: 0.071|x9: 0.000|x10: 0.000|x11: 0.138|x12: 0.131|x13: 0.167|x14: 0.000|x15: 0.063|x16: 0.059|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.077|x4: 0.064|x5: 0.064|x6: 0.056|x7: 0.061|x8: 0.057|x9: 0.053|x10: 0.053|x11: 0.061|x12: 0.061|x13: 0.063|x14: 0.053|x15: 0.056|x16: 0.056|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.117|x3: 0.369|x4: 0.143|x5: 0.000|x6: 0.169|x7: 0.078|x8: 0.000|x9: 0.000|x10: 0.134|x11: 0.000|x12: 0.097|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.133|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.085|x3: 0.403|x4: 0.142|x5: 0.114|x6: 0.042|x7: 0.020|x8: 0.023|x9: 0.000|x10: 0.033|x11: 0.024|x12: 0.079|x13: 0.058|x14: 0.000|x15: 0.047|x16: 0.077|x17: 0.000
 </t>
         </is>
       </c>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Background The misuse of prescription opioids (MUPO) is a leading public health concern. Social media are playing an expanded role in public health research, but there are few methods for estimating established epidemiological metrics from social media. The purpose of this study was to demonstrate that the geographic variation of social media posts mentioning prescription opioid misuse strongly correlates with government estimates of MUPO in the last month. Methods We wrote software to acquire publicly available tweets from Twitter from 2012 to 2014 that contained at least one keyword related to prescription opioid use (n = 3,611,528). A medical toxicologist and emergency physician curated the list of keywords. We used the semantic distance (SemD) to automatically quantify the similarity of meaning between tweets and identify tweets that mentioned MUPO. We defined the SemD between two words as the shortest distance between the two corresponding word-centroids. Each word-centroid represented all recognized meanings of a word. We validated this automatic identification with manual curation. We used Twitter metadata to estimate the location of each tweet. We compared our estimated geographic distribution with the 2013-2015 National Surveys on Drug Usage and Health (NSDUH). Results Tweets that mentioned MUPO formed a distinct cluster far away from semantically unrelated tweets. The state-bystate correlation between Twitter and NSDUH was highly significant across all NSDUH survey years. The correlation was strongest between Twitter and NSDUH data from those aged 18-25 (r = 0.94, p &lt; 0.01 for 2012; r = 0.94, p &lt; 0.01 for 2013; r = 0.71, p = 0.02 for 2014). The correlation was driven by discussions of opioid use, even after controlling for geographic variation in Twitter usage. Conclusions Mentions of MUPO on Twitter correlate strongly with state-by-state NSDUH estimates of MUPO. We have also demonstrated that a natural language processing can be used to analyze social media to provide insights for syndromic toxicosurveillance.</t>
+          <t xml:space="preserve"> background the misuse of prescription opioids (mupo) is a leading public health concern. social media are playing an expanded role in public health research, but there are few methods for estimating established epidemiological metrics from social media. the purpose of this study was to demonstrate that the geographic variation of social media posts mentioning prescription opioid misuse strongly correlates with government estimates of mupo in the last month. methods we wrote software to acquire publicly available tweets from twitter from 2012 to 2014 that contained at least one keyword related to prescription opioid use (n = 3,611,528). a medical toxicologist and emergency physician curated the list of keywords. we used the semantic distance (semd) to automatically quantify the similarity of meaning between tweets and identify tweets that mentioned mupo. we defined the semd between two words as the shortest distance between the two corresponding word centroids. each word centroid represented all recognized meanings of a word. we validated this automatic identification with manual curation. we used twitter metadata to estimate the location of each tweet. we compared our estimated geographic distribution with the 2013 2015 national surveys on drug usage and health (nsduh). results tweets that mentioned mupo formed a distinct cluster far away from semantically unrelated tweets. the state bystate correlation between twitter and nsduh was highly significant across all nsduh survey years. the correlation was strongest between twitter and nsduh data from those aged 18 25 (r = 0.94, p &lt; 0.01 for 2012; r = 0.94, p &lt; 0.01 for 2013; r = 0.71, p = 0.02 for 2014). the correlation was driven by discussions of opioid use, even after controlling for geographic variation in twitter usage. conclusions mentions of mupo on twitter correlate strongly with state by state nsduh estimates of mupo. we have also demonstrated that a natural language processing can be used to analyze social media to provide insights for syndromic toxicosurveillance.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1491,16 +1491,16 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[3, 4, 11]</t>
+          <t>[1, 3, 4, 11]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.109|x2: 0.000|x3: 0.402|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.066|x11: 0.208|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.239|x2: 0.000|x3: 0.286|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.145|x11: 0.102|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.080|x17: 0.000
 LDA -&gt; x1: 0.132|x2: 0.214|x3: 0.218|x4: 0.335|x5: 0.073|x6: 0.000|x7: 0.101|x8: 0.055|x9: 0.120|x10: 0.118|x11: 0.171|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.211|x16: 0.072|x17: 0.000
-TOP2VEC -&gt; x1: 0.239|x2: 0.288|x3: 0.075|x4: 0.567|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.269|x9: 0.211|x10: 0.137|x11: 0.306|x12: 0.186|x13: 0.311|x14: 0.269|x15: 0.000|x16: 0.280|x17: 0.000
-MEAN -&gt; x1: 0.160|x2: 0.167|x3: 0.232|x4: 0.278|x5: 0.082|x6: 0.000|x7: 0.034|x8: 0.108|x9: 0.110|x10: 0.107|x11: 0.228|x12: 0.062|x13: 0.104|x14: 0.090|x15: 0.070|x16: 0.118|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.062|x3: 0.066|x4: 0.069|x5: 0.057|x6: 0.052|x7: 0.054|x8: 0.058|x9: 0.058|x10: 0.058|x11: 0.066|x12: 0.056|x13: 0.058|x14: 0.057|x15: 0.056|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.164|x2: 0.000|x3: 0.129|x4: 0.187|x5: 0.101|x6: 0.000|x7: 0.080|x8: 0.232|x9: 0.109|x10: 0.107|x11: 0.239|x12: 0.076|x13: 0.079|x14: 0.103|x15: 0.000|x16: 0.085|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.134|x2: 0.053|x3: 0.283|x4: 0.130|x5: 0.044|x6: 0.000|x7: 0.045|x8: 0.072|x9: 0.057|x10: 0.093|x11: 0.128|x12: 0.019|x13: 0.020|x14: 0.026|x15: 0.053|x16: 0.059|x17: 0.000
 </t>
         </is>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Generating novel graph structures that optimize given objectives while obeying some given underlying rules is fundamental for chemistry, biology and social science research. This is especially important in the task of molecular graph generation, whose goal is to discover novel molecules with desired properties such as drug-likeness and synthetic accessibility, while obeying physical laws such as chemical valency. However, designing models to find molecules that optimize desired properties while incorporating highly complex and non-differentiable rules remains to be a challenging task. Here we propose Graph Convolutional Policy Network (GCPN), a general graph convolutional network based model for goaldirected graph generation through reinforcement learning. The model is trained to optimize domain-specific rewards and adversarial loss through policy gradient, and acts in an environment that incorporates domain-specific rules. Experimental results show that GCPN can achieve 61% improvement on chemical property optimization over state-of-the-art baselines while resembling known molecules, and achieve 184% improvement on the constrained property optimization task.</t>
+          <t xml:space="preserve"> generating novel graph structures that optimize given objectives while obeying some given underlying rules is fundamental for chemistry, biology and social science research. this is especially important in the task of molecular graph generation, whose goal is to discover novel molecules with desired properties such as drug likeness and synthetic accessibility, while obeying physical laws such as chemical valency. however, designing models to find molecules that optimize desired properties while incorporating highly complex and non differentiable rules remains to be a challenging task. here we propose graph convolutional policy network (gcpn), a general graph convolutional network based model for goaldirected graph generation through reinforcement learning. the model is trained to optimize domain specific rewards and adversarial loss through policy gradient, and acts in an environment that incorporates domain specific rules. experimental results show that gcpn can achieve 61% improvement on chemical property optimization over state of the art baselines while resembling known molecules, and achieve 184% improvement on the constrained property optimization task.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1521,16 +1521,16 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[12, 16]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.452|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.261|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.073|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.144|x10: 0.000|x11: 0.073|x12: 0.193|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.121|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.298|x3: 0.000|x4: 0.180|x5: 0.000|x6: 0.000|x7: 0.079|x8: 0.272|x9: 0.295|x10: 0.067|x11: 0.000|x12: 0.184|x13: 0.000|x14: 0.000|x15: 0.133|x16: 0.312|x17: 0.000
-TOP2VEC -&gt; x1: 0.196|x2: 0.000|x3: 0.138|x4: 0.406|x5: 0.349|x6: 0.222|x7: 0.387|x8: 0.297|x9: 0.359|x10: 0.088|x11: 0.180|x12: 0.191|x13: 0.063|x14: 0.125|x15: 0.064|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.099|x3: 0.197|x4: 0.195|x5: 0.116|x6: 0.074|x7: 0.155|x8: 0.190|x9: 0.218|x10: 0.051|x11: 0.147|x12: 0.125|x13: 0.021|x14: 0.042|x15: 0.066|x16: 0.164|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.064|x4: 0.064|x5: 0.059|x6: 0.056|x7: 0.061|x8: 0.063|x9: 0.065|x10: 0.055|x11: 0.061|x12: 0.059|x13: 0.054|x14: 0.055|x15: 0.056|x16: 0.062|x17: 0.052
+TOP2VEC -&gt; x1: 0.133|x2: 0.000|x3: 0.086|x4: 0.078|x5: 0.222|x6: 0.000|x7: 0.197|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.058|x12: 0.246|x13: 0.101|x14: 0.136|x15: 0.000|x16: 0.142|x17: 0.000
+BERTOPIC -&gt; x1: 0.197|x2: 0.146|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.093|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.114|x12: 0.090|x13: 0.346|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.083|x2: 0.111|x3: 0.022|x4: 0.083|x5: 0.056|x6: 0.000|x7: 0.092|x8: 0.068|x9: 0.110|x10: 0.017|x11: 0.061|x12: 0.178|x13: 0.112|x14: 0.034|x15: 0.033|x16: 0.144|x17: 0.000
 </t>
         </is>
       </c>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Discrete hidden Markov models (HMMs) were applied to classify pregnancy disorders. The observation sequence was generated by transforming RR and systolic blood pressure time series using symbolic dynamics. Time series were recorded from 15 women with pregnancy-induced hypertension, 34 with preeclampsia and 41 controls beyond 30th gestational week. HMMs with five to ten hidden states were found to be sufficient to characterize different blood pressure variability, whereas significant classification in RR-based HMMs was found using fifteen hidden states. Pregnancy disorders preeclampsia and pregnancy induced hypertension revealed different patho-physiological autonomous regulation supposing different etiology of both disorders.</t>
+          <t xml:space="preserve"> discrete hidden markov models (hmms) were applied to classify pregnancy disorders. the observation sequence was generated by transforming rr and systolic blood pressure time series using symbolic dynamics. time series were recorded from 15 women with pregnancy induced hypertension, 34 with preeclampsia and 41 controls beyond 30th gestational week. hmms with five to ten hidden states were found to be sufficient to characterize different blood pressure variability, whereas significant classification in rr based hmms was found using fifteen hidden states. pregnancy disorders preeclampsia and pregnancy induced hypertension revealed different patho physiological autonomous regulation supposing different etiology of both disorders.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1551,16 +1551,16 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 10]</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.364|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.165|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.226|x4: 0.000|x5: 0.148|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.099|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.208|x3: 0.379|x4: 0.000|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.190|x9: 0.060|x10: 0.367|x11: 0.000|x12: 0.000|x13: 0.187|x14: 0.203|x15: 0.000|x16: 0.054|x17: 0.000
-TOP2VEC -&gt; x1: 0.201|x2: 0.000|x3: 0.298|x4: 0.242|x5: 0.268|x6: 0.069|x7: 0.465|x8: 0.253|x9: 0.095|x10: 0.076|x11: 0.190|x12: 0.326|x13: 0.099|x14: 0.000|x15: 0.000|x16: 0.156|x17: 0.000
-MEAN -&gt; x1: 0.067|x2: 0.069|x3: 0.347|x4: 0.081|x5: 0.168|x6: 0.023|x7: 0.155|x8: 0.148|x9: 0.052|x10: 0.148|x11: 0.119|x12: 0.109|x13: 0.095|x14: 0.068|x15: 0.000|x16: 0.070|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.057|x3: 0.075|x4: 0.057|x5: 0.063|x6: 0.054|x7: 0.062|x8: 0.061|x9: 0.056|x10: 0.061|x11: 0.060|x12: 0.059|x13: 0.058|x14: 0.057|x15: 0.053|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.106|x3: 0.413|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.150|x8: 0.109|x9: 0.000|x10: 0.413|x11: 0.194|x12: 0.066|x13: 0.169|x14: 0.000|x15: 0.000|x16: 0.200|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.078|x3: 0.379|x4: 0.000|x5: 0.096|x6: 0.000|x7: 0.038|x8: 0.075|x9: 0.015|x10: 0.220|x11: 0.048|x12: 0.016|x13: 0.089|x14: 0.051|x15: 0.000|x16: 0.064|x17: 0.000
 </t>
         </is>
       </c>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Substance use and abuse is a significant public health problem in the United States. Group-based intervention programs offer a promising means of reducing substance abuse. While effective, inappropriate intervention groups can result in an increase in deviant behaviors among participants, a process known as deviancy training. In this paper, we present GUIDE, an AI-based decision aid that leverages social network information to optimize the structure of the intervention groups.</t>
+          <t xml:space="preserve"> substance use and abuse is a significant public health problem in the united states. group based intervention programs offer a promising means of reducing substance abuse. while effective, inappropriate intervention groups can result in an increase in deviant behaviors among participants, a process known as deviancy training. in this paper, we present guide, an ai based decision aid that leverages social network information to optimize the structure of the intervention groups.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1586,11 +1586,11 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.063|x2: 0.000|x3: 0.587|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.054|x11: 0.236|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.098|x2: 0.000|x3: 0.300|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.090|x10: 0.000|x11: 0.068|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.082|x17: 0.000
 LDA -&gt; x1: 0.224|x2: 0.064|x3: 0.290|x4: 0.183|x5: 0.000|x6: 0.000|x7: 0.051|x8: 0.100|x9: 0.184|x10: 0.135|x11: 0.000|x12: 0.096|x13: 0.389|x14: 0.000|x15: 0.000|x16: 0.104|x17: 0.000
-TOP2VEC -&gt; x1: 0.115|x2: 0.165|x3: 0.210|x4: 0.000|x5: 0.190|x6: 0.059|x7: 0.000|x8: 0.213|x9: 0.400|x10: 0.059|x11: 0.282|x12: 0.247|x13: 0.000|x14: 0.360|x15: 0.243|x16: 0.121|x17: 0.000
-MEAN -&gt; x1: 0.134|x2: 0.076|x3: 0.333|x4: 0.061|x5: 0.063|x6: 0.020|x7: 0.017|x8: 0.104|x9: 0.195|x10: 0.083|x11: 0.173|x12: 0.114|x13: 0.130|x14: 0.120|x15: 0.081|x16: 0.075|x17: 0.000
-SOFTMAX -&gt; x1: 0.060|x2: 0.057|x3: 0.074|x4: 0.056|x5: 0.056|x6: 0.054|x7: 0.054|x8: 0.059|x9: 0.064|x10: 0.057|x11: 0.063|x12: 0.059|x13: 0.060|x14: 0.060|x15: 0.057|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.066|x3: 0.111|x4: 0.000|x5: 0.067|x6: 0.272|x7: 0.161|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.151|x12: 0.311|x13: 0.000|x14: 0.097|x15: 0.143|x16: 0.209|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.081|x2: 0.032|x3: 0.300|x4: 0.046|x5: 0.017|x6: 0.068|x7: 0.053|x8: 0.025|x9: 0.069|x10: 0.034|x11: 0.055|x12: 0.102|x13: 0.097|x14: 0.024|x15: 0.036|x16: 0.099|x17: 0.000
 </t>
         </is>
       </c>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We seek to automate the design of molecules based on specific chemical properties. In computational terms, this task involves continuous embedding and generation of molecular graphs. Our primary contribution is the direct realization of molecular graphs, a task previously approached by generating linear SMILES strings instead of graphs. Our junction tree variational autoencoder generates molecular graphs in two phases, by first generating a tree-structured scaffold over chemical substructures, and then combining them into a molecule with a graph message passing network. This approach allows us to incrementally expand molecules while maintaining chemical validity at every step. We evaluate our model on multiple tasks ranging from molecular generation to optimization. Across these tasks, our model outperforms previous state-of-the-art baselines by a significant margin.</t>
+          <t xml:space="preserve"> we seek to automate the design of molecules based on specific chemical properties. in computational terms, this task involves continuous embedding and generation of molecular graphs. our primary contribution is the direct realization of molecular graphs, a task previously approached by generating linear smiles strings instead of graphs. our junction tree variational autoencoder generates molecular graphs in two phases, by first generating a tree structured scaffold over chemical substructures, and then combining them into a molecule with a graph message passing network. this approach allows us to incrementally expand molecules while maintaining chemical validity at every step. we evaluate our model on multiple tasks ranging from molecular generation to optimization. across these tasks, our model outperforms previous state of the art baselines by a significant margin.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1611,16 +1611,16 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[7, 9]</t>
+          <t>[4, 9, 12, 13]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.300|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.173|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.127|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.092|x10: 0.000|x11: 0.000|x12: 0.200|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.068|x3: 0.000|x4: 0.197|x5: 0.054|x6: 0.000|x7: 0.226|x8: 0.254|x9: 0.308|x10: 0.063|x11: 0.122|x12: 0.079|x13: 0.000|x14: 0.000|x15: 0.313|x16: 0.136|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.262|x3: 0.000|x4: 0.301|x5: 0.443|x6: 0.407|x7: 0.601|x8: 0.309|x9: 0.369|x10: 0.152|x11: 0.094|x12: 0.306|x13: 0.151|x14: 0.171|x15: 0.158|x16: 0.311|x17: 0.000
-MEAN -&gt; x1: 0.074|x2: 0.110|x3: 0.100|x4: 0.166|x5: 0.166|x6: 0.136|x7: 0.242|x8: 0.187|x9: 0.226|x10: 0.072|x11: 0.130|x12: 0.128|x13: 0.050|x14: 0.057|x15: 0.157|x16: 0.149|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.057|x4: 0.061|x5: 0.061|x6: 0.059|x7: 0.066|x8: 0.062|x9: 0.065|x10: 0.056|x11: 0.059|x12: 0.059|x13: 0.054|x14: 0.055|x15: 0.061|x16: 0.060|x17: 0.052
+TOP2VEC -&gt; x1: 0.113|x2: 0.000|x3: 0.000|x4: 0.178|x5: 0.262|x6: 0.000|x7: 0.184|x8: 0.126|x9: 0.184|x10: 0.203|x11: 0.095|x12: 0.449|x13: 0.182|x14: 0.360|x15: 0.000|x16: 0.059|x17: 0.000
+BERTOPIC -&gt; x1: 0.164|x2: 0.121|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.068|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.091|x12: 0.068|x13: 0.474|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.069|x2: 0.047|x3: 0.000|x4: 0.125|x5: 0.079|x6: 0.000|x7: 0.119|x8: 0.095|x9: 0.146|x10: 0.066|x11: 0.077|x12: 0.199|x13: 0.164|x14: 0.090|x15: 0.078|x16: 0.049|x17: 0.000
 </t>
         </is>
       </c>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Cancer has been characterized as a heterogeneous disease consisting of many different subtypes. The early diag-13 nosis and prognosis of a cancer type have become a necessity in cancer research, as it can facilitate the subsequent 14 clinical management of patients. The importance of classifying cancer patients into high or low risk groups has 15 led many research teams, from the biomedical and the bioinformatics field, to study the application of machine 16 learning (ML) methods. Therefore, these techniques have been utilized as an aim to model the progression and 17 treatment of cancerous conditions. In addition, the ability of ML tools to detect key features from complex 18 datasets reveals their importance. A variety of these techniques, including Artificial Neural Networks (ANNs), 19 Bayesian Networks (BNs), Support Vector Machines (SVMs) and Decision Trees (DTs) have been widely applied 20 in cancer research for the development of predictive models, resulting in effective and accurate decision making. 21 Even though it is evident that the use of ML methods can improve our understanding of cancer progression, an 22 appropriate level of validation is needed in order for these methods to be considered in the everyday clinical prac-23 tice. In this work, we present a review of recent ML approaches employed in the modeling of cancer progression. 24 The predictive models discussed here are based on various supervised ML techniques as well as on different input 25 features and data samples. Given the growing trend on the application of ML methods in cancer research, we 26 present here the most recent publications that employ these techniques as an aim to model cancer risk or patient 27 outcomes.</t>
+          <t xml:space="preserve"> cancer has been characterized as a heterogeneous disease consisting of many different subtypes. the early diag 13 nosis and prognosis of a cancer type have become a necessity in cancer research, as it can facilitate the subsequent 14 clinical management of patients. the importance of classifying cancer patients into high or low risk groups has 15 led many research teams, from the biomedical and the bioinformatics field, to study the application of machine 16 learning (ml) methods. therefore, these techniques have been utilized as an aim to model the progression and 17 treatment of cancerous conditions. in addition, the ability of ml tools to detect key features from complex 18 datasets reveals their importance. a variety of these techniques, including artificial neural networks (anns), 19 bayesian networks (bns), support vector machines (svms) and decision trees (dts) have been widely applied 20 in cancer research for the development of predictive models, resulting in effective and accurate decision making. 21 even though it is evident that the use of ml methods can improve our understanding of cancer progression, an 22 appropriate level of validation is needed in order for these methods to be considered in the everyday clinical prac 23 tice. in this work, we present a review of recent ml approaches employed in the modeling of cancer progression. 24 the predictive models discussed here are based on various supervised ml techniques as well as on different input 25 features and data samples. given the growing trend on the application of ml methods in cancer research, we 26 present here the most recent publications that employ these techniques as an aim to model cancer risk or patient 27 outcomes.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1641,16 +1641,16 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[3, 4]</t>
+          <t>[3, 9]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.939|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.499|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.402|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.159|x10: 0.000|x11: 0.082|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.182|x3: 0.295|x4: 0.397|x5: 0.177|x6: 0.000|x7: 0.070|x8: 0.000|x9: 0.264|x10: 0.000|x11: 0.000|x12: 0.066|x13: 0.093|x14: 0.000|x15: 0.134|x16: 0.142|x17: 0.000
-TOP2VEC -&gt; x1: 0.240|x2: 0.315|x3: 0.343|x4: 0.231|x5: 0.397|x6: 0.142|x7: 0.376|x8: 0.319|x9: 0.201|x10: 0.097|x11: 0.087|x12: 0.133|x13: 0.105|x14: 0.284|x15: 0.183|x16: 0.198|x17: 0.000
-MEAN -&gt; x1: 0.080|x2: 0.166|x3: 0.379|x4: 0.209|x5: 0.191|x6: 0.047|x7: 0.149|x8: 0.106|x9: 0.155|x10: 0.032|x11: 0.195|x12: 0.066|x13: 0.066|x14: 0.095|x15: 0.106|x16: 0.114|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.075|x4: 0.064|x5: 0.063|x6: 0.054|x7: 0.060|x8: 0.057|x9: 0.060|x10: 0.053|x11: 0.063|x12: 0.055|x13: 0.055|x14: 0.057|x15: 0.057|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.176|x8: 0.000|x9: 0.207|x10: 0.190|x11: 0.255|x12: 0.137|x13: 0.080|x14: 0.144|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.046|x3: 0.299|x4: 0.099|x5: 0.044|x6: 0.000|x7: 0.062|x8: 0.000|x9: 0.158|x10: 0.047|x11: 0.084|x12: 0.051|x13: 0.043|x14: 0.036|x15: 0.034|x16: 0.036|x17: 0.000
 </t>
         </is>
       </c>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Pre-eclampsia is a multi-system disorder of pregnancy with major maternal and perinatal implications. Emerging therapeutic strategies are most likely to be maximally effective if commenced weeks or even months prior to the clinical presentation of the disease. Although widespread plasma alterations precede the clinical onset of pre-eclampsia, no single plasma constituent has emerged as a sensitive or specific predictor of risk. Consequently, currently available methods of identifying the condition prior to clinical presentation are of limited clinical use. We have exploited genetic programming, a powerful data mining method, to identify patterns of metabolites that distinguish plasma from patients with pre-eclampsia from that taken from healthy, matched controls. High-resolution gas chromatography time-of-flight mass spectrometry (GC-tof-MS) was performed on 87 plasma samples from women with pre-eclampsia and 87 matched controls. Normalised peak intensity data were fed into the Genetic Programming (GP) system which was set up to produce a model that gave an output of 1 for patients and 0 for controls. The model was trained on 50% of the data generated and tested on a separate hold-out set of 50%. The model generated by GP from the GC-tof-MS data identified a metabolomic pattern that could be used to produce two simple rules that together discriminate pre-eclampsia from normal pregnant controls using just 3 of the metabolite peak variables, with a sensitivity of 100% and a specificity of 98%. Thus, preeclampsia can be diagnosed at the level of small-molecule metabolism in blood plasma. These findings justify a prospective assessment of metabolomic technology as a screening tool for pre-eclampsia, while identification of the metabolites involved may lead to an improved understanding of the aetiological basis of pre-eclampsia and thus the development of targeted therapies.</t>
+          <t xml:space="preserve"> pre eclampsia is a multi system disorder of pregnancy with major maternal and perinatal implications. emerging therapeutic strategies are most likely to be maximally effective if commenced weeks or even months prior to the clinical presentation of the disease. although widespread plasma alterations precede the clinical onset of pre eclampsia, no single plasma constituent has emerged as a sensitive or specific predictor of risk. consequently, currently available methods of identifying the condition prior to clinical presentation are of limited clinical use. we have exploited genetic programming, a powerful data mining method, to identify patterns of metabolites that distinguish plasma from patients with pre eclampsia from that taken from healthy, matched controls. high resolution gas chromatography time of flight mass spectrometry (gc tof ms) was performed on 87 plasma samples from women with pre eclampsia and 87 matched controls. normalised peak intensity data were fed into the genetic programming (gp) system which was set up to produce a model that gave an output of 1 for patients and 0 for controls. the model was trained on 50% of the data generated and tested on a separate hold out set of 50%. the model generated by gp from the gc tof ms data identified a metabolomic pattern that could be used to produce two simple rules that together discriminate pre eclampsia from normal pregnant controls using just 3 of the metabolite peak variables, with a sensitivity of 100% and a specificity of 98%. thus, preeclampsia can be diagnosed at the level of small molecule metabolism in blood plasma. these findings justify a prospective assessment of metabolomic technology as a screening tool for pre eclampsia, while identification of the metabolites involved may lead to an improved understanding of the aetiological basis of pre eclampsia and thus the development of targeted therapies.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1676,11 +1676,11 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.531|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.337|x4: 0.134|x5: 0.113|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.084|x13: 0.078|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.113|x3: 0.229|x4: 0.204|x5: 0.250|x6: 0.068|x7: 0.055|x8: 0.124|x9: 0.000|x10: 0.082|x11: 0.078|x12: 0.082|x13: 0.000|x14: 0.139|x15: 0.205|x16: 0.191|x17: 0.000
-TOP2VEC -&gt; x1: 0.174|x2: 0.270|x3: 0.187|x4: 0.333|x5: 0.251|x6: 0.088|x7: 0.390|x8: 0.170|x9: 0.000|x10: 0.127|x11: 0.189|x12: 0.258|x13: 0.230|x14: 0.087|x15: 0.000|x16: 0.261|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.127|x3: 0.305|x4: 0.179|x5: 0.167|x6: 0.052|x7: 0.148|x8: 0.098|x9: 0.000|x10: 0.070|x11: 0.169|x12: 0.113|x13: 0.077|x14: 0.075|x15: 0.068|x16: 0.151|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.071|x4: 0.063|x5: 0.062|x6: 0.055|x7: 0.061|x8: 0.058|x9: 0.053|x10: 0.056|x11: 0.062|x12: 0.059|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.061|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.078|x3: 0.237|x4: 0.100|x5: 0.111|x6: 0.000|x7: 0.196|x8: 0.000|x9: 0.000|x10: 0.073|x11: 0.186|x12: 0.307|x13: 0.096|x14: 0.000|x15: 0.000|x16: 0.190|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.048|x3: 0.326|x4: 0.110|x5: 0.118|x6: 0.017|x7: 0.063|x8: 0.031|x9: 0.000|x10: 0.039|x11: 0.066|x12: 0.118|x13: 0.043|x14: 0.035|x15: 0.051|x16: 0.095|x17: 0.000
 </t>
         </is>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Hypertensive disorders are the leading cause of deaths during pregnancy. Risk pregnancy accompaniment is essential to reduce these complications. Decision support systems (DSS) are important tools to patients' accompaniment. These systems provide relevant information to health experts about clinical condition of the patient anywhere and anytime. In this paper, a model that uses the Naïve Bayesian classifier is introduced and its performance is evaluated in comparison with the Data Mining (DM) classifier named J48 Decision Tree. This study includes the modeling, performance evaluation, and comparison between models that could be used to assess pregnancy complications. Evaluation analysis of the results is performed through the use of Confusion Matrix indicators. The founded results show that J48 decision tree classifier performs better for almost all the used indicators, confirming its promising accuracy for identifying hypertensive disorders on pregnancy.</t>
+          <t xml:space="preserve"> hypertensive disorders are the leading cause of deaths during pregnancy. risk pregnancy accompaniment is essential to reduce these complications. decision support systems (dss) are important tools to patients accompaniment. these systems provide relevant information to health experts about clinical condition of the patient anywhere and anytime. in this paper, a model that uses the naïve bayesian classifier is introduced and its performance is evaluated in comparison with the data mining (dm) classifier named j48 decision tree. this study includes the modeling, performance evaluation, and comparison between models that could be used to assess pregnancy complications. evaluation analysis of the results is performed through the use of confusion matrix indicators. the founded results show that j48 decision tree classifier performs better for almost all the used indicators, confirming its promising accuracy for identifying hypertensive disorders on pregnancy.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1701,16 +1701,16 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 13]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.779|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.304|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.355|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.066|x10: 0.000|x11: 0.064|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.411|x4: 0.070|x5: 0.168|x6: 0.087|x7: 0.056|x8: 0.000|x9: 0.000|x10: 0.087|x11: 0.000|x12: 0.078|x13: 0.308|x14: 0.146|x15: 0.274|x16: 0.134|x17: 0.000
-TOP2VEC -&gt; x1: 0.170|x2: 0.139|x3: 0.375|x4: 0.000|x5: 0.181|x6: 0.118|x7: 0.330|x8: 0.167|x9: 0.000|x10: 0.000|x11: 0.095|x12: 0.273|x13: 0.252|x14: 0.373|x15: 0.189|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.046|x3: 0.429|x4: 0.023|x5: 0.116|x6: 0.068|x7: 0.129|x8: 0.056|x9: 0.000|x10: 0.029|x11: 0.133|x12: 0.117|x13: 0.187|x14: 0.173|x15: 0.154|x16: 0.045|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.081|x4: 0.054|x5: 0.059|x6: 0.056|x7: 0.060|x8: 0.056|x9: 0.053|x10: 0.054|x11: 0.060|x12: 0.059|x13: 0.064|x14: 0.063|x15: 0.062|x16: 0.055|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.300|x4: 0.000|x5: 0.000|x6: 0.119|x7: 0.101|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.167|x12: 0.377|x13: 0.203|x14: 0.260|x15: 0.061|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.392|x4: 0.018|x5: 0.042|x6: 0.052|x7: 0.039|x8: 0.000|x9: 0.017|x10: 0.022|x11: 0.058|x12: 0.114|x13: 0.128|x14: 0.102|x15: 0.084|x16: 0.034|x17: 0.000
 </t>
         </is>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bronchopulmonary dysplasia (BPD), necrotizing enterocolitis (NEC), and retinopathy of prematurity (ROP) are severe complications affecting Very Low Birth Weight (VLBW) infants. Our findings show that data gathered in the intensive care unit during the first 24 or 72 hours of care can be used to predict whether a VLBW infant is at risk of developing BPD. Using Gaussian process classification, we achieved classification results with areas under the receiver operator characteristic curve of 0.85 (standard error (SE) 0.05) for 24h and 0.87 (SE 0.06) for 72h BPD data. This compares favourably with results achieved using the clinical standard SNAP-II and SNAPPE-II scores. Sensitivity for BPD was 0.52 (SE 0.06). Sensitivity for NEC and ROP was close to zero, suggesting that NEC and ROP can not be reliably predicted with this approach from our data set.</t>
+          <t xml:space="preserve"> bronchopulmonary dysplasia (bpd), necrotizing enterocolitis (nec), and retinopathy of prematurity (rop) are severe complications affecting very low birth weight (vlbw) infants. our findings show that data gathered in the intensive care unit during the first 24 or 72 hours of care can be used to predict whether a vlbw infant is at risk of developing bpd. using gaussian process classification, we achieved classification results with areas under the receiver operator characteristic curve of 0.85 (standard error (se) 0.05) for 24h and 0.87 (se 0.06) for 72h bpd data. this compares favourably with results achieved using the clinical standard snap ii and snappe ii scores. sensitivity for bpd was 0.52 (se 0.06). sensitivity for nec and rop was close to zero, suggesting that nec and rop can not be reliably predicted with this approach from our data set.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1731,16 +1731,16 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[2, 3, 4]</t>
+          <t>[2, 3, 4, 10]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.401|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.190|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.171|x3: 0.230|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.111|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.133|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.404|x3: 0.182|x4: 0.498|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.091|x9: 0.118|x10: 0.281|x11: 0.000|x12: 0.000|x13: 0.080|x14: 0.165|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.278|x2: 0.584|x3: 0.190|x4: 0.304|x5: 0.121|x6: 0.000|x7: 0.238|x8: 0.355|x9: 0.225|x10: 0.093|x11: 0.230|x12: 0.427|x13: 0.177|x14: 0.276|x15: 0.085|x16: 0.190|x17: 0.000
-MEAN -&gt; x1: 0.093|x2: 0.301|x3: 0.258|x4: 0.267|x5: 0.040|x6: 0.000|x7: 0.079|x8: 0.149|x9: 0.115|x10: 0.125|x11: 0.140|x12: 0.142|x13: 0.086|x14: 0.147|x15: 0.028|x16: 0.063|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.070|x3: 0.067|x4: 0.068|x5: 0.054|x6: 0.052|x7: 0.056|x8: 0.060|x9: 0.058|x10: 0.059|x11: 0.060|x12: 0.060|x13: 0.057|x14: 0.060|x15: 0.053|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.075|x2: 0.205|x3: 0.335|x4: 0.127|x5: 0.210|x6: 0.085|x7: 0.267|x8: 0.000|x9: 0.122|x10: 0.500|x11: 0.228|x12: 0.000|x13: 0.322|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.019|x2: 0.195|x3: 0.312|x4: 0.156|x5: 0.053|x6: 0.021|x7: 0.067|x8: 0.023|x9: 0.060|x10: 0.223|x11: 0.057|x12: 0.000|x13: 0.101|x14: 0.041|x15: 0.033|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In cardiac magnetic resonance imaging, fully-automatic segmentation of the heart enables precise structural and functional measurements to be taken, e.g. from short-axis MR images of the left-ventricle. In this work we propose a recurrent fully-convolutional network (RFCN) that learns image representations from the full stack of 2D slices and has the ability to leverage inter-slice spatial dependences through internal memory units. RFCN combines anatomical detection and segmentation into a single architecture that is trained end-to-end thus significantly reducing computational time, simplifying the segmentation pipeline, and potentially enabling real-time applications. We report on an investigation of RFCN using two datasets, including the publicly available MICCAI 2009 Challenge dataset. Comparisons have been carried out between fully convolutional networks and deep restricted Boltzmann machines, including a recurrent version that leverages inter-slice spatial correlation. Our studies suggest that RFCN produces state-of-the-art results and can substantially improve the delineation of contours near the apex of the heart.</t>
+          <t xml:space="preserve"> in cardiac magnetic resonance imaging, fully automatic segmentation of the heart enables precise structural and functional measurements to be taken, e.g. from short axis mr images of the left ventricle. in this work we propose a recurrent fully convolutional network (rfcn) that learns image representations from the full stack of 2d slices and has the ability to leverage inter slice spatial dependences through internal memory units. rfcn combines anatomical detection and segmentation into a single architecture that is trained end to end thus significantly reducing computational time, simplifying the segmentation pipeline, and potentially enabling real time applications. we report on an investigation of rfcn using two datasets, including the publicly available miccai 2009 challenge dataset. comparisons have been carried out between fully convolutional networks and deep restricted boltzmann machines, including a recurrent version that leverages inter slice spatial correlation. our studies suggest that rfcn produces state of the art results and can substantially improve the delineation of contours near the apex of the heart.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1761,16 +1761,16 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[4, 5, 7, 9]</t>
+          <t>[5, 7, 9, 11, 16]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.444|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.257|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.138|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.144|x10: 0.000|x11: 0.138|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.142|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.074|x3: 0.079|x4: 0.219|x5: 0.195|x6: 0.000|x7: 0.144|x8: 0.000|x9: 0.246|x10: 0.000|x11: 0.071|x12: 0.145|x13: 0.090|x14: 0.214|x15: 0.056|x16: 0.286|x17: 0.000
-TOP2VEC -&gt; x1: 0.183|x2: 0.146|x3: 0.000|x4: 0.551|x5: 0.449|x6: 0.366|x7: 0.588|x8: 0.288|x9: 0.406|x10: 0.107|x11: 0.211|x12: 0.320|x13: 0.061|x14: 0.186|x15: 0.000|x16: 0.220|x17: 0.000
-MEAN -&gt; x1: 0.061|x2: 0.073|x3: 0.174|x4: 0.240|x5: 0.214|x6: 0.122|x7: 0.215|x8: 0.096|x9: 0.217|x10: 0.036|x11: 0.180|x12: 0.155|x13: 0.050|x14: 0.133|x15: 0.019|x16: 0.169|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.056|x3: 0.062|x4: 0.066|x5: 0.064|x6: 0.058|x7: 0.064|x8: 0.057|x9: 0.064|x10: 0.054|x11: 0.062|x12: 0.060|x13: 0.054|x14: 0.059|x15: 0.053|x16: 0.061|x17: 0.052
+TOP2VEC -&gt; x1: 0.104|x2: 0.000|x3: 0.000|x4: 0.163|x5: 0.223|x6: 0.154|x7: 0.351|x8: 0.000|x9: 0.197|x10: 0.000|x11: 0.384|x12: 0.122|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.135|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.354|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.026|x2: 0.019|x3: 0.020|x4: 0.095|x5: 0.139|x6: 0.039|x7: 0.124|x8: 0.000|x9: 0.147|x10: 0.000|x11: 0.148|x12: 0.067|x13: 0.023|x14: 0.053|x15: 0.103|x16: 0.141|x17: 0.000
 </t>
         </is>
       </c>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Anticipating the future actions of a human is a widely studied problem in robotics that requires spatiotemporal reasoning. In this work we propose a deep learning approach for anticipation in sensory-rich robotics applications. We introduce a sensory-fusion architecture which jointly learns to anticipate and fuse information from multiple sensory streams. Our architecture consists of Recurrent Neural Networks (RNNs) that use Long Short-Term Memory (LSTM) units to capture long temporal dependencies. We train our architecture in a sequence-to-sequence prediction manner, and it explicitly learns to predict the future given only a partial temporal context. We further introduce a novel loss layer for anticipation which prevents over-fitting and encourages early anticipation. We use our architecture to anticipate driving maneuvers several seconds before they happen on a natural driving data set of 1180 miles. The context for maneuver anticipation comes from multiple sensors installed on the vehicle. Our approach shows significant improvement over the state-of-the-art in maneuver anticipation by increasing the precision from 77.4% to 90.5% and recall from 71.2% to 87.4%.</t>
+          <t xml:space="preserve"> anticipating the future actions of a human is a widely studied problem in robotics that requires spatiotemporal reasoning. in this work we propose a deep learning approach for anticipation in sensory rich robotics applications. we introduce a sensory fusion architecture which jointly learns to anticipate and fuse information from multiple sensory streams. our architecture consists of recurrent neural networks (rnns) that use long short term memory (lstm) units to capture long temporal dependencies. we train our architecture in a sequence to sequence prediction manner, and it explicitly learns to predict the future given only a partial temporal context. we further introduce a novel loss layer for anticipation which prevents over fitting and encourages early anticipation. we use our architecture to anticipate driving maneuvers several seconds before they happen on a natural driving data set of 1180 miles. the context for maneuver anticipation comes from multiple sensors installed on the vehicle. our approach shows significant improvement over the state of the art in maneuver anticipation by increasing the precision from 77.4% to 90.5% and recall from 71.2% to 87.4%.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1791,16 +1791,16 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[3, 9, 13, 14, 15]</t>
+          <t>[9, 13, 15]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.445|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.257|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.130|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.141|x14: 0.000|x15: 0.205|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.075|x3: 0.140|x4: 0.197|x5: 0.000|x6: 0.000|x7: 0.094|x8: 0.000|x9: 0.351|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.226|x14: 0.239|x15: 0.447|x16: 0.053|x17: 0.000
-TOP2VEC -&gt; x1: 0.312|x2: 0.342|x3: 0.069|x4: 0.276|x5: 0.128|x6: 0.307|x7: 0.471|x8: 0.360|x9: 0.435|x10: 0.109|x11: 0.254|x12: 0.454|x13: 0.470|x14: 0.435|x15: 0.417|x16: 0.223|x17: 0.000
-MEAN -&gt; x1: 0.104|x2: 0.139|x3: 0.218|x4: 0.157|x5: 0.043|x6: 0.102|x7: 0.188|x8: 0.120|x9: 0.262|x10: 0.036|x11: 0.170|x12: 0.151|x13: 0.232|x14: 0.224|x15: 0.288|x16: 0.092|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.063|x4: 0.059|x5: 0.053|x6: 0.056|x7: 0.061|x8: 0.057|x9: 0.066|x10: 0.052|x11: 0.060|x12: 0.059|x13: 0.064|x14: 0.063|x15: 0.067|x16: 0.055|x17: 0.051
+TOP2VEC -&gt; x1: 0.162|x2: 0.000|x3: 0.166|x4: 0.000|x5: 0.000|x6: 0.257|x7: 0.342|x8: 0.000|x9: 0.141|x10: 0.000|x11: 0.139|x12: 0.103|x13: 0.292|x14: 0.180|x15: 0.219|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.175|x2: 0.127|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.092|x12: 0.000|x13: 0.500|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.084|x2: 0.050|x3: 0.076|x4: 0.049|x5: 0.000|x6: 0.064|x7: 0.109|x8: 0.000|x9: 0.155|x10: 0.000|x11: 0.058|x12: 0.026|x13: 0.290|x14: 0.105|x15: 0.218|x16: 0.013|x17: 0.000
 </t>
         </is>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Three criteria are suggested to help design a Clinical Decision Support System (CDSS) that would have a better chance of being successfully deployed in a clinical environment. These criteria have been successfully applied to a CDSS designed to estimate outcomes for neonatal intensive care unit (NICU) patients. The CDSS was deployed in a pilot study at the Children's Hospital of Eastern Ontario (CHEO)'s NICU. The results of the study showed that the accuracy was deemed acceptable by the physicians and the CDSS would meet their expectations when ready for deployment in a clinical environment.</t>
+          <t xml:space="preserve"> three criteria are suggested to help design a clinical decision support system (cdss) that would have a better chance of being successfully deployed in a clinical environment. these criteria have been successfully applied to a cdss designed to estimate outcomes for neonatal intensive care unit (nicu) patients. the cdss was deployed in a pilot study at the childrens hospital of eastern ontario (cheo)s nicu. the results of the study showed that the accuracy was deemed acceptable by the physicians and the cdss would meet their expectations when ready for deployment in a clinical environment.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1821,16 +1821,16 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[3, 4]</t>
+          <t>[3, 7]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.426|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.205|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.347|x3: 0.174|x4: 0.241|x5: 0.000|x6: 0.081|x7: 0.368|x8: 0.000|x9: 0.149|x10: 0.000|x11: 0.159|x12: 0.057|x13: 0.182|x14: 0.000|x15: 0.000|x16: 0.063|x17: 0.000
-TOP2VEC -&gt; x1: 0.171|x2: 0.000|x3: 0.339|x4: 0.386|x5: 0.295|x6: 0.000|x7: 0.067|x8: 0.201|x9: 0.205|x10: 0.118|x11: 0.000|x12: 0.161|x13: 0.222|x14: 0.222|x15: 0.000|x16: 0.241|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.116|x3: 0.313|x4: 0.209|x5: 0.098|x6: 0.027|x7: 0.145|x8: 0.067|x9: 0.118|x10: 0.039|x11: 0.121|x12: 0.073|x13: 0.135|x14: 0.074|x15: 0.000|x16: 0.101|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.073|x4: 0.065|x5: 0.059|x6: 0.055|x7: 0.061|x8: 0.057|x9: 0.060|x10: 0.055|x11: 0.060|x12: 0.057|x13: 0.061|x14: 0.057|x15: 0.053|x16: 0.059|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.334|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.119|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.294|x3: 0.174|x4: 0.000|x5: 0.092|x6: 0.097|x7: 0.419|x8: 0.000|x9: 0.158|x10: 0.107|x11: 0.155|x12: 0.056|x13: 0.180|x14: 0.000|x15: 0.000|x16: 0.088|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.058|x3: 0.144|x4: 0.218|x5: 0.067|x6: 0.000|x7: 0.282|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.058|x12: 0.243|x13: 0.057|x14: 0.138|x15: 0.000|x16: 0.150|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.088|x3: 0.288|x4: 0.055|x5: 0.040|x6: 0.024|x7: 0.175|x8: 0.000|x9: 0.069|x10: 0.027|x11: 0.053|x12: 0.075|x13: 0.059|x14: 0.035|x15: 0.000|x16: 0.059|x17: 0.000
 </t>
         </is>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Driver's fatigue is one of the major causes of traffic accidents, particularly for drivers of large vehicles (such as buses and heavy trucks) due to prolonged driving periods and boredom in working conditions. In this paper, we propose a vision-based fatigue detection system for bus driver monitoring, which is easy and flexible for deployment in buses and large vehicles. The system consists of modules of head-shoulder detection, face detection, eye detection, eye openness estimation, fusion, drowsiness measure percentage of eyelid closure (PERCLOS) estimation, and fatigue level classification. The core innovative techniques are as follows: 1) an approach to estimate the continuous level of eye openness based on spectral regression; and 2) a fusion algorithm to estimate the eye state based on adaptive integration on the multimodel detections of both eyes. A robust measure of PERCLOS on the continuous level of eye openness is defined, and the driver states are classified on it. In experiments, systematic evaluations and analysis of proposed algorithms, as well as comparison with ground truth on PERCLOS measurements, are performed. The experimental results show the advantages of the system on accuracy and robustness for the challenging situations when a camera of an oblique viewing angle to the driver's face is used for driving state monitoring.</t>
+          <t xml:space="preserve"> drivers fatigue is one of the major causes of traffic accidents, particularly for drivers of large vehicles (such as buses and heavy trucks) due to prolonged driving periods and boredom in working conditions. in this paper, we propose a vision based fatigue detection system for bus driver monitoring, which is easy and flexible for deployment in buses and large vehicles. the system consists of modules of head shoulder detection, face detection, eye detection, eye openness estimation, fusion, drowsiness measure percentage of eyelid closure (perclos) estimation, and fatigue level classification. the core innovative techniques are as follows: 1) an approach to estimate the continuous level of eye openness based on spectral regression; and 2) a fusion algorithm to estimate the eye state based on adaptive integration on the multimodel detections of both eyes. a robust measure of perclos on the continuous level of eye openness is defined, and the driver states are classified on it. in experiments, systematic evaluations and analysis of proposed algorithms, as well as comparison with ground truth on perclos measurements, are performed. the experimental results show the advantages of the system on accuracy and robustness for the challenging situations when a camera of an oblique viewing angle to the drivers face is used for driving state monitoring.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1856,11 +1856,11 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.490|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.278|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.222|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.214|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.317|x3: 0.295|x4: 0.318|x5: 0.103|x6: 0.000|x7: 0.066|x8: 0.000|x9: 0.247|x10: 0.133|x11: 0.129|x12: 0.000|x13: 0.149|x14: 0.000|x15: 0.000|x16: 0.062|x17: 0.000
-TOP2VEC -&gt; x1: 0.070|x2: 0.321|x3: 0.445|x4: 0.122|x5: 0.217|x6: 0.136|x7: 0.000|x8: 0.117|x9: 0.165|x10: 0.148|x11: 0.268|x12: 0.174|x13: 0.000|x14: 0.154|x15: 0.192|x16: 0.302|x17: 0.000
-MEAN -&gt; x1: 0.023|x2: 0.213|x3: 0.410|x4: 0.147|x5: 0.107|x6: 0.045|x7: 0.022|x8: 0.039|x9: 0.137|x10: 0.094|x11: 0.225|x12: 0.058|x13: 0.050|x14: 0.051|x15: 0.064|x16: 0.122|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.065|x3: 0.079|x4: 0.061|x5: 0.059|x6: 0.055|x7: 0.054|x8: 0.055|x9: 0.060|x10: 0.058|x11: 0.066|x12: 0.056|x13: 0.055|x14: 0.055|x15: 0.056|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.169|x3: 0.173|x4: 0.145|x5: 0.096|x6: 0.140|x7: 0.101|x8: 0.061|x9: 0.000|x10: 0.174|x11: 0.308|x12: 0.060|x13: 0.102|x14: 0.000|x15: 0.000|x16: 0.172|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.121|x3: 0.297|x4: 0.116|x5: 0.050|x6: 0.035|x7: 0.042|x8: 0.015|x9: 0.062|x10: 0.077|x11: 0.163|x12: 0.015|x13: 0.063|x14: 0.000|x15: 0.000|x16: 0.059|x17: 0.000
 </t>
         </is>
       </c>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The rate of depression is growing at an alarming rate. A study found that people are more likely to open up to a talking computer than a human. The aim of this paper is to motivate a person going through low phase of his life and to avoid ill-effects of depression. We propose a chatbot that can enable positivity boosting conversation with the user. The chatbot will personalize its replies as per user to keep the conversation engaging. It is made emotionally supportive by training it over a motivating dialogue corpus. The corpus is extended with the users historical chat data from social media platforms. Tensorflow framework and high power GPU is required by server for training. The advantage of such a system is that instead of reaching a phase requiring a visit to a psychiatrist, an online free service will reach many people, will mediate ill-effects of depression and contribute to the betterment of society.</t>
+          <t xml:space="preserve"> the rate of depression is growing at an alarming rate. a study found that people are more likely to open up to a talking computer than a human. the aim of this paper is to motivate a person going through low phase of his life and to avoid ill effects of depression. we propose a chatbot that can enable positivity boosting conversation with the user. the chatbot will personalize its replies as per user to keep the conversation engaging. it is made emotionally supportive by training it over a motivating dialogue corpus. the corpus is extended with the users historical chat data from social media platforms. tensorflow framework and high power gpu is required by server for training. the advantage of such a system is that instead of reaching a phase requiring a visit to a psychiatrist, an online free service will reach many people, will mediate ill effects of depression and contribute to the betterment of society.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1881,16 +1881,16 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[3, 8]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.078|x2: 0.000|x3: 0.333|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.206|x9: 0.000|x10: 0.000|x11: 0.147|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.096|x2: 0.000|x3: 0.301|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.238|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.140|x3: 0.094|x4: 0.236|x5: 0.000|x6: 0.000|x7: 0.125|x8: 0.443|x9: 0.468|x10: 0.108|x11: 0.108|x12: 0.000|x13: 0.097|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.139|x2: 0.000|x3: 0.091|x4: 0.336|x5: 0.340|x6: 0.335|x7: 0.257|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.168|x13: 0.124|x14: 0.000|x15: 0.185|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.072|x2: 0.047|x3: 0.173|x4: 0.191|x5: 0.113|x6: 0.112|x7: 0.127|x8: 0.269|x9: 0.156|x10: 0.036|x11: 0.085|x12: 0.056|x13: 0.074|x14: 0.000|x15: 0.062|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.064|x4: 0.065|x5: 0.060|x6: 0.060|x7: 0.061|x8: 0.070|x9: 0.063|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.058|x14: 0.053|x15: 0.057|x16: 0.053|x17: 0.053
+TOP2VEC -&gt; x1: 0.131|x2: 0.000|x3: 0.153|x4: 0.084|x5: 0.000|x6: 0.194|x7: 0.136|x8: 0.079|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.141|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.149|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.035|x3: 0.262|x4: 0.080|x5: 0.000|x6: 0.049|x7: 0.065|x8: 0.190|x9: 0.117|x10: 0.027|x11: 0.027|x12: 0.035|x13: 0.024|x14: 0.000|x15: 0.000|x16: 0.037|x17: 0.000
 </t>
         </is>
       </c>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this paper, we describe a process of constructing proxy variables that represent adult learners' time management strategies in an online course. Based upon previous research, three values were selected from a data set. According to the result of empirical validation, an (ir)regularity of the learning interval was proven to be correlative with and predict learning performance. As indicated in previous research, regularity of learning is a strong indicator to explain learners' consistent endeavors. This study demonstrates the possibility of using learning analytics to address a learner's specific competence on the basis of a theoretical background. Implications for the learning analytics field seeking a pedagogical theory-driven approach are discussed.</t>
+          <t xml:space="preserve"> in this paper, we describe a process of constructing proxy variables that represent adult learners time management strategies in an online course. based upon previous research, three values were selected from a data set. according to the result of empirical validation, an (ir)regularity of the learning interval was proven to be correlative with and predict learning performance. as indicated in previous research, regularity of learning is a strong indicator to explain learners consistent endeavors. this study demonstrates the possibility of using learning analytics to address a learners specific competence on the basis of a theoretical background. implications for the learning analytics field seeking a pedagogical theory driven approach are discussed.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1911,16 +1911,16 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[4, 11]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.484|x4: 0.142|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.280|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.348|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.147|x10: 0.000|x11: 0.063|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.123|x3: 0.109|x4: 0.362|x5: 0.093|x6: 0.000|x7: 0.124|x8: 0.113|x9: 0.169|x10: 0.101|x11: 0.000|x12: 0.133|x13: 0.173|x14: 0.000|x15: 0.123|x16: 0.198|x17: 0.000
-TOP2VEC -&gt; x1: 0.102|x2: 0.373|x3: 0.000|x4: 0.656|x5: 0.322|x6: 0.182|x7: 0.253|x8: 0.083|x9: 0.243|x10: 0.097|x11: 0.367|x12: 0.282|x13: 0.355|x14: 0.386|x15: 0.000|x16: 0.198|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.165|x3: 0.197|x4: 0.334|x5: 0.139|x6: 0.061|x7: 0.126|x8: 0.066|x9: 0.137|x10: 0.066|x11: 0.216|x12: 0.138|x13: 0.176|x14: 0.129|x15: 0.041|x16: 0.132|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.061|x3: 0.063|x4: 0.072|x5: 0.059|x6: 0.055|x7: 0.059|x8: 0.055|x9: 0.059|x10: 0.055|x11: 0.064|x12: 0.059|x13: 0.062|x14: 0.059|x15: 0.054|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.142|x2: 0.089|x3: 0.000|x4: 0.478|x5: 0.124|x6: 0.000|x7: 0.116|x8: 0.179|x9: 0.000|x10: 0.118|x11: 0.072|x12: 0.119|x13: 0.112|x14: 0.000|x15: 0.000|x16: 0.065|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.035|x2: 0.053|x3: 0.027|x4: 0.422|x5: 0.054|x6: 0.000|x7: 0.060|x8: 0.073|x9: 0.079|x10: 0.055|x11: 0.034|x12: 0.063|x13: 0.071|x14: 0.000|x15: 0.031|x16: 0.066|x17: 0.000
 </t>
         </is>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Although standard behavioral interventions for autism spectrum disorder (ASD) are effective therapies for social deficits, they face criticism for being time-intensive and overdependent on specialists. Earlier starting age of therapy is a strong predictor of later success, but waitlists for therapies can be 18 months long. To address these complications, we developed Superpower Glass, a machine-learning-assisted software system that runs on Google Glass and an Android smartphone, designed for use during social interactions. This pilot exploratory study examines our prototype tool's potential for social-affective learning for children with autism. We sent our tool home with 14 families and assessed changes from intake to conclusion through the Social Responsiveness Scale (SRS-2), a facial affect recognition task (EGG), and qualitative parent reports. A repeated-measures one-way ANOVA demonstrated a decrease in SRS-2 total scores by an average 7.14 points (F(1,13) = 33.20, p = &lt;.001, higher scores indicate higher ASD severity). EGG scores also increased by an average 9.55 correct responses (F(1,10) = 11.89, p = &lt;.01). Parents reported increased eye contact and greater social acuity. This feasibility study supports using mobile technologies for potential therapeutic purposes.</t>
+          <t xml:space="preserve"> although standard behavioral interventions for autism spectrum disorder (asd) are effective therapies for social deficits, they face criticism for being time intensive and overdependent on specialists. earlier starting age of therapy is a strong predictor of later success, but waitlists for therapies can be 18 months long. to address these complications, we developed superpower glass, a machine learning assisted software system that runs on google glass and an android smartphone, designed for use during social interactions. this pilot exploratory study examines our prototype tools potential for social affective learning for children with autism. we sent our tool home with 14 families and assessed changes from intake to conclusion through the social responsiveness scale (srs 2), a facial affect recognition task (egg), and qualitative parent reports. a repeated measures one way anova demonstrated a decrease in srs 2 total scores by an average 7.14 points (f(1,13) = 33.20, p = &lt;.001, higher scores indicate higher asd severity). egg scores also increased by an average 9.55 correct responses (f(1,10) = 11.89, p = &lt;.01). parents reported increased eye contact and greater social acuity. this feasibility study supports using mobile technologies for potential therapeutic purposes.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1941,16 +1941,16 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>[1, 4, 14]</t>
+          <t>[1, 4]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.275|x2: 0.000|x3: 0.416|x4: 0.079|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.238|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.292|x2: 0.000|x3: 0.000|x4: 0.142|x5: 0.071|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.108|x10: 0.070|x11: 0.071|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.233|x2: 0.158|x3: 0.082|x4: 0.267|x5: 0.277|x6: 0.054|x7: 0.129|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.369|x15: 0.000|x16: 0.093|x17: 0.000
-TOP2VEC -&gt; x1: 0.182|x2: 0.200|x3: 0.059|x4: 0.384|x5: 0.312|x6: 0.134|x7: 0.168|x8: 0.222|x9: 0.118|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.139|x14: 0.364|x15: 0.000|x16: 0.197|x17: 0.000
-MEAN -&gt; x1: 0.230|x2: 0.120|x3: 0.186|x4: 0.243|x5: 0.196|x6: 0.063|x7: 0.099|x8: 0.074|x9: 0.092|x10: 0.032|x11: 0.079|x12: 0.000|x13: 0.046|x14: 0.244|x15: 0.000|x16: 0.097|x17: 0.000
-SOFTMAX -&gt; x1: 0.066|x2: 0.059|x3: 0.063|x4: 0.067|x5: 0.064|x6: 0.056|x7: 0.058|x8: 0.057|x9: 0.058|x10: 0.054|x11: 0.057|x12: 0.053|x13: 0.055|x14: 0.067|x15: 0.053|x16: 0.058|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.090|x3: 0.265|x4: 0.183|x5: 0.115|x6: 0.173|x7: 0.158|x8: 0.000|x9: 0.212|x10: 0.145|x11: 0.053|x12: 0.052|x13: 0.000|x14: 0.000|x15: 0.059|x16: 0.131|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.279|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.131|x2: 0.062|x3: 0.087|x4: 0.218|x5: 0.116|x6: 0.057|x7: 0.072|x8: 0.000|x9: 0.119|x10: 0.054|x11: 0.031|x12: 0.013|x13: 0.000|x14: 0.092|x15: 0.015|x16: 0.056|x17: 0.000
 </t>
         </is>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper explores the phenomena of the emergence of the use of artificial intelligence in teaching and learning in higher education. It investigates educational implications of emerging technologies on the way students learn and how institutions teach and evolve. Recent technological advancements and the increasing speed of adopting new technologies in higher education are explored in order to predict the future nature of higher education in a world where artificial intelligence is part of the fabric of our universities. We pinpoint some challenges for institutions of higher education and student learning in the adoption of these technologies for teaching, learning, student support, and administration and explore further directions for research.</t>
+          <t xml:space="preserve"> this paper explores the phenomena of the emergence of the use of artificial intelligence in teaching and learning in higher education. it investigates educational implications of emerging technologies on the way students learn and how institutions teach and evolve. recent technological advancements and the increasing speed of adopting new technologies in higher education are explored in order to predict the future nature of higher education in a world where artificial intelligence is part of the fabric of our universities. we pinpoint some challenges for institutions of higher education and student learning in the adoption of these technologies for teaching, learning, student support, and administration and explore further directions for research.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1976,11 +1976,11 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.350|x4: 0.498|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.067|x11: 0.202|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.217|x3: 0.000|x4: 0.621|x5: 0.000|x6: 0.000|x7: 0.412|x8: 0.000|x9: 0.209|x10: 0.000|x11: 0.058|x12: 0.123|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.180|x17: 0.000
-TOP2VEC -&gt; x1: 0.193|x2: 0.113|x3: 0.000|x4: 0.712|x5: 0.306|x6: 0.000|x7: 0.229|x8: 0.252|x9: 0.000|x10: 0.000|x11: 0.065|x12: 0.176|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000
-MEAN -&gt; x1: 0.064|x2: 0.110|x3: 0.117|x4: 0.499|x5: 0.102|x6: 0.000|x7: 0.214|x8: 0.084|x9: 0.070|x10: 0.022|x11: 0.109|x12: 0.100|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.078|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.059|x3: 0.060|x4: 0.088|x5: 0.059|x6: 0.053|x7: 0.066|x8: 0.058|x9: 0.057|x10: 0.054|x11: 0.059|x12: 0.059|x13: 0.053|x14: 0.053|x15: 0.053|x16: 0.058|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.067|x10: 0.000|x11: 0.056|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.217|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.412|x8: 0.000|x9: 0.209|x10: 0.000|x11: 0.058|x12: 0.123|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.180|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.472|x5: 0.095|x6: 0.093|x7: 0.457|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.159|x12: 0.294|x13: 0.208|x14: 0.160|x15: 0.000|x16: 0.078|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.054|x3: 0.000|x4: 0.493|x5: 0.024|x6: 0.023|x7: 0.217|x8: 0.000|x9: 0.069|x10: 0.000|x11: 0.068|x12: 0.104|x13: 0.052|x14: 0.040|x15: 0.000|x16: 0.064|x17: 0.000
 </t>
         </is>
       </c>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Social robots can offer tremendous possibilities for autism spectrum disorder (ASD) interventions. To date, most studies with this population have used short, isolated encounters in controlled laboratory settings. Our study focused on a 1-month, home-based intervention for increasing social communication skills of 12 children with ASD between 6 and 12 years old using an autonomous social robot. The children engaged in a triadic interaction with a caregiver and the robot for 30 min every day to complete activities on emotional storytelling, perspective-taking, and sequencing. The robot encouraged engagement, adapted the difficulty of the activities to the child's past performance, and modeled positive social skills. The system maintained engagement over the 1-month deployment, and children showed improvement on joint attention skills with adults when not in the presence of the robot. These results were also consistent with caregiver questionnaires. Caregivers reported less prompting over time and overall increased communication.</t>
+          <t xml:space="preserve"> social robots can offer tremendous possibilities for autism spectrum disorder (asd) interventions. to date, most studies with this population have used short, isolated encounters in controlled laboratory settings. our study focused on a 1 month, home based intervention for increasing social communication skills of 12 children with asd between 6 and 12 years old using an autonomous social robot. the children engaged in a triadic interaction with a caregiver and the robot for 30 min every day to complete activities on emotional storytelling, perspective taking, and sequencing. the robot encouraged engagement, adapted the difficulty of the activities to the childs past performance, and modeled positive social skills. the system maintained engagement over the 1 month deployment, and children showed improvement on joint attention skills with adults when not in the presence of the robot. these results were also consistent with caregiver questionnaires. caregivers reported less prompting over time and overall increased communication.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2001,16 +2001,16 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[3, 4, 5]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.196|x2: 0.000|x3: 0.281|x4: 0.189|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.133|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.152|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.314|x2: 0.000|x3: 0.149|x4: 0.280|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.075|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.159|x17: 0.000
 LDA -&gt; x1: 0.102|x2: 0.124|x3: 0.211|x4: 0.330|x5: 0.240|x6: 0.000|x7: 0.112|x8: 0.154|x9: 0.232|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.076|x14: 0.114|x15: 0.053|x16: 0.073|x17: 0.000
-TOP2VEC -&gt; x1: 0.078|x2: 0.117|x3: 0.115|x4: 0.436|x5: 0.493|x6: 0.217|x7: 0.378|x8: 0.076|x9: 0.134|x10: 0.000|x11: 0.000|x12: 0.166|x13: 0.186|x14: 0.000|x15: 0.000|x16: 0.098|x17: 0.000
-MEAN -&gt; x1: 0.125|x2: 0.080|x3: 0.202|x4: 0.318|x5: 0.244|x6: 0.072|x7: 0.163|x8: 0.077|x9: 0.122|x10: 0.000|x11: 0.044|x12: 0.055|x13: 0.087|x14: 0.038|x15: 0.018|x16: 0.108|x17: 0.000
-SOFTMAX -&gt; x1: 0.060|x2: 0.057|x3: 0.065|x4: 0.073|x5: 0.067|x6: 0.057|x7: 0.062|x8: 0.057|x9: 0.060|x10: 0.053|x11: 0.055|x12: 0.056|x13: 0.058|x14: 0.055|x15: 0.054|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.097|x3: 0.080|x4: 0.239|x5: 0.082|x6: 0.145|x7: 0.214|x8: 0.081|x9: 0.156|x10: 0.116|x11: 0.076|x12: 0.156|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.126|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.104|x2: 0.055|x3: 0.110|x4: 0.337|x5: 0.080|x6: 0.036|x7: 0.082|x8: 0.059|x9: 0.097|x10: 0.048|x11: 0.019|x12: 0.039|x13: 0.019|x14: 0.029|x15: 0.013|x16: 0.090|x17: 0.000
 </t>
         </is>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Four is yet to be achieved. This paper presents an artefact named "Ambient learning-Knowledge as a Service model" for describing how actionable knowledge can be extracted from ambient learning systems to support improvement and consequently facilitate the achievement of Sustainable Development Goal Four. A creative process was adopted to guide the development of the model. The process involved carrying out problem analysis through literature review, designing the model by combining ambient learning and Knowledge as a Service concepts and demonstrating its application by developing a prototype. Evaluation results revealed that C4.5 algorithm that is implemented in Waikato Environment for Knowledge Analysis (WEKA) software is suitable for extracting knowledge from ambient learning systems while Swi-prolog software can be applied to create a tool for knowledge delivery.</t>
+          <t xml:space="preserve"> four is yet to be achieved. this paper presents an artefact named "ambient learning knowledge as a service model" for describing how actionable knowledge can be extracted from ambient learning systems to support improvement and consequently facilitate the achievement of sustainable development goal four. a creative process was adopted to guide the development of the model. the process involved carrying out problem analysis through literature review, designing the model by combining ambient learning and knowledge as a service concepts and demonstrating its application by developing a prototype. evaluation results revealed that c4.5 algorithm that is implemented in waikato environment for knowledge analysis (weka) software is suitable for extracting knowledge from ambient learning systems while swi prolog software can be applied to create a tool for knowledge delivery.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2031,16 +2031,16 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>[3, 4]</t>
+          <t>[4, 12]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.572|x4: 0.108|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.331|x12: 0.055|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.290|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.089|x10: 0.000|x11: 0.085|x12: 0.093|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.194|x3: 0.197|x4: 0.283|x5: 0.000|x6: 0.083|x7: 0.102|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.181|x13: 0.051|x14: 0.291|x15: 0.164|x16: 0.274|x17: 0.000
-TOP2VEC -&gt; x1: 0.177|x2: 0.223|x3: 0.202|x4: 0.473|x5: 0.212|x6: 0.000|x7: 0.377|x8: 0.212|x9: 0.152|x10: 0.096|x11: 0.091|x12: 0.332|x13: 0.172|x14: 0.000|x15: 0.000|x16: 0.196|x17: 0.000
-MEAN -&gt; x1: 0.059|x2: 0.139|x3: 0.300|x4: 0.288|x5: 0.071|x6: 0.028|x7: 0.159|x8: 0.071|x9: 0.051|x10: 0.032|x11: 0.140|x12: 0.190|x13: 0.074|x14: 0.097|x15: 0.055|x16: 0.157|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.071|x4: 0.070|x5: 0.056|x6: 0.054|x7: 0.061|x8: 0.056|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.063|x13: 0.056|x14: 0.058|x15: 0.055|x16: 0.061|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.136|x5: 0.000|x6: 0.141|x7: 0.298|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.256|x12: 0.299|x13: 0.259|x14: 0.120|x15: 0.132|x16: 0.113|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.312|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.049|x3: 0.049|x4: 0.255|x5: 0.000|x6: 0.056|x7: 0.100|x8: 0.000|x9: 0.022|x10: 0.000|x11: 0.085|x12: 0.143|x13: 0.077|x14: 0.103|x15: 0.074|x16: 0.097|x17: 0.000
 </t>
         </is>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Multiple studies have been conducted on Project LISTEN, an intelligent tutoring system (ITS) used to analyze educational learning through case analysis of students' interactions with ITS. Studies have defined the phenomenon by exploring 'what happens when/if' questions and analyzing these in the context of the specified phenomenon occurrence. While ITS often focus on student decisions regarding when and how to use the system's resources, we suggest further analysis and monitoring are needed to get the best results from these systems. In this study, we argue that boys interact differently with ITS than girls. This finding is evident in results from both the Bayesian Knowledge Tracing and Learning Curve Analysis models.</t>
+          <t xml:space="preserve"> multiple studies have been conducted on project listen, an intelligent tutoring system (its) used to analyze educational learning through case analysis of students interactions with its. studies have defined the phenomenon by exploring what happens when/if questions and analyzing these in the context of the specified phenomenon occurrence. while its often focus on student decisions regarding when and how to use the systems resources, we suggest further analysis and monitoring are needed to get the best results from these systems. in this study, we argue that boys interact differently with its than girls. this finding is evident in results from both the bayesian knowledge tracing and learning curve analysis models.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2066,11 +2066,11 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.498|x4: 0.110|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.288|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.430|x3: 0.000|x4: 0.588|x5: 0.180|x6: 0.208|x7: 0.057|x8: 0.000|x9: 0.208|x10: 0.094|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000
-TOP2VEC -&gt; x1: 0.208|x2: 0.162|x3: 0.000|x4: 0.496|x5: 0.353|x6: 0.255|x7: 0.426|x8: 0.211|x9: 0.076|x10: 0.087|x11: 0.000|x12: 0.000|x13: 0.294|x14: 0.259|x15: 0.100|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.069|x2: 0.197|x3: 0.166|x4: 0.369|x5: 0.177|x6: 0.154|x7: 0.161|x8: 0.070|x9: 0.095|x10: 0.060|x11: 0.096|x12: 0.000|x13: 0.098|x14: 0.086|x15: 0.033|x16: 0.078|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.064|x3: 0.062|x4: 0.076|x5: 0.063|x6: 0.061|x7: 0.062|x8: 0.056|x9: 0.058|x10: 0.056|x11: 0.058|x12: 0.052|x13: 0.058|x14: 0.057|x15: 0.054|x16: 0.057|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.354|x5: 0.089|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.068|x10: 0.000|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.430|x3: 0.000|x4: 0.500|x5: 0.180|x6: 0.208|x7: 0.057|x8: 0.000|x9: 0.208|x10: 0.094|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.056|x17: 0.000
+TOP2VEC -&gt; x1: 0.211|x2: 0.000|x3: 0.000|x4: 0.310|x5: 0.000|x6: 0.107|x7: 0.179|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.167|x12: 0.106|x13: 0.085|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.053|x2: 0.108|x3: 0.000|x4: 0.416|x5: 0.067|x6: 0.079|x7: 0.059|x8: 0.000|x9: 0.069|x10: 0.023|x11: 0.058|x12: 0.027|x13: 0.021|x14: 0.000|x15: 0.000|x16: 0.014|x17: 0.000
 </t>
         </is>
       </c>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this paper we review the contribution of our original work titled BSimulating Instructional Roles Through Pedagogical Agents^published in the International Journal of Artificial Intelligence and Education (Baylor and Kim in Computers and Human Behavior, 25(2), 450-457, 2005). Our original work operationalized three instructional roles as simulated through pedagogical agents, and demonstrated the effectiveness of these agent roles on learning and motivation. Since the publication of our work, pedagogical agent research has expanded its scope from the provision of intelligent guidance to a broad interest in agents' social and affective support for learners. We discuss current progress in pedagogical agent roles and capabilities, and speculate about the future of agent role design. We expect that optimizing the roles of artificial beings including on-screen agents and robots will continue to interest the educational technology community as these technologies continue to evolve. Pedagogical agents . Experimental research . Virtual humans . Interface design Overview of Original Paper Motivation In the early 2000s, there was some empirical support that the presence of a pedagogical agent facilitated deeper learning and enhanced motivation (Atkinson 2002; Moreno</t>
+          <t xml:space="preserve"> in this paper we review the contribution of our original work titled bsimulating instructional roles through pedagogical agents^published in the international journal of artificial intelligence and education (baylor and kim in computers and human behavior, 25(2), 450 457, 2005). our original work operationalized three instructional roles as simulated through pedagogical agents, and demonstrated the effectiveness of these agent roles on learning and motivation. since the publication of our work, pedagogical agent research has expanded its scope from the provision of intelligent guidance to a broad interest in agents social and affective support for learners. we discuss current progress in pedagogical agent roles and capabilities, and speculate about the future of agent role design. we expect that optimizing the roles of artificial beings including on screen agents and robots will continue to interest the educational technology community as these technologies continue to evolve. pedagogical agents . experimental research . virtual humans . interface design overview of original paper motivation in the early 2000s, there was some empirical support that the presence of a pedagogical agent facilitated deeper learning and enhanced motivation (atkinson 2002; moreno</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2091,16 +2091,16 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>[4, 5, 13]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.395|x4: 0.114|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.228|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.179|x5: 0.085|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.077|x10: 0.000|x11: 0.064|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.147|x4: 0.142|x5: 0.136|x6: 0.000|x7: 0.080|x8: 0.232|x9: 0.300|x10: 0.222|x11: 0.054|x12: 0.081|x13: 0.212|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.157|x2: 0.082|x3: 0.000|x4: 0.643|x5: 0.518|x6: 0.195|x7: 0.491|x8: 0.131|x9: 0.144|x10: 0.000|x11: 0.000|x12: 0.381|x13: 0.388|x14: 0.151|x15: 0.000|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.052|x2: 0.051|x3: 0.181|x4: 0.252|x5: 0.212|x6: 0.065|x7: 0.190|x8: 0.121|x9: 0.148|x10: 0.074|x11: 0.094|x12: 0.154|x13: 0.200|x14: 0.050|x15: 0.000|x16: 0.082|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.063|x4: 0.067|x5: 0.065|x6: 0.056|x7: 0.063|x8: 0.059|x9: 0.061|x10: 0.056|x11: 0.058|x12: 0.061|x13: 0.064|x14: 0.055|x15: 0.052|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.422|x5: 0.000|x6: 0.153|x7: 0.158|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.098|x12: 0.094|x13: 0.098|x14: 0.000|x15: 0.000|x16: 0.076|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.018|x3: 0.037|x4: 0.311|x5: 0.055|x6: 0.038|x7: 0.060|x8: 0.058|x9: 0.094|x10: 0.056|x11: 0.054|x12: 0.044|x13: 0.078|x14: 0.000|x15: 0.000|x16: 0.055|x17: 0.000
 </t>
         </is>
       </c>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In the computer domain, the objective to be reached in order to give opportunities equality to all persons is defined as Digital Equity. However, different international organizations are working to reach this goal. The analysis of the key points for reaching this objective and how international organizations (International Telecommunications Union, United Nations, International Federation for Information Processing) are working for this goal will be presented in the paper.</t>
+          <t xml:space="preserve"> in the computer domain, the objective to be reached in order to give opportunities equality to all persons is defined as digital equity. however, different international organizations are working to reach this goal. the analysis of the key points for reaching this objective and how international organizations (international telecommunications union, united nations, international federation for information processing) are working for this goal will be presented in the paper.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2121,16 +2121,16 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>[4, 8, 10]</t>
+          <t>[1, 5, 8, 10]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.263|x4: 0.000|x5: 0.083|x6: 0.000|x7: 0.000|x8: 0.163|x9: 0.000|x10: 0.188|x11: 0.152|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.069|x3: 0.000|x4: 0.000|x5: 0.097|x6: 0.000|x7: 0.000|x8: 0.094|x9: 0.085|x10: 0.130|x11: 0.081|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.156|x3: 0.000|x4: 0.199|x5: 0.244|x6: 0.000|x7: 0.000|x8: 0.267|x9: 0.000|x10: 0.433|x11: 0.000|x12: 0.166|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.354|x17: 0.000
-TOP2VEC -&gt; x1: 0.243|x2: 0.214|x3: 0.000|x4: 0.556|x5: 0.181|x6: 0.000|x7: 0.000|x8: 0.240|x9: 0.000|x10: 0.080|x11: 0.184|x12: 0.264|x13: 0.315|x14: 0.084|x15: 0.000|x16: 0.163|x17: 0.000
-MEAN -&gt; x1: 0.081|x2: 0.123|x3: 0.088|x4: 0.233|x5: 0.170|x6: 0.000|x7: 0.000|x8: 0.223|x9: 0.000|x10: 0.234|x11: 0.112|x12: 0.143|x13: 0.105|x14: 0.028|x15: 0.000|x16: 0.172|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.058|x4: 0.067|x5: 0.063|x6: 0.053|x7: 0.053|x8: 0.066|x9: 0.053|x10: 0.067|x11: 0.059|x12: 0.061|x13: 0.059|x14: 0.055|x15: 0.053|x16: 0.063|x17: 0.053
+TOP2VEC -&gt; x1: 0.435|x2: 0.000|x3: 0.000|x4: 0.112|x5: 0.156|x6: 0.000|x7: 0.244|x8: 0.294|x9: 0.198|x10: 0.188|x11: 0.085|x12: 0.083|x13: 0.074|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.285|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.106|x9: 0.107|x10: 0.282|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.180|x2: 0.056|x3: 0.000|x4: 0.078|x5: 0.124|x6: 0.000|x7: 0.061|x8: 0.190|x9: 0.097|x10: 0.258|x11: 0.042|x12: 0.062|x13: 0.018|x14: 0.000|x15: 0.000|x16: 0.089|x17: 0.000
 </t>
         </is>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this mixed-method study, we examined the design and potential impact of a mixed-reality integrated learning environment (MILE) in providing the simulated and immersive teaching practice for university teaching assistants. A virtual-reality-based learning platform integrating a Kinect-enabled sensorimotor interface was developed and used by twenty three university teaching assistants. Qualitative and quantitative data on the participants' participation behaviors, engagement, and perceptions were collected via video/screen recording, interview, surveys on teaching self-efficacy and sense of presence, and eye tracking. Results indicated that the MILE reinforced sense of presence and supported the performance of an ample range of virtual teaching tasks/actions with avatar-embodied live gesturing. The environmental fidelity in the mixed-reality learning spaces, the design and arrangement of virtual agents and avatars, and the affordance of embodied gesturing and walking are salient MILE design features that affected participants' sense of presence and their virtual teaching performance.</t>
+          <t xml:space="preserve"> in this mixed method study, we examined the design and potential impact of a mixed reality integrated learning environment (mile) in providing the simulated and immersive teaching practice for university teaching assistants. a virtual reality based learning platform integrating a kinect enabled sensorimotor interface was developed and used by twenty three university teaching assistants. qualitative and quantitative data on the participants participation behaviors, engagement, and perceptions were collected via video/screen recording, interview, surveys on teaching self efficacy and sense of presence, and eye tracking. results indicated that the mile reinforced sense of presence and supported the performance of an ample range of virtual teaching tasks/actions with avatar embodied live gesturing. the environmental fidelity in the mixed reality learning spaces, the design and arrangement of virtual agents and avatars, and the affordance of embodied gesturing and walking are salient mile design features that affected participants sense of presence and their virtual teaching performance.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2151,16 +2151,16 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[4, 11]</t>
+          <t>[4, 11, 14]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.333|x4: 0.118|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.217|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.324|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.179|x3: 0.099|x4: 0.350|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.180|x9: 0.203|x10: 0.135|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.350|x15: 0.083|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.155|x2: 0.235|x3: 0.061|x4: 0.456|x5: 0.456|x6: 0.155|x7: 0.238|x8: 0.146|x9: 0.000|x10: 0.076|x11: 0.364|x12: 0.209|x13: 0.229|x14: 0.244|x15: 0.000|x16: 0.156|x17: 0.000
-MEAN -&gt; x1: 0.052|x2: 0.138|x3: 0.164|x4: 0.308|x5: 0.152|x6: 0.052|x7: 0.079|x8: 0.109|x9: 0.068|x10: 0.070|x11: 0.274|x12: 0.070|x13: 0.076|x14: 0.198|x15: 0.028|x16: 0.052|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.062|x4: 0.071|x5: 0.061|x6: 0.055|x7: 0.057|x8: 0.058|x9: 0.056|x10: 0.056|x11: 0.069|x12: 0.056|x13: 0.057|x14: 0.064|x15: 0.054|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.242|x5: 0.165|x6: 0.064|x7: 0.091|x8: 0.000|x9: 0.000|x10: 0.116|x11: 0.138|x12: 0.164|x13: 0.123|x14: 0.152|x15: 0.110|x16: 0.106|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.045|x3: 0.025|x4: 0.354|x5: 0.041|x6: 0.016|x7: 0.023|x8: 0.045|x9: 0.051|x10: 0.063|x11: 0.125|x12: 0.041|x13: 0.031|x14: 0.126|x15: 0.048|x16: 0.027|x17: 0.000
 </t>
         </is>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> How can we help an investigator to efficiently connect the dots and uncover the network of individuals involved in a criminal activity based on the evidence of their connections, such as visiting the same address, or transacting with the same bank account? We formulate this problem as Active Search of Connections, which finds target entities that share evidence of different types with a given lead, where their relevance to the case is queried interactively from the investigator. We present RedThread, an efficient solution for inferring related and relevant nodes while incorporating the user's feedback to guide the inference. Our experiments focus on case building for combating human trafficking, where the investigator follows leads to expose organized activities, i.e. different escort advertisements that are connected and possibly orchestrated. RedThread is a local algorithm and enables online case building when mining millions of ads posted in one of the largest classified advertising websites. The results of RedThread are interpretable, as they explain how the results are connected to the initial lead. We experimentally show that RedThread learns the importance of the different types and different pieces of evidence, while the former could be transferred between cases.</t>
+          <t xml:space="preserve"> how can we help an investigator to efficiently connect the dots and uncover the network of individuals involved in a criminal activity based on the evidence of their connections, such as visiting the same address, or transacting with the same bank account? we formulate this problem as active search of connections, which finds target entities that share evidence of different types with a given lead, where their relevance to the case is queried interactively from the investigator. we present redthread, an efficient solution for inferring related and relevant nodes while incorporating the users feedback to guide the inference. our experiments focus on case building for combating human trafficking, where the investigator follows leads to expose organized activities, i.e. different escort advertisements that are connected and possibly orchestrated. redthread is a local algorithm and enables online case building when mining millions of ads posted in one of the largest classified advertising websites. the results of redthread are interpretable, as they explain how the results are connected to the initial lead. we experimentally show that redthread learns the importance of the different types and different pieces of evidence, while the former could be transferred between cases.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2181,16 +2181,16 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>[3, 4, 9]</t>
+          <t>[9, 16]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.440|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.256|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.092|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.090|x7: 0.000|x8: 0.000|x9: 0.109|x10: 0.000|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.139|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.101|x3: 0.097|x4: 0.237|x5: 0.075|x6: 0.000|x7: 0.104|x8: 0.150|x9: 0.389|x10: 0.000|x11: 0.000|x12: 0.203|x13: 0.155|x14: 0.000|x15: 0.000|x16: 0.308|x17: 0.000
-TOP2VEC -&gt; x1: 0.101|x2: 0.254|x3: 0.133|x4: 0.409|x5: 0.294|x6: 0.169|x7: 0.234|x8: 0.128|x9: 0.331|x10: 0.079|x11: 0.193|x12: 0.364|x13: 0.227|x14: 0.172|x15: 0.116|x16: 0.161|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.118|x3: 0.224|x4: 0.215|x5: 0.123|x6: 0.056|x7: 0.113|x8: 0.093|x9: 0.240|x10: 0.026|x11: 0.149|x12: 0.189|x13: 0.127|x14: 0.057|x15: 0.039|x16: 0.187|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.059|x3: 0.065|x4: 0.065|x5: 0.059|x6: 0.055|x7: 0.058|x8: 0.057|x9: 0.066|x10: 0.054|x11: 0.061|x12: 0.063|x13: 0.059|x14: 0.055|x15: 0.054|x16: 0.063|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.232|x3: 0.000|x4: 0.221|x5: 0.000|x6: 0.084|x7: 0.087|x8: 0.062|x9: 0.000|x10: 0.117|x11: 0.132|x12: 0.119|x13: 0.098|x14: 0.000|x15: 0.139|x16: 0.150|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.084|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.083|x3: 0.024|x4: 0.115|x5: 0.040|x6: 0.044|x7: 0.048|x8: 0.053|x9: 0.125|x10: 0.029|x11: 0.063|x12: 0.081|x13: 0.063|x14: 0.000|x15: 0.035|x16: 0.274|x17: 0.000
 </t>
         </is>
       </c>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Computers are increasingly used to make decisions that have significant impact on people's lives. Often, these predictions can affect different population subgroups disproportionately. As a result, the issue of fairness has received much recent interest, and a number of fairness-enhanced classifiers have appeared in the literature. This paper seeks to study the following questions: how do these different techniques fundamentally compare to one another, and what accounts for the differences? Specifically, we seek to bring attention to many under-appreciated aspects of such fairness-enhancing interventions that require investigation for these algorithms to receive broad adoption. We present the results of an open benchmark we have developed that lets us compare a number of different algorithms under a variety of fairness measures and existing datasets. We find that although different algorithms tend to prefer specific formulations of fairness preservations, many of these measures strongly correlate with one another. In addition, we find that fairness-preserving algorithms tend to be sensitive to fluctuations in dataset composition (simulated in our benchmark by varying training-test splits) and to different forms of preprocessing, indicating that fairness interventions might be more brittle than previously thought. • Computing methodologies → Machine learning; • Software and its engineering → Software libraries and repositories;</t>
+          <t xml:space="preserve"> computers are increasingly used to make decisions that have significant impact on peoples lives. often, these predictions can affect different population subgroups disproportionately. as a result, the issue of fairness has received much recent interest, and a number of fairness enhanced classifiers have appeared in the literature. this paper seeks to study the following questions: how do these different techniques fundamentally compare to one another, and what accounts for the differences? specifically, we seek to bring attention to many under appreciated aspects of such fairness enhancing interventions that require investigation for these algorithms to receive broad adoption. we present the results of an open benchmark we have developed that lets us compare a number of different algorithms under a variety of fairness measures and existing datasets. we find that although different algorithms tend to prefer specific formulations of fairness preservations, many of these measures strongly correlate with one another. in addition, we find that fairness preserving algorithms tend to be sensitive to fluctuations in dataset composition (simulated in our benchmark by varying training test splits) and to different forms of preprocessing, indicating that fairness interventions might be more brittle than previously thought. • computing methodologies → machine learning; • software and its engineering → software libraries and repositories;</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2211,16 +2211,16 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.486|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.285|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.079|x2: 0.000|x3: 0.079|x4: 0.100|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.125|x10: 0.000|x11: 0.148|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.177|x4: 0.216|x5: 0.218|x6: 0.000|x7: 0.000|x8: 0.140|x9: 0.124|x10: 0.000|x11: 0.000|x12: 0.078|x13: 0.218|x14: 0.276|x15: 0.128|x16: 0.175|x17: 0.000
-TOP2VEC -&gt; x1: 0.148|x2: 0.069|x3: 0.092|x4: 0.163|x5: 0.172|x6: 0.000|x7: 0.000|x8: 0.151|x9: 0.097|x10: 0.000|x11: 0.063|x12: 0.321|x13: 0.234|x14: 0.320|x15: 0.322|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.049|x2: 0.046|x3: 0.251|x4: 0.126|x5: 0.130|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.074|x10: 0.000|x11: 0.116|x12: 0.133|x13: 0.151|x14: 0.198|x15: 0.150|x16: 0.058|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.056|x3: 0.069|x4: 0.061|x5: 0.061|x6: 0.053|x7: 0.053|x8: 0.059|x9: 0.058|x10: 0.053|x11: 0.060|x12: 0.061|x13: 0.062|x14: 0.065|x15: 0.062|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.065|x2: 0.063|x3: 0.000|x4: 0.234|x5: 0.000|x6: 0.054|x7: 0.218|x8: 0.068|x9: 0.200|x10: 0.060|x11: 0.254|x12: 0.088|x13: 0.254|x14: 0.139|x15: 0.081|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.033|x3: 0.189|x4: 0.138|x5: 0.055|x6: 0.014|x7: 0.055|x8: 0.052|x9: 0.112|x10: 0.015|x11: 0.100|x12: 0.041|x13: 0.118|x14: 0.104|x15: 0.052|x16: 0.044|x17: 0.000
 </t>
         </is>
       </c>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Human trafficking is among the most challenging law enforcement problems which demands persistent fight against from all over the globe. In this study, we leverage readily available data from the website "Backpage"-used for classified advertisement-to discern potential patterns of human trafficking activities which manifest online and identify most likely trafficking related advertisements. Due to the lack of ground truth, we rely on two human analysts -one human trafficking victim survivor and one from law enforcement, for hand-labeling the small portion of the crawled data. We then present a semisupervised learning approach that is trained on the available labeled and unlabeled data and evaluated on unseen data with further verification of experts.</t>
+          <t xml:space="preserve"> human trafficking is among the most challenging law enforcement problems which demands persistent fight against from all over the globe. in this study, we leverage readily available data from the website "backpage" used for classified advertisement to discern potential patterns of human trafficking activities which manifest online and identify most likely trafficking related advertisements. due to the lack of ground truth, we rely on two human analysts one human trafficking victim survivor and one from law enforcement, for hand labeling the small portion of the crawled data. we then present a semisupervised learning approach that is trained on the available labeled and unlabeled data and evaluated on unseen data with further verification of experts.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2241,16 +2241,16 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[4, 5, 14, 16]</t>
+          <t>[2, 4, 5, 14, 16]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.275|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.159|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.515|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.082|x15: 0.070|x16: 0.500|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.241|x3: 0.000|x4: 0.296|x5: 0.291|x6: 0.110|x7: 0.053|x8: 0.000|x9: 0.191|x10: 0.000|x11: 0.061|x12: 0.097|x13: 0.000|x14: 0.230|x15: 0.000|x16: 0.250|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.309|x3: 0.120|x4: 0.433|x5: 0.585|x6: 0.486|x7: 0.195|x8: 0.000|x9: 0.000|x10: 0.140|x11: 0.231|x12: 0.151|x13: 0.000|x14: 0.441|x15: 0.143|x16: 0.287|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.183|x3: 0.132|x4: 0.243|x5: 0.264|x6: 0.199|x7: 0.082|x8: 0.000|x9: 0.064|x10: 0.047|x11: 0.150|x12: 0.082|x13: 0.000|x14: 0.224|x15: 0.048|x16: 0.346|x17: 0.000
-SOFTMAX -&gt; x1: 0.052|x2: 0.062|x3: 0.059|x4: 0.066|x5: 0.067|x6: 0.063|x7: 0.056|x8: 0.052|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.056|x13: 0.052|x14: 0.065|x15: 0.054|x16: 0.073|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.279|x3: 0.112|x4: 0.188|x5: 0.248|x6: 0.319|x7: 0.064|x8: 0.000|x9: 0.000|x10: 0.162|x11: 0.081|x12: 0.110|x13: 0.233|x14: 0.309|x15: 0.351|x16: 0.409|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.130|x3: 0.028|x4: 0.121|x5: 0.135|x6: 0.107|x7: 0.029|x8: 0.000|x9: 0.048|x10: 0.040|x11: 0.035|x12: 0.052|x13: 0.058|x14: 0.155|x15: 0.105|x16: 0.415|x17: 0.000
 </t>
         </is>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We appreciate the help of Michael Gallagher, a retired police officer, who currently works with a domestic violence agency in the jurisdiction studied. He provided important information on the meaning of some of our variables and on related law enforcement procedures. We also received important assistance on the prosecutorial context of domestic violence from Marian G. Braccia, Deputy District Attorney in the District Attorney's Office of the jurisdiction. Thanks also go to the anonymous reviewers of this article.</t>
+          <t xml:space="preserve"> we appreciate the help of michael gallagher, a retired police officer, who currently works with a domestic violence agency in the jurisdiction studied. he provided important information on the meaning of some of our variables and on related law enforcement procedures. we also received important assistance on the prosecutorial context of domestic violence from marian g. braccia, deputy district attorney in the district attorneys office of the jurisdiction. thanks also go to the anonymous reviewers of this article.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2271,16 +2271,16 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>[5, 14, 15, 16]</t>
+          <t>[5, 12, 14, 15, 16]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.121|x4: 0.000|x5: 0.182|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.070|x12: 0.081|x13: 0.000|x14: 0.068|x15: 0.000|x16: 0.143|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.193|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.082|x13: 0.000|x14: 0.074|x15: 0.000|x16: 0.219|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.163|x3: 0.000|x4: 0.000|x5: 0.184|x6: 0.000|x7: 0.082|x8: 0.000|x9: 0.000|x10: 0.134|x11: 0.000|x12: 0.207|x13: 0.000|x14: 0.274|x15: 0.370|x16: 0.406|x17: 0.000
-TOP2VEC -&gt; x1: 0.141|x2: 0.233|x3: 0.000|x4: 0.183|x5: 0.395|x6: 0.000|x7: 0.000|x8: 0.171|x9: 0.000|x10: 0.190|x11: 0.000|x12: 0.000|x13: 0.054|x14: 0.386|x15: 0.335|x16: 0.388|x17: 0.000
-MEAN -&gt; x1: 0.047|x2: 0.132|x3: 0.040|x4: 0.061|x5: 0.254|x6: 0.000|x7: 0.027|x8: 0.057|x9: 0.000|x10: 0.108|x11: 0.023|x12: 0.096|x13: 0.018|x14: 0.243|x15: 0.235|x16: 0.313|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.061|x3: 0.055|x4: 0.056|x5: 0.068|x6: 0.053|x7: 0.055|x8: 0.056|x9: 0.053|x10: 0.059|x11: 0.054|x12: 0.058|x13: 0.054|x14: 0.068|x15: 0.067|x16: 0.073|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.137|x5: 0.065|x6: 0.080|x7: 0.215|x8: 0.194|x9: 0.072|x10: 0.000|x11: 0.000|x12: 0.226|x13: 0.139|x14: 0.234|x15: 0.298|x16: 0.072|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.108|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.041|x3: 0.000|x4: 0.034|x5: 0.137|x6: 0.020|x7: 0.074|x8: 0.048|x9: 0.018|x10: 0.034|x11: 0.000|x12: 0.129|x13: 0.035|x14: 0.145|x15: 0.167|x16: 0.299|x17: 0.000
 </t>
         </is>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this work we investigate gender-based inequalities in the context of resume search engines, which are tools that allow recruiters to proactively search for candidates based on keywords and filters. If these ranking algorithms take demographic features into account (directly or indirectly), they may produce rankings that disadvantage some candidates. We collect search results from Indeed, Monster, and CareerBuilder based on 35 job titles in 20 U. S. cities, resulting in data on 855K job candidates. Using statistical tests, we examine whether these search engines produce rankings that exhibit two types of indirect discrimination: individual and group unfairness. Furthermore, we use controlled experiments to show that these websites do not use inferred gender of candidates as explicit features in their ranking algorithms.</t>
+          <t xml:space="preserve"> in this work we investigate gender based inequalities in the context of resume search engines, which are tools that allow recruiters to proactively search for candidates based on keywords and filters. if these ranking algorithms take demographic features into account (directly or indirectly), they may produce rankings that disadvantage some candidates. we collect search results from indeed, monster, and careerbuilder based on 35 job titles in 20 u. s. cities, resulting in data on 855k job candidates. using statistical tests, we examine whether these search engines produce rankings that exhibit two types of indirect discrimination: individual and group unfairness. furthermore, we use controlled experiments to show that these websites do not use inferred gender of candidates as explicit features in their ranking algorithms.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2301,16 +2301,16 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>[5, 11]</t>
+          <t>[5, 8, 11, 14]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.272|x4: 0.000|x5: 0.110|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.269|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.301|x6: 0.000|x7: 0.000|x8: 0.138|x9: 0.000|x10: 0.000|x11: 0.198|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.093|x3: 0.058|x4: 0.114|x5: 0.302|x6: 0.000|x7: 0.000|x8: 0.436|x9: 0.111|x10: 0.107|x11: 0.100|x12: 0.000|x13: 0.000|x14: 0.347|x15: 0.058|x16: 0.093|x17: 0.000
-TOP2VEC -&gt; x1: 0.089|x2: 0.000|x3: 0.000|x4: 0.122|x5: 0.295|x6: 0.239|x7: 0.280|x8: 0.103|x9: 0.301|x10: 0.000|x11: 0.513|x12: 0.233|x13: 0.243|x14: 0.207|x15: 0.120|x16: 0.057|x17: 0.000
-MEAN -&gt; x1: 0.030|x2: 0.031|x3: 0.110|x4: 0.079|x5: 0.236|x6: 0.080|x7: 0.093|x8: 0.180|x9: 0.137|x10: 0.036|x11: 0.290|x12: 0.078|x13: 0.081|x14: 0.185|x15: 0.059|x16: 0.050|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.055|x3: 0.059|x4: 0.057|x5: 0.067|x6: 0.057|x7: 0.058|x8: 0.063|x9: 0.061|x10: 0.055|x11: 0.071|x12: 0.057|x13: 0.057|x14: 0.064|x15: 0.056|x16: 0.056|x17: 0.053
+TOP2VEC -&gt; x1: 0.087|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.252|x6: 0.063|x7: 0.140|x8: 0.129|x9: 0.178|x10: 0.058|x11: 0.482|x12: 0.193|x13: 0.000|x14: 0.167|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.022|x2: 0.023|x3: 0.014|x4: 0.029|x5: 0.339|x6: 0.016|x7: 0.035|x8: 0.176|x9: 0.072|x10: 0.041|x11: 0.195|x12: 0.048|x13: 0.000|x14: 0.129|x15: 0.014|x16: 0.023|x17: 0.000
 </t>
         </is>
       </c>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The blind application of machine learning runs the risk of amplifying biases present in data. Such a danger is facing us with word embedding, a popular framework to represent text data as vectors which has been used in many machine learning and natural language processing tasks. We show that even word embeddings trained on Google News articles exhibit female/male gender stereotypes to a disturbing extent. This raises concerns because their widespread use, as we describe, often tends to amplify these biases. Geometrically, gender bias is first shown to be captured by a direction in the word embedding. Second, gender neutral words are shown to be linearly separable from gender definition words in the word embedding. Using these properties, we provide a methodology for modifying an embedding to remove gender stereotypes, such as the association between the words receptionist and female, while maintaining desired associations such as between the words queen and female. Using crowd-worker evaluation as well as standard benchmarks, we empirically demonstrate that our algorithms significantly reduce gender bias in embeddings while preserving the its useful properties such as the ability to cluster related concepts and to solve analogy tasks. The resulting embeddings can be used in applications without amplifying gender bias.</t>
+          <t xml:space="preserve"> the blind application of machine learning runs the risk of amplifying biases present in data. such a danger is facing us with word embedding, a popular framework to represent text data as vectors which has been used in many machine learning and natural language processing tasks. we show that even word embeddings trained on google news articles exhibit female/male gender stereotypes to a disturbing extent. this raises concerns because their widespread use, as we describe, often tends to amplify these biases. geometrically, gender bias is first shown to be captured by a direction in the word embedding. second, gender neutral words are shown to be linearly separable from gender definition words in the word embedding. using these properties, we provide a methodology for modifying an embedding to remove gender stereotypes, such as the association between the words receptionist and female, while maintaining desired associations such as between the words queen and female. using crowd worker evaluation as well as standard benchmarks, we empirically demonstrate that our algorithms significantly reduce gender bias in embeddings while preserving the its useful properties such as the ability to cluster related concepts and to solve analogy tasks. the resulting embeddings can be used in applications without amplifying gender bias.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2331,16 +2331,16 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[5, 8]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.247|x4: 0.000|x5: 0.226|x6: 0.000|x7: 0.000|x8: 0.059|x9: 0.000|x10: 0.000|x11: 0.143|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.106|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.093|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.126|x3: 0.147|x4: 0.145|x5: 0.227|x6: 0.054|x7: 0.000|x8: 0.334|x9: 0.065|x10: 0.131|x11: 0.000|x12: 0.083|x13: 0.226|x14: 0.000|x15: 0.086|x16: 0.196|x17: 0.000
-TOP2VEC -&gt; x1: 0.193|x2: 0.000|x3: 0.000|x4: 0.401|x5: 0.298|x6: 0.000|x7: 0.373|x8: 0.222|x9: 0.158|x10: 0.056|x11: 0.000|x12: 0.117|x13: 0.220|x14: 0.144|x15: 0.270|x16: 0.115|x17: 0.000
-MEAN -&gt; x1: 0.064|x2: 0.042|x3: 0.132|x4: 0.182|x5: 0.250|x6: 0.018|x7: 0.124|x8: 0.205|x9: 0.075|x10: 0.062|x11: 0.048|x12: 0.067|x13: 0.149|x14: 0.048|x15: 0.119|x16: 0.104|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.061|x4: 0.064|x5: 0.068|x6: 0.054|x7: 0.060|x8: 0.065|x9: 0.057|x10: 0.057|x11: 0.056|x12: 0.057|x13: 0.062|x14: 0.056|x15: 0.060|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.098|x2: 0.000|x3: 0.119|x4: 0.336|x5: 0.257|x6: 0.000|x7: 0.231|x8: 0.063|x9: 0.147|x10: 0.122|x11: 0.076|x12: 0.118|x13: 0.202|x14: 0.130|x15: 0.075|x16: 0.072|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.025|x2: 0.031|x3: 0.067|x4: 0.147|x5: 0.371|x6: 0.014|x7: 0.058|x8: 0.122|x9: 0.053|x10: 0.063|x11: 0.019|x12: 0.050|x13: 0.107|x14: 0.032|x15: 0.040|x16: 0.067|x17: 0.000
 </t>
         </is>
       </c>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Technology-facilitated sexual violence (TFSV) refers to a range of behaviors where digital technologies are used to facilitate both virtual and face-to-face sexually based harms. Such behaviors include online sexual harassment, gender-and sexuality-based harassment, cyberstalking, image-based sexual exploitation, and the use of a carriage service to coerce a victim into an unwanted sexual act. This article reviews the current state of knowledge on these different dimensions, drawing on existing empirical studies. While there is a growing body of research into technology-facilitated harms perpetrated against children and adolescents, there is a dearth of qualitative and quantitative research on TFSV against adults. Moreover, few of the existing studies provide reliable data on the nature, scope, and impacts of TFSV. Preliminary studies, however, indicate that some harms, much like sexual violence more broadly, may be predominantly gender-, sexuality-, and age-based, with young women being overrepresented as victims in some categories. This review collects the empirical evidence to date regarding the prevalence and gender-based nature of TFSV against adults and discusses the implications for policy and programs, as well as suggestions for future research.</t>
+          <t xml:space="preserve"> technology facilitated sexual violence (tfsv) refers to a range of behaviors where digital technologies are used to facilitate both virtual and face to face sexually based harms. such behaviors include online sexual harassment, gender and sexuality based harassment, cyberstalking, image based sexual exploitation, and the use of a carriage service to coerce a victim into an unwanted sexual act. this article reviews the current state of knowledge on these different dimensions, drawing on existing empirical studies. while there is a growing body of research into technology facilitated harms perpetrated against children and adolescents, there is a dearth of qualitative and quantitative research on tfsv against adults. moreover, few of the existing studies provide reliable data on the nature, scope, and impacts of tfsv. preliminary studies, however, indicate that some harms, much like sexual violence more broadly, may be predominantly gender , sexuality , and age based, with young women being overrepresented as victims in some categories. this review collects the empirical evidence to date regarding the prevalence and gender based nature of tfsv against adults and discusses the implications for policy and programs, as well as suggestions for future research.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2366,11 +2366,11 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.388|x4: 0.000|x5: 0.365|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.224|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.339|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.469|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.085|x10: 0.000|x11: 0.070|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.366|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.113|x3: 0.000|x4: 0.332|x5: 0.381|x6: 0.000|x7: 0.148|x8: 0.113|x9: 0.216|x10: 0.000|x11: 0.068|x12: 0.000|x13: 0.000|x14: 0.176|x15: 0.099|x16: 0.175|x17: 0.000
-TOP2VEC -&gt; x1: 0.101|x2: 0.000|x3: 0.078|x4: 0.167|x5: 0.517|x6: 0.236|x7: 0.000|x8: 0.125|x9: 0.000|x10: 0.088|x11: 0.132|x12: 0.178|x13: 0.055|x14: 0.232|x15: 0.000|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.038|x3: 0.155|x4: 0.166|x5: 0.415|x6: 0.079|x7: 0.049|x8: 0.079|x9: 0.072|x10: 0.029|x11: 0.141|x12: 0.059|x13: 0.018|x14: 0.136|x15: 0.033|x16: 0.231|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.062|x5: 0.080|x6: 0.057|x7: 0.056|x8: 0.057|x9: 0.057|x10: 0.054|x11: 0.061|x12: 0.056|x13: 0.054|x14: 0.061|x15: 0.055|x16: 0.067|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.104|x3: 0.000|x4: 0.139|x5: 0.185|x6: 0.289|x7: 0.245|x8: 0.000|x9: 0.000|x10: 0.085|x11: 0.085|x12: 0.082|x13: 0.000|x14: 0.061|x15: 0.000|x16: 0.146|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.296|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.155|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.054|x3: 0.000|x4: 0.118|x5: 0.333|x6: 0.072|x7: 0.098|x8: 0.028|x9: 0.075|x10: 0.021|x11: 0.056|x12: 0.021|x13: 0.000|x14: 0.059|x15: 0.025|x16: 0.211|x17: 0.000
 </t>
         </is>
       </c>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This study analyzes 3 digital games for development in Africa, examining them as individual texts that operate as part of a broader international development discourse, and as political economic products with implications for international development and gaming industries. A conceptual framework is proposed as part of this process. By looking at individual games alongside the organizations and funding structures behind them, I argue that digital games, as a new technological platform, do not in-and-of themselves present a revolutionary approach to development across Africa; rather, they both reinforce and subvert dominant approaches already at play.</t>
+          <t xml:space="preserve"> this study analyzes 3 digital games for development in africa, examining them as individual texts that operate as part of a broader international development discourse, and as political economic products with implications for international development and gaming industries. a conceptual framework is proposed as part of this process. by looking at individual games alongside the organizations and funding structures behind them, i argue that digital games, as a new technological platform, do not in and of themselves present a revolutionary approach to development across africa; rather, they both reinforce and subvert dominant approaches already at play.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2391,16 +2391,16 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>[3, 9]</t>
+          <t>[7, 9]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.278|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.087|x10: 0.180|x11: 0.157|x12: 0.073|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.179|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.184|x10: 0.084|x11: 0.119|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.248|x3: 0.236|x4: 0.065|x5: 0.064|x6: 0.000|x7: 0.147|x8: 0.000|x9: 0.152|x10: 0.288|x11: 0.000|x12: 0.193|x13: 0.000|x14: 0.125|x15: 0.000|x16: 0.302|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.088|x3: 0.332|x4: 0.432|x5: 0.177|x6: 0.107|x7: 0.359|x8: 0.174|x9: 0.460|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.153|x14: 0.288|x15: 0.173|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.112|x3: 0.282|x4: 0.166|x5: 0.081|x6: 0.036|x7: 0.168|x8: 0.058|x9: 0.233|x10: 0.156|x11: 0.052|x12: 0.089|x13: 0.051|x14: 0.138|x15: 0.058|x16: 0.101|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.070|x4: 0.062|x5: 0.057|x6: 0.055|x7: 0.062|x8: 0.056|x9: 0.067|x10: 0.062|x11: 0.056|x12: 0.058|x13: 0.055|x14: 0.061|x15: 0.056|x16: 0.058|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.229|x5: 0.189|x6: 0.000|x7: 0.371|x8: 0.000|x9: 0.162|x10: 0.000|x11: 0.291|x12: 0.145|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.101|x9: 0.478|x10: 0.090|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.062|x3: 0.104|x4: 0.073|x5: 0.063|x6: 0.000|x7: 0.129|x8: 0.025|x9: 0.244|x10: 0.115|x11: 0.102|x12: 0.084|x13: 0.000|x14: 0.031|x15: 0.000|x16: 0.076|x17: 0.000
 </t>
         </is>
       </c>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Improved understanding of geographical variation and inequity in health status, wealth and access to resources within countries is increasingly being recognized as central to meeting development goals. Development and health indicators assessed at national or subnational scale can often conceal important inequities, with the rural poor often least well represented. The ability to target limited resources is fundamental, especially in an international context where funding for health and development comes under pressure. This has recently prompted the exploration of the potential of spatial interpolation methods based on geolocated clusters from national household survey data for the high-resolution mapping of features such as population age structures, vaccination coverage and access to sanitation. It remains unclear, however, how predictable these different factors are across different settings, variables and between demographic groups. Here we test the accuracy of spatial interpolation methods in producing gender-disaggregated high-resolution maps of the rates of literacy, stunting and the use of modern contraceptive methods from a combination of geolocated demographic and health surveys cluster data and geospatial covariates. Bayesian geostatistical and machine learning modelling methods were tested across four low-income countries and varying gridded environmental and socio-economic covariate datasets to build 1Â1 km spatial resolution maps with uncertainty estimates. Results show the potential of the approach in producing high-resolution maps of key gender-disaggregated socio-economic indicators, with explained variance through cross-validation being as high as 74-75% for female literacy in Nigeria and Kenya, and in the 50-70% range for many other variables. However, substantial variations by both country and variable were seen, with many variables showing poor mapping accuracies in the range of 2-30% explained variance using both geostatistical and machine learning approaches. The analyses offer a robust basis for the construction of timely maps with levels of detail that support geographically stratified decision-making and the monitoring of progress towards development goals. However, the great variability in results between countries and variables highlights the challenges in applying these interpolation methods universally across multiple countries, and the importance of validation and quantifying uncertainty if this is undertaken.</t>
+          <t xml:space="preserve"> improved understanding of geographical variation and inequity in health status, wealth and access to resources within countries is increasingly being recognized as central to meeting development goals. development and health indicators assessed at national or subnational scale can often conceal important inequities, with the rural poor often least well represented. the ability to target limited resources is fundamental, especially in an international context where funding for health and development comes under pressure. this has recently prompted the exploration of the potential of spatial interpolation methods based on geolocated clusters from national household survey data for the high resolution mapping of features such as population age structures, vaccination coverage and access to sanitation. it remains unclear, however, how predictable these different factors are across different settings, variables and between demographic groups. here we test the accuracy of spatial interpolation methods in producing gender disaggregated high resolution maps of the rates of literacy, stunting and the use of modern contraceptive methods from a combination of geolocated demographic and health surveys cluster data and geospatial covariates. bayesian geostatistical and machine learning modelling methods were tested across four low income countries and varying gridded environmental and socio economic covariate datasets to build 1â1 km spatial resolution maps with uncertainty estimates. results show the potential of the approach in producing high resolution maps of key gender disaggregated socio economic indicators, with explained variance through cross validation being as high as 74 75% for female literacy in nigeria and kenya, and in the 50 70% range for many other variables. however, substantial variations by both country and variable were seen, with many variables showing poor mapping accuracies in the range of 2 30% explained variance using both geostatistical and machine learning approaches. the analyses offer a robust basis for the construction of timely maps with levels of detail that support geographically stratified decision making and the monitoring of progress towards development goals. however, the great variability in results between countries and variables highlights the challenges in applying these interpolation methods universally across multiple countries, and the importance of validation and quantifying uncertainty if this is undertaken.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2421,16 +2421,16 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[3, 4, 16]</t>
+          <t>[4, 16]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.750|x4: 0.055|x5: 0.067|x6: 0.092|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.200|x11: 0.330|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.085|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.082|x2: 0.060|x3: 0.245|x4: 0.103|x5: 0.133|x6: 0.087|x7: 0.000|x8: 0.000|x9: 0.090|x10: 0.103|x11: 0.086|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.113|x17: 0.000
 LDA -&gt; x1: 0.164|x2: 0.199|x3: 0.113|x4: 0.355|x5: 0.145|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.074|x10: 0.000|x11: 0.144|x12: 0.165|x13: 0.000|x14: 0.153|x15: 0.000|x16: 0.308|x17: 0.000
-TOP2VEC -&gt; x1: 0.137|x2: 0.296|x3: 0.164|x4: 0.218|x5: 0.178|x6: 0.121|x7: 0.188|x8: 0.200|x9: 0.206|x10: 0.120|x11: 0.056|x12: 0.151|x13: 0.000|x14: 0.184|x15: 0.072|x16: 0.246|x17: 0.000
-MEAN -&gt; x1: 0.100|x2: 0.165|x3: 0.259|x4: 0.210|x5: 0.130|x6: 0.071|x7: 0.063|x8: 0.067|x9: 0.093|x10: 0.107|x11: 0.177|x12: 0.105|x13: 0.000|x14: 0.112|x15: 0.024|x16: 0.213|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.062|x3: 0.068|x4: 0.065|x5: 0.060|x6: 0.056|x7: 0.056|x8: 0.056|x9: 0.058|x10: 0.058|x11: 0.063|x12: 0.058|x13: 0.052|x14: 0.059|x15: 0.054|x16: 0.065|x17: 0.052
+TOP2VEC -&gt; x1: 0.089|x2: 0.057|x3: 0.065|x4: 0.181|x5: 0.167|x6: 0.061|x7: 0.143|x8: 0.139|x9: 0.055|x10: 0.000|x11: 0.169|x12: 0.076|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.133|x17: 0.000
+BERTOPIC -&gt; x1: 0.107|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.073|x9: 0.000|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.111|x2: 0.079|x3: 0.106|x4: 0.160|x5: 0.111|x6: 0.037|x7: 0.036|x8: 0.053|x9: 0.055|x10: 0.050|x11: 0.100|x12: 0.060|x13: 0.000|x14: 0.038|x15: 0.000|x16: 0.139|x17: 0.000
 </t>
         </is>
       </c>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Compactness and landscape connectivity are essential properties for effective functioning of conservation reserves. In this article we introduce a linear integer programming model to determine optimal configuration of a conservation reserve with such properties. Connectivity can be defined either as structural (physical) connectivity or functional connectivity; the model developed here addresses both properties. We apply the model to identify the optimal conservation management areas for protection of Gopher Tortoise (GT) in a military installation, Ft. Benning, Georgia, which serves as a safe refuge for this 'at risk' species. The recent expansion in the military mission of the installation increases the pressure on scarce GT habitat areas, which requires moving some of the existent populations in those areas to suitably chosen new conservation management areas within the boundaries of the installation. Using the model, we find the most suitable and spatially coherent management areas outside the heavily used training areas.</t>
+          <t xml:space="preserve"> compactness and landscape connectivity are essential properties for effective functioning of conservation reserves. in this article we introduce a linear integer programming model to determine optimal configuration of a conservation reserve with such properties. connectivity can be defined either as structural (physical) connectivity or functional connectivity; the model developed here addresses both properties. we apply the model to identify the optimal conservation management areas for protection of gopher tortoise (gt) in a military installation, ft. benning, georgia, which serves as a safe refuge for this at risk species. the recent expansion in the military mission of the installation increases the pressure on scarce gt habitat areas, which requires moving some of the existent populations in those areas to suitably chosen new conservation management areas within the boundaries of the installation. using the model, we find the most suitable and spatially coherent management areas outside the heavily used training areas.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2451,16 +2451,16 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[11, 14, 15]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.314|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.233|x12: 0.000|x13: 0.000|x14: 0.082|x15: 0.398|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.237|x3: 0.127|x4: 0.136|x5: 0.000|x6: 0.199|x7: 0.000|x8: 0.250|x9: 0.000|x10: 0.061|x11: 0.080|x12: 0.000|x13: 0.000|x14: 0.105|x15: 0.625|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.182|x3: 0.000|x4: 0.054|x5: 0.000|x6: 0.134|x7: 0.170|x8: 0.000|x9: 0.198|x10: 0.000|x11: 0.135|x12: 0.288|x13: 0.153|x14: 0.207|x15: 0.330|x16: 0.105|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.139|x3: 0.147|x4: 0.063|x5: 0.000|x6: 0.111|x7: 0.057|x8: 0.083|x9: 0.066|x10: 0.020|x11: 0.149|x12: 0.096|x13: 0.051|x14: 0.131|x15: 0.409|x16: 0.035|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.061|x3: 0.062|x4: 0.057|x5: 0.053|x6: 0.060|x7: 0.057|x8: 0.058|x9: 0.057|x10: 0.055|x11: 0.062|x12: 0.059|x13: 0.056|x14: 0.061|x15: 0.080|x16: 0.055|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.147|x12: 0.063|x13: 0.000|x14: 0.085|x15: 0.500|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.237|x3: 0.127|x4: 0.136|x5: 0.000|x6: 0.199|x7: 0.000|x8: 0.250|x9: 0.000|x10: 0.061|x11: 0.080|x12: 0.000|x13: 0.000|x14: 0.105|x15: 0.500|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.073|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.145|x6: 0.000|x7: 0.271|x8: 0.000|x9: 0.136|x10: 0.000|x11: 0.304|x12: 0.095|x13: 0.000|x14: 0.336|x15: 0.171|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.018|x2: 0.059|x3: 0.032|x4: 0.034|x5: 0.036|x6: 0.050|x7: 0.068|x8: 0.063|x9: 0.034|x10: 0.015|x11: 0.133|x12: 0.040|x13: 0.000|x14: 0.132|x15: 0.418|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Negotiation and active involvement with participation of water managers, experts, stakeholders and representatives of the general public requires decision support tools (Environmental Decision Support Systems; EDSS) that build on transparency and flexibility in order to reach sound action plans and management instruments. One possible EDSS for active involvement of stakeholders is application of Bayesian networks (Bns). The paper gives an example of a case study (The Danish case) where farmers and hydrologists disputed the degree to which pesticide application affected the quality of deep groundwater. Instead of selecting one opinion or another, the decision was made to include both in the Bns. By adopting this approach, it was possible to view the results from either point of view, accepting the reality of the situation, not becoming mired in an insoluble conflict, and in this way laying the foundation for future compromises. The paper explores Bns as a tool for acting on and dealing with management of groundwater protection. Bns allow stakeholders' divergent values, interests and beliefs to be surfaced and negotiated in participatory processes for areas where conventional physically based groundwater models are insufficient due to lack of data, physical understanding, flexibility or lack of integration capability. In this way, the agency will be able to address the institutional arrangement influencing groundwater protection in all its complexity.</t>
+          <t xml:space="preserve"> negotiation and active involvement with participation of water managers, experts, stakeholders and representatives of the general public requires decision support tools (environmental decision support systems; edss) that build on transparency and flexibility in order to reach sound action plans and management instruments. one possible edss for active involvement of stakeholders is application of bayesian networks (bns). the paper gives an example of a case study (the danish case) where farmers and hydrologists disputed the degree to which pesticide application affected the quality of deep groundwater. instead of selecting one opinion or another, the decision was made to include both in the bns. by adopting this approach, it was possible to view the results from either point of view, accepting the reality of the situation, not becoming mired in an insoluble conflict, and in this way laying the foundation for future compromises. the paper explores bns as a tool for acting on and dealing with management of groundwater protection. bns allow stakeholders divergent values, interests and beliefs to be surfaced and negotiated in participatory processes for areas where conventional physically based groundwater models are insufficient due to lack of data, physical understanding, flexibility or lack of integration capability. in this way, the agency will be able to address the institutional arrangement influencing groundwater protection in all its complexity.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2481,16 +2481,16 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>[3, 6, 12, 13]</t>
+          <t>[6, 16]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.080|x2: 0.000|x3: 0.510|x4: 0.000|x5: 0.000|x6: 0.224|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.091|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.237|x7: 0.000|x8: 0.000|x9: 0.153|x10: 0.000|x11: 0.118|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.091|x16: 0.065|x17: 0.000
 LDA -&gt; x1: 0.057|x2: 0.061|x3: 0.144|x4: 0.104|x5: 0.117|x6: 0.149|x7: 0.134|x8: 0.000|x9: 0.121|x10: 0.000|x11: 0.075|x12: 0.144|x13: 0.152|x14: 0.200|x15: 0.119|x16: 0.242|x17: 0.000
-TOP2VEC -&gt; x1: 0.157|x2: 0.163|x3: 0.000|x4: 0.164|x5: 0.074|x6: 0.279|x7: 0.290|x8: 0.103|x9: 0.100|x10: 0.123|x11: 0.208|x12: 0.492|x13: 0.478|x14: 0.338|x15: 0.207|x16: 0.251|x17: 0.000
-MEAN -&gt; x1: 0.098|x2: 0.075|x3: 0.215|x4: 0.089|x5: 0.064|x6: 0.217|x7: 0.141|x8: 0.034|x9: 0.074|x10: 0.041|x11: 0.197|x12: 0.212|x13: 0.210|x14: 0.179|x15: 0.109|x16: 0.164|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.064|x4: 0.057|x5: 0.055|x6: 0.064|x7: 0.060|x8: 0.054|x9: 0.056|x10: 0.054|x11: 0.063|x12: 0.064|x13: 0.064|x14: 0.062|x15: 0.058|x16: 0.061|x17: 0.052
+TOP2VEC -&gt; x1: 0.144|x2: 0.000|x3: 0.000|x4: 0.063|x5: 0.068|x6: 0.000|x7: 0.176|x8: 0.000|x9: 0.000|x10: 0.080|x11: 0.189|x12: 0.285|x13: 0.273|x14: 0.099|x15: 0.105|x16: 0.228|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.073|x2: 0.015|x3: 0.036|x4: 0.042|x5: 0.046|x6: 0.222|x7: 0.077|x8: 0.000|x9: 0.069|x10: 0.020|x11: 0.095|x12: 0.107|x13: 0.106|x14: 0.075|x15: 0.079|x16: 0.134|x17: 0.000
 </t>
         </is>
       </c>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> produced by the Artificial Intelligence for Ecosystem Services (ARIES) platform (with ESS supply defined as carbon storage and flood regulation, and demand specified as recreation and water use). These are then used for (iii) a joint spatial prioritisation of biodiversity and ESS employing Marxan with Zones, laying out the spatial representation of multiple management zones. Given the transboundary setting of the Danube River Basin, we also run comparative analyses including the country-level purchasing power parity (PPP)adjusted gross domestic product (GDP) and each country's percent cover of the total basin area as potential cost factors, illustrating a scheme for balancing the share of establishing specific zones among countries. We demonstrate how emphasizing various biodiversity or ESS targets in an EBM model-coupling framework can be used to cost-effectively test various spatially explicit management options across a multi-national case study. We further discuss possible limitations, future developments, and requirements for effectively managing a balance between biodiversity and ESS supply and demand in freshwater ecosystems.</t>
+          <t xml:space="preserve"> produced by the artificial intelligence for ecosystem services (aries) platform (with ess supply defined as carbon storage and flood regulation, and demand specified as recreation and water use). these are then used for (iii) a joint spatial prioritisation of biodiversity and ess employing marxan with zones, laying out the spatial representation of multiple management zones. given the transboundary setting of the danube river basin, we also run comparative analyses including the country level purchasing power parity (ppp)adjusted gross domestic product (gdp) and each countrys percent cover of the total basin area as potential cost factors, illustrating a scheme for balancing the share of establishing specific zones among countries. we demonstrate how emphasizing various biodiversity or ess targets in an ebm model coupling framework can be used to cost effectively test various spatially explicit management options across a multi national case study. we further discuss possible limitations, future developments, and requirements for effectively managing a balance between biodiversity and ess supply and demand in freshwater ecosystems.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2516,11 +2516,11 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.297|x4: 0.000|x5: 0.000|x6: 0.290|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.157|x11: 0.172|x12: 0.000|x13: 0.000|x14: 0.163|x15: 0.345|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.334|x7: 0.000|x8: 0.000|x9: 0.102|x10: 0.098|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.140|x15: 0.500|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.110|x3: 0.116|x4: 0.000|x5: 0.056|x6: 0.298|x7: 0.000|x8: 0.122|x9: 0.109|x10: 0.209|x11: 0.087|x12: 0.000|x13: 0.109|x14: 0.295|x15: 0.309|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.120|x2: 0.151|x3: 0.000|x4: 0.236|x5: 0.259|x6: 0.425|x7: 0.247|x8: 0.072|x9: 0.134|x10: 0.000|x11: 0.293|x12: 0.201|x13: 0.425|x14: 0.378|x15: 0.384|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.040|x2: 0.087|x3: 0.138|x4: 0.079|x5: 0.105|x6: 0.338|x7: 0.082|x8: 0.065|x9: 0.081|x10: 0.122|x11: 0.184|x12: 0.067|x13: 0.178|x14: 0.279|x15: 0.346|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.059|x4: 0.056|x5: 0.057|x6: 0.072|x7: 0.056|x8: 0.055|x9: 0.056|x10: 0.058|x11: 0.062|x12: 0.055|x13: 0.061|x14: 0.068|x15: 0.073|x16: 0.051|x17: 0.051
+TOP2VEC -&gt; x1: 0.143|x2: 0.000|x3: 0.000|x4: 0.067|x5: 0.000|x6: 0.107|x7: 0.149|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.092|x12: 0.202|x13: 0.000|x14: 0.227|x15: 0.060|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.028|x3: 0.029|x4: 0.017|x5: 0.014|x6: 0.310|x7: 0.037|x8: 0.030|x9: 0.053|x10: 0.077|x11: 0.045|x12: 0.051|x13: 0.027|x14: 0.166|x15: 0.217|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Deciding where to implement conservation actions in order to meet conservation targets efficiently is an important component of systematic conservation planning. Mathematical optimisation is a quantitative and transparent framework for solving these problems. Despite several advantages of exact methods such as integer linear programming (ILP), most conservation planning problems to date have been solved using heuristic approaches such as simulated annealing (SA). We explain how to implement common conservation planning problems (e.g. Marxan and Marxan With Zones) in an ILP framework and how these formulations can be extended to account for spatial dependencies among planning units, such as those arising from environmental flows (e.g. rivers). Using simulated datasets, we demonstrate that ILP outperforms SA with respect to both solution quality (how close it is to optimality) and processing time over a range of problem sizes. For modestly sized quadratic problems (100,000 spatial units and 10 species), for example, a processing time of approximately 14 h was required for SA to achieve a solution within 19% of optimality, while ILP achieved solutions within 0.5% of optimality within 30 s. For the largest quadratic problems we evaluated processing time exceeding one day was required for SA to achieve a solution within 49% of optimality, while ILP achieved solutions within 0.5% of optimality in approximately one hour. Heuristics are conceptually simple and can be applied to large and non-linear objective functions but unlike ILP, produce solutions of unknown quality. We also discuss how ILP approaches also facilitate quantification of trade-off curves and sensitivity analysis. When solving linear or quadratic conservation planning problems we recommend using ILP over heuristic approaches whenever possible.</t>
+          <t xml:space="preserve"> deciding where to implement conservation actions in order to meet conservation targets efficiently is an important component of systematic conservation planning. mathematical optimisation is a quantitative and transparent framework for solving these problems. despite several advantages of exact methods such as integer linear programming (ilp), most conservation planning problems to date have been solved using heuristic approaches such as simulated annealing (sa). we explain how to implement common conservation planning problems (e.g. marxan and marxan with zones) in an ilp framework and how these formulations can be extended to account for spatial dependencies among planning units, such as those arising from environmental flows (e.g. rivers). using simulated datasets, we demonstrate that ilp outperforms sa with respect to both solution quality (how close it is to optimality) and processing time over a range of problem sizes. for modestly sized quadratic problems (100,000 spatial units and 10 species), for example, a processing time of approximately 14 h was required for sa to achieve a solution within 19% of optimality, while ilp achieved solutions within 0.5% of optimality within 30 s. for the largest quadratic problems we evaluated processing time exceeding one day was required for sa to achieve a solution within 49% of optimality, while ilp achieved solutions within 0.5% of optimality in approximately one hour. heuristics are conceptually simple and can be applied to large and non linear objective functions but unlike ilp, produce solutions of unknown quality. we also discuss how ilp approaches also facilitate quantification of trade off curves and sensitivity analysis. when solving linear or quadratic conservation planning problems we recommend using ilp over heuristic approaches whenever possible.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2541,16 +2541,16 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>[3, 7, 11, 15]</t>
+          <t>[7, 11, 13, 15]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.426|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.246|x12: 0.000|x13: 0.066|x14: 0.091|x15: 0.146|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.076|x4: 0.000|x5: 0.000|x6: 0.073|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.113|x12: 0.104|x13: 0.076|x14: 0.075|x15: 0.205|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.071|x3: 0.155|x4: 0.111|x5: 0.116|x6: 0.055|x7: 0.248|x8: 0.112|x9: 0.128|x10: 0.000|x11: 0.141|x12: 0.000|x13: 0.169|x14: 0.125|x15: 0.387|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.136|x2: 0.107|x3: 0.066|x4: 0.298|x5: 0.309|x6: 0.174|x7: 0.375|x8: 0.137|x9: 0.116|x10: 0.000|x11: 0.244|x12: 0.410|x13: 0.237|x14: 0.184|x15: 0.162|x16: 0.088|x17: 0.000
-MEAN -&gt; x1: 0.045|x2: 0.059|x3: 0.216|x4: 0.136|x5: 0.142|x6: 0.076|x7: 0.208|x8: 0.083|x9: 0.081|x10: 0.000|x11: 0.211|x12: 0.137|x13: 0.157|x14: 0.133|x15: 0.232|x16: 0.029|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.056|x3: 0.065|x4: 0.060|x5: 0.060|x6: 0.056|x7: 0.064|x8: 0.057|x9: 0.057|x10: 0.052|x11: 0.065|x12: 0.060|x13: 0.061|x14: 0.060|x15: 0.066|x16: 0.054|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.446|x8: 0.000|x9: 0.113|x10: 0.000|x11: 0.190|x12: 0.149|x13: 0.215|x14: 0.085|x15: 0.112|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.145|x12: 0.000|x13: 0.232|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.018|x3: 0.058|x4: 0.028|x5: 0.029|x6: 0.032|x7: 0.174|x8: 0.028|x9: 0.060|x10: 0.000|x11: 0.148|x12: 0.063|x13: 0.173|x14: 0.072|x15: 0.176|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Among the emerged metaheuristic optimization techniques, ant colony optimization (ACO) has received considerable attentions in water resources and environmental planning and management during last decade. Different versions of ACO have proved to be flexible and powerful in solving number of spatially and temporally complex water resources problems in discrete and continuous domains with single and/or multiple objectives. Reviewing large number of peer reviewed journal papers and few valuable conference papers, we intend to touch the characteristics of ant algorithms and critically review their state-of-the-art applications in water resources and environmental management problems, both in discrete and continuous domains. The paper seeks to promote Opportunities, advantages and disadvantages of the algorithm as applied to different areas of water resources problems both in research and practice. It also intends to identify and present the major and seminal contributions of ant algorithms and their findings in organized areas of reservoir operation and surface water management, water distribution systems, urban drainage and sewer systems, groundwater managements, environmental and watershed management. Current trends and challenges in ACO algorithms are discussed and called for increased attempts to carry out convergence analysis as an active area of interest.</t>
+          <t xml:space="preserve"> among the emerged metaheuristic optimization techniques, ant colony optimization (aco) has received considerable attentions in water resources and environmental planning and management during last decade. different versions of aco have proved to be flexible and powerful in solving number of spatially and temporally complex water resources problems in discrete and continuous domains with single and/or multiple objectives. reviewing large number of peer reviewed journal papers and few valuable conference papers, we intend to touch the characteristics of ant algorithms and critically review their state of the art applications in water resources and environmental management problems, both in discrete and continuous domains. the paper seeks to promote opportunities, advantages and disadvantages of the algorithm as applied to different areas of water resources problems both in research and practice. it also intends to identify and present the major and seminal contributions of ant algorithms and their findings in organized areas of reservoir operation and surface water management, water distribution systems, urban drainage and sewer systems, groundwater managements, environmental and watershed management. current trends and challenges in aco algorithms are discussed and called for increased attempts to carry out convergence analysis as an active area of interest.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2571,16 +2571,16 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>[3, 6, 15]</t>
+          <t>[6, 11]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.431|x4: 0.000|x5: 0.000|x6: 0.803|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.322|x12: 0.000|x13: 0.000|x14: 0.093|x15: 0.086|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.061|x10: 0.000|x11: 0.163|x12: 0.139|x13: 0.000|x14: 0.000|x15: 0.146|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.157|x4: 0.000|x5: 0.111|x6: 0.296|x7: 0.000|x8: 0.098|x9: 0.155|x10: 0.093|x11: 0.138|x12: 0.093|x13: 0.116|x14: 0.135|x15: 0.248|x16: 0.180|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.248|x3: 0.090|x4: 0.267|x5: 0.213|x6: 0.000|x7: 0.133|x8: 0.097|x9: 0.000|x10: 0.094|x11: 0.000|x12: 0.280|x13: 0.193|x14: 0.368|x15: 0.273|x16: 0.192|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.083|x3: 0.226|x4: 0.089|x5: 0.108|x6: 0.265|x7: 0.044|x8: 0.065|x9: 0.052|x10: 0.062|x11: 0.153|x12: 0.124|x13: 0.103|x14: 0.199|x15: 0.202|x16: 0.124|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.066|x4: 0.057|x5: 0.058|x6: 0.068|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.056|x11: 0.061|x12: 0.059|x13: 0.058|x14: 0.064|x15: 0.064|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.185|x5: 0.177|x6: 0.000|x7: 0.184|x8: 0.000|x9: 0.000|x10: 0.071|x11: 0.208|x12: 0.126|x13: 0.000|x14: 0.181|x15: 0.000|x16: 0.156|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.039|x4: 0.046|x5: 0.072|x6: 0.324|x7: 0.046|x8: 0.025|x9: 0.054|x10: 0.041|x11: 0.127|x12: 0.089|x13: 0.029|x14: 0.079|x15: 0.098|x16: 0.084|x17: 0.000
 </t>
         </is>
       </c>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The increasing incorporation of Artificial Intelligence in the form of automated systems into decision-making procedures highlights not only the importance of decision theory for automated systems but also the need for these decision procedures to be explainable to the people involved in them. Traditional realist accounts of explanation, wherein explanation is a relation that holds (or does not hold) eternally between an explanans and an explanandum, are not adequate to account for the notion of explanation required for artificial decision procedures. We offer an alternative account of explanation as used in the context of automated decision-making that makes explanation an epistemic phenomenon, and one that is dependent on context. This account of explanation better accounts for the way that we talk about, and use, explanations and derived concepts, such as 'explanatory power', and also allows us to differentiate between reasons or causes on the one hand, which do not need to have an epistemic aspect, and explanations on the other, which do have such an aspect. Against this theoretical backdrop we then review existing approaches to explanation in Artificial Intelligence and Machine Learning, and suggest desiderata which truly explainable decision systems should fulfill. 1. Many people are good at constructing post-hoc rationalizations of their decisions (especially, but clearly not exclusively, in the case of intuitive, spontaneous and/or "unconscious" decisions), but generally we do not count these rationalizations as adequate explanations.</t>
+          <t xml:space="preserve"> the increasing incorporation of artificial intelligence in the form of automated systems into decision making procedures highlights not only the importance of decision theory for automated systems but also the need for these decision procedures to be explainable to the people involved in them. traditional realist accounts of explanation, wherein explanation is a relation that holds (or does not hold) eternally between an explanans and an explanandum, are not adequate to account for the notion of explanation required for artificial decision procedures. we offer an alternative account of explanation as used in the context of automated decision making that makes explanation an epistemic phenomenon, and one that is dependent on context. this account of explanation better accounts for the way that we talk about, and use, explanations and derived concepts, such as explanatory power, and also allows us to differentiate between reasons or causes on the one hand, which do not need to have an epistemic aspect, and explanations on the other, which do have such an aspect. against this theoretical backdrop we then review existing approaches to explanation in artificial intelligence and machine learning, and suggest desiderata which truly explainable decision systems should fulfill. 1. many people are good at constructing post hoc rationalizations of their decisions (especially, but clearly not exclusively, in the case of intuitive, spontaneous and/or "unconscious" decisions), but generally we do not count these rationalizations as adequate explanations.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2601,16 +2601,16 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[4, 16]</t>
+          <t>[4, 7, 12, 16]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.424|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.245|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.287|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.080|x3: 0.000|x4: 0.326|x5: 0.000|x6: 0.079|x7: 0.126|x8: 0.000|x9: 0.084|x10: 0.000|x11: 0.000|x12: 0.338|x13: 0.000|x14: 0.223|x15: 0.074|x16: 0.491|x17: 0.000
-TOP2VEC -&gt; x1: 0.170|x2: 0.155|x3: 0.109|x4: 0.321|x5: 0.372|x6: 0.215|x7: 0.369|x8: 0.192|x9: 0.161|x10: 0.099|x11: 0.000|x12: 0.231|x13: 0.224|x14: 0.000|x15: 0.122|x16: 0.202|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.078|x3: 0.177|x4: 0.216|x5: 0.124|x6: 0.098|x7: 0.165|x8: 0.064|x9: 0.082|x10: 0.033|x11: 0.082|x12: 0.190|x13: 0.075|x14: 0.074|x15: 0.065|x16: 0.231|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.063|x4: 0.065|x5: 0.060|x6: 0.058|x7: 0.062|x8: 0.056|x9: 0.057|x10: 0.055|x11: 0.057|x12: 0.064|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.066|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.158|x5: 0.156|x6: 0.060|x7: 0.220|x8: 0.000|x9: 0.000|x10: 0.155|x11: 0.094|x12: 0.147|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.193|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.203|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.273|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.020|x3: 0.000|x4: 0.121|x5: 0.111|x6: 0.035|x7: 0.137|x8: 0.000|x9: 0.021|x10: 0.039|x11: 0.024|x12: 0.190|x13: 0.000|x14: 0.056|x15: 0.019|x16: 0.171|x17: 0.000
 </t>
         </is>
       </c>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We live in an age of paradox. Systems using artificial intelligence match or surpass human level performance in more and more domains, leveraging rapid advances in other technologies and driving soaring stock prices. Yet measured productivity growth has declined by half over the past decade, and real income has stagnated since the late 1990s for a majority of Americans. We describe four potential explanations for this clash of expectations and statistics: false hopes, mismeasurement, redistribution, and implementation lags. While a case can be made for each, we argue that lags have likely been the biggest contributor to the paradox. The most impressive capabilities of AI, particularly those based on machine learning, have not yet diffused widely. More importantly, like other general purpose technologies, their full effects won't be realized until waves of complementary innovations are developed and implemented. The required adjustment costs, organizational changes, and new skills can be modeled as a kind of intangible capital. A portion of the value of this intangible capital is already reflected in the market value of firms. However, going forward, national statistics could fail to measure the full benefits of the new technologies and some may even have the wrong sign.</t>
+          <t xml:space="preserve"> we live in an age of paradox. systems using artificial intelligence match or surpass human level performance in more and more domains, leveraging rapid advances in other technologies and driving soaring stock prices. yet measured productivity growth has declined by half over the past decade, and real income has stagnated since the late 1990s for a majority of americans. we describe four potential explanations for this clash of expectations and statistics: false hopes, mismeasurement, redistribution, and implementation lags. while a case can be made for each, we argue that lags have likely been the biggest contributor to the paradox. the most impressive capabilities of ai, particularly those based on machine learning, have not yet diffused widely. more importantly, like other general purpose technologies, their full effects wont be realized until waves of complementary innovations are developed and implemented. the required adjustment costs, organizational changes, and new skills can be modeled as a kind of intangible capital. a portion of the value of this intangible capital is already reflected in the market value of firms. however, going forward, national statistics could fail to measure the full benefits of the new technologies and some may even have the wrong sign.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2631,16 +2631,16 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>[4, 9]</t>
+          <t>[4, 8, 9, 10]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.367|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.069|x8: 0.121|x9: 0.163|x10: 0.101|x11: 0.212|x12: 0.000|x13: 0.070|x14: 0.069|x15: 0.000|x16: 0.056|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.082|x2: 0.000|x3: 0.110|x4: 0.085|x5: 0.000|x6: 0.000|x7: 0.094|x8: 0.116|x9: 0.218|x10: 0.081|x11: 0.062|x12: 0.000|x13: 0.000|x14: 0.084|x15: 0.000|x16: 0.069|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.179|x3: 0.051|x4: 0.218|x5: 0.000|x6: 0.000|x7: 0.073|x8: 0.195|x9: 0.272|x10: 0.238|x11: 0.000|x12: 0.130|x13: 0.079|x14: 0.163|x15: 0.000|x16: 0.222|x17: 0.000
-TOP2VEC -&gt; x1: 0.159|x2: 0.227|x3: 0.000|x4: 0.406|x5: 0.236|x6: 0.000|x7: 0.080|x8: 0.212|x9: 0.262|x10: 0.102|x11: 0.000|x12: 0.185|x13: 0.146|x14: 0.118|x15: 0.000|x16: 0.208|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.135|x3: 0.139|x4: 0.208|x5: 0.079|x6: 0.000|x7: 0.074|x8: 0.176|x9: 0.232|x10: 0.147|x11: 0.071|x12: 0.105|x13: 0.098|x14: 0.117|x15: 0.000|x16: 0.162|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.061|x4: 0.065|x5: 0.057|x6: 0.053|x7: 0.057|x8: 0.063|x9: 0.067|x10: 0.061|x11: 0.057|x12: 0.059|x13: 0.058|x14: 0.059|x15: 0.053|x16: 0.062|x17: 0.053
+TOP2VEC -&gt; x1: 0.234|x2: 0.111|x3: 0.000|x4: 0.416|x5: 0.070|x6: 0.000|x7: 0.130|x8: 0.186|x9: 0.262|x10: 0.180|x11: 0.141|x12: 0.064|x13: 0.134|x14: 0.114|x15: 0.092|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.100|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.079|x2: 0.072|x3: 0.040|x4: 0.180|x5: 0.018|x6: 0.000|x7: 0.074|x8: 0.149|x9: 0.313|x10: 0.124|x11: 0.051|x12: 0.049|x13: 0.053|x14: 0.090|x15: 0.023|x16: 0.073|x17: 0.000
 </t>
         </is>
       </c>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We summarize a framework for the study of the implications of automation and AI on the demand for labor, wages, and employment. Our task-based framework emphasizes the displacement effect that automation creates as machines and AI replace labor in tasks that it used to perform. This displacement effect tends to reduce the demand for labor and wages. But it is counteracted by a productivity effect, resulting from the cost savings generated by automation, which increase the demand for labor in non-automated tasks. The productivity effect is complemented by additional capital accumulation and the deepening of automation (improvements of existing machinery), both of which further increase the demand for labor. These countervailing effects are incomplete. Even when they are strong, automation in-creases output per worker more than wages and reduce the share of labor in national income. The more powerful countervailing force against automation is the creation of new labor-intensive tasks, which reinstates labor in new activities and tends to increase the labor share to counterbalance the impact of automation. Our framework also highlights the constraints and imperfections that slow down the adjustment of the economy and the labor market to automation and weaken the resulting productivity gains from this transformation: a mismatch between the skill requirements of new technologies, and the possibility that automation is being introduced at an excessive rate, possibly at the expense of other productivity-enhancing technologies.</t>
+          <t xml:space="preserve"> we summarize a framework for the study of the implications of automation and ai on the demand for labor, wages, and employment. our task based framework emphasizes the displacement effect that automation creates as machines and ai replace labor in tasks that it used to perform. this displacement effect tends to reduce the demand for labor and wages. but it is counteracted by a productivity effect, resulting from the cost savings generated by automation, which increase the demand for labor in non automated tasks. the productivity effect is complemented by additional capital accumulation and the deepening of automation (improvements of existing machinery), both of which further increase the demand for labor. these countervailing effects are incomplete. even when they are strong, automation in creases output per worker more than wages and reduce the share of labor in national income. the more powerful countervailing force against automation is the creation of new labor intensive tasks, which reinstates labor in new activities and tends to increase the labor share to counterbalance the impact of automation. our framework also highlights the constraints and imperfections that slow down the adjustment of the economy and the labor market to automation and weaken the resulting productivity gains from this transformation: a mismatch between the skill requirements of new technologies, and the possibility that automation is being introduced at an excessive rate, possibly at the expense of other productivity enhancing technologies.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2661,16 +2661,16 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[8, 10]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.209|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.448|x9: 0.000|x10: 0.000|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.092|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.488|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.201|x4: 0.117|x5: 0.000|x6: 0.000|x7: 0.129|x8: 0.245|x9: 0.167|x10: 0.216|x11: 0.000|x12: 0.146|x13: 0.000|x14: 0.262|x15: 0.153|x16: 0.183|x17: 0.000
-TOP2VEC -&gt; x1: 0.124|x2: 0.373|x3: 0.000|x4: 0.199|x5: 0.353|x6: 0.116|x7: 0.110|x8: 0.199|x9: 0.241|x10: 0.081|x11: 0.000|x12: 0.194|x13: 0.000|x14: 0.175|x15: 0.000|x16: 0.165|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.124|x3: 0.137|x4: 0.105|x5: 0.118|x6: 0.039|x7: 0.080|x8: 0.297|x9: 0.136|x10: 0.099|x11: 0.040|x12: 0.113|x13: 0.000|x14: 0.146|x15: 0.051|x16: 0.116|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.061|x4: 0.059|x5: 0.060|x6: 0.055|x7: 0.058|x8: 0.072|x9: 0.061|x10: 0.059|x11: 0.055|x12: 0.060|x13: 0.053|x14: 0.062|x15: 0.056|x16: 0.060|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.138|x5: 0.000|x6: 0.000|x7: 0.129|x8: 0.293|x9: 0.065|x10: 0.162|x11: 0.077|x12: 0.171|x13: 0.000|x14: 0.073|x15: 0.178|x16: 0.194|x17: 0.000
+BERTOPIC -&gt; x1: 0.132|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.000|x10: 0.131|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.033|x2: 0.023|x3: 0.050|x4: 0.064|x5: 0.000|x6: 0.000|x7: 0.065|x8: 0.381|x9: 0.058|x10: 0.127|x11: 0.019|x12: 0.079|x13: 0.000|x14: 0.084|x15: 0.083|x16: 0.094|x17: 0.000
 </t>
         </is>
       </c>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The combination of increased availability of large amounts of finegrained human behavioral data and advances in machine learning is presiding over a growing reliance on algorithms to address complex societal problems. Algorithmic decision-making processes might lead to more objective and thus potentially fairer decisions than those made by humans who may be influenced by greed, prejudice, fatigue, or hunger. However, algorithmic decision-making has been criticized for its potential to enhance discrimination, information and power asymmetry, and opacity. In this paper we provide an overview of available technical solutions to enhance fairness, accountability and transparency in algorithmic decision-making. We also highlight the criticality and urgency to engage multi-disciplinary teams of researchers, practitioners, policy makers and citizens to co-develop, deploy and evaluate in the real-world algorithmic decision-making processes designed to maximize fairness and transparency. In doing so, we describe the Open Algortihms (OPAL) project as a step towards</t>
+          <t xml:space="preserve"> the combination of increased availability of large amounts of finegrained human behavioral data and advances in machine learning is presiding over a growing reliance on algorithms to address complex societal problems. algorithmic decision making processes might lead to more objective and thus potentially fairer decisions than those made by humans who may be influenced by greed, prejudice, fatigue, or hunger. however, algorithmic decision making has been criticized for its potential to enhance discrimination, information and power asymmetry, and opacity. in this paper we provide an overview of available technical solutions to enhance fairness, accountability and transparency in algorithmic decision making. we also highlight the criticality and urgency to engage multi disciplinary teams of researchers, practitioners, policy makers and citizens to co develop, deploy and evaluate in the real world algorithmic decision making processes designed to maximize fairness and transparency. in doing so, we describe the open algortihms (opal) project as a step towards</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2691,16 +2691,16 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[12, 16]</t>
+          <t>[5, 16]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.466|x4: 0.000|x5: 0.054|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.054|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.133|x3: 0.000|x4: 0.000|x5: 0.128|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.095|x10: 0.000|x11: 0.091|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.089|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.098|x3: 0.084|x4: 0.240|x5: 0.170|x6: 0.000|x7: 0.134|x8: 0.114|x9: 0.067|x10: 0.000|x11: 0.000|x12: 0.220|x13: 0.133|x14: 0.236|x15: 0.000|x16: 0.323|x17: 0.000
-TOP2VEC -&gt; x1: 0.128|x2: 0.261|x3: 0.000|x4: 0.079|x5: 0.268|x6: 0.200|x7: 0.356|x8: 0.104|x9: 0.164|x10: 0.110|x11: 0.132|x12: 0.497|x13: 0.360|x14: 0.212|x15: 0.000|x16: 0.226|x17: 0.000
-MEAN -&gt; x1: 0.043|x2: 0.120|x3: 0.183|x4: 0.106|x5: 0.164|x6: 0.067|x7: 0.163|x8: 0.073|x9: 0.077|x10: 0.037|x11: 0.134|x12: 0.239|x13: 0.164|x14: 0.150|x15: 0.000|x16: 0.201|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.063|x4: 0.058|x5: 0.062|x6: 0.056|x7: 0.062|x8: 0.056|x9: 0.057|x10: 0.054|x11: 0.060|x12: 0.067|x13: 0.062|x14: 0.061|x15: 0.052|x16: 0.064|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.117|x5: 0.104|x6: 0.000|x7: 0.272|x8: 0.000|x9: 0.147|x10: 0.135|x11: 0.128|x12: 0.210|x13: 0.139|x14: 0.000|x15: 0.000|x16: 0.299|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.493|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.058|x3: 0.021|x4: 0.089|x5: 0.224|x6: 0.000|x7: 0.102|x8: 0.028|x9: 0.077|x10: 0.034|x11: 0.055|x12: 0.108|x13: 0.068|x14: 0.059|x15: 0.000|x16: 0.178|x17: 0.000
 </t>
         </is>
       </c>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We examine how susceptible jobs are to computerisation. To assess this, we begin by implementing a novel methodology to estimate the probability of computerisation for 702 detailed occupations, using a Gaussian process classifier. Based on these estimates, we examine expected impacts of future computerisation on US labour market outcomes, with the primary objective of analysing the number of jobs at risk and the relationship between an occupation's probability of computerisation, wages and educational attainment. According to our estimates, about 47 percent of total US employment is at risk. We further provide evidence that wages and educational attainment exhibit a strong negative relationship with an occupation's probability of computerisation.</t>
+          <t xml:space="preserve"> we examine how susceptible jobs are to computerisation. to assess this, we begin by implementing a novel methodology to estimate the probability of computerisation for 702 detailed occupations, using a gaussian process classifier. based on these estimates, we examine expected impacts of future computerisation on us labour market outcomes, with the primary objective of analysing the number of jobs at risk and the relationship between an occupations probability of computerisation, wages and educational attainment. according to our estimates, about 47 percent of total us employment is at risk. we further provide evidence that wages and educational attainment exhibit a strong negative relationship with an occupations probability of computerisation.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2721,16 +2721,16 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>[3, 8]</t>
+          <t>[3, 4, 8, 10]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.181|x4: 0.094|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.274|x9: 0.000|x10: 0.000|x11: 0.095|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.183|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.327|x4: 0.237|x5: 0.000|x6: 0.000|x7: 0.182|x8: 0.491|x9: 0.000|x10: 0.268|x11: 0.000|x12: 0.000|x13: 0.119|x14: 0.000|x15: 0.000|x16: 0.075|x17: 0.000
-TOP2VEC -&gt; x1: 0.197|x2: 0.000|x3: 0.227|x4: 0.211|x5: 0.421|x6: 0.000|x7: 0.000|x8: 0.245|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.193|x13: 0.000|x14: 0.000|x15: 0.063|x16: 0.078|x17: 0.000
-MEAN -&gt; x1: 0.066|x2: 0.041|x3: 0.245|x4: 0.181|x5: 0.140|x6: 0.000|x7: 0.061|x8: 0.337|x9: 0.000|x10: 0.089|x11: 0.032|x12: 0.064|x13: 0.040|x14: 0.000|x15: 0.021|x16: 0.051|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.069|x4: 0.065|x5: 0.062|x6: 0.054|x7: 0.057|x8: 0.076|x9: 0.054|x10: 0.059|x11: 0.056|x12: 0.058|x13: 0.056|x14: 0.054|x15: 0.055|x16: 0.057|x17: 0.054
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.185|x4: 0.243|x5: 0.232|x6: 0.078|x7: 0.261|x8: 0.272|x9: 0.000|x10: 0.171|x11: 0.173|x12: 0.077|x13: 0.265|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.143|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.000|x10: 0.144|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.036|x2: 0.031|x3: 0.128|x4: 0.166|x5: 0.058|x6: 0.020|x7: 0.111|x8: 0.441|x9: 0.000|x10: 0.146|x11: 0.043|x12: 0.019|x13: 0.096|x14: 0.000|x15: 0.000|x16: 0.019|x17: 0.000
 </t>
         </is>
       </c>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>This paper presents a comprehensive review of 179 studies which employ operational research or and artificial intelligence ai techniques in the assessment of bank performance we first discuss numerous applications of data envelopment analysis which is the most widely applied or technique in the field then we discuss applications of other techniques such as neural networks support vector machines and multicriteria decision aid that have also been used in recent years in bank failure prediction studies and the assessment of bank creditworthiness and underperformance</t>
+          <t>this paper presents a comprehensive review of 179 studies which employ operational research or and artificial intelligence ai techniques in the assessment of bank performance we first discuss numerous applications of data envelopment analysis which is the most widely applied or technique in the field then we discuss applications of other techniques such as neural networks support vector machines and multicriteria decision aid that have also been used in recent years in bank failure prediction studies and the assessment of bank creditworthiness and underperformance</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2751,16 +2751,16 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>[3, 13, 14]</t>
+          <t>[10, 14]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.678|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.392|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.176|x10: 0.000|x11: 0.156|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.058|x3: 0.215|x4: 0.000|x5: 0.190|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.111|x10: 0.248|x11: 0.000|x12: 0.068|x13: 0.345|x14: 0.413|x15: 0.000|x16: 0.172|x17: 0.000
-TOP2VEC -&gt; x1: 0.166|x2: 0.080|x3: 0.101|x4: 0.292|x5: 0.398|x6: 0.207|x7: 0.302|x8: 0.196|x9: 0.367|x10: 0.104|x11: 0.078|x12: 0.386|x13: 0.313|x14: 0.399|x15: 0.381|x16: 0.213|x17: 0.000
-MEAN -&gt; x1: 0.055|x2: 0.046|x3: 0.272|x4: 0.097|x5: 0.196|x6: 0.069|x7: 0.101|x8: 0.065|x9: 0.159|x10: 0.117|x11: 0.157|x12: 0.151|x13: 0.219|x14: 0.271|x15: 0.127|x16: 0.128|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.054|x3: 0.068|x4: 0.057|x5: 0.063|x6: 0.055|x7: 0.057|x8: 0.055|x9: 0.060|x10: 0.058|x11: 0.060|x12: 0.060|x13: 0.064|x14: 0.067|x15: 0.058|x16: 0.058|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.059|x6: 0.119|x7: 0.244|x8: 0.000|x9: 0.141|x10: 0.203|x11: 0.101|x12: 0.112|x13: 0.000|x14: 0.296|x15: 0.069|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.063|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.125|x9: 0.000|x10: 0.122|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.016|x2: 0.014|x3: 0.054|x4: 0.000|x5: 0.062|x6: 0.030|x7: 0.061|x8: 0.031|x9: 0.107|x10: 0.143|x11: 0.064|x12: 0.045|x13: 0.086|x14: 0.177|x15: 0.017|x16: 0.043|x17: 0.000
 </t>
         </is>
       </c>
@@ -2771,7 +2771,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Reliable water level forecasting for reservoir inflow is essential for reservoir operation. The objective of this paper is to develop and apply two hybrid models for daily water level forecasting and investigate their accuracy. These two hybrid models are wavelet-based artificial neural network (WANN) and wavelet-based adaptive neuro-fuzzy inference system (WANFIS). Wavelet decomposition is employed to decompose an input time series into approximation and detail components. The decomposed time series are used as inputs to artificial neural networks (ANN) and adaptive neuro-fuzzy inference system (ANFIS) for WANN and WANFIS models, respectively. Based on statistical performance indexes, the WANN and WANFIS models are found to produce better efficiency than the ANN and ANFIS models. WANFIS7-sym10 yields the best performance among all other models. It is found that wavelet decomposition improves the accuracy of ANN and ANFIS. This study evaluates the accuracy of the WANN and WANFIS models for different mother wavelets, including Daubechies, Symmlet and Coiflet wavelets. It is found that the model performance is dependent on input sets and mother wavelets, and the wavelet decomposition using mother wavelet, db10, can further improve the efficiency of ANN and ANFIS models. Results obtained from this study indicate that the conjunction of wavelet decomposition and artificial intelligence models can be a useful tool for accurate forecasting daily water level and can yield better efficiency than the conventional forecasting models.</t>
+          <t xml:space="preserve"> reliable water level forecasting for reservoir inflow is essential for reservoir operation. the objective of this paper is to develop and apply two hybrid models for daily water level forecasting and investigate their accuracy. these two hybrid models are wavelet based artificial neural network (wann) and wavelet based adaptive neuro fuzzy inference system (wanfis). wavelet decomposition is employed to decompose an input time series into approximation and detail components. the decomposed time series are used as inputs to artificial neural networks (ann) and adaptive neuro fuzzy inference system (anfis) for wann and wanfis models, respectively. based on statistical performance indexes, the wann and wanfis models are found to produce better efficiency than the ann and anfis models. wanfis7 sym10 yields the best performance among all other models. it is found that wavelet decomposition improves the accuracy of ann and anfis. this study evaluates the accuracy of the wann and wanfis models for different mother wavelets, including daubechies, symmlet and coiflet wavelets. it is found that the model performance is dependent on input sets and mother wavelets, and the wavelet decomposition using mother wavelet, db10, can further improve the efficiency of ann and anfis models. results obtained from this study indicate that the conjunction of wavelet decomposition and artificial intelligence models can be a useful tool for accurate forecasting daily water level and can yield better efficiency than the conventional forecasting models.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2781,16 +2781,16 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[6, 9, 14]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.543|x4: 0.000|x5: 0.000|x6: 0.154|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.314|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.415|x7: 0.074|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.061|x3: 0.089|x4: 0.092|x5: 0.000|x6: 0.317|x7: 0.079|x8: 0.086|x9: 0.295|x10: 0.140|x11: 0.000|x12: 0.075|x13: 0.000|x14: 0.346|x15: 0.000|x16: 0.139|x17: 0.000
-TOP2VEC -&gt; x1: 0.174|x2: 0.265|x3: 0.000|x4: 0.126|x5: 0.077|x6: 0.247|x7: 0.419|x8: 0.194|x9: 0.215|x10: 0.000|x11: 0.197|x12: 0.386|x13: 0.269|x14: 0.138|x15: 0.066|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.092|x2: 0.109|x3: 0.196|x4: 0.073|x5: 0.026|x6: 0.239|x7: 0.166|x8: 0.093|x9: 0.170|x10: 0.047|x11: 0.170|x12: 0.154|x13: 0.090|x14: 0.161|x15: 0.022|x16: 0.081|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.059|x3: 0.064|x4: 0.056|x5: 0.054|x6: 0.067|x7: 0.062|x8: 0.058|x9: 0.062|x10: 0.055|x11: 0.062|x12: 0.061|x13: 0.057|x14: 0.062|x15: 0.054|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.171|x8: 0.000|x9: 0.240|x10: 0.057|x11: 0.228|x12: 0.160|x13: 0.112|x14: 0.144|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.026|x2: 0.015|x3: 0.022|x4: 0.023|x5: 0.000|x6: 0.308|x7: 0.081|x8: 0.021|x9: 0.134|x10: 0.049|x11: 0.057|x12: 0.059|x13: 0.028|x14: 0.122|x15: 0.000|x16: 0.035|x17: 0.000
 </t>
         </is>
       </c>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Electricity is an important asset that influences not only the economy, but political or social security of a country. Reliable and accurate planning and prediction of electricity demand for a country are therefore vital. In this paper, electricity demand in Ontario province of Canada from the year 1976e2005 is modeled by using an (adaptive neuro fuzzy inference system) ANFIS. A neuro fuzzy structure can be defined as an ANN (artificial neural network) which is trained by experimental data to find the parameters of (fuzzy inference system) FIS. Inputs for the model include number of employment, (gross domestic product) GDP, population, dwelling count and two meteorological parameters related to annual weather temperature. The data were collected and screened using statistical methods. Then, based on the data, a neuro-fuzzy model for the electricity demand is built. It was found that electricity demand is most sensitive to employment.</t>
+          <t xml:space="preserve"> electricity is an important asset that influences not only the economy, but political or social security of a country. reliable and accurate planning and prediction of electricity demand for a country are therefore vital. in this paper, electricity demand in ontario province of canada from the year 1976e2005 is modeled by using an (adaptive neuro fuzzy inference system) anfis. a neuro fuzzy structure can be defined as an ann (artificial neural network) which is trained by experimental data to find the parameters of (fuzzy inference system) fis. inputs for the model include number of employment, (gross domestic product) gdp, population, dwelling count and two meteorological parameters related to annual weather temperature. the data were collected and screened using statistical methods. then, based on the data, a neuro fuzzy model for the electricity demand is built. it was found that electricity demand is most sensitive to employment.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2816,11 +2816,11 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.361|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.205|x8: 0.156|x9: 0.000|x10: 0.000|x11: 0.214|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.338|x8: 0.342|x9: 0.145|x10: 0.000|x11: 0.093|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.223|x3: 0.136|x4: 0.099|x5: 0.000|x6: 0.126|x7: 0.437|x8: 0.000|x9: 0.354|x10: 0.000|x11: 0.141|x12: 0.056|x13: 0.083|x14: 0.000|x15: 0.000|x16: 0.061|x17: 0.000
-TOP2VEC -&gt; x1: 0.147|x2: 0.184|x3: 0.000|x4: 0.066|x5: 0.000|x6: 0.407|x7: 0.548|x8: 0.146|x9: 0.425|x10: 0.000|x11: 0.350|x12: 0.107|x13: 0.449|x14: 0.000|x15: 0.191|x16: 0.056|x17: 0.000
-MEAN -&gt; x1: 0.083|x2: 0.136|x3: 0.166|x4: 0.055|x5: 0.000|x6: 0.178|x7: 0.381|x8: 0.101|x9: 0.260|x10: 0.000|x11: 0.235|x12: 0.054|x13: 0.177|x14: 0.000|x15: 0.064|x16: 0.039|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.060|x3: 0.062|x4: 0.055|x5: 0.052|x6: 0.062|x7: 0.076|x8: 0.058|x9: 0.068|x10: 0.052|x11: 0.066|x12: 0.055|x13: 0.062|x14: 0.052|x15: 0.056|x16: 0.054|x17: 0.052
+TOP2VEC -&gt; x1: 0.107|x2: 0.000|x3: 0.000|x4: 0.129|x5: 0.097|x6: 0.054|x7: 0.407|x8: 0.000|x9: 0.182|x10: 0.081|x11: 0.358|x12: 0.136|x13: 0.311|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.451|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.115|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.053|x2: 0.056|x3: 0.034|x4: 0.057|x5: 0.024|x6: 0.045|x7: 0.408|x8: 0.086|x9: 0.170|x10: 0.020|x11: 0.148|x12: 0.077|x13: 0.098|x14: 0.000|x15: 0.000|x16: 0.015|x17: 0.000
 </t>
         </is>
       </c>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In the cities and regions of the twentieth first century a radical turn is taking place as information and communication technologies are converging with the innovation-led regional economies, innovative clusters and agglomerations. Intelligent cities are part of the orientation towards the creation of environments that improve our cognitive skills, our ability to learn, foresee, and innovate. The paper discusses the driving forces sustaining the rise of intelligent cities, such as the globalization of innovation clusters and networks, open innovation, and web-based collaborative environments. Then we look at the movements shaping them -local initiatives around the world, European Living Labs, and applications developed by large companies like IBM, MS and CISCO. The last part of the paper focuses on the planning challenges for building intelligent cities and interactive systems of innovation. We discuss the problem of integration among the physical, institutional and digital dimensions of intelligent cities and the 'bridges' that connect these three spatialities.</t>
+          <t xml:space="preserve"> in the cities and regions of the twentieth first century a radical turn is taking place as information and communication technologies are converging with the innovation led regional economies, innovative clusters and agglomerations. intelligent cities are part of the orientation towards the creation of environments that improve our cognitive skills, our ability to learn, foresee, and innovate. the paper discusses the driving forces sustaining the rise of intelligent cities, such as the globalization of innovation clusters and networks, open innovation, and web based collaborative environments. then we look at the movements shaping them local initiatives around the world, european living labs, and applications developed by large companies like ibm, ms and cisco. the last part of the paper focuses on the planning challenges for building intelligent cities and interactive systems of innovation. we discuss the problem of integration among the physical, institutional and digital dimensions of intelligent cities and the bridges that connect these three spatialities.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2841,16 +2841,16 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>[9, 11, 12]</t>
+          <t>[9, 11]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.302|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.084|x10: 0.000|x11: 1.006|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.186|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.127|x4: 0.082|x5: 0.000|x6: 0.000|x7: 0.121|x8: 0.193|x9: 0.457|x10: 0.103|x11: 0.272|x12: 0.125|x13: 0.070|x14: 0.091|x15: 0.000|x16: 0.178|x17: 0.000
-TOP2VEC -&gt; x1: 0.065|x2: 0.189|x3: 0.000|x4: 0.229|x5: 0.113|x6: 0.182|x7: 0.294|x8: 0.064|x9: 0.417|x10: 0.051|x11: 0.288|x12: 0.592|x13: 0.345|x14: 0.288|x15: 0.235|x16: 0.105|x17: 0.000
-MEAN -&gt; x1: 0.022|x2: 0.063|x3: 0.143|x4: 0.104|x5: 0.038|x6: 0.061|x7: 0.139|x8: 0.086|x9: 0.319|x10: 0.052|x11: 0.353|x12: 0.208|x13: 0.138|x14: 0.126|x15: 0.078|x16: 0.094|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.055|x3: 0.060|x4: 0.058|x5: 0.054|x6: 0.055|x7: 0.060|x8: 0.057|x9: 0.072|x10: 0.055|x11: 0.074|x12: 0.064|x13: 0.060|x14: 0.059|x15: 0.056|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.082|x5: 0.000|x6: 0.000|x7: 0.155|x8: 0.101|x9: 0.153|x10: 0.000|x11: 0.297|x12: 0.152|x13: 0.083|x14: 0.207|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.032|x4: 0.041|x5: 0.000|x6: 0.000|x7: 0.069|x8: 0.074|x9: 0.199|x10: 0.026|x11: 0.392|x12: 0.069|x13: 0.038|x14: 0.075|x15: 0.000|x16: 0.045|x17: 0.000
 </t>
         </is>
       </c>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Problem statement: Recent commercial and residential development have substantially impacted the fluxes and quality of water that recharge the aquifers and discharges to streams, lakes and wetlands and, ultimately, is recycled for potable use. Whereas the contaminant sources may be varied in scope and composition, these issues of urban water sustainability are of public health concern at all levels of economic development worldwide, and require cheap and innovative environmental sensing capabilities and interactive monitoring networks, as well as tailored distributed water treatment technologies. To address this need, a roundtable was organized to explore the potential role of advances in biotechnology and bioengineering to aid in developing causative relationships between spatial and temporal changes in urbanization patterns and groundwater and surface water quality parameters, and to address aspects of socioeconomic constraints in implementing sustainable exploitation of water resources. Workshop outcomes: An interactive framework for quantitative analysis of the coupling between human and natural systems requires integrating information derived from online and offline point measurements with Geographic Information Systems (GIS)-based remote sensing imagery analysis, groundwater -</t>
+          <t xml:space="preserve"> problem statement: recent commercial and residential development have substantially impacted the fluxes and quality of water that recharge the aquifers and discharges to streams, lakes and wetlands and, ultimately, is recycled for potable use. whereas the contaminant sources may be varied in scope and composition, these issues of urban water sustainability are of public health concern at all levels of economic development worldwide, and require cheap and innovative environmental sensing capabilities and interactive monitoring networks, as well as tailored distributed water treatment technologies. to address this need, a roundtable was organized to explore the potential role of advances in biotechnology and bioengineering to aid in developing causative relationships between spatial and temporal changes in urbanization patterns and groundwater and surface water quality parameters, and to address aspects of socioeconomic constraints in implementing sustainable exploitation of water resources. workshop outcomes: an interactive framework for quantitative analysis of the coupling between human and natural systems requires integrating information derived from online and offline point measurements with geographic information systems (gis) based remote sensing imagery analysis, groundwater </t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2871,16 +2871,16 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>[3, 6, 11, 12]</t>
+          <t>[6, 11]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.285|x4: 0.000|x5: 0.000|x6: 0.738|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.294|x12: 0.147|x13: 0.083|x14: 0.059|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.075|x4: 0.063|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.087|x10: 0.000|x11: 0.230|x12: 0.117|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.191|x4: 0.160|x5: 0.068|x6: 0.345|x7: 0.090|x8: 0.000|x9: 0.146|x10: 0.000|x11: 0.181|x12: 0.153|x13: 0.000|x14: 0.117|x15: 0.152|x16: 0.217|x17: 0.000
-TOP2VEC -&gt; x1: 0.085|x2: 0.000|x3: 0.168|x4: 0.337|x5: 0.166|x6: 0.314|x7: 0.406|x8: 0.105|x9: 0.227|x10: 0.078|x11: 0.476|x12: 0.365|x13: 0.166|x14: 0.217|x15: 0.274|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.000|x3: 0.215|x4: 0.165|x5: 0.078|x6: 0.386|x7: 0.166|x8: 0.035|x9: 0.124|x10: 0.026|x11: 0.317|x12: 0.221|x13: 0.083|x14: 0.131|x15: 0.142|x16: 0.126|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.051|x3: 0.064|x4: 0.060|x5: 0.055|x6: 0.075|x7: 0.060|x8: 0.053|x9: 0.058|x10: 0.053|x11: 0.070|x12: 0.064|x13: 0.056|x14: 0.058|x15: 0.059|x16: 0.058|x17: 0.051
+TOP2VEC -&gt; x1: 0.063|x2: 0.000|x3: 0.000|x4: 0.181|x5: 0.063|x6: 0.228|x7: 0.395|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.320|x12: 0.208|x13: 0.067|x14: 0.136|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.016|x2: 0.000|x3: 0.066|x4: 0.101|x5: 0.033|x6: 0.393|x7: 0.121|x8: 0.000|x9: 0.058|x10: 0.000|x11: 0.183|x12: 0.119|x13: 0.017|x14: 0.063|x15: 0.038|x16: 0.054|x17: 0.000
 </t>
         </is>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This chapter presents a methodology for maintenance optimization for heterogeneous infrastructure systems, i.e., systems composed of multiple facilities with different characteristics such as environments, materials and deterioration processes. We present a two-stage bottom-up approach. In the first step, optimal and near-optimal maintenance policies for each facility are found and used as inputs for the system-level optimization. In the second step, the problem is formulated as a constrained combinatorial optimization problem, where the best combination of facility-level optimal and near-optimal solutions is identified. An Evolutionary Algorithm (EA) is adopted to solve the combinatorial optimization problem. Its performance is evaluated using a hypothetical system of pavement sections. We find that a near-optimal solution (within less than 0.1% difference from the optimal solution) can be obtained in most cases. Numerical experiments show the potential of the proposed algorithm to solve the maintenance optimization problem for realistic heterogeneous systems.</t>
+          <t xml:space="preserve"> this chapter presents a methodology for maintenance optimization for heterogeneous infrastructure systems, i.e., systems composed of multiple facilities with different characteristics such as environments, materials and deterioration processes. we present a two stage bottom up approach. in the first step, optimal and near optimal maintenance policies for each facility are found and used as inputs for the system level optimization. in the second step, the problem is formulated as a constrained combinatorial optimization problem, where the best combination of facility level optimal and near optimal solutions is identified. an evolutionary algorithm (ea) is adopted to solve the combinatorial optimization problem. its performance is evaluated using a hypothetical system of pavement sections. we find that a near optimal solution (within less than 0.1% difference from the optimal solution) can be obtained in most cases. numerical experiments show the potential of the proposed algorithm to solve the maintenance optimization problem for realistic heterogeneous systems.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2901,16 +2901,16 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>[3, 14]</t>
+          <t>[9, 14]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.340|x4: 0.000|x5: 0.000|x6: 0.069|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.197|x12: 0.088|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.073|x7: 0.000|x8: 0.000|x9: 0.071|x10: 0.000|x11: 0.068|x12: 0.179|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.154|x3: 0.262|x4: 0.410|x5: 0.000|x6: 0.000|x7: 0.091|x8: 0.000|x9: 0.339|x10: 0.000|x11: 0.000|x12: 0.080|x13: 0.000|x14: 0.348|x15: 0.000|x16: 0.136|x17: 0.000
-TOP2VEC -&gt; x1: 0.160|x2: 0.288|x3: 0.336|x4: 0.105|x5: 0.222|x6: 0.271|x7: 0.272|x8: 0.182|x9: 0.191|x10: 0.101|x11: 0.238|x12: 0.312|x13: 0.227|x14: 0.410|x15: 0.161|x16: 0.206|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.147|x3: 0.313|x4: 0.172|x5: 0.074|x6: 0.113|x7: 0.121|x8: 0.061|x9: 0.177|x10: 0.034|x11: 0.145|x12: 0.160|x13: 0.076|x14: 0.253|x15: 0.054|x16: 0.114|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.071|x4: 0.062|x5: 0.056|x6: 0.058|x7: 0.059|x8: 0.055|x9: 0.062|x10: 0.054|x11: 0.060|x12: 0.061|x13: 0.056|x14: 0.067|x15: 0.055|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.187|x3: 0.000|x4: 0.099|x5: 0.000|x6: 0.081|x7: 0.189|x8: 0.000|x9: 0.169|x10: 0.092|x11: 0.080|x12: 0.087|x13: 0.161|x14: 0.215|x15: 0.051|x16: 0.127|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.189|x12: 0.000|x13: 0.206|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.085|x3: 0.065|x4: 0.127|x5: 0.000|x6: 0.038|x7: 0.070|x8: 0.000|x9: 0.145|x10: 0.023|x11: 0.084|x12: 0.086|x13: 0.092|x14: 0.141|x15: 0.013|x16: 0.066|x17: 0.000
 </t>
         </is>
       </c>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>The impact of the industrial and digital information revolutions has undoubtedly been substantial on practically all aspects of our society life firms and employment will the forthcoming ai revolution produce similar farreaching effects by examining analogous inventions of the industrial digital and ai revolutions this article claims that the latter is on target and that it would bring extensive changes that will also affect all aspects of our society and life in addition its impact on firms and employment will be considerable resulting in richly interconnected organizations with decision making based on the analysis and exploitation of big data and intensified global competition among firms people will be capable of buying good and obtaining services from anywhere in the world using the internet and exploiting the unlimited additional benefits that will open through the widespread usage of ai inventions the paper concludes that significant competitive advantages will continue to accrue to those utilizing the internet widely and willing to take entrepreneurial risks in order to turn innovative productsservices into worldwide commercial success stories the greatest challenge facing societies and firms would be utilising the benefits of availing ai technologies providing vast opportunities for both new productsservices and immense productivity improvements while avoiding the dangers and disadvantages in terms of increased unemployment and greater wealth inequalities</t>
+          <t>the impact of the industrial and digital information revolutions has undoubtedly been substantial on practically all aspects of our society life firms and employment will the forthcoming ai revolution produce similar farreaching effects by examining analogous inventions of the industrial digital and ai revolutions this article claims that the latter is on target and that it would bring extensive changes that will also affect all aspects of our society and life in addition its impact on firms and employment will be considerable resulting in richly interconnected organizations with decision making based on the analysis and exploitation of big data and intensified global competition among firms people will be capable of buying good and obtaining services from anywhere in the world using the internet and exploiting the unlimited additional benefits that will open through the widespread usage of ai inventions the paper concludes that significant competitive advantages will continue to accrue to those utilizing the internet widely and willing to take entrepreneurial risks in order to turn innovative productsservices into worldwide commercial success stories the greatest challenge facing societies and firms would be utilising the benefits of availing ai technologies providing vast opportunities for both new productsservices and immense productivity improvements while avoiding the dangers and disadvantages in terms of increased unemployment and greater wealth inequalities</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2936,11 +2936,11 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.068|x2: 0.000|x3: 0.286|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.312|x9: 0.108|x10: 0.000|x11: 0.170|x12: 0.000|x13: 0.115|x14: 0.107|x15: 0.000|x16: 0.061|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.085|x2: 0.000|x3: 0.071|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.268|x9: 0.183|x10: 0.000|x11: 0.103|x12: 0.000|x13: 0.064|x14: 0.099|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.062|x4: 0.058|x5: 0.117|x6: 0.000|x7: 0.066|x8: 0.287|x9: 0.248|x10: 0.153|x11: 0.000|x12: 0.108|x13: 0.099|x14: 0.403|x15: 0.000|x16: 0.218|x17: 0.000
-TOP2VEC -&gt; x1: 0.132|x2: 0.149|x3: 0.081|x4: 0.293|x5: 0.134|x6: 0.000|x7: 0.071|x8: 0.165|x9: 0.254|x10: 0.065|x11: 0.202|x12: 0.174|x13: 0.189|x14: 0.408|x15: 0.174|x16: 0.133|x17: 0.000
-MEAN -&gt; x1: 0.067|x2: 0.050|x3: 0.143|x4: 0.117|x5: 0.084|x6: 0.000|x7: 0.046|x8: 0.255|x9: 0.203|x10: 0.073|x11: 0.124|x12: 0.094|x13: 0.134|x14: 0.306|x15: 0.058|x16: 0.138|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.061|x4: 0.059|x5: 0.057|x6: 0.052|x7: 0.055|x8: 0.068|x9: 0.064|x10: 0.056|x11: 0.059|x12: 0.058|x13: 0.060|x14: 0.071|x15: 0.056|x16: 0.060|x17: 0.052
+TOP2VEC -&gt; x1: 0.145|x2: 0.081|x3: 0.000|x4: 0.169|x5: 0.000|x6: 0.000|x7: 0.288|x8: 0.000|x9: 0.211|x10: 0.060|x11: 0.361|x12: 0.127|x13: 0.000|x14: 0.137|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.057|x2: 0.020|x3: 0.033|x4: 0.057|x5: 0.029|x6: 0.000|x7: 0.088|x8: 0.139|x9: 0.286|x10: 0.053|x11: 0.116|x12: 0.059|x13: 0.041|x14: 0.160|x15: 0.000|x16: 0.055|x17: 0.000
 </t>
         </is>
       </c>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Market abuse has attracted much attention from financial regulators around the world but it is difficult to fully prevent. One of the reasons is the lack of thoroughly studies of the market abuse strategies and the corresponding effective market abuse approaches. In this paper, the strategies of reported price manipulation cases are analysed as well as the related empirical studies. A transformation is then defined to convert the time-varying financial trading data into pseudostationary time series, where machine learning algorithms can be easily applied to the detection of the price manipulation. The evaluation experiments conducted on four stocks from NASDAQ show a promising improved performance for effectively detecting such manipulation cases. I.</t>
+          <t xml:space="preserve"> market abuse has attracted much attention from financial regulators around the world but it is difficult to fully prevent. one of the reasons is the lack of thoroughly studies of the market abuse strategies and the corresponding effective market abuse approaches. in this paper, the strategies of reported price manipulation cases are analysed as well as the related empirical studies. a transformation is then defined to convert the time varying financial trading data into pseudostationary time series, where machine learning algorithms can be easily applied to the detection of the price manipulation. the evaluation experiments conducted on four stocks from nasdaq show a promising improved performance for effectively detecting such manipulation cases. i.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2961,16 +2961,16 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>[3, 8]</t>
+          <t>[4, 8, 10, 16]</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.448|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.114|x9: 0.000|x10: 0.000|x11: 0.259|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.141|x3: 0.000|x4: 0.072|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.155|x9: 0.094|x10: 0.000|x11: 0.090|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.070|x17: 0.000
 LDA -&gt; x1: 0.135|x2: 0.253|x3: 0.118|x4: 0.220|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.427|x9: 0.000|x10: 0.386|x11: 0.000|x12: 0.000|x13: 0.193|x14: 0.087|x15: 0.000|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.056|x2: 0.000|x3: 0.170|x4: 0.278|x5: 0.342|x6: 0.095|x7: 0.222|x8: 0.090|x9: 0.110|x10: 0.081|x11: 0.057|x12: 0.323|x13: 0.000|x14: 0.114|x15: 0.140|x16: 0.165|x17: 0.000
-MEAN -&gt; x1: 0.063|x2: 0.084|x3: 0.246|x4: 0.166|x5: 0.114|x6: 0.032|x7: 0.074|x8: 0.210|x9: 0.037|x10: 0.156|x11: 0.105|x12: 0.108|x13: 0.064|x14: 0.067|x15: 0.047|x16: 0.055|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.058|x3: 0.068|x4: 0.063|x5: 0.060|x6: 0.055|x7: 0.057|x8: 0.066|x9: 0.055|x10: 0.062|x11: 0.059|x12: 0.059|x13: 0.057|x14: 0.057|x15: 0.056|x16: 0.056|x17: 0.053
+TOP2VEC -&gt; x1: 0.256|x2: 0.000|x3: 0.164|x4: 0.289|x5: 0.146|x6: 0.000|x7: 0.101|x8: 0.186|x9: 0.000|x10: 0.312|x11: 0.062|x12: 0.060|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.259|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.098|x2: 0.098|x3: 0.070|x4: 0.145|x5: 0.037|x6: 0.000|x7: 0.025|x8: 0.192|x9: 0.024|x10: 0.175|x11: 0.038|x12: 0.015|x13: 0.048|x14: 0.022|x15: 0.000|x16: 0.207|x17: 0.000
 </t>
         </is>
       </c>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Society is increasingly relying on data-driven predictive models for automated decision making. This is not by design, but due to the nature and noisiness of observational data, such models may systematically disadvantage people belonging to certain categories or groups, instead of relying solely on individual merits. This may happen even if the computing process is fair and well-intentioned. Discriminationaware data mining studies of how to make predictive models free from discrimination, when the historical data, on which they are built, may be biased, incomplete, or even contain past discriminatory decisions. Discrimination-aware data mining is an emerging research discipline, and there is no firm consensus yet of how to measure the performance of algorithms. The goal of this survey is to review various discrimination measures that have been used, analytically and computationally analyze their performance, and highlight implications of using one or another measure. We also describe measures from other disciplines, which have not been used for measuring discrimination, but potentially could be suitable for this purpose. This survey is primarily intended for researchers in data mining and machine learning as a step towards producing a unifying view of performance criteria when developing new algorithms for non-discriminatory predictive modeling. In addition, practitioners and policy makers could use this study when diagnosing potential discrimination by predictive models.</t>
+          <t xml:space="preserve"> society is increasingly relying on data driven predictive models for automated decision making. this is not by design, but due to the nature and noisiness of observational data, such models may systematically disadvantage people belonging to certain categories or groups, instead of relying solely on individual merits. this may happen even if the computing process is fair and well intentioned. discriminationaware data mining studies of how to make predictive models free from discrimination, when the historical data, on which they are built, may be biased, incomplete, or even contain past discriminatory decisions. discrimination aware data mining is an emerging research discipline, and there is no firm consensus yet of how to measure the performance of algorithms. the goal of this survey is to review various discrimination measures that have been used, analytically and computationally analyze their performance, and highlight implications of using one or another measure. we also describe measures from other disciplines, which have not been used for measuring discrimination, but potentially could be suitable for this purpose. this survey is primarily intended for researchers in data mining and machine learning as a step towards producing a unifying view of performance criteria when developing new algorithms for non discriminatory predictive modeling. in addition, practitioners and policy makers could use this study when diagnosing potential discrimination by predictive models.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2991,16 +2991,16 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.640|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.370|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.188|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.100|x10: 0.094|x11: 0.093|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.243|x3: 0.059|x4: 0.218|x5: 0.248|x6: 0.000|x7: 0.173|x8: 0.000|x9: 0.161|x10: 0.000|x11: 0.074|x12: 0.115|x13: 0.000|x14: 0.163|x15: 0.097|x16: 0.269|x17: 0.000
-TOP2VEC -&gt; x1: 0.143|x2: 0.103|x3: 0.103|x4: 0.310|x5: 0.265|x6: 0.000|x7: 0.296|x8: 0.155|x9: 0.138|x10: 0.096|x11: 0.132|x12: 0.080|x13: 0.216|x14: 0.114|x15: 0.000|x16: 0.197|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.115|x3: 0.221|x4: 0.176|x5: 0.171|x6: 0.000|x7: 0.156|x8: 0.052|x9: 0.100|x10: 0.032|x11: 0.192|x12: 0.065|x13: 0.072|x14: 0.092|x15: 0.032|x16: 0.156|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.060|x3: 0.066|x4: 0.063|x5: 0.063|x6: 0.053|x7: 0.062|x8: 0.056|x9: 0.059|x10: 0.055|x11: 0.064|x12: 0.057|x13: 0.057|x14: 0.058|x15: 0.055|x16: 0.062|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.139|x5: 0.122|x6: 0.000|x7: 0.194|x8: 0.145|x9: 0.213|x10: 0.077|x11: 0.166|x12: 0.322|x13: 0.000|x14: 0.129|x15: 0.000|x16: 0.182|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.061|x3: 0.015|x4: 0.089|x5: 0.264|x6: 0.000|x7: 0.092|x8: 0.036|x9: 0.118|x10: 0.043|x11: 0.083|x12: 0.109|x13: 0.000|x14: 0.073|x15: 0.024|x16: 0.113|x17: 0.000
 </t>
         </is>
       </c>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t xml:space="preserve"> On the background of the increasing amount of discriminatory challenges facing artificial intelligence applications, this paper examines the requirements that are needed to comply with European non-discrimination law to prevent discrimination in the automated online job advertising business. This paper explains under which circumstance the automated targeting of job advertisements can amount to direct or indirect discrimination. The paper concludes with technical recommendations to dismantle the dangers of automated job advertising. Various options like influencing the pre-processing of big data and altering the algorithmic models are evaluated. This paper also examines the possibilities of using techniques like data mining and machine learning to actively battle direct and indirect discrimination. The European non-discrimination directives 2000/43/EC, 2000/78/EC, and 2006/ 54/EC which prohibit direct and indirect discrimination in the field of employment on the grounds of race or ethnic origin, sex, sexual orientation, religious belief, age and disability are used as a legal framework.</t>
+          <t xml:space="preserve"> on the background of the increasing amount of discriminatory challenges facing artificial intelligence applications, this paper examines the requirements that are needed to comply with european non discrimination law to prevent discrimination in the automated online job advertising business. this paper explains under which circumstance the automated targeting of job advertisements can amount to direct or indirect discrimination. the paper concludes with technical recommendations to dismantle the dangers of automated job advertising. various options like influencing the pre processing of big data and altering the algorithmic models are evaluated. this paper also examines the possibilities of using techniques like data mining and machine learning to actively battle direct and indirect discrimination. the european non discrimination directives 2000/43/ec, 2000/78/ec, and 2006/ 54/ec which prohibit direct and indirect discrimination in the field of employment on the grounds of race or ethnic origin, sex, sexual orientation, religious belief, age and disability are used as a legal framework.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3021,16 +3021,16 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[5, 8]</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.380|x4: 0.000|x5: 0.103|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.244|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.174|x6: 0.000|x7: 0.000|x8: 0.158|x9: 0.075|x10: 0.000|x11: 0.080|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.078|x3: 0.055|x4: 0.138|x5: 0.276|x6: 0.000|x7: 0.132|x8: 0.161|x9: 0.169|x10: 0.211|x11: 0.000|x12: 0.113|x13: 0.104|x14: 0.132|x15: 0.000|x16: 0.249|x17: 0.000
-TOP2VEC -&gt; x1: 0.058|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.170|x6: 0.130|x7: 0.210|x8: 0.097|x9: 0.313|x10: 0.092|x11: 0.277|x12: 0.221|x13: 0.110|x14: 0.169|x15: 0.168|x16: 0.188|x17: 0.000
-MEAN -&gt; x1: 0.019|x2: 0.026|x3: 0.145|x4: 0.046|x5: 0.183|x6: 0.043|x7: 0.114|x8: 0.086|x9: 0.161|x10: 0.101|x11: 0.174|x12: 0.111|x13: 0.071|x14: 0.100|x15: 0.056|x16: 0.146|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.056|x5: 0.064|x6: 0.056|x7: 0.060|x8: 0.058|x9: 0.063|x10: 0.059|x11: 0.064|x12: 0.060|x13: 0.057|x14: 0.059|x15: 0.057|x16: 0.062|x17: 0.054
+TOP2VEC -&gt; x1: 0.242|x2: 0.000|x3: 0.000|x4: 0.081|x5: 0.095|x6: 0.000|x7: 0.093|x8: 0.247|x9: 0.000|x10: 0.191|x11: 0.276|x12: 0.179|x13: 0.000|x14: 0.132|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.060|x2: 0.020|x3: 0.014|x4: 0.055|x5: 0.261|x6: 0.000|x7: 0.056|x8: 0.141|x9: 0.061|x10: 0.100|x11: 0.089|x12: 0.073|x13: 0.026|x14: 0.066|x15: 0.000|x16: 0.062|x17: 0.000
 </t>
         </is>
       </c>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve"> There is a long cartographic tradition of describing cities through a focus on the characteristics of their residents. A review of the history of this type of urban social analysis highlights some persistent challenges. In this paper existing geodemographic approaches are extended through coupling the Kohonen Self-Organizing Map algorithm (SOM), a data-mining technique, with geographic information systems (GIS). This approach allows the construction of linked maps of social (attribute) and geographic space. This novel type of geodemographic classification allows ad hoc hierarchical groupings and exploration of the relationship between social similarity and geographic proximity. It allows one to filter complex demographic datasets and is capable of highlighting general social patterns while retaining the fundamental social fingerprints of a city. A dataset describing 79 attributes of the 2217 census tracts in New York City is analyzed to illustrate the technique. Pairs of social and geographic maps are formally compared using simple pattern metrics. Our analysis of New York City calls into question some assumptions about the functional form of spatial relationships that underlie many modeling and statistical techniques.</t>
+          <t xml:space="preserve"> there is a long cartographic tradition of describing cities through a focus on the characteristics of their residents. a review of the history of this type of urban social analysis highlights some persistent challenges. in this paper existing geodemographic approaches are extended through coupling the kohonen self organizing map algorithm (som), a data mining technique, with geographic information systems (gis). this approach allows the construction of linked maps of social (attribute) and geographic space. this novel type of geodemographic classification allows ad hoc hierarchical groupings and exploration of the relationship between social similarity and geographic proximity. it allows one to filter complex demographic datasets and is capable of highlighting general social patterns while retaining the fundamental social fingerprints of a city. a dataset describing 79 attributes of the 2217 census tracts in new york city is analyzed to illustrate the technique. pairs of social and geographic maps are formally compared using simple pattern metrics. our analysis of new york city calls into question some assumptions about the functional form of spatial relationships that underlie many modeling and statistical techniques.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3056,11 +3056,11 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.145|x2: 0.000|x3: 0.403|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.795|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.216|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.056|x10: 0.052|x11: 0.500|x12: 0.059|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.076|x2: 0.108|x3: 0.167|x4: 0.000|x5: 0.247|x6: 0.000|x7: 0.000|x8: 0.156|x9: 0.000|x10: 0.080|x11: 0.485|x12: 0.000|x13: 0.000|x14: 0.138|x15: 0.288|x16: 0.075|x17: 0.000
-TOP2VEC -&gt; x1: 0.186|x2: 0.247|x3: 0.000|x4: 0.322|x5: 0.257|x6: 0.220|x7: 0.377|x8: 0.212|x9: 0.180|x10: 0.086|x11: 0.446|x12: 0.472|x13: 0.240|x14: 0.253|x15: 0.306|x16: 0.177|x17: 0.000
-MEAN -&gt; x1: 0.136|x2: 0.118|x3: 0.190|x4: 0.107|x5: 0.168|x6: 0.073|x7: 0.126|x8: 0.123|x9: 0.060|x10: 0.055|x11: 0.477|x12: 0.157|x13: 0.080|x14: 0.130|x15: 0.198|x16: 0.084|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.062|x4: 0.057|x5: 0.061|x6: 0.055|x7: 0.058|x8: 0.058|x9: 0.054|x10: 0.054|x11: 0.082|x12: 0.060|x13: 0.055|x14: 0.058|x15: 0.062|x16: 0.056|x17: 0.051
+TOP2VEC -&gt; x1: 0.127|x2: 0.056|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.231|x8: 0.000|x9: 0.155|x10: 0.123|x11: 0.483|x12: 0.346|x13: 0.113|x14: 0.068|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.105|x2: 0.041|x3: 0.042|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.058|x8: 0.039|x9: 0.053|x10: 0.064|x11: 0.492|x12: 0.101|x13: 0.028|x14: 0.051|x15: 0.072|x16: 0.019|x17: 0.000
 </t>
         </is>
       </c>
@@ -3071,7 +3071,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We present AIDR (Artificial Intelligence for Disaster Response), a platform designed to perform automatic classification of crisis-related microblog communications. AIDR enables humans and machines to work together to apply human intelligence to large-scale data at high speed. The objective of AIDR is to classify messages that people post during disasters into a set of user-defined categories of information (e.g., "needs", "damage", etc.) For this purpose, the system continuously ingests data from Twitter, processes it (i.e., using machine learning classification techniques) and leverages human-participation (through crowdsourcing) in real-time. AIDR has been successfully tested to classify informative vs. non-informative tweets posted during the 2013 Pakistan Earthquake. Overall, we achieved a classification quality (measured using AUC) of 80%. AIDR is available at http://aidr.qcri.org/.</t>
+          <t xml:space="preserve"> we present aidr (artificial intelligence for disaster response), a platform designed to perform automatic classification of crisis related microblog communications. aidr enables humans and machines to work together to apply human intelligence to large scale data at high speed. the objective of aidr is to classify messages that people post during disasters into a set of user defined categories of information (e.g., "needs", "damage", etc.) for this purpose, the system continuously ingests data from twitter, processes it (i.e., using machine learning classification techniques) and leverages human participation (through crowdsourcing) in real time. aidr has been successfully tested to classify informative vs. non informative tweets posted during the 2013 pakistan earthquake. overall, we achieved a classification quality (measured using auc) of 80%. aidr is available at http://aidr.qcri.org/.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3081,16 +3081,16 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[2, 10, 13, 16]</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.523|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.335|x12: 0.000|x13: 0.103|x14: 0.000|x15: 0.000|x16: 0.094|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.132|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.124|x9: 0.000|x10: 0.000|x11: 0.123|x12: 0.000|x13: 0.153|x14: 0.000|x15: 0.000|x16: 0.166|x17: 0.000
 LDA -&gt; x1: 0.064|x2: 0.156|x3: 0.000|x4: 0.136|x5: 0.192|x6: 0.000|x7: 0.093|x8: 0.161|x9: 0.145|x10: 0.243|x11: 0.099|x12: 0.139|x13: 0.000|x14: 0.122|x15: 0.000|x16: 0.269|x17: 0.000
-TOP2VEC -&gt; x1: 0.152|x2: 0.000|x3: 0.000|x4: 0.270|x5: 0.209|x6: 0.349|x7: 0.061|x8: 0.176|x9: 0.153|x10: 0.064|x11: 0.108|x12: 0.381|x13: 0.187|x14: 0.264|x15: 0.142|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.072|x2: 0.052|x3: 0.167|x4: 0.135|x5: 0.134|x6: 0.116|x7: 0.052|x8: 0.113|x9: 0.100|x10: 0.102|x11: 0.181|x12: 0.173|x13: 0.097|x14: 0.129|x15: 0.047|x16: 0.165|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.062|x4: 0.060|x5: 0.060|x6: 0.059|x7: 0.056|x8: 0.059|x9: 0.058|x10: 0.058|x11: 0.063|x12: 0.063|x13: 0.058|x14: 0.060|x15: 0.055|x16: 0.062|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.109|x3: 0.000|x4: 0.122|x5: 0.141|x6: 0.069|x7: 0.234|x8: 0.094|x9: 0.102|x10: 0.353|x11: 0.070|x12: 0.114|x13: 0.169|x14: 0.000|x15: 0.000|x16: 0.156|x17: 0.000
+BERTOPIC -&gt; x1: 0.500|x2: 0.394|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.357|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.141|x2: 0.165|x3: 0.000|x4: 0.098|x5: 0.083|x6: 0.017|x7: 0.082|x8: 0.095|x9: 0.062|x10: 0.149|x11: 0.073|x12: 0.063|x13: 0.170|x14: 0.031|x15: 0.000|x16: 0.148|x17: 0.000
 </t>
         </is>
       </c>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper presents the results of attempt to perform modeling of SO 2 concentration in urban area in vicinity of copper smelter in Bor (Serbia), using ANFIS methodological approach. The aim of obtained model was to develop a prediction tool that will be used to calculate potential SO 2 concentration, above prescribed limitation, based on input parameters. As predictors, both technogenic and meteorological input parameters were considered. Accordingly, the dependence of SO 2 concentration was modeled as the function of wind speed, wind direction, air temperature, humidity and amount sulfur emitted from the pyrometallurgical process of sulfidic copper concentration treatment.</t>
+          <t xml:space="preserve"> this paper presents the results of attempt to perform modeling of so 2 concentration in urban area in vicinity of copper smelter in bor (serbia), using anfis methodological approach. the aim of obtained model was to develop a prediction tool that will be used to calculate potential so 2 concentration, above prescribed limitation, based on input parameters. as predictors, both technogenic and meteorological input parameters were considered. accordingly, the dependence of so 2 concentration was modeled as the function of wind speed, wind direction, air temperature, humidity and amount sulfur emitted from the pyrometallurgical process of sulfidic copper concentration treatment.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3111,16 +3111,16 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>[7, 11]</t>
+          <t>[7, 11, 13]</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.425|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.385|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.367|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.085|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.087|x2: 0.221|x3: 0.172|x4: 0.160|x5: 0.159|x6: 0.000|x7: 0.424|x8: 0.057|x9: 0.112|x10: 0.090|x11: 0.083|x12: 0.000|x13: 0.204|x14: 0.000|x15: 0.000|x16: 0.051|x17: 0.000
-TOP2VEC -&gt; x1: 0.249|x2: 0.239|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.246|x7: 0.526|x8: 0.260|x9: 0.187|x10: 0.074|x11: 0.283|x12: 0.272|x13: 0.382|x14: 0.065|x15: 0.196|x16: 0.152|x17: 0.000
-MEAN -&gt; x1: 0.112|x2: 0.153|x3: 0.199|x4: 0.053|x5: 0.053|x6: 0.082|x7: 0.308|x8: 0.106|x9: 0.100|x10: 0.055|x11: 0.250|x12: 0.091|x13: 0.195|x14: 0.022|x15: 0.065|x16: 0.068|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.061|x3: 0.064|x4: 0.055|x5: 0.055|x6: 0.057|x7: 0.071|x8: 0.058|x9: 0.058|x10: 0.055|x11: 0.067|x12: 0.057|x13: 0.064|x14: 0.054|x15: 0.056|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.106|x3: 0.000|x4: 0.000|x5: 0.088|x6: 0.000|x7: 0.500|x8: 0.000|x9: 0.210|x10: 0.184|x11: 0.350|x12: 0.295|x13: 0.409|x14: 0.157|x15: 0.065|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.089|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.365|x12: 0.000|x13: 0.159|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.044|x2: 0.082|x3: 0.043|x4: 0.040|x5: 0.062|x6: 0.000|x7: 0.231|x8: 0.014|x9: 0.080|x10: 0.068|x11: 0.291|x12: 0.074|x13: 0.193|x14: 0.039|x15: 0.038|x16: 0.013|x17: 0.000
 </t>
         </is>
       </c>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This study presents basic concepts and applications of Artificial Intelligence System (AIS) for development of intelligent transport systems in smart cities in India. With growing urbanization the government has now realized the need for developing smart cities that can cope with the challenges of urban living and also be magnets for investment in India. Transport system in smart cities should be accessible, safe, environmentally friendly, faster, comfortable and affordable without compromising the future needs. The Indian cities largely lacks of Intelligent Transport System in India and there are various problems such as inefficient public transport system, severe congestion, increasing incidence of road accidents, inadequate parking spaces and a rapidly increasing energy cost etc. Therefore, development of Intelligent Transportation System is essential for smart cities due to concerns regarding the environmental, economic, and social equity. Artificial Intelligence is a key technology to resolve these issues. Therefore, there is an urgent need to adopt Artificial Intelligence system for development of Intelligent Transport System to better understand and control its operations in smart cities. Hence, the main objective of this study is to present some basic concepts of Artificial Intelligence and its applications for development of Intelligent Transport System in smart cities in India. This study concludes that Artificial Intelligence system needs to be adopted to develop smart public transport system, intelligent traffic management and control, smart traveller information system, smart parking management and safe mobility &amp; emergency system in smart cities. It is expected that this study will pave the way for development of Intelligent Transport System in smart cities in India.</t>
+          <t xml:space="preserve"> this study presents basic concepts and applications of artificial intelligence system (ais) for development of intelligent transport systems in smart cities in india. with growing urbanization the government has now realized the need for developing smart cities that can cope with the challenges of urban living and also be magnets for investment in india. transport system in smart cities should be accessible, safe, environmentally friendly, faster, comfortable and affordable without compromising the future needs. the indian cities largely lacks of intelligent transport system in india and there are various problems such as inefficient public transport system, severe congestion, increasing incidence of road accidents, inadequate parking spaces and a rapidly increasing energy cost etc. therefore, development of intelligent transportation system is essential for smart cities due to concerns regarding the environmental, economic, and social equity. artificial intelligence is a key technology to resolve these issues. therefore, there is an urgent need to adopt artificial intelligence system for development of intelligent transport system to better understand and control its operations in smart cities. hence, the main objective of this study is to present some basic concepts of artificial intelligence and its applications for development of intelligent transport system in smart cities in india. this study concludes that artificial intelligence system needs to be adopted to develop smart public transport system, intelligent traffic management and control, smart traveller information system, smart parking management and safe mobility &amp; emergency system in smart cities. it is expected that this study will pave the way for development of intelligent transport system in smart cities in india.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3141,16 +3141,16 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>[3, 11]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.299|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.080|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.099|x3: 0.324|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.109|x8: 0.065|x9: 0.198|x10: 0.136|x11: 0.649|x12: 0.057|x13: 0.087|x14: 0.000|x15: 0.000|x16: 0.096|x17: 0.000
-TOP2VEC -&gt; x1: 0.064|x2: 0.000|x3: 0.107|x4: 0.239|x5: 0.000|x6: 0.203|x7: 0.314|x8: 0.066|x9: 0.217|x10: 0.067|x11: 0.495|x12: 0.263|x13: 0.210|x14: 0.064|x15: 0.167|x16: 0.137|x17: 0.000
-MEAN -&gt; x1: 0.021|x2: 0.033|x3: 0.243|x4: 0.080|x5: 0.000|x6: 0.068|x7: 0.141|x8: 0.044|x9: 0.138|x10: 0.068|x11: 0.498|x12: 0.106|x13: 0.099|x14: 0.021|x15: 0.056|x16: 0.078|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.055|x3: 0.067|x4: 0.057|x5: 0.053|x6: 0.057|x7: 0.061|x8: 0.055|x9: 0.061|x10: 0.057|x11: 0.087|x12: 0.059|x13: 0.058|x14: 0.054|x15: 0.056|x16: 0.057|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.079|x8: 0.000|x9: 0.067|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.099|x3: 0.324|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.109|x8: 0.065|x9: 0.198|x10: 0.136|x11: 0.500|x12: 0.057|x13: 0.087|x14: 0.000|x15: 0.000|x16: 0.096|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.104|x5: 0.000|x6: 0.116|x7: 0.218|x8: 0.000|x9: 0.099|x10: 0.000|x11: 0.364|x12: 0.197|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.025|x3: 0.081|x4: 0.026|x5: 0.000|x6: 0.029|x7: 0.101|x8: 0.016|x9: 0.091|x10: 0.034|x11: 0.466|x12: 0.063|x13: 0.022|x14: 0.000|x15: 0.000|x16: 0.024|x17: 0.000
 </t>
         </is>
       </c>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A License plate recognition (LPR) system can be divided into the following steps: preprocessing, plate region extraction, plate region thresholding, character segmentation, character recognition and post-processing. For step 2, a combination of color and shape information of plate is used and a satisfactory extraction result is achieved. For step 3, first channel is selected, then threshold is computed and finally the region is thresholded. For step 4, the character is segmented along vertical, horizontal direction and some tentative optimizations are applied. For step 5, minimum Euclidean distance based template matching is used. And for those confusing characters such as '8' &amp; 'B' and '0' &amp; 'D', a special processing is necessary. And for the final step, validity is checked by machine and manual. The experiment performed by program based on aforementioned algorithms indicates that our LPR system based on color image processing is quite quick and accurate.</t>
+          <t xml:space="preserve"> a license plate recognition (lpr) system can be divided into the following steps: preprocessing, plate region extraction, plate region thresholding, character segmentation, character recognition and post processing. for step 2, a combination of color and shape information of plate is used and a satisfactory extraction result is achieved. for step 3, first channel is selected, then threshold is computed and finally the region is thresholded. for step 4, the character is segmented along vertical, horizontal direction and some tentative optimizations are applied. for step 5, minimum euclidean distance based template matching is used. and for those confusing characters such as 8 &amp; b and 0 &amp; d, a special processing is necessary. and for the final step, validity is checked by machine and manual. the experiment performed by program based on aforementioned algorithms indicates that our lpr system based on color image processing is quite quick and accurate.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3171,16 +3171,16 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[8, 9, 12, 16]</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.351|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.209|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.181|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.218|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.000|x4: 0.099|x5: 0.000|x6: 0.000|x7: 0.132|x8: 0.314|x9: 0.227|x10: 0.077|x11: 0.069|x12: 0.116|x13: 0.000|x14: 0.468|x15: 0.000|x16: 0.196|x17: 0.000
-TOP2VEC -&gt; x1: 0.197|x2: 0.143|x3: 0.000|x4: 0.361|x5: 0.281|x6: 0.142|x7: 0.260|x8: 0.266|x9: 0.118|x10: 0.093|x11: 0.152|x12: 0.295|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.191|x17: 0.000
-MEAN -&gt; x1: 0.066|x2: 0.088|x3: 0.117|x4: 0.153|x5: 0.094|x6: 0.047|x7: 0.130|x8: 0.194|x9: 0.115|x10: 0.057|x11: 0.143|x12: 0.137|x13: 0.000|x14: 0.156|x15: 0.000|x16: 0.129|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.058|x3: 0.060|x4: 0.062|x5: 0.059|x6: 0.056|x7: 0.061|x8: 0.065|x9: 0.060|x10: 0.056|x11: 0.062|x12: 0.061|x13: 0.053|x14: 0.062|x15: 0.053|x16: 0.061|x17: 0.053
+TOP2VEC -&gt; x1: 0.246|x2: 0.236|x3: 0.000|x4: 0.087|x5: 0.068|x6: 0.124|x7: 0.286|x8: 0.359|x9: 0.295|x10: 0.275|x11: 0.136|x12: 0.327|x13: 0.075|x14: 0.076|x15: 0.000|x16: 0.154|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.062|x2: 0.090|x3: 0.000|x4: 0.046|x5: 0.017|x6: 0.031|x7: 0.104|x8: 0.214|x9: 0.131|x10: 0.088|x11: 0.051|x12: 0.165|x13: 0.019|x14: 0.136|x15: 0.000|x16: 0.213|x17: 0.000
 </t>
         </is>
       </c>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A new nonlinear artificial intelligence ensemble prediction (NAIEP) model has been developed for predicting typhoon intensity based on multiple neural networks with the same expected output and using an evolutionary genetic algorithm (GA). The model is validated with short-range forecasts of typhoon intensity in the South China Sea (SCS); results show that the NAIEP model is clearly better than the climatology and persistence (CLIPER) model for 24-h forecasts of typhoon intensity. Using identical predictors and sample cases, predictions of the genetic neural network (GNN) ensemble prediction (GNNEP) model are compared with the single-GNN prediction model, and it has been proven theoretically that the former is more accurate. Computation and analysis of the generalization capacity of GNNEP also demonstrate that the prediction of the ensemble model integrates predictions of its optimized ensemble members, so the generalization capacity of the ensemble prediction model is also enhanced. This model better addresses the "overfitting" problem that generally exists in the traditional neural network approach to practical weather prediction.</t>
+          <t xml:space="preserve"> a new nonlinear artificial intelligence ensemble prediction (naiep) model has been developed for predicting typhoon intensity based on multiple neural networks with the same expected output and using an evolutionary genetic algorithm (ga). the model is validated with short range forecasts of typhoon intensity in the south china sea (scs); results show that the naiep model is clearly better than the climatology and persistence (cliper) model for 24 h forecasts of typhoon intensity. using identical predictors and sample cases, predictions of the genetic neural network (gnn) ensemble prediction (gnnep) model are compared with the single gnn prediction model, and it has been proven theoretically that the former is more accurate. computation and analysis of the generalization capacity of gnnep also demonstrate that the prediction of the ensemble model integrates predictions of its optimized ensemble members, so the generalization capacity of the ensemble prediction model is also enhanced. this model better addresses the "overfitting" problem that generally exists in the traditional neural network approach to practical weather prediction.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3201,16 +3201,16 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>[6, 7, 9, 11]</t>
+          <t>[2, 9, 13]</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.706|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.408|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.119|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.189|x10: 0.000|x11: 0.088|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.135|x3: 0.063|x4: 0.311|x5: 0.093|x6: 0.403|x7: 0.106|x8: 0.000|x9: 0.395|x10: 0.126|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.128|x16: 0.062|x17: 0.000
-TOP2VEC -&gt; x1: 0.161|x2: 0.432|x3: 0.000|x4: 0.272|x5: 0.145|x6: 0.342|x7: 0.622|x8: 0.183|x9: 0.410|x10: 0.066|x11: 0.360|x12: 0.210|x13: 0.367|x14: 0.000|x15: 0.126|x16: 0.135|x17: 0.000
-MEAN -&gt; x1: 0.054|x2: 0.189|x3: 0.188|x4: 0.194|x5: 0.079|x6: 0.248|x7: 0.202|x8: 0.061|x9: 0.268|x10: 0.064|x11: 0.256|x12: 0.070|x13: 0.122|x14: 0.000|x15: 0.085|x16: 0.066|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.062|x4: 0.063|x5: 0.056|x6: 0.066|x7: 0.063|x8: 0.055|x9: 0.068|x10: 0.055|x11: 0.067|x12: 0.055|x13: 0.058|x14: 0.052|x15: 0.056|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.291|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.173|x8: 0.000|x9: 0.203|x10: 0.230|x11: 0.106|x12: 0.218|x13: 0.313|x14: 0.145|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.181|x2: 0.129|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.338|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.045|x2: 0.168|x3: 0.016|x4: 0.078|x5: 0.023|x6: 0.101|x7: 0.070|x8: 0.000|x9: 0.197|x10: 0.089|x11: 0.049|x12: 0.055|x13: 0.163|x14: 0.036|x15: 0.032|x16: 0.015|x17: 0.000
 </t>
         </is>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Automatic video analysis from urban surveillance cameras is a fast-emerging field based on computer vision techniques. We present here a comprehensive review of the state-of-the-art computer vision for traffic video with a critical analysis and an outlook to future research directions. This field is of increasing relevance for intelligent transport systems (ITSs). The decreasing hardware cost and, therefore, the increasing deployment of cameras have opened a wide application field for video analytics. Several monitoring objectives such as congestion, traffic rule violation, and vehicle interaction can be targeted using cameras that were typically originally installed for human operators. Systems for the detection and classification of vehicles on highways have successfully been using classical visual surveillance techniques such as background estimation and motion tracking for some time. The urban domain is more challenging with respect to traffic density, lower camera angles that lead to a high degree of occlusion, and the variety of road users. Methods from object categorization and 3-D modeling have inspired more advanced techniques to tackle these challenges. There is no commonly used data set or benchmark challenge, which makes the direct comparison of the proposed algorithms difficult. In addition, evaluation under challenging weather conditions (e.g., rain, fog, and darkness) would be desirable but is rarely performed. Future work should be directed toward robust combined detectors and classifiers for all road users, with a focus on realistic conditions during evaluation.</t>
+          <t xml:space="preserve"> automatic video analysis from urban surveillance cameras is a fast emerging field based on computer vision techniques. we present here a comprehensive review of the state of the art computer vision for traffic video with a critical analysis and an outlook to future research directions. this field is of increasing relevance for intelligent transport systems (itss). the decreasing hardware cost and, therefore, the increasing deployment of cameras have opened a wide application field for video analytics. several monitoring objectives such as congestion, traffic rule violation, and vehicle interaction can be targeted using cameras that were typically originally installed for human operators. systems for the detection and classification of vehicles on highways have successfully been using classical visual surveillance techniques such as background estimation and motion tracking for some time. the urban domain is more challenging with respect to traffic density, lower camera angles that lead to a high degree of occlusion, and the variety of road users. methods from object categorization and 3 d modeling have inspired more advanced techniques to tackle these challenges. there is no commonly used data set or benchmark challenge, which makes the direct comparison of the proposed algorithms difficult. in addition, evaluation under challenging weather conditions (e.g., rain, fog, and darkness) would be desirable but is rarely performed. future work should be directed toward robust combined detectors and classifiers for all road users, with a focus on realistic conditions during evaluation.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3236,11 +3236,11 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.614|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.529|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.116|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.079|x10: 0.000|x11: 0.433|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.063|x3: 0.280|x4: 0.163|x5: 0.181|x6: 0.000|x7: 0.111|x8: 0.073|x9: 0.111|x10: 0.059|x11: 0.287|x12: 0.000|x13: 0.204|x14: 0.053|x15: 0.157|x16: 0.080|x17: 0.000
-TOP2VEC -&gt; x1: 0.083|x2: 0.159|x3: 0.326|x4: 0.155|x5: 0.202|x6: 0.186|x7: 0.000|x8: 0.057|x9: 0.000|x10: 0.168|x11: 0.433|x12: 0.000|x13: 0.208|x14: 0.165|x15: 0.204|x16: 0.344|x17: 0.000
-MEAN -&gt; x1: 0.028|x2: 0.074|x3: 0.369|x4: 0.106|x5: 0.127|x6: 0.062|x7: 0.037|x8: 0.043|x9: 0.037|x10: 0.076|x11: 0.406|x12: 0.000|x13: 0.137|x14: 0.073|x15: 0.120|x16: 0.141|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.076|x4: 0.058|x5: 0.060|x6: 0.056|x7: 0.054|x8: 0.055|x9: 0.054|x10: 0.057|x11: 0.079|x12: 0.052|x13: 0.060|x14: 0.056|x15: 0.059|x16: 0.060|x17: 0.052
+TOP2VEC -&gt; x1: 0.088|x2: 0.000|x3: 0.286|x4: 0.079|x5: 0.173|x6: 0.073|x7: 0.149|x8: 0.000|x9: 0.000|x10: 0.140|x11: 0.202|x12: 0.148|x13: 0.160|x14: 0.000|x15: 0.000|x16: 0.140|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.022|x2: 0.016|x3: 0.170|x4: 0.060|x5: 0.088|x6: 0.018|x7: 0.065|x8: 0.018|x9: 0.048|x10: 0.050|x11: 0.355|x12: 0.037|x13: 0.091|x14: 0.013|x15: 0.039|x16: 0.055|x17: 0.000
 </t>
         </is>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t xml:space="preserve"> losses that matter most are not even captured by these statistics, because there's no way to put a dollar value on them. Engineers have been chipping away at these staggering numbers for a long time. Air bags and seat belts save tens of thousands of people a year. Supercomputers now let designers create car frames and bodies that protect the people inside by absorbing as much of the energy of a crash as possible. As a result, the number of fatalities per million miles of vehicle travel has decreased. But the ultimate solution, and the only one that will save far more lives, limbs, and money, is to keep cars from smashing into each other in the first place. That is exactly what engineers in the United States, Europe, and Japan are trying to do. They are applying advanced microprocessors, radars, high-speed ICs, and signal-processing chips and algorithms in R&amp;D programs that mark an about-face in the automotive industry: from safety systems that kick in after an accident occurs, attempting to minimize injury and damage, to ones that prevent collisions altogether. The first collision-avoidance features are already on the road, as pricey adaptive cruise control options on a small group of luxury cars. Over the next few years, these systems</t>
+          <t xml:space="preserve"> losses that matter most are not even captured by these statistics, because theres no way to put a dollar value on them. engineers have been chipping away at these staggering numbers for a long time. air bags and seat belts save tens of thousands of people a year. supercomputers now let designers create car frames and bodies that protect the people inside by absorbing as much of the energy of a crash as possible. as a result, the number of fatalities per million miles of vehicle travel has decreased. but the ultimate solution, and the only one that will save far more lives, limbs, and money, is to keep cars from smashing into each other in the first place. that is exactly what engineers in the united states, europe, and japan are trying to do. they are applying advanced microprocessors, radars, high speed ics, and signal processing chips and algorithms in r&amp;d programs that mark an about face in the automotive industry: from safety systems that kick in after an accident occurs, attempting to minimize injury and damage, to ones that prevent collisions altogether. the first collision avoidance features are already on the road, as pricey adaptive cruise control options on a small group of luxury cars. over the next few years, these systems</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3261,16 +3261,16 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>[3, 9, 11, 14]</t>
+          <t>[7, 9, 11, 13, 14]</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.283|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.220|x8: 0.000|x9: 0.176|x10: 0.000|x11: 0.143|x12: 0.000|x13: 0.000|x14: 0.067|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.167|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.260|x8: 0.000|x9: 0.185|x10: 0.000|x11: 0.131|x12: 0.000|x13: 0.000|x14: 0.072|x15: 0.088|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.174|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.124|x8: 0.072|x9: 0.467|x10: 0.000|x11: 0.145|x12: 0.099|x13: 0.202|x14: 0.368|x15: 0.000|x16: 0.168|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.189|x4: 0.257|x5: 0.296|x6: 0.162|x7: 0.000|x8: 0.074|x9: 0.330|x10: 0.122|x11: 0.493|x12: 0.350|x13: 0.106|x14: 0.392|x15: 0.250|x16: 0.249|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.215|x4: 0.086|x5: 0.099|x6: 0.054|x7: 0.115|x8: 0.049|x9: 0.325|x10: 0.041|x11: 0.261|x12: 0.150|x13: 0.103|x14: 0.276|x15: 0.083|x16: 0.139|x17: 0.000
-SOFTMAX -&gt; x1: 0.052|x2: 0.052|x3: 0.065|x4: 0.057|x5: 0.057|x6: 0.055|x7: 0.058|x8: 0.055|x9: 0.072|x10: 0.054|x11: 0.068|x12: 0.060|x13: 0.058|x14: 0.069|x15: 0.057|x16: 0.060|x17: 0.052
+TOP2VEC -&gt; x1: 0.167|x2: 0.183|x3: 0.064|x4: 0.000|x5: 0.000|x6: 0.081|x7: 0.290|x8: 0.000|x9: 0.197|x10: 0.000|x11: 0.135|x12: 0.269|x13: 0.171|x14: 0.363|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.203|x12: 0.000|x13: 0.192|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.042|x2: 0.046|x3: 0.101|x4: 0.000|x5: 0.000|x6: 0.020|x7: 0.169|x8: 0.018|x9: 0.212|x10: 0.000|x11: 0.153|x12: 0.092|x13: 0.141|x14: 0.201|x15: 0.022|x16: 0.042|x17: 0.000
 </t>
         </is>
       </c>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Harmful algal blooms, which are considered a serious environmental problem nowadays, occur in coastal waters in many parts of the world. They cause acute ecological damage and ensuing economic losses, due to fish kills and shellfish poisoning as well as public health threats posed by toxic blooms. Recently, data-driven models including machine-learning (ML) techniques have been employed to mimic dynamics of algal blooms. One of the most important steps in the application of a ML technique is the selection of significant model input variables. In the present paper, we use two extensively used ML techniques, artificial neural networks (ANN) and genetic programming (GP) for selecting the significant input variables. The efficacy of these techniques is first demonstrated on a test problem with known dependence and then they are applied to a real-world case study of water quality data from Tolo Harbour, Hong Kong. These ML techniques overcome some of the limitations of the currently used techniques for input variable selection, a review of which is also presented. The interpretation of the weights of the trained ANN and the GP evolved equations demonstrate their ability to identify the ecologically significant variables precisely. The significant variables suggested by the ML techniques also indicate chlorophyll-a (Chla) itself to be the most significant input in predicting the algal blooms, suggesting an auto-regressive nature or persistence in the algal bloom dynamics, which may be related to the long flushing time in the semi-enclosed coastal waters. The study also confirms the previous understanding that the algal blooms in coastal waters of Hong Kong often occur with a life cycle of the order of 1-2 weeks.</t>
+          <t xml:space="preserve"> harmful algal blooms, which are considered a serious environmental problem nowadays, occur in coastal waters in many parts of the world. they cause acute ecological damage and ensuing economic losses, due to fish kills and shellfish poisoning as well as public health threats posed by toxic blooms. recently, data driven models including machine learning (ml) techniques have been employed to mimic dynamics of algal blooms. one of the most important steps in the application of a ml technique is the selection of significant model input variables. in the present paper, we use two extensively used ml techniques, artificial neural networks (ann) and genetic programming (gp) for selecting the significant input variables. the efficacy of these techniques is first demonstrated on a test problem with known dependence and then they are applied to a real world case study of water quality data from tolo harbour, hong kong. these ml techniques overcome some of the limitations of the currently used techniques for input variable selection, a review of which is also presented. the interpretation of the weights of the trained ann and the gp evolved equations demonstrate their ability to identify the ecologically significant variables precisely. the significant variables suggested by the ml techniques also indicate chlorophyll a (chla) itself to be the most significant input in predicting the algal blooms, suggesting an auto regressive nature or persistence in the algal bloom dynamics, which may be related to the long flushing time in the semi enclosed coastal waters. the study also confirms the previous understanding that the algal blooms in coastal waters of hong kong often occur with a life cycle of the order of 1 2 weeks.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3291,16 +3291,16 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[6, 14]</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.491|x4: 0.000|x5: 0.000|x6: 0.253|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.284|x12: 0.000|x13: 0.000|x14: 0.178|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.157|x3: 0.000|x4: 0.127|x5: 0.237|x6: 0.133|x7: 0.000|x8: 0.158|x9: 0.093|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.673|x15: 0.133|x16: 0.110|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.303|x3: 0.076|x4: 0.210|x5: 0.202|x6: 0.147|x7: 0.197|x8: 0.144|x9: 0.177|x10: 0.089|x11: 0.186|x12: 0.101|x13: 0.094|x14: 0.302|x15: 0.000|x16: 0.182|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.153|x3: 0.189|x4: 0.112|x5: 0.146|x6: 0.177|x7: 0.066|x8: 0.101|x9: 0.090|x10: 0.030|x11: 0.156|x12: 0.034|x13: 0.031|x14: 0.327|x15: 0.044|x16: 0.097|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.062|x3: 0.064|x4: 0.059|x5: 0.061|x6: 0.063|x7: 0.056|x8: 0.058|x9: 0.058|x10: 0.054|x11: 0.062|x12: 0.055|x13: 0.054|x14: 0.073|x15: 0.055|x16: 0.058|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.089|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.069|x12: 0.000|x13: 0.000|x14: 0.226|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.157|x3: 0.000|x4: 0.127|x5: 0.237|x6: 0.133|x7: 0.000|x8: 0.158|x9: 0.093|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.133|x16: 0.110|x17: 0.000
+TOP2VEC -&gt; x1: 0.065|x2: 0.213|x3: 0.057|x4: 0.132|x5: 0.087|x6: 0.000|x7: 0.122|x8: 0.000|x9: 0.118|x10: 0.180|x11: 0.131|x12: 0.192|x13: 0.000|x14: 0.235|x15: 0.000|x16: 0.065|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.016|x2: 0.092|x3: 0.037|x4: 0.065|x5: 0.081|x6: 0.158|x7: 0.030|x8: 0.039|x9: 0.053|x10: 0.045|x11: 0.050|x12: 0.048|x13: 0.000|x14: 0.365|x15: 0.033|x16: 0.044|x17: 0.000
 </t>
         </is>
       </c>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Forest fires importantly influence our environment and lives. The ability of accurately predicting the area that may be involved in a forest fire event may help in optimizing fire management efforts. Given the complexity of the task, powerful computational tools are needed for predicting the amount of area that will be burned during a forest fire. The purpose of this study was to develop an intelligent system based on genetic programming for the prediction of burned areas, using only data related to the forest under analysis and meteorological data. We used geometric semantic genetic programming based on recently defined geometric semantic genetic operators for genetic programming. Experimental results, achieved using a database of 517 forest fire events between 2000 and 2003, showed the appropriateness of the proposed system for the prediction of the burned areas. In particular, results obtained with geometric semantic genetic programming were significantly better than those produced by standard genetic programming and other state of the art machine learning methods on both training and out-of-sample data. This study suggests that deeper investigation of genetic programming in the field of forest fires prediction may be productive. giere que investigaciones más profundas de programación genética en el campo de la predicción de los incendios forestales pueden ser productivas.</t>
+          <t xml:space="preserve"> forest fires importantly influence our environment and lives. the ability of accurately predicting the area that may be involved in a forest fire event may help in optimizing fire management efforts. given the complexity of the task, powerful computational tools are needed for predicting the amount of area that will be burned during a forest fire. the purpose of this study was to develop an intelligent system based on genetic programming for the prediction of burned areas, using only data related to the forest under analysis and meteorological data. we used geometric semantic genetic programming based on recently defined geometric semantic genetic operators for genetic programming. experimental results, achieved using a database of 517 forest fire events between 2000 and 2003, showed the appropriateness of the proposed system for the prediction of the burned areas. in particular, results obtained with geometric semantic genetic programming were significantly better than those produced by standard genetic programming and other state of the art machine learning methods on both training and out of sample data. this study suggests that deeper investigation of genetic programming in the field of forest fires prediction may be productive. giere que investigaciones más profundas de programación genética en el campo de la predicción de los incendios forestales pueden ser productivas.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3326,11 +3326,11 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.359|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.207|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.455|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.064|x2: 0.090|x3: 0.072|x4: 0.159|x5: 0.064|x6: 0.000|x7: 0.000|x8: 0.278|x9: 0.000|x10: 0.204|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.108|x15: 0.695|x16: 0.085|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.223|x3: 0.068|x4: 0.078|x5: 0.087|x6: 0.109|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.075|x11: 0.130|x12: 0.059|x13: 0.089|x14: 0.200|x15: 0.221|x16: 0.154|x17: 0.000
-MEAN -&gt; x1: 0.021|x2: 0.104|x3: 0.166|x4: 0.079|x5: 0.050|x6: 0.036|x7: 0.000|x8: 0.093|x9: 0.000|x10: 0.093|x11: 0.112|x12: 0.020|x13: 0.030|x14: 0.103|x15: 0.392|x16: 0.079|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.064|x4: 0.058|x5: 0.057|x6: 0.056|x7: 0.054|x8: 0.059|x9: 0.054|x10: 0.059|x11: 0.060|x12: 0.055|x13: 0.056|x14: 0.060|x15: 0.080|x16: 0.058|x17: 0.054
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.107|x3: 0.000|x4: 0.077|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.064|x2: 0.090|x3: 0.072|x4: 0.159|x5: 0.064|x6: 0.000|x7: 0.000|x8: 0.278|x9: 0.000|x10: 0.204|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.108|x15: 0.500|x16: 0.085|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.135|x3: 0.000|x4: 0.060|x5: 0.142|x6: 0.000|x7: 0.129|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.109|x12: 0.054|x13: 0.171|x14: 0.118|x15: 0.227|x16: 0.172|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.016|x2: 0.083|x3: 0.018|x4: 0.074|x5: 0.051|x6: 0.000|x7: 0.032|x8: 0.070|x9: 0.000|x10: 0.051|x11: 0.027|x12: 0.014|x13: 0.043|x14: 0.057|x15: 0.432|x16: 0.064|x17: 0.000
 </t>
         </is>
       </c>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t xml:space="preserve"> As pedestrians are one of the most vulnerable traffic participants, their motion prediction is of utmost importance for intelligent transportation systems. Predicting motions of pedestrians is especially hard since they move in less structured environments and have less inertia compared to road vehicles. To account for this uncertainty, we present an approach for probabilistic prediction of pedestrian motion using Markov chains. In contrast to previous work, we not only consider motion models, constraints from a semantic map, and various goals, but also explicitly adapt the prediction based on crash probabilities with other traffic participants. Also, our approach works in any situation; this is typically challenging for pure machine learning techniques that learn behaviors for a particular road section and which might consequently struggle with a different road section. The usefulness of combining the aforementioned aspects in a single approach is demonstrated by an evaluation using recordings of real pedestrians.</t>
+          <t xml:space="preserve"> as pedestrians are one of the most vulnerable traffic participants, their motion prediction is of utmost importance for intelligent transportation systems. predicting motions of pedestrians is especially hard since they move in less structured environments and have less inertia compared to road vehicles. to account for this uncertainty, we present an approach for probabilistic prediction of pedestrian motion using markov chains. in contrast to previous work, we not only consider motion models, constraints from a semantic map, and various goals, but also explicitly adapt the prediction based on crash probabilities with other traffic participants. also, our approach works in any situation; this is typically challenging for pure machine learning techniques that learn behaviors for a particular road section and which might consequently struggle with a different road section. the usefulness of combining the aforementioned aspects in a single approach is demonstrated by an evaluation using recordings of real pedestrians.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3351,16 +3351,16 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>[3, 4, 7, 11]</t>
+          <t>[3, 4, 11]</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.553|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.298|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.151|x4: 0.116|x5: 0.070|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.081|x10: 0.000|x11: 0.082|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.139|x3: 0.191|x4: 0.379|x5: 0.134|x6: 0.000|x7: 0.176|x8: 0.120|x9: 0.260|x10: 0.077|x11: 0.068|x12: 0.000|x13: 0.189|x14: 0.000|x15: 0.000|x16: 0.086|x17: 0.000
-TOP2VEC -&gt; x1: 0.256|x2: 0.193|x3: 0.168|x4: 0.387|x5: 0.292|x6: 0.275|x7: 0.487|x8: 0.300|x9: 0.217|x10: 0.082|x11: 0.284|x12: 0.335|x13: 0.275|x14: 0.081|x15: 0.065|x16: 0.168|x17: 0.000
-MEAN -&gt; x1: 0.085|x2: 0.111|x3: 0.286|x4: 0.255|x5: 0.142|x6: 0.092|x7: 0.221|x8: 0.140|x9: 0.159|x10: 0.053|x11: 0.217|x12: 0.112|x13: 0.155|x14: 0.027|x15: 0.022|x16: 0.085|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.067|x5: 0.060|x6: 0.057|x7: 0.064|x8: 0.059|x9: 0.061|x10: 0.054|x11: 0.064|x12: 0.058|x13: 0.060|x14: 0.053|x15: 0.053|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.126|x2: 0.138|x3: 0.208|x4: 0.184|x5: 0.057|x6: 0.255|x7: 0.244|x8: 0.140|x9: 0.126|x10: 0.000|x11: 0.141|x12: 0.063|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.215|x12: 0.000|x13: 0.180|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.032|x2: 0.069|x3: 0.137|x4: 0.170|x5: 0.065|x6: 0.064|x7: 0.105|x8: 0.089|x9: 0.117|x10: 0.019|x11: 0.127|x12: 0.016|x13: 0.092|x14: 0.000|x15: 0.000|x16: 0.021|x17: 0.000
 </t>
         </is>
       </c>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t xml:space="preserve"> With the recent advances in the field of artificial intelligence, an increasing number of decision-making tasks are delegated to software systems. A key requirement for the success and adoption of such systems is that users must trust system choices or even fully automated decisions. To achieve this, explanation facilities have been widely investigated as a means of establishing trust in these systems since the early years of expert systems. With today's increasingly sophisticated machine learning algorithms, new challenges in the context of explanations, accountability, and trust towards such systems constantly arise. In this work, we systematically review the literature on explanations in advice-giving systems. This is a family of systems that includes recommender systems, which is one of the most successful classes of advicegiving software in practice. We investigate the purposes of explanations as well as how they are generated, presented to users, and evaluated. As a result, we derive a novel comprehensive taxonomy of aspects to be considered when designing explanation facilities for current and future decision support systems. The taxonomy includes a variety of different facets, such as explanation objective, responsiveness, content and presentation. Moreover, we identified several challenges that remain unaddressed so far, for example related to fine-grained issues associated with the presentation of explanations and how explanation facilities are evaluated.</t>
+          <t xml:space="preserve"> with the recent advances in the field of artificial intelligence, an increasing number of decision making tasks are delegated to software systems. a key requirement for the success and adoption of such systems is that users must trust system choices or even fully automated decisions. to achieve this, explanation facilities have been widely investigated as a means of establishing trust in these systems since the early years of expert systems. with todays increasingly sophisticated machine learning algorithms, new challenges in the context of explanations, accountability, and trust towards such systems constantly arise. in this work, we systematically review the literature on explanations in advice giving systems. this is a family of systems that includes recommender systems, which is one of the most successful classes of advicegiving software in practice. we investigate the purposes of explanations as well as how they are generated, presented to users, and evaluated. as a result, we derive a novel comprehensive taxonomy of aspects to be considered when designing explanation facilities for current and future decision support systems. the taxonomy includes a variety of different facets, such as explanation objective, responsiveness, content and presentation. moreover, we identified several challenges that remain unaddressed so far, for example related to fine grained issues associated with the presentation of explanations and how explanation facilities are evaluated.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3381,16 +3381,16 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>[3, 14]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.454|x4: 0.000|x5: 0.000|x6: 0.053|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.263|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.080|x5: 0.080|x6: 0.074|x7: 0.000|x8: 0.000|x9: 0.070|x10: 0.000|x11: 0.070|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.094|x4: 0.074|x5: 0.264|x6: 0.114|x7: 0.000|x8: 0.146|x9: 0.158|x10: 0.070|x11: 0.000|x12: 0.080|x13: 0.150|x14: 0.311|x15: 0.148|x16: 0.210|x17: 0.000
-TOP2VEC -&gt; x1: 0.173|x2: 0.317|x3: 0.140|x4: 0.062|x5: 0.299|x6: 0.344|x7: 0.080|x8: 0.183|x9: 0.084|x10: 0.000|x11: 0.213|x12: 0.340|x13: 0.226|x14: 0.295|x15: 0.263|x16: 0.089|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.106|x3: 0.229|x4: 0.045|x5: 0.188|x6: 0.170|x7: 0.027|x8: 0.110|x9: 0.081|x10: 0.023|x11: 0.158|x12: 0.140|x13: 0.125|x14: 0.202|x15: 0.137|x16: 0.100|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.066|x4: 0.055|x5: 0.063|x6: 0.062|x7: 0.054|x8: 0.059|x9: 0.057|x10: 0.054|x11: 0.062|x12: 0.060|x13: 0.059|x14: 0.064|x15: 0.060|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.078|x3: 0.000|x4: 0.139|x5: 0.092|x6: 0.000|x7: 0.249|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.171|x12: 0.110|x13: 0.175|x14: 0.096|x15: 0.096|x16: 0.112|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.322|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.019|x3: 0.024|x4: 0.073|x5: 0.109|x6: 0.047|x7: 0.062|x8: 0.037|x9: 0.137|x10: 0.018|x11: 0.060|x12: 0.047|x13: 0.081|x14: 0.102|x15: 0.061|x16: 0.081|x17: 0.000
 </t>
         </is>
       </c>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rapid progress in machine learning and artificial intelligence (AI) has brought increasing attention to the potential impacts of AI technologies on society. In this paper we discuss one such potential impact: the problem of accidents in machine learning systems, defined as unintended and harmful behavior that may emerge from poor design of real-world AI systems. We present a list of five practical research problems related to accident risk, categorized according to whether the problem originates from having the wrong objective function ("avoiding side effects" and "avoiding reward hacking"), an objective function that is too expensive to evaluate frequently ("scalable supervision"), or undesirable behavior during the learning process ("safe exploration" and "distributional shift"). We review previous work in these areas as well as suggesting research directions with a focus on relevance to cutting-edge AI systems. Finally, we consider the high-level question of how to think most productively about the safety of forward-looking applications of AI.</t>
+          <t xml:space="preserve"> rapid progress in machine learning and artificial intelligence (ai) has brought increasing attention to the potential impacts of ai technologies on society. in this paper we discuss one such potential impact: the problem of accidents in machine learning systems, defined as unintended and harmful behavior that may emerge from poor design of real world ai systems. we present a list of five practical research problems related to accident risk, categorized according to whether the problem originates from having the wrong objective function ("avoiding side effects" and "avoiding reward hacking"), an objective function that is too expensive to evaluate frequently ("scalable supervision"), or undesirable behavior during the learning process ("safe exploration" and "distributional shift"). we review previous work in these areas as well as suggesting research directions with a focus on relevance to cutting edge ai systems. finally, we consider the high level question of how to think most productively about the safety of forward looking applications of ai.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3411,16 +3411,16 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>[3, 11]</t>
+          <t>[4, 11]</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.643|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.412|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.082|x4: 0.226|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.126|x10: 0.000|x11: 0.170|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.127|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.081|x2: 0.000|x3: 0.238|x4: 0.149|x5: 0.128|x6: 0.000|x7: 0.149|x8: 0.187|x9: 0.165|x10: 0.000|x11: 0.236|x12: 0.000|x13: 0.241|x14: 0.056|x15: 0.114|x16: 0.076|x17: 0.000
-TOP2VEC -&gt; x1: 0.165|x2: 0.085|x3: 0.236|x4: 0.160|x5: 0.305|x6: 0.131|x7: 0.128|x8: 0.163|x9: 0.127|x10: 0.000|x11: 0.163|x12: 0.142|x13: 0.294|x14: 0.440|x15: 0.227|x16: 0.085|x17: 0.000
-MEAN -&gt; x1: 0.082|x2: 0.028|x3: 0.325|x4: 0.103|x5: 0.144|x6: 0.044|x7: 0.092|x8: 0.117|x9: 0.097|x10: 0.000|x11: 0.271|x12: 0.047|x13: 0.178|x14: 0.165|x15: 0.114|x16: 0.054|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.054|x3: 0.073|x4: 0.058|x5: 0.061|x6: 0.055|x7: 0.058|x8: 0.059|x9: 0.058|x10: 0.053|x11: 0.069|x12: 0.055|x13: 0.063|x14: 0.062|x15: 0.059|x16: 0.055|x17: 0.053
+TOP2VEC -&gt; x1: 0.124|x2: 0.140|x3: 0.000|x4: 0.118|x5: 0.056|x6: 0.174|x7: 0.202|x8: 0.000|x9: 0.000|x10: 0.077|x11: 0.124|x12: 0.218|x13: 0.000|x14: 0.149|x15: 0.072|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.169|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.226|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.093|x2: 0.035|x3: 0.080|x4: 0.123|x5: 0.046|x6: 0.043|x7: 0.088|x8: 0.047|x9: 0.073|x10: 0.019|x11: 0.133|x12: 0.055|x13: 0.117|x14: 0.051|x15: 0.078|x16: 0.019|x17: 0.000
 </t>
         </is>
       </c>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The current globalization is faced by the challenge to meet the continuously growing worldwide demand for capital and consumer goods by simultaneously ensuring a sustainable evolvement of human existence in its social, environmental and economic dimensions. In order to cope with this challenge, industrial value creation must be geared towards sustainability. Currently, the industrial value creation in the early industrialized countries is shaped by the development towards the fourth stage of industrialization, the so-called Industry 4.0. This development provides immense opportunities for the realization of sustainable manufacturing. This paper will present a state of the art review of Industry 4.0 based on recent developments in research and practice. Subsequently, an overview of different opportunities for sustainable manufacturing in Industry 4.0 will be presented. A use case for the retrofitting of manufacturing equipment as a specific opportunity for sustainable manufacturing in Industry 4.0 will be exemplarily outlined.</t>
+          <t xml:space="preserve"> the current globalization is faced by the challenge to meet the continuously growing worldwide demand for capital and consumer goods by simultaneously ensuring a sustainable evolvement of human existence in its social, environmental and economic dimensions. in order to cope with this challenge, industrial value creation must be geared towards sustainability. currently, the industrial value creation in the early industrialized countries is shaped by the development towards the fourth stage of industrialization, the so called industry 4.0. this development provides immense opportunities for the realization of sustainable manufacturing. this paper will present a state of the art review of industry 4.0 based on recent developments in research and practice. subsequently, an overview of different opportunities for sustainable manufacturing in industry 4.0 will be presented. a use case for the retrofitting of manufacturing equipment as a specific opportunity for sustainable manufacturing in industry 4.0 will be exemplarily outlined.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3446,11 +3446,11 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.196|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 1.062|x10: 0.000|x11: 0.143|x12: 0.195|x13: 0.000|x14: 0.069|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.077|x4: 0.000|x5: 0.089|x6: 0.000|x7: 0.154|x8: 0.137|x9: 0.584|x10: 0.155|x11: 0.088|x12: 0.068|x13: 0.079|x14: 0.000|x15: 0.125|x16: 0.142|x17: 0.000
-TOP2VEC -&gt; x1: 0.118|x2: 0.118|x3: 0.000|x4: 0.284|x5: 0.000|x6: 0.126|x7: 0.200|x8: 0.192|x9: 0.499|x10: 0.070|x11: 0.300|x12: 0.508|x13: 0.160|x14: 0.000|x15: 0.083|x16: 0.144|x17: 0.000
-MEAN -&gt; x1: 0.039|x2: 0.080|x3: 0.091|x4: 0.095|x5: 0.030|x6: 0.042|x7: 0.118|x8: 0.110|x9: 0.500|x10: 0.075|x11: 0.177|x12: 0.254|x13: 0.080|x14: 0.023|x15: 0.069|x16: 0.095|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.057|x4: 0.057|x5: 0.054|x6: 0.055|x7: 0.059|x8: 0.058|x9: 0.086|x10: 0.056|x11: 0.062|x12: 0.067|x13: 0.057|x14: 0.054|x15: 0.056|x16: 0.058|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.500|x10: 0.000|x11: 0.091|x12: 0.144|x13: 0.000|x14: 0.057|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.122|x3: 0.077|x4: 0.000|x5: 0.089|x6: 0.000|x7: 0.154|x8: 0.137|x9: 0.500|x10: 0.155|x11: 0.088|x12: 0.068|x13: 0.079|x14: 0.000|x15: 0.125|x16: 0.142|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.184|x8: 0.051|x9: 0.337|x10: 0.000|x11: 0.104|x12: 0.381|x13: 0.181|x14: 0.000|x15: 0.119|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.030|x3: 0.019|x4: 0.000|x5: 0.022|x6: 0.000|x7: 0.085|x8: 0.047|x9: 0.459|x10: 0.039|x11: 0.071|x12: 0.148|x13: 0.065|x14: 0.014|x15: 0.061|x16: 0.036|x17: 0.000
 </t>
         </is>
       </c>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Climate impact studies in hydrology often rely on climate change information at fine spatial resolution. However, general circulation models (GCMs), which are among the most advanced tools for estimating future climate change scenarios, operate on a coarse scale. Therefore the output from a GCM has to be downscaled to obtain the information relevant to hydrologic studies. In this paper, a support vector machine (SVM) approach is proposed for statistical downscaling of precipitation at monthly time scale. The effectiveness of this approach is illustrated through its application to meteorological sub-divisions (MSDs) in India. First, climate variables affecting spatio-temporal variation of precipitation at each MSD in India are identified. Following this, the data pertaining to the identified climate variables (predictors) at each MSD are classified using cluster analysis to form two groups, representing wet and dry seasons. For each MSD, SVM-based downscaling model (DM) is developed for season(s) with significant rainfall using principal components extracted from the predictors as input and the contemporaneous precipitation observed at the MSD as an output. The proposed DM is shown to be superior to conventional downscaling using multi-layer back-propagation artificial neural networks. Subsequently, the SVM-based DM is applied to future climate predictions from the second generation Coupled Global Climate Model (CGCM2) to obtain future projections of precipitation for the MSDs. The results are then analyzed to assess the impact of climate change on precipitation over India. It is shown that SVMs provide a promising alternative to conventional artificial neural networks for statistical downscaling, and are suitable for conducting climate impact studies.</t>
+          <t xml:space="preserve"> the climate impact studies in hydrology often rely on climate change information at fine spatial resolution. however, general circulation models (gcms), which are among the most advanced tools for estimating future climate change scenarios, operate on a coarse scale. therefore the output from a gcm has to be downscaled to obtain the information relevant to hydrologic studies. in this paper, a support vector machine (svm) approach is proposed for statistical downscaling of precipitation at monthly time scale. the effectiveness of this approach is illustrated through its application to meteorological sub divisions (msds) in india. first, climate variables affecting spatio temporal variation of precipitation at each msd in india are identified. following this, the data pertaining to the identified climate variables (predictors) at each msd are classified using cluster analysis to form two groups, representing wet and dry seasons. for each msd, svm based downscaling model (dm) is developed for season(s) with significant rainfall using principal components extracted from the predictors as input and the contemporaneous precipitation observed at the msd as an output. the proposed dm is shown to be superior to conventional downscaling using multi layer back propagation artificial neural networks. subsequently, the svm based dm is applied to future climate predictions from the second generation coupled global climate model (cgcm2) to obtain future projections of precipitation for the msds. the results are then analyzed to assess the impact of climate change on precipitation over india. it is shown that svms provide a promising alternative to conventional artificial neural networks for statistical downscaling, and are suitable for conducting climate impact studies.</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3471,16 +3471,16 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>[3, 11, 13]</t>
+          <t>[9, 13]</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.553|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.320|x12: 0.000|x13: 0.947|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.087|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.500|x14: 0.061|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.063|x3: 0.292|x4: 0.193|x5: 0.000|x6: 0.000|x7: 0.055|x8: 0.170|x9: 0.204|x10: 0.000|x11: 0.080|x12: 0.073|x13: 0.344|x14: 0.232|x15: 0.000|x16: 0.115|x17: 0.000
-TOP2VEC -&gt; x1: 0.209|x2: 0.245|x3: 0.201|x4: 0.148|x5: 0.131|x6: 0.110|x7: 0.437|x8: 0.264|x9: 0.364|x10: 0.067|x11: 0.338|x12: 0.326|x13: 0.268|x14: 0.336|x15: 0.194|x16: 0.136|x17: 0.000
-MEAN -&gt; x1: 0.070|x2: 0.102|x3: 0.331|x4: 0.114|x5: 0.044|x6: 0.037|x7: 0.164|x8: 0.145|x9: 0.189|x10: 0.022|x11: 0.246|x12: 0.133|x13: 0.371|x14: 0.189|x15: 0.065|x16: 0.084|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.071|x4: 0.057|x5: 0.053|x6: 0.053|x7: 0.060|x8: 0.059|x9: 0.062|x10: 0.052|x11: 0.065|x12: 0.058|x13: 0.074|x14: 0.062|x15: 0.055|x16: 0.056|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.082|x5: 0.000|x6: 0.000|x7: 0.228|x8: 0.000|x9: 0.223|x10: 0.107|x11: 0.262|x12: 0.286|x13: 0.231|x14: 0.074|x15: 0.128|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.130|x2: 0.093|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.500|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.032|x2: 0.039|x3: 0.073|x4: 0.069|x5: 0.000|x6: 0.000|x7: 0.071|x8: 0.043|x9: 0.128|x10: 0.027|x11: 0.086|x12: 0.090|x13: 0.394|x14: 0.092|x15: 0.032|x16: 0.029|x17: 0.000
 </t>
         </is>
       </c>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A fully automated system for the identification of possible oil spills present on Synthetic Aperture Radar (SAR) satellite images based on artificial intelligence fuzzy logic has been developed. Oil spills are recognized by experts as dark patterns of characteristic shape, in particular context. The system analyzes the satellite images and assigns the probability of a dark image shape to be an oil spill. The output consists of several images and tables providing the user with all relevant information for decision-making. The case study area was the Aegean Sea in Greece. The system responded very satisfactorily for all 35 images processed. The complete algorithmic procedure was coded in MS Visual CCC 6.0 in a stand-alone dynamic link library (dll) to be linked with any sort of application under any variant of MS Windows operating system.</t>
+          <t xml:space="preserve"> a fully automated system for the identification of possible oil spills present on synthetic aperture radar (sar) satellite images based on artificial intelligence fuzzy logic has been developed. oil spills are recognized by experts as dark patterns of characteristic shape, in particular context. the system analyzes the satellite images and assigns the probability of a dark image shape to be an oil spill. the output consists of several images and tables providing the user with all relevant information for decision making. the case study area was the aegean sea in greece. the system responded very satisfactorily for all 35 images processed. the complete algorithmic procedure was coded in ms visual ccc 6.0 in a stand alone dynamic link library (dll) to be linked with any sort of application under any variant of ms windows operating system.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3501,16 +3501,16 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>[4, 11, 12, 14]</t>
+          <t>[6, 9, 12, 14]</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.452|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.261|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.115|x10: 0.117|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.108|x15: 0.165|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.099|x4: 0.194|x5: 0.000|x6: 0.000|x7: 0.093|x8: 0.156|x9: 0.345|x10: 0.000|x11: 0.000|x12: 0.165|x13: 0.156|x14: 0.391|x15: 0.000|x16: 0.222|x17: 0.000
-TOP2VEC -&gt; x1: 0.171|x2: 0.194|x3: 0.000|x4: 0.412|x5: 0.235|x6: 0.544|x7: 0.358|x8: 0.160|x9: 0.169|x10: 0.064|x11: 0.399|x12: 0.478|x13: 0.363|x14: 0.338|x15: 0.075|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.065|x3: 0.184|x4: 0.202|x5: 0.078|x6: 0.167|x7: 0.151|x8: 0.105|x9: 0.171|x10: 0.021|x11: 0.220|x12: 0.214|x13: 0.173|x14: 0.243|x15: 0.025|x16: 0.118|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.062|x4: 0.063|x5: 0.056|x6: 0.061|x7: 0.060|x8: 0.057|x9: 0.061|x10: 0.053|x11: 0.064|x12: 0.064|x13: 0.061|x14: 0.066|x15: 0.053|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.072|x5: 0.115|x6: 0.195|x7: 0.348|x8: 0.000|x9: 0.143|x10: 0.000|x11: 0.329|x12: 0.379|x13: 0.247|x14: 0.226|x15: 0.118|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.025|x4: 0.067|x5: 0.029|x6: 0.174|x7: 0.110|x8: 0.039|x9: 0.151|x10: 0.029|x11: 0.082|x12: 0.136|x13: 0.101|x14: 0.181|x15: 0.071|x16: 0.056|x17: 0.000
 </t>
         </is>
       </c>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Understanding the specific relationships between ecological and socioeconomic conditions and marine tenure is likely to contribute to successful functioning of self-governance institutions for common-pool resources. Complex interrelationships of factors influencing fishing activities of coastal communities and implementation of customary marine tenure over their waters can be represented in a Bayesian belief network model. We developed a Bayesian belief network model that includes the links between factors for fishing communities in the Kei Islands in Indonesia, based on indepth local surveys. Our results showed that the cumulative impacts of multiple factors on key social, economic, and environmental outcomes can be much larger than the impact from a single source, which implies that management or policy intervention could be more effective when addressing multiple factors simultaneously. The local community's perception of fish stock abundance trends was the single most important factor influencing social, economic, and environmental outcomes of their community-based management system. The frequency of which outsiders were sighted in territorial waters was strongly (negatively) linked to weak or strong implementation of a customary tenure (Sasi) and the occurrence of intervillage and intravillage conflict. Ecological variables also drive these conflicts, which illustrates the close connection between ecological and social outcomes, and the importance of considering social-ecological systems as a whole.</t>
+          <t xml:space="preserve"> understanding the specific relationships between ecological and socioeconomic conditions and marine tenure is likely to contribute to successful functioning of self governance institutions for common pool resources. complex interrelationships of factors influencing fishing activities of coastal communities and implementation of customary marine tenure over their waters can be represented in a bayesian belief network model. we developed a bayesian belief network model that includes the links between factors for fishing communities in the kei islands in indonesia, based on indepth local surveys. our results showed that the cumulative impacts of multiple factors on key social, economic, and environmental outcomes can be much larger than the impact from a single source, which implies that management or policy intervention could be more effective when addressing multiple factors simultaneously. the local communitys perception of fish stock abundance trends was the single most important factor influencing social, economic, and environmental outcomes of their community based management system. the frequency of which outsiders were sighted in territorial waters was strongly (negatively) linked to weak or strong implementation of a customary tenure (sasi) and the occurrence of intervillage and intravillage conflict. ecological variables also drive these conflicts, which illustrates the close connection between ecological and social outcomes, and the importance of considering social ecological systems as a whole.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3531,16 +3531,16 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>[11, 14]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.121|x2: 0.000|x3: 0.359|x4: 0.000|x5: 0.000|x6: 0.217|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.208|x12: 0.000|x13: 0.000|x14: 0.541|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.147|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.285|x7: 0.000|x8: 0.000|x9: 0.111|x10: 0.000|x11: 0.070|x12: 0.086|x13: 0.000|x14: 0.418|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.158|x2: 0.184|x3: 0.101|x4: 0.081|x5: 0.125|x6: 0.172|x7: 0.077|x8: 0.000|x9: 0.289|x10: 0.000|x11: 0.104|x12: 0.000|x13: 0.119|x14: 0.344|x15: 0.000|x16: 0.065|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.186|x3: 0.000|x4: 0.226|x5: 0.226|x6: 0.210|x7: 0.328|x8: 0.123|x9: 0.181|x10: 0.064|x11: 0.298|x12: 0.259|x13: 0.269|x14: 0.449|x15: 0.093|x16: 0.130|x17: 0.000
-MEAN -&gt; x1: 0.134|x2: 0.124|x3: 0.154|x4: 0.103|x5: 0.117|x6: 0.200|x7: 0.135|x8: 0.041|x9: 0.157|x10: 0.021|x11: 0.203|x12: 0.086|x13: 0.129|x14: 0.431|x15: 0.031|x16: 0.065|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.060|x4: 0.057|x5: 0.058|x6: 0.063|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.053|x11: 0.063|x12: 0.056|x13: 0.059|x14: 0.079|x15: 0.053|x16: 0.055|x17: 0.052
+TOP2VEC -&gt; x1: 0.107|x2: 0.000|x3: 0.000|x4: 0.104|x5: 0.069|x6: 0.000|x7: 0.177|x8: 0.000|x9: 0.000|x10: 0.087|x11: 0.084|x12: 0.131|x13: 0.143|x14: 0.274|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.103|x2: 0.046|x3: 0.025|x4: 0.046|x5: 0.049|x6: 0.114|x7: 0.063|x8: 0.000|x9: 0.100|x10: 0.022|x11: 0.065|x12: 0.054|x13: 0.065|x14: 0.384|x15: 0.000|x16: 0.016|x17: 0.000
 </t>
         </is>
       </c>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Wallis, Alofi, and Futuna are three small islands in the central Pacific Ocean, characterized by different reef geomorphologies. Following a request from the local Environment Service, we developed an indicative conservation plan for each island with two objectives: (1) representing 20% of the extent of each coral reef habitat within no-take areas while (2) keeping all subsistence fishing grounds open for extraction. The first objective was more ambitious than the current Convention on Biological Diversity (Aichi) targets. We found that both objectives could not be achieved simultaneously and that large compromises are needed. Due to the small size of these islands, and the dependence of local communities on coral reef resources, the fishery objective significantly limited the extent of most habitats available for conservation. The problem is exacerbated if the conservation plan uses larger conservation units and more complex habitat typologies. Our results indicate that international conservation guidelines should be carefully adapted to small Pacific islands and that incentives to make feasible the necessary reductions in available fishing grounds will probably be needed.</t>
+          <t xml:space="preserve"> wallis, alofi, and futuna are three small islands in the central pacific ocean, characterized by different reef geomorphologies. following a request from the local environment service, we developed an indicative conservation plan for each island with two objectives: (1) representing 20% of the extent of each coral reef habitat within no take areas while (2) keeping all subsistence fishing grounds open for extraction. the first objective was more ambitious than the current convention on biological diversity (aichi) targets. we found that both objectives could not be achieved simultaneously and that large compromises are needed. due to the small size of these islands, and the dependence of local communities on coral reef resources, the fishery objective significantly limited the extent of most habitats available for conservation. the problem is exacerbated if the conservation plan uses larger conservation units and more complex habitat typologies. our results indicate that international conservation guidelines should be carefully adapted to small pacific islands and that incentives to make feasible the necessary reductions in available fishing grounds will probably be needed.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3566,11 +3566,11 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.182|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.152|x11: 0.105|x12: 0.000|x13: 0.057|x14: 0.549|x15: 0.168|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.150|x4: 0.070|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.158|x9: 0.000|x10: 0.000|x11: 0.064|x12: 0.077|x13: 0.204|x14: 0.443|x15: 0.523|x16: 0.132|x17: 0.000
-TOP2VEC -&gt; x1: 0.109|x2: 0.119|x3: 0.000|x4: 0.000|x5: 0.133|x6: 0.000|x7: 0.000|x8: 0.065|x9: 0.000|x10: 0.086|x11: 0.269|x12: 0.365|x13: 0.314|x14: 0.669|x15: 0.573|x16: 0.176|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.040|x3: 0.111|x4: 0.023|x5: 0.044|x6: 0.000|x7: 0.000|x8: 0.074|x9: 0.000|x10: 0.079|x11: 0.146|x12: 0.147|x13: 0.192|x14: 0.481|x15: 0.389|x16: 0.103|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.054|x3: 0.058|x4: 0.053|x5: 0.055|x6: 0.052|x7: 0.052|x8: 0.056|x9: 0.052|x10: 0.057|x11: 0.060|x12: 0.061|x13: 0.063|x14: 0.084|x15: 0.077|x16: 0.058|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.197|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.292|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.150|x4: 0.070|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.158|x9: 0.000|x10: 0.000|x11: 0.064|x12: 0.077|x13: 0.204|x14: 0.443|x15: 0.500|x16: 0.132|x17: 0.000
+TOP2VEC -&gt; x1: 0.118|x2: 0.086|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.083|x7: 0.086|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.116|x12: 0.285|x13: 0.162|x14: 0.406|x15: 0.350|x16: 0.115|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.029|x2: 0.021|x3: 0.038|x4: 0.017|x5: 0.000|x6: 0.021|x7: 0.021|x8: 0.039|x9: 0.000|x10: 0.049|x11: 0.045|x12: 0.091|x13: 0.091|x14: 0.462|x15: 0.285|x16: 0.062|x17: 0.000
 </t>
         </is>
       </c>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The competition for marine space is a recognized challenge, and the implementation of new activities, such as those emerging from Blue Growth initiatives, may amplify this competition. The marine spatial planning (MSP) framework requires decision makers to analyse spatially explicit environmental and socio-economic data to determine where user conflicts are or might emerge and consider several potential management scenarios. In the present research, a spatially explicit Bayesian belief network (BBN) was applied for this purpose. The BBN was developed to analyse the potential reallocation of artisanal fishing effort to alternative sites due to the introduction of a new, non-take area: an offshore aquaculture site along the Basque continental shelf. The constructed model combined discrete, operational fisheries data, continuous environmental data, and expert judgment to produce fishing activity suitability maps for three different métiers (longlines, nets and traps). The BBN was run with various effort reallocation scenarios for each metier, and the best alternative fishing locations were identified based on environmental suitability, past revenue, and past fishing presence. The closure had a lesser effect on net and longline activity, displacing 10% and 7% of local fishing effort respectively. Comparatively, 50% of all local effort by traps took place within the closed grounds, and few alternative sites were identified. Nets were found to have the greatest number of alternative fishing grounds surrounding the aquaculture site. The present research demonstrates how BBNs can support spatially explicit scenario building and user-user conflict analysis for sustainable and successful ecosystem-based marine spatial planning.</t>
+          <t xml:space="preserve"> the competition for marine space is a recognized challenge, and the implementation of new activities, such as those emerging from blue growth initiatives, may amplify this competition. the marine spatial planning (msp) framework requires decision makers to analyse spatially explicit environmental and socio economic data to determine where user conflicts are or might emerge and consider several potential management scenarios. in the present research, a spatially explicit bayesian belief network (bbn) was applied for this purpose. the bbn was developed to analyse the potential reallocation of artisanal fishing effort to alternative sites due to the introduction of a new, non take area: an offshore aquaculture site along the basque continental shelf. the constructed model combined discrete, operational fisheries data, continuous environmental data, and expert judgment to produce fishing activity suitability maps for three different métiers (longlines, nets and traps). the bbn was run with various effort reallocation scenarios for each metier, and the best alternative fishing locations were identified based on environmental suitability, past revenue, and past fishing presence. the closure had a lesser effect on net and longline activity, displacing 10% and 7% of local fishing effort respectively. comparatively, 50% of all local effort by traps took place within the closed grounds, and few alternative sites were identified. nets were found to have the greatest number of alternative fishing grounds surrounding the aquaculture site. the present research demonstrates how bbns can support spatially explicit scenario building and user user conflict analysis for sustainable and successful ecosystem based marine spatial planning.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3596,11 +3596,11 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.356|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.246|x12: 0.000|x13: 0.000|x14: 0.574|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.053|x2: 0.000|x3: 0.144|x4: 0.125|x5: 0.080|x6: 0.000|x7: 0.088|x8: 0.000|x9: 0.161|x10: 0.000|x11: 0.097|x12: 0.070|x13: 0.167|x14: 0.646|x15: 0.067|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.062|x2: 0.056|x3: 0.054|x4: 0.201|x5: 0.292|x6: 0.143|x7: 0.281|x8: 0.000|x9: 0.166|x10: 0.096|x11: 0.178|x12: 0.115|x13: 0.270|x14: 0.467|x15: 0.302|x16: 0.196|x17: 0.000
-MEAN -&gt; x1: 0.038|x2: 0.019|x3: 0.185|x4: 0.109|x5: 0.124|x6: 0.048|x7: 0.123|x8: 0.000|x9: 0.109|x10: 0.032|x11: 0.174|x12: 0.061|x13: 0.146|x14: 0.489|x15: 0.123|x16: 0.106|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.053|x3: 0.063|x4: 0.058|x5: 0.059|x6: 0.055|x7: 0.059|x8: 0.052|x9: 0.058|x10: 0.054|x11: 0.062|x12: 0.056|x13: 0.061|x14: 0.085|x15: 0.059|x16: 0.058|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.059|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.095|x10: 0.000|x11: 0.126|x12: 0.072|x13: 0.000|x14: 0.472|x15: 0.080|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.053|x2: 0.000|x3: 0.144|x4: 0.125|x5: 0.080|x6: 0.000|x7: 0.088|x8: 0.000|x9: 0.161|x10: 0.000|x11: 0.097|x12: 0.070|x13: 0.167|x14: 0.500|x15: 0.067|x16: 0.122|x17: 0.000
+TOP2VEC -&gt; x1: 0.095|x2: 0.000|x3: 0.000|x4: 0.081|x5: 0.000|x6: 0.000|x7: 0.142|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.087|x12: 0.134|x13: 0.164|x14: 0.293|x15: 0.062|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.037|x2: 0.000|x3: 0.051|x4: 0.052|x5: 0.020|x6: 0.000|x7: 0.057|x8: 0.000|x9: 0.064|x10: 0.000|x11: 0.077|x12: 0.069|x13: 0.083|x14: 0.441|x15: 0.052|x16: 0.030|x17: 0.000
 </t>
         </is>
       </c>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Artificial intelligence techniques of neural network and fuzzy systems were applied as alternative methods to determine beach litter grading, based on litter surveys of the Antalya coastline (the Turkish Riviera). Litter measurements were categorized and assessed by artificial intelligence techniques, which lead to a new litter categorization system. The constructed neural network satisfactorily predicted the grading of the Antalya beaches and litter categories based on the number of litter items in the general litter category. It has been concluded that, neural networks could be used for high-speed predictions of litter items and beach grading, when the characteristics of the main litter category was determined by field studies. This can save on field effort when fast and reliable estimations of litter categories are required for management or research studies of beaches--especially those concerned with health and safety, and it has economic implications. The main advantages in using fuzzy systems are that they consider linguistic adjectival definitions, e.g. many/few, etc. As a result, additional information inherent in linguistic comments/refinements and judgments made during field studies can be incorporated in grading systems.</t>
+          <t xml:space="preserve"> artificial intelligence techniques of neural network and fuzzy systems were applied as alternative methods to determine beach litter grading, based on litter surveys of the antalya coastline (the turkish riviera). litter measurements were categorized and assessed by artificial intelligence techniques, which lead to a new litter categorization system. the constructed neural network satisfactorily predicted the grading of the antalya beaches and litter categories based on the number of litter items in the general litter category. it has been concluded that, neural networks could be used for high speed predictions of litter items and beach grading, when the characteristics of the main litter category was determined by field studies. this can save on field effort when fast and reliable estimations of litter categories are required for management or research studies of beaches especially those concerned with health and safety, and it has economic implications. the main advantages in using fuzzy systems are that they consider linguistic adjectival definitions, e.g. many/few, etc. as a result, additional information inherent in linguistic comments/refinements and judgments made during field studies can be incorporated in grading systems.</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3621,16 +3621,16 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>[3, 9, 14]</t>
+          <t>[9, 14]</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.653|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.374|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.100|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.124|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.142|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.084|x3: 0.149|x4: 0.222|x5: 0.163|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.489|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.454|x15: 0.088|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.148|x2: 0.214|x3: 0.243|x4: 0.055|x5: 0.296|x6: 0.000|x7: 0.112|x8: 0.186|x9: 0.189|x10: 0.088|x11: 0.131|x12: 0.323|x13: 0.147|x14: 0.403|x15: 0.256|x16: 0.180|x17: 0.000
-MEAN -&gt; x1: 0.049|x2: 0.099|x3: 0.297|x4: 0.092|x5: 0.153|x6: 0.000|x7: 0.094|x8: 0.062|x9: 0.226|x10: 0.029|x11: 0.168|x12: 0.108|x13: 0.049|x14: 0.286|x15: 0.115|x16: 0.060|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.058|x3: 0.071|x4: 0.058|x5: 0.061|x6: 0.052|x7: 0.058|x8: 0.056|x9: 0.066|x10: 0.054|x11: 0.062|x12: 0.058|x13: 0.055|x14: 0.070|x15: 0.059|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.061|x2: 0.137|x3: 0.000|x4: 0.062|x5: 0.000|x6: 0.000|x7: 0.138|x8: 0.000|x9: 0.114|x10: 0.143|x11: 0.148|x12: 0.082|x13: 0.235|x14: 0.332|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.015|x2: 0.055|x3: 0.062|x4: 0.071|x5: 0.041|x6: 0.000|x7: 0.077|x8: 0.000|x9: 0.182|x10: 0.036|x11: 0.037|x12: 0.020|x13: 0.059|x14: 0.357|x15: 0.022|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Predicting when and where key oceanic processes will be encountered is problematic in dynamic coastal waters where diverse physical, chemical, and biological factors interact in varied and rapidly changing combinations. Defining key processes often requires efficient sampling of specific water masses and prompt sample return for subsequent analyses. This compound challenge motivated our efforts to develop mobile autonomous process sampling (MAPS) for use with autonomous underwater vehicles (AUVs). With this system, features are recognized by artificial intelligence that integrates AUV sensor data to estimate probabilistic states for adaptive control of survey navigation and triggering of targeted water samplers. To demonstrate the utility of the MAPS/AUV system, we focused on intermediate nepheloid layers (INLs), episodic transport events that may play a role in zooplankton ecology. During multiple field tests in Monterey Bay, California, the MAPS/AUV system recognized, mapped, and sampled INLs. Invertebrate larvae contained in the water samples were subsequently characterized with molecular probes developed for high-throughput screening. Preliminary results support the hypothesis that INLs function as vehicles for episodic larval transport. Applying MAPS within a greater coastal ocean observing system permitted description of regional oceanographic dynamics that influenced the patterns and scales of INL and larval transport.</t>
+          <t xml:space="preserve"> predicting when and where key oceanic processes will be encountered is problematic in dynamic coastal waters where diverse physical, chemical, and biological factors interact in varied and rapidly changing combinations. defining key processes often requires efficient sampling of specific water masses and prompt sample return for subsequent analyses. this compound challenge motivated our efforts to develop mobile autonomous process sampling (maps) for use with autonomous underwater vehicles (auvs). with this system, features are recognized by artificial intelligence that integrates auv sensor data to estimate probabilistic states for adaptive control of survey navigation and triggering of targeted water samplers. to demonstrate the utility of the maps/auv system, we focused on intermediate nepheloid layers (inls), episodic transport events that may play a role in zooplankton ecology. during multiple field tests in monterey bay, california, the maps/auv system recognized, mapped, and sampled inls. invertebrate larvae contained in the water samples were subsequently characterized with molecular probes developed for high throughput screening. preliminary results support the hypothesis that inls function as vehicles for episodic larval transport. applying maps within a greater coastal ocean observing system permitted description of regional oceanographic dynamics that influenced the patterns and scales of inl and larval transport.</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3651,16 +3651,16 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>[6, 9, 11, 14]</t>
+          <t>[6, 9, 14]</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.403|x4: 0.000|x5: 0.000|x6: 0.445|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.266|x12: 0.000|x13: 0.000|x14: 0.283|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.100|x10: 0.000|x11: 0.145|x12: 0.000|x13: 0.000|x14: 0.244|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.103|x4: 0.081|x5: 0.059|x6: 0.112|x7: 0.129|x8: 0.083|x9: 0.266|x10: 0.112|x11: 0.000|x12: 0.061|x13: 0.122|x14: 0.375|x15: 0.196|x16: 0.120|x17: 0.000
-TOP2VEC -&gt; x1: 0.183|x2: 0.120|x3: 0.078|x4: 0.087|x5: 0.000|x6: 0.264|x7: 0.396|x8: 0.242|x9: 0.485|x10: 0.064|x11: 0.359|x12: 0.186|x13: 0.289|x14: 0.145|x15: 0.282|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.061|x2: 0.040|x3: 0.195|x4: 0.056|x5: 0.020|x6: 0.274|x7: 0.175|x8: 0.108|x9: 0.250|x10: 0.059|x11: 0.208|x12: 0.082|x13: 0.137|x14: 0.267|x15: 0.159|x16: 0.084|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.054|x3: 0.063|x4: 0.055|x5: 0.053|x6: 0.068|x7: 0.061|x8: 0.057|x9: 0.066|x10: 0.055|x11: 0.064|x12: 0.056|x13: 0.059|x14: 0.067|x15: 0.060|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.098|x6: 0.174|x7: 0.112|x8: 0.000|x9: 0.131|x10: 0.000|x11: 0.195|x12: 0.184|x13: 0.079|x14: 0.161|x15: 0.000|x16: 0.073|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.026|x4: 0.020|x5: 0.039|x6: 0.197|x7: 0.060|x8: 0.021|x9: 0.124|x10: 0.028|x11: 0.085|x12: 0.061|x13: 0.050|x14: 0.320|x15: 0.049|x16: 0.048|x17: 0.000
 </t>
         </is>
       </c>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Canada's Pacific coast is one region where there is a renewed commitment to pursue marine spatial planning (MSP). The British Columbia Marine Conservation Analysis (BCMCA) project aimed to set the stage for MSP, and was designed to provide resource managers, scientists, decision-makers, and stakeholders with a new set of resources to inform coast-wide integrated marine planning and management initiatives. Geographic Information Systems and the decision support tool Marxan were used to develop two main products: (1) an atlas of known marine ecological values and human uses; and (2) analyses of areas of conservation value and human use value. 110 biophysical datasets and 78 human use datasets were collated and refined where applicable, as identified through five ecological expert workshops, one expert review of physical marine classification and representation, and guidance from the human use data working group. Ecological data richness maps and Marxan results show the importance of nearshore and continental shelf regions. Data richness maps for the six categories of human uses show that all, except shipping and transport, are also closely linked to the shoreline and continental shelf. An example ecological Marxan solution identifying areas of conservation value overlapped human use sector footprints by percentages ranging from 92% (i.e., 92% of planning units selected by Marxan also contain commercial fisheries) to 3%. The experience of the BCMCA project has the potential to provide valuable guidance to regions seeking to jump-start planning processes by collating spatial information and carrying out exploratory analyses.</t>
+          <t xml:space="preserve"> canadas pacific coast is one region where there is a renewed commitment to pursue marine spatial planning (msp). the british columbia marine conservation analysis (bcmca) project aimed to set the stage for msp, and was designed to provide resource managers, scientists, decision makers, and stakeholders with a new set of resources to inform coast wide integrated marine planning and management initiatives. geographic information systems and the decision support tool marxan were used to develop two main products: (1) an atlas of known marine ecological values and human uses; and (2) analyses of areas of conservation value and human use value. 110 biophysical datasets and 78 human use datasets were collated and refined where applicable, as identified through five ecological expert workshops, one expert review of physical marine classification and representation, and guidance from the human use data working group. ecological data richness maps and marxan results show the importance of nearshore and continental shelf regions. data richness maps for the six categories of human uses show that all, except shipping and transport, are also closely linked to the shoreline and continental shelf. an example ecological marxan solution identifying areas of conservation value overlapped human use sector footprints by percentages ranging from 92% (i.e., 92% of planning units selected by marxan also contain commercial fisheries) to 3%. the experience of the bcmca project has the potential to provide valuable guidance to regions seeking to jump start planning processes by collating spatial information and carrying out exploratory analyses.</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3681,16 +3681,16 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>[11, 14]</t>
+          <t>[9, 11, 13, 14]</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.399|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.114|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.597|x15: 0.091|x16: 0.121|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.197|x10: 0.000|x11: 0.155|x12: 0.059|x13: 0.000|x14: 0.500|x15: 0.130|x16: 0.161|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.147|x4: 0.110|x5: 0.131|x6: 0.073|x7: 0.000|x8: 0.000|x9: 0.168|x10: 0.000|x11: 0.167|x12: 0.153|x13: 0.169|x14: 0.354|x15: 0.084|x16: 0.264|x17: 0.000
-TOP2VEC -&gt; x1: 0.159|x2: 0.301|x3: 0.000|x4: 0.212|x5: 0.171|x6: 0.000|x7: 0.212|x8: 0.140|x9: 0.195|x10: 0.065|x11: 0.173|x12: 0.319|x13: 0.398|x14: 0.461|x15: 0.420|x16: 0.132|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.100|x3: 0.182|x4: 0.107|x5: 0.101|x6: 0.024|x7: 0.071|x8: 0.047|x9: 0.159|x10: 0.022|x11: 0.203|x12: 0.157|x13: 0.189|x14: 0.438|x15: 0.198|x16: 0.172|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.057|x3: 0.062|x4: 0.057|x5: 0.057|x6: 0.053|x7: 0.055|x8: 0.054|x9: 0.060|x10: 0.052|x11: 0.063|x12: 0.060|x13: 0.062|x14: 0.080|x15: 0.063|x16: 0.061|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.260|x8: 0.000|x9: 0.162|x10: 0.108|x11: 0.171|x12: 0.223|x13: 0.410|x14: 0.193|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.037|x4: 0.027|x5: 0.033|x6: 0.018|x7: 0.065|x8: 0.000|x9: 0.132|x10: 0.027|x11: 0.123|x12: 0.109|x13: 0.145|x14: 0.387|x15: 0.054|x16: 0.106|x17: 0.000
 </t>
         </is>
       </c>
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Although conservation planning research has influenced conservation actions globally in the last two decades, successful implementation of systematic conservation plans in regions where customary marine tenure exists has been minimal. In such regions, local community knowledge and understanding of socioeconomic realities may offer the best spatially explicit information for analysis, since required socioeconomic data are not available at scales relevant to conservation planning. Here we describe the process undertaken by the Kadavu Yaubula Management Support Team, a team of researchers from The University of the South Pacific and the local communities to assess whether systematic conservation planning tools can be effectively applied and useful in a customary governance context, using a case study from Fiji. Through a participatory approach and with the aim of meeting local-scale conservation and fisheries needs, a spatial conservation planning tool, Marxan with Zones, was used to reconfigure a collection of locally designed marine protected areas in the province of Kadavu in order to achieve broader objectives. At the local scale, the real value of such tools has been in the process of identifying and conceptualising management issues, working with communities to collate data through participatory techniques, and in engaging communities in management decision making. The output and use of the tool has been of secondary value. The outcome was invaluable for developing marine protected area network design approaches that combine traditional knowledge with ecological features in a manner appropriate to a Melanesian context.</t>
+          <t xml:space="preserve"> although conservation planning research has influenced conservation actions globally in the last two decades, successful implementation of systematic conservation plans in regions where customary marine tenure exists has been minimal. in such regions, local community knowledge and understanding of socioeconomic realities may offer the best spatially explicit information for analysis, since required socioeconomic data are not available at scales relevant to conservation planning. here we describe the process undertaken by the kadavu yaubula management support team, a team of researchers from the university of the south pacific and the local communities to assess whether systematic conservation planning tools can be effectively applied and useful in a customary governance context, using a case study from fiji. through a participatory approach and with the aim of meeting local scale conservation and fisheries needs, a spatial conservation planning tool, marxan with zones, was used to reconfigure a collection of locally designed marine protected areas in the province of kadavu in order to achieve broader objectives. at the local scale, the real value of such tools has been in the process of identifying and conceptualising management issues, working with communities to collate data through participatory techniques, and in engaging communities in management decision making. the output and use of the tool has been of secondary value. the outcome was invaluable for developing marine protected area network design approaches that combine traditional knowledge with ecological features in a manner appropriate to a melanesian context.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3711,16 +3711,16 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>[14, 15]</t>
+          <t>[11, 14, 15]</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.470|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.273|x12: 0.000|x13: 0.000|x14: 0.559|x15: 0.257|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.077|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.204|x10: 0.000|x11: 0.129|x12: 0.000|x13: 0.000|x14: 0.462|x15: 0.393|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.070|x3: 0.088|x4: 0.188|x5: 0.093|x6: 0.061|x7: 0.000|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.159|x12: 0.099|x13: 0.085|x14: 0.367|x15: 0.324|x16: 0.127|x17: 0.000
-TOP2VEC -&gt; x1: 0.154|x2: 0.250|x3: 0.000|x4: 0.182|x5: 0.155|x6: 0.229|x7: 0.000|x8: 0.132|x9: 0.127|x10: 0.000|x11: 0.137|x12: 0.337|x13: 0.360|x14: 0.432|x15: 0.224|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.051|x2: 0.107|x3: 0.186|x4: 0.123|x5: 0.083|x6: 0.097|x7: 0.000|x8: 0.044|x9: 0.095|x10: 0.000|x11: 0.190|x12: 0.145|x13: 0.148|x14: 0.433|x15: 0.268|x16: 0.077|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.058|x3: 0.062|x4: 0.059|x5: 0.056|x6: 0.057|x7: 0.052|x8: 0.054|x9: 0.057|x10: 0.052|x11: 0.063|x12: 0.060|x13: 0.060|x14: 0.080|x15: 0.068|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.056|x7: 0.172|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.225|x12: 0.138|x13: 0.153|x14: 0.188|x15: 0.115|x16: 0.078|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.018|x3: 0.041|x4: 0.047|x5: 0.023|x6: 0.029|x7: 0.043|x8: 0.000|x9: 0.090|x10: 0.000|x11: 0.128|x12: 0.059|x13: 0.059|x14: 0.379|x15: 0.208|x16: 0.051|x17: 0.000
 </t>
         </is>
       </c>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The environmental and economic impacts of exotic fungal species on natural and plantation forests has been historically catastrophic. Recorded surveillance and control actions are challenging because they are costly, time-consuming, and hazardous in remote areas. Prolonged periods of testing and observation of site-based tests have limitations to verify the rapid proliferation of exotic pathogens and deterioration rates in hosts. Recent remote sensing approaches have offered fast, broad-scale and affordable surveys, and additional indicators that can complement on-ground tests. This paper proposes a framework that consolidates site-based insights and remote sensing capabilities to detect and segment deteriorations by fungal pathogens in natural and plantation forests. This approach is illustrated with an experimentation case of myrtle rust (Austropuccinia psidii) on paperbark tea trees (Melaleuca quinquenervia) in New South Wales (NSW), Australia. The method integrates unmanned aerial vehicles (UAVs), hyperspectral image sensors, and data processing algorithms using machine learning. Imagery is acquired using a Headwall Nano-Hyperspec R camera, orthorectified in Headwall SpectralView R , and processed in Python programming language using eXtreme Gradient Boosting (XGBoost), Geospatial Data Abstraction Library (GDAL) and Scikit-learn third-party libraries. In total, 11,385 samples were extracted and labelled into five classes: two classes for deterioration status and three classes for background objects. Insights reveal individual detection rates of 95% for healthy trees, 97% for deteriorated trees and a global multiclass detection rate of 97%. The methodology is versatile to be applied to additional datasets taken with different image sensors, and the processing of large datasets with freeware tools.</t>
+          <t xml:space="preserve"> the environmental and economic impacts of exotic fungal species on natural and plantation forests has been historically catastrophic. recorded surveillance and control actions are challenging because they are costly, time consuming, and hazardous in remote areas. prolonged periods of testing and observation of site based tests have limitations to verify the rapid proliferation of exotic pathogens and deterioration rates in hosts. recent remote sensing approaches have offered fast, broad scale and affordable surveys, and additional indicators that can complement on ground tests. this paper proposes a framework that consolidates site based insights and remote sensing capabilities to detect and segment deteriorations by fungal pathogens in natural and plantation forests. this approach is illustrated with an experimentation case of myrtle rust (austropuccinia psidii) on paperbark tea trees (melaleuca quinquenervia) in new south wales (nsw), australia. the method integrates unmanned aerial vehicles (uavs), hyperspectral image sensors, and data processing algorithms using machine learning. imagery is acquired using a headwall nano hyperspec r camera, orthorectified in headwall spectralview r , and processed in python programming language using extreme gradient boosting (xgboost), geospatial data abstraction library (gdal) and scikit learn third party libraries. in total, 11,385 samples were extracted and labelled into five classes: two classes for deterioration status and three classes for background objects. insights reveal individual detection rates of 95% for healthy trees, 97% for deteriorated trees and a global multiclass detection rate of 97%. the methodology is versatile to be applied to additional datasets taken with different image sensors, and the processing of large datasets with freeware tools.</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3741,16 +3741,16 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>[3, 15]</t>
+          <t>[14, 15]</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.561|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.307|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.181|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.193|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.072|x9: 0.065|x10: 0.000|x11: 0.062|x12: 0.073|x13: 0.000|x14: 0.063|x15: 0.366|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.164|x3: 0.172|x4: 0.218|x5: 0.095|x6: 0.000|x7: 0.000|x8: 0.200|x9: 0.070|x10: 0.098|x11: 0.060|x12: 0.063|x13: 0.056|x14: 0.198|x15: 0.302|x16: 0.123|x17: 0.000
-TOP2VEC -&gt; x1: 0.172|x2: 0.126|x3: 0.128|x4: 0.227|x5: 0.211|x6: 0.093|x7: 0.103|x8: 0.197|x9: 0.152|x10: 0.000|x11: 0.207|x12: 0.269|x13: 0.206|x14: 0.175|x15: 0.163|x16: 0.084|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.097|x3: 0.267|x4: 0.149|x5: 0.102|x6: 0.031|x7: 0.034|x8: 0.132|x9: 0.074|x10: 0.033|x11: 0.191|x12: 0.111|x13: 0.087|x14: 0.124|x15: 0.216|x16: 0.069|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.061|x5: 0.059|x6: 0.055|x7: 0.055|x8: 0.060|x9: 0.057|x10: 0.055|x11: 0.064|x12: 0.059|x13: 0.058|x14: 0.060|x15: 0.066|x16: 0.057|x17: 0.053
+TOP2VEC -&gt; x1: 0.167|x2: 0.000|x3: 0.064|x4: 0.110|x5: 0.000|x6: 0.108|x7: 0.063|x8: 0.054|x9: 0.099|x10: 0.000|x11: 0.063|x12: 0.187|x13: 0.083|x14: 0.324|x15: 0.178|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.042|x2: 0.041|x3: 0.107|x4: 0.082|x5: 0.024|x6: 0.027|x7: 0.016|x8: 0.081|x9: 0.058|x10: 0.025|x11: 0.046|x12: 0.081|x13: 0.035|x14: 0.146|x15: 0.337|x16: 0.031|x17: 0.000
 </t>
         </is>
       </c>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conservation planning is integral to strategic and effective operations of conservation organizations. Drawing upon biological sciences, conservation planning has historically made limited use of social data. We offer an approach for integrating data on social well-being into conservation planning that captures and places into context the spatial patterns and trends in human needs and capacities. This hierarchical approach provides a nested framework for characterizing and mapping data on social well-being in 5 domains: economic well-being, health, political empowerment, education, and culture. These 5 domains each have multiple attributes; each attribute may be characterized by one or more indicators. Through existing or novel data that display spatial and temporal heterogeneity in social well-being, conservation scientists, planners, and decision makers may measure, benchmark, map, and integrate these data within conservation planning processes. Selecting indicators and integrating these data into conservation planning is an iterative, participatory process tailored to the local context and planning goals. Social well-being data complement biophysical and threat-oriented social data within conservation planning processes to inform decisions regarding where and how to conserve biodiversity, provide a structure for exploring socioecological relationships, and to foster adaptive management. Building upon existing conservation planning methods and insights from multiple disciplines, this approach to putting people on the map can readily merge with current planning practices to facilitate more rigorous decision making.</t>
+          <t xml:space="preserve"> conservation planning is integral to strategic and effective operations of conservation organizations. drawing upon biological sciences, conservation planning has historically made limited use of social data. we offer an approach for integrating data on social well being into conservation planning that captures and places into context the spatial patterns and trends in human needs and capacities. this hierarchical approach provides a nested framework for characterizing and mapping data on social well being in 5 domains: economic well being, health, political empowerment, education, and culture. these 5 domains each have multiple attributes; each attribute may be characterized by one or more indicators. through existing or novel data that display spatial and temporal heterogeneity in social well being, conservation scientists, planners, and decision makers may measure, benchmark, map, and integrate these data within conservation planning processes. selecting indicators and integrating these data into conservation planning is an iterative, participatory process tailored to the local context and planning goals. social well being data complement biophysical and threat oriented social data within conservation planning processes to inform decisions regarding where and how to conserve biodiversity, provide a structure for exploring socioecological relationships, and to foster adaptive management. building upon existing conservation planning methods and insights from multiple disciplines, this approach to putting people on the map can readily merge with current planning practices to facilitate more rigorous decision making.</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3771,16 +3771,16 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>[3, 11, 15]</t>
+          <t>[11, 15]</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.119|x2: 0.000|x3: 0.459|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.293|x12: 0.000|x13: 0.000|x14: 0.165|x15: 0.189|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.093|x2: 0.000|x3: 0.160|x4: 0.162|x5: 0.102|x6: 0.000|x7: 0.000|x8: 0.092|x9: 0.000|x10: 0.079|x11: 0.160|x12: 0.107|x13: 0.148|x14: 0.000|x15: 0.552|x16: 0.165|x17: 0.000
-TOP2VEC -&gt; x1: 0.131|x2: 0.280|x3: 0.000|x4: 0.148|x5: 0.111|x6: 0.000|x7: 0.000|x8: 0.080|x9: 0.129|x10: 0.085|x11: 0.186|x12: 0.409|x13: 0.451|x14: 0.389|x15: 0.435|x16: 0.175|x17: 0.000
-MEAN -&gt; x1: 0.114|x2: 0.093|x3: 0.207|x4: 0.103|x5: 0.071|x6: 0.000|x7: 0.000|x8: 0.057|x9: 0.043|x10: 0.055|x11: 0.213|x12: 0.172|x13: 0.200|x14: 0.185|x15: 0.375|x16: 0.113|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.057|x3: 0.064|x4: 0.058|x5: 0.056|x6: 0.052|x7: 0.052|x8: 0.055|x9: 0.054|x10: 0.055|x11: 0.064|x12: 0.062|x13: 0.064|x14: 0.063|x15: 0.076|x16: 0.058|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.163|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.074|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.093|x10: 0.000|x11: 0.158|x12: 0.000|x13: 0.000|x14: 0.111|x15: 0.255|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.093|x2: 0.000|x3: 0.160|x4: 0.162|x5: 0.102|x6: 0.000|x7: 0.000|x8: 0.092|x9: 0.000|x10: 0.079|x11: 0.160|x12: 0.107|x13: 0.148|x14: 0.000|x15: 0.500|x16: 0.165|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.059|x10: 0.000|x11: 0.190|x12: 0.288|x13: 0.172|x14: 0.202|x15: 0.168|x16: 0.059|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.064|x2: 0.000|x3: 0.040|x4: 0.040|x5: 0.044|x6: 0.000|x7: 0.042|x8: 0.023|x9: 0.038|x10: 0.020|x11: 0.127|x12: 0.099|x13: 0.080|x14: 0.078|x15: 0.356|x16: 0.056|x17: 0.000
 </t>
         </is>
       </c>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ecoacoustic monitoring has proved to be a viable approach to capture ecological data related to animal communities. While experts can manually annotate audio samples, the analysis of large datasets can be significantly facilitated by automatic pattern recognition methods. Unsupervised learning methods, which do not require labelled data, are particularly well suited to analyse poorly documented habitats, such as tropical environments. Here we propose a new method, named Multiresolution Analysis of Acoustic Diversity (MAAD), to automate the detection of relevant structure in audio data. MAAD was designed to decompose the acoustic community into few elementary components (soundtypes) based on their time-frequency attributes. First, we used the short-time Fourier transform to detect regions of interest (ROIs) in the time-frequency domain. Then, we characterised these ROIs by (1) estimating the median frequency and (2) by running a 2D wavelet analysis at multiple scales and angles. Finally, we grouped the ROIs using a model-based subspace clustering technique so that ROIs were automatically annotated and clustered into soundtypes. To test the performance of the automatic method, we applied MAAD to two distinct tropical environments in French Guiana, a lowland high rainforest and a rock savanna, and we compared manual and automatic annotations using the adjusted Rand index. The similarity between the manual and automated partitions was high and consistent, indicating that the clusters found are intelligible and can be used for further analysis. Moreover, the weight of the features estimated by the clustering process revealed important information about the structure of the acoustic communities. In particular, the median frequency had the strongest effect on modelling the clusters and on classification performance, suggesting a role in community organisation. The number of clusters found in MAAD can be regarded as an estimation of the soundtype richness in a given environment. MAAD is a comprehensive and promising method to automatically analyse passive acoustic recordings. Combining MAAD and manual analysis would maximally exploit the strengths of both human reasoning and computer algorithms. Thereby, the composition of the acoustic community could be estimated accurately, quickly and at large scale.</t>
+          <t xml:space="preserve"> ecoacoustic monitoring has proved to be a viable approach to capture ecological data related to animal communities. while experts can manually annotate audio samples, the analysis of large datasets can be significantly facilitated by automatic pattern recognition methods. unsupervised learning methods, which do not require labelled data, are particularly well suited to analyse poorly documented habitats, such as tropical environments. here we propose a new method, named multiresolution analysis of acoustic diversity (maad), to automate the detection of relevant structure in audio data. maad was designed to decompose the acoustic community into few elementary components (soundtypes) based on their time frequency attributes. first, we used the short time fourier transform to detect regions of interest (rois) in the time frequency domain. then, we characterised these rois by (1) estimating the median frequency and (2) by running a 2d wavelet analysis at multiple scales and angles. finally, we grouped the rois using a model based subspace clustering technique so that rois were automatically annotated and clustered into soundtypes. to test the performance of the automatic method, we applied maad to two distinct tropical environments in french guiana, a lowland high rainforest and a rock savanna, and we compared manual and automatic annotations using the adjusted rand index. the similarity between the manual and automated partitions was high and consistent, indicating that the clusters found are intelligible and can be used for further analysis. moreover, the weight of the features estimated by the clustering process revealed important information about the structure of the acoustic communities. in particular, the median frequency had the strongest effect on modelling the clusters and on classification performance, suggesting a role in community organisation. the number of clusters found in maad can be regarded as an estimation of the soundtype richness in a given environment. maad is a comprehensive and promising method to automatically analyse passive acoustic recordings. combining maad and manual analysis would maximally exploit the strengths of both human reasoning and computer algorithms. thereby, the composition of the acoustic community could be estimated accurately, quickly and at large scale.</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3801,16 +3801,16 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[14, 15]</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.616|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.051|x9: 0.000|x10: 0.000|x11: 0.355|x12: 0.000|x13: 0.000|x14: 0.055|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.194|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.095|x9: 0.098|x10: 0.000|x11: 0.081|x12: 0.000|x13: 0.000|x14: 0.154|x15: 0.085|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.133|x3: 0.087|x4: 0.208|x5: 0.088|x6: 0.000|x7: 0.133|x8: 0.070|x9: 0.192|x10: 0.071|x11: 0.000|x12: 0.072|x13: 0.000|x14: 0.295|x15: 0.344|x16: 0.128|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.137|x3: 0.000|x4: 0.331|x5: 0.136|x6: 0.339|x7: 0.305|x8: 0.162|x9: 0.242|x10: 0.000|x11: 0.177|x12: 0.179|x13: 0.237|x14: 0.293|x15: 0.209|x16: 0.086|x17: 0.000
-MEAN -&gt; x1: 0.047|x2: 0.090|x3: 0.196|x4: 0.180|x5: 0.075|x6: 0.113|x7: 0.146|x8: 0.094|x9: 0.145|x10: 0.024|x11: 0.177|x12: 0.084|x13: 0.079|x14: 0.214|x15: 0.184|x16: 0.071|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.064|x4: 0.063|x5: 0.057|x6: 0.059|x7: 0.061|x8: 0.058|x9: 0.061|x10: 0.054|x11: 0.063|x12: 0.057|x13: 0.057|x14: 0.065|x15: 0.063|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.055|x3: 0.000|x4: 0.117|x5: 0.000|x6: 0.054|x7: 0.231|x8: 0.110|x9: 0.164|x10: 0.158|x11: 0.096|x12: 0.216|x13: 0.121|x14: 0.137|x15: 0.103|x16: 0.075|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.047|x3: 0.070|x4: 0.081|x5: 0.022|x6: 0.014|x7: 0.091|x8: 0.069|x9: 0.114|x10: 0.057|x11: 0.044|x12: 0.072|x13: 0.030|x14: 0.146|x15: 0.258|x16: 0.051|x17: 0.000
 </t>
         </is>
       </c>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Through extensive research, ecosystem services have been mapped using both survey-based and biophysical approaches, but comparative mapping of public values and those quantified using models has been lacking. In this paper, we mapped hot and cold spots for perceived and modeled ecosystem services by synthesizing results from a social-values mapping study of residents living near the Pike-San Isabel National Forest (PSI), located in the Southern Rocky Mountains, with corresponding biophysically modeled ecosystem services. Social-value maps for the PSI were developed using the Social Values for Ecosystem Services tool, providing statistically modeled continuous value surfaces for 12 value types, including aesthetic, biodiversity, and life-sustaining values. Biophysically modeled maps of carbon sequestration and storage, scenic viewsheds, sediment regulation, and water yield were generated using the Artificial Intelligence for Ecosystem Services tool. Hotspots for both perceived and modeled services were disproportionately located within the PSI's wilderness areas. Additionally, we used regression analysis to evaluate spatial relationships between perceived biodiversity and cultural ecosystem services and corresponding biophysical model outputs. Our goal was to determine whether publicly valued locations for aesthetic, biodiversity, and life-sustaining values relate meaningfully to results from corresponding biophysical ecosystem service models. We found weak relationships between perceived and biophysically modeled services, indicating that public perception of ecosystem service provisioning regions is limited. We believe that biophysical and social approaches to ecosystem service mapping can serve as methodological complements that can advance ecosystem services-based resource management, benefitting resource managers by showing potential locations of synergy or conflict between areas supplying ecosystem services and those valued by the public.</t>
+          <t xml:space="preserve"> through extensive research, ecosystem services have been mapped using both survey based and biophysical approaches, but comparative mapping of public values and those quantified using models has been lacking. in this paper, we mapped hot and cold spots for perceived and modeled ecosystem services by synthesizing results from a social values mapping study of residents living near the pike san isabel national forest (psi), located in the southern rocky mountains, with corresponding biophysically modeled ecosystem services. social value maps for the psi were developed using the social values for ecosystem services tool, providing statistically modeled continuous value surfaces for 12 value types, including aesthetic, biodiversity, and life sustaining values. biophysically modeled maps of carbon sequestration and storage, scenic viewsheds, sediment regulation, and water yield were generated using the artificial intelligence for ecosystem services tool. hotspots for both perceived and modeled services were disproportionately located within the psis wilderness areas. additionally, we used regression analysis to evaluate spatial relationships between perceived biodiversity and cultural ecosystem services and corresponding biophysical model outputs. our goal was to determine whether publicly valued locations for aesthetic, biodiversity, and life sustaining values relate meaningfully to results from corresponding biophysical ecosystem service models. we found weak relationships between perceived and biophysically modeled services, indicating that public perception of ecosystem service provisioning regions is limited. we believe that biophysical and social approaches to ecosystem service mapping can serve as methodological complements that can advance ecosystem services based resource management, benefitting resource managers by showing potential locations of synergy or conflict between areas supplying ecosystem services and those valued by the public.</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3831,16 +3831,16 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>[6, 11, 15]</t>
+          <t>[6, 11, 14, 15]</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.070|x2: 0.000|x3: 0.261|x4: 0.000|x5: 0.000|x6: 0.189|x7: 0.000|x8: 0.000|x9: 0.192|x10: 0.000|x11: 0.193|x12: 0.000|x13: 0.000|x14: 0.091|x15: 0.334|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.102|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.195|x7: 0.000|x8: 0.000|x9: 0.249|x10: 0.000|x11: 0.081|x12: 0.000|x13: 0.000|x14: 0.213|x15: 0.500|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.080|x2: 0.079|x3: 0.117|x4: 0.166|x5: 0.111|x6: 0.235|x7: 0.000|x8: 0.000|x9: 0.155|x10: 0.000|x11: 0.187|x12: 0.000|x13: 0.000|x14: 0.299|x15: 0.301|x16: 0.090|x17: 0.000
-TOP2VEC -&gt; x1: 0.069|x2: 0.102|x3: 0.000|x4: 0.214|x5: 0.130|x6: 0.281|x7: 0.244|x8: 0.095|x9: 0.175|x10: 0.000|x11: 0.238|x12: 0.139|x13: 0.089|x14: 0.110|x15: 0.061|x16: 0.070|x17: 0.000
-MEAN -&gt; x1: 0.073|x2: 0.061|x3: 0.126|x4: 0.127|x5: 0.080|x6: 0.235|x7: 0.081|x8: 0.032|x9: 0.174|x10: 0.000|x11: 0.206|x12: 0.046|x13: 0.030|x14: 0.167|x15: 0.232|x16: 0.053|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.060|x4: 0.060|x5: 0.057|x6: 0.067|x7: 0.057|x8: 0.055|x9: 0.063|x10: 0.053|x11: 0.065|x12: 0.056|x13: 0.055|x14: 0.063|x15: 0.067|x16: 0.056|x17: 0.053
+TOP2VEC -&gt; x1: 0.065|x2: 0.000|x3: 0.000|x4: 0.101|x5: 0.000|x6: 0.175|x7: 0.092|x8: 0.000|x9: 0.056|x10: 0.089|x11: 0.241|x12: 0.147|x13: 0.000|x14: 0.148|x15: 0.097|x16: 0.062|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.062|x2: 0.020|x3: 0.029|x4: 0.067|x5: 0.028|x6: 0.151|x7: 0.023|x8: 0.000|x9: 0.115|x10: 0.022|x11: 0.128|x12: 0.037|x13: 0.000|x14: 0.165|x15: 0.349|x16: 0.038|x17: 0.000
 </t>
         </is>
       </c>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Effective sustainable forest management for broad areas needs consistent country-wide forest inventory data. A stand-level inventory is appropriate as a minimum unit for local and regional forest management. South Korea currently produces a forest type map that contains only four categorical parameters. Stand height is a crucial forest attribute for understanding forest ecosystems that is currently missing and should be included in future forest type maps. Estimation of forest stand height is challenging in South Korea because stands exist in small and irregular patches on highly rugged terrain. In this study, we proposed stand height estimation models suitable for rugged terrain with highly mixed tree species. An arithmetic mean height was used as a target variable. Plot-level height estimation models were first developed using 20 descriptive statistics from airborne Light Detection and Ranging (LiDAR) data and three machine learning approaches-support vector regression (SVR), modified regression trees (RT) and random forest (RF). Two schemes (i.e., central plot-based (Scheme 1) and stand-based (Scheme 2)) for expanding from the plot level to the stand level were then investigated. The results showed varied performance metrics (i.e., coefficient of determination, root mean square error, and mean bias) by model for forest height estimation at the plot level. There was no statistically significant difference among the three mean plot height models (i.e., SVR, RT and RF) in terms of estimated heights and bias (p-values &gt; 0.05). The stand-level validation based on all tree measurements for three selected stands produced varied results by scheme and machine learning used. It implies that additional reference data should be used for a more thorough stand-level validation to identify statistically robust approaches in the future. Nonetheless, the research findings from this study can be used as a guide for estimating stand heights for forests in rugged terrain and with complex composition of tree species.</t>
+          <t xml:space="preserve"> effective sustainable forest management for broad areas needs consistent country wide forest inventory data. a stand level inventory is appropriate as a minimum unit for local and regional forest management. south korea currently produces a forest type map that contains only four categorical parameters. stand height is a crucial forest attribute for understanding forest ecosystems that is currently missing and should be included in future forest type maps. estimation of forest stand height is challenging in south korea because stands exist in small and irregular patches on highly rugged terrain. in this study, we proposed stand height estimation models suitable for rugged terrain with highly mixed tree species. an arithmetic mean height was used as a target variable. plot level height estimation models were first developed using 20 descriptive statistics from airborne light detection and ranging (lidar) data and three machine learning approaches support vector regression (svr), modified regression trees (rt) and random forest (rf). two schemes (i.e., central plot based (scheme 1) and stand based (scheme 2)) for expanding from the plot level to the stand level were then investigated. the results showed varied performance metrics (i.e., coefficient of determination, root mean square error, and mean bias) by model for forest height estimation at the plot level. there was no statistically significant difference among the three mean plot height models (i.e., svr, rt and rf) in terms of estimated heights and bias (p values &gt; 0.05). the stand level validation based on all tree measurements for three selected stands produced varied results by scheme and machine learning used. it implies that additional reference data should be used for a more thorough stand level validation to identify statistically robust approaches in the future. nonetheless, the research findings from this study can be used as a guide for estimating stand heights for forests in rugged terrain and with complex composition of tree species.</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3861,16 +3861,16 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>[3, 15]</t>
+          <t>[4, 15]</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.405|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.234|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.469|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.070|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.076|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.092|x2: 0.132|x3: 0.152|x4: 0.276|x5: 0.000|x6: 0.000|x7: 0.074|x8: 0.068|x9: 0.278|x10: 0.082|x11: 0.159|x12: 0.000|x13: 0.067|x14: 0.000|x15: 0.440|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.163|x2: 0.055|x3: 0.136|x4: 0.111|x5: 0.198|x6: 0.164|x7: 0.300|x8: 0.230|x9: 0.197|x10: 0.000|x11: 0.106|x12: 0.099|x13: 0.057|x14: 0.212|x15: 0.237|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.085|x2: 0.062|x3: 0.231|x4: 0.129|x5: 0.066|x6: 0.055|x7: 0.124|x8: 0.099|x9: 0.158|x10: 0.027|x11: 0.166|x12: 0.033|x13: 0.042|x14: 0.071|x15: 0.382|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.067|x4: 0.060|x5: 0.057|x6: 0.056|x7: 0.060|x8: 0.058|x9: 0.062|x10: 0.054|x11: 0.062|x12: 0.055|x13: 0.055|x14: 0.057|x15: 0.077|x16: 0.053|x17: 0.053
+TOP2VEC -&gt; x1: 0.093|x2: 0.000|x3: 0.110|x4: 0.169|x5: 0.235|x6: 0.155|x7: 0.193|x8: 0.211|x9: 0.109|x10: 0.000|x11: 0.147|x12: 0.128|x13: 0.103|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.046|x2: 0.033|x3: 0.066|x4: 0.129|x5: 0.059|x6: 0.039|x7: 0.067|x8: 0.070|x9: 0.116|x10: 0.021|x11: 0.076|x12: 0.032|x13: 0.043|x14: 0.000|x15: 0.360|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tropical forest condition has important implications for biodiversity, climate change and human needs. Structural features of forests can serve as useful indicators of forest condition and have the potential to be assessed with remotely sensed imagery, which can provide quantitative information on forest ecosystems at high temporal and spatial resolutions. Herein, we investigate the utility of remote sensing for assessing, predicting and mapping two important forest structural features, stem density and basal area, in tropical, littoral forests in southeastern Madagascar. We analysed the relationships of basal area and stem density measurements to the Normalised Difference Vegetation Index (NDVI) and radiance measurements in bands 3, 4, 5 and 7 from the Landsat Enhanced Thematic Mapper Plus (ETM+). Strong relationships were identified among all of the individual bands and field based measurements of basal area ( pb0.01) while there were weak and insignificant relationships among spectral response and stem density measurements. NDVI was not significantly correlated with basal area but was strongly and significantly correlated with stem density (r=À0.69, pb0.01) when using a subset of the data, which represented extreme values. We used an artificial neural network (ANN) to predict basal area from radiance values in bands 3, 4, 5 and 7 and to produce a predictive map of basal area for the entire forest landscape. The ANNs produced strong and significant relationships between predicted and actual measures of basal area using a jackknife method (r=0.79, pb0.01) and when using a larger data set (r=0.82, pb0.01). The map of predicted basal area produced by the ANN was assessed in relation to a pre-existing map of forest condition derived from a semiquantitative field assessment. The predictive map of basal area provided finer detail on stand structural heterogeneity, captured known climatic influences on forest structure and displayed trends of basal area associated with degree of human accessibility. These findings demonstrate the utility of ANNs for integrating satellite data from the Landsat ETM+ spectral bands 3, 4, 5 and 7 with limited field survey data to assess patterns in basal area at the landscape scale.</t>
+          <t xml:space="preserve"> tropical forest condition has important implications for biodiversity, climate change and human needs. structural features of forests can serve as useful indicators of forest condition and have the potential to be assessed with remotely sensed imagery, which can provide quantitative information on forest ecosystems at high temporal and spatial resolutions. herein, we investigate the utility of remote sensing for assessing, predicting and mapping two important forest structural features, stem density and basal area, in tropical, littoral forests in southeastern madagascar. we analysed the relationships of basal area and stem density measurements to the normalised difference vegetation index (ndvi) and radiance measurements in bands 3, 4, 5 and 7 from the landsat enhanced thematic mapper plus (etm+). strong relationships were identified among all of the individual bands and field based measurements of basal area ( pb0.01) while there were weak and insignificant relationships among spectral response and stem density measurements. ndvi was not significantly correlated with basal area but was strongly and significantly correlated with stem density (r=à0.69, pb0.01) when using a subset of the data, which represented extreme values. we used an artificial neural network (ann) to predict basal area from radiance values in bands 3, 4, 5 and 7 and to produce a predictive map of basal area for the entire forest landscape. the anns produced strong and significant relationships between predicted and actual measures of basal area using a jackknife method (r=0.79, pb0.01) and when using a larger data set (r=0.82, pb0.01). the map of predicted basal area produced by the ann was assessed in relation to a pre existing map of forest condition derived from a semiquantitative field assessment. the predictive map of basal area provided finer detail on stand structural heterogeneity, captured known climatic influences on forest structure and displayed trends of basal area associated with degree of human accessibility. these findings demonstrate the utility of anns for integrating satellite data from the landsat etm+ spectral bands 3, 4, 5 and 7 with limited field survey data to assess patterns in basal area at the landscape scale.</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3896,11 +3896,11 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.337|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.195|x12: 0.000|x13: 0.081|x14: 0.000|x15: 0.738|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.085|x3: 0.138|x4: 0.122|x5: 0.000|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.176|x10: 0.000|x11: 0.000|x12: 0.055|x13: 0.125|x14: 0.116|x15: 0.728|x16: 0.106|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.175|x5: 0.222|x6: 0.139|x7: 0.141|x8: 0.063|x9: 0.214|x10: 0.119|x11: 0.182|x12: 0.201|x13: 0.113|x14: 0.258|x15: 0.317|x16: 0.243|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.028|x3: 0.158|x4: 0.099|x5: 0.074|x6: 0.046|x7: 0.104|x8: 0.021|x9: 0.130|x10: 0.040|x11: 0.126|x12: 0.085|x13: 0.106|x14: 0.124|x15: 0.439|x16: 0.116|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.054|x3: 0.062|x4: 0.058|x5: 0.057|x6: 0.055|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.055|x11: 0.060|x12: 0.058|x13: 0.059|x14: 0.060|x15: 0.082|x16: 0.060|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.091|x10: 0.000|x11: 0.065|x12: 0.000|x13: 0.082|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.085|x3: 0.138|x4: 0.122|x5: 0.000|x6: 0.000|x7: 0.170|x8: 0.000|x9: 0.176|x10: 0.000|x11: 0.000|x12: 0.055|x13: 0.125|x14: 0.116|x15: 0.500|x16: 0.106|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.171|x5: 0.056|x6: 0.121|x7: 0.170|x8: 0.061|x9: 0.100|x10: 0.068|x11: 0.160|x12: 0.093|x13: 0.183|x14: 0.103|x15: 0.157|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.021|x3: 0.034|x4: 0.073|x5: 0.014|x6: 0.030|x7: 0.085|x8: 0.015|x9: 0.092|x10: 0.017|x11: 0.056|x12: 0.037|x13: 0.098|x14: 0.055|x15: 0.414|x16: 0.027|x17: 0.000
 </t>
         </is>
       </c>
@@ -3911,7 +3911,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marxan is the most widely used conservation planning software in the world and is designed for solving complex conservation planning problems in landscapes and seascapes. In this paper we describe a substantial extension of Marxan called Marxan with Zones, a decision support tool that provides landuse zoning options in geographical regions for biodiversity conservation. We describe new functions designed to enhance the original Marxan software and expand on its utility as a decision support tool. The major new element in the decision problem is allowing any parcel of land or sea to be allocated to a specific zone, not just reserved or unreserved. Each zone then has the option of its own actions, objectives and constraints, with the flexibility to define the contribution of each zone to achieve targets for pre-specified features (e.g. species or habitats). The objective is to minimize the total cost of implementing the zoning plan while ensuring a variety of conservation and land-use objectives are achieved. We outline the capabilities, limitations and additional data requirements of this new software and perform a comparison with the original version of Marxan. We feature a number of case studies to demonstrate the functionality of the software and highlight its flexibility to address a range of complex spatial planning problems. These studies demonstrate the design of multiple-use marine parks in both Western Australia and California, and the zoning of forest use in East Kalimantan.</t>
+          <t xml:space="preserve"> marxan is the most widely used conservation planning software in the world and is designed for solving complex conservation planning problems in landscapes and seascapes. in this paper we describe a substantial extension of marxan called marxan with zones, a decision support tool that provides landuse zoning options in geographical regions for biodiversity conservation. we describe new functions designed to enhance the original marxan software and expand on its utility as a decision support tool. the major new element in the decision problem is allowing any parcel of land or sea to be allocated to a specific zone, not just reserved or unreserved. each zone then has the option of its own actions, objectives and constraints, with the flexibility to define the contribution of each zone to achieve targets for pre specified features (e.g. species or habitats). the objective is to minimize the total cost of implementing the zoning plan while ensuring a variety of conservation and land use objectives are achieved. we outline the capabilities, limitations and additional data requirements of this new software and perform a comparison with the original version of marxan. we feature a number of case studies to demonstrate the functionality of the software and highlight its flexibility to address a range of complex spatial planning problems. these studies demonstrate the design of multiple use marine parks in both western australia and california, and the zoning of forest use in east kalimantan.</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3926,11 +3926,11 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.391|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.233|x12: 0.000|x13: 0.000|x14: 0.174|x15: 0.262|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.102|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.075|x10: 0.000|x11: 0.114|x12: 0.000|x13: 0.052|x14: 0.177|x15: 0.373|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.053|x3: 0.062|x4: 0.105|x5: 0.068|x6: 0.000|x7: 0.000|x8: 0.115|x9: 0.095|x10: 0.201|x11: 0.199|x12: 0.098|x13: 0.000|x14: 0.205|x15: 0.477|x16: 0.141|x17: 0.000
-TOP2VEC -&gt; x1: 0.149|x2: 0.183|x3: 0.000|x4: 0.070|x5: 0.000|x6: 0.249|x7: 0.168|x8: 0.133|x9: 0.214|x10: 0.054|x11: 0.346|x12: 0.450|x13: 0.384|x14: 0.464|x15: 0.353|x16: 0.111|x17: 0.000
-MEAN -&gt; x1: 0.050|x2: 0.079|x3: 0.151|x4: 0.059|x5: 0.023|x6: 0.083|x7: 0.056|x8: 0.083|x9: 0.103|x10: 0.085|x11: 0.259|x12: 0.183|x13: 0.128|x14: 0.281|x15: 0.364|x16: 0.084|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.060|x4: 0.055|x5: 0.053|x6: 0.056|x7: 0.055|x8: 0.056|x9: 0.057|x10: 0.056|x11: 0.067|x12: 0.062|x13: 0.059|x14: 0.069|x15: 0.075|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.315|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.363|x12: 0.184|x13: 0.131|x14: 0.331|x15: 0.176|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.013|x3: 0.041|x4: 0.026|x5: 0.017|x6: 0.000|x7: 0.079|x8: 0.029|x9: 0.043|x10: 0.050|x11: 0.169|x12: 0.071|x13: 0.046|x14: 0.178|x15: 0.382|x16: 0.035|x17: 0.000
 </t>
         </is>
       </c>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Despite extensive research demonstrating the benefits of applying cost-effective conservation techniques, such as optimization, a large gap remains between the evidence from research and the actions of professions as they design and implement conservation programs. This study examines this gap through an international survey of conservation professionals who are familiar with cost-effective conservation techniques. The primary results of this study, replicate previous results from a smaller sample of agricultural preservation professionals, and show that the vast majority of survey respondents viewed cost-effectiveness as a virtue, but ultimately do not consider it as important as other program design criteria. These results reinforce the idea that advocates of cost-effective conservation need to address concerns about fairness and transparency and remedy gaps in the knowledge and expertise of professionals involved. Finally, the lack of incentive to conservation professionals to change their practices is a challenge that calls for public pressure and encouragement for experimentation and evidence-based policy to improve the cost effectiveness of conservation.</t>
+          <t xml:space="preserve"> despite extensive research demonstrating the benefits of applying cost effective conservation techniques, such as optimization, a large gap remains between the evidence from research and the actions of professions as they design and implement conservation programs. this study examines this gap through an international survey of conservation professionals who are familiar with cost effective conservation techniques. the primary results of this study, replicate previous results from a smaller sample of agricultural preservation professionals, and show that the vast majority of survey respondents viewed cost effectiveness as a virtue, but ultimately do not consider it as important as other program design criteria. these results reinforce the idea that advocates of cost effective conservation need to address concerns about fairness and transparency and remedy gaps in the knowledge and expertise of professionals involved. finally, the lack of incentive to conservation professionals to change their practices is a challenge that calls for public pressure and encouragement for experimentation and evidence based policy to improve the cost effectiveness of conservation.</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3951,16 +3951,16 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>[3, 11, 14]</t>
+          <t>[11, 14, 15]</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.420|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.079|x11: 0.243|x12: 0.000|x13: 0.000|x14: 0.165|x15: 0.096|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.086|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.097|x10: 0.000|x11: 0.097|x12: 0.078|x13: 0.000|x14: 0.152|x15: 0.165|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.114|x3: 0.116|x4: 0.075|x5: 0.089|x6: 0.000|x7: 0.000|x8: 0.182|x9: 0.000|x10: 0.196|x11: 0.237|x12: 0.069|x13: 0.070|x14: 0.347|x15: 0.213|x16: 0.111|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.108|x3: 0.126|x4: 0.000|x5: 0.164|x6: 0.000|x7: 0.000|x8: 0.110|x9: 0.088|x10: 0.090|x11: 0.258|x12: 0.000|x13: 0.262|x14: 0.566|x15: 0.238|x16: 0.183|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.074|x3: 0.221|x4: 0.025|x5: 0.084|x6: 0.000|x7: 0.000|x8: 0.097|x9: 0.029|x10: 0.122|x11: 0.246|x12: 0.023|x13: 0.111|x14: 0.338|x15: 0.182|x16: 0.098|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.054|x5: 0.058|x6: 0.053|x7: 0.053|x8: 0.058|x9: 0.055|x10: 0.060|x11: 0.068|x12: 0.054|x13: 0.059|x14: 0.074|x15: 0.064|x16: 0.058|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.076|x3: 0.000|x4: 0.000|x5: 0.126|x6: 0.000|x7: 0.113|x8: 0.000|x9: 0.000|x10: 0.060|x11: 0.197|x12: 0.067|x13: 0.000|x14: 0.285|x15: 0.075|x16: 0.137|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.047|x3: 0.029|x4: 0.040|x5: 0.054|x6: 0.000|x7: 0.028|x8: 0.046|x9: 0.024|x10: 0.064|x11: 0.133|x12: 0.054|x13: 0.017|x14: 0.196|x15: 0.238|x16: 0.062|x17: 0.000
 </t>
         </is>
       </c>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Surveying threatened and invasive species to obtain accurate population estimates is an important but challenging task that requires a considerable investment in time and resources. Estimates using existing ground-based monitoring techniques, such as camera traps and surveys performed on foot, are known to be resource intensive, potentially inaccurate and imprecise, and difficult to validate. Recent developments in unmanned aerial vehicles (UAV), artificial intelligence and miniaturized thermal imaging systems represent a new opportunity for wildlife experts to inexpensively survey relatively large areas. The system presented in this paper includes thermal image acquisition as well as a video processing pipeline to perform object detection, classification and tracking of wildlife in forest or open areas. The system is tested on thermal video data from ground based and test flight footage, and is found to be able to detect all the target wildlife located in the surveyed area. The system is flexible in that the user can readily define the types of objects to classify and the object characteristics that should be considered during classification.</t>
+          <t xml:space="preserve"> surveying threatened and invasive species to obtain accurate population estimates is an important but challenging task that requires a considerable investment in time and resources. estimates using existing ground based monitoring techniques, such as camera traps and surveys performed on foot, are known to be resource intensive, potentially inaccurate and imprecise, and difficult to validate. recent developments in unmanned aerial vehicles (uav), artificial intelligence and miniaturized thermal imaging systems represent a new opportunity for wildlife experts to inexpensively survey relatively large areas. the system presented in this paper includes thermal image acquisition as well as a video processing pipeline to perform object detection, classification and tracking of wildlife in forest or open areas. the system is tested on thermal video data from ground based and test flight footage, and is found to be able to detect all the target wildlife located in the surveyed area. the system is flexible in that the user can readily define the types of objects to classify and the object characteristics that should be considered during classification.</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3981,16 +3981,16 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>[5, 11, 15]</t>
+          <t>[15]</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.454|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.270|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.264|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.104|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.061|x3: 0.000|x4: 0.094|x5: 0.125|x6: 0.000|x7: 0.113|x8: 0.150|x9: 0.251|x10: 0.151|x11: 0.097|x12: 0.000|x13: 0.000|x14: 0.241|x15: 0.437|x16: 0.100|x17: 0.000
-TOP2VEC -&gt; x1: 0.143|x2: 0.192|x3: 0.080|x4: 0.274|x5: 0.478|x6: 0.406|x7: 0.252|x8: 0.183|x9: 0.223|x10: 0.147|x11: 0.277|x12: 0.417|x13: 0.158|x14: 0.249|x15: 0.457|x16: 0.300|x17: 0.000
-MEAN -&gt; x1: 0.048|x2: 0.084|x3: 0.178|x4: 0.123|x5: 0.201|x6: 0.135|x7: 0.122|x8: 0.111|x9: 0.158|x10: 0.099|x11: 0.215|x12: 0.139|x13: 0.053|x14: 0.163|x15: 0.386|x16: 0.133|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.056|x3: 0.061|x4: 0.058|x5: 0.062|x6: 0.058|x7: 0.058|x8: 0.057|x9: 0.060|x10: 0.056|x11: 0.063|x12: 0.059|x13: 0.054|x14: 0.060|x15: 0.075|x16: 0.058|x17: 0.051
+TOP2VEC -&gt; x1: 0.296|x2: 0.096|x3: 0.000|x4: 0.115|x5: 0.101|x6: 0.000|x7: 0.111|x8: 0.000|x9: 0.000|x10: 0.120|x11: 0.128|x12: 0.226|x13: 0.063|x14: 0.173|x15: 0.089|x16: 0.187|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.074|x2: 0.039|x3: 0.000|x4: 0.052|x5: 0.056|x6: 0.000|x7: 0.056|x8: 0.037|x9: 0.063|x10: 0.068|x11: 0.082|x12: 0.057|x13: 0.016|x14: 0.104|x15: 0.382|x16: 0.072|x17: 0.000
 </t>
         </is>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Data on numbers and distribution of free-ranging giant panda are essential to the formulation of effective conservation strategies. There is still no ideal method to identify individuals and sex this species. The traditional bite-size method using bamboo fragments in their feces lacks accuracy. The modern DNA-based estimation is expensive and demands fresh samples. The lack of identifiable individual features on panda pelage and no apparent sexual dimorphism impede reliable estimation from camera trap images. Here, we propose an innovative and non-invasive technique to identify and sex this species using a footprint identification technique (FIT). It is based on a pairwise comparison of trails (unbroken series of footprints) using discriminant analysis, with a Ward's clustering method. We collected footprints from 30 captive animals to train our algorithm and used another 11 animals for model validation. The accuracy for individual identification was &gt; 90% for individuals with more than six footprints and 89% with fewer footprints per trail. The accuracy for sex discrimination was about 84% using a single footprint and 91% using trails. This cost-effective method provides a promising future for monitoring wild panda populations and understanding their dynamics and especially useful for monitoring reintroduced animals after the detachment of GPS collars. The data collection protocol is straightforward and accessible to citizen scientists and conservation professionals alike.</t>
+          <t xml:space="preserve"> data on numbers and distribution of free ranging giant panda are essential to the formulation of effective conservation strategies. there is still no ideal method to identify individuals and sex this species. the traditional bite size method using bamboo fragments in their feces lacks accuracy. the modern dna based estimation is expensive and demands fresh samples. the lack of identifiable individual features on panda pelage and no apparent sexual dimorphism impede reliable estimation from camera trap images. here, we propose an innovative and non invasive technique to identify and sex this species using a footprint identification technique (fit). it is based on a pairwise comparison of trails (unbroken series of footprints) using discriminant analysis, with a wards clustering method. we collected footprints from 30 captive animals to train our algorithm and used another 11 animals for model validation. the accuracy for individual identification was &gt; 90% for individuals with more than six footprints and 89% with fewer footprints per trail. the accuracy for sex discrimination was about 84% using a single footprint and 91% using trails. this cost effective method provides a promising future for monitoring wild panda populations and understanding their dynamics and especially useful for monitoring reintroduced animals after the detachment of gps collars. the data collection protocol is straightforward and accessible to citizen scientists and conservation professionals alike.</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4011,16 +4011,16 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>[3, 11, 15]</t>
+          <t>[11, 12, 15]</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.525|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.291|x12: 0.225|x13: 0.000|x14: 0.000|x15: 0.062|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.101|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.089|x12: 0.290|x13: 0.000|x14: 0.000|x15: 0.199|x16: 0.098|x17: 0.000
 LDA -&gt; x1: 0.135|x2: 0.063|x3: 0.114|x4: 0.169|x5: 0.195|x6: 0.000|x7: 0.000|x8: 0.116|x9: 0.065|x10: 0.061|x11: 0.236|x12: 0.095|x13: 0.000|x14: 0.000|x15: 0.367|x16: 0.203|x17: 0.000
-TOP2VEC -&gt; x1: 0.107|x2: 0.082|x3: 0.170|x4: 0.106|x5: 0.212|x6: 0.261|x7: 0.386|x8: 0.162|x9: 0.224|x10: 0.055|x11: 0.114|x12: 0.184|x13: 0.000|x14: 0.249|x15: 0.311|x16: 0.113|x17: 0.000
-MEAN -&gt; x1: 0.080|x2: 0.048|x3: 0.261|x4: 0.092|x5: 0.136|x6: 0.087|x7: 0.129|x8: 0.093|x9: 0.097|x10: 0.039|x11: 0.214|x12: 0.168|x13: 0.000|x14: 0.083|x15: 0.247|x16: 0.105|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.068|x4: 0.058|x5: 0.060|x6: 0.057|x7: 0.060|x8: 0.058|x9: 0.058|x10: 0.055|x11: 0.065|x12: 0.062|x13: 0.053|x14: 0.057|x15: 0.067|x16: 0.058|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.087|x3: 0.143|x4: 0.075|x5: 0.116|x6: 0.109|x7: 0.181|x8: 0.000|x9: 0.000|x10: 0.054|x11: 0.237|x12: 0.191|x13: 0.257|x14: 0.066|x15: 0.082|x16: 0.152|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.034|x2: 0.037|x3: 0.089|x4: 0.061|x5: 0.078|x6: 0.027|x7: 0.045|x8: 0.029|x9: 0.016|x10: 0.029|x11: 0.141|x12: 0.144|x13: 0.064|x14: 0.017|x15: 0.287|x16: 0.113|x17: 0.000
 </t>
         </is>
       </c>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t xml:space="preserve"> With the increasing number of surveillance cameras in both indoor and outdoor locations, there is a grown demand for an intelligent system that detects abnormal events. Although human action recognition is a highly reached topic in computer vision, abnormal behavior detection is lately attracting more research attention. Indeed, several systems are proposed in order to ensure human safety. In this paper, we are interested in the study of the two main steps composing a video surveillance system which are the behavior representation and the behavior modeling. Techniques related to feature extraction and description for behavior representation are reviewed. Classification methods and frameworks for behavior modeling are also provided. Moreover, available datasets and metrics for performance evaluation are presented. Finally, examples of existing video surveillance systems used in real world are described.</t>
+          <t xml:space="preserve"> with the increasing number of surveillance cameras in both indoor and outdoor locations, there is a grown demand for an intelligent system that detects abnormal events. although human action recognition is a highly reached topic in computer vision, abnormal behavior detection is lately attracting more research attention. indeed, several systems are proposed in order to ensure human safety. in this paper, we are interested in the study of the two main steps composing a video surveillance system which are the behavior representation and the behavior modeling. techniques related to feature extraction and description for behavior representation are reviewed. classification methods and frameworks for behavior modeling are also provided. moreover, available datasets and metrics for performance evaluation are presented. finally, examples of existing video surveillance systems used in real world are described.</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4041,16 +4041,16 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>[3, 11, 16]</t>
+          <t>[3, 6, 12, 16]</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.538|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.322|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.067|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.116|x12: 0.155|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.175|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.062|x3: 0.171|x4: 0.233|x5: 0.139|x6: 0.000|x7: 0.060|x8: 0.078|x9: 0.223|x10: 0.063|x11: 0.075|x12: 0.201|x13: 0.000|x14: 0.205|x15: 0.000|x16: 0.309|x17: 0.000
-TOP2VEC -&gt; x1: 0.194|x2: 0.000|x3: 0.417|x4: 0.222|x5: 0.347|x6: 0.415|x7: 0.054|x8: 0.219|x9: 0.000|x10: 0.136|x11: 0.359|x12: 0.000|x13: 0.139|x14: 0.261|x15: 0.196|x16: 0.278|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.021|x3: 0.363|x4: 0.152|x5: 0.162|x6: 0.138|x7: 0.038|x8: 0.099|x9: 0.074|x10: 0.066|x11: 0.252|x12: 0.067|x13: 0.046|x14: 0.155|x15: 0.065|x16: 0.218|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.053|x3: 0.075|x4: 0.061|x5: 0.061|x6: 0.060|x7: 0.054|x8: 0.058|x9: 0.056|x10: 0.056|x11: 0.067|x12: 0.056|x13: 0.055|x14: 0.061|x15: 0.056|x16: 0.065|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.059|x3: 0.383|x4: 0.140|x5: 0.142|x6: 0.238|x7: 0.200|x8: 0.000|x9: 0.000|x10: 0.122|x11: 0.193|x12: 0.277|x13: 0.193|x14: 0.196|x15: 0.117|x16: 0.165|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.030|x3: 0.139|x4: 0.093|x5: 0.070|x6: 0.184|x7: 0.065|x8: 0.020|x9: 0.056|x10: 0.046|x11: 0.096|x12: 0.158|x13: 0.048|x14: 0.100|x15: 0.029|x16: 0.162|x17: 0.000
 </t>
         </is>
       </c>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Visual surveillance in dynamic scenes, especially for humans and vehicles, is currently one of the most active research topics in computer vision. It has a wide spectrum of promising applications, including access control in special areas, human identification at a distance, crowd flux statistics and congestion analysis, detection of anomalous behaviors, and interactive surveillance using multiple cameras, etc. In general, the processing framework of visual surveillance in dynamic scenes includes the following stages: modeling of environments, detection of motion, classification of moving objects, tracking, understanding and description of behaviors, human identification, and fusion of data from multiple cameras. We review recent developments and general strategies of all these stages. Finally, we analyze possible research directions, e.g., occlusion handling, a combination of twoand three-dimensional tracking, a combination of motion analysis and biometrics, anomaly detection and behavior prediction, content-based retrieval of surveillance videos, behavior understanding and natural language description, fusion of information from multiple sensors, and remote surveillance.</t>
+          <t xml:space="preserve"> visual surveillance in dynamic scenes, especially for humans and vehicles, is currently one of the most active research topics in computer vision. it has a wide spectrum of promising applications, including access control in special areas, human identification at a distance, crowd flux statistics and congestion analysis, detection of anomalous behaviors, and interactive surveillance using multiple cameras, etc. in general, the processing framework of visual surveillance in dynamic scenes includes the following stages: modeling of environments, detection of motion, classification of moving objects, tracking, understanding and description of behaviors, human identification, and fusion of data from multiple cameras. we review recent developments and general strategies of all these stages. finally, we analyze possible research directions, e.g., occlusion handling, a combination of twoand three dimensional tracking, a combination of motion analysis and biometrics, anomaly detection and behavior prediction, content based retrieval of surveillance videos, behavior understanding and natural language description, fusion of information from multiple sensors, and remote surveillance.</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4071,16 +4071,16 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>[3, 4, 11]</t>
+          <t>[4, 11]</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.528|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.305|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.112|x12: 0.000|x13: 0.000|x14: 0.097|x15: 0.109|x16: 0.138|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.142|x3: 0.101|x4: 0.406|x5: 0.052|x6: 0.000|x7: 0.000|x8: 0.199|x9: 0.099|x10: 0.096|x11: 0.184|x12: 0.061|x13: 0.071|x14: 0.086|x15: 0.241|x16: 0.081|x17: 0.000
-TOP2VEC -&gt; x1: 0.267|x2: 0.276|x3: 0.246|x4: 0.228|x5: 0.164|x6: 0.376|x7: 0.290|x8: 0.326|x9: 0.172|x10: 0.113|x11: 0.318|x12: 0.372|x13: 0.203|x14: 0.357|x15: 0.332|x16: 0.232|x17: 0.000
-MEAN -&gt; x1: 0.089|x2: 0.139|x3: 0.282|x4: 0.211|x5: 0.072|x6: 0.125|x7: 0.097|x8: 0.175|x9: 0.090|x10: 0.070|x11: 0.269|x12: 0.144|x13: 0.091|x14: 0.148|x15: 0.191|x16: 0.104|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.059|x3: 0.068|x4: 0.063|x5: 0.055|x6: 0.058|x7: 0.056|x8: 0.061|x9: 0.056|x10: 0.055|x11: 0.067|x12: 0.059|x13: 0.056|x14: 0.059|x15: 0.062|x16: 0.057|x17: 0.051
+TOP2VEC -&gt; x1: 0.000|x2: 0.118|x3: 0.215|x4: 0.125|x5: 0.113|x6: 0.079|x7: 0.106|x8: 0.000|x9: 0.000|x10: 0.068|x11: 0.198|x12: 0.135|x13: 0.065|x14: 0.187|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.073|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.284|x12: 0.083|x13: 0.098|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.065|x3: 0.079|x4: 0.133|x5: 0.041|x6: 0.020|x7: 0.045|x8: 0.050|x9: 0.025|x10: 0.041|x11: 0.194|x12: 0.070|x13: 0.059|x14: 0.092|x15: 0.087|x16: 0.055|x17: 0.000
 </t>
         </is>
       </c>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Serious games can be used to improve people's social awareness by letting them experience difficult social situations and learn from these experiences. However, we assert that, when moving beyond the strict realism that social simulations offer, techniques from role play may be used that offer more possibilities for feedback and reflection. We discuss the design of two such serious games for interpersonal skills training in the domain of law enforcement. These games feature intelligent virtual agents with which trainees have to interact across different scenarios to improve their social awareness. By interacting with the virtual agents, trainees experience how their behaviour influences the course of the intervention and its outcomes. We discuss how we intend to improve the learning experience in these serious games by including meta-techniques from role play. We close by describing the current and future implementations of our serious games.</t>
+          <t xml:space="preserve"> serious games can be used to improve peoples social awareness by letting them experience difficult social situations and learn from these experiences. however, we assert that, when moving beyond the strict realism that social simulations offer, techniques from role play may be used that offer more possibilities for feedback and reflection. we discuss the design of two such serious games for interpersonal skills training in the domain of law enforcement. these games feature intelligent virtual agents with which trainees have to interact across different scenarios to improve their social awareness. by interacting with the virtual agents, trainees experience how their behaviour influences the course of the intervention and its outcomes. we discuss how we intend to improve the learning experience in these serious games by including meta techniques from role play. we close by describing the current and future implementations of our serious games.</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4101,16 +4101,16 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.176|x2: 0.000|x3: 0.366|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.212|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.219|x2: 0.000|x3: 0.000|x4: 0.129|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.088|x10: 0.000|x11: 0.084|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.062|x2: 0.168|x3: 0.118|x4: 0.176|x5: 0.133|x6: 0.000|x7: 0.116|x8: 0.376|x9: 0.106|x10: 0.092|x11: 0.100|x12: 0.080|x13: 0.118|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
-TOP2VEC -&gt; x1: 0.258|x2: 0.274|x3: 0.070|x4: 0.362|x5: 0.426|x6: 0.000|x7: 0.144|x8: 0.234|x9: 0.075|x10: 0.000|x11: 0.080|x12: 0.376|x13: 0.464|x14: 0.211|x15: 0.184|x16: 0.073|x17: 0.000
-MEAN -&gt; x1: 0.165|x2: 0.147|x3: 0.185|x4: 0.179|x5: 0.186|x6: 0.000|x7: 0.086|x8: 0.203|x9: 0.060|x10: 0.031|x11: 0.130|x12: 0.152|x13: 0.194|x14: 0.070|x15: 0.061|x16: 0.083|x17: 0.000
-SOFTMAX -&gt; x1: 0.062|x2: 0.061|x3: 0.063|x4: 0.063|x5: 0.063|x6: 0.052|x7: 0.057|x8: 0.064|x9: 0.056|x10: 0.054|x11: 0.060|x12: 0.061|x13: 0.064|x14: 0.056|x15: 0.056|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.404|x5: 0.170|x6: 0.162|x7: 0.329|x8: 0.060|x9: 0.000|x10: 0.197|x11: 0.139|x12: 0.299|x13: 0.000|x14: 0.142|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.349|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.070|x2: 0.042|x3: 0.030|x4: 0.177|x5: 0.163|x6: 0.041|x7: 0.111|x8: 0.109|x9: 0.049|x10: 0.072|x11: 0.081|x12: 0.095|x13: 0.030|x14: 0.035|x15: 0.000|x16: 0.044|x17: 0.000
 </t>
         </is>
       </c>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This paper envisions a future where autonomous agents are used to foster and support pro-social behavior in a hybrid society of humans and machines. Pro-social behavior occurs when people and agents perform costly actions that benefit others. Acts such as helping others voluntarily, donating to charity, providing informations or sharing resources, are all forms of pro-social behavior. We discuss two questions that challenge a purely utilitarian view of human decision making and contextualize its role in hybrid societies: i) What are the conditions and mechanisms that lead societies of agents and humans to be more pro-social? ii) How can we engineer autonomous entities (agents and robots) that lead to more altruistic and cooperative behaviors in a hybrid society? We propose using social simulations, game theory, population dynamics, and studies with people in virtual or real environments (with robots) where both agents and humans interact. This research will constitute the basis for establishing the foundations for the new field of Pro-social Computing, aiming at understanding, predicting and promoting pro-sociality among humans, through artificial agents and multiagent systems.</t>
+          <t xml:space="preserve"> this paper envisions a future where autonomous agents are used to foster and support pro social behavior in a hybrid society of humans and machines. pro social behavior occurs when people and agents perform costly actions that benefit others. acts such as helping others voluntarily, donating to charity, providing informations or sharing resources, are all forms of pro social behavior. we discuss two questions that challenge a purely utilitarian view of human decision making and contextualize its role in hybrid societies: i) what are the conditions and mechanisms that lead societies of agents and humans to be more pro social? ii) how can we engineer autonomous entities (agents and robots) that lead to more altruistic and cooperative behaviors in a hybrid society? we propose using social simulations, game theory, population dynamics, and studies with people in virtual or real environments (with robots) where both agents and humans interact. this research will constitute the basis for establishing the foundations for the new field of pro social computing, aiming at understanding, predicting and promoting pro sociality among humans, through artificial agents and multiagent systems.</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4131,16 +4131,16 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>[1, 3, 5, 14, 16]</t>
+          <t>[1, 5, 16]</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.198|x2: 0.000|x3: 0.449|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.260|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.182|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.319|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.120|x15: 0.000|x16: 0.227|x17: 0.000
 LDA -&gt; x1: 0.161|x2: 0.099|x3: 0.122|x4: 0.072|x5: 0.269|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.156|x10: 0.000|x11: 0.000|x12: 0.211|x13: 0.151|x14: 0.190|x15: 0.000|x16: 0.387|x17: 0.000
-TOP2VEC -&gt; x1: 0.250|x2: 0.234|x3: 0.236|x4: 0.191|x5: 0.512|x6: 0.139|x7: 0.207|x8: 0.228|x9: 0.000|x10: 0.000|x11: 0.102|x12: 0.085|x13: 0.409|x14: 0.623|x15: 0.271|x16: 0.104|x17: 0.000
-MEAN -&gt; x1: 0.203|x2: 0.111|x3: 0.269|x4: 0.088|x5: 0.256|x6: 0.046|x7: 0.069|x8: 0.076|x9: 0.052|x10: 0.000|x11: 0.120|x12: 0.099|x13: 0.187|x14: 0.230|x15: 0.090|x16: 0.224|x17: 0.000
-SOFTMAX -&gt; x1: 0.063|x2: 0.058|x3: 0.068|x4: 0.056|x5: 0.067|x6: 0.054|x7: 0.055|x8: 0.056|x9: 0.055|x10: 0.052|x11: 0.058|x12: 0.057|x13: 0.062|x14: 0.065|x15: 0.057|x16: 0.065|x17: 0.052
+TOP2VEC -&gt; x1: 0.220|x2: 0.000|x3: 0.116|x4: 0.216|x5: 0.257|x6: 0.183|x7: 0.152|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.094|x12: 0.091|x13: 0.000|x14: 0.142|x15: 0.000|x16: 0.082|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.195|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.189|x17: 0.000
+MEAN -&gt; x1: 0.175|x2: 0.025|x3: 0.060|x4: 0.072|x5: 0.180|x6: 0.046|x7: 0.038|x8: 0.000|x9: 0.039|x10: 0.000|x11: 0.023|x12: 0.075|x13: 0.038|x14: 0.113|x15: 0.000|x16: 0.221|x17: 0.000
 </t>
         </is>
       </c>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t xml:space="preserve"> During last decade the scientific research on Unmanned Aerial Vehicless (UAVs) increased spectacularly and led to the design of multiple types of aerial platforms. The major challenge today is the development of autonomously operating aerial agents capable of completing missions independently of human interaction. To this extent, visual sensing techniques have been integrated in the control pipeline of the UAVs in order to enhance their navigation and guidance skills. The aim of this article is to present a comprehensive literature review on vision based applications for UAVs focusing mainly on current developments and trends. These applications are sorted in different categories according to the research topics among various research groups. More specifically vision based position-attitude control, pose estimation and mapping, obstacle detection as well as target tracking are the identified components towards autonomous agents. Aerial platforms could reach greater level of autonomy by integrating all these technologies onboard. Additionally, throughout this article the concept of fusion multiple sensors is highlighted, while an overview on the challenges C. Kanellakis ( ) • G.</t>
+          <t xml:space="preserve"> during last decade the scientific research on unmanned aerial vehicless (uavs) increased spectacularly and led to the design of multiple types of aerial platforms. the major challenge today is the development of autonomously operating aerial agents capable of completing missions independently of human interaction. to this extent, visual sensing techniques have been integrated in the control pipeline of the uavs in order to enhance their navigation and guidance skills. the aim of this article is to present a comprehensive literature review on vision based applications for uavs focusing mainly on current developments and trends. these applications are sorted in different categories according to the research topics among various research groups. more specifically vision based position attitude control, pose estimation and mapping, obstacle detection as well as target tracking are the identified components towards autonomous agents. aerial platforms could reach greater level of autonomy by integrating all these technologies onboard. additionally, throughout this article the concept of fusion multiple sensors is highlighted, while an overview on the challenges c. kanellakis ( ) • g.</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4161,16 +4161,16 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>[3, 5, 11]</t>
+          <t>[3, 11, 15]</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.501|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.304|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.122|x6: 0.100|x7: 0.000|x8: 0.000|x9: 0.205|x10: 0.000|x11: 0.178|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.146|x3: 0.392|x4: 0.000|x5: 0.112|x6: 0.000|x7: 0.000|x8: 0.105|x9: 0.179|x10: 0.000|x11: 0.180|x12: 0.080|x13: 0.239|x14: 0.138|x15: 0.108|x16: 0.142|x17: 0.000
-TOP2VEC -&gt; x1: 0.165|x2: 0.000|x3: 0.216|x4: 0.373|x5: 0.538|x6: 0.086|x7: 0.283|x8: 0.179|x9: 0.118|x10: 0.076|x11: 0.251|x12: 0.294|x13: 0.220|x14: 0.287|x15: 0.170|x16: 0.155|x17: 0.000
-MEAN -&gt; x1: 0.055|x2: 0.049|x3: 0.369|x4: 0.124|x5: 0.204|x6: 0.029|x7: 0.094|x8: 0.095|x9: 0.099|x10: 0.025|x11: 0.245|x12: 0.125|x13: 0.153|x14: 0.141|x15: 0.093|x16: 0.099|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.055|x3: 0.075|x4: 0.059|x5: 0.064|x6: 0.054|x7: 0.057|x8: 0.057|x9: 0.057|x10: 0.053|x11: 0.067|x12: 0.059|x13: 0.061|x14: 0.060|x15: 0.057|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.175|x4: 0.063|x5: 0.113|x6: 0.109|x7: 0.298|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.270|x12: 0.234|x13: 0.192|x14: 0.178|x15: 0.066|x16: 0.067|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.380|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.037|x3: 0.142|x4: 0.016|x5: 0.087|x6: 0.052|x7: 0.074|x8: 0.026|x9: 0.096|x10: 0.000|x11: 0.157|x12: 0.078|x13: 0.108|x14: 0.079|x15: 0.138|x16: 0.052|x17: 0.000
 </t>
         </is>
       </c>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Drones are increasingly being used for various purposes from recording footage in inaccessible areas to delivering packages. A rise in drone usage introduces privacy and security concerns about flying boundaries, what data drones collect in public and private spaces, and how that data is stored and disseminated. However, commercial and personal drone regulations focusing on privacy and security have been fairly minimal in the United States. To inform privacy and security guidelines for drone design and regulation, we need to understand users' perceptions about drones, privacy, and security. In this paper, we describe a laboratory study with 20 participants who interacted with a real or model drone to elicit user perceptions of privacy and security issues around drones. We present our results, discuss the implications of our work, and make recommendations to improve drone design and regulations that enhance individual privacy and security.</t>
+          <t xml:space="preserve"> drones are increasingly being used for various purposes from recording footage in inaccessible areas to delivering packages. a rise in drone usage introduces privacy and security concerns about flying boundaries, what data drones collect in public and private spaces, and how that data is stored and disseminated. however, commercial and personal drone regulations focusing on privacy and security have been fairly minimal in the united states. to inform privacy and security guidelines for drone design and regulation, we need to understand users perceptions about drones, privacy, and security. in this paper, we describe a laboratory study with 20 participants who interacted with a real or model drone to elicit user perceptions of privacy and security issues around drones. we present our results, discuss the implications of our work, and make recommendations to improve drone design and regulations that enhance individual privacy and security.</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4191,16 +4191,16 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>[2, 11]</t>
+          <t>[11, 16]</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.337|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.266|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.147|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.103|x7: 0.000|x8: 0.000|x9: 0.090|x10: 0.000|x11: 0.179|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.303|x3: 0.126|x4: 0.228|x5: 0.000|x6: 0.000|x7: 0.090|x8: 0.000|x9: 0.118|x10: 0.000|x11: 0.285|x12: 0.161|x13: 0.061|x14: 0.194|x15: 0.000|x16: 0.253|x17: 0.000
-TOP2VEC -&gt; x1: 0.178|x2: 0.383|x3: 0.000|x4: 0.226|x5: 0.000|x6: 0.074|x7: 0.230|x8: 0.185|x9: 0.223|x10: 0.064|x11: 0.447|x12: 0.371|x13: 0.333|x14: 0.364|x15: 0.249|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.059|x2: 0.229|x3: 0.155|x4: 0.151|x5: 0.000|x6: 0.025|x7: 0.107|x8: 0.062|x9: 0.114|x10: 0.021|x11: 0.333|x12: 0.177|x13: 0.131|x14: 0.186|x15: 0.083|x16: 0.128|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.066|x3: 0.061|x4: 0.061|x5: 0.052|x6: 0.054|x7: 0.058|x8: 0.056|x9: 0.059|x10: 0.053|x11: 0.073|x12: 0.062|x13: 0.060|x14: 0.063|x15: 0.057|x16: 0.059|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.153|x5: 0.000|x6: 0.000|x7: 0.224|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.431|x12: 0.085|x13: 0.205|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.113|x3: 0.032|x4: 0.095|x5: 0.000|x6: 0.026|x7: 0.079|x8: 0.000|x9: 0.052|x10: 0.000|x11: 0.224|x12: 0.061|x13: 0.066|x14: 0.049|x15: 0.000|x16: 0.188|x17: 0.000
 </t>
         </is>
       </c>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Automated driving can fundamentally change road transportation 26 and improve 27 quality of life however at present the role of humans in automated vehicles 28 (avs) is not clearly established interviews were conducted in april and may 29 2015 with twelve expert researchers in the field of human factors (hf) of 30 automated driving to identify commonalities and distinctive perspectives 31 regarding hf challenges in the development of avs the experts indicated that 32 an av up to sae level 4 should inform its driver about the avs capabilities and 33 operational status and ensure safety while changing between automated and 34 manual modes hf research should particularly address interactions between 35 avs human drivers and vulnerable road users additionally driver training 36 programs may have to be modified to ensure that humans are capable of using 37 avs finally a reflection on the interviews is provided showing discordance 38 between the interviewees statementswhich appear to be in line with a long 39 history of work on human factors research and the rapid development of 40 automation technology we expect our perspective to be instrumental for 41 stakeholders involved in av development and instructive to other parties</t>
+          <t>automated driving can fundamentally change road transportation 26 and improve 27 quality of life however at present the role of humans in automated vehicles 28 (avs) is not clearly established interviews were conducted in april and may 29 2015 with twelve expert researchers in the field of human factors (hf) of 30 automated driving to identify commonalities and distinctive perspectives 31 regarding hf challenges in the development of avs the experts indicated that 32 an av up to sae level 4 should inform its driver about the avs capabilities and 33 operational status and ensure safety while changing between automated and 34 manual modes hf research should particularly address interactions between 35 avs human drivers and vulnerable road users additionally driver training 36 programs may have to be modified to ensure that humans are capable of using 37 avs finally a reflection on the interviews is provided showing discordance 38 between the interviewees statementswhich appear to be in line with a long 39 history of work on human factors research and the rapid development of 40 automation technology we expect our perspective to be instrumental for 41 stakeholders involved in av development and instructive to other parties</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4221,16 +4221,16 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[9, 11, 13, 14, 16]</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.379|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.082|x10: 0.000|x11: 0.284|x12: 0.056|x13: 0.087|x14: 0.000|x15: 0.000|x16: 0.155|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.090|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.152|x10: 0.000|x11: 0.136|x12: 0.000|x13: 0.092|x14: 0.097|x15: 0.000|x16: 0.181|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.106|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.229|x8: 0.148|x9: 0.448|x10: 0.000|x11: 0.000|x12: 0.183|x13: 0.131|x14: 0.286|x15: 0.000|x16: 0.291|x17: 0.000
-TOP2VEC -&gt; x1: 0.102|x2: 0.000|x3: 0.000|x4: 0.159|x5: 0.135|x6: 0.218|x7: 0.246|x8: 0.109|x9: 0.241|x10: 0.060|x11: 0.263|x12: 0.328|x13: 0.246|x14: 0.188|x15: 0.255|x16: 0.122|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.000|x3: 0.162|x4: 0.053|x5: 0.045|x6: 0.073|x7: 0.158|x8: 0.086|x9: 0.257|x10: 0.020|x11: 0.182|x12: 0.189|x13: 0.154|x14: 0.158|x15: 0.085|x16: 0.189|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.053|x3: 0.062|x4: 0.055|x5: 0.055|x6: 0.057|x7: 0.062|x8: 0.057|x9: 0.068|x10: 0.054|x11: 0.063|x12: 0.064|x13: 0.061|x14: 0.062|x15: 0.057|x16: 0.064|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.154|x5: 0.000|x6: 0.000|x7: 0.217|x8: 0.090|x9: 0.190|x10: 0.138|x11: 0.204|x12: 0.201|x13: 0.221|x14: 0.204|x15: 0.000|x16: 0.060|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.212|x12: 0.000|x13: 0.183|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.026|x4: 0.061|x5: 0.000|x6: 0.000|x7: 0.112|x8: 0.059|x9: 0.198|x10: 0.035|x11: 0.138|x12: 0.096|x13: 0.157|x14: 0.147|x15: 0.000|x16: 0.133|x17: 0.000
 </t>
         </is>
       </c>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Background aids is a worrying public health issue in china and lacks timely and effective surveillance with the diffusion and adoption of the internet the `big data aggregated from internet search engines which contain users information on the concern or reality of their health status provide a new opportunity for aids surveillance this paper uses search engine data to monitor and forecast aids in china methods a machine learning method artificial neural networks (anns) is used to forecast aids incidences and deaths search trend data related to aids from the largest chinese search engine baiducom are collected and selected as the input variables of anns and officially reported actual aids incidences and deaths are used as the output variable three criteria the mean absolute percentage error the root mean squared percentage error and the index of agreement are used to test the forecasting performance of the ann method results based on the monthly time series data from january 2011 to june 2017 this article finds that under the three criteria the ann method can lead to satisfactory forecasting of aids incidences and deaths regardless of the change in the number of search queries conclusions despite the inability to selfdetect hiv/aids through online searching internetbased data should be adopted as a timely costeffective complement to a traditional aids surveillance system</t>
+          <t>background aids is a worrying public health issue in china and lacks timely and effective surveillance with the diffusion and adoption of the internet the `big data aggregated from internet search engines which contain users information on the concern or reality of their health status provide a new opportunity for aids surveillance this paper uses search engine data to monitor and forecast aids in china methods a machine learning method artificial neural networks (anns) is used to forecast aids incidences and deaths search trend data related to aids from the largest chinese search engine baiducom are collected and selected as the input variables of anns and officially reported actual aids incidences and deaths are used as the output variable three criteria the mean absolute percentage error the root mean squared percentage error and the index of agreement are used to test the forecasting performance of the ann method results based on the monthly time series data from january 2011 to june 2017 this article finds that under the three criteria the ann method can lead to satisfactory forecasting of aids incidences and deaths regardless of the change in the number of search queries conclusions despite the inability to selfdetect hiv/aids through online searching internetbased data should be adopted as a timely costeffective complement to a traditional aids surveillance system</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4251,16 +4251,16 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[2, 3]</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.733|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.295|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.127|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.077|x9: 0.000|x10: 0.000|x11: 0.073|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.249|x3: 0.253|x4: 0.308|x5: 0.063|x6: 0.000|x7: 0.128|x8: 0.301|x9: 0.094|x10: 0.099|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.110|x15: 0.119|x16: 0.094|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.246|x3: 0.301|x4: 0.179|x5: 0.260|x6: 0.056|x7: 0.000|x8: 0.067|x9: 0.000|x10: 0.000|x11: 0.237|x12: 0.000|x13: 0.000|x14: 0.277|x15: 0.000|x16: 0.108|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.165|x3: 0.351|x4: 0.162|x5: 0.108|x6: 0.019|x7: 0.043|x8: 0.123|x9: 0.031|x10: 0.033|x11: 0.177|x12: 0.000|x13: 0.000|x14: 0.129|x15: 0.040|x16: 0.067|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.063|x3: 0.076|x4: 0.063|x5: 0.060|x6: 0.055|x7: 0.056|x8: 0.061|x9: 0.055|x10: 0.056|x11: 0.064|x12: 0.054|x13: 0.054|x14: 0.061|x15: 0.056|x16: 0.058|x17: 0.054
+TOP2VEC -&gt; x1: 0.000|x2: 0.150|x3: 0.058|x4: 0.000|x5: 0.147|x6: 0.000|x7: 0.181|x8: 0.000|x9: 0.163|x10: 0.087|x11: 0.264|x12: 0.067|x13: 0.081|x14: 0.061|x15: 0.065|x16: 0.087|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.132|x3: 0.328|x4: 0.077|x5: 0.053|x6: 0.000|x7: 0.077|x8: 0.095|x9: 0.064|x10: 0.047|x11: 0.084|x12: 0.017|x13: 0.020|x14: 0.043|x15: 0.046|x16: 0.045|x17: 0.000
 </t>
         </is>
       </c>
@@ -4271,7 +4271,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Introduction artificial intelligence is a branch of computer science capable of analysing complex medical data their potential to exploit meaningful relationship with in a data set can be used in the diagnosis treatment and predicting outcome in many clinical scenarios methods medline and internet searches were carried out using the keywords artificial intelligence and neural networks (computer) further references were obtained by crossreferencing from key articles an overview of different artificial intelligent techniques is presented in this paper along with the review of important clinical applications results the proficiency of artificial intelligent techniques has been explored in almost every field of medicine artificial neural network was the most commonly used analytical tool whilst other artificial intelligent techniques such as fuzzy expert systems evolutionary computation and hybrid intelligent systems have all been used in different clinical settings discussion artificial intelligence techniques have the potential to be applied in almost every field of medicine there is need for further clinical trials which are appropriately designed before these emergent techniques find application in the real clinical setting</t>
+          <t>introduction artificial intelligence is a branch of computer science capable of analysing complex medical data their potential to exploit meaningful relationship with in a data set can be used in the diagnosis treatment and predicting outcome in many clinical scenarios methods medline and internet searches were carried out using the keywords artificial intelligence and neural networks (computer) further references were obtained by crossreferencing from key articles an overview of different artificial intelligent techniques is presented in this paper along with the review of important clinical applications results the proficiency of artificial intelligent techniques has been explored in almost every field of medicine artificial neural network was the most commonly used analytical tool whilst other artificial intelligent techniques such as fuzzy expert systems evolutionary computation and hybrid intelligent systems have all been used in different clinical settings discussion artificial intelligence techniques have the potential to be applied in almost every field of medicine there is need for further clinical trials which are appropriately designed before these emergent techniques find application in the real clinical setting</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4281,16 +4281,16 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>[3, 11, 13]</t>
+          <t>[3, 13]</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.761|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.440|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.061|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.091|x10: 0.000|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.056|x3: 0.169|x4: 0.119|x5: 0.321|x6: 0.000|x7: 0.000|x8: 0.131|x9: 0.149|x10: 0.098|x11: 0.136|x12: 0.057|x13: 0.206|x14: 0.000|x15: 0.194|x16: 0.184|x17: 0.000
-TOP2VEC -&gt; x1: 0.220|x2: 0.303|x3: 0.171|x4: 0.224|x5: 0.102|x6: 0.000|x7: 0.234|x8: 0.198|x9: 0.099|x10: 0.174|x11: 0.160|x12: 0.291|x13: 0.424|x14: 0.251|x15: 0.394|x16: 0.356|x17: 0.000
-MEAN -&gt; x1: 0.073|x2: 0.120|x3: 0.280|x4: 0.114|x5: 0.141|x6: 0.000|x7: 0.078|x8: 0.110|x9: 0.083|x10: 0.091|x11: 0.245|x12: 0.116|x13: 0.210|x14: 0.084|x15: 0.196|x16: 0.180|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.069|x4: 0.058|x5: 0.060|x6: 0.052|x7: 0.056|x8: 0.058|x9: 0.056|x10: 0.057|x11: 0.066|x12: 0.058|x13: 0.064|x14: 0.056|x15: 0.063|x16: 0.062|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.158|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.202|x8: 0.000|x9: 0.087|x10: 0.072|x11: 0.190|x12: 0.325|x13: 0.317|x14: 0.272|x15: 0.069|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.054|x3: 0.183|x4: 0.030|x5: 0.080|x6: 0.000|x7: 0.050|x8: 0.033|x9: 0.082|x10: 0.042|x11: 0.098|x12: 0.096|x13: 0.131|x14: 0.068|x15: 0.066|x16: 0.046|x17: 0.000
 </t>
         </is>
       </c>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Objectives to introduce and summarize current research in the field of public health and epidemiology informatics methods the 2017 literature concerning public health and epidemiology informatics was searched in pubmed and web of science and the returned references were reviewed by the two section editors to select 14 candidate best papers these papers were then peerreviewed by external reviewers to provide the editorial team with an enlightened vision to select the best papers results among the 843 references retrieved from pubmed and web of science two were finally selected as best papers the first one analyzes the relationship between the disease social/ mass media and public emotions to understand public overreaction (leading to a noticeable reduction of social and economic activities) in the context of a nationwide outbreak of middle east respiratory syndrome (mers) in korea in 2015 the second paper concerns a new methodology to deidentify patient notes in electronic health records based on artificial neural networks that outperformed existing methods conclusions surveillance is still a productive topic in public health informatics but other very important topics in public health are appearing for example the use of artificial intelligence approaches is increasing</t>
+          <t>objectives to introduce and summarize current research in the field of public health and epidemiology informatics methods the 2017 literature concerning public health and epidemiology informatics was searched in pubmed and web of science and the returned references were reviewed by the two section editors to select 14 candidate best papers these papers were then peerreviewed by external reviewers to provide the editorial team with an enlightened vision to select the best papers results among the 843 references retrieved from pubmed and web of science two were finally selected as best papers the first one analyzes the relationship between the disease social/ mass media and public emotions to understand public overreaction (leading to a noticeable reduction of social and economic activities) in the context of a nationwide outbreak of middle east respiratory syndrome (mers) in korea in 2015 the second paper concerns a new methodology to deidentify patient notes in electronic health records based on artificial neural networks that outperformed existing methods conclusions surveillance is still a productive topic in public health informatics but other very important topics in public health are appearing for example the use of artificial intelligence approaches is increasing</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4311,16 +4311,16 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>[3, 11]</t>
+          <t>[3, 11, 14]</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.821|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.437|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.054|x2: 0.000|x3: 0.384|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.109|x10: 0.000|x11: 0.165|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.080|x2: 0.059|x3: 0.271|x4: 0.077|x5: 0.000|x6: 0.000|x7: 0.169|x8: 0.197|x9: 0.062|x10: 0.185|x11: 0.278|x12: 0.061|x13: 0.000|x14: 0.225|x15: 0.052|x16: 0.104|x17: 0.000
-TOP2VEC -&gt; x1: 0.094|x2: 0.153|x3: 0.149|x4: 0.118|x5: 0.058|x6: 0.000|x7: 0.000|x8: 0.059|x9: 0.000|x10: 0.094|x11: 0.311|x12: 0.151|x13: 0.283|x14: 0.266|x15: 0.250|x16: 0.192|x17: 0.000
-MEAN -&gt; x1: 0.058|x2: 0.071|x3: 0.307|x4: 0.065|x5: 0.019|x6: 0.000|x7: 0.056|x8: 0.086|x9: 0.021|x10: 0.093|x11: 0.342|x12: 0.071|x13: 0.094|x14: 0.164|x15: 0.101|x16: 0.099|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.072|x4: 0.057|x5: 0.054|x6: 0.053|x7: 0.056|x8: 0.058|x9: 0.054|x10: 0.058|x11: 0.075|x12: 0.057|x13: 0.058|x14: 0.063|x15: 0.059|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.094|x4: 0.000|x5: 0.000|x6: 0.127|x7: 0.248|x8: 0.000|x9: 0.054|x10: 0.000|x11: 0.103|x12: 0.094|x13: 0.099|x14: 0.267|x15: 0.141|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.033|x2: 0.015|x3: 0.312|x4: 0.019|x5: 0.000|x6: 0.032|x7: 0.104|x8: 0.049|x9: 0.056|x10: 0.046|x11: 0.136|x12: 0.039|x13: 0.025|x14: 0.123|x15: 0.048|x16: 0.026|x17: 0.000
 </t>
         </is>
       </c>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>The optical microscope is one of the most widely used tools for diagnosing infectious diseases in the developing world due to its reliance on trained microscopists field microscopy often suffers from poor sensitivity specificity and reproducibility the goal of this work called the autoscope is a lowcost automated digital microscope coupled with a set of computer vision and classification algorithms which can accurately diagnose of a variety of infectious diseases targeting usecases in the developing world our initial target is malaria because of the high difficulty of the task and because manual microscopy is currently a central but highly imperfect tool for malaria work in the field in addition to diagnosis the algorithm performs species identification and quantitation of parasite load parameters which are critical in many field applications but which are not effectively determined by rapid diagnostic tests (rdts)</t>
+          <t>the optical microscope is one of the most widely used tools for diagnosing infectious diseases in the developing world due to its reliance on trained microscopists field microscopy often suffers from poor sensitivity specificity and reproducibility the goal of this work called the autoscope is a lowcost automated digital microscope coupled with a set of computer vision and classification algorithms which can accurately diagnose of a variety of infectious diseases targeting usecases in the developing world our initial target is malaria because of the high difficulty of the task and because manual microscopy is currently a central but highly imperfect tool for malaria work in the field in addition to diagnosis the algorithm performs species identification and quantitation of parasite load parameters which are critical in many field applications but which are not effectively determined by rapid diagnostic tests (rdts)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4346,11 +4346,11 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.665|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.089|x11: 0.205|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.136|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.100|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.109|x2: 0.071|x3: 0.441|x4: 0.114|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.196|x9: 0.000|x10: 0.173|x11: 0.055|x12: 0.000|x13: 0.135|x14: 0.000|x15: 0.455|x16: 0.070|x17: 0.000
-TOP2VEC -&gt; x1: 0.094|x2: 0.181|x3: 0.149|x4: 0.257|x5: 0.061|x6: 0.428|x7: 0.410|x8: 0.136|x9: 0.360|x10: 0.092|x11: 0.135|x12: 0.311|x13: 0.175|x14: 0.000|x15: 0.151|x16: 0.188|x17: 0.000
-MEAN -&gt; x1: 0.068|x2: 0.084|x3: 0.363|x4: 0.124|x5: 0.020|x6: 0.143|x7: 0.137|x8: 0.111|x9: 0.120|x10: 0.118|x11: 0.132|x12: 0.104|x13: 0.103|x14: 0.000|x15: 0.202|x16: 0.086|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.075|x4: 0.059|x5: 0.053|x6: 0.060|x7: 0.060|x8: 0.059|x9: 0.059|x10: 0.059|x11: 0.060|x12: 0.058|x13: 0.058|x14: 0.052|x15: 0.064|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.157|x2: 0.000|x3: 0.289|x4: 0.123|x5: 0.063|x6: 0.225|x7: 0.348|x8: 0.152|x9: 0.065|x10: 0.055|x11: 0.066|x12: 0.064|x13: 0.099|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.067|x2: 0.018|x3: 0.432|x4: 0.059|x5: 0.016|x6: 0.056|x7: 0.087|x8: 0.087|x9: 0.016|x10: 0.091|x11: 0.030|x12: 0.016|x13: 0.059|x14: 0.000|x15: 0.139|x16: 0.017|x17: 0.000
 </t>
         </is>
       </c>
@@ -4361,7 +4361,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Background the aim of this study is to validate the fetal medicine foundation (fmf) multiple logistic regression algorithm for prediction of risk of preeclampsia in an australian population this model which predicts risk using the population rate of preeclampsia a variety of demographic factors mean maternal arterial blood pressure (map) uterine artery pi (uta pi) and pregnancyassociated plasma protein a (pappa) has been shown to predict earlyonset preeclampsia (delivery prior to 34 weeks) in 95% of women at a 10% falsepositive rate methods all women who attended first trimester screening at the royal prince alfred hospital had their body mass index (bmi) map and uta pi assessed in addition to factors traditionally used to assess aneuploidy (including pappa mom) after delivery risks of earlyonset (delivery prior to 34 weeks) preeclampsia late preeclampsia and gestational hypertension were calculated using the fmf risk algorithm results a total of 3099 women were screened and delivered locally 3066 (989%) women had all data to perform preeclampsia screening available this included 3014 (983%) women with a live birth where risks of early preeclampsia were calculated twelve women were delivered before 34 weeks because of early preeclampsia with a prevalence of early preeclampsia of 1 in 256 pregnancies risks generated through the use of maternal history map uta pi and pappa detected 417 and 917% of early preeclampsia at a falsepositive rate of 5 and 10% respectively conclusions this study shows that the fmf early preeclampsia algorithm is effective in an australian population</t>
+          <t>background the aim of this study is to validate the fetal medicine foundation (fmf) multiple logistic regression algorithm for prediction of risk of preeclampsia in an australian population this model which predicts risk using the population rate of preeclampsia a variety of demographic factors mean maternal arterial blood pressure (map) uterine artery pi (uta pi) and pregnancyassociated plasma protein a (pappa) has been shown to predict earlyonset preeclampsia (delivery prior to 34 weeks) in 95% of women at a 10% falsepositive rate methods all women who attended first trimester screening at the royal prince alfred hospital had their body mass index (bmi) map and uta pi assessed in addition to factors traditionally used to assess aneuploidy (including pappa mom) after delivery risks of earlyonset (delivery prior to 34 weeks) preeclampsia late preeclampsia and gestational hypertension were calculated using the fmf risk algorithm results a total of 3099 women were screened and delivered locally 3066 (989%) women had all data to perform preeclampsia screening available this included 3014 (983%) women with a live birth where risks of early preeclampsia were calculated twelve women were delivered before 34 weeks because of early preeclampsia with a prevalence of early preeclampsia of 1 in 256 pregnancies risks generated through the use of maternal history map uta pi and pappa detected 417 and 917% of early preeclampsia at a falsepositive rate of 5 and 10% respectively conclusions this study shows that the fmf early preeclampsia algorithm is effective in an australian population</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4371,16 +4371,16 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>[3, 5, 13]</t>
+          <t>[3, 5, 11]</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.440|x4: 0.000|x5: 0.264|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.154|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.412|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.126|x12: 0.000|x13: 0.091|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.082|x2: 0.072|x3: 0.215|x4: 0.192|x5: 0.360|x6: 0.086|x7: 0.064|x8: 0.111|x9: 0.111|x10: 0.000|x11: 0.085|x12: 0.000|x13: 0.238|x14: 0.105|x15: 0.000|x16: 0.098|x17: 0.000
-TOP2VEC -&gt; x1: 0.205|x2: 0.131|x3: 0.201|x4: 0.198|x5: 0.276|x6: 0.148|x7: 0.453|x8: 0.173|x9: 0.000|x10: 0.000|x11: 0.131|x12: 0.217|x13: 0.382|x14: 0.171|x15: 0.176|x16: 0.100|x17: 0.000
-MEAN -&gt; x1: 0.096|x2: 0.068|x3: 0.285|x4: 0.130|x5: 0.300|x6: 0.078|x7: 0.172|x8: 0.095|x9: 0.037|x10: 0.000|x11: 0.123|x12: 0.072|x13: 0.206|x14: 0.092|x15: 0.059|x16: 0.066|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.070|x4: 0.060|x5: 0.071|x6: 0.057|x7: 0.062|x8: 0.058|x9: 0.054|x10: 0.052|x11: 0.059|x12: 0.056|x13: 0.065|x14: 0.058|x15: 0.056|x16: 0.056|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.126|x4: 0.070|x5: 0.102|x6: 0.120|x7: 0.197|x8: 0.000|x9: 0.144|x10: 0.000|x11: 0.278|x12: 0.000|x13: 0.000|x14: 0.084|x15: 0.167|x16: 0.224|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.021|x2: 0.018|x3: 0.313|x4: 0.065|x5: 0.240|x6: 0.052|x7: 0.065|x8: 0.028|x9: 0.064|x10: 0.000|x11: 0.122|x12: 0.000|x13: 0.082|x14: 0.047|x15: 0.042|x16: 0.080|x17: 0.000
 </t>
         </is>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Identifying robust survival subgroups of hepatocellular carcinoma hcc will significantly improve patient care currently endeavor of integrating multiomics data to explicitly predict hcc survival from multiple patient cohorts is lacking to fill in this gap we present a deep learning dl based model on hcc that robustly differentiates survival subpopulations of patients in six cohorts we build the dl based survivalsensitive model on 360 hcc patients data using rnaseq mirnaseq and methylation data from tcga which predicts prognosis as good as an alternative model where genomics and clinical data are both considered this dl based model provides two optimal subgroups of patients with significant survival differences p713e6 and good model fitness cindex068 more aggressive subtype is associated with frequent tp53 inactivation mutations higher expression of stemness markers krt19 epcam and tumor marker birc5 and activated wnt and akt signaling pathways we validated this multiomics model on five external datasets of various omics types lirijp cohort n230 cindex075 nci cohort n221 cindex067 chinese cohort n166 cindex069 etabm36 cohort n40 cindex077 and hawaiian cohort n27 cindex082 this is the first study to employ deep learning to identify multiomics features linked to the differential survival of hcc patients given its robustness over multiple cohorts we expect this workflow to be useful at predicting hcc prognosis prediction</t>
+          <t>identifying robust survival subgroups of hepatocellular carcinoma hcc will significantly improve patient care currently endeavor of integrating multiomics data to explicitly predict hcc survival from multiple patient cohorts is lacking to fill in this gap we present a deep learning dl based model on hcc that robustly differentiates survival subpopulations of patients in six cohorts we build the dl based survivalsensitive model on 360 hcc patients data using rnaseq mirnaseq and methylation data from tcga which predicts prognosis as good as an alternative model where genomics and clinical data are both considered this dl based model provides two optimal subgroups of patients with significant survival differences p713e6 and good model fitness cindex068 more aggressive subtype is associated with frequent tp53 inactivation mutations higher expression of stemness markers krt19 epcam and tumor marker birc5 and activated wnt and akt signaling pathways we validated this multiomics model on five external datasets of various omics types lirijp cohort n230 cindex075 nci cohort n221 cindex067 chinese cohort n166 cindex069 etabm36 cohort n40 cindex077 and hawaiian cohort n27 cindex082 this is the first study to employ deep learning to identify multiomics features linked to the differential survival of hcc patients given its robustness over multiple cohorts we expect this workflow to be useful at predicting hcc prognosis prediction</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4401,16 +4401,16 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 15]</t>
+          <t>[3, 4]</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.469|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.271|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.193|x3: 0.126|x4: 0.516|x5: 0.080|x6: 0.074|x7: 0.000|x8: 0.000|x9: 0.079|x10: 0.000|x11: 0.101|x12: 0.000|x13: 0.071|x14: 0.119|x15: 0.460|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.178|x2: 0.081|x3: 0.109|x4: 0.346|x5: 0.267|x6: 0.426|x7: 0.622|x8: 0.219|x9: 0.310|x10: 0.064|x11: 0.229|x12: 0.140|x13: 0.250|x14: 0.318|x15: 0.154|x16: 0.131|x17: 0.000
-MEAN -&gt; x1: 0.059|x2: 0.091|x3: 0.235|x4: 0.282|x5: 0.116|x6: 0.167|x7: 0.167|x8: 0.073|x9: 0.130|x10: 0.021|x11: 0.200|x12: 0.047|x13: 0.107|x14: 0.146|x15: 0.205|x16: 0.044|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.069|x5: 0.058|x6: 0.061|x7: 0.061|x8: 0.056|x9: 0.059|x10: 0.053|x11: 0.063|x12: 0.054|x13: 0.058|x14: 0.060|x15: 0.064|x16: 0.054|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.154|x4: 0.166|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.193|x3: 0.126|x4: 0.500|x5: 0.080|x6: 0.074|x7: 0.000|x8: 0.000|x9: 0.079|x10: 0.000|x11: 0.101|x12: 0.000|x13: 0.071|x14: 0.119|x15: 0.460|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.077|x2: 0.000|x3: 0.000|x4: 0.146|x5: 0.000|x6: 0.213|x7: 0.316|x8: 0.000|x9: 0.000|x10: 0.155|x11: 0.081|x12: 0.153|x13: 0.281|x14: 0.155|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.019|x2: 0.048|x3: 0.195|x4: 0.203|x5: 0.020|x6: 0.072|x7: 0.079|x8: 0.000|x9: 0.020|x10: 0.039|x11: 0.045|x12: 0.038|x13: 0.088|x14: 0.068|x15: 0.115|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>We present a method for predicting preterm infant inhospital mortality using bayesian gaussian process classification we combined features extracted from sensor measurements made during the first 72 hours of care for 598 very low birth weight infants of birth weight 1500 g with standard clinical features calculated on arrival at the neonatal intensive care unit time periods of 12 18 24 36 48 and 72 hours were evaluated we achieved a classification result with area under the receiver operating characteristic curve of 0948 which is in excess of the results achieved by using the clinical standard snapii and snappeii scores</t>
+          <t>we present a method for predicting preterm infant inhospital mortality using bayesian gaussian process classification we combined features extracted from sensor measurements made during the first 72 hours of care for 598 very low birth weight infants of birth weight 1500 g with standard clinical features calculated on arrival at the neonatal intensive care unit time periods of 12 18 24 36 48 and 72 hours were evaluated we achieved a classification result with area under the receiver operating characteristic curve of 0948 which is in excess of the results achieved by using the clinical standard snapii and snappeii scores</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4431,16 +4431,16 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[2, 3, 9]</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.473|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.197|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.088|x3: 0.315|x4: 0.000|x5: 0.076|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.097|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.318|x3: 0.133|x4: 0.297|x5: 0.170|x6: 0.000|x7: 0.140|x8: 0.000|x9: 0.282|x10: 0.096|x11: 0.000|x12: 0.000|x13: 0.102|x14: 0.204|x15: 0.000|x16: 0.078|x17: 0.000
-TOP2VEC -&gt; x1: 0.159|x2: 0.257|x3: 0.101|x4: 0.130|x5: 0.207|x6: 0.462|x7: 0.264|x8: 0.209|x9: 0.268|x10: 0.096|x11: 0.213|x12: 0.457|x13: 0.162|x14: 0.309|x15: 0.291|x16: 0.197|x17: 0.000
-MEAN -&gt; x1: 0.053|x2: 0.192|x3: 0.236|x4: 0.142|x5: 0.126|x6: 0.154|x7: 0.135|x8: 0.070|x9: 0.183|x10: 0.064|x11: 0.137|x12: 0.152|x13: 0.088|x14: 0.171|x15: 0.097|x16: 0.092|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.063|x3: 0.066|x4: 0.060|x5: 0.059|x6: 0.061|x7: 0.059|x8: 0.056|x9: 0.062|x10: 0.055|x11: 0.060|x12: 0.060|x13: 0.057|x14: 0.062|x15: 0.057|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.073|x2: 0.232|x3: 0.343|x4: 0.000|x5: 0.092|x6: 0.051|x7: 0.052|x8: 0.163|x9: 0.269|x10: 0.143|x11: 0.168|x12: 0.429|x13: 0.105|x14: 0.198|x15: 0.000|x16: 0.113|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.500|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.018|x2: 0.160|x3: 0.323|x4: 0.074|x5: 0.084|x6: 0.013|x7: 0.048|x8: 0.041|x9: 0.138|x10: 0.060|x11: 0.042|x12: 0.107|x13: 0.052|x14: 0.101|x15: 0.024|x16: 0.048|x17: 0.000
 </t>
         </is>
       </c>
@@ -4451,7 +4451,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>A common barrier to healthcare for psychiatric conditions is the stigma associated with these disorders perceived stigma prevents many from reporting their symptoms stigma is a particularly pervasive problem among military service members preventing them from reporting symptoms of combatrelated conditions like posttraumatic stress disorder ptsd however research shows increased reporting by service members when anonymous assessments are used for example service members report more symptoms of ptsd when they anonymously answer the postdeployment health assessment pdha symptom checklist compared to the official pdha which is identifiable and linked to their military records to investigate the factors that influence reporting of psychological symptoms by service members we used a transformative technology automated virtual humans that interview people about their symptoms such virtual human interviewers allow simultaneous use of two techniques for eliciting disclosure that would otherwise be incompatible they afford anonymity while also building rapport we examined whether virtual human interviewers could increase disclosure of mental health symptoms among activeduty service members that just returned from a yearlong deployment in afghanistan service members reported more symptoms during a conversation with a virtual human interviewer than on the official pdha they also reported more to a virtual human interviewer than on an anonymized pdha a second larger sample of activeduty and former service members found a similar effect that approached statistical significance because respondents in both studies shared more with virtual human interviewers than an anonymized pdhaeven though both conditions control for stigma and ramifications for service members military recordsvirtual human interviewers that build rapport may provide a superior option to encourage reporting</t>
+          <t>a common barrier to healthcare for psychiatric conditions is the stigma associated with these disorders perceived stigma prevents many from reporting their symptoms stigma is a particularly pervasive problem among military service members preventing them from reporting symptoms of combatrelated conditions like posttraumatic stress disorder ptsd however research shows increased reporting by service members when anonymous assessments are used for example service members report more symptoms of ptsd when they anonymously answer the postdeployment health assessment pdha symptom checklist compared to the official pdha which is identifiable and linked to their military records to investigate the factors that influence reporting of psychological symptoms by service members we used a transformative technology automated virtual humans that interview people about their symptoms such virtual human interviewers allow simultaneous use of two techniques for eliciting disclosure that would otherwise be incompatible they afford anonymity while also building rapport we examined whether virtual human interviewers could increase disclosure of mental health symptoms among activeduty service members that just returned from a yearlong deployment in afghanistan service members reported more symptoms during a conversation with a virtual human interviewer than on the official pdha they also reported more to a virtual human interviewer than on an anonymized pdha a second larger sample of activeduty and former service members found a similar effect that approached statistical significance because respondents in both studies shared more with virtual human interviewers than an anonymized pdhaeven though both conditions control for stigma and ramifications for service members military recordsvirtual human interviewers that build rapport may provide a superior option to encourage reporting</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4466,11 +4466,11 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.306|x4: 0.000|x5: 0.000|x6: 0.081|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.202|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.069|x3: 0.259|x4: 0.000|x5: 0.000|x6: 0.082|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.079|x15: 0.000|x16: 0.250|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.221|x3: 0.235|x4: 0.000|x5: 0.068|x6: 0.188|x7: 0.000|x8: 0.078|x9: 0.149|x10: 0.168|x11: 0.000|x12: 0.162|x13: 0.063|x14: 0.116|x15: 0.076|x16: 0.295|x17: 0.000
-TOP2VEC -&gt; x1: 0.109|x2: 0.104|x3: 0.275|x4: 0.000|x5: 0.271|x6: 0.199|x7: 0.118|x8: 0.115|x9: 0.051|x10: 0.127|x11: 0.094|x12: 0.105|x13: 0.142|x14: 0.198|x15: 0.000|x16: 0.260|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.108|x3: 0.272|x4: 0.000|x5: 0.113|x6: 0.156|x7: 0.039|x8: 0.064|x9: 0.067|x10: 0.098|x11: 0.072|x12: 0.089|x13: 0.068|x14: 0.105|x15: 0.025|x16: 0.252|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.070|x4: 0.053|x5: 0.060|x6: 0.063|x7: 0.056|x8: 0.057|x9: 0.057|x10: 0.059|x11: 0.057|x12: 0.058|x13: 0.057|x14: 0.059|x15: 0.055|x16: 0.069|x17: 0.053
+TOP2VEC -&gt; x1: 0.087|x2: 0.105|x3: 0.000|x4: 0.000|x5: 0.121|x6: 0.000|x7: 0.142|x8: 0.090|x9: 0.000|x10: 0.152|x11: 0.051|x12: 0.172|x13: 0.120|x14: 0.133|x15: 0.000|x16: 0.200|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.116|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.022|x2: 0.099|x3: 0.124|x4: 0.000|x5: 0.076|x6: 0.068|x7: 0.036|x8: 0.042|x9: 0.037|x10: 0.080|x11: 0.013|x12: 0.083|x13: 0.046|x14: 0.082|x15: 0.019|x16: 0.311|x17: 0.000
 </t>
         </is>
       </c>
@@ -4481,7 +4481,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>This contribution provides a review of fundamental goals development and future perspectives of driver assistance systems mobility is a fundamental desire of mankind virtually any society strives for safe and efficient mobility at low ecological and economic costs nevertheless its technical implementation significantly differs among societies depending on their culture and their degree of industrialization a potential evolutionary roadmap for driver assistance systems is discussed emerging from systems based on proprioceptive sensors such as abs or esc we review the progress incented by the use of exteroceptive sensors such as radar video or lidar while the ultimate goal of automated and cooperative traffic still remains a vision of the future intermediate steps towards that aim can be realized through systems that mitigate or avoid collisions in selected driving situations research extends the stateoftheart in automated driving in urban traffic and in cooperative driving the latter addressing communication and collaboration between different vehicles as well as cooperative vehicle operation by its driver and its machine intelligence these steps are considered important for the interim period until reliable unsupervised automated driving for all conceivable traffic situations becomes available the prospective evolution of driver assistance systems will be stimulated by several technological societal and market trends the paper closes with a view on current research fields</t>
+          <t>this contribution provides a review of fundamental goals development and future perspectives of driver assistance systems mobility is a fundamental desire of mankind virtually any society strives for safe and efficient mobility at low ecological and economic costs nevertheless its technical implementation significantly differs among societies depending on their culture and their degree of industrialization a potential evolutionary roadmap for driver assistance systems is discussed emerging from systems based on proprioceptive sensors such as abs or esc we review the progress incented by the use of exteroceptive sensors such as radar video or lidar while the ultimate goal of automated and cooperative traffic still remains a vision of the future intermediate steps towards that aim can be realized through systems that mitigate or avoid collisions in selected driving situations research extends the stateoftheart in automated driving in urban traffic and in cooperative driving the latter addressing communication and collaboration between different vehicles as well as cooperative vehicle operation by its driver and its machine intelligence these steps are considered important for the interim period until reliable unsupervised automated driving for all conceivable traffic situations becomes available the prospective evolution of driver assistance systems will be stimulated by several technological societal and market trends the paper closes with a view on current research fields</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4491,16 +4491,16 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>[3, 9, 11]</t>
+          <t>[7, 9, 10, 11]</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.471|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.132|x11: 0.366|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.127|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.142|x10: 0.108|x11: 0.287|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.152|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.257|x8: 0.000|x9: 0.382|x10: 0.180|x11: 0.134|x12: 0.151|x13: 0.188|x14: 0.149|x15: 0.000|x16: 0.227|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.265|x3: 0.175|x4: 0.142|x5: 0.103|x6: 0.000|x7: 0.000|x8: 0.125|x9: 0.221|x10: 0.072|x11: 0.299|x12: 0.311|x13: 0.280|x14: 0.321|x15: 0.192|x16: 0.147|x17: 0.000
-MEAN -&gt; x1: 0.041|x2: 0.088|x3: 0.266|x4: 0.047|x5: 0.034|x6: 0.000|x7: 0.086|x8: 0.042|x9: 0.201|x10: 0.128|x11: 0.266|x12: 0.154|x13: 0.156|x14: 0.157|x15: 0.064|x16: 0.125|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.069|x4: 0.055|x5: 0.054|x6: 0.053|x7: 0.057|x8: 0.055|x9: 0.064|x10: 0.060|x11: 0.069|x12: 0.061|x13: 0.061|x14: 0.061|x15: 0.056|x16: 0.060|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.318|x8: 0.198|x9: 0.251|x10: 0.237|x11: 0.087|x12: 0.095|x13: 0.076|x14: 0.149|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.070|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.144|x8: 0.050|x9: 0.194|x10: 0.131|x11: 0.252|x12: 0.062|x13: 0.066|x14: 0.074|x15: 0.000|x16: 0.057|x17: 0.000
 </t>
         </is>
       </c>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>The discussion about womens access to and use of digital information and communication technologies ict in developing countries has been inconclusive so far some claim that women are rather technophobic and that men are much better users of digital tools while others argue that women enthusiastically embrace digital communication this article puts this question to an empirical test we analyze data sets from 12 latin american and 13 african countries from 200508 this is believed to be the most extensive empirical study in this field so far the results are surprisingly consistent and revealing the reason why fewer women access and use ict is a direct result of their unfavorable conditions with respect to employment education and income when controlling for these variables women turn out to be more active users of digital tools than men this turns the alleged digital gender divide into an opportunity given womens affinity for ict and given that digital technologies are tools that can improve living conditions ict represent a concrete and tangible opportunity to tackle longstanding challenges of gender inequalities in developing countries including access to employment income education and health services</t>
+          <t>the discussion about womens access to and use of digital information and communication technologies ict in developing countries has been inconclusive so far some claim that women are rather technophobic and that men are much better users of digital tools while others argue that women enthusiastically embrace digital communication this article puts this question to an empirical test we analyze data sets from 12 latin american and 13 african countries from 200508 this is believed to be the most extensive empirical study in this field so far the results are surprisingly consistent and revealing the reason why fewer women access and use ict is a direct result of their unfavorable conditions with respect to employment education and income when controlling for these variables women turn out to be more active users of digital tools than men this turns the alleged digital gender divide into an opportunity given womens affinity for ict and given that digital technologies are tools that can improve living conditions ict represent a concrete and tangible opportunity to tackle longstanding challenges of gender inequalities in developing countries including access to employment income education and health services</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4521,16 +4521,16 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>[4, 5, 10]</t>
+          <t>[4, 5, 9, 10]</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.223|x4: 0.143|x5: 0.479|x6: 0.000|x7: 0.000|x8: 0.211|x9: 0.000|x10: 0.456|x11: 0.140|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.153|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.157|x9: 0.120|x10: 0.262|x11: 0.086|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.196|x3: 0.000|x4: 0.394|x5: 0.337|x6: 0.000|x7: 0.078|x8: 0.124|x9: 0.294|x10: 0.279|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.117|x17: 0.000
-TOP2VEC -&gt; x1: 0.127|x2: 0.306|x3: 0.077|x4: 0.424|x5: 0.250|x6: 0.304|x7: 0.344|x8: 0.200|x9: 0.218|x10: 0.000|x11: 0.000|x12: 0.264|x13: 0.000|x14: 0.095|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.042|x2: 0.167|x3: 0.100|x4: 0.321|x5: 0.355|x6: 0.101|x7: 0.141|x8: 0.178|x9: 0.171|x10: 0.245|x11: 0.047|x12: 0.088|x13: 0.000|x14: 0.032|x15: 0.000|x16: 0.039|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.061|x3: 0.057|x4: 0.072|x5: 0.074|x6: 0.057|x7: 0.060|x8: 0.062|x9: 0.062|x10: 0.066|x11: 0.054|x12: 0.057|x13: 0.052|x14: 0.054|x15: 0.052|x16: 0.054|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.056|x3: 0.000|x4: 0.267|x5: 0.190|x6: 0.083|x7: 0.399|x8: 0.107|x9: 0.170|x10: 0.192|x11: 0.161|x12: 0.117|x13: 0.093|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.063|x3: 0.000|x4: 0.204|x5: 0.382|x6: 0.021|x7: 0.119|x8: 0.097|x9: 0.146|x10: 0.183|x11: 0.062|x12: 0.029|x13: 0.023|x14: 0.000|x15: 0.000|x16: 0.029|x17: 0.000
 </t>
         </is>
       </c>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Intelligent tutoring systems its are computer programs that model learners psychological states to provide individualized instruction they have been developed for diverse subject areas eg algebra medicine law reading to help learners acquire domainspecific cognitive and metacognitive knowledge a metaanalysis was conducted on research that compared the outcomes from students learning from its to those learning from nonits learning environments the metaanalysis examined how effect sizes varied with type of its type of comparison treatment received by learners type of learning outcome whether knowledge to be learned was procedural or declarative and other factors after a search of major bibliographic databases 107 effect sizes involving 14321 participants were extracted and analyzed the use of its was associated with greater achievement in comparison with teacherled largegroup instruction g  42 nonits computerbased instruction g  57 and textbooks or workbooks g  35 there was no significant difference between learning from its and learning from individualized human tutoring g  11 or smallgroup instruction g  05 significant positive mean effect sizes were found regardless of whether the its was used as the principal means of instruction a supplement to teacherled instruction an integral component of teacherled instruction or an aid to homework significant positive effect sizes were found at all levels of education in almost all subject domains evaluated and whether or not the its provided feedback or modeled student misconceptions the claim that its are relatively effective tools for learning is consistent with our analysis of potential publication bias</t>
+          <t>intelligent tutoring systems its are computer programs that model learners psychological states to provide individualized instruction they have been developed for diverse subject areas eg algebra medicine law reading to help learners acquire domainspecific cognitive and metacognitive knowledge a metaanalysis was conducted on research that compared the outcomes from students learning from its to those learning from nonits learning environments the metaanalysis examined how effect sizes varied with type of its type of comparison treatment received by learners type of learning outcome whether knowledge to be learned was procedural or declarative and other factors after a search of major bibliographic databases 107 effect sizes involving 14321 participants were extracted and analyzed the use of its was associated with greater achievement in comparison with teacherled largegroup instruction g 42 nonits computerbased instruction g 57 and textbooks or workbooks g 35 there was no significant difference between learning from its and learning from individualized human tutoring g 11 or smallgroup instruction g 05 significant positive mean effect sizes were found regardless of whether the its was used as the principal means of instruction a supplement to teacherled instruction an integral component of teacherled instruction or an aid to homework significant positive effect sizes were found at all levels of education in almost all subject domains evaluated and whether or not the its provided feedback or modeled student misconceptions the claim that its are relatively effective tools for learning is consistent with our analysis of potential publication bias</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4551,16 +4551,16 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>[3, 4]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.368|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.076|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.073|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.254|x3: 0.109|x4: 0.480|x5: 0.074|x6: 0.000|x7: 0.000|x8: 0.091|x9: 0.121|x10: 0.000|x11: 0.000|x12: 0.108|x13: 0.059|x14: 0.213|x15: 0.141|x16: 0.170|x17: 0.000
-TOP2VEC -&gt; x1: 0.118|x2: 0.184|x3: 0.083|x4: 0.442|x5: 0.286|x6: 0.000|x7: 0.207|x8: 0.143|x9: 0.000|x10: 0.091|x11: 0.104|x12: 0.152|x13: 0.077|x14: 0.118|x15: 0.000|x16: 0.187|x17: 0.000
-MEAN -&gt; x1: 0.039|x2: 0.146|x3: 0.223|x4: 0.430|x5: 0.120|x6: 0.000|x7: 0.069|x8: 0.078|x9: 0.040|x10: 0.030|x11: 0.126|x12: 0.087|x13: 0.045|x14: 0.110|x15: 0.047|x16: 0.119|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.061|x3: 0.066|x4: 0.081|x5: 0.060|x6: 0.053|x7: 0.057|x8: 0.057|x9: 0.055|x10: 0.055|x11: 0.060|x12: 0.058|x13: 0.055|x14: 0.059|x15: 0.055|x16: 0.060|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.393|x5: 0.144|x6: 0.000|x7: 0.065|x8: 0.000|x9: 0.056|x10: 0.057|x11: 0.165|x12: 0.103|x13: 0.067|x14: 0.086|x15: 0.097|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.500|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.063|x3: 0.027|x4: 0.468|x5: 0.054|x6: 0.000|x7: 0.016|x8: 0.023|x9: 0.063|x10: 0.014|x11: 0.041|x12: 0.053|x13: 0.032|x14: 0.075|x15: 0.078|x16: 0.043|x17: 0.000
 </t>
         </is>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>In line with a long research tradition focused on the use of information and communication technology for development ict4d we explore the role of artificial intelligence ai4d we start with a rather technical review of four of the characteristic traits of deep learning technologies which leads to natural metaphors for international development based on the empirical evidence of 24 case studies we derive four characteristics of the use of ai4d that align with the four technological traits in isolation each one of them presents a plethora of opportunities to contribute to international development especially to the attainment of the sustainable development goals sdgs however in combination they create a clear tension between a looming threat of a hegemonic intelligence indoctrination pushed by global economies of scale and the potential promise to not only honor but to celebrate local diversity with the help of flexible ai designs we conclude that the latter cannot be achieved without an active public policy dialogue on the international level and a determined effort on the national levels especially in developing countries the study provides terminology and concepts to identify and frame the arising discussions</t>
+          <t>in line with a long research tradition focused on the use of information and communication technology for development ict4d we explore the role of artificial intelligence ai4d we start with a rather technical review of four of the characteristic traits of deep learning technologies which leads to natural metaphors for international development based on the empirical evidence of 24 case studies we derive four characteristics of the use of ai4d that align with the four technological traits in isolation each one of them presents a plethora of opportunities to contribute to international development especially to the attainment of the sustainable development goals sdgs however in combination they create a clear tension between a looming threat of a hegemonic intelligence indoctrination pushed by global economies of scale and the potential promise to not only honor but to celebrate local diversity with the help of flexible ai designs we conclude that the latter cannot be achieved without an active public policy dialogue on the international level and a determined effort on the national levels especially in developing countries the study provides terminology and concepts to identify and frame the arising discussions</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4586,11 +4586,11 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.055|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.074|x10: 0.372|x11: 0.282|x12: 0.131|x13: 0.065|x14: 0.096|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.106|x3: 0.000|x4: 0.134|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.207|x10: 0.259|x11: 0.123|x12: 0.108|x13: 0.000|x14: 0.114|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.095|x3: 0.000|x4: 0.375|x5: 0.000|x6: 0.000|x7: 0.087|x8: 0.153|x9: 0.326|x10: 0.000|x11: 0.000|x12: 0.140|x13: 0.000|x14: 0.409|x15: 0.086|x16: 0.150|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.356|x3: 0.000|x4: 0.519|x5: 0.201|x6: 0.000|x7: 0.182|x8: 0.271|x9: 0.350|x10: 0.099|x11: 0.000|x12: 0.178|x13: 0.289|x14: 0.379|x15: 0.228|x16: 0.203|x17: 0.000
-MEAN -&gt; x1: 0.074|x2: 0.150|x3: 0.159|x4: 0.310|x5: 0.067|x6: 0.000|x7: 0.090|x8: 0.141|x9: 0.250|x10: 0.157|x11: 0.094|x12: 0.149|x13: 0.118|x14: 0.295|x15: 0.105|x16: 0.118|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.060|x4: 0.070|x5: 0.055|x6: 0.051|x7: 0.056|x8: 0.059|x9: 0.066|x10: 0.060|x11: 0.056|x12: 0.060|x13: 0.058|x14: 0.069|x15: 0.057|x16: 0.058|x17: 0.051
+TOP2VEC -&gt; x1: 0.079|x2: 0.000|x3: 0.000|x4: 0.328|x5: 0.000|x6: 0.000|x7: 0.286|x8: 0.000|x9: 0.089|x10: 0.071|x11: 0.172|x12: 0.226|x13: 0.181|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.113|x9: 0.392|x10: 0.101|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.020|x2: 0.050|x3: 0.000|x4: 0.209|x5: 0.000|x6: 0.000|x7: 0.093|x8: 0.066|x9: 0.253|x10: 0.108|x11: 0.074|x12: 0.119|x13: 0.045|x14: 0.131|x15: 0.021|x16: 0.038|x17: 0.000
 </t>
         </is>
       </c>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Protecting the worlds freshwater resources requires diagnosing threats over a broad range of scales fromglobal to local here we present the first worldwide synthesis to jointly consider human and biodiversity perspectives on water security using a spatial framework that quantifies multiple stressors and accounts for downstream impacts we find that nearly 80 of the worlds population is exposed to high levels of threat to water security massive investment in water technology enables rich nations to offset high stressor levels without remedying their underlying causes whereas less wealthy nations remain vulnerable a similar lack of precautionary investment jeopardizes biodiversity with habitats associated with 65 of continental discharge classified as moderately to highly threatened the cumulative threat framework offers a tool for prioritizing policy and management responses to this crisis and underscores the necessity of limiting threats at their source instead of through costly remediation of symptoms in order to assure global water security for both humans and freshwater biodiversity</t>
+          <t>protecting the worlds freshwater resources requires diagnosing threats over a broad range of scales fromglobal to local here we present the first worldwide synthesis to jointly consider human and biodiversity perspectives on water security using a spatial framework that quantifies multiple stressors and accounts for downstream impacts we find that nearly 80 of the worlds population is exposed to high levels of threat to water security massive investment in water technology enables rich nations to offset high stressor levels without remedying their underlying causes whereas less wealthy nations remain vulnerable a similar lack of precautionary investment jeopardizes biodiversity with habitats associated with 65 of continental discharge classified as moderately to highly threatened the cumulative threat framework offers a tool for prioritizing policy and management responses to this crisis and underscores the necessity of limiting threats at their source instead of through costly remediation of symptoms in order to assure global water security for both humans and freshwater biodiversity</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4616,11 +4616,11 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.132|x4: 0.000|x5: 0.000|x6: 0.741|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.076|x12: 0.000|x13: 0.125|x14: 0.148|x15: 0.278|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.060|x2: 0.122|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.500|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.058|x14: 0.091|x15: 0.445|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.188|x4: 0.135|x5: 0.000|x6: 0.192|x7: 0.083|x8: 0.109|x9: 0.000|x10: 0.000|x11: 0.114|x12: 0.000|x13: 0.203|x14: 0.438|x15: 0.358|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.163|x2: 0.361|x3: 0.000|x4: 0.088|x5: 0.064|x6: 0.208|x7: 0.224|x8: 0.151|x9: 0.114|x10: 0.000|x11: 0.128|x12: 0.208|x13: 0.324|x14: 0.260|x15: 0.369|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.054|x2: 0.120|x3: 0.107|x4: 0.074|x5: 0.021|x6: 0.300|x7: 0.102|x8: 0.087|x9: 0.038|x10: 0.000|x11: 0.106|x12: 0.069|x13: 0.217|x14: 0.282|x15: 0.335|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.059|x3: 0.058|x4: 0.056|x5: 0.053|x6: 0.071|x7: 0.058|x8: 0.057|x9: 0.054|x10: 0.052|x11: 0.058|x12: 0.056|x13: 0.065|x14: 0.069|x15: 0.073|x16: 0.052|x17: 0.052
+TOP2VEC -&gt; x1: 0.103|x2: 0.330|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.155|x7: 0.191|x8: 0.075|x9: 0.107|x10: 0.000|x11: 0.145|x12: 0.194|x13: 0.343|x14: 0.150|x15: 0.277|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.041|x2: 0.113|x3: 0.047|x4: 0.034|x5: 0.000|x6: 0.212|x7: 0.069|x8: 0.046|x9: 0.027|x10: 0.000|x11: 0.065|x12: 0.048|x13: 0.151|x14: 0.170|x15: 0.395|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Although storytelling often has negative connotations within science narrative formats of communication should not be disregarded when communicating science to nonexpert audiences narratives offer increased comprehension interest and engagement nonexperts get most of their science information from mass media content which is itself already biased toward narrative formats narratives are also intrinsically persuasive which offers science communicators tactics for persuading otherwise resistant audiences although such use also raises ethical considerations future intersections of narrative research with ongoing discussions in science communication are introduced</t>
+          <t>although storytelling often has negative connotations within science narrative formats of communication should not be disregarded when communicating science to nonexpert audiences narratives offer increased comprehension interest and engagement nonexperts get most of their science information from mass media content which is itself already biased toward narrative formats narratives are also intrinsically persuasive which offers science communicators tactics for persuading otherwise resistant audiences although such use also raises ethical considerations future intersections of narrative research with ongoing discussions in science communication are introduced</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4641,16 +4641,16 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>[9, 14]</t>
+          <t>[7, 9, 13, 14]</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.158|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.091|x12: 0.000|x13: 0.000|x14: 0.097|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.212|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.162|x8: 0.206|x9: 0.602|x10: 0.053|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.414|x15: 0.101|x16: 0.069|x17: 0.000
-TOP2VEC -&gt; x1: 0.242|x2: 0.327|x3: 0.225|x4: 0.000|x5: 0.346|x6: 0.000|x7: 0.221|x8: 0.256|x9: 0.344|x10: 0.108|x11: 0.269|x12: 0.166|x13: 0.457|x14: 0.531|x15: 0.332|x16: 0.222|x17: 0.000
-MEAN -&gt; x1: 0.081|x2: 0.109|x3: 0.198|x4: 0.000|x5: 0.115|x6: 0.000|x7: 0.128|x8: 0.154|x9: 0.281|x10: 0.054|x11: 0.120|x12: 0.055|x13: 0.152|x14: 0.337|x15: 0.145|x16: 0.097|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.058|x3: 0.063|x4: 0.052|x5: 0.058|x6: 0.052|x7: 0.059|x8: 0.061|x9: 0.069|x10: 0.055|x11: 0.059|x12: 0.055|x13: 0.061|x14: 0.073|x15: 0.060|x16: 0.057|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.106|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.122|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.212|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.162|x8: 0.206|x9: 0.500|x10: 0.053|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.414|x15: 0.101|x16: 0.069|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.156|x4: 0.000|x5: 0.000|x6: 0.065|x7: 0.253|x8: 0.000|x9: 0.250|x10: 0.261|x11: 0.114|x12: 0.110|x13: 0.341|x14: 0.223|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.251|x2: 0.187|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.083|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.122|x12: 0.089|x13: 0.252|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.063|x2: 0.047|x3: 0.092|x4: 0.000|x5: 0.000|x6: 0.016|x7: 0.125|x8: 0.051|x9: 0.214|x10: 0.079|x11: 0.059|x12: 0.050|x13: 0.148|x14: 0.190|x15: 0.025|x16: 0.017|x17: 0.000
 </t>
         </is>
       </c>
@@ -4661,7 +4661,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Reliable data on economic livelihoods remain scarce in the developing world hampering efforts to study these outcomes and to design policies that improve them here we demonstrate an accurate inexpensive and scalable method for estimating consumption expenditure and asset wealth from highresolution satellite imagery using survey and satellite data from five african countriesnigeriatanzania uganda malawi and rwandawe show how a convolutional neural network can be trained to identify image features that can explain up to 75of the variation in locallevel economic outcomes our method which requires only publicly available data could transform efforts to track and target poverty in developing countries it also demonstrates how powerful machine learning techniques can be applied in a setting with limited training data suggesting broad potential application across many scientific domains</t>
+          <t>reliable data on economic livelihoods remain scarce in the developing world hampering efforts to study these outcomes and to design policies that improve them here we demonstrate an accurate inexpensive and scalable method for estimating consumption expenditure and asset wealth from highresolution satellite imagery using survey and satellite data from five african countriesnigeriatanzania uganda malawi and rwandawe show how a convolutional neural network can be trained to identify image features that can explain up to 75of the variation in locallevel economic outcomes our method which requires only publicly available data could transform efforts to track and target poverty in developing countries it also demonstrates how powerful machine learning techniques can be applied in a setting with limited training data suggesting broad potential application across many scientific domains</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4671,16 +4671,16 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>[4, 9]</t>
+          <t>[1, 4, 9, 10]</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.114|x2: 0.000|x3: 0.543|x4: 0.066|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.262|x11: 0.314|x12: 0.096|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.189|x2: 0.000|x3: 0.000|x4: 0.195|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.093|x10: 0.297|x11: 0.000|x12: 0.134|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.067|x2: 0.221|x3: 0.063|x4: 0.338|x5: 0.054|x6: 0.000|x7: 0.100|x8: 0.130|x9: 0.375|x10: 0.216|x11: 0.000|x12: 0.000|x13: 0.054|x14: 0.000|x15: 0.132|x16: 0.071|x17: 0.000
-TOP2VEC -&gt; x1: 0.163|x2: 0.000|x3: 0.000|x4: 0.689|x5: 0.312|x6: 0.000|x7: 0.389|x8: 0.212|x9: 0.422|x10: 0.085|x11: 0.000|x12: 0.000|x13: 0.267|x14: 0.229|x15: 0.079|x16: 0.174|x17: 0.000
-MEAN -&gt; x1: 0.115|x2: 0.074|x3: 0.188|x4: 0.301|x5: 0.122|x6: 0.000|x7: 0.163|x8: 0.114|x9: 0.266|x10: 0.187|x11: 0.105|x12: 0.032|x13: 0.107|x14: 0.076|x15: 0.070|x16: 0.082|x17: 0.000
-SOFTMAX -&gt; x1: 0.058|x2: 0.056|x3: 0.063|x4: 0.070|x5: 0.059|x6: 0.052|x7: 0.061|x8: 0.058|x9: 0.068|x10: 0.063|x11: 0.058|x12: 0.054|x13: 0.058|x14: 0.056|x15: 0.056|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.265|x2: 0.000|x3: 0.000|x4: 0.426|x5: 0.189|x6: 0.000|x7: 0.146|x8: 0.168|x9: 0.167|x10: 0.319|x11: 0.090|x12: 0.087|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.172|x17: 0.000
+BERTOPIC -&gt; x1: 0.133|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.075|x9: 0.000|x10: 0.103|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.163|x2: 0.055|x3: 0.016|x4: 0.240|x5: 0.061|x6: 0.000|x7: 0.062|x8: 0.093|x9: 0.159|x10: 0.234|x11: 0.022|x12: 0.055|x13: 0.013|x14: 0.000|x15: 0.033|x16: 0.061|x17: 0.000
 </t>
         </is>
       </c>
@@ -4691,7 +4691,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Just one of todays standard tablet devices possesses the equivalent processing power of more than 5000 desktop computers from the mid1980s the height of the nasa space shuttle programme storing 1gb of data in 1997 would have cost you more than 10000 a year today it costs you approximately 003 in 2001 the first human genome was sequenced it took more than a decade and cost 27 billion today a genome can be sequenced in a few hours and for less than a thousand dollars1 the first app appeared in 2008 when apple founder steve jobs enabled outside developers to create applications for the iphone today not even a decade later the app economy is worth 13 trillion more than the total revenue for the global pharmaceutical market whatsapp which was created in 2009 sends 55 billion messages a day2 news about everything from celebrity gossip to bad air quality now travels fast and globally the forum has termed this period of accelerating innovation in science and technology  the transformative change in data and technology capabilities combined with a merging of digital physical and biological realms  and its impact on society as the fourth industrial revolution it is not only transforming social networks and scientific research it is also radically reshaping the agenda for industries governments and the international community in the same way that the fourth industrial revolution is reshaping healthcare mobility and education systems worldwide it can reshape how the environmental community and its related institutions work scientists tell us we are facing more and more urgent global environmental challenges than ever before this is despite all the international environmental agreements that have been established since the 1970s environmental professionals are aware they cannot be complacent the policybased and institutional approaches that worked 40 years ago are necessary but no longer appear sufficient on their own to manage our growing environmental challenges while their goals and targets are often sound their ability to deliver the environmental outcomes required needs to be augmented as a result there is increasing interest and great potential in exploring how the science data and technology innovations driving the fourth industrial revolution could also be applied to improving environmental and natural resource management arrangements this includes through technology and systems innovations that we might not yet even be able to imagine if technology is starting to transform how we look after our health surely it can also be harnessed to help transform how we look after our environment for example where is the wearable tech for measuring not only a persons heart rate but also the quality of the air they breathe there is also a growing realization that these rapid advances in science and technology could also have unintended negative consequences on nature and people which will need to be recognized managed and avoided with new technology comes the need for improved and more agile governance for the fourth industrial revolution to be the first fully sustainable industrial revolution an effective enabling environment approaches that help governments create smart safeguards protocols policies and effective oversight and recourse mechanisms needs to be put in place to avoid any unintended consequences and to ensure that society and nature benefit from this revolution for example if there were wearable sensors to measure the quality of the air people breathe then who would control access to the data that was collected and how would it be used governments civil society and industry have important roles to play to help answer these questions and develop principles and usage guidelines a means of bringing stakeholders together to codevelop ways that make the most of these science and technology developments is needed these will need to help us better understand and manage nature and our environment and avoid creating negative or unforeseen outcomes this focus on developing policy principles must run alongside and interact with any acceleration programmes that promote the innovation and wider deployment of science and technology for environmental management this is the heart of the challenge in practical terms how can the environmental sector be helped to harness the science and technology revolution that is reshaping our wider economy and society so that current arrangements can be enhanced to better manage the environmental systems that sustain planet earth given the increasing pressure nature faces from human activity at the same time how can policy principles and protocols be developed for use across the environmental sector so that risks from these new technologies to individuals society or the environment itself are minimized and the opportunities maximized</t>
+          <t>just one of todays standard tablet devices possesses the equivalent processing power of more than 5000 desktop computers from the mid1980s the height of the nasa space shuttle programme storing 1gb of data in 1997 would have cost you more than 10000 a year today it costs you approximately 003 in 2001 the first human genome was sequenced it took more than a decade and cost 27 billion today a genome can be sequenced in a few hours and for less than a thousand dollars1 the first app appeared in 2008 when apple founder steve jobs enabled outside developers to create applications for the iphone today not even a decade later the app economy is worth 13 trillion more than the total revenue for the global pharmaceutical market whatsapp which was created in 2009 sends 55 billion messages a day2 news about everything from celebrity gossip to bad air quality now travels fast and globally the forum has termed this period of accelerating innovation in science and technology the transformative change in data and technology capabilities combined with a merging of digital physical and biological realms and its impact on society as the fourth industrial revolution it is not only transforming social networks and scientific research it is also radically reshaping the agenda for industries governments and the international community in the same way that the fourth industrial revolution is reshaping healthcare mobility and education systems worldwide it can reshape how the environmental community and its related institutions work scientists tell us we are facing more and more urgent global environmental challenges than ever before this is despite all the international environmental agreements that have been established since the 1970s environmental professionals are aware they cannot be complacent the policybased and institutional approaches that worked 40 years ago are necessary but no longer appear sufficient on their own to manage our growing environmental challenges while their goals and targets are often sound their ability to deliver the environmental outcomes required needs to be augmented as a result there is increasing interest and great potential in exploring how the science data and technology innovations driving the fourth industrial revolution could also be applied to improving environmental and natural resource management arrangements this includes through technology and systems innovations that we might not yet even be able to imagine if technology is starting to transform how we look after our health surely it can also be harnessed to help transform how we look after our environment for example where is the wearable tech for measuring not only a persons heart rate but also the quality of the air they breathe there is also a growing realization that these rapid advances in science and technology could also have unintended negative consequences on nature and people which will need to be recognized managed and avoided with new technology comes the need for improved and more agile governance for the fourth industrial revolution to be the first fully sustainable industrial revolution an effective enabling environment approaches that help governments create smart safeguards protocols policies and effective oversight and recourse mechanisms needs to be put in place to avoid any unintended consequences and to ensure that society and nature benefit from this revolution for example if there were wearable sensors to measure the quality of the air people breathe then who would control access to the data that was collected and how would it be used governments civil society and industry have important roles to play to help answer these questions and develop principles and usage guidelines a means of bringing stakeholders together to codevelop ways that make the most of these science and technology developments is needed these will need to help us better understand and manage nature and our environment and avoid creating negative or unforeseen outcomes this focus on developing policy principles must run alongside and interact with any acceleration programmes that promote the innovation and wider deployment of science and technology for environmental management this is the heart of the challenge in practical terms how can the environmental sector be helped to harness the science and technology revolution that is reshaping our wider economy and society so that current arrangements can be enhanced to better manage the environmental systems that sustain planet earth given the increasing pressure nature faces from human activity at the same time how can policy principles and protocols be developed for use across the environmental sector so that risks from these new technologies to individuals society or the environment itself are minimized and the opportunities maximized</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4701,16 +4701,16 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>[9, 11, 14]</t>
+          <t>[7, 9, 12, 14]</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.062|x2: 0.000|x3: 0.329|x4: 0.000|x5: 0.000|x6: 0.061|x7: 0.141|x8: 0.065|x9: 0.134|x10: 0.147|x11: 0.292|x12: 0.197|x13: 0.089|x14: 0.217|x15: 0.000|x16: 0.100|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.095|x4: 0.065|x5: 0.000|x6: 0.071|x7: 0.149|x8: 0.000|x9: 0.273|x10: 0.000|x11: 0.197|x12: 0.178|x13: 0.000|x14: 0.173|x15: 0.000|x16: 0.077|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.079|x4: 0.112|x5: 0.000|x6: 0.000|x7: 0.165|x8: 0.072|x9: 0.372|x10: 0.076|x11: 0.136|x12: 0.148|x13: 0.062|x14: 0.302|x15: 0.087|x16: 0.210|x17: 0.000
-TOP2VEC -&gt; x1: 0.106|x2: 0.111|x3: 0.000|x4: 0.239|x5: 0.110|x6: 0.000|x7: 0.209|x8: 0.114|x9: 0.225|x10: 0.071|x11: 0.199|x12: 0.068|x13: 0.241|x14: 0.381|x15: 0.207|x16: 0.145|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.037|x3: 0.136|x4: 0.117|x5: 0.037|x6: 0.020|x7: 0.171|x8: 0.084|x9: 0.244|x10: 0.098|x11: 0.209|x12: 0.137|x13: 0.131|x14: 0.300|x15: 0.098|x16: 0.151|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.054|x3: 0.060|x4: 0.059|x5: 0.054|x6: 0.053|x7: 0.062|x8: 0.057|x9: 0.066|x10: 0.057|x11: 0.064|x12: 0.060|x13: 0.059|x14: 0.070|x15: 0.057|x16: 0.061|x17: 0.052
+TOP2VEC -&gt; x1: 0.077|x2: 0.000|x3: 0.000|x4: 0.222|x5: 0.000|x6: 0.000|x7: 0.218|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.082|x12: 0.141|x13: 0.148|x14: 0.250|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.203|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.407|x13: 0.110|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.019|x2: 0.000|x3: 0.043|x4: 0.100|x5: 0.000|x6: 0.018|x7: 0.183|x8: 0.018|x9: 0.161|x10: 0.019|x11: 0.104|x12: 0.218|x13: 0.080|x14: 0.181|x15: 0.022|x16: 0.072|x17: 0.000
 </t>
         </is>
       </c>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>As robots and other computerassisted technologies take over tasks previously performed by labor there is increasing concern about the future of jobs and wages we analyze the effect of the increase in industrial robot usage between 1990 and 2007 on us local labor markets using a model in which robots compete against human labor in the production of different tasks we show that robots may reduce employment and wages and that the local labor market effects of robots can be estimated by regressing the change in employment and wages on the exposure to robots in each local labor marketdefined from the national penetration of robots into each industry and the local distribution of employment across industries using this approach we estimate large and robust negative effects of robots on employment and wages across commuting zones we bolster this evidence by showing that the commuting zones most exposed to robots in the post1990 era do not exhibit any differential trends before 1990 the impact of robots is distinct from the impact of imports from china and mexico the decline of routine jobs offshoring other types of it capital and the total capital stock in fact exposure to robots is only weakly correlated with these other variables according to our estimates one more robot per thousand workers reduces the employment to population ratio by about 018034 percentage points and wages by 02505 percent</t>
+          <t>as robots and other computerassisted technologies take over tasks previously performed by labor there is increasing concern about the future of jobs and wages we analyze the effect of the increase in industrial robot usage between 1990 and 2007 on us local labor markets using a model in which robots compete against human labor in the production of different tasks we show that robots may reduce employment and wages and that the local labor market effects of robots can be estimated by regressing the change in employment and wages on the exposure to robots in each local labor marketdefined from the national penetration of robots into each industry and the local distribution of employment across industries using this approach we estimate large and robust negative effects of robots on employment and wages across commuting zones we bolster this evidence by showing that the commuting zones most exposed to robots in the post1990 era do not exhibit any differential trends before 1990 the impact of robots is distinct from the impact of imports from china and mexico the decline of routine jobs offshoring other types of it capital and the total capital stock in fact exposure to robots is only weakly correlated with these other variables according to our estimates one more robot per thousand workers reduces the employment to population ratio by about 018034 percentage points and wages by 02505 percent</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4731,16 +4731,16 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>[8, 9, 14]</t>
+          <t>[2, 8, 9, 10, 14]</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.203|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.389|x9: 0.099|x10: 0.000|x11: 0.117|x12: 0.000|x13: 0.000|x14: 0.087|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.082|x2: 0.109|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.163|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.074|x14: 0.104|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.271|x3: 0.000|x4: 0.217|x5: 0.000|x6: 0.000|x7: 0.077|x8: 0.096|x9: 0.291|x10: 0.263|x11: 0.000|x12: 0.085|x13: 0.000|x14: 0.350|x15: 0.080|x16: 0.091|x17: 0.000
-TOP2VEC -&gt; x1: 0.087|x2: 0.143|x3: 0.000|x4: 0.217|x5: 0.250|x6: 0.000|x7: 0.103|x8: 0.118|x9: 0.215|x10: 0.100|x11: 0.142|x12: 0.000|x13: 0.116|x14: 0.385|x15: 0.103|x16: 0.206|x17: 0.000
-MEAN -&gt; x1: 0.029|x2: 0.138|x3: 0.068|x4: 0.144|x5: 0.083|x6: 0.000|x7: 0.060|x8: 0.201|x9: 0.202|x10: 0.121|x11: 0.087|x12: 0.028|x13: 0.039|x14: 0.274|x15: 0.061|x16: 0.099|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.061|x3: 0.057|x4: 0.062|x5: 0.058|x6: 0.053|x7: 0.057|x8: 0.065|x9: 0.065|x10: 0.060|x11: 0.058|x12: 0.055|x13: 0.055|x14: 0.070|x15: 0.057|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.146|x2: 0.170|x3: 0.077|x4: 0.185|x5: 0.234|x6: 0.000|x7: 0.000|x8: 0.225|x9: 0.143|x10: 0.313|x11: 0.000|x12: 0.110|x13: 0.000|x14: 0.257|x15: 0.000|x16: 0.100|x17: 0.000
+BERTOPIC -&gt; x1: 0.093|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.000|x10: 0.090|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.081|x2: 0.138|x3: 0.019|x4: 0.100|x5: 0.058|x6: 0.000|x7: 0.019|x8: 0.330|x9: 0.149|x10: 0.166|x11: 0.000|x12: 0.049|x13: 0.019|x14: 0.178|x15: 0.020|x16: 0.048|x17: 0.000
 </t>
         </is>
       </c>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>The time may have finally come for artificial intelligence ai after periods of hype followed by several ai winters over the past 60 years today announcements of technical breakthroughs enabling superhuman performance by machines follow one another in rapid succession ai now powers so many realworld applications ranging from facial recognition to language translators and assistants like siri and alexa that we barely notice it along with these consumer applications companies across sectors are increasingly harnessing ais power in their operations embracing ai promises considerable benefits for businesses and economies through its contributions to productivity growth and innovation already adopters are starting to reap benefits but adoption is still at a relatively early stage and uneven and ai readiness varies widely among companies sectors and countries at the same time ais impact on work is likely to be profound some occupations as well as demand for some skills will decline while others grow and many change as people work alongside everevolving and increasingly capable machines while most scenarios we have developed suggest that more jobs will be created than lost to automation the transition is likely to be disruptive and occupations and skill requirements will shift significantly ai also has the potential to contribute to tackling pressing societal challenges from healthcare to climate change and humanitarian crises but it could also introduce or exacerbate social challenges through its use and misuse and challenges related to bias privacy and cybersecurity given its economic and other benefits policy makers and business leaders should embrace ai but put in place measures to facilitate adoption soften the disruptive transitions that will accompany it and place a new focus on responsible use this briefing note draws on ongoing research by the mckinsey global institute into ai technologies and their uses limitations and impact it concludes with a set of issues that policy makers and business leaders will need to address a list of the main sources used in the note and suggestions for further reading appear at the end</t>
+          <t>the time may have finally come for artificial intelligence ai after periods of hype followed by several ai winters over the past 60 years today announcements of technical breakthroughs enabling superhuman performance by machines follow one another in rapid succession ai now powers so many realworld applications ranging from facial recognition to language translators and assistants like siri and alexa that we barely notice it along with these consumer applications companies across sectors are increasingly harnessing ais power in their operations embracing ai promises considerable benefits for businesses and economies through its contributions to productivity growth and innovation already adopters are starting to reap benefits but adoption is still at a relatively early stage and uneven and ai readiness varies widely among companies sectors and countries at the same time ais impact on work is likely to be profound some occupations as well as demand for some skills will decline while others grow and many change as people work alongside everevolving and increasingly capable machines while most scenarios we have developed suggest that more jobs will be created than lost to automation the transition is likely to be disruptive and occupations and skill requirements will shift significantly ai also has the potential to contribute to tackling pressing societal challenges from healthcare to climate change and humanitarian crises but it could also introduce or exacerbate social challenges through its use and misuse and challenges related to bias privacy and cybersecurity given its economic and other benefits policy makers and business leaders should embrace ai but put in place measures to facilitate adoption soften the disruptive transitions that will accompany it and place a new focus on responsible use this briefing note draws on ongoing research by the mckinsey global institute into ai technologies and their uses limitations and impact it concludes with a set of issues that policy makers and business leaders will need to address a list of the main sources used in the note and suggestions for further reading appear at the end</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4761,16 +4761,16 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>[3, 8, 9, 13]</t>
+          <t>[8, 9]</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.076|x2: 0.000|x3: 0.361|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.077|x8: 0.203|x9: 0.081|x10: 0.000|x11: 0.232|x12: 0.127|x13: 0.369|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.113|x8: 0.228|x9: 0.199|x10: 0.000|x11: 0.141|x12: 0.067|x13: 0.205|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.174|x4: 0.063|x5: 0.000|x6: 0.000|x7: 0.081|x8: 0.347|x9: 0.308|x10: 0.084|x11: 0.098|x12: 0.072|x13: 0.212|x14: 0.058|x15: 0.201|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.221|x2: 0.172|x3: 0.097|x4: 0.261|x5: 0.304|x6: 0.000|x7: 0.347|x8: 0.252|x9: 0.259|x10: 0.092|x11: 0.000|x12: 0.328|x13: 0.316|x14: 0.293|x15: 0.158|x16: 0.189|x17: 0.000
-MEAN -&gt; x1: 0.099|x2: 0.057|x3: 0.211|x4: 0.108|x5: 0.101|x6: 0.000|x7: 0.169|x8: 0.267|x9: 0.216|x10: 0.059|x11: 0.110|x12: 0.176|x13: 0.299|x14: 0.117|x15: 0.120|x16: 0.103|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.055|x3: 0.064|x4: 0.057|x5: 0.057|x6: 0.051|x7: 0.061|x8: 0.067|x9: 0.064|x10: 0.055|x11: 0.057|x12: 0.061|x13: 0.069|x14: 0.058|x15: 0.058|x16: 0.057|x17: 0.051
+TOP2VEC -&gt; x1: 0.060|x2: 0.000|x3: 0.000|x4: 0.281|x5: 0.121|x6: 0.000|x7: 0.228|x8: 0.125|x9: 0.150|x10: 0.188|x11: 0.237|x12: 0.136|x13: 0.000|x14: 0.000|x15: 0.077|x16: 0.085|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.168|x9: 0.302|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.015|x2: 0.000|x3: 0.044|x4: 0.086|x5: 0.030|x6: 0.000|x7: 0.106|x8: 0.217|x9: 0.240|x10: 0.068|x11: 0.119|x12: 0.069|x13: 0.104|x14: 0.015|x15: 0.070|x16: 0.052|x17: 0.000
 </t>
         </is>
       </c>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>In recent years there has been a revival of concerns that automation and digitalisation might after all result in a jobless future the debate has been fuelled by studies for the us and europe arguing that a substantial share of jobs is at risk of computerisation these studies follow an occupationbased approach proposed by frey and osborne 2013 ie they assume that whole occupations rather than single jobtasks are automated by technology as we argue this might lead to an overestimation of job automatibility as occupations labelled as highrisk occupations often still contain a substantial share of tasks that are hard to automate our paper serves two purposes firstly we estimate the job automatibility of jobs for 21 oecd countries based on a taskbased approach in contrast to other studies we take into account the heterogeneity of workers tasks within occupations overall we find that on average across the 21 oecd countries 9  of jobs are automatable the threat from technological advances thus seems much less pronounced compared to the occupationbased approach we further find heterogeneities across oecd countries for instance while the share of automatable jobs is 6  in korea the corresponding share is 12  in austria differences between countries may reflect general differences in workplace organisation differences in previous investments into automation technologies as well as differences in the education of workers across countries the second purpose of this paper is to critically reflect on the recent line of studies that generate figures on the risk of computerisation and to provide a comprehensive discussion on possible adjustment processes of firms and workers to automation and digitalisation in particular we argue that the estimated share of jobs at risk must not be equated with actual or expected employment losses from technological advances for three reasons first the utilisation of new technologies is a slow process due to economic legal and societal hurdles so that technological substitution often does not take place as expected second even if new technologies are introduced workers can adjust to changing technological endowments by switching tasks thus preventing technological unemployment third technological change also generates additional jobs through demand for new technologies and through higher competitiveness the main conclusion from our paper is that automation and digitalisation are unlikely to destroy large numbers of jobs however low qualified workers are likely to bear the brunt of the adjustment costs as the automatibility of their jobs is higher compared to highly qualified workers therefore the likely challenge for the future lies in coping with rising inequality and ensuring sufficient retraining especially for low qualified workers</t>
+          <t>in recent years there has been a revival of concerns that automation and digitalisation might after all result in a jobless future the debate has been fuelled by studies for the us and europe arguing that a substantial share of jobs is at risk of computerisation these studies follow an occupationbased approach proposed by frey and osborne 2013 ie they assume that whole occupations rather than single jobtasks are automated by technology as we argue this might lead to an overestimation of job automatibility as occupations labelled as highrisk occupations often still contain a substantial share of tasks that are hard to automate our paper serves two purposes firstly we estimate the job automatibility of jobs for 21 oecd countries based on a taskbased approach in contrast to other studies we take into account the heterogeneity of workers tasks within occupations overall we find that on average across the 21 oecd countries 9 of jobs are automatable the threat from technological advances thus seems much less pronounced compared to the occupationbased approach we further find heterogeneities across oecd countries for instance while the share of automatable jobs is 6 in korea the corresponding share is 12 in austria differences between countries may reflect general differences in workplace organisation differences in previous investments into automation technologies as well as differences in the education of workers across countries the second purpose of this paper is to critically reflect on the recent line of studies that generate figures on the risk of computerisation and to provide a comprehensive discussion on possible adjustment processes of firms and workers to automation and digitalisation in particular we argue that the estimated share of jobs at risk must not be equated with actual or expected employment losses from technological advances for three reasons first the utilisation of new technologies is a slow process due to economic legal and societal hurdles so that technological substitution often does not take place as expected second even if new technologies are introduced workers can adjust to changing technological endowments by switching tasks thus preventing technological unemployment third technological change also generates additional jobs through demand for new technologies and through higher competitiveness the main conclusion from our paper is that automation and digitalisation are unlikely to destroy large numbers of jobs however low qualified workers are likely to bear the brunt of the adjustment costs as the automatibility of their jobs is higher compared to highly qualified workers therefore the likely challenge for the future lies in coping with rising inequality and ensuring sufficient retraining especially for low qualified workers</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4791,16 +4791,16 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>[3, 8]</t>
+          <t>[8, 9]</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.119|x2: 0.000|x3: 0.360|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.433|x9: 0.000|x10: 0.225|x11: 0.208|x12: 0.000|x13: 0.059|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.154|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.500|x9: 0.181|x10: 0.089|x11: 0.106|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.110|x3: 0.207|x4: 0.169|x5: 0.000|x6: 0.000|x7: 0.146|x8: 0.397|x9: 0.275|x10: 0.206|x11: 0.000|x12: 0.070|x13: 0.052|x14: 0.068|x15: 0.000|x16: 0.119|x17: 0.000
-TOP2VEC -&gt; x1: 0.212|x2: 0.129|x3: 0.124|x4: 0.370|x5: 0.166|x6: 0.000|x7: 0.193|x8: 0.275|x9: 0.182|x10: 0.000|x11: 0.097|x12: 0.099|x13: 0.125|x14: 0.071|x15: 0.000|x16: 0.079|x17: 0.000
-MEAN -&gt; x1: 0.110|x2: 0.080|x3: 0.230|x4: 0.180|x5: 0.055|x6: 0.000|x7: 0.113|x8: 0.369|x9: 0.152|x10: 0.144|x11: 0.102|x12: 0.056|x13: 0.079|x14: 0.046|x15: 0.000|x16: 0.066|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.057|x3: 0.066|x4: 0.063|x5: 0.056|x6: 0.053|x7: 0.059|x8: 0.076|x9: 0.061|x10: 0.061|x11: 0.058|x12: 0.056|x13: 0.057|x14: 0.055|x15: 0.053|x16: 0.056|x17: 0.053
+TOP2VEC -&gt; x1: 0.140|x2: 0.000|x3: 0.070|x4: 0.215|x5: 0.000|x6: 0.067|x7: 0.106|x8: 0.314|x9: 0.228|x10: 0.000|x11: 0.064|x12: 0.174|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.150|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.488|x9: 0.000|x10: 0.154|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.111|x2: 0.028|x3: 0.069|x4: 0.096|x5: 0.000|x6: 0.017|x7: 0.063|x8: 0.425|x9: 0.171|x10: 0.112|x11: 0.042|x12: 0.061|x13: 0.013|x14: 0.017|x15: 0.000|x16: 0.030|x17: 0.000
 </t>
         </is>
       </c>
@@ -4826,11 +4826,11 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.330|x4: 0.000|x5: 0.000|x6: 0.088|x7: 0.000|x8: 0.000|x9: 0.201|x10: 0.000|x11: 0.191|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.054|x4: 0.087|x5: 0.165|x6: 0.111|x7: 0.191|x8: 0.062|x9: 0.552|x10: 0.118|x11: 0.064|x12: 0.064|x13: 0.000|x14: 0.000|x15: 0.209|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.235|x3: 0.000|x4: 0.287|x5: 0.101|x6: 0.097|x7: 0.090|x8: 0.066|x9: 0.426|x10: 0.084|x11: 0.000|x12: 0.188|x13: 0.246|x14: 0.092|x15: 0.276|x16: 0.172|x17: 0.000
-MEAN -&gt; x1: 0.000|x2: 0.078|x3: 0.128|x4: 0.125|x5: 0.089|x6: 0.099|x7: 0.094|x8: 0.043|x9: 0.376|x10: 0.067|x11: 0.085|x12: 0.084|x13: 0.082|x14: 0.031|x15: 0.162|x16: 0.105|x17: 0.000
-SOFTMAX -&gt; x1: 0.053|x2: 0.058|x3: 0.060|x4: 0.060|x5: 0.058|x6: 0.059|x7: 0.058|x8: 0.056|x9: 0.077|x10: 0.057|x11: 0.058|x12: 0.058|x13: 0.058|x14: 0.055|x15: 0.063|x16: 0.059|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.111|x7: 0.000|x8: 0.000|x9: 0.315|x10: 0.000|x11: 0.065|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.054|x4: 0.087|x5: 0.165|x6: 0.111|x7: 0.191|x8: 0.062|x9: 0.500|x10: 0.118|x11: 0.064|x12: 0.064|x13: 0.000|x14: 0.000|x15: 0.209|x16: 0.143|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.205|x5: 0.000|x6: 0.000|x7: 0.181|x8: 0.000|x9: 0.375|x10: 0.000|x11: 0.111|x12: 0.127|x13: 0.000|x14: 0.140|x15: 0.153|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.014|x4: 0.073|x5: 0.041|x6: 0.056|x7: 0.093|x8: 0.016|x9: 0.422|x10: 0.029|x11: 0.060|x12: 0.048|x13: 0.000|x14: 0.035|x15: 0.091|x16: 0.036|x17: 0.000
 </t>
         </is>
       </c>
@@ -4841,7 +4841,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>The 2030 agenda is enthusiastic about the great potential for accelerating human progress brought by information and communications technology and global interconnectedness at the same time however the un now acknowledges the dark side of innovation and the new challenges of cybersecurity threats the risks to jobs and privacy unleashed by artificial intelligence and the use of military related cyber operations and cyberattacks as with climate change increasing inequalities or power concentration those challenges cannot be solved by countries acting in isolation and urgently require strengthened multilateralism at the same time a major technological shift is necessary to implement the global transition  required by the 2030 agenda  towards less resourceintensive and more resilient economic and social development models most of that technology already exists but new strategies are needed to generalize it at global level</t>
+          <t>the 2030 agenda is enthusiastic about the great potential for accelerating human progress brought by information and communications technology and global interconnectedness at the same time however the un now acknowledges the dark side of innovation and the new challenges of cybersecurity threats the risks to jobs and privacy unleashed by artificial intelligence and the use of military related cyber operations and cyberattacks as with climate change increasing inequalities or power concentration those challenges cannot be solved by countries acting in isolation and urgently require strengthened multilateralism at the same time a major technological shift is necessary to implement the global transition required by the 2030 agenda towards less resourceintensive and more resilient economic and social development models most of that technology already exists but new strategies are needed to generalize it at global level</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4851,16 +4851,16 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>[7, 9, 13]</t>
+          <t>[9, 13]</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.061|x2: 0.000|x3: 0.308|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.115|x8: 0.148|x9: 0.131|x10: 0.065|x11: 0.220|x12: 0.000|x13: 0.543|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.217|x2: 0.000|x3: 0.201|x4: 0.000|x5: 0.000|x6: 0.103|x7: 0.169|x8: 0.000|x9: 0.638|x10: 0.000|x11: 0.000|x12: 0.097|x13: 0.252|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000
-TOP2VEC -&gt; x1: 0.140|x2: 0.000|x3: 0.000|x4: 0.154|x5: 0.000|x6: 0.218|x7: 0.616|x8: 0.139|x9: 0.629|x10: 0.000|x11: 0.373|x12: 0.265|x13: 0.572|x14: 0.230|x15: 0.277|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.139|x2: 0.000|x3: 0.169|x4: 0.051|x5: 0.000|x6: 0.107|x7: 0.261|x8: 0.096|x9: 0.377|x10: 0.022|x11: 0.198|x12: 0.121|x13: 0.417|x14: 0.077|x15: 0.092|x16: 0.048|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.051|x3: 0.061|x4: 0.054|x5: 0.051|x6: 0.057|x7: 0.067|x8: 0.057|x9: 0.075|x10: 0.052|x11: 0.063|x12: 0.058|x13: 0.078|x14: 0.055|x15: 0.056|x16: 0.054|x17: 0.051
+          <t xml:space="preserve">NMF -&gt; x1: 0.101|x2: 0.000|x3: 0.088|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.138|x8: 0.177|x9: 0.220|x10: 0.000|x11: 0.079|x12: 0.000|x13: 0.408|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.217|x2: 0.000|x3: 0.201|x4: 0.000|x5: 0.000|x6: 0.103|x7: 0.169|x8: 0.000|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.097|x13: 0.252|x14: 0.000|x15: 0.000|x16: 0.143|x17: 0.000
+TOP2VEC -&gt; x1: 0.114|x2: 0.000|x3: 0.000|x4: 0.068|x5: 0.000|x6: 0.000|x7: 0.149|x8: 0.000|x9: 0.358|x10: 0.213|x11: 0.109|x12: 0.051|x13: 0.226|x14: 0.062|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.108|x2: 0.000|x3: 0.072|x4: 0.017|x5: 0.000|x6: 0.026|x7: 0.114|x8: 0.044|x9: 0.269|x10: 0.053|x11: 0.047|x12: 0.037|x13: 0.221|x14: 0.015|x15: 0.000|x16: 0.036|x17: 0.000
 </t>
         </is>
       </c>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Advocates of algorithmic techniques like data mining argue that these techniques eliminate human biases from the decisionmaking process but an algorithm is only as good as the data it works with data is frequently imperfect in ways that allow these algorithms to inherit the prejudices of prior decision makers in other cases data may simply reflect the widespread biases that persist in society at large in still others data mining can discover surprisingly useful regularities that are really just preexisting patterns of exclusion and inequality unthinking reliance on data mining can deny historically disadvantaged and vulnerable groups full participation in society worse still because the resulting discrimination is almost always an unintentional emergent property of the algorithms use rather than a conscious choice by its programmers it can be unusually hard to identify the source of the problem or to explain it to a court</t>
+          <t>advocates of algorithmic techniques like data mining argue that these techniques eliminate human biases from the decisionmaking process but an algorithm is only as good as the data it works with data is frequently imperfect in ways that allow these algorithms to inherit the prejudices of prior decision makers in other cases data may simply reflect the widespread biases that persist in society at large in still others data mining can discover surprisingly useful regularities that are really just preexisting patterns of exclusion and inequality unthinking reliance on data mining can deny historically disadvantaged and vulnerable groups full participation in society worse still because the resulting discrimination is almost always an unintentional emergent property of the algorithms use rather than a conscious choice by its programmers it can be unusually hard to identify the source of the problem or to explain it to a court</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4881,16 +4881,16 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>[3, 4, 5]</t>
+          <t>[5, 16]</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.434|x4: 0.000|x5: 0.062|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.251|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.142|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.204|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.151|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.218|x3: 0.166|x4: 0.245|x5: 0.357|x6: 0.132|x7: 0.000|x8: 0.137|x9: 0.000|x10: 0.130|x11: 0.000|x12: 0.000|x13: 0.236|x14: 0.059|x15: 0.000|x16: 0.141|x17: 0.000
-TOP2VEC -&gt; x1: 0.078|x2: 0.182|x3: 0.313|x4: 0.483|x5: 0.527|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.204|x11: 0.237|x12: 0.205|x13: 0.284|x14: 0.251|x15: 0.088|x16: 0.419|x17: 0.000
-MEAN -&gt; x1: 0.026|x2: 0.133|x3: 0.304|x4: 0.242|x5: 0.306|x6: 0.044|x7: 0.000|x8: 0.046|x9: 0.000|x10: 0.112|x11: 0.163|x12: 0.068|x13: 0.173|x14: 0.103|x15: 0.029|x16: 0.187|x17: 0.000
-SOFTMAX -&gt; x1: 0.054|x2: 0.060|x3: 0.071|x4: 0.067|x5: 0.071|x6: 0.055|x7: 0.052|x8: 0.055|x9: 0.052|x10: 0.058|x11: 0.061|x12: 0.056|x13: 0.062|x14: 0.058|x15: 0.054|x16: 0.063|x17: 0.052
+TOP2VEC -&gt; x1: 0.328|x2: 0.243|x3: 0.171|x4: 0.193|x5: 0.102|x6: 0.000|x7: 0.117|x8: 0.193|x9: 0.000|x10: 0.254|x11: 0.244|x12: 0.295|x13: 0.000|x14: 0.220|x15: 0.059|x16: 0.351|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.500|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.094|x17: 0.000
+MEAN -&gt; x1: 0.117|x2: 0.115|x3: 0.084|x4: 0.109|x5: 0.291|x6: 0.033|x7: 0.029|x8: 0.083|x9: 0.000|x10: 0.096|x11: 0.061|x12: 0.074|x13: 0.059|x14: 0.070|x15: 0.015|x16: 0.184|x17: 0.000
 </t>
         </is>
       </c>
@@ -4901,7 +4901,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Globalization have created new opportunities but also difficult problems for community psychologists a economic changes which have created new jobs in different areas of the world and promoted the emergence of a sharing economy but also fostered huge disparities both within and across countries b political changes such as increased polarization and the growth of nationalist and populist parties which amplify divisiveness but go along with a transformation of the notion of citizenship and identity c technological changes brought about by the artificial intelligence revolution which opens up both opportunities and dangers for job prospects and by the diffusion of social networks able of both promoting political participation and increasing political polarization finally aims that community psychologists could pursue to help develop the opportunities and reduce the problems that emerge from these changes are discussed</t>
+          <t>globalization have created new opportunities but also difficult problems for community psychologists a economic changes which have created new jobs in different areas of the world and promoted the emergence of a sharing economy but also fostered huge disparities both within and across countries b political changes such as increased polarization and the growth of nationalist and populist parties which amplify divisiveness but go along with a transformation of the notion of citizenship and identity c technological changes brought about by the artificial intelligence revolution which opens up both opportunities and dangers for job prospects and by the diffusion of social networks able of both promoting political participation and increasing political polarization finally aims that community psychologists could pursue to help develop the opportunities and reduce the problems that emerge from these changes are discussed</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4911,16 +4911,16 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>[3, 8, 13]</t>
+          <t>[5, 8, 13]</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.103|x2: 0.000|x3: 0.287|x4: 0.000|x5: 0.082|x6: 0.000|x7: 0.000|x8: 0.119|x9: 0.000|x10: 0.000|x11: 0.177|x12: 0.000|x13: 0.431|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.110|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.093|x6: 0.000|x7: 0.000|x8: 0.173|x9: 0.091|x10: 0.000|x11: 0.070|x12: 0.000|x13: 0.251|x14: 0.000|x15: 0.095|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.061|x2: 0.000|x3: 0.173|x4: 0.000|x5: 0.251|x6: 0.000|x7: 0.074|x8: 0.331|x9: 0.273|x10: 0.081|x11: 0.112|x12: 0.000|x13: 0.202|x14: 0.063|x15: 0.078|x16: 0.122|x17: 0.000
-TOP2VEC -&gt; x1: 0.166|x2: 0.327|x3: 0.196|x4: 0.347|x5: 0.160|x6: 0.000|x7: 0.000|x8: 0.159|x9: 0.080|x10: 0.098|x11: 0.120|x12: 0.187|x13: 0.286|x14: 0.258|x15: 0.081|x16: 0.201|x17: 0.000
-MEAN -&gt; x1: 0.110|x2: 0.109|x3: 0.218|x4: 0.116|x5: 0.165|x6: 0.000|x7: 0.025|x8: 0.203|x9: 0.118|x10: 0.060|x11: 0.137|x12: 0.062|x13: 0.306|x14: 0.107|x15: 0.053|x16: 0.108|x17: 0.000
-SOFTMAX -&gt; x1: 0.059|x2: 0.058|x3: 0.065|x4: 0.059|x5: 0.062|x6: 0.052|x7: 0.054|x8: 0.064|x9: 0.059|x10: 0.056|x11: 0.060|x12: 0.056|x13: 0.071|x14: 0.058|x15: 0.055|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.237|x5: 0.151|x6: 0.068|x7: 0.164|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.090|x12: 0.118|x13: 0.228|x14: 0.195|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.137|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.229|x9: 0.099|x10: 0.180|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.077|x2: 0.000|x3: 0.043|x4: 0.059|x5: 0.124|x6: 0.017|x7: 0.059|x8: 0.183|x9: 0.116|x10: 0.065|x11: 0.068|x12: 0.030|x13: 0.170|x14: 0.065|x15: 0.043|x16: 0.030|x17: 0.000
 </t>
         </is>
       </c>
@@ -4931,7 +4931,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Advances in artificial intelligence and robotics may be leading to a new industrial revolution this paper presents a model with the minimum necessary features to analyze the implications for inequality and output two assumptions are key robot capital is distinct from traditional capital in its degree of substitutability with human labor and only capitalists and skilled workers save we analyze a range of variants that reflect widely different views of how automation may transform the labor market our main results are surprisingly robust automation is good for growth and bad for equality in the benchmark model real wages fall in the short run and eventually rise but eventually can easily take generations</t>
+          <t>advances in artificial intelligence and robotics may be leading to a new industrial revolution this paper presents a model with the minimum necessary features to analyze the implications for inequality and output two assumptions are key robot capital is distinct from traditional capital in its degree of substitutability with human labor and only capitalists and skilled workers save we analyze a range of variants that reflect widely different views of how automation may transform the labor market our main results are surprisingly robust automation is good for growth and bad for equality in the benchmark model real wages fall in the short run and eventually rise but eventually can easily take generations</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4941,16 +4941,16 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>[3, 7, 9]</t>
+          <t>[7, 8, 9, 10]</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.432|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.205|x9: 0.000|x10: 0.000|x11: 0.249|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.091|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.242|x9: 0.103|x10: 0.000|x11: 0.084|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.134|x3: 0.158|x4: 0.276|x5: 0.161|x6: 0.000|x7: 0.201|x8: 0.000|x9: 0.415|x10: 0.198|x11: 0.000|x12: 0.000|x13: 0.065|x14: 0.119|x15: 0.000|x16: 0.093|x17: 0.000
-TOP2VEC -&gt; x1: 0.167|x2: 0.285|x3: 0.172|x4: 0.151|x5: 0.197|x6: 0.090|x7: 0.400|x8: 0.208|x9: 0.245|x10: 0.113|x11: 0.147|x12: 0.222|x13: 0.197|x14: 0.204|x15: 0.084|x16: 0.231|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.139|x3: 0.254|x4: 0.142|x5: 0.120|x6: 0.030|x7: 0.200|x8: 0.138|x9: 0.220|x10: 0.104|x11: 0.132|x12: 0.074|x13: 0.087|x14: 0.108|x15: 0.028|x16: 0.108|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.067|x4: 0.060|x5: 0.059|x6: 0.054|x7: 0.064|x8: 0.060|x9: 0.065|x10: 0.058|x11: 0.060|x12: 0.056|x13: 0.057|x14: 0.058|x15: 0.054|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.120|x3: 0.000|x4: 0.146|x5: 0.000|x6: 0.000|x7: 0.298|x8: 0.215|x9: 0.098|x10: 0.293|x11: 0.085|x12: 0.086|x13: 0.223|x14: 0.063|x15: 0.000|x16: 0.074|x17: 0.000
+BERTOPIC -&gt; x1: 0.180|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.332|x9: 0.085|x10: 0.182|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.045|x2: 0.063|x3: 0.062|x4: 0.105|x5: 0.040|x6: 0.000|x7: 0.125|x8: 0.197|x9: 0.175|x10: 0.168|x11: 0.042|x12: 0.021|x13: 0.072|x14: 0.046|x15: 0.000|x16: 0.042|x17: 0.000
 </t>
         </is>
       </c>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>This study presents applications of artificial intelligence for development of sustainable transport systems in smart cities in india there is huge gap between the demand and supply of the public transport in most of the urban cities in india due to rapid urbanization india has realize the importance of developing smart cities to improve the quality of life of people and to captivate foreign investment to build superior quality of infrastructure in india the majority of the indian cities are facing the problem of congestion safety inadequate public transport facilities inappropriate information inadequate parking spaces and environmental pollution sustainable transport system can eliminate these problems by providing safer faster comfortable efficient and environment friendly system and can help in development of smart cities by the implementation of intelligent transport system hence there is urgent need to develop intelligent transport system in indian cities which can play a key role in development of sustainable transport system therefore the main requirement is to adopt artificial intelligence for development of smart cities in india the main objective of this article is to present the major application of intelligent transport system for the development of sustainable transport system in smart cities this study can be used in the implementation of intelligent transport system for development of sustainable transport system in smart cities in india</t>
+          <t>this study presents applications of artificial intelligence for development of sustainable transport systems in smart cities in india there is huge gap between the demand and supply of the public transport in most of the urban cities in india due to rapid urbanization india has realize the importance of developing smart cities to improve the quality of life of people and to captivate foreign investment to build superior quality of infrastructure in india the majority of the indian cities are facing the problem of congestion safety inadequate public transport facilities inappropriate information inadequate parking spaces and environmental pollution sustainable transport system can eliminate these problems by providing safer faster comfortable efficient and environment friendly system and can help in development of smart cities by the implementation of intelligent transport system hence there is urgent need to develop intelligent transport system in indian cities which can play a key role in development of sustainable transport system therefore the main requirement is to adopt artificial intelligence for development of smart cities in india the main objective of this article is to present the major application of intelligent transport system for the development of sustainable transport system in smart cities this study can be used in the implementation of intelligent transport system for development of sustainable transport system in smart cities in india</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4976,11 +4976,11 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.197|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 1.154|x12: 0.053|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.280|x4: 0.064|x5: 0.000|x6: 0.000|x7: 0.059|x8: 0.070|x9: 0.222|x10: 0.000|x11: 0.749|x12: 0.072|x13: 0.083|x14: 0.071|x15: 0.071|x16: 0.078|x17: 0.000
-TOP2VEC -&gt; x1: 0.109|x2: 0.000|x3: 0.000|x4: 0.204|x5: 0.000|x6: 0.254|x7: 0.278|x8: 0.000|x9: 0.158|x10: 0.000|x11: 0.734|x12: 0.380|x13: 0.538|x14: 0.258|x15: 0.195|x16: 0.078|x17: 0.000
-MEAN -&gt; x1: 0.036|x2: 0.000|x3: 0.159|x4: 0.089|x5: 0.000|x6: 0.085|x7: 0.112|x8: 0.023|x9: 0.127|x10: 0.000|x11: 0.500|x12: 0.168|x13: 0.194|x14: 0.110|x15: 0.089|x16: 0.052|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.053|x3: 0.062|x4: 0.058|x5: 0.053|x6: 0.057|x7: 0.059|x8: 0.054|x9: 0.060|x10: 0.053|x11: 0.087|x12: 0.062|x13: 0.064|x14: 0.059|x15: 0.058|x16: 0.056|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.094|x10: 0.000|x11: 0.500|x12: 0.057|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.000|x3: 0.280|x4: 0.064|x5: 0.000|x6: 0.000|x7: 0.059|x8: 0.070|x9: 0.222|x10: 0.000|x11: 0.500|x12: 0.072|x13: 0.083|x14: 0.071|x15: 0.071|x16: 0.078|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.299|x8: 0.000|x9: 0.095|x10: 0.000|x11: 0.471|x12: 0.270|x13: 0.085|x14: 0.108|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.500|x12: 0.000|x13: 0.081|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.000|x3: 0.070|x4: 0.016|x5: 0.000|x6: 0.000|x7: 0.090|x8: 0.018|x9: 0.103|x10: 0.000|x11: 0.493|x12: 0.100|x13: 0.062|x14: 0.045|x15: 0.018|x16: 0.019|x17: 0.000
 </t>
         </is>
       </c>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Ecologists have a variety of tools for collecting and analyzing data but relatively few tools that facilitate ecological reasoning up to this time simulation models have been the basic means of organizing ecological knowledge in a way that can be rapidly processed by computer technologies for computerbased manipulation of knowledge have been developed in artificial intelligence the areas of ecological science in which this technology is likely to prove important include modelling and simulation integration of qualitative and quantitative knowledge theoretical development and natural resource management researchers and managers in both basic and applied ecology will be affected by these developments as aiderived technologies are added to the ecological toolkit</t>
+          <t>ecologists have a variety of tools for collecting and analyzing data but relatively few tools that facilitate ecological reasoning up to this time simulation models have been the basic means of organizing ecological knowledge in a way that can be rapidly processed by computer technologies for computerbased manipulation of knowledge have been developed in artificial intelligence the areas of ecological science in which this technology is likely to prove important include modelling and simulation integration of qualitative and quantitative knowledge theoretical development and natural resource management researchers and managers in both basic and applied ecology will be affected by these developments as aiderived technologies are added to the ecological toolkit</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5001,16 +5001,16 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>[6, 9, 14]</t>
+          <t>[7, 9, 14, 15]</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.417|x4: 0.000|x5: 0.000|x6: 0.081|x7: 0.000|x8: 0.000|x9: 0.154|x10: 0.071|x11: 0.241|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.069|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.090|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.252|x7: 0.137|x8: 0.088|x9: 0.511|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.058|x14: 0.285|x15: 0.400|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.094|x2: 0.408|x3: 0.000|x4: 0.389|x5: 0.286|x6: 0.278|x7: 0.407|x8: 0.129|x9: 0.347|x10: 0.000|x11: 0.000|x12: 0.100|x13: 0.191|x14: 0.540|x15: 0.000|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.061|x2: 0.136|x3: 0.139|x4: 0.130|x5: 0.095|x6: 0.204|x7: 0.181|x8: 0.072|x9: 0.334|x10: 0.024|x11: 0.080|x12: 0.033|x13: 0.083|x14: 0.262|x15: 0.156|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.060|x3: 0.060|x4: 0.059|x5: 0.057|x6: 0.064|x7: 0.062|x8: 0.056|x9: 0.073|x10: 0.053|x11: 0.056|x12: 0.054|x13: 0.057|x14: 0.068|x15: 0.061|x16: 0.052|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.112|x7: 0.000|x8: 0.000|x9: 0.250|x10: 0.089|x11: 0.000|x12: 0.087|x13: 0.000|x14: 0.000|x15: 0.165|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.090|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.252|x7: 0.137|x8: 0.088|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.058|x14: 0.285|x15: 0.400|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.096|x5: 0.086|x6: 0.000|x7: 0.343|x8: 0.000|x9: 0.133|x10: 0.000|x11: 0.118|x12: 0.114|x13: 0.117|x14: 0.364|x15: 0.199|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.492|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.022|x2: 0.000|x3: 0.000|x4: 0.024|x5: 0.022|x6: 0.091|x7: 0.120|x8: 0.022|x9: 0.221|x10: 0.022|x11: 0.030|x12: 0.050|x13: 0.044|x14: 0.162|x15: 0.314|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Machine learning algorithms have increased tremendously in power in recent years but have yet to be fully utilized in many ecology and sustainable resource management domains such as wildlife reserve design forest fire management and invasive species spread one thing these domains have in common is that they contain dynamics that can be characterized as a spatially spreading process ssp which requires many parameters to be set precisely to model the dynamics spread rates and directional biases of the elements which are spreading we present related work in artificial intelligence and machine learning for ssp sustainability domains including forest wildfire prediction we then introduce a novel approach for learning in ssp domains using reinforcement learning rl where fire is the agent at any cell in the landscape and the set of actions the fire can take from a location at any point in time includes spreading north south east or west or not spreading this approach inverts the usual rl setup since the dynamics of the corresponding markov decision process mdp is a known function for immed iate wildfire spread meanwhile we learn an agent policy for a predictive model of the dynamics of a complex spatial process rewards are provided for correctly classifying which cells are on fire or not compared with satellite and other related data we examine the behavior of five rl algorithms on this problem value iteration policy iteration qlearning monte carlo tree search and asynchronous advantage actorcritic a3c we compare to a gaussian processbased supervised learning approach and also discuss the relation of our approach to manually constructed stateoftheart methods from forest wildfire modeling we validate our approach with satellite image data of two massive wildfire events in northern alberta canada the fort mcmurray fire of 2016 and the richardson fire of 2011 the results show that we can learn predictive agentbased policies as models of spatial dynamics using rl on readily available satellite images that other methods and have many additional advantages in terms of generalizability and interpretability</t>
+          <t>machine learning algorithms have increased tremendously in power in recent years but have yet to be fully utilized in many ecology and sustainable resource management domains such as wildlife reserve design forest fire management and invasive species spread one thing these domains have in common is that they contain dynamics that can be characterized as a spatially spreading process ssp which requires many parameters to be set precisely to model the dynamics spread rates and directional biases of the elements which are spreading we present related work in artificial intelligence and machine learning for ssp sustainability domains including forest wildfire prediction we then introduce a novel approach for learning in ssp domains using reinforcement learning rl where fire is the agent at any cell in the landscape and the set of actions the fire can take from a location at any point in time includes spreading north south east or west or not spreading this approach inverts the usual rl setup since the dynamics of the corresponding markov decision process mdp is a known function for immed iate wildfire spread meanwhile we learn an agent policy for a predictive model of the dynamics of a complex spatial process rewards are provided for correctly classifying which cells are on fire or not compared with satellite and other related data we examine the behavior of five rl algorithms on this problem value iteration policy iteration qlearning monte carlo tree search and asynchronous advantage actorcritic a3c we compare to a gaussian processbased supervised learning approach and also discuss the relation of our approach to manually constructed stateoftheart methods from forest wildfire modeling we validate our approach with satellite image data of two massive wildfire events in northern alberta canada the fort mcmurray fire of 2016 and the richardson fire of 2011 the results show that we can learn predictive agentbased policies as models of spatial dynamics using rl on readily available satellite images that other methods and have many additional advantages in terms of generalizability and interpretability</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5031,16 +5031,16 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>[3, 4, 11, 15]</t>
+          <t>[4, 15]</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.723|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.418|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.150|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.185|x3: 0.157|x4: 0.381|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.186|x9: 0.075|x10: 0.000|x11: 0.186|x12: 0.000|x13: 0.148|x14: 0.000|x15: 0.502|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.261|x2: 0.000|x3: 0.000|x4: 0.303|x5: 0.164|x6: 0.144|x7: 0.379|x8: 0.290|x9: 0.317|x10: 0.000|x11: 0.206|x12: 0.334|x13: 0.405|x14: 0.247|x15: 0.327|x16: 0.087|x17: 0.000
-MEAN -&gt; x1: 0.087|x2: 0.062|x3: 0.219|x4: 0.228|x5: 0.055|x6: 0.048|x7: 0.126|x8: 0.159|x9: 0.131|x10: 0.000|x11: 0.270|x12: 0.111|x13: 0.184|x14: 0.082|x15: 0.326|x16: 0.029|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.064|x4: 0.065|x5: 0.055|x6: 0.054|x7: 0.059|x8: 0.061|x9: 0.059|x10: 0.052|x11: 0.068|x12: 0.058|x13: 0.062|x14: 0.056|x15: 0.072|x16: 0.053|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.159|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.084|x10: 0.000|x11: 0.080|x12: 0.072|x13: 0.000|x14: 0.000|x15: 0.348|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.185|x3: 0.157|x4: 0.381|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.186|x9: 0.075|x10: 0.000|x11: 0.186|x12: 0.000|x13: 0.148|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.121|x5: 0.000|x6: 0.071|x7: 0.142|x8: 0.000|x9: 0.090|x10: 0.000|x11: 0.182|x12: 0.135|x13: 0.115|x14: 0.109|x15: 0.143|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.046|x3: 0.039|x4: 0.165|x5: 0.000|x6: 0.018|x7: 0.036|x8: 0.046|x9: 0.062|x10: 0.000|x11: 0.112|x12: 0.052|x13: 0.066|x14: 0.027|x15: 0.373|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>The ability of ai systems to transform vast amounts of complex ambiguous information into insight has the potential to reveal longheld secrets and help solve some of the worlds most enduring problems  however like all powerful technologies great care must be taken in its development and deployment to reap the societal benefits of ai systems we will first need to trust them and make sure that they follow the same ethical principles moral values professional codes and social norms that we humans would follow in the same scenario research and educational efforts as well as carefully designed regulations must be put in place to achieve this goal  international business machines corporation ibm is actively engaged both internally as well as with its collaborators and competitors in global discussions about how to make ai ethical and as beneficial as possible for people as society</t>
+          <t>the ability of ai systems to transform vast amounts of complex ambiguous information into insight has the potential to reveal longheld secrets and help solve some of the worlds most enduring problems however like all powerful technologies great care must be taken in its development and deployment to reap the societal benefits of ai systems we will first need to trust them and make sure that they follow the same ethical principles moral values professional codes and social norms that we humans would follow in the same scenario research and educational efforts as well as carefully designed regulations must be put in place to achieve this goal international business machines corporation ibm is actively engaged both internally as well as with its collaborators and competitors in global discussions about how to make ai ethical and as beneficial as possible for people as society</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5061,16 +5061,16 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[7, 9, 16]</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.112|x2: 0.000|x3: 0.308|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.076|x8: 0.000|x9: 0.102|x10: 0.000|x11: 0.178|x12: 0.080|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.176|x17: 0.000
-LDA -&gt; x1: 0.079|x2: 0.064|x3: 0.076|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.161|x8: 0.166|x9: 0.606|x10: 0.000|x11: 0.000|x12: 0.101|x13: 0.092|x14: 0.250|x15: 0.067|x16: 0.159|x17: 0.000
-TOP2VEC -&gt; x1: 0.265|x2: 0.252|x3: 0.000|x4: 0.143|x5: 0.219|x6: 0.000|x7: 0.346|x8: 0.269|x9: 0.097|x10: 0.093|x11: 0.000|x12: 0.367|x13: 0.376|x14: 0.282|x15: 0.229|x16: 0.191|x17: 0.000
-MEAN -&gt; x1: 0.152|x2: 0.105|x3: 0.128|x4: 0.048|x5: 0.073|x6: 0.000|x7: 0.194|x8: 0.145|x9: 0.233|x10: 0.031|x11: 0.059|x12: 0.182|x13: 0.156|x14: 0.177|x15: 0.098|x16: 0.175|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.058|x3: 0.059|x4: 0.055|x5: 0.056|x6: 0.052|x7: 0.064|x8: 0.060|x9: 0.066|x10: 0.054|x11: 0.055|x12: 0.063|x13: 0.061|x14: 0.062|x15: 0.058|x16: 0.062|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.106|x2: 0.000|x3: 0.081|x4: 0.000|x5: 0.076|x6: 0.000|x7: 0.074|x8: 0.000|x9: 0.187|x10: 0.000|x11: 0.070|x12: 0.000|x13: 0.000|x14: 0.074|x15: 0.000|x16: 0.172|x17: 0.000
+LDA -&gt; x1: 0.079|x2: 0.064|x3: 0.076|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.161|x8: 0.166|x9: 0.500|x10: 0.000|x11: 0.000|x12: 0.101|x13: 0.092|x14: 0.250|x15: 0.067|x16: 0.159|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.151|x3: 0.000|x4: 0.133|x5: 0.000|x6: 0.000|x7: 0.430|x8: 0.302|x9: 0.148|x10: 0.000|x11: 0.169|x12: 0.230|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.046|x2: 0.054|x3: 0.039|x4: 0.033|x5: 0.019|x6: 0.000|x7: 0.166|x8: 0.117|x9: 0.209|x10: 0.000|x11: 0.060|x12: 0.083|x13: 0.023|x14: 0.081|x15: 0.017|x16: 0.208|x17: 0.000
 </t>
         </is>
       </c>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Over recent years we have witnessed an exponential growth in the use of automation to power decisions that impact our lives and societies while these bring many potential benefits eg reducing human bias speeding up decisionmaking they are also fraught with risk eg increasing machine bias rendering the decisionmaking more opaque and remote to people a consideration for the fairness accountability and transparency of these processes is therefore fundamental omidyar networks governance  citizen engagement initiative started funding and advocating for open data in 2012 following the snowden revelations in the summer of 2013 we included privacy and surveillance reform as part of those efforts realizing that openness and privacy were closely related we focused on helping develop a framework governing the collection of access to storage and usage of and rights over data more recently we started looking at the impact of these data releases under a new light as both processing power and access to data increased decisions made by both government and corporate sector actors were becoming increasingly automated if governments use algorithms to screen immigrants and allocate social services it is vital that we know how to interrogate and hold these systems accountable our main aim is to increase individuals control and agency over the decisions that impact their lives and ultimately societies we believe that the accountability and transparency agenda would benefit from better understanding and ultimately scrutinizing automated decisionmaking to explore some of these questions we partnered with upturn to map out the landscape of public scrutiny of automated decisionmaking both in terms of what civil society was or was not doing in this nascent sector and what laws regulations were or were not in place to help regulate it as the study developed it became clear that it could pave the way for a more textured as well as practical understanding of algorithmic transparency omidyar network will explore some of these issues further in a companion paper to be released later this year our hope is that this report will help civil society actors consider how much they have to gain in empowering the public and their audiences to effectively scrutinize understand and help govern automated decisions we also hope that it will start laying a policy framework for this governance adding to the growing and rich literature on the social and economic impact of such decisions finally we hope that the reports findings and analysis will help inform other funders decisions in this important and growing field as it will our own</t>
+          <t>over recent years we have witnessed an exponential growth in the use of automation to power decisions that impact our lives and societies while these bring many potential benefits eg reducing human bias speeding up decisionmaking they are also fraught with risk eg increasing machine bias rendering the decisionmaking more opaque and remote to people a consideration for the fairness accountability and transparency of these processes is therefore fundamental omidyar networks governance citizen engagement initiative started funding and advocating for open data in 2012 following the snowden revelations in the summer of 2013 we included privacy and surveillance reform as part of those efforts realizing that openness and privacy were closely related we focused on helping develop a framework governing the collection of access to storage and usage of and rights over data more recently we started looking at the impact of these data releases under a new light as both processing power and access to data increased decisions made by both government and corporate sector actors were becoming increasingly automated if governments use algorithms to screen immigrants and allocate social services it is vital that we know how to interrogate and hold these systems accountable our main aim is to increase individuals control and agency over the decisions that impact their lives and ultimately societies we believe that the accountability and transparency agenda would benefit from better understanding and ultimately scrutinizing automated decisionmaking to explore some of these questions we partnered with upturn to map out the landscape of public scrutiny of automated decisionmaking both in terms of what civil society was or was not doing in this nascent sector and what laws regulations were or were not in place to help regulate it as the study developed it became clear that it could pave the way for a more textured as well as practical understanding of algorithmic transparency omidyar network will explore some of these issues further in a companion paper to be released later this year our hope is that this report will help civil society actors consider how much they have to gain in empowering the public and their audiences to effectively scrutinize understand and help govern automated decisions we also hope that it will start laying a policy framework for this governance adding to the growing and rich literature on the social and economic impact of such decisions finally we hope that the reports findings and analysis will help inform other funders decisions in this important and growing field as it will our own</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5091,16 +5091,16 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>[3, 14]</t>
+          <t>[9, 14, 16]</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.103|x2: 0.000|x3: 0.470|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.070|x9: 0.000|x10: 0.000|x11: 0.308|x12: 0.062|x13: 0.080|x14: 0.061|x15: 0.000|x16: 0.145|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.097|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.066|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.204|x10: 0.000|x11: 0.178|x12: 0.000|x13: 0.000|x14: 0.073|x15: 0.000|x16: 0.169|x17: 0.000
 LDA -&gt; x1: 0.000|x2: 0.080|x3: 0.154|x4: 0.063|x5: 0.129|x6: 0.000|x7: 0.130|x8: 0.148|x9: 0.153|x10: 0.124|x11: 0.000|x12: 0.140|x13: 0.172|x14: 0.273|x15: 0.000|x16: 0.253|x17: 0.000
-TOP2VEC -&gt; x1: 0.144|x2: 0.158|x3: 0.138|x4: 0.197|x5: 0.259|x6: 0.250|x7: 0.101|x8: 0.157|x9: 0.251|x10: 0.074|x11: 0.123|x12: 0.146|x13: 0.285|x14: 0.322|x15: 0.147|x16: 0.151|x17: 0.000
-MEAN -&gt; x1: 0.082|x2: 0.079|x3: 0.254|x4: 0.087|x5: 0.129|x6: 0.083|x7: 0.077|x8: 0.125|x9: 0.135|x10: 0.066|x11: 0.144|x12: 0.116|x13: 0.179|x14: 0.219|x15: 0.049|x16: 0.183|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.056|x3: 0.067|x4: 0.057|x5: 0.059|x6: 0.057|x7: 0.056|x8: 0.059|x9: 0.060|x10: 0.056|x11: 0.060|x12: 0.059|x13: 0.062|x14: 0.065|x15: 0.055|x16: 0.063|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.113|x5: 0.139|x6: 0.105|x7: 0.161|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.223|x12: 0.095|x13: 0.000|x14: 0.170|x15: 0.074|x16: 0.069|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.322|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.024|x2: 0.020|x3: 0.039|x4: 0.044|x5: 0.083|x6: 0.026|x7: 0.073|x8: 0.037|x9: 0.169|x10: 0.031|x11: 0.100|x12: 0.059|x13: 0.043|x14: 0.129|x15: 0.019|x16: 0.123|x17: 0.000
 </t>
         </is>
       </c>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Protected areas are an effective tool for reducing biodiversity loss current legislation distinguishes various types of marine protected areas each allowing different levels of resource extraction however almost all of the theory for spatial conservation planning is focused on identifying notake reserves the current approaches to zoning for multiple types of protected areas could result in suboptimal plans in terms of protecting biodiversity and minimizing negative socioeconomic impacts we overcame these limitations in the first application of the multizone planning tool marxan with zones to design a network of four types of protected areas in the context of californias marine life protection act we have produced a zoning configuration that entails mean value losses of less than 9 for every fishery without compromising conservation goals we also found that a spatial numerical optimization tool that allows for multiple zones outperforms a tool that can identify one zone ie marine reserves in two ways first the overall impact on the fishing industry is reduced and second a more equitable impact on different fishing sectors is achieved finally we examined the tradeoffs between representing biodiversity features and impacting fisheries our approach is applicable to both marine and terrestrial conservation planning and delivers an ecosystembased management outcome that balances conservation and industry objectives</t>
+          <t>protected areas are an effective tool for reducing biodiversity loss current legislation distinguishes various types of marine protected areas each allowing different levels of resource extraction however almost all of the theory for spatial conservation planning is focused on identifying notake reserves the current approaches to zoning for multiple types of protected areas could result in suboptimal plans in terms of protecting biodiversity and minimizing negative socioeconomic impacts we overcame these limitations in the first application of the multizone planning tool marxan with zones to design a network of four types of protected areas in the context of californias marine life protection act we have produced a zoning configuration that entails mean value losses of less than 9 for every fishery without compromising conservation goals we also found that a spatial numerical optimization tool that allows for multiple zones outperforms a tool that can identify one zone ie marine reserves in two ways first the overall impact on the fishing industry is reduced and second a more equitable impact on different fishing sectors is achieved finally we examined the tradeoffs between representing biodiversity features and impacting fisheries our approach is applicable to both marine and terrestrial conservation planning and delivers an ecosystembased management outcome that balances conservation and industry objectives</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5126,11 +5126,11 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.328|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.190|x12: 0.000|x13: 0.000|x14: 0.747|x15: 0.579|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.081|x3: 0.074|x4: 0.085|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.130|x9: 0.163|x10: 0.000|x11: 0.119|x12: 0.000|x13: 0.059|x14: 0.430|x15: 0.679|x16: 0.000|x17: 0.000
-TOP2VEC -&gt; x1: 0.172|x2: 0.205|x3: 0.000|x4: 0.000|x5: 0.073|x6: 0.000|x7: 0.239|x8: 0.204|x9: 0.223|x10: 0.000|x11: 0.198|x12: 0.213|x13: 0.224|x14: 0.507|x15: 0.338|x16: 0.000|x17: 0.000
-MEAN -&gt; x1: 0.057|x2: 0.095|x3: 0.134|x4: 0.028|x5: 0.024|x6: 0.000|x7: 0.080|x8: 0.111|x9: 0.129|x10: 0.000|x11: 0.169|x12: 0.071|x13: 0.095|x14: 0.477|x15: 0.446|x16: 0.000|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.059|x4: 0.054|x5: 0.053|x6: 0.052|x7: 0.056|x8: 0.058|x9: 0.059|x10: 0.052|x11: 0.062|x12: 0.056|x13: 0.057|x14: 0.084|x15: 0.081|x16: 0.052|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.102|x10: 0.000|x11: 0.054|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.500|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.081|x3: 0.074|x4: 0.085|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.130|x9: 0.163|x10: 0.000|x11: 0.119|x12: 0.000|x13: 0.059|x14: 0.430|x15: 0.500|x16: 0.000|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.133|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.105|x12: 0.287|x13: 0.000|x14: 0.403|x15: 0.215|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.020|x3: 0.018|x4: 0.021|x5: 0.000|x6: 0.000|x7: 0.033|x8: 0.032|x9: 0.066|x10: 0.000|x11: 0.069|x12: 0.072|x13: 0.015|x14: 0.458|x15: 0.304|x16: 0.000|x17: 0.000
 </t>
         </is>
       </c>
@@ -5141,7 +5141,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>The national oceanic and atmospheric administrations noaa integrated coral observing network icon has been operational since 2000 and works closely with most us government and many international environmental partners involved in coral reef research the icon program has pioneered the use of artificial intelligence techniques to assess near realtime data streams from environment sensor networks such as the seakeys network florida keys the australia institute of marine science weather network noaas coral reef ecosystem division network in the pacific and its own integrated coral observing network icon of stations in the caribbean besides its innovative approach to coral monitoring station deployments the icon program recently pioneered techniques for the near realtime integration of satellite in situ and radar data sources for purposes of ecological forecasting of such events as coral bleaching coral spawning upwelling and other marine behavioral or physical oceanographic events the icon program has also ushered in the use of pulseamplitude modulating fluorometry to measure near realtime physiological recording of response to environmental stress during coral bleaching thus providing even better ecological forecasting capabilities through artificial intelligence and data integrative techniques herewith we describe these techniques along with a report on new coral calcification instrumentation augmenting the icon network sensor array</t>
+          <t>the national oceanic and atmospheric administrations noaa integrated coral observing network icon has been operational since 2000 and works closely with most us government and many international environmental partners involved in coral reef research the icon program has pioneered the use of artificial intelligence techniques to assess near realtime data streams from environment sensor networks such as the seakeys network florida keys the australia institute of marine science weather network noaas coral reef ecosystem division network in the pacific and its own integrated coral observing network icon of stations in the caribbean besides its innovative approach to coral monitoring station deployments the icon program recently pioneered techniques for the near realtime integration of satellite in situ and radar data sources for purposes of ecological forecasting of such events as coral bleaching coral spawning upwelling and other marine behavioral or physical oceanographic events the icon program has also ushered in the use of pulseamplitude modulating fluorometry to measure near realtime physiological recording of response to environmental stress during coral bleaching thus providing even better ecological forecasting capabilities through artificial intelligence and data integrative techniques herewith we describe these techniques along with a report on new coral calcification instrumentation augmenting the icon network sensor array</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5151,16 +5151,16 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>[5, 14]</t>
+          <t>[9, 14]</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.433|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.250|x12: 0.000|x13: 0.000|x14: 0.274|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.177|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.398|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.099|x2: 0.000|x3: 0.000|x4: 0.138|x5: 0.416|x6: 0.138|x7: 0.108|x8: 0.000|x9: 0.286|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.064|x14: 0.411|x15: 0.000|x16: 0.160|x17: 0.000
-TOP2VEC -&gt; x1: 0.095|x2: 0.143|x3: 0.000|x4: 0.000|x5: 0.225|x6: 0.283|x7: 0.329|x8: 0.110|x9: 0.279|x10: 0.078|x11: 0.230|x12: 0.161|x13: 0.233|x14: 0.513|x15: 0.147|x16: 0.160|x17: 0.000
-MEAN -&gt; x1: 0.065|x2: 0.048|x3: 0.144|x4: 0.046|x5: 0.213|x6: 0.140|x7: 0.146|x8: 0.037|x9: 0.188|x10: 0.026|x11: 0.160|x12: 0.054|x13: 0.099|x14: 0.395|x15: 0.049|x16: 0.107|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.055|x3: 0.060|x4: 0.055|x5: 0.065|x6: 0.060|x7: 0.061|x8: 0.054|x9: 0.063|x10: 0.054|x11: 0.061|x12: 0.055|x13: 0.058|x14: 0.078|x15: 0.055|x16: 0.058|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.123|x7: 0.138|x8: 0.000|x9: 0.059|x10: 0.000|x11: 0.203|x12: 0.198|x13: 0.170|x14: 0.462|x15: 0.247|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.025|x2: 0.000|x3: 0.000|x4: 0.035|x5: 0.104|x6: 0.065|x7: 0.062|x8: 0.000|x9: 0.130|x10: 0.000|x11: 0.051|x12: 0.050|x13: 0.058|x14: 0.443|x15: 0.062|x16: 0.040|x17: 0.000
 </t>
         </is>
       </c>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Marine cabled videoobservatories allow the nondestructive sampling of species at frequencies and durations that have never been attained before nevertheless the lack of appropriate methods to automatically process video imagery limits this technology for the purposes of ecosystem monitoring automation is a prerequisite to deal with the huge quantities of video footage captured by cameras which can then transform these devices into true autonomous sensors in this study we have developed a novel methodology that is based on genetic programming for contentbased image analysis our aim was to capture the temporal dynamics of fish abundance we processed more than 20000 images that were acquired in a challenging realworld coastal scenario at the obseaemso testingsite the images were collected at 30min frequency continuously for two years over day and night the highly variable environmental conditions allowed us to test the effectiveness of our approach under changing light radiation water turbidity background confusion and biofouling growth on the camera housing the automated recognition results were highly correlated with the manual counts and they were highly reliable when used to track fish variations at different hourly daily and monthly time scales in addition our methodology could be easily transferred to other cabled videoobservatories</t>
+          <t>marine cabled videoobservatories allow the nondestructive sampling of species at frequencies and durations that have never been attained before nevertheless the lack of appropriate methods to automatically process video imagery limits this technology for the purposes of ecosystem monitoring automation is a prerequisite to deal with the huge quantities of video footage captured by cameras which can then transform these devices into true autonomous sensors in this study we have developed a novel methodology that is based on genetic programming for contentbased image analysis our aim was to capture the temporal dynamics of fish abundance we processed more than 20000 images that were acquired in a challenging realworld coastal scenario at the obseaemso testingsite the images were collected at 30min frequency continuously for two years over day and night the highly variable environmental conditions allowed us to test the effectiveness of our approach under changing light radiation water turbidity background confusion and biofouling growth on the camera housing the automated recognition results were highly correlated with the manual counts and they were highly reliable when used to track fish variations at different hourly daily and monthly time scales in addition our methodology could be easily transferred to other cabled videoobservatories</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5181,16 +5181,16 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>[3, 11, 14]</t>
+          <t>[8, 11, 14]</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.460|x4: 0.000|x5: 0.000|x6: 0.099|x7: 0.000|x8: 0.056|x9: 0.000|x10: 0.000|x11: 0.266|x12: 0.000|x13: 0.000|x14: 0.216|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.201|x7: 0.000|x8: 0.095|x9: 0.000|x10: 0.000|x11: 0.106|x12: 0.000|x13: 0.000|x14: 0.311|x15: 0.083|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.085|x2: 0.098|x3: 0.149|x4: 0.118|x5: 0.000|x6: 0.059|x7: 0.072|x8: 0.162|x9: 0.270|x10: 0.000|x11: 0.145|x12: 0.000|x13: 0.000|x14: 0.423|x15: 0.151|x16: 0.088|x17: 0.000
-TOP2VEC -&gt; x1: 0.187|x2: 0.000|x3: 0.138|x4: 0.356|x5: 0.138|x6: 0.246|x7: 0.408|x8: 0.214|x9: 0.170|x10: 0.087|x11: 0.399|x12: 0.195|x13: 0.227|x14: 0.293|x15: 0.122|x16: 0.179|x17: 0.000
-MEAN -&gt; x1: 0.091|x2: 0.033|x3: 0.249|x4: 0.158|x5: 0.046|x6: 0.135|x7: 0.160|x8: 0.144|x9: 0.146|x10: 0.029|x11: 0.270|x12: 0.065|x13: 0.076|x14: 0.310|x15: 0.091|x16: 0.089|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.054|x3: 0.066|x4: 0.061|x5: 0.054|x6: 0.059|x7: 0.061|x8: 0.060|x9: 0.060|x10: 0.053|x11: 0.068|x12: 0.055|x13: 0.056|x14: 0.071|x15: 0.057|x16: 0.057|x17: 0.052
+TOP2VEC -&gt; x1: 0.000|x2: 0.116|x3: 0.000|x4: 0.074|x5: 0.000|x6: 0.139|x7: 0.280|x8: 0.223|x9: 0.121|x10: 0.090|x11: 0.292|x12: 0.121|x13: 0.102|x14: 0.078|x15: 0.000|x16: 0.057|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.500|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.021|x2: 0.053|x3: 0.037|x4: 0.048|x5: 0.000|x6: 0.100|x7: 0.088|x8: 0.120|x9: 0.098|x10: 0.023|x11: 0.136|x12: 0.030|x13: 0.025|x14: 0.328|x15: 0.058|x16: 0.036|x17: 0.000
 </t>
         </is>
       </c>
@@ -5201,7 +5201,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Having accurate detailed and uptodate information about the location and behavior of animals in the wild would improve our ability to study and conserve ecosystems we investigate the ability to automatically accurately and inexpensively collect such data which could help catalyze the transformation of many fields of ecology wildlife biology zoology conservation biology and animal behavior into big data sciences motionsensor camera traps enable collecting wildlife pictures inexpensively unobtrusively and frequently however extracting information from these pictures remains an expensive timeconsuming manual task we demonstrate that such information can be automatically extracted by deep learning a cuttingedge type of artificial intelligence we train deep convolutional neural networks to identify count and describe the behaviors of 48 species in the 32 millionimage snapshot serengeti dataset our deep neural networks automatically identify animals with 938 accuracy and we expect that number to improve rapidly in years to come more importantly if our system classifies only images it is confident about our system can automate animal identification for 993 of the data while still performing at the same 966 accuracy as that of crowdsourced teams of human volunteers saving 84 y ie 17000 h at 40 hwk of human labeling effort on this 32 millionimage dataset those efficiency gains highlight the importance of using deep neural networks to automate data extraction from cameratrap images reducing a roadblock for this widely used technology our results suggest that deep learning could enable the inexpensive unobtrusive highvolume and even realtime collection of a wealth of information about vast numbers of animals in the wild</t>
+          <t>having accurate detailed and uptodate information about the location and behavior of animals in the wild would improve our ability to study and conserve ecosystems we investigate the ability to automatically accurately and inexpensively collect such data which could help catalyze the transformation of many fields of ecology wildlife biology zoology conservation biology and animal behavior into big data sciences motionsensor camera traps enable collecting wildlife pictures inexpensively unobtrusively and frequently however extracting information from these pictures remains an expensive timeconsuming manual task we demonstrate that such information can be automatically extracted by deep learning a cuttingedge type of artificial intelligence we train deep convolutional neural networks to identify count and describe the behaviors of 48 species in the 32 millionimage snapshot serengeti dataset our deep neural networks automatically identify animals with 938 accuracy and we expect that number to improve rapidly in years to come more importantly if our system classifies only images it is confident about our system can automate animal identification for 993 of the data while still performing at the same 966 accuracy as that of crowdsourced teams of human volunteers saving 84 y ie 17000 h at 40 hwk of human labeling effort on this 32 millionimage dataset those efficiency gains highlight the importance of using deep neural networks to automate data extraction from cameratrap images reducing a roadblock for this widely used technology our results suggest that deep learning could enable the inexpensive unobtrusive highvolume and even realtime collection of a wealth of information about vast numbers of animals in the wild</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5211,16 +5211,16 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>[4, 11, 15]</t>
+          <t>[4, 15]</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.679|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.392|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.069|x3: 0.000|x4: 0.090|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.099|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.096|x15: 0.228|x16: 0.112|x17: 0.000
 LDA -&gt; x1: 0.096|x2: 0.117|x3: 0.000|x4: 0.382|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.108|x9: 0.170|x10: 0.000|x11: 0.000|x12: 0.158|x13: 0.000|x14: 0.183|x15: 0.386|x16: 0.220|x17: 0.000
-TOP2VEC -&gt; x1: 0.236|x2: 0.428|x3: 0.000|x4: 0.316|x5: 0.218|x6: 0.279|x7: 0.348|x8: 0.318|x9: 0.371|x10: 0.118|x11: 0.252|x12: 0.425|x13: 0.195|x14: 0.369|x15: 0.255|x16: 0.243|x17: 0.000
-MEAN -&gt; x1: 0.111|x2: 0.182|x3: 0.167|x4: 0.233|x5: 0.073|x6: 0.093|x7: 0.116|x8: 0.142|x9: 0.180|x10: 0.039|x11: 0.215|x12: 0.194|x13: 0.065|x14: 0.184|x15: 0.214|x16: 0.154|x17: 0.000
-SOFTMAX -&gt; x1: 0.057|x2: 0.061|x3: 0.060|x4: 0.064|x5: 0.055|x6: 0.056|x7: 0.057|x8: 0.059|x9: 0.061|x10: 0.053|x11: 0.063|x12: 0.062|x13: 0.055|x14: 0.061|x15: 0.063|x16: 0.060|x17: 0.051
+TOP2VEC -&gt; x1: 0.063|x2: 0.157|x3: 0.000|x4: 0.102|x5: 0.054|x6: 0.237|x7: 0.116|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.221|x13: 0.000|x14: 0.141|x15: 0.191|x16: 0.059|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.040|x2: 0.086|x3: 0.000|x4: 0.143|x5: 0.013|x6: 0.059|x7: 0.029|x8: 0.027|x9: 0.067|x10: 0.000|x11: 0.069|x12: 0.095|x13: 0.000|x14: 0.105|x15: 0.326|x16: 0.098|x17: 0.000
 </t>
         </is>
       </c>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Species and ecosystems worldwide continue to decline and disappear in spite of decades of investment in conservation efforts systematic conservation planning scp is a field of study designed to improve conservation programs by identifying land configurations that if protected would most efficiently sustain biodiversity despite contributing to species persistence in landscapes scp has been criticized for replacing sitebased conservation plans that often consider social context in contrast land system science lss an emerging field that explores the process of landuse and landcover change integrates social systems and processes into conservation analyses we suggest that by incorporating insights from lss on social processes eg livelihood adaptation or agricultural intensification scp can enhance the legitimacy of conservation plans thereby reducing the gap between conservation planning and implementation this represents a necessary first step for scp to reinvent itself as a decisionsupport tool that helps to reconcile the longstanding divide between landscapelevel species conservation and social needs</t>
+          <t>species and ecosystems worldwide continue to decline and disappear in spite of decades of investment in conservation efforts systematic conservation planning scp is a field of study designed to improve conservation programs by identifying land configurations that if protected would most efficiently sustain biodiversity despite contributing to species persistence in landscapes scp has been criticized for replacing sitebased conservation plans that often consider social context in contrast land system science lss an emerging field that explores the process of landuse and landcover change integrates social systems and processes into conservation analyses we suggest that by incorporating insights from lss on social processes eg livelihood adaptation or agricultural intensification scp can enhance the legitimacy of conservation plans thereby reducing the gap between conservation planning and implementation this represents a necessary first step for scp to reinvent itself as a decisionsupport tool that helps to reconcile the longstanding divide between landscapelevel species conservation and social needs</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -5246,11 +5246,11 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.109|x2: 0.000|x3: 0.331|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.191|x12: 0.000|x13: 0.122|x14: 0.169|x15: 0.426|x16: 0.000|x17: 0.000
-LDA -&gt; x1: 0.151|x2: 0.107|x3: 0.196|x4: 0.124|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.101|x11: 0.000|x12: 0.000|x13: 0.264|x14: 0.143|x15: 0.676|x16: 0.057|x17: 0.000
-TOP2VEC -&gt; x1: 0.150|x2: 0.393|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.106|x9: 0.157|x10: 0.000|x11: 0.230|x12: 0.311|x13: 0.463|x14: 0.393|x15: 0.472|x16: 0.085|x17: 0.000
-MEAN -&gt; x1: 0.137|x2: 0.167|x3: 0.176|x4: 0.041|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.035|x9: 0.052|x10: 0.034|x11: 0.141|x12: 0.104|x13: 0.283|x14: 0.235|x15: 0.466|x16: 0.047|x17: 0.000
-SOFTMAX -&gt; x1: 0.060|x2: 0.062|x3: 0.062|x4: 0.054|x5: 0.052|x6: 0.052|x7: 0.052|x8: 0.054|x9: 0.055|x10: 0.054|x11: 0.060|x12: 0.058|x13: 0.069|x14: 0.066|x15: 0.083|x16: 0.055|x17: 0.052
+          <t xml:space="preserve">NMF -&gt; x1: 0.151|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.101|x14: 0.114|x15: 0.500|x16: 0.000|x17: 0.000
+LDA -&gt; x1: 0.151|x2: 0.107|x3: 0.196|x4: 0.124|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.101|x11: 0.000|x12: 0.000|x13: 0.264|x14: 0.143|x15: 0.500|x16: 0.057|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.065|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.120|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.074|x12: 0.329|x13: 0.279|x14: 0.310|x15: 0.280|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.076|x2: 0.043|x3: 0.049|x4: 0.031|x5: 0.000|x6: 0.000|x7: 0.030|x8: 0.000|x9: 0.000|x10: 0.025|x11: 0.018|x12: 0.082|x13: 0.161|x14: 0.142|x15: 0.445|x16: 0.014|x17: 0.000
 </t>
         </is>
       </c>
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Identifying the boundary of a species niche from observational and environmental data is a common problem in ecology and conservation biology and a variety of techniques have been developed or applied to model niches and predict distributions here we examine the performance of some pattern recognition methods as ecological niche models enms particularly oneclass pattern recognition is a flexible and seldom used methodology for modeling ecological niches and distributions from presenceonly data the development of oneclass methods that perform comparably to twoclass methods for presenceabsence data would remove modeling decisions about sampling pseudoabsences or background data points when absence points are unavailable 2 we studied 9 methods for oneclass classification and 7 methods for twoclass classification 5 common to both all primarily used in pattern recognition and therefore not common in species distribution and ecological niche modeling across a set of 106 mountain plant species for which presenceabsence data was available we assessed accuracy using standard metrics and compared tradeoffs in omission and commission errors between classification groups as well as effects of prevalence and spatial autocorrelation on accuracy oneclass models fit to presenceonly data were comparable to twoclass models fit to presenceabsence data when performance was evaluated with a measure weighting omission and commission errors equally oneclass models were superior for reducing omission errors ie yielding higher sensitivity and twoclasses models were superior for reducing commission errors ie yielding higher specificity for these methods spatial autocorrelation was only influential when prevalence was low 4 these results differ from previous efforts to evaluate alternative modelling approaches to build enm and are particularly noteworthy because data are from exhaustively sampled populations minimizing false absence records accurate transferable models of species ecological niches and distributions are needed to advance ecological research and are crucial for effective environmental planning and conservation the patternrecognition approaches studied here show good potential for future modeling studies this study also provides an introduction to promising methods for ecological modeling inherited from the pattern recognition discipline</t>
+          <t>identifying the boundary of a species niche from observational and environmental data is a common problem in ecology and conservation biology and a variety of techniques have been developed or applied to model niches and predict distributions here we examine the performance of some pattern recognition methods as ecological niche models enms particularly oneclass pattern recognition is a flexible and seldom used methodology for modeling ecological niches and distributions from presenceonly data the development of oneclass methods that perform comparably to twoclass methods for presenceabsence data would remove modeling decisions about sampling pseudoabsences or background data points when absence points are unavailable 2 we studied 9 methods for oneclass classification and 7 methods for twoclass classification 5 common to both all primarily used in pattern recognition and therefore not common in species distribution and ecological niche modeling across a set of 106 mountain plant species for which presenceabsence data was available we assessed accuracy using standard metrics and compared tradeoffs in omission and commission errors between classification groups as well as effects of prevalence and spatial autocorrelation on accuracy oneclass models fit to presenceonly data were comparable to twoclass models fit to presenceabsence data when performance was evaluated with a measure weighting omission and commission errors equally oneclass models were superior for reducing omission errors ie yielding higher sensitivity and twoclasses models were superior for reducing commission errors ie yielding higher specificity for these methods spatial autocorrelation was only influential when prevalence was low 4 these results differ from previous efforts to evaluate alternative modelling approaches to build enm and are particularly noteworthy because data are from exhaustively sampled populations minimizing false absence records accurate transferable models of species ecological niches and distributions are needed to advance ecological research and are crucial for effective environmental planning and conservation the patternrecognition approaches studied here show good potential for future modeling studies this study also provides an introduction to promising methods for ecological modeling inherited from the pattern recognition discipline</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5271,16 +5271,16 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>[3, 11, 15]</t>
+          <t>[15]</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.688|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.398|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.054|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.123|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.060|x10: 0.000|x11: 0.073|x12: 0.128|x13: 0.000|x14: 0.000|x15: 0.206|x16: 0.062|x17: 0.000
 LDA -&gt; x1: 0.103|x2: 0.121|x3: 0.116|x4: 0.305|x5: 0.131|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.101|x11: 0.183|x12: 0.059|x13: 0.115|x14: 0.083|x15: 0.396|x16: 0.108|x17: 0.000
-TOP2VEC -&gt; x1: 0.000|x2: 0.084|x3: 0.000|x4: 0.000|x5: 0.195|x6: 0.158|x7: 0.253|x8: 0.000|x9: 0.000|x10: 0.095|x11: 0.239|x12: 0.075|x13: 0.111|x14: 0.247|x15: 0.213|x16: 0.195|x17: 0.000
-MEAN -&gt; x1: 0.034|x2: 0.068|x3: 0.205|x4: 0.102|x5: 0.109|x6: 0.053|x7: 0.084|x8: 0.000|x9: 0.000|x10: 0.065|x11: 0.273|x12: 0.045|x13: 0.075|x14: 0.110|x15: 0.221|x16: 0.101|x17: 0.000
-SOFTMAX -&gt; x1: 0.055|x2: 0.057|x3: 0.066|x4: 0.059|x5: 0.060|x6: 0.056|x7: 0.058|x8: 0.054|x9: 0.054|x10: 0.057|x11: 0.070|x12: 0.056|x13: 0.058|x14: 0.060|x15: 0.067|x16: 0.059|x17: 0.054
+TOP2VEC -&gt; x1: 0.000|x2: 0.067|x3: 0.000|x4: 0.000|x5: 0.142|x6: 0.000|x7: 0.303|x8: 0.000|x9: 0.000|x10: 0.183|x11: 0.208|x12: 0.252|x13: 0.207|x14: 0.255|x15: 0.253|x16: 0.129|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.500|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.026|x2: 0.047|x3: 0.060|x4: 0.076|x5: 0.068|x6: 0.000|x7: 0.076|x8: 0.000|x9: 0.015|x10: 0.071|x11: 0.116|x12: 0.110|x13: 0.081|x14: 0.085|x15: 0.339|x16: 0.075|x17: 0.000
 </t>
         </is>
       </c>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>We apply recently developed spatial biosurveillance techniques to the law enforcement domain with the goal of helping local police departments to rapidly detect and respond to or better yet to predict and prevent emerging spatial patterns of crime background geographic surveillance techniques have become increasingly important in law enforcement and crime prevention new methods for mapping crime 1 and for automatically detecting crime hot spots 2 using electronic case reports have increased situational awareness and enabled more rapid police response to emerging high crime areas additionally recent work in crime forecasting 34 has enabled law enforcement officials to predict and prevent rises in crime using a variety of leading indicator data however current crime detection and forecasting methods require a coarse aggregation of cases eg by month by square mile due to both computational considerations and the relatively small number of serious crimes these limitations reduce the spatial and temporal precision with which departments can pinpoint clusters of crime as well as their ability to rapidly respond to these clusters thus we propose the use of expectationbased spatial scan statistic methods 56 originally developed for the biosurveillance domain which can use a finer aggregation of data and can efficiently search for emerging spacetime clusters of varying size and duration we will use these methods both for detection of clusters of violent crime and for prediction of such clusters by detecting clusters of leading indicator crimes</t>
+          <t>we apply recently developed spatial biosurveillance techniques to the law enforcement domain with the goal of helping local police departments to rapidly detect and respond to or better yet to predict and prevent emerging spatial patterns of crime background geographic surveillance techniques have become increasingly important in law enforcement and crime prevention new methods for mapping crime 1 and for automatically detecting crime hot spots 2 using electronic case reports have increased situational awareness and enabled more rapid police response to emerging high crime areas additionally recent work in crime forecasting 34 has enabled law enforcement officials to predict and prevent rises in crime using a variety of leading indicator data however current crime detection and forecasting methods require a coarse aggregation of cases eg by month by square mile due to both computational considerations and the relatively small number of serious crimes these limitations reduce the spatial and temporal precision with which departments can pinpoint clusters of crime as well as their ability to rapidly respond to these clusters thus we propose the use of expectationbased spatial scan statistic methods 56 originally developed for the biosurveillance domain which can use a finer aggregation of data and can efficiently search for emerging spacetime clusters of varying size and duration we will use these methods both for detection of clusters of violent crime and for prediction of such clusters by detecting clusters of leading indicator crimes</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5301,16 +5301,16 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>[3, 11, 16]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.328|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.195|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.175|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.446|x17: 0.000
 LDA -&gt; x1: 0.092|x2: 0.146|x3: 0.216|x4: 0.064|x5: 0.096|x6: 0.000|x7: 0.000|x8: 0.167|x9: 0.100|x10: 0.000|x11: 0.207|x12: 0.254|x13: 0.000|x14: 0.064|x15: 0.000|x16: 0.415|x17: 0.000
-TOP2VEC -&gt; x1: 0.078|x2: 0.101|x3: 0.137|x4: 0.168|x5: 0.268|x6: 0.129|x7: 0.000|x8: 0.088|x9: 0.070|x10: 0.143|x11: 0.370|x12: 0.257|x13: 0.098|x14: 0.310|x15: 0.240|x16: 0.293|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.082|x3: 0.227|x4: 0.077|x5: 0.121|x6: 0.043|x7: 0.000|x8: 0.085|x9: 0.057|x10: 0.048|x11: 0.257|x12: 0.170|x13: 0.033|x14: 0.125|x15: 0.080|x16: 0.294|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.057|x3: 0.066|x4: 0.057|x5: 0.060|x6: 0.055|x7: 0.053|x8: 0.058|x9: 0.056|x10: 0.055|x11: 0.068|x12: 0.063|x13: 0.055|x14: 0.060|x15: 0.057|x16: 0.071|x17: 0.053
+TOP2VEC -&gt; x1: 0.000|x2: 0.000|x3: 0.077|x4: 0.079|x5: 0.213|x6: 0.062|x7: 0.092|x8: 0.000|x9: 0.000|x10: 0.073|x11: 0.060|x12: 0.100|x13: 0.000|x14: 0.067|x15: 0.147|x16: 0.278|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.023|x2: 0.036|x3: 0.073|x4: 0.036|x5: 0.077|x6: 0.016|x7: 0.023|x8: 0.042|x9: 0.025|x10: 0.018|x11: 0.067|x12: 0.088|x13: 0.000|x14: 0.033|x15: 0.037|x16: 0.410|x17: 0.000
 </t>
         </is>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Bullying is widespread in european schools despite multiple intervention strategies having been proposed over the years the present study investigates the effects of a novel virtual learning strategy fearnot to tackle bullying in both uk and german samples the approach is intended primarily for victims to increase their coping skills and further to heighten empathy and defence of victims by noninvolved bystanders this paper focuses on the defender role applying quantitative as well as qualitative methodology the present study found that fearnot helped noninvolved children to become defenders in the german subsample while it had no such effect in the uk subsample german new defenders children who are initially uninvolved But are nominated as defenders by their peers after the intervention period were found to be significantly more popular at baseline and to show more cognitive empathy theory of mind for the virtual victims as compared to permanently noninvolved pupils moreover gender interacts with becoming a defender in its effects on affective empathy with emotional contagion being particularly associated with new defender status among girls the findings are discussed in relation to previous research on antibullying intervention strategies and cultural differences in bullying prevalence rates and intervention outcomes</t>
+          <t>bullying is widespread in european schools despite multiple intervention strategies having been proposed over the years the present study investigates the effects of a novel virtual learning strategy fearnot to tackle bullying in both uk and german samples the approach is intended primarily for victims to increase their coping skills and further to heighten empathy and defence of victims by noninvolved bystanders this paper focuses on the defender role applying quantitative as well as qualitative methodology the present study found that fearnot helped noninvolved children to become defenders in the german subsample while it had no such effect in the uk subsample german new defenders children who are initially uninvolved but are nominated as defenders by their peers after the intervention period were found to be significantly more popular at baseline and to show more cognitive empathy theory of mind for the virtual victims as compared to permanently noninvolved pupils moreover gender interacts with becoming a defender in its effects on affective empathy with emotional contagion being particularly associated with new defender status among girls the findings are discussed in relation to previous research on antibullying intervention strategies and cultural differences in bullying prevalence rates and intervention outcomes</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5331,16 +5331,16 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>[2, 3, 4, 16]</t>
+          <t>[2, 4, 16]</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.328|x4: 0.194|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.168|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.365|x17: 0.000
-LDA -&gt; x1: 0.000|x2: 0.304|x3: 0.115|x4: 0.501|x5: 0.061|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.226|x13: 0.109|x14: 0.000|x15: 0.119|x16: 0.385|x17: 0.000
-TOP2VEC -&gt; x1: 0.169|x2: 0.391|x3: 0.201|x4: 0.430|x5: 0.145|x6: 0.000|x7: 0.062|x8: 0.220|x9: 0.182|x10: 0.139|x11: 0.106|x12: 0.000|x13: 0.122|x14: 0.137|x15: 0.000|x16: 0.284|x17: 0.000
-MEAN -&gt; x1: 0.056|x2: 0.232|x3: 0.214|x4: 0.375|x5: 0.069|x6: 0.000|x7: 0.021|x8: 0.073|x9: 0.061|x10: 0.046|x11: 0.091|x12: 0.075|x13: 0.077|x14: 0.046|x15: 0.040|x16: 0.345|x17: 0.000
-SOFTMAX -&gt; x1: 0.056|x2: 0.066|x3: 0.065|x4: 0.076|x5: 0.056|x6: 0.053|x7: 0.054|x8: 0.056|x9: 0.056|x10: 0.055|x11: 0.058|x12: 0.057|x13: 0.057|x14: 0.055|x15: 0.055|x16: 0.074|x17: 0.053
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.122|x4: 0.235|x5: 0.080|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.059|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.291|x17: 0.000
+LDA -&gt; x1: 0.000|x2: 0.304|x3: 0.115|x4: 0.500|x5: 0.061|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.226|x13: 0.109|x14: 0.000|x15: 0.119|x16: 0.385|x17: 0.000
+TOP2VEC -&gt; x1: 0.000|x2: 0.194|x3: 0.000|x4: 0.334|x5: 0.000|x6: 0.000|x7: 0.097|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.060|x12: 0.157|x13: 0.000|x14: 0.064|x15: 0.000|x16: 0.400|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.500|x17: 0.000
+MEAN -&gt; x1: 0.000|x2: 0.125|x3: 0.059|x4: 0.267|x5: 0.035|x6: 0.000|x7: 0.024|x8: 0.000|x9: 0.015|x10: 0.000|x11: 0.015|x12: 0.096|x13: 0.027|x14: 0.016|x15: 0.030|x16: 0.394|x17: 0.000
 </t>
         </is>
       </c>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Understanding video events the translation of lowlevel content in video sequences into high level semantic concepts is a research topic that has received much interest in recent years important applications of this work include smart surveillance systems semantic video database indexing and in teractive systems this technology can be applied to several video domains including airport terminal parking lot trac subway stations aerial surveillance and sign language data in this work we survey the two main components of the event understanding process abstraction and event modeling abstraction is the process of molding the data into informative units to be used as input to the event model event modeling is devoted to describing events of interest formally and enabling recognition of these events as they occur in the video sequence event modeling can be further decomposed in the categories of pattern recognition methods state event models and semantic event models in this survey we discuss this proposed taxonomy of the literature oer a unifying terminology and discuss popular abstraction schemes eg motion history images and event modeling formalisms eg hidden markov model and their use in video event understanding using extensive examples from the literature finally we consider the applica tion domain of video event understanding in light of the proposed taxonomy and propose future directions for research in this  eld</t>
+          <t>understanding video events the translation of lowlevel content in video sequences into high level semantic concepts is a research topic that has received much interest in recent years important applications of this work include smart surveillance systems semantic video database indexing and in teractive systems this technology can be applied to several video domains including airport terminal parking lot trac subway stations aerial surveillance and sign language data in this work we survey the two main components of the event understanding process abstraction and event modeling abstraction is the process of molding the data into informative units to be used as input to the event model event modeling is devoted to describing events of interest formally and enabling recognition of these events as they occur in the video sequence event modeling can be further decomposed in the categories of pattern recognition methods state event models and semantic event models in this survey we discuss this proposed taxonomy of the literature oer a unifying terminology and discuss popular abstraction schemes eg motion history images and event modeling formalisms eg hidden markov model and their use in video event understanding using extensive examples from the literature finally we consider the applica tion domain of video event understanding in light of the proposed taxonomy and propose future directions for research in this eld</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5361,16 +5361,16 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[13]</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.477|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.276|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+          <t xml:space="preserve">NMF -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.335|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
 LDA -&gt; x1: 0.306|x2: 0.097|x3: 0.171|x4: 0.089|x5: 0.206|x6: 0.072|x7: 0.126|x8: 0.074|x9: 0.223|x10: 0.061|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.073|x15: 0.210|x16: 0.113|x17: 0.000
-TOP2VEC -&gt; x1: 0.123|x2: 0.118|x3: 0.319|x4: 0.307|x5: 0.236|x6: 0.072|x7: 0.205|x8: 0.143|x9: 0.183|x10: 0.112|x11: 0.228|x12: 0.301|x13: 0.185|x14: 0.171|x15: 0.130|x16: 0.230|x17: 0.000
-MEAN -&gt; x1: 0.143|x2: 0.072|x3: 0.322|x4: 0.132|x5: 0.147|x6: 0.048|x7: 0.110|x8: 0.072|x9: 0.135|x10: 0.058|x11: 0.168|x12: 0.100|x13: 0.062|x14: 0.081|x15: 0.114|x16: 0.114|x17: 0.000
-SOFTMAX -&gt; x1: 0.061|x2: 0.056|x3: 0.073|x4: 0.060|x5: 0.061|x6: 0.055|x7: 0.059|x8: 0.056|x9: 0.060|x10: 0.056|x11: 0.062|x12: 0.058|x13: 0.056|x14: 0.057|x15: 0.059|x16: 0.059|x17: 0.053
+TOP2VEC -&gt; x1: 0.143|x2: 0.200|x3: 0.000|x4: 0.071|x5: 0.080|x6: 0.000|x7: 0.160|x8: 0.000|x9: 0.000|x10: 0.247|x11: 0.219|x12: 0.119|x13: 0.053|x14: 0.169|x15: 0.000|x16: 0.000|x17: 0.000
+BERTOPIC -&gt; x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.156|x12: 0.000|x13: 0.239|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000
+MEAN -&gt; x1: 0.112|x2: 0.074|x3: 0.043|x4: 0.040|x5: 0.072|x6: 0.018|x7: 0.071|x8: 0.018|x9: 0.056|x10: 0.077|x11: 0.094|x12: 0.030|x13: 0.157|x14: 0.060|x15: 0.053|x16: 0.028|x17: 0.000
 </t>
         </is>
       </c>

</xml_diff>